<commit_message>
Redone the random number generator. Updated Guide quests.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="79">
   <si>
     <t>id</t>
   </si>
@@ -137,49 +137,34 @@
     <t>&lt;p&gt;I want you to get to level 10. I do not want you to do this manually. Instead we are going to &lt;a href="/information/automation" target="_blank"&gt;explore&lt;/a&gt; for an hour. During this time you may gain a Faction level for Surface. The map you are currently on.&lt;/p&gt;&lt;p&gt;&lt;a href="/information/factions" target="_blank"&gt;Factions&lt;/a&gt; can be seen on your character sheet (tab) under the tab: Factions. As you kill creatures you gain faction points. As you level the faction, you can get what are called &lt;a href="/information/random-enchants" target="_blank"&gt;Unique’s&lt;/a&gt;. These can be powerful items and you may only have one equipped at a time.&lt;/p&gt;&lt;p&gt;To do this:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- First, find a monster in the drop down list you can kill in one hit.&lt;/p&gt;&lt;p&gt;- Next, click the Exploration green button.&lt;/p&gt;&lt;p&gt;- Select the monster you could kill, 1 hour, Attack.&lt;/p&gt;&lt;p&gt;- Click explore&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;Select the action Fight from the list of actions behind this modal.&lt;/p&gt;&lt;p&gt;- Find a monster you can kill in one shot.&lt;/p&gt;&lt;p&gt;- Next, close the fight section, select Exploration from the actions section&lt;/p&gt;&lt;p&gt;- Select the monster you could kill, 1 hour, 20 levels and Attack.&lt;/p&gt;&lt;p&gt;- Tap explore&lt;/p&gt;&lt;p&gt;Exploring will allow you to log out and idling gain items, exp, gold and possible quest item if the monster drops a quest item. There are things you cannot do while exploring such as change equipment, buy items from the &lt;a href="/information/shop" target="_blank"&gt;shop&lt;/a&gt; or &lt;a href="/information/market-board" target="_blank"&gt;market board&lt;/a&gt;. You will be told if you can do an action or not while exploring.&lt;/p&gt;&lt;p&gt;Exploration messages will appear, while logged in, in the Exploration chat tab below.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>Your own equipment</t>
-  </si>
-  <si>
-    <t>You spent the last week exploring the area around the town. Killing rats and other creatures you feel strong enough to take on. You return the INN every night and wait. You were once told, by your parents, to search out The Guide. A mysterious man who can help you on your adventures.&lt;br /&gt; &lt;br /&gt; Alas it has been a week and you have not seen him. You don’t even know what to look for or who to look for.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;I want you to equip some new gear. You might have by now, but chances are you have a ton of magical items from that Exploration you did. Your goal here is to raise your stats.&lt;/p&gt;&lt;p&gt;All &lt;a href="/information/equipment" target="_blank"&gt;base gear&lt;/a&gt; you can buy from the &lt;a href="/information/shop" target="_blank"&gt;shop&lt;/a&gt; will raise your stats by a %. The more expensive the gear, the better the stats. The items you have been finding lots of, are &lt;a href="/information/enchanting" target="_blank"&gt;enchanted&lt;/a&gt; with whats called Affixes. These enchantments give side effects to gear, such as damage, stats, stat reductions and so on.&lt;/p&gt;&lt;p&gt;I want you to raise your stats to 25 through equipment.&lt;/p&gt;&lt;p&gt;To do this:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Click the Character Sheet tab and on the right hand side you will see your inventory. Go through these items and look for ones that give +X% to your stats.&lt;/p&gt;&lt;p&gt;- You may have to visit the shop to buy some more expensive base items that raise the stats higher.&lt;/p&gt;&lt;p&gt;- To visit the shop, click the Hamburger icon in the top left, to open the menu.&lt;/p&gt;&lt;p&gt;- Click the shop, and select Buy from the General Shop&lt;/p&gt;&lt;p&gt;- Filter by what you are looking for and then sort by cost.&lt;/p&gt;&lt;p&gt;- You can click Compare to compare and replace or auto equip, the item&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;Tap the tab: Character Sheet and select, from the drop down list – Inventory management.&lt;/p&gt;&lt;p&gt;- Go through your items looking for ones that will add +X% to your stats.&lt;/p&gt;&lt;p&gt;- You may have to visit the shop by tapping the Hamburger icon at the top left of the screen.&lt;/p&gt;&lt;p&gt;- Tap on shop.&lt;/p&gt;&lt;p&gt;- Tap on Buy under General Shop.&lt;/p&gt;&lt;p&gt;- Filter by what you are looking for and sort by cost.&lt;/p&gt;&lt;p&gt;- You can tap Compare to compare and replace or auto equip, the item&lt;/p&gt;&lt;p&gt;Equipment comes in many forms and effects the strength of your character. The better the equipment and its enchantments, the better chance you have to take on stronger enemies. You cannot buy enchanted gear, but later we will look at making it.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>The Guide Appears</t>
-  </si>
-  <si>
-    <t>You feel more powerful. Better equipment, even a Unique you were gifted for fighting and clearing monsters around the town. You have a sense that nothing can take you down. You have heard of the more fowl beasts, but every time you try and kill one, you end up wounded, close to death.&lt;br /&gt; &lt;br /&gt; You rest, you heal your wounds and you try again, only to get smacked around like a rag doll.&lt;br /&gt; &lt;br /&gt; You sit alone in the INN, sitting by the fire. Drinking your failures away. A man sits at your table, no older then 25. he is dressed in a fedora hat, with a feather, blue leather pants and red tunic. He seems out of place, colorful. Cheerful.&lt;br /&gt; &lt;br /&gt; “I have been looking for you my child.” he states.&lt;br /&gt; &lt;br /&gt; “I am The Guide and by the looks of it you don't need much guidance child.”&lt;br /&gt; &lt;br /&gt; he laughs and studies you up and down. He can see the shiny item you possess.&lt;br /&gt; &lt;br /&gt; “A unique.” he states. “I haven’t seen one of those for a long time. You can get better ones, but you are not ready to visit the Queen just yet. No, instead you need to be able to take on more fearsome creatures.”&lt;br /&gt; &lt;br /&gt; You take a moment and explain about some of the creatures you try and take down only to be beaten to the brink of death.&lt;br /&gt; &lt;br /&gt; “Ahh yes, you need some skill child. Lets work on your ability to hit creatures with your weapon.”</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Now we focus on your &lt;a href="/information/skill-information" target="_blank"&gt;skills&lt;/a&gt;. You shiny unique might be able to take down some creatures but as you are finding it, its harder to take down the stronger beasts. To do this we must begin training in one of our skills. We can do this through exploration. Lets begin:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Please Note: &lt;/strong&gt;At this stage you may notice the amount of drops you were getting from enemies may have just fallen off a cliff. As we introduce you to skills, I will also introduce you to looting in the next quest which will slowly help you get more drops from enemies.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Click the Character Sheet tab&lt;/p&gt;&lt;p&gt;- Scroll down to skills.&lt;/p&gt;&lt;p&gt;- Find Accuracy, click train, select 10% of your XP and train the skill.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Tap the Character Sheet tab.&lt;/p&gt;&lt;p&gt;- Select Manage Skills&lt;/p&gt;&lt;p&gt;- Tap Train on the Accuracy Skill&lt;/p&gt;&lt;p&gt;- Select 10% of your XP and train the skill&lt;/p&gt;&lt;p&gt;What you have done is state: I want to sacrifice 10% of the XP I would get from killing monsters to place towards training my skill.&lt;/p&gt;&lt;p&gt;If you killed a Sewer Rat - you will get a quest item called Heart of the Eye which gives you bonus XP and Skill Bonus towards accuracy. You can see this in your Inventory section under quest items. All quest items are used automatically. You can click on the accuracy skill in the skill table to see the applied bonuses.&lt;/p&gt;&lt;p&gt;Some enchanted gear might have accuracy modifiers on them, if so - swap them out for the gear that effects your accuracy.&lt;/p&gt;&lt;p&gt;Heretics and Arcane Alchemists should switch their attack at this stage to &lt;a href="/information/combat" target="_blank"&gt;attack and cast or cast and attack&lt;/a&gt; and equip at least one or two damage spells. Prophets should also switch as well to get healing effects even with out a spell. Heretics can cast for a small percentage of their int with out a spell equipped, in case you cannot afford one yet, as well as Arcane Alchemists. Rangers could also equip a healing spell and use Cast and Attack or Attack and cast for healing bonuses as well&lt;/p&gt;</t>
+    <t>The Letter</t>
+  </si>
+  <si>
+    <t>You explore, you slaughter, you bathe in the enemies blood before you. You collect the shiny loot. You were gifted a green unique item from the towns people as a way of thanking you for your hard work.&lt;br /&gt; &lt;br /&gt; They told you that there are many other places one could explore, but that you could continue around here gain more favor with the people of the Surface plane.&lt;br /&gt; &lt;br /&gt; You wait for days and then weeks at the INN, where the hell is The Guide?&lt;br /&gt; &lt;br /&gt; “A letter for you” the barmaid states as she drops off your ale. You open it and read the following:&lt;br /&gt; &lt;br /&gt; Child. Listen, I am The Guide, alas I am investigating a situation. There is a magical spell upon your very being that allows the creatures you slaughter to gift you with the bounty of loot you have now, but that won’t last forever.&lt;br /&gt; &lt;br /&gt; You have to learn how to properly loot. You also have to have to learn how to wield your weapon, even casters can get into sticky situations where they need a weapon, and if you can’t hit anything – death will greet you faster then I.&lt;br /&gt; &lt;br /&gt; I also want you to investigate your gear, visit a shop. You gear is what makes you child. Know that.&lt;br /&gt; &lt;br /&gt; -- The Guide&lt;br /&gt; &lt;br /&gt; That’s it? Just barks orders through paper at you? You look around and contemplate doing what he want’s knowing full well you could just bugger off on your own adventure.&lt;br /&gt; &lt;br /&gt; By morning you have made up your mind on what to do.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We are going to learn about two things today: &lt;a href="/information/character-stats" target="_blank"&gt;Stats&lt;/a&gt; and &lt;a href="/information/skill-information" target="_blank"&gt;Skills&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;Characters under level 12, get a boost to their looting skill making drops a lot more fun. How ever as you will soon reach level 12 you will see the drop rate disappear. This is where skills come in handy.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Click the Character Sheet tab&lt;/p&gt;&lt;p&gt;- Scroll down to skills.&lt;/p&gt;&lt;p&gt;- Find Accuracy, click train, select 10% of your XP and train the skill.&lt;/p&gt;&lt;p&gt;Follow these same steps to train Looting after clicking Stop training on Accuracy.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Tap the Character Sheet tab.&lt;/p&gt;&lt;p&gt;- Select Manage Skills&lt;/p&gt;&lt;p&gt;- Tap Train on the Accuracy Skill&lt;/p&gt;&lt;p&gt;- Select 10% of your XP and train the skill&lt;/p&gt;&lt;p&gt;Follow these same steps to train Looting after clicking Stop training on Accuracy.&lt;/p&gt;&lt;p&gt;At any time you may click on the skill name to see applicable bonuses, xp, level and so on, The Skill Bonus refers to the bonus the skill applies when using it, such as for Accuracy or Looting. These skills take a while to level and later on you can even get enchanted gear with skill modifiers on them.&lt;/p&gt;&lt;p&gt;Next up, Stats. This ones easy. All character get 1 point into their stats with 1 extra point into their “damage stat.” Gear, especially enchanted gear, raises this by % which all stacks together to give you “Modded stats”.&lt;/p&gt;&lt;p&gt;The more expensive the gear, the better it is for you, enchanted can be better then &lt;a href="/information/shop" target="_blank"&gt;store gear&lt;/a&gt;, depending on the enchant. As you may know, that shiny unique boosted your stats. So Now, I need you to either buy or equip some drop gear:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Click the Character Sheet tab and on the right hand side you will see your inventory. Go through these items and look for ones that give +X% to your stats.&lt;/p&gt;&lt;p&gt;- You may have to visit the shop to buy some more expensive base items that raise the stats higher.&lt;/p&gt;&lt;p&gt;- To visit the shop, click the Hamburger icon in the top left, to open the menu.&lt;/p&gt;&lt;p&gt;- Click the shop, and select Buy from the General Shop&lt;/p&gt;&lt;p&gt;- Filter by what you are looking for and then sort by cost.&lt;/p&gt;&lt;p&gt;- You can click Compare to compare and replace or auto equip, the item&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;-&amp;nbsp;&lt;/strong&gt;Tap the tab: Character Sheet and select, from the drop down list – Inventory management.&lt;/p&gt;&lt;p&gt;- Go through your items looking for ones that will add +X% to your stats.&lt;/p&gt;&lt;p&gt;- You may have to visit the shop by tapping the Hamburger icon at the top left of the screen.&lt;/p&gt;&lt;p&gt;- Tap on shop.&lt;/p&gt;&lt;p&gt;- Tap on Buy under General Shop.&lt;/p&gt;&lt;p&gt;- Filter by what you are looking for and sort by cost.&lt;/p&gt;&lt;p&gt;- You can tap Compare to compare and replace or auto equip, the item&lt;/p&gt;&lt;p&gt;You can read up more on &lt;a href="/information/gear-progression" target="_blank"&gt;gear progression&lt;/a&gt; for more details. Tlessa is a pretty linear straight forward game with some mechanics thrown in to make it more fun. Now go have fun!&lt;/p&gt;</t>
   </si>
   <si>
     <t>Accuracy</t>
   </si>
   <si>
-    <t>Plundering and Looting</t>
-  </si>
-  <si>
-    <t>“Look at all your shiny objects, enchanted gear. It just spills through your pockets.” The Guide watches as you try and carry all this loot back from your latest adventure.&lt;br /&gt; &lt;br /&gt; “Child, most of that is probably useless.”&lt;br /&gt; &lt;br /&gt; You look at him and explain its dropping like candy. Why not take it?&lt;br /&gt; &lt;br /&gt; “Sigh, soon – I can’t say when, you will loose all that shiny gear and you will have to properly loot your enemies.”&lt;br /&gt; &lt;br /&gt; Soon? What is he talking about?</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Lets learn a new skill, one you will need very soon. Looting. You will find this in the same list as the Accuracy skill. You will stop training Accuracy, and start training Looting. This time, lets put a bit more XP: 20% towards the skill. Then explore for an hour.&lt;/p&gt;&lt;p&gt;Looting is whats used for getting all those items that were dropping, and will continue to do so until you are level 12 or your looting is 10% or more, which you can see if you click on the skill name to view the skill information.&lt;/p&gt;&lt;p&gt;After viewing what items you want to keep, I want you to disenchant them all. This will give you a new currency called Gold Dust, which is used in some Quests (not these) as well as a skill called Alchemy.&lt;/p&gt;&lt;p&gt;Right now focus on looting and disenchanting to get a total amount of 200 Gold Dust or more.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>Looting</t>
   </si>
   <si>
     <t>Kill em faster!</t>
   </si>
   <si>
-    <t>“Faster! Kill them faster child!”&lt;br /&gt; &lt;br /&gt; The Guide is watching you from the sidelines, watching you slowly kill the creatures before you. For a week now you have been slaughtering creatures and training. Learning how to hit better, how to loot properly.&lt;br /&gt; &lt;br /&gt; “Faster! You are way too slow!”</t>
+    <t>You stand before your enemy, blood drips from the weapon in your hand. Rage fills your eyes. Death has come for your enemy.&lt;br /&gt; &lt;br /&gt; “Slaughter them child!”&lt;br /&gt; &lt;br /&gt; You look behind you, blood drips down your face.&lt;br /&gt; &lt;br /&gt; An old haggard man stands behind you a short distance.&lt;br /&gt; &lt;br /&gt; “Don’t focus on me child. Kill the creature!”&lt;br /&gt; &lt;br /&gt; You turn and lunge at your enemy before they can see you. Your enchantments rage before you and your weapon slaughters the creature before you. Blood and gore soaks the ground around you.&lt;br /&gt; &lt;br /&gt; “Next time--” The old man begins as his voice gets close to you.&lt;br /&gt; &lt;br /&gt; “—Next time! Kill em faster!”&lt;br /&gt; &lt;br /&gt; You awaken from your dream, clutching your weapon.&lt;br /&gt; &lt;br /&gt; What happened? Was that real?</t>
   </si>
   <si>
     <t>&lt;p&gt;If you spent any time manually attacking, which will happen in some cases – such as with raid critters and some special locations in game, you will notice that the timer for attacking is very slow. You have to wait a whole 10 seconds!&lt;/p&gt;&lt;p&gt;So lets train Fighters Resilience skill to level 20 this will reduce the fight time out bar by a smidge, you can see the percentage if you click on the skill name i the skill section.&lt;/p&gt;&lt;p&gt;One of the pieces of information on this skill is that it has a Fighters Timeout Mod on it, which was raised to a max of 50 seconds, can cut down manual fighting by 5 seconds.&lt;/p&gt;&lt;p&gt;This skill will also raise your Armour Class and Damage over time.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Fighter's Resilience</t>
+  </si>
+  <si>
+    <t>Surface</t>
   </si>
   <si>
     <t>Blacksmiths Life</t>
@@ -606,7 +591,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AH12"/>
+  <dimension ref="A1:AH10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -615,9 +600,9 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="3.428" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="22.28" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="1863.831" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="2553.948" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="3700.668" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="24.708" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="24.708" bestFit="true" customWidth="true" style="0"/>
@@ -813,37 +798,67 @@
       <c r="D4" t="s">
         <v>42</v>
       </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4">
+        <v>25</v>
+      </c>
       <c r="W4">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="AG4">
-        <v>250</v>
+        <v>1000</v>
       </c>
       <c r="AH4">
-        <v>25</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:34">
       <c r="A5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5">
+        <v>50</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
         <v>43</v>
       </c>
-      <c r="C5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5">
-        <v>5</v>
+      <c r="I5">
+        <v>50</v>
+      </c>
+      <c r="J5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
       </c>
       <c r="AG5">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="AH5">
         <v>100</v>
@@ -851,28 +866,34 @@
     </row>
     <row r="6" spans="1:34">
       <c r="A6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E6">
+        <v>75</v>
+      </c>
+      <c r="F6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6">
+        <v>30</v>
+      </c>
+      <c r="H6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6">
         <v>20</v>
       </c>
-      <c r="F6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
-      <c r="AE6">
-        <v>250</v>
+      <c r="N6" t="s">
+        <v>55</v>
       </c>
       <c r="AG6">
         <v>1000</v>
@@ -883,107 +904,116 @@
     </row>
     <row r="7" spans="1:34">
       <c r="A7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E7">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="F7" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="G7">
+        <v>30</v>
+      </c>
+      <c r="H7" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7">
         <v>20</v>
       </c>
+      <c r="N7" t="s">
+        <v>61</v>
+      </c>
+      <c r="W7">
+        <v>200</v>
+      </c>
       <c r="AG7">
-        <v>500</v>
+        <v>10000</v>
       </c>
       <c r="AH7">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:34">
       <c r="A8">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E8">
-        <v>75</v>
+        <v>300</v>
       </c>
       <c r="F8" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="G8">
         <v>15</v>
       </c>
       <c r="H8" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="I8">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="N8" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="AG8">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="AH8">
-        <v>75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:34">
       <c r="A9">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="E9">
-        <v>150</v>
+        <v>400</v>
       </c>
       <c r="F9" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="G9">
-        <v>15</v>
+        <v>250</v>
       </c>
       <c r="H9" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="I9">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="N9" t="s">
-        <v>66</v>
-      </c>
-      <c r="W9">
-        <v>200</v>
+        <v>72</v>
       </c>
       <c r="AG9">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="AH9">
         <v>100</v>
@@ -991,125 +1021,49 @@
     </row>
     <row r="10" spans="1:34">
       <c r="A10">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E10">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="F10" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="G10">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="H10" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="I10">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="N10" t="s">
-        <v>72</v>
+        <v>78</v>
+      </c>
+      <c r="P10">
+        <v>1000</v>
+      </c>
+      <c r="AE10">
+        <v>5000</v>
+      </c>
+      <c r="AF10">
+        <v>500</v>
       </c>
       <c r="AG10">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="AH10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:34">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" t="s">
         <v>75</v>
-      </c>
-      <c r="E11">
-        <v>400</v>
-      </c>
-      <c r="F11" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11">
-        <v>100</v>
-      </c>
-      <c r="H11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I11">
-        <v>25</v>
-      </c>
-      <c r="N11" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG11">
-        <v>100000</v>
-      </c>
-      <c r="AH11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" t="s">
-        <v>79</v>
-      </c>
-      <c r="D12" t="s">
-        <v>80</v>
-      </c>
-      <c r="E12">
-        <v>500</v>
-      </c>
-      <c r="F12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G12">
-        <v>15</v>
-      </c>
-      <c r="H12" t="s">
-        <v>82</v>
-      </c>
-      <c r="I12">
-        <v>15</v>
-      </c>
-      <c r="N12" t="s">
-        <v>83</v>
-      </c>
-      <c r="P12">
-        <v>250</v>
-      </c>
-      <c r="AE12">
-        <v>10000</v>
-      </c>
-      <c r="AF12">
-        <v>500</v>
-      </c>
-      <c r="AG12">
-        <v>100000</v>
-      </c>
-      <c r="AH12">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding more to Guide Quests.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="99">
   <si>
     <t>id</t>
   </si>
@@ -44,6 +44,24 @@
     <t>required_secondary_skill_level</t>
   </si>
   <si>
+    <t>required_skill_type</t>
+  </si>
+  <si>
+    <t>required_skill_type_level</t>
+  </si>
+  <si>
+    <t>required_mercenary_type</t>
+  </si>
+  <si>
+    <t>required_secondary_mercenary_type</t>
+  </si>
+  <si>
+    <t>required_mercenary_level</t>
+  </si>
+  <si>
+    <t>required_secondary_mercenary_level</t>
+  </si>
+  <si>
     <t>required_faction_id</t>
   </si>
   <si>
@@ -59,6 +77,9 @@
     <t>required_quest_item_id</t>
   </si>
   <si>
+    <t>secondary_quest_item_id</t>
+  </si>
+  <si>
     <t>required_gold</t>
   </si>
   <si>
@@ -155,7 +176,7 @@
     <t>Kill em faster!</t>
   </si>
   <si>
-    <t>You stand before your enemy, blood drips from the weapon in your hand. Rage fills your eyes. Death has come for your enemy.&lt;br /&gt; &lt;br /&gt; “Slaughter them child!”&lt;br /&gt; &lt;br /&gt; You look behind you, blood drips down your face.&lt;br /&gt; &lt;br /&gt; An old haggard man stands behind you a short distance.&lt;br /&gt; &lt;br /&gt; “Don’t focus on me child. Kill the creature!”&lt;br /&gt; &lt;br /&gt; You turn and lunge at your enemy before they can see you. Your enchantments rage before you and your weapon slaughters the creature before you. Blood and gore soaks the ground around you.&lt;br /&gt; &lt;br /&gt; “Next time--” The old man begins as his voice gets close to you.&lt;br /&gt; &lt;br /&gt; “—Next time! Kill em faster!”&lt;br /&gt; &lt;br /&gt; You awaken from your dream, clutching your weapon.&lt;br /&gt; &lt;br /&gt; What happened? Was that real?</t>
+    <t>You stand before your enemy, blood drips from the weapon in your hand. Rage fills your eyes. Death has come for your enemy.&lt;br /&gt; &lt;br /&gt; “Slaughter them child!”&lt;br /&gt; &lt;br /&gt; You look behind you, blood drips down your face.&lt;br /&gt; &lt;br /&gt; An old haggard man stands behind you a short distance.&lt;br /&gt; &lt;br /&gt; “Don’t focus on me child. Kill the creature!”&lt;br /&gt; &lt;br /&gt; You turn and lunge at your enemy before they can see you. Your enchantments rage before you and your weapon slaughters the creature before you. Blood and gore soaks the ground around you.&lt;br /&gt; &lt;br /&gt; “Next time--” The old man begins as his voice gets closer to you.&lt;br /&gt; &lt;br /&gt; “—Next time! Kill em faster!”&lt;br /&gt; &lt;br /&gt; You awaken from your dream, clutching your weapon.&lt;br /&gt; &lt;br /&gt; What happened? Was that real?</t>
   </si>
   <si>
     <t>&lt;p&gt;If you spent any time manually attacking, which will happen in some cases – such as with raid critters and some special locations in game, you will notice that the timer for attacking is very slow. You have to wait a whole 10 seconds!&lt;/p&gt;&lt;p&gt;So lets train Fighters Resilience skill to level 20 this will reduce the fight time out bar by a smidge, you can see the percentage if you click on the skill name i the skill section.&lt;/p&gt;&lt;p&gt;One of the pieces of information on this skill is that it has a Fighters Timeout Mod on it, which was raised to a max of 50 seconds, can cut down manual fighting by 5 seconds.&lt;/p&gt;&lt;p&gt;This skill will also raise your Armour Class and Damage over time.&lt;/p&gt;</t>
@@ -170,36 +191,21 @@
     <t>Blacksmiths Life</t>
   </si>
   <si>
-    <t>You have been practicing your skills. Slowly learning how to manage your weapon better.&lt;br /&gt; &lt;br /&gt; “That will do child. Enough hunting for the day. Lets have a warm bath shall we?”&lt;br /&gt; &lt;br /&gt; You follow him back to the INN and retire to the upstairs room, dimly lit by a single candle under the glow of the setting sun.&lt;br /&gt; &lt;br /&gt; You bathe away the blood, the gore, the darkness. You are left with the stain on your soul, a dark sense of death. It haunts you and terrorizes you.&lt;br /&gt; &lt;br /&gt; A knock at your door as you get out of the bath and begin to dress.&lt;br /&gt; &lt;br /&gt; “Child, I want to discuss crafting with you for a moment.” Comes the familiar voice of The Guide.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Today we are going to learn about &lt;a href="/information/crafting" target="_blank"&gt;crafting&lt;/a&gt;. There are various types of crafting, but for now lets focus on simple weapons.&lt;/p&gt;&lt;p&gt;One thing to know about crafting is that it cannot be automated and it can eventually surpass the shop gear which stops at about 2 Billion Gold. Your character can craft items up to 36+ Billion Gold.&lt;/p&gt;&lt;p&gt;To get started:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Click the Craft/Enchant Button and select craft.&lt;/p&gt;&lt;p&gt;- Select Weapons&lt;/p&gt;&lt;p&gt;- Select Broken Dagger&lt;/p&gt;&lt;p&gt;- Click Craft.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- From the Action Section select Craft&lt;/p&gt;&lt;p&gt;- Click the Craft/Enchant Button and select craft.&lt;/p&gt;&lt;p&gt;- Select Weapons&lt;/p&gt;&lt;p&gt;- Select Broken Dagger&lt;/p&gt;&lt;p&gt;- Click Craft.&lt;/p&gt;&lt;p&gt;Your server message section will tell you if you succeed or not. Remember you cannot automate this, so turn on Exploration. You can also get a quest item by visiting a &lt;a href="/information/locations" target="_blank"&gt;location&lt;/a&gt;: Ruined Port City Of Kalize.&lt;/p&gt;&lt;p&gt;This item is known as a &lt;a href="/information/quest-items" target="_blank"&gt;quest item&lt;/a&gt; and will be used automatically with no input from you.&lt;/p&gt;&lt;p&gt;To access this location:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Click teleport under the map.&lt;/p&gt;&lt;p&gt;- Select the location: Ruined Port City Of Kalize from the locations drop down.&lt;/p&gt;&lt;p&gt;- Click Teleport assuming you can afford the cost.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile&lt;/strong&gt;:&lt;/p&gt;&lt;p&gt;- Select Map from the action drop down&lt;/p&gt;&lt;p&gt;- Click teleport under the map.&lt;/p&gt;&lt;p&gt;- Select the location: Ruined Port City Of Kalize from the locations drop down.&lt;/p&gt;&lt;p&gt;- Click Teleport assuming you can afford the cost.&lt;/p&gt;&lt;p&gt;You have now just moved across the map and gotten a quest item which will help you a little bit with crafting. You can see the bonus this item provides by going to your skills section and clicking on the crafting tab and clicking on the weapon crafting skill.&lt;/p&gt;&lt;p&gt;You can also find the item you found In your inventory section under quest items – which do not count towards your &lt;a href="/information/equipment-sets" target="_blank"&gt;75 Item Inventory limit&lt;/a&gt;.&lt;/p&gt;</t>
+    <t>Sitting in the INN, you stare into the large fire place with the wood burning and the crackling of the wood. It’s almost as if time stops for a moment and you can gather your thoughts.&lt;br /&gt; &lt;br /&gt; All you do is slaughter creatures, gather loot and slowly get better at hitting the enemies and even slightly faster.&lt;br /&gt; &lt;br /&gt; The flames of the fire seem to stand still, the smell of the fire has dissipated from the air. You look around and no one is moving, like they have been frozen in time.&lt;br /&gt; &lt;br /&gt; You turn back to the fire and see a young man, about twenty-five standing before the fire, his back to you. You call out to him, and he doesn’t turn around but he does speak.&lt;br /&gt; &lt;br /&gt; “Child. I have found something most mysterious. The gates have opened.”&lt;br /&gt; &lt;br /&gt; The gates? What gates?&lt;br /&gt; &lt;br /&gt; “Listen to me child.” The young man turns and faces you. You recognize the face, The Old Man from the dream, but he is much younger now.&lt;br /&gt; &lt;br /&gt; “I need you to speak with the local blacksmith, work with him for a while. Train a different set of skills. Important skills. I need you to craft your own gear.”&lt;br /&gt; &lt;br /&gt; You tell him that the gear you have found, the stuff you can buy from the local blacksmith is better then what you can craft.&lt;br /&gt; &lt;br /&gt; “True, however, you can craft even more powerful gear then that of which you can buy.”&lt;br /&gt; &lt;br /&gt; Before you can ask further questions the flames returning to their burning motion, the wood crackles, the INN is full of voices again and the smell of food fills the air.&lt;br /&gt; &lt;br /&gt; Where did he go?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Today we are going to learn about &lt;a href="/information/crafting" target="_blank"&gt;crafting&lt;/a&gt;. There are various types of crafting, but for now lets focus on simple weapons.&lt;/p&gt;&lt;p&gt;One thing to know about crafting is that it cannot be automated and it can eventually surpass the shop gear which stops at about 2 Billion Gold. Your character can craft items up to 36+ Billion Gold.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;: You can explore and craft at the same time, which is ideal. Just put on a show, explore till you are required level and craft until required level(s). You can close the Exploration section and do other actions while your character is exploring. You can re-open this section by clicking or selecting Exploration from the action section/drop down section for mobile. &lt;/p&gt;&lt;p&gt;To get started:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Click the Craft/Enchant Button and select craft.&lt;/p&gt;&lt;p&gt;- Select Weapons&lt;/p&gt;&lt;p&gt;- Select Broken Dagger&lt;/p&gt;&lt;p&gt;- Click Craft.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- From the Action Section select Craft&lt;/p&gt;&lt;p&gt;- Click the Craft/Enchant Button and select craft.&lt;/p&gt;&lt;p&gt;- Select Weapons&lt;/p&gt;&lt;p&gt;- Select Broken Dagger&lt;/p&gt;&lt;p&gt;- Click Craft.&lt;/p&gt;&lt;p&gt;Your server message section will tell you if you succeed or not. Remember you cannot automate this, so turn on Exploration. You can also get a quest item by visiting a &lt;a href="/information/locations" target="_blank"&gt;location&lt;/a&gt;: Ruined Port City Of Kalize.&lt;/p&gt;&lt;p&gt;This item is known as a &lt;a href="/information/quest-items" target="_blank"&gt;quest item&lt;/a&gt; and will be used automatically with no input from you.&lt;/p&gt;&lt;p&gt;To access this location:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Click teleport under the map.&lt;/p&gt;&lt;p&gt;- Select the location: Ruined Port City Of Kalize from the locations drop down.&lt;/p&gt;&lt;p&gt;- Click Teleport assuming you can afford the cost.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile&lt;/strong&gt;:&lt;/p&gt;&lt;p&gt;- Select Map from the action drop down&lt;/p&gt;&lt;p&gt;- Click teleport under the map.&lt;/p&gt;&lt;p&gt;- Select the location: Ruined Port City Of Kalize from the locations drop down.&lt;/p&gt;&lt;p&gt;- Click Teleport assuming you can afford the cost.&lt;/p&gt;&lt;p&gt;You have now just moved across the map and gotten a quest item which will help you a little bit with crafting. You can see the bonus this item provides by going to your skills section and clicking on the crafting tab and clicking on the weapon crafting skill.&lt;/p&gt;&lt;p&gt;Repeat this process to find the second quest item. You can - on desktop - click on locations to see what they drop if they drop anything at all.&lt;/p&gt;&lt;p&gt;You can also find the item you found In your inventory section under quest items – which do not count towards your &lt;a href="/information/equipment-sets" target="_blank"&gt;75 Item Inventory limit&lt;/a&gt;.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Weapon Crafting</t>
   </si>
   <si>
-    <t>Criticality</t>
+    <t>Armour Crafting</t>
   </si>
   <si>
     <t>Weaponsmith's Book</t>
   </si>
   <si>
-    <t>Sour Muscles</t>
-  </si>
-  <si>
-    <t>You have trained under the tutelage of the towns blacksmith who is also the elder of the town. He has taught you what you know, to get the basics out of the way.&lt;br /&gt; &lt;br /&gt; Today we learn about Armour. Today your muscles hurt</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Today lets craft some Armour. Eventually, for both weapons and Armour, you will out craft the store. As you progress further in the game and delve into new planes, you'll get higher level drops. Level in this case refers to the crafting level.&lt;/p&gt;&lt;p&gt;Purgatory contains drops of up to level 300, this is well beyond what the shops sells, but the character can craft up to level 400.&lt;/p&gt;&lt;p&gt;A final tip, shields are great for vampires as they increase the vampires durability, which in turns increases their damage. Some weapons like staves, bows and hammers are two handed weapons.&lt;/p&gt;&lt;p&gt;Lets craft some new Armour:&lt;/p&gt;&lt;p&gt;For both mobile and desktop, follow the same steps as before to craft weapons, but this time select Armour. Unlike weapons Armour is not separated by types.&lt;/p&gt;&lt;p&gt;Travel around the map visiting locations until you find the desired book which will help with Armour crafting.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Armour Crafting</t>
-  </si>
-  <si>
-    <t>Dodge</t>
-  </si>
-  <si>
     <t>Blacksmith's Book</t>
   </si>
   <si>
@@ -233,6 +239,9 @@
     <t>Quick Feet</t>
   </si>
   <si>
+    <t>Labyrinth</t>
+  </si>
+  <si>
     <t>Key of the Labyrinth</t>
   </si>
   <si>
@@ -252,6 +261,57 @@
   </si>
   <si>
     <t>Enchanter's Book</t>
+  </si>
+  <si>
+    <t>Traveling To Dungeons</t>
+  </si>
+  <si>
+    <t>You have come a long way since you first set out. Learning more of the world, learning more about your self and developing your skills.&lt;br /&gt; &lt;br /&gt; You sit under the tree outside of town and watch the merchants go by. A few stop and ask if you would like to purchase some of their wares, a few have some interesting knickknacks, and a few others have some food worth buying.&lt;br /&gt; &lt;br /&gt; As the day passes by and the sun begins to set you think of heading back to town to wash, relax and get a good nights sleep.&lt;br /&gt; &lt;br /&gt; “Hello there” comes an unfamiliar voice.&lt;br /&gt; &lt;br /&gt; You look and see a man in a Fedora, Green Tunic and Black leather pants. He seems older, but moves as if he is younger then his age.&lt;br /&gt; &lt;br /&gt; He comes closer and introduces him self, “I am The Poet and have been sent by The Guide to ask a favor of you, one from him.”&lt;br /&gt; &lt;br /&gt; You ask why he doesn’t come himself and ask this favor.&lt;br /&gt; &lt;br /&gt; “There is a darkness that is seeping from the depths into all the Planes. It is corrupting the Planes and causing the creatures to become vile and wicked. The Guide is busy investigating something deep with in Dungeons. Where he wants you to meet him.”&lt;br /&gt; &lt;br /&gt; You remember how you go to labyrinth, how hard can it be to get to Dungeons? You agree and The Poet tells you how to set off.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This is another &lt;a href="/information/quests" target="_blank"&gt;quest&lt;/a&gt; where we are going to a new &lt;a href="/information/planes" target="_blank"&gt;plane&lt;/a&gt;. How ever, to get there we have to complete a few quests.&lt;/p&gt;&lt;p&gt;Quests are how a lot of Tlessas features are unlocked for players. These quests, much like Guide Quests, will have a story – before and after completion – as well as explicit instructions on how to complete them, much like these.&lt;/p&gt;&lt;p&gt;Since you already know how to &lt;a href="/information/traverse" target="_blank"&gt;traverse&lt;/a&gt;, we just need to get you a quest item that allows you to traverse down to Dungeons.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Click the Quests tab&lt;/p&gt;&lt;p&gt;- Here you can see a list of quests for the plane you are on (if you are not on surface, select the Surface plane from the Planes drop down.)&lt;/p&gt;&lt;p&gt;- On the Surface quests you will see a quest (to the left) called Light The Way, complete the quests working down the tree until you complete it. Locked Quests are red, quests you can complete are Blue and Completed Quests are Green.&lt;/p&gt;&lt;p&gt;- Much like Guide Quests, you can see your completed quests in the sidebar (Hamburger menu to the top left) under: Quest Log → Completed Quests.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Tap the Quests tab&lt;/p&gt;&lt;p&gt;- Here you can see a list of quests for the plane you are on (if you are not on surface, select the Surface plane from the Planes drop down.)&lt;/p&gt;&lt;p&gt;- On the Surface quests you will see a quest (to the left – you can scroll left/right) called Light The Way, complete the quests working down the tree until you complete it. Locked Quests are red, quests you can complete are Blue and Completed Quests are Green.&lt;/p&gt;&lt;p&gt;- Much like Guide Quests, you can see your completed quests in the sidebar (Hamburger menu to the top left) under: Quest Log → Completed Quests.&lt;/p&gt;&lt;p&gt;Quests, much like Enchanting are vitally important to progress not only the over all story of the game, but also to get access to new features, new planes and so on of the game.&lt;/p&gt;&lt;p&gt;Each Plane will tell a story that all come together to tell a general story of The Creator (not the game Creator – an NPC) Quest chains going straight down tell their own story.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Ring Crafting</t>
+  </si>
+  <si>
+    <t>Dungeons</t>
+  </si>
+  <si>
+    <t>Light the way</t>
+  </si>
+  <si>
+    <t>Torch</t>
+  </si>
+  <si>
+    <t>Ring Crafter's Book</t>
+  </si>
+  <si>
+    <t>Death is something special</t>
+  </si>
+  <si>
+    <t>The Dungeons plane crawls with death. There is a darkness that seeps across the ground, infecting and infesting everything that it touches. You seem to be immune to it. You know there is shadow in the distance that is watching you. A shade like creature that only makes it’s self visible every now and then to your eyes.&lt;br /&gt; &lt;br /&gt; “Child!” Comes a familiar voice. The Guide, young, handsome and every changing comes up to you.&lt;br /&gt; &lt;br /&gt; “You have come down the Dungeons. A place of ruins, crypts, caves and other bits of darkness that one can explore for loot.”&lt;br /&gt; &lt;br /&gt; You ask him about the darkness crawling across the land and the shade like creature you can see off in the distance.&lt;br /&gt; &lt;br /&gt; “The darkness is caused by the gates of Shadow Planes, which has opened. The shade creature is the Shade Lord. He is seeking something, something that escaped the darkness beneath the pits of Hell. Alas to take on any of these creatures you need to get stronger!”</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Now we learn about a new feature: &lt;a href="/information/class-skills" target="_blank"&gt;Class Skills&lt;/a&gt; and Class Bonus.&lt;/p&gt;&lt;p&gt;Class Skills are different for each &lt;a href="/information/races-and-classes#3" target="_blank"&gt;class&lt;/a&gt; in the game. Every class has a skill which you can see on your skills table under Training Tab. It has an icon beside it and is in orange text.&lt;/p&gt;&lt;p&gt;This skill important to level because it allows you to increase your Class Bonus which can be seen on the character sheet to the left, under inventory count or on mobile under Class Details, at the bottom of the details section.&lt;/p&gt;&lt;p&gt;Every class has a special attack that fires automatically based on Three Things:&lt;/p&gt;&lt;p&gt;- Class Bonus % (the higher, the more chance for the special to fire)&lt;/p&gt;&lt;p&gt;- Weapons&lt;/p&gt;&lt;p&gt;- Attack type&lt;/p&gt;&lt;p&gt;For example, Heretics:&lt;/p&gt;&lt;p&gt;With a damage spell equipped you have a small chance to cast another spell. Enemies cannot avoid this.&lt;/p&gt;&lt;p&gt;This means while casting and with at least one damage spell, based on the % of your class bonus you can cast another spell, automatically. Each class has its own special which you can read about in the help docs for your specific class.&lt;/p&gt;&lt;p&gt;To do this:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop/Mobile&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- The instructions state to level a Effects Class skill type to the specified level. To do this, go to your character sheet section, in your skill section – train the skill with the orange text to the specified level.&lt;/p&gt;&lt;p&gt;That’s it. Now you might not see your class bonus fire off much at first, but over time, keep leveling this skill and you will start to see your special fire off automatically when manually fighting.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Mercenary for hire</t>
+  </si>
+  <si>
+    <t>You managed to survive long enough to drag your broken, bruised and bloody body back to the surface. You stop at an abandoned farm to mend your wounds and rest after such excursions.&lt;br /&gt; &lt;br /&gt; The farm looks familiar, but the names of the people that lived here has escaped your mind. You pay it no heed as you spend your time at this farm.&lt;br /&gt; &lt;br /&gt; A knock at the door, you open it and there stand The Poet.&lt;br /&gt; &lt;br /&gt; “Hello child.” He pushes past you and lets him self in.&lt;br /&gt; &lt;br /&gt; “You came back here.” he states.&lt;br /&gt; &lt;br /&gt; You look at him, confused.&lt;br /&gt; &lt;br /&gt; “Do you not know where you are child? You are home.”&lt;br /&gt; &lt;br /&gt; It comes back to you, your home. Abandoned. No parent, no one. Where did they go? You ask The poet in a rush, frantic and worried about your parents.&lt;br /&gt; &lt;br /&gt; “Child. Calm your self. They are here, some where. You’ll have to find them eventually.”&lt;br /&gt; &lt;br /&gt; Find them? What has he done with them? You start to get angry but The Port waves his hand and calmness washes over you.&lt;br /&gt; &lt;br /&gt; “For now I need you to head down to Labyrinth and complete some tasks to unlock Mercenaries. They can help you with getting shiny coins, dust and shards and later on some Copper.”&lt;br /&gt; &lt;br /&gt; My parents, where are they?&lt;br /&gt; &lt;br /&gt; “They are not where you think, they are not whom you think. I have lifted the spell that you lived with for so long. Do this, and I will tell you more.”&lt;br /&gt; &lt;br /&gt; He refuses to discuss the matter anymore.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Lets learn about &lt;a href="/information/currencies" target="_blank"&gt;currencies&lt;/a&gt;. You know about Gold Dust – that it can be used in quests and Alchemy.&lt;/p&gt;&lt;p&gt;You also know about Gold, the core currency. Shards and Copper Coins are another two types of currencies. Both can be earned from a feature called &lt;a href="/information/slots" target="_blank"&gt;Slots&lt;/a&gt;. However, there is a way to cheat the system and that’s to level &lt;a href="/information/mercenary" target="_blank"&gt;Mercenaries&lt;/a&gt;. You will need to complete a quest in Labyrinth. You can see this by going to the quests tab and selecting Labyrinth from the Planes drop down. Look for the quest: &lt;strong&gt;&lt;u&gt;Powers of The Children&lt;/u&gt;&lt;/strong&gt; to the right.&lt;/p&gt;&lt;p&gt;You can also see these quests if you traverse down to Labyrinth and then select the Quests tab.&lt;/p&gt;&lt;p&gt;Complete this quest to unlock a new feature called Mercenaries, who as they are leveled up will help you with getting more and more currencies from Slots and Farming creatures.&lt;/p&gt;&lt;p&gt;You can see these mercenaries who you must purchase by going to your character sheet and tapping/clicking the tab: Mercenaries. You can purchase them after completing the quest line above.&lt;/p&gt;&lt;p&gt;As you level these Mercenaries, you will eventually be able to reincarnate them – at their max level – and re-level them up to get even more % bonus towards currency drops. Some currencies such as Copper Coins only drop on a specific plane called Purgatory which you are not strong enough for yet, thus Slots will not drop them as you are missing an item to get into Purgatory.&lt;/p&gt;&lt;p&gt;For now, lets focus on Gold Dust and Shards, which you can do through Slots:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- In the actions section click Slots.&lt;/p&gt;&lt;p&gt;- Play slots or, if you cannot afford slots, kill monsters to get the currency requirements of this quest.&lt;/p&gt;&lt;p&gt;- Level a specific mercenary to the required level by killing creatures.&lt;/p&gt;&lt;p&gt;You can craft and play slots and explore at the same time. Which will be needed for this particular quest.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile&lt;/strong&gt;:&lt;/p&gt;&lt;p&gt;- In the actions section select Slots from the action drop down.&lt;/p&gt;&lt;p&gt;- Play slots or, if you cannot afford slots, kill monsters to get the currency requirements of this quest.&lt;/p&gt;&lt;p&gt;- Level a specific mercenary to the required level by killing creatures.&lt;/p&gt;&lt;p&gt;You can only do one action at a time on mobile, for example craft or play slots while exploration is running.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>child-of-gold-dust</t>
+  </si>
+  <si>
+    <t>child-of-shards</t>
+  </si>
+  <si>
+    <t>Powers of the children</t>
   </si>
 </sst>
 </file>
@@ -591,7 +651,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AH10"/>
+  <dimension ref="A1:AO12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -600,8 +660,8 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="3.428" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="22.28" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="1863.831" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="31.707" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="1869.686" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="3700.668" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="24.708" bestFit="true" customWidth="true" style="0"/>
@@ -609,33 +669,40 @@
     <col min="8" max="8" width="29.421" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="36.42" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="23.423" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="26.993" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="24.708" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="21.138" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="26.993" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="16.425" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="22.28" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="18.71" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="30.564" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="28.136" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="39.99" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="29.421" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="41.133" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="23.423" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="24.708" bestFit="true" customWidth="true" style="0"/>
     <col min="19" max="19" width="26.993" bestFit="true" customWidth="true" style="0"/>
     <col min="20" max="20" width="26.993" bestFit="true" customWidth="true" style="0"/>
-    <col min="21" max="21" width="26.993" bestFit="true" customWidth="true" style="0"/>
-    <col min="22" max="22" width="26.993" bestFit="true" customWidth="true" style="0"/>
-    <col min="23" max="23" width="17.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="24" max="24" width="15.282" bestFit="true" customWidth="true" style="0"/>
-    <col min="25" max="25" width="15.282" bestFit="true" customWidth="true" style="0"/>
-    <col min="26" max="26" width="15.282" bestFit="true" customWidth="true" style="0"/>
-    <col min="27" max="27" width="15.282" bestFit="true" customWidth="true" style="0"/>
-    <col min="28" max="28" width="15.282" bestFit="true" customWidth="true" style="0"/>
-    <col min="29" max="29" width="15.282" bestFit="true" customWidth="true" style="0"/>
+    <col min="21" max="21" width="28.136" bestFit="true" customWidth="true" style="0"/>
+    <col min="22" max="22" width="16.425" bestFit="true" customWidth="true" style="0"/>
+    <col min="23" max="23" width="22.28" bestFit="true" customWidth="true" style="0"/>
+    <col min="24" max="24" width="18.71" bestFit="true" customWidth="true" style="0"/>
+    <col min="25" max="25" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="26" max="26" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="27" max="27" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="28" max="28" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="29" max="29" width="26.993" bestFit="true" customWidth="true" style="0"/>
     <col min="30" max="30" width="17.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="31" max="31" width="19.995" bestFit="true" customWidth="true" style="0"/>
-    <col min="32" max="32" width="16.425" bestFit="true" customWidth="true" style="0"/>
-    <col min="33" max="33" width="13.997" bestFit="true" customWidth="true" style="0"/>
-    <col min="34" max="34" width="11.711" bestFit="true" customWidth="true" style="0"/>
+    <col min="31" max="31" width="15.282" bestFit="true" customWidth="true" style="0"/>
+    <col min="32" max="32" width="15.282" bestFit="true" customWidth="true" style="0"/>
+    <col min="33" max="33" width="15.282" bestFit="true" customWidth="true" style="0"/>
+    <col min="34" max="34" width="15.282" bestFit="true" customWidth="true" style="0"/>
+    <col min="35" max="35" width="15.282" bestFit="true" customWidth="true" style="0"/>
+    <col min="36" max="36" width="15.282" bestFit="true" customWidth="true" style="0"/>
+    <col min="37" max="37" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="38" max="38" width="19.995" bestFit="true" customWidth="true" style="0"/>
+    <col min="39" max="39" width="16.425" bestFit="true" customWidth="true" style="0"/>
+    <col min="40" max="40" width="13.997" bestFit="true" customWidth="true" style="0"/>
+    <col min="41" max="41" width="11.711" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:41">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -738,332 +805,516 @@
       <c r="AH1" t="s">
         <v>33</v>
       </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:41">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E2">
         <v>2</v>
       </c>
-      <c r="AG2">
+      <c r="AN2">
         <v>500</v>
       </c>
-      <c r="AH2">
+      <c r="AO2">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:34">
+    <row r="3" spans="1:41">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E3">
         <v>10</v>
       </c>
-      <c r="AG3">
+      <c r="AN3">
         <v>500</v>
       </c>
-      <c r="AH3">
+      <c r="AO3">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:34">
+    <row r="4" spans="1:41">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E4">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
         <v>50</v>
       </c>
-      <c r="F4" t="s">
-        <v>43</v>
-      </c>
       <c r="G4">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="I4">
-        <v>25</v>
-      </c>
-      <c r="W4">
+        <v>15</v>
+      </c>
+      <c r="AD4">
         <v>60</v>
       </c>
-      <c r="AG4">
+      <c r="AN4">
         <v>1000</v>
       </c>
-      <c r="AH4">
+      <c r="AO4">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:34">
+    <row r="5" spans="1:41">
       <c r="A5">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E5">
+        <v>60</v>
+      </c>
+      <c r="F5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
         <v>50</v>
       </c>
-      <c r="F5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5">
-        <v>30</v>
-      </c>
-      <c r="H5" t="s">
-        <v>43</v>
-      </c>
       <c r="I5">
-        <v>50</v>
-      </c>
-      <c r="J5" t="s">
-        <v>49</v>
-      </c>
-      <c r="K5">
+        <v>20</v>
+      </c>
+      <c r="P5" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q5">
         <v>2</v>
       </c>
-      <c r="AG5">
+      <c r="AN5">
         <v>10000</v>
       </c>
-      <c r="AH5">
+      <c r="AO5">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:34">
+    <row r="6" spans="1:41">
       <c r="A6">
         <v>7</v>
       </c>
       <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6">
+        <v>120</v>
+      </c>
+      <c r="F6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I6">
+        <v>15</v>
+      </c>
+      <c r="T6" t="s">
+        <v>62</v>
+      </c>
+      <c r="U6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD6">
+        <v>100</v>
+      </c>
+      <c r="AN6">
+        <v>1000</v>
+      </c>
+      <c r="AO6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7">
+        <v>160</v>
+      </c>
+      <c r="F7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7">
+        <v>15</v>
+      </c>
+      <c r="T7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN7">
+        <v>10000</v>
+      </c>
+      <c r="AO7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8">
+        <v>220</v>
+      </c>
+      <c r="F8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8">
+        <v>250</v>
+      </c>
+      <c r="H8" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8">
         <v>50</v>
       </c>
-      <c r="C6" t="s">
+      <c r="P8" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8" t="s">
+        <v>74</v>
+      </c>
+      <c r="T8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD8">
+        <v>250</v>
+      </c>
+      <c r="AN8">
+        <v>100000</v>
+      </c>
+      <c r="AO8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41">
+      <c r="A9">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9">
+        <v>250</v>
+      </c>
+      <c r="F9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>80</v>
+      </c>
+      <c r="I9">
+        <v>20</v>
+      </c>
+      <c r="P9" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q9">
+        <v>2</v>
+      </c>
+      <c r="T9" t="s">
+        <v>81</v>
+      </c>
+      <c r="W9">
+        <v>1000</v>
+      </c>
+      <c r="AD9">
+        <v>300</v>
+      </c>
+      <c r="AL9">
+        <v>5000</v>
+      </c>
+      <c r="AM9">
+        <v>500</v>
+      </c>
+      <c r="AN9">
+        <v>100000</v>
+      </c>
+      <c r="AO9">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41">
+      <c r="A10">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10">
+        <v>300</v>
+      </c>
+      <c r="F10" t="s">
         <v>51</v>
       </c>
-      <c r="D6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6">
-        <v>75</v>
-      </c>
-      <c r="F6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6">
+      <c r="G10">
+        <v>50</v>
+      </c>
+      <c r="H10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I10">
+        <v>20</v>
+      </c>
+      <c r="P10" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10" t="s">
+        <v>86</v>
+      </c>
+      <c r="S10" t="s">
+        <v>87</v>
+      </c>
+      <c r="T10" t="s">
+        <v>88</v>
+      </c>
+      <c r="U10" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD10">
+        <v>400</v>
+      </c>
+      <c r="AN10">
+        <v>250000</v>
+      </c>
+      <c r="AO10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41">
+      <c r="A11">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11">
+        <v>400</v>
+      </c>
+      <c r="F11" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11">
         <v>30</v>
       </c>
-      <c r="H6" t="s">
-        <v>54</v>
-      </c>
-      <c r="I6">
-        <v>20</v>
-      </c>
-      <c r="N6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AG6">
+      <c r="J11">
+        <v>13</v>
+      </c>
+      <c r="K11">
+        <v>25</v>
+      </c>
+      <c r="P11" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q11">
+        <v>2</v>
+      </c>
+      <c r="AD11">
+        <v>500</v>
+      </c>
+      <c r="AL11">
+        <v>10000</v>
+      </c>
+      <c r="AM11">
+        <v>200</v>
+      </c>
+      <c r="AN11">
+        <v>100000</v>
+      </c>
+      <c r="AO11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41">
+      <c r="A12">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12">
+        <v>500</v>
+      </c>
+      <c r="F12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12">
+        <v>30</v>
+      </c>
+      <c r="H12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I12">
+        <v>50</v>
+      </c>
+      <c r="J12">
+        <v>13</v>
+      </c>
+      <c r="K12">
+        <v>30</v>
+      </c>
+      <c r="L12" t="s">
+        <v>96</v>
+      </c>
+      <c r="M12" t="s">
+        <v>97</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q12">
+        <v>3</v>
+      </c>
+      <c r="S12" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD12">
+        <v>600</v>
+      </c>
+      <c r="AL12">
         <v>1000</v>
       </c>
-      <c r="AH6">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34">
-      <c r="A7">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7">
-        <v>150</v>
-      </c>
-      <c r="F7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G7">
-        <v>30</v>
-      </c>
-      <c r="H7" t="s">
-        <v>60</v>
-      </c>
-      <c r="I7">
-        <v>20</v>
-      </c>
-      <c r="N7" t="s">
-        <v>61</v>
-      </c>
-      <c r="W7">
-        <v>200</v>
-      </c>
-      <c r="AG7">
-        <v>10000</v>
-      </c>
-      <c r="AH7">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34">
-      <c r="A8">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8">
-        <v>300</v>
-      </c>
-      <c r="F8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G8">
-        <v>15</v>
-      </c>
-      <c r="H8" t="s">
-        <v>66</v>
-      </c>
-      <c r="I8">
-        <v>15</v>
-      </c>
-      <c r="N8" t="s">
-        <v>67</v>
-      </c>
-      <c r="AG8">
-        <v>10000</v>
-      </c>
-      <c r="AH8">
+      <c r="AM12">
+        <v>1000</v>
+      </c>
+      <c r="AN12">
+        <v>1000000</v>
+      </c>
+      <c r="AO12">
         <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:34">
-      <c r="A9">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9">
-        <v>400</v>
-      </c>
-      <c r="F9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9">
-        <v>250</v>
-      </c>
-      <c r="H9" t="s">
-        <v>71</v>
-      </c>
-      <c r="I9">
-        <v>50</v>
-      </c>
-      <c r="N9" t="s">
-        <v>72</v>
-      </c>
-      <c r="AG9">
-        <v>100000</v>
-      </c>
-      <c r="AH9">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:34">
-      <c r="A10">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10">
-        <v>500</v>
-      </c>
-      <c r="F10" t="s">
-        <v>76</v>
-      </c>
-      <c r="G10">
-        <v>100</v>
-      </c>
-      <c r="H10" t="s">
-        <v>77</v>
-      </c>
-      <c r="I10">
-        <v>100</v>
-      </c>
-      <c r="N10" t="s">
-        <v>78</v>
-      </c>
-      <c r="P10">
-        <v>1000</v>
-      </c>
-      <c r="AE10">
-        <v>5000</v>
-      </c>
-      <c r="AF10">
-        <v>500</v>
-      </c>
-      <c r="AG10">
-        <v>100000</v>
-      </c>
-      <c r="AH10">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes, fixes and Guide Quests Updates
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -215,7 +215,7 @@
     <t>You are exhausted, tired, confused.&lt;br /&gt; &lt;br /&gt; “Child” comes a familiar voice as you sit up on your bed.&lt;br /&gt; &lt;br /&gt; The INN is creaky, noisy and musty. The single candle flame that burns in the room barley illuminates the room.&lt;br /&gt; &lt;br /&gt; As he walks from the shadows The Guide stands before you, not young and handsome, but old and wise, dressed in robes. His skin is brown from the sun.&lt;br /&gt; &lt;br /&gt; “Downstairs sits a woman, an attractive woman.” he states.&lt;br /&gt; &lt;br /&gt; “She will teach you about magic and its properties, specifically in the art of enchanting and disenchanting.”&lt;br /&gt; &lt;br /&gt; You ask him why he can’t teach you and he deflects the question.&lt;br /&gt; &lt;br /&gt; “Go now child. She isn’t to be kept waiting.”&lt;br /&gt; &lt;br /&gt; You head down the stairs to meet the Enchantress.&lt;br /&gt; &lt;br /&gt; She waits for you at a table, a woman in black, instantly recognizable by her long black hair and pale complexion. She radiates beauty.&lt;br /&gt; &lt;br /&gt; You walk over and sit down at the table. “Hello child.” She starts, he voice is soft and entrancing. “have you heard of the queen?” You shake your head no. “She has gifted you with some of those green shiny unique’s in your inventory.”&lt;br /&gt; &lt;br /&gt; You remember those. Killing monsters gets you faction with the plane and its people and as a reward they give you a shiny green item that makes you feel much much stronger.&lt;br /&gt; &lt;br /&gt; “She can give you more powerful ones, but you have to face the most fearsome of creatures to earn her attention. In the mean time lets discuss the art of magic. Lets start small with spells …”</t>
   </si>
   <si>
-    <t>&lt;p&gt;Lets start learning about spells.&lt;/p&gt;&lt;p&gt;You have just spent a ton f time crafting weapons and Armour, we will repeat this to craft spells. Spells are useful for caster classes, as well as any one who wants to use them.&lt;/p&gt;&lt;p&gt;Damage spells and Staves (Two Handed weapons) can raise the characters intelligence, both of which can be bought from the shop or crafted.&lt;/p&gt;&lt;p&gt;Healing spells are great for characters who want to do Cast and attack or Attack and Cast, like Prophets.&lt;/p&gt;&lt;p&gt;To get the quest item required, you will need to kill: Umbering Spirit Lord on Surface. This creature is further down the list and may require you to upgrade your gear through the shop before being able to take him down. This creature has a 15% chance to drop the item, so exploration might be a good choice here.&lt;/p&gt;</t>
+    <t>&lt;p&gt;&lt;strong&gt;Note: &lt;/strong&gt;This quest can take up to 2 hours to complete. Do not feel like you have to rush through it.&lt;/p&gt;&lt;p&gt;Lets start learning about spells.&lt;/p&gt;&lt;p&gt;You have just spent a ton f time crafting weapons and Armour, we will repeat this to craft spells. Spells are useful for caster classes, as well as any one who wants to use them.&lt;/p&gt;&lt;p&gt;Damage spells and Staves (Two Handed weapons) can raise the characters intelligence, both of which can be bought from the shop or crafted.&lt;/p&gt;&lt;p&gt;Healing spells are great for characters who want to do Cast and attack or Attack and Cast, like Prophets.&lt;/p&gt;&lt;p&gt;To get the quest item required, you will need to kill: Umbering Spirit Lord on Surface. This creature is further down the list and may require you to upgrade your gear through the shop before being able to take him down. This creature has a 15% chance to drop the item, so exploration might be a good choice here.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Spell Crafting</t>
@@ -230,10 +230,10 @@
     <t>Go To Labyrinth</t>
   </si>
   <si>
-    <t>You have been under the Enchantress’s tutelage for weeks now. She has been teaching the you about the art of magic and how it can be used to weave together powerful spells that can be enchanted onto items.&lt;br /&gt; &lt;br /&gt; You are waiting for her in the forest outside of the town you have been practically living in. She doesn’t appear and some time goes by.&lt;br /&gt; &lt;br /&gt; The old man appears, The Guide. Almost from thin air, one moment nothing, next he’s in front of you.&lt;br /&gt; &lt;br /&gt; “She isn’t coming.” He states.&lt;br /&gt; &lt;br /&gt; “Something foul is afoot and I need you to do some investigating for me. Find the Key of labyrinth child. Do it quickly.”</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Time to stop training and fight a monster. This will drop weather you use exploration or not. Fine the Key of labyrinth by fighting the Labyrinth Fiend.&lt;/p&gt;&lt;p&gt;To make it easier lets also raise our looting skill.&lt;/p&gt;&lt;p&gt;Once you have the key, lets:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;Click traverse under the map.&lt;/p&gt;&lt;p&gt;- Select Labyrinth from the plane drop down.&lt;/p&gt;&lt;p&gt;- Click traverse.&lt;/p&gt;&lt;p&gt;- Welcome to labyrinth. Monsters down here have the same strength as surface but are new.&lt;/p&gt;&lt;p&gt;- Kill enough until your faction level with surface is level 1.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- From the action drop down select Map Movement&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;Click traverse under the map.&lt;/p&gt;&lt;p&gt;- Select Labyrinth from the plane drop down.&lt;/p&gt;&lt;p&gt;- Click traverse.&lt;/p&gt;&lt;p&gt;- Welcome to labyrinth. Monsters down here have the same strength as surface but are new.&lt;/p&gt;&lt;p&gt;- Kill enough until your faction level with surface is level 1.&lt;/p&gt;</t>
+    <t>You have been under the Enchantress’s tutelage for weeks now. She has been teaching the you about the art of magic and how it can be used to weave together powerful spells.&lt;br /&gt; &lt;br /&gt; She has told you that if you wait for her in the forest outside of town she will teach you the next step: Enchanting. She explained it is the use of powerful magic that can imbue items, such as weapons, armour, rings and even other spells with potent abilities that can turn the tide of a battle, similar to the items you find on the enemies corpses.&lt;br /&gt; &lt;br /&gt; You are waiting for her in the forest outside of the town you have been practically living in. She doesn’t appear and some time goes by.&lt;br /&gt; &lt;br /&gt; The old man appears, The Guide. Almost from thin air, one moment nothing, next he’s in front of you.&lt;br /&gt; &lt;br /&gt; “She isn’t coming.” He states.&lt;br /&gt; &lt;br /&gt; “Something foul is afoot and I need you to do some investigating for me. Find the Key of labyrinth child. Do it quickly.”</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Time to stop training and fight a monster. This will drop weather you use exploration or not. Find the Key of Labyrinth by fighting the Labyrinth Fiend on Surface&lt;/p&gt;&lt;p&gt;To make it easier lets also raise our looting skill.&lt;/p&gt;&lt;p&gt;Once you have the key, lets:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;Click traverse under the map.&lt;/p&gt;&lt;p&gt;- Select Labyrinth from the plane drop down.&lt;/p&gt;&lt;p&gt;- Click traverse.&lt;/p&gt;&lt;p&gt;- Welcome to labyrinth. Monsters down here have the same strength as surface but are new.&lt;/p&gt;&lt;p&gt;- Kill enough until your faction level with surface is level 1.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- From the action drop down select Map Movement&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;Click traverse under the map.&lt;/p&gt;&lt;p&gt;- Select Labyrinth from the plane drop down.&lt;/p&gt;&lt;p&gt;- Click traverse.&lt;/p&gt;&lt;p&gt;- Welcome to labyrinth. Monsters down here have the same strength as surface but are new.&lt;/p&gt;&lt;p&gt;- Kill enough until your faction level with surface is level 1.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Quick Feet</t>
@@ -1057,13 +1057,13 @@
         <v>51</v>
       </c>
       <c r="G8">
-        <v>250</v>
+        <v>25</v>
       </c>
       <c r="H8" t="s">
         <v>73</v>
       </c>
       <c r="I8">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="P8" t="s">
         <v>74</v>
@@ -1107,13 +1107,13 @@
         <v>79</v>
       </c>
       <c r="G9">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H9" t="s">
         <v>80</v>
       </c>
       <c r="I9">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="P9" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
Remove the scheduled event import/export fucntionality.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -194,7 +194,7 @@
     <t>Sitting in the INN, you stare into the large fire place with the wood burning and the crackling of the wood. It’s almost as if time stops for a moment and you can gather your thoughts.&lt;br /&gt; &lt;br /&gt; All you do is slaughter creatures, gather loot and slowly get better at hitting the enemies and even slightly faster.&lt;br /&gt; &lt;br /&gt; The flames of the fire seem to stand still, the smell of the fire has dissipated from the air. You look around and no one is moving, like they have been frozen in time.&lt;br /&gt; &lt;br /&gt; You turn back to the fire and see a young man, about twenty-five standing before the fire, his back to you. You call out to him, and he doesn’t turn around but he does speak.&lt;br /&gt; &lt;br /&gt; “Child. I have found something most mysterious. The gates have opened.”&lt;br /&gt; &lt;br /&gt; The gates? What gates?&lt;br /&gt; &lt;br /&gt; “Listen to me child.” The young man turns and faces you. You recognize the face, The Old Man from the dream, but he is much younger now.&lt;br /&gt; &lt;br /&gt; “I need you to speak with the local blacksmith, work with him for a while. Train a different set of skills. Important skills. I need you to craft your own gear.”&lt;br /&gt; &lt;br /&gt; You tell him that the gear you have found, the stuff you can buy from the local blacksmith is better then what you can craft.&lt;br /&gt; &lt;br /&gt; “True, however, you can craft even more powerful gear then that of which you can buy.”&lt;br /&gt; &lt;br /&gt; Before you can ask further questions the flames returning to their burning motion, the wood crackles, the INN is full of voices again and the smell of food fills the air.&lt;br /&gt; &lt;br /&gt; Where did he go?</t>
   </si>
   <si>
-    <t>&lt;p&gt;Today we are going to learn about &lt;a href="/information/crafting" target="_blank"&gt;crafting&lt;/a&gt;. There are various types of crafting, but we want to focus on weapons and Armour for now.&lt;/p&gt;&lt;p&gt;At first you will fail a lot, even with the suggested &lt;a href="/information/quest-items" target="_blank"&gt;quest items&lt;/a&gt; this quest will take roughly &lt;strong&gt;4 hours to complete&lt;/strong&gt;. Do not worry about trying to rush through it. Instead focus on your gear that you get from exploration and if any of it increases your Weapon Crafting or Armour Crafting – equip it.&lt;/p&gt;&lt;p&gt;Eventually you will craft beyond what the &lt;a href="/information/shop" target="_blank"&gt;shop&lt;/a&gt; sells. The Shop stops at two billion gold, where as players can craft up to 36+ Billion gold items that are much better then shop gear.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Crafting cannot be automated.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- First we want to find the items we need, quest items are automatically used. You can open the Teleport Map Action to then select the location: Ruined Port City Of Kalize (X/Y): 32/368 and click teleport if you can afford the cost. This will get you the: Weapon Smith’s Book which adds 25% to Skill Bonus and XP.&lt;/p&gt;&lt;p&gt;- Repeat the above step to then go to: Dragon cliffs (X/Y): 192/176 to get the Blacksmith’s book for the same bonuses towards Armour Crafting.&lt;/p&gt;&lt;p&gt;Both of these can be upgraded later on when we have access to Labyrinth. There are some One Off &lt;a href="/information/quests" target="_blank"&gt;quests&lt;/a&gt; that will upgrade these.&lt;/p&gt;&lt;p&gt;- Now lets craft, first set up exploration for an hour or two – or what ever you feel like doing, Exploration will run while logged out. Remember to set it up with a monster you can kill in one hit.&lt;/p&gt;&lt;p&gt;- Close exploration and then from the drop down Craft/Enchant select craft, select weapons, select Broken Dagger and then click craft.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Select Map from the actions drop down.&lt;/p&gt;&lt;p&gt;- Click Teleport from the actions under the map.&lt;/p&gt;&lt;p&gt;- Select the location: Ruined Port City Of Kalize (X/Y): 32/368 and click teleport if you can afford the cost. This will get you the: Weapon Smith’s Book which adds 25% to Skill Bonus and XP.&lt;/p&gt;&lt;p&gt;- Repeat the above step to then go to: Dragon cliffs (X/Y): 192/176 to get the Blacksmith’s book for the same bonuses towards Armour Crafting.&lt;/p&gt;&lt;p&gt;Both of these can be upgraded later on when we have access to Labyrinth. There are some One off &lt;a href="/information/quests" target="_blank"&gt;quests&lt;/a&gt; that will upgrade these.&lt;/p&gt;&lt;p&gt;- Now lets craft, first set up exploration for an hour or two – or what ever you feel like doing, Exploration will run while logged out. Remember to set it up with a monster you can kill in one hit.&lt;/p&gt;&lt;p&gt;- Close exploration, select Craft from the drop down and then select Craft from the Craft/Enchant&lt;/p&gt;&lt;p&gt;- Select Weapons, Broken Dagger – Click craft.&lt;/p&gt;&lt;p&gt;- When ready, click Change Type, select Armour, select an Armour to craft and click craft.&lt;/p&gt;&lt;p&gt;Over time new items will be added to the list. That’s all there is to it. When you are ready, click Change Type, select Armour, pick an item to craft and repeat.&lt;/p&gt;</t>
+    <t>&lt;p&gt;Today we are going to learn about &lt;a href="/information/crafting" target="_blank"&gt;crafting&lt;/a&gt;. There are various types of crafting, but we want to focus on weapons and Armour for now.&lt;/p&gt;&lt;p&gt;At first you will fail a lot, even with the suggested &lt;a href="/information/quest-items" target="_blank"&gt;quest items&lt;/a&gt; this quest will take roughly &lt;strong&gt;4 hours to complete&lt;/strong&gt;. Do not worry about trying to rush through it. Instead focus on your gear that you get from exploration and if any of it increases your Weapon Crafting or Armour Crafting – equip it.&lt;/p&gt;&lt;p&gt;Eventually you will craft beyond what the &lt;a href="/information/shop" target="_blank"&gt;shop&lt;/a&gt; sells. The Shop stops at two billion gold, where as players can craft up to 36+ Billion gold items that are much better then shop gear.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Crafting cannot be automated. Keep an eye on Server Messages section to see successes, failures and if you have new items to craft.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- First we want to find the items we need, quest items are automatically used. You can open the Teleport Map Action to then select the location: Ruined Port City Of Kalize (X/Y): 32/368 and click teleport if you can afford the cost. This will get you the: Weapon Smith’s Book which adds 25% to Skill Bonus and XP.&lt;/p&gt;&lt;p&gt;- Repeat the above step to then go to: Dragon cliffs (X/Y): 192/176 to get the Blacksmith’s book for the same bonuses towards Armour Crafting.&lt;/p&gt;&lt;p&gt;Both of these can be upgraded later on when we have access to Labyrinth. There are some One Off &lt;a href="/information/quests" target="_blank"&gt;quests&lt;/a&gt; that will upgrade these.&lt;/p&gt;&lt;p&gt;- Now lets craft, first set up exploration for an hour or two – or what ever you feel like doing, Exploration will run while logged out. Remember to set it up with a monster you can kill in one hit.&lt;/p&gt;&lt;p&gt;- Close exploration and then from the drop down Craft/Enchant select craft, select weapons, select Broken Dagger and then click craft.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Select Map from the actions drop down.&lt;/p&gt;&lt;p&gt;- Click Teleport from the actions under the map.&lt;/p&gt;&lt;p&gt;- Select the location: Ruined Port City Of Kalize (X/Y): 32/368 and click teleport if you can afford the cost. This will get you the: Weapon Smith’s Book which adds 25% to Skill Bonus and XP.&lt;/p&gt;&lt;p&gt;- Repeat the above step to then go to: Dragon cliffs (X/Y): 192/176 to get the Blacksmith’s book for the same bonuses towards Armour Crafting.&lt;/p&gt;&lt;p&gt;Both of these can be upgraded later on when we have access to Labyrinth. There are some One off &lt;a href="/information/quests" target="_blank"&gt;quests&lt;/a&gt; that will upgrade these.&lt;/p&gt;&lt;p&gt;- Now lets craft, first set up exploration for an hour or two – or what ever you feel like doing, Exploration will run while logged out. Remember to set it up with a monster you can kill in one hit.&lt;/p&gt;&lt;p&gt;- Close exploration, select Craft from the drop down and then select Craft from the Craft/Enchant&lt;/p&gt;&lt;p&gt;- Select Weapons, Broken Dagger – Click craft.&lt;/p&gt;&lt;p&gt;- When ready, click Change Type, select Armour, select an Armour to craft and click craft.&lt;/p&gt;&lt;p&gt;Over time new items will be added to the list. That’s all there is to it. When you are ready, click Change Type, select Armour, pick an item to craft and repeat.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Weapon Crafting</t>
@@ -293,7 +293,7 @@
     <t>The Dungeons plane crawls with death. There is a darkness that seeps across the ground, infecting and infesting everything that it touches. You seem to be immune to it. You know there is shadow in the distance that is watching you. A shade like creature that only makes it’s self visible every now and then to your eyes.&lt;br /&gt; &lt;br /&gt; “Child!” Comes a familiar voice. The Guide, young, handsome and every changing comes up to you.&lt;br /&gt; &lt;br /&gt; “You have come down the Dungeons. A place of ruins, crypts, caves and other bits of darkness that one can explore for loot.”&lt;br /&gt; &lt;br /&gt; You ask him about the darkness crawling across the land and the shade like creature you can see off in the distance.&lt;br /&gt; &lt;br /&gt; “The darkness is caused by the gates of Shadow Planes, which has opened. The shade creature is the Shade Lord. He is seeking something, something that escaped the darkness beneath the pits of Hell. Alas to take on any of these creatures you need to get stronger!”</t>
   </si>
   <si>
-    <t>&lt;p&gt;Now we learn about a new feature: &lt;a href="/information/class-skills" target="_blank"&gt;Class Skills&lt;/a&gt; and Class Bonus.&lt;/p&gt;&lt;p&gt;Class Skills are different for each &lt;a href="/information/races-and-classes#3" target="_blank"&gt;class&lt;/a&gt; in the game. Every class has a skill which you can see on your skills table under Training Tab. It has an icon beside it and is in orange text.&lt;/p&gt;&lt;p&gt;This skill important to level because it allows you to increase your Class Bonus which can be seen on the character sheet to the left, under inventory count or on mobile under Class Details, at the bottom of the details section.&lt;/p&gt;&lt;p&gt;Every class has a special attack that fires automatically based on Three Things:&lt;/p&gt;&lt;p&gt;- Class Bonus % (the higher, the more chance for the special to fire)&lt;/p&gt;&lt;p&gt;- Weapons&lt;/p&gt;&lt;p&gt;- Attack type&lt;/p&gt;&lt;p&gt;For example, Heretics:&lt;/p&gt;&lt;p&gt;With a damage spell equipped you have a small chance to cast another spell. Enemies cannot avoid this.&lt;/p&gt;&lt;p&gt;This means while casting and with at least one damage spell, based on the % of your class bonus you can cast another spell, automatically. Each class has its own special which you can read about in the help docs for your specific class.&lt;/p&gt;&lt;p&gt;To do this:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop/Mobile&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- The instructions state to level a Effects Class skill type to the specified level. To do this, go to your character sheet section, in your skill section – train the skill with the orange text to the specified level.&lt;/p&gt;&lt;p&gt;That’s it. Now you might not see your class bonus fire off much at first, but over time, keep leveling this skill and you will start to see your special fire off automatically when manually fighting.&lt;/p&gt;</t>
+    <t>&lt;p&gt;Now we learn about a new feature: &lt;a href="/information/class-skills" target="_blank"&gt;Class Skills&lt;/a&gt; and Class Bonus.&lt;/p&gt;&lt;p&gt;Class Skills are different for each &lt;a href="/information/races-and-classes#3" target="_blank"&gt;class&lt;/a&gt; in the game. Every class has a skill which you can see on your skills table under Training Tab. It has an icon beside it and is in orange text.&lt;/p&gt;&lt;p&gt;This skill important to level because it allows you to increase your Class Bonus which can be seen on the character sheet to the left, under inventory count or on mobile under Class Details, at the bottom of the details section.&lt;/p&gt;&lt;p&gt;Every class has a special attack that fires automatically based on Three Things:&lt;/p&gt;&lt;p&gt;- Class Bonus % (the higher, the more chance for the special to fire)&lt;/p&gt;&lt;p&gt;- Weapons&lt;/p&gt;&lt;p&gt;- Attack type&lt;/p&gt;&lt;p&gt;For example, Heretics:&lt;/p&gt;&lt;p&gt;With a damage spell equipped you have a small chance to cast another spell. Enemies cannot avoid this.&lt;/p&gt;&lt;p&gt;This means while casting and with at least one damage spell, based on the % of your class bonus you can cast another spell, automatically. Each class has its own special which you can read about in the help docs for your specific class.&lt;/p&gt;&lt;p&gt;To do this:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop/Mobile&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- The instructions state to level a Effects Class to the specified level. To do this, go to your character sheet section, in your skill section – train the skill with the orange text to the specified level.&lt;/p&gt;&lt;p&gt;- To Get the Gold Dust you can disenchant items that drop you no longer need, or craft some items, enchant them and disenchant them. Now is the time to explore the &lt;a href="/information/enchanting" target="_blank"&gt;Enchanting&lt;/a&gt; list in the docs to see what types of enchantments you can apply to your equipment so you can start creating a gear set geared towards your needs.&lt;/p&gt;&lt;p&gt;That’s it. Now you might not see your class bonus fire off much at first, but over time, keep leveling this skill and you will start to see your special fire off automatically when manually fighting.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Mercenary for hire</t>
@@ -662,7 +662,7 @@
     <col min="1" max="1" width="3.428" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="31.707" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="1869.686" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="3751.37" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="3871.769" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="24.708" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="24.708" bestFit="true" customWidth="true" style="0"/>
@@ -1209,12 +1209,6 @@
       <c r="E11">
         <v>400</v>
       </c>
-      <c r="F11" t="s">
-        <v>80</v>
-      </c>
-      <c r="G11">
-        <v>30</v>
-      </c>
       <c r="J11">
         <v>13</v>
       </c>
@@ -1222,13 +1216,13 @@
         <v>25</v>
       </c>
       <c r="P11" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="Q11">
         <v>2</v>
       </c>
       <c r="AD11">
-        <v>500</v>
+        <v>750</v>
       </c>
       <c r="AL11">
         <v>10000</v>
@@ -1260,22 +1254,22 @@
         <v>500</v>
       </c>
       <c r="F12" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="G12">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H12" t="s">
         <v>79</v>
       </c>
       <c r="I12">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="J12">
         <v>13</v>
       </c>
       <c r="K12">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="L12" t="s">
         <v>96</v>
@@ -1299,7 +1293,7 @@
         <v>98</v>
       </c>
       <c r="AD12">
-        <v>600</v>
+        <v>900</v>
       </c>
       <c r="AL12">
         <v>1000</v>

</xml_diff>

<commit_message>
Updated dependencies, minor fixes and changes
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="102">
   <si>
     <t>id</t>
   </si>
@@ -312,6 +312,15 @@
   </si>
   <si>
     <t>Powers of the children</t>
+  </si>
+  <si>
+    <t>A place to call home</t>
+  </si>
+  <si>
+    <t>You are exhausted, emotionally, mentally and physically. You fight, you kill, you train, you craft and enchant. You sit under a tree with a small fire burning as the moon rises high in the night sky. You notice how bright, how clear, how large the moon is in the night sky.&lt;br /&gt; &lt;br /&gt; As you sit and mull over the last few months, your mind wonders back to what The Poet stated, about the abandoned house, your house, your family house.&lt;br /&gt; &lt;br /&gt; Are they dead? Are they alive? Where are they? Winy did they leave the farm? So many questions, yet no answers.&lt;br /&gt; &lt;br /&gt; A slight breeze kicks up and the flames flicker and dance in the night.&lt;br /&gt; &lt;br /&gt; A voice comes from the shadows of the night, beyond the flames light and reach.&lt;br /&gt; &lt;br /&gt; “Child, I am back.” Comes the voice of The Guide.&lt;br /&gt; &lt;br /&gt; You look up from your fire and see The Guide, he is young again, keeps changing between young and old. Alas he looks bruised, broken and is limping.&lt;br /&gt; &lt;br /&gt; You ask him what happened but he shrugs it off. “it is not important. What is though is that you put your feet up. Gather some soldiers, build some walls, create a home for your self.”&lt;br /&gt; &lt;br /&gt; You tell him what The Poet said about your parents.&lt;br /&gt; &lt;br /&gt; “Silly child, there is so much for you to learn. Alas for now, Lets get you to settle down and call some place home.”&lt;br /&gt; &lt;br /&gt; You insist he explains more, but he refuse’s and starts to get angry at your demands.&lt;br /&gt; &lt;br /&gt; “Now you listen here, there is a darkness descending on this world, one escaping the pits of hell, some of it I am sure you have learned about, others you don’t know yet, but soon will. All will be answered in time. But for now, you have a job to do.”&lt;br /&gt; &lt;br /&gt; You think for a moment of refusing until you get the answers, but a swath of land you can call your own does sound enticing.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Lets take a break from questing, crafting, enchanting and fighting and lets focus on kingdoms and what they can provide for you.&lt;/p&gt;&lt;p&gt;You can settle a &lt;a href="/information/kingdoms" target="_blank"&gt;kingdom&lt;/a&gt; for free once, assuming you have no kingdoms.&lt;/p&gt;&lt;p&gt;Each kingdom after the first one will cost 10,000 Gold x the amount of kingdoms you already own.&lt;/p&gt;&lt;p&gt;Your first kingdom, again assuming you have no kingdoms, will have a 7 day protection on it, meaning no one can attack it.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; the quest requires a kingdom level, this means you need you need to level the buildings, by resources or gold, over time to reach the required objective. You can level one building or multiple as the kingdom level is a sum of all the building levels in one kingdom.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;Find a place on either Surface, Labyrinth or Dungeons where you can access and what to settle a kingdom.&lt;/p&gt;&lt;p&gt;- Click Settle Kingdom under the map and give your kingdom a name.&lt;/p&gt;&lt;p&gt;- Now you can click on the Kingdoms tab and see your kingdom&lt;/p&gt;&lt;p&gt;- From there you can click on the kingdom name and see further details.&lt;/p&gt;&lt;p&gt;- On the map you will see an icon on the map that represents your kingdom and you can also click on that to get basic details as well as teleport to it, assuming you have the gold to teleport the distance.&lt;/p&gt;&lt;p&gt;- When you click on the kingdom via the kingdoms tab, you can see information like buildings and units as well as kingdom resources that will replenish over time, every hour.&lt;/p&gt;&lt;p&gt;- Lets recruit some units and upgrade our buildings which can be done with either resources, as stated, or gold. Both of which will require (real world) time to recruit the units and build the buildings.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;Find a place on either Surface, Labyrinth or Dungeons where you can access and what to settle a kingdom.&lt;/p&gt;&lt;p&gt;- In the Actions drop down, select Map Movement&lt;/p&gt;&lt;p&gt;- Tap Settle Kingdom under the map and give your kingdom a name.&lt;/p&gt;&lt;p&gt;- Now you can tap on the Kingdoms tab and see your kingdom&lt;/p&gt;&lt;p&gt;- From there you can tap on the kingdom name and see further details.&lt;/p&gt;&lt;p&gt;- On the map you will see your kingdom icon, but due to how the map works on mobile, you wont be able to tap on it for basic details unlike on desktop. How ever if you tap Teleport you can choose from a list of your kingdoms on that Plane to teleport to.&lt;/p&gt;&lt;p&gt;- When you tap on the kingdom via the kingdoms tab, you can see information like buildings and units as well as kingdom resources that will replenish over time, every hour.&lt;/p&gt;&lt;p&gt;- Lets recruit some units and upgrade our buildings which can be done with either resources, as stated, or gold. Both of which will require (real world) time to recruit the units and build the buildings.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -651,7 +660,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AO12"/>
+  <dimension ref="A1:AO13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -661,7 +670,7 @@
   <cols>
     <col min="1" max="1" width="3.428" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="31.707" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="1869.686" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="2197.749" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="3871.769" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="24.708" bestFit="true" customWidth="true" style="0"/>
@@ -1308,6 +1317,35 @@
         <v>100</v>
       </c>
     </row>
+    <row r="13" spans="1:41">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y13">
+        <v>1</v>
+      </c>
+      <c r="Z13">
+        <v>5</v>
+      </c>
+      <c r="AA13">
+        <v>100</v>
+      </c>
+      <c r="AN13">
+        <v>1000</v>
+      </c>
+      <c r="AO13">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Lots of fixes and minor changes.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="110">
   <si>
     <t>id</t>
   </si>
@@ -62,6 +62,9 @@
     <t>required_secondary_mercenary_level</t>
   </si>
   <si>
+    <t>required_class_specials_equipped</t>
+  </si>
+  <si>
     <t>required_faction_id</t>
   </si>
   <si>
@@ -293,7 +296,7 @@
     <t>The Dungeons plane crawls with death. There is a darkness that seeps across the ground, infecting and infesting everything that it touches. You seem to be immune to it. You know there is shadow in the distance that is watching you. A shade like creature that only makes it’s self visible every now and then to your eyes.&lt;br /&gt; &lt;br /&gt; “Child!” Comes a familiar voice. The Guide, young, handsome and every changing comes up to you.&lt;br /&gt; &lt;br /&gt; “You have come down the Dungeons. A place of ruins, crypts, caves and other bits of darkness that one can explore for loot.”&lt;br /&gt; &lt;br /&gt; You ask him about the darkness crawling across the land and the shade like creature you can see off in the distance.&lt;br /&gt; &lt;br /&gt; “The darkness is caused by the gates of Shadow Planes, which has opened. The shade creature is the Shade Lord. He is seeking something, something that escaped the darkness beneath the pits of Hell. Alas to take on any of these creatures you need to get stronger!”</t>
   </si>
   <si>
-    <t>&lt;p&gt;Now we learn about a new feature: &lt;a href="/information/class-skills" target="_blank"&gt;Class Skills&lt;/a&gt; and Class Bonus.&lt;/p&gt;&lt;p&gt;Class Skills are different for each &lt;a href="/information/races-and-classes#3" target="_blank"&gt;class&lt;/a&gt; in the game. Every class has a skill which you can see on your skills table under Training Tab. It has an icon beside it and is in orange text.&lt;/p&gt;&lt;p&gt;This skill important to level because it allows you to increase your Class Bonus which can be seen on the character sheet to the left, under inventory count or on mobile under Class Details, at the bottom of the details section.&lt;/p&gt;&lt;p&gt;Every class has a special attack that fires automatically based on Three Things:&lt;/p&gt;&lt;p&gt;- Class Bonus % (the higher, the more chance for the special to fire)&lt;/p&gt;&lt;p&gt;- Weapons&lt;/p&gt;&lt;p&gt;- Attack type&lt;/p&gt;&lt;p&gt;For example, Heretics:&lt;/p&gt;&lt;p&gt;With a damage spell equipped you have a small chance to cast another spell. Enemies cannot avoid this.&lt;/p&gt;&lt;p&gt;This means while casting and with at least one damage spell, based on the % of your class bonus you can cast another spell, automatically. Each class has its own special which you can read about in the help docs for your specific class.&lt;/p&gt;&lt;p&gt;To do this:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop/Mobile&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- The instructions state to level a Effects Class to the specified level. To do this, go to your character sheet section, in your skill section – train the skill with the orange text to the specified level.&lt;/p&gt;&lt;p&gt;- To Get the Gold Dust you can disenchant items that drop you no longer need, or craft some items, enchant them and disenchant them. Now is the time to explore the &lt;a href="/information/enchanting" target="_blank"&gt;Enchanting&lt;/a&gt; list in the docs to see what types of enchantments you can apply to your equipment so you can start creating a gear set geared towards your needs.&lt;/p&gt;&lt;p&gt;That’s it. Now you might not see your class bonus fire off much at first, but over time, keep leveling this skill and you will start to see your special fire off automatically when manually fighting.&lt;/p&gt;</t>
+    <t>&lt;p&gt;Now we learn about a new feature: &lt;a href="/information/class-skills" target="_blank"&gt;Class Skills&lt;/a&gt; and Class Bonus.&lt;/p&gt;&lt;p&gt;Class Skills are different for each &lt;a href="/information/races-and-classes#3" target="_blank"&gt;class&lt;/a&gt; in the game. Every class has a skill which you can see on your skills table under Training Tab. It has an icon beside it and is in orange text.&lt;/p&gt;&lt;p&gt;This skill important to level because it allows you to increase your Class Bonus which can be seen on the character sheet to the left, under inventory count or on mobile under Class Details, at the bottom of the details section.&lt;/p&gt;&lt;p&gt;Every class has a special attack that fires automatically based on Three Things:&lt;/p&gt;&lt;p&gt;- Class Bonus % (the higher, the more chance for the special to fire)&lt;/p&gt;&lt;p&gt;- Weapons&lt;/p&gt;&lt;p&gt;- Attack type&lt;/p&gt;&lt;p&gt;\For example, Heretics:&lt;/p&gt;&lt;p&gt;With a damage spell equipped you have a small chance to cast another spell. Enemies cannot avoid this.&lt;/p&gt;&lt;p&gt;This means while casting and with at least one damage spell, based on the % of your class bonus you can cast another spell, automatically. Each class has its own special which you can read about in the help docs for your specific class.&lt;/p&gt;&lt;p&gt;To do this:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop/Mobile&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- The instructions state to level a Effects Class to the specified level. To do this, go to your character sheet section, in your skill section – train the skill with the orange text to the specified level.&lt;/p&gt;&lt;p&gt;- To Get the Gold Dust you can disenchant items that drop you no longer need, or craft some items, enchant them and disenchant them. Now is the time to explore the &lt;a href="/information/enchanting" target="_blank"&gt;Enchanting&lt;/a&gt; list in the docs to see what types of enchantments you can apply to your equipment so you can start creating a gear set geared towards your needs.&lt;/p&gt;&lt;p&gt;That’s it. Now you might not see your class bonus fire off much at first, but over time, keep leveling this skill and you will start to see your special fire off automatically when manually fighting.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Mercenary for hire</t>
@@ -321,6 +324,27 @@
   </si>
   <si>
     <t>&lt;p&gt;Lets take a break from questing, crafting, enchanting and fighting and lets focus on kingdoms and what they can provide for you.&lt;/p&gt;&lt;p&gt;You can settle a &lt;a href="/information/kingdoms" target="_blank"&gt;kingdom&lt;/a&gt; for free once, assuming you have no kingdoms.&lt;/p&gt;&lt;p&gt;Each kingdom after the first one will cost 10,000 Gold x the amount of kingdoms you already own.&lt;/p&gt;&lt;p&gt;Your first kingdom, again assuming you have no kingdoms, will have a 7 day protection on it, meaning no one can attack it.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; the quest requires a kingdom level, this means you need you need to level the buildings, by resources or gold, over time to reach the required objective. You can level one building or multiple as the kingdom level is a sum of all the building levels in one kingdom.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;Find a place on either Surface, Labyrinth or Dungeons where you can access and what to settle a kingdom.&lt;/p&gt;&lt;p&gt;- Click Settle Kingdom under the map and give your kingdom a name.&lt;/p&gt;&lt;p&gt;- Now you can click on the Kingdoms tab and see your kingdom&lt;/p&gt;&lt;p&gt;- From there you can click on the kingdom name and see further details.&lt;/p&gt;&lt;p&gt;- On the map you will see an icon on the map that represents your kingdom and you can also click on that to get basic details as well as teleport to it, assuming you have the gold to teleport the distance.&lt;/p&gt;&lt;p&gt;- When you click on the kingdom via the kingdoms tab, you can see information like buildings and units as well as kingdom resources that will replenish over time, every hour.&lt;/p&gt;&lt;p&gt;- Lets recruit some units and upgrade our buildings which can be done with either resources, as stated, or gold. Both of which will require (real world) time to recruit the units and build the buildings.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;Find a place on either Surface, Labyrinth or Dungeons where you can access and what to settle a kingdom.&lt;/p&gt;&lt;p&gt;- In the Actions drop down, select Map Movement&lt;/p&gt;&lt;p&gt;- Tap Settle Kingdom under the map and give your kingdom a name.&lt;/p&gt;&lt;p&gt;- Now you can tap on the Kingdoms tab and see your kingdom&lt;/p&gt;&lt;p&gt;- From there you can tap on the kingdom name and see further details.&lt;/p&gt;&lt;p&gt;- On the map you will see your kingdom icon, but due to how the map works on mobile, you wont be able to tap on it for basic details unlike on desktop. How ever if you tap Teleport you can choose from a list of your kingdoms on that Plane to teleport to.&lt;/p&gt;&lt;p&gt;- When you tap on the kingdom via the kingdoms tab, you can see information like buildings and units as well as kingdom resources that will replenish over time, every hour.&lt;/p&gt;&lt;p&gt;- Lets recruit some units and upgrade our buildings which can be done with either resources, as stated, or gold. Both of which will require (real world) time to recruit the units and build the buildings.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Growing the population</t>
+  </si>
+  <si>
+    <t>You managed to build a small town, people come to live here as there is tons of work, farming, construction and even a developing industrial and military aspect. You look for new ways to grow the kingdom and to make the people happy as well as building more homes and forms of work for the people.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Now that we have settled a kingdom, lets look into a new set of skills, which instead of killing creatures, takes real world time to complete. These are called Kingdom Passives which, as the name states, help your kingdom(s) grow over time. Each passive is only unlocked after the parent passive reaches a specific level.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Click on the character sheet tab&lt;/p&gt;&lt;p&gt;- In the skill section, click on Kingdom Passives&lt;/p&gt;&lt;p&gt;- Click on Kingdom Management and click train&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Tap on the character sheet tab&lt;/p&gt;&lt;p&gt;- Select Skill Management from the drop down&lt;/p&gt;&lt;p&gt;- Tap on the Kingdom Passive tab&lt;/p&gt;&lt;p&gt;- Tap on the Kingdom Management in the tree and click train.&lt;/p&gt;&lt;p&gt;These skills, as stated, take real world time to train and will continue to train even if you are logged out.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Kingdom Management</t>
+  </si>
+  <si>
+    <t>Mastering your own specialties</t>
+  </si>
+  <si>
+    <t>You sit before the fire of your home, sifting through papers and contemplating what the next project will be.&lt;br /&gt; &lt;br /&gt; One of your counselors knocks on the door and you rise to greet them, beckoning them to come in.&lt;br /&gt; &lt;br /&gt; “Your majesty, there is a letter from a man known as The Guide, for you to meet him at the Dragon Cliffs.”&lt;br /&gt; &lt;br /&gt; You take the letter and read it twice.&lt;br /&gt; &lt;br /&gt; After two days of preparations, you set out, alone, towards your destination. It takes two weeks to arrive at your destination. You make you way to the cliffs, shaped like a dragons head and see the guide sitting on ground looking ahead. He is young again.&lt;br /&gt; &lt;br /&gt; You approach him and announce your self. He stands and turns to greet you.&lt;br /&gt; &lt;br /&gt; “Child. I have news of your parents. They are dead.”&lt;br /&gt; &lt;br /&gt; The world stops for what seems like an eternity. Dead, how could they be dead. You set out not so long ago, you worked so hard to get to where you are. But the news of your parents being dead ---&lt;br /&gt; &lt;br /&gt; “Child! Pay attention.” A screeching voice interrupts your racing thoughts.&lt;br /&gt; &lt;br /&gt; “They were never your parents. It was all an illusion set up by The Poet.”&lt;br /&gt; &lt;br /&gt; Your entire life is a lie…</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Today we are going to learn about &lt;a href="/information/class-ranks" target="_blank"&gt;Class Ranks&lt;/a&gt;. Class Ranks allows a character to do a couple of things:&lt;/p&gt;&lt;p&gt;- Switch classes at any time&lt;/p&gt;&lt;p&gt;- Gain more attack towards specific weapons&lt;/p&gt;&lt;p&gt;- Equip Special abilities that can do damage and increase aspects of your character&lt;/p&gt;&lt;p&gt;- Unlock new classes&lt;/p&gt;&lt;p&gt;A character may only have a total of three specialties equipped an of the three only one may of a specialty that deals damage.&lt;/p&gt;&lt;p&gt;Finally, specialties unlock as you level the class rank. So lets get into how to manage your class ranks on your character:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Click on Character Sheet tab&lt;/p&gt;&lt;p&gt;- Click the orange button called Class Ranks&lt;/p&gt;&lt;p&gt;- Here you see a list of the games classes including some, marked by star, that require you to level other class ranks to specific levels.&lt;/p&gt;&lt;p&gt;- Click on your class in the list.&lt;/p&gt;&lt;p&gt;- Here you can you see details about your class, including the class masteries. These masteries are leveled over time by your having the weapon/spell type equipped at the time of fighting monsters.&lt;/p&gt;&lt;p&gt; - Above the class name is a red circle with a minus through it, clicking this will close this section, where as clicking X or the cancel button will close the class masteries modal.&lt;/p&gt;&lt;p&gt;- Next click “Manage Specialties”, this will open a secondary modal.&lt;/p&gt;&lt;p&gt;- These are specialties that unlock at the class rank level, you should – by now – have two specialties you can equip.&lt;/p&gt;&lt;p&gt;- You can investigate the specialties to see what they do. There are two types: Ones that increase specific attributes of your character over time, which are leveled by just fighting monsters and ones that do damage – which fire automatically when fighting monsters.&lt;/p&gt;&lt;p&gt;- Equip the required amount of specialties.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Tap on Character Sheet tab&lt;/p&gt;&lt;p&gt;- Open the top section and tap on the orange button called Class Ranks&lt;/p&gt;&lt;p&gt;- Here you see a list of the games classes including some, marked by star, that require you to level other class ranks to specific levels.&lt;/p&gt;&lt;p&gt;- Click on your class in the list.&lt;/p&gt;&lt;p&gt;- Here you can you see details about your class, including the class masteries. These masteries are leveled over time by your having the weapon/spell type equipped at the time of fighting monsters.&lt;/p&gt;&lt;p&gt; - Above the class name is a red circle with a minus through it, clicking this will close this section, where as clicking X or the cancel button will close the class masteries modal.&lt;/p&gt;&lt;p&gt;- Next click “Manage Specialties”, this will open a secondary modal.&lt;/p&gt;&lt;p&gt;- These are specialties that unlock at the class rank level, you should – by now – have two specialties you can equip.&lt;/p&gt;&lt;p&gt;- You can investigate the specialties to see what they do. There are two types: Ones that increase specific attributes of your character over time, which are leveled by just fighting monsters and ones that do damage – which fire automatically when fighting monsters.&lt;/p&gt;&lt;p&gt;- Equip the required amount of specialties.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;: Under Equipped Specialties, you can unequipped them to then equip other specialties from other classes. As you switch classes and play around, you can mix and match specialties equipped for maximum damage and stats.&lt;/p&gt;&lt;p&gt;All of these specialties, masteries and class ranks will level over time by you killing monsters. No XP will be sacrificed like when you train skills, instead this is a separate XP curve for each of the sections.&lt;/p&gt;&lt;p&gt;You server message section will also, as you may have seen, show you when you get levels in class specialties, ranks or masteries.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -660,7 +684,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AO13"/>
+  <dimension ref="A1:AP15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -669,9 +693,9 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="3.428" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="31.707" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="36.42" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="2197.749" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="3871.769" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="4361.221" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="24.708" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="24.708" bestFit="true" customWidth="true" style="0"/>
@@ -683,35 +707,36 @@
     <col min="13" max="13" width="39.99" bestFit="true" customWidth="true" style="0"/>
     <col min="14" max="14" width="29.421" bestFit="true" customWidth="true" style="0"/>
     <col min="15" max="15" width="41.133" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="23.423" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="26.993" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="24.708" bestFit="true" customWidth="true" style="0"/>
-    <col min="19" max="19" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="38.848" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="23.423" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="19" max="19" width="24.708" bestFit="true" customWidth="true" style="0"/>
     <col min="20" max="20" width="26.993" bestFit="true" customWidth="true" style="0"/>
-    <col min="21" max="21" width="31.707" bestFit="true" customWidth="true" style="0"/>
-    <col min="22" max="22" width="16.425" bestFit="true" customWidth="true" style="0"/>
-    <col min="23" max="23" width="22.28" bestFit="true" customWidth="true" style="0"/>
-    <col min="24" max="24" width="18.71" bestFit="true" customWidth="true" style="0"/>
-    <col min="25" max="25" width="21.138" bestFit="true" customWidth="true" style="0"/>
-    <col min="26" max="26" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="21" max="21" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="22" max="22" width="31.707" bestFit="true" customWidth="true" style="0"/>
+    <col min="23" max="23" width="16.425" bestFit="true" customWidth="true" style="0"/>
+    <col min="24" max="24" width="22.28" bestFit="true" customWidth="true" style="0"/>
+    <col min="25" max="25" width="18.71" bestFit="true" customWidth="true" style="0"/>
+    <col min="26" max="26" width="21.138" bestFit="true" customWidth="true" style="0"/>
     <col min="27" max="27" width="26.993" bestFit="true" customWidth="true" style="0"/>
     <col min="28" max="28" width="26.993" bestFit="true" customWidth="true" style="0"/>
     <col min="29" max="29" width="26.993" bestFit="true" customWidth="true" style="0"/>
-    <col min="30" max="30" width="17.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="31" max="31" width="15.282" bestFit="true" customWidth="true" style="0"/>
+    <col min="30" max="30" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="31" max="31" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="32" max="32" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="33" max="33" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="34" max="34" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="35" max="35" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="36" max="36" width="15.282" bestFit="true" customWidth="true" style="0"/>
-    <col min="37" max="37" width="17.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="38" max="38" width="19.995" bestFit="true" customWidth="true" style="0"/>
-    <col min="39" max="39" width="16.425" bestFit="true" customWidth="true" style="0"/>
-    <col min="40" max="40" width="13.997" bestFit="true" customWidth="true" style="0"/>
-    <col min="41" max="41" width="11.711" bestFit="true" customWidth="true" style="0"/>
+    <col min="37" max="37" width="15.282" bestFit="true" customWidth="true" style="0"/>
+    <col min="38" max="38" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="39" max="39" width="19.995" bestFit="true" customWidth="true" style="0"/>
+    <col min="40" max="40" width="16.425" bestFit="true" customWidth="true" style="0"/>
+    <col min="41" max="41" width="13.997" bestFit="true" customWidth="true" style="0"/>
+    <col min="42" max="42" width="11.711" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41">
+    <row r="1" spans="1:42">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -835,353 +860,353 @@
       <c r="AO1" t="s">
         <v>40</v>
       </c>
+      <c r="AP1" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="2" spans="1:41">
+    <row r="2" spans="1:42">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E2">
         <v>2</v>
       </c>
-      <c r="AN2">
+      <c r="AO2">
         <v>500</v>
       </c>
-      <c r="AO2">
+      <c r="AP2">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:41">
+    <row r="3" spans="1:42">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E3">
         <v>10</v>
       </c>
-      <c r="AN3">
+      <c r="AO3">
         <v>500</v>
       </c>
-      <c r="AO3">
+      <c r="AP3">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:41">
+    <row r="4" spans="1:42">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E4">
         <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G4">
         <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I4">
         <v>15</v>
       </c>
-      <c r="AD4">
+      <c r="AE4">
         <v>60</v>
       </c>
-      <c r="AN4">
+      <c r="AO4">
         <v>1000</v>
       </c>
-      <c r="AO4">
+      <c r="AP4">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:41">
+    <row r="5" spans="1:42">
       <c r="A5">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E5">
         <v>60</v>
       </c>
       <c r="F5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G5">
         <v>15</v>
       </c>
       <c r="H5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I5">
         <v>20</v>
       </c>
-      <c r="P5" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q5">
+      <c r="Q5" t="s">
+        <v>57</v>
+      </c>
+      <c r="R5">
         <v>2</v>
       </c>
-      <c r="AN5">
+      <c r="AO5">
         <v>10000</v>
       </c>
-      <c r="AO5">
+      <c r="AP5">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:41">
+    <row r="6" spans="1:42">
       <c r="A6">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E6">
         <v>120</v>
       </c>
       <c r="F6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G6">
         <v>15</v>
       </c>
       <c r="H6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I6">
         <v>15</v>
       </c>
-      <c r="T6" t="s">
-        <v>62</v>
-      </c>
       <c r="U6" t="s">
         <v>63</v>
       </c>
-      <c r="AD6">
+      <c r="V6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE6">
         <v>100</v>
       </c>
-      <c r="AN6">
+      <c r="AO6">
         <v>1000</v>
       </c>
-      <c r="AO6">
+      <c r="AP6">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:41">
+    <row r="7" spans="1:42">
       <c r="A7">
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E7">
         <v>160</v>
       </c>
       <c r="F7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G7">
         <v>15</v>
       </c>
       <c r="H7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I7">
         <v>15</v>
       </c>
-      <c r="T7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AH7">
+      <c r="U7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI7">
         <v>150</v>
       </c>
-      <c r="AN7">
+      <c r="AO7">
         <v>10000</v>
       </c>
-      <c r="AO7">
+      <c r="AP7">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:41">
+    <row r="8" spans="1:42">
       <c r="A8">
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E8">
         <v>220</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G8">
         <v>25</v>
       </c>
       <c r="H8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I8">
         <v>10</v>
       </c>
-      <c r="P8" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q8">
+      <c r="Q8" t="s">
+        <v>75</v>
+      </c>
+      <c r="R8">
         <v>1</v>
       </c>
-      <c r="R8" t="s">
-        <v>74</v>
-      </c>
-      <c r="T8" t="s">
+      <c r="S8" t="s">
         <v>75</v>
       </c>
-      <c r="AD8">
+      <c r="U8" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE8">
         <v>250</v>
       </c>
-      <c r="AN8">
+      <c r="AO8">
         <v>100000</v>
       </c>
-      <c r="AO8">
+      <c r="AP8">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:41">
+    <row r="9" spans="1:42">
       <c r="A9">
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E9">
         <v>250</v>
       </c>
       <c r="F9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G9">
         <v>15</v>
       </c>
       <c r="H9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I9">
         <v>12</v>
       </c>
-      <c r="T9" t="s">
-        <v>81</v>
-      </c>
-      <c r="W9">
+      <c r="U9" t="s">
+        <v>82</v>
+      </c>
+      <c r="X9">
         <v>1000</v>
       </c>
-      <c r="AD9">
+      <c r="AE9">
         <v>300</v>
       </c>
-      <c r="AL9">
+      <c r="AM9">
         <v>5000</v>
       </c>
-      <c r="AM9">
+      <c r="AN9">
         <v>500</v>
       </c>
-      <c r="AN9">
+      <c r="AO9">
         <v>100000</v>
       </c>
-      <c r="AO9">
+      <c r="AP9">
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:41">
+    <row r="10" spans="1:42">
       <c r="A10">
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E10">
         <v>300</v>
       </c>
       <c r="F10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G10">
         <v>50</v>
       </c>
       <c r="H10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I10">
         <v>10</v>
       </c>
-      <c r="P10" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q10">
+      <c r="Q10" t="s">
+        <v>87</v>
+      </c>
+      <c r="R10">
         <v>1</v>
-      </c>
-      <c r="R10" t="s">
-        <v>86</v>
       </c>
       <c r="S10" t="s">
         <v>87</v>
@@ -1192,31 +1217,34 @@
       <c r="U10" t="s">
         <v>89</v>
       </c>
-      <c r="AD10">
+      <c r="V10" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE10">
         <v>400</v>
       </c>
-      <c r="AN10">
+      <c r="AO10">
         <v>250000</v>
       </c>
-      <c r="AO10">
+      <c r="AP10">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:41">
+    <row r="11" spans="1:42">
       <c r="A11">
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E11">
-        <v>400</v>
+        <v>350</v>
       </c>
       <c r="J11">
         <v>13</v>
@@ -1224,67 +1252,43 @@
       <c r="K11">
         <v>25</v>
       </c>
-      <c r="P11" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q11">
-        <v>2</v>
-      </c>
-      <c r="AD11">
-        <v>750</v>
-      </c>
-      <c r="AL11">
+      <c r="AE11">
+        <v>600</v>
+      </c>
+      <c r="AM11">
         <v>10000</v>
       </c>
-      <c r="AM11">
+      <c r="AN11">
         <v>200</v>
       </c>
-      <c r="AN11">
+      <c r="AO11">
         <v>100000</v>
       </c>
-      <c r="AO11">
+      <c r="AP11">
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:41">
+    <row r="12" spans="1:42">
       <c r="A12">
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C12" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D12" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E12">
-        <v>500</v>
-      </c>
-      <c r="F12" t="s">
-        <v>60</v>
-      </c>
-      <c r="G12">
-        <v>25</v>
-      </c>
-      <c r="H12" t="s">
-        <v>79</v>
-      </c>
-      <c r="I12">
-        <v>25</v>
-      </c>
-      <c r="J12">
-        <v>13</v>
-      </c>
-      <c r="K12">
-        <v>50</v>
+        <v>400</v>
       </c>
       <c r="L12" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M12" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="N12">
         <v>1</v>
@@ -1292,57 +1296,106 @@
       <c r="O12">
         <v>1</v>
       </c>
-      <c r="P12" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q12">
-        <v>3</v>
-      </c>
-      <c r="S12" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD12">
-        <v>900</v>
-      </c>
-      <c r="AL12">
-        <v>1000</v>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="T12" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE12">
+        <v>800</v>
       </c>
       <c r="AM12">
         <v>1000</v>
       </c>
       <c r="AN12">
+        <v>1000</v>
+      </c>
+      <c r="AO12">
         <v>1000000</v>
       </c>
-      <c r="AO12">
+      <c r="AP12">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:41">
+    <row r="13" spans="1:42">
       <c r="A13">
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z13">
+        <v>1</v>
+      </c>
+      <c r="AA13">
+        <v>5</v>
+      </c>
+      <c r="AB13">
         <v>100</v>
       </c>
-      <c r="D13" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y13">
-        <v>1</v>
-      </c>
-      <c r="Z13">
-        <v>5</v>
-      </c>
-      <c r="AA13">
-        <v>100</v>
-      </c>
-      <c r="AN13">
+      <c r="AO13">
         <v>1000</v>
       </c>
-      <c r="AO13">
+      <c r="AP13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:42">
+      <c r="A14">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA14">
+        <v>10</v>
+      </c>
+      <c r="AB14">
+        <v>200</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>106</v>
+      </c>
+      <c r="AO14">
+        <v>2500</v>
+      </c>
+      <c r="AP14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42">
+      <c r="A15">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" t="s">
+        <v>109</v>
+      </c>
+      <c r="P15">
+        <v>2</v>
+      </c>
+      <c r="AO15">
+        <v>20000</v>
+      </c>
+      <c r="AP15">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Guide quests are goo enough for now, as I itterate on them
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="110">
   <si>
     <t>id</t>
   </si>
@@ -167,7 +167,7 @@
     <t>You explore, you slaughter, you bathe in the enemies blood before you. You collect the shiny loot. You were gifted a green unique item from the towns people as a way of thanking you for your hard work.&lt;br /&gt; &lt;br /&gt; They told you that there are many other places one could explore, but that you could continue around here gain more favor with the people of the Surface plane.&lt;br /&gt; &lt;br /&gt; You wait for days and then weeks at the INN, where the hell is The Guide?&lt;br /&gt; &lt;br /&gt; “A letter for you” the barmaid states as she drops off your ale. You open it and read the following:&lt;br /&gt; &lt;br /&gt; Child. Listen, I am The Guide, alas I am investigating a situation. There is a magical spell upon your very being that allows the creatures you slaughter to gift you with the bounty of loot you have now, but that won’t last forever.&lt;br /&gt; &lt;br /&gt; You have to learn how to properly loot. You also have to have to learn how to wield your weapon, even casters can get into sticky situations where they need a weapon, and if you can’t hit anything – death will greet you faster then I.&lt;br /&gt; &lt;br /&gt; I also want you to investigate your gear, visit a shop. You gear is what makes you child. Know that.&lt;br /&gt; &lt;br /&gt; -- The Guide&lt;br /&gt; &lt;br /&gt; That’s it? Just barks orders through paper at you? You look around and contemplate doing what he want’s knowing full well you could just bugger off on your own adventure.&lt;br /&gt; &lt;br /&gt; By morning you have made up your mind on what to do.</t>
   </si>
   <si>
-    <t>&lt;p&gt;We are going to learn about two things today: &lt;a href="/information/character-stats" target="_blank"&gt;Stats&lt;/a&gt; and &lt;a href="/information/skill-information" target="_blank"&gt;Skills&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;Characters under level 12, get a boost to their looting skill making drops a lot more fun. How ever as you will soon reach level 12 you will see the drop rate disappear. This is where skills come in handy.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Click the Character Sheet tab&lt;/p&gt;&lt;p&gt;- Scroll down to skills.&lt;/p&gt;&lt;p&gt;- Find Accuracy, click train, select 10% of your XP and train the skill.&lt;/p&gt;&lt;p&gt;Follow these same steps to train Looting after clicking Stop training on Accuracy.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Tap the Character Sheet tab.&lt;/p&gt;&lt;p&gt;- Select Manage Skills&lt;/p&gt;&lt;p&gt;- Tap Train on the Accuracy Skill&lt;/p&gt;&lt;p&gt;- Select 10% of your XP and train the skill&lt;/p&gt;&lt;p&gt;Follow these same steps to train Looting after clicking Stop training on Accuracy.&lt;/p&gt;&lt;p&gt;At any time you may click on the skill name to see applicable bonuses, xp, level and so on, The Skill Bonus refers to the bonus the skill applies when using it, such as for Accuracy or Looting. These skills take a while to level and later on you can even get enchanted gear with skill modifiers on them.&lt;/p&gt;&lt;p&gt;Next up, Stats. This ones easy. All character get 1 point into their stats with 1 extra point into their “damage stat.” Gear, especially enchanted gear, raises this by % which all stacks together to give you “Modded stats”.&lt;/p&gt;&lt;p&gt;The more expensive the gear, the better it is for you, enchanted can be better then &lt;a href="/information/shop" target="_blank"&gt;store gear&lt;/a&gt;, depending on the enchant. As you may know, that shiny unique boosted your stats. So Now, I need you to either buy or equip some drop gear:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Click the Character Sheet tab and on the right hand side you will see your inventory. Go through these items and look for ones that give +X% to your stats.&lt;/p&gt;&lt;p&gt;- You may have to visit the shop to buy some more expensive base items that raise the stats higher.&lt;/p&gt;&lt;p&gt;- To visit the shop, click the Hamburger icon in the top left, to open the menu.&lt;/p&gt;&lt;p&gt;- Click the shop, and select Buy from the General Shop&lt;/p&gt;&lt;p&gt;- Filter by what you are looking for and then sort by cost.&lt;/p&gt;&lt;p&gt;- You can click Compare to compare and replace or auto equip, the item&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;-&amp;nbsp;&lt;/strong&gt;Tap the tab: Character Sheet and select, from the drop down list – Inventory management.&lt;/p&gt;&lt;p&gt;- Go through your items looking for ones that will add +X% to your stats.&lt;/p&gt;&lt;p&gt;- You may have to visit the shop by tapping the Hamburger icon at the top left of the screen.&lt;/p&gt;&lt;p&gt;- Tap on shop.&lt;/p&gt;&lt;p&gt;- Tap on Buy under General Shop.&lt;/p&gt;&lt;p&gt;- Filter by what you are looking for and sort by cost.&lt;/p&gt;&lt;p&gt;- You can tap Compare to compare and replace or auto equip, the item&lt;/p&gt;&lt;p&gt;You can read up more on &lt;a href="/information/gear-progression" target="_blank"&gt;gear progression&lt;/a&gt; for more details. Tlessa is a pretty linear straight forward game with some mechanics thrown in to make it more fun. Now go have fun!&lt;/p&gt;</t>
+    <t>&lt;p&gt;We are going to learn about two things today: &lt;a href="/information/character-stats" target="_blank"&gt;Stats&lt;/a&gt; and &lt;a href="/information/skill-information" target="_blank"&gt;Skills&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;Characters under level 12, get a boost to their looting skill making drops a lot more fun. How ever as you will soon reach level 12 you will see the drop rate disappear. This is where skills come in handy.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Click the Character Sheet tab&lt;/p&gt;&lt;p&gt;- Scroll down to skills.&lt;/p&gt;&lt;p&gt;- Find Accuracy, click train, select 10% of your XP and train the skill.&lt;/p&gt;&lt;p&gt;Follow these same steps to train Looting after clicking Stop training on Accuracy.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Tap the Character Sheet tab.&lt;/p&gt;&lt;p&gt;- Select Manage Skills&lt;/p&gt;&lt;p&gt;- Tap Train on the Accuracy Skill&lt;/p&gt;&lt;p&gt;- Select 10% of your XP and train the skill&lt;/p&gt;&lt;p&gt;Follow these same steps to train Looting after clicking Stop training on Accuracy.&lt;/p&gt;&lt;p&gt;At any time you may click on the skill name to see applicable bonuses, xp, level and so on, The Skill Bonus refers to the bonus the skill applies when using it, such as for Accuracy or Looting. These skills take a while to level and later on you can even get &lt;a href="/information/enchanting" target="_blank"&gt;enchanted&lt;/a&gt; gear with skill modifiers on them.&lt;/p&gt;&lt;p&gt;Next up, Stats. This ones easy. All character get 1 point into their stats with 1 extra point into their “damage stat.” upon level up. &lt;/p&gt;&lt;p&gt;Gear, especially enchanted gear, raises this by % which all stacks together to give you “Modded stats”. Which you can see by clicking/tapping Character Sheet, then for desktop - click Additional Information, and you will see on the right side of the modal - Modded stats. For Mobile, click on the plus icon to open the top section, scroll to the orange buttons and tap the same one.&lt;/p&gt;&lt;p&gt;The more expensive the gear (Base gear with no enchants), the better it is for you, enchanted can be better then &lt;a href="/information/shop" target="_blank"&gt;store gear&lt;/a&gt;, depending on the enchant. As you may know, that shiny unique boosted your stats. So Now, I need you to either buy or equip some drop gear to raise your modded stats to the desired level:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Click the Character Sheet tab and on the right hand side you will see your inventory. Go through these items and look for ones that give +X% to your stats.&lt;/p&gt;&lt;p&gt;- You may have to visit the shop to buy some more expensive base items that raise the stats higher.&lt;/p&gt;&lt;p&gt;- To visit the shop, click the Hamburger icon in the top left, to open the menu.&lt;/p&gt;&lt;p&gt;- Click the shop, and select Buy from the General Shop&lt;/p&gt;&lt;p&gt;- Filter by what you are looking for and then sort by cost.&lt;/p&gt;&lt;p&gt;- You can click Compare to compare and replace or auto equip, the item&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;-&amp;nbsp;&lt;/strong&gt;Tap the tab: Character Sheet and select, from the drop down list – Inventory management.&lt;/p&gt;&lt;p&gt;- Go through your items looking for ones that will add +X% to your stats.&lt;/p&gt;&lt;p&gt;- You may have to visit the shop by tapping the Hamburger icon at the top left of the screen.&lt;/p&gt;&lt;p&gt;- Tap on shop.&lt;/p&gt;&lt;p&gt;- Tap on Buy under General Shop.&lt;/p&gt;&lt;p&gt;- Filter by what you are looking for and sort by cost.&lt;/p&gt;&lt;p&gt;- You can tap Compare to compare and replace or auto equip, the item&lt;/p&gt;&lt;p&gt;You can read up more on &lt;a href="/information/gear-progression" target="_blank"&gt;gear progression&lt;/a&gt; for more details. Tlessa is a pretty linear straight forward game with some mechanics thrown in to make it more fun. Now go have fun!&lt;/p&gt;</t>
   </si>
   <si>
     <t>Accuracy</t>
@@ -182,7 +182,7 @@
     <t>You stand before your enemy, blood drips from the weapon in your hand. Rage fills your eyes. Death has come for your enemy.&lt;br /&gt; &lt;br /&gt; “Slaughter them child!”&lt;br /&gt; &lt;br /&gt; You look behind you, blood drips down your face.&lt;br /&gt; &lt;br /&gt; An old haggard man stands behind you a short distance.&lt;br /&gt; &lt;br /&gt; “Don’t focus on me child. Kill the creature!”&lt;br /&gt; &lt;br /&gt; You turn and lunge at your enemy before they can see you. Your enchantments rage before you and your weapon slaughters the creature before you. Blood and gore soaks the ground around you.&lt;br /&gt; &lt;br /&gt; “Next time--” The old man begins as his voice gets closer to you.&lt;br /&gt; &lt;br /&gt; “—Next time! Kill em faster!”&lt;br /&gt; &lt;br /&gt; You awaken from your dream, clutching your weapon.&lt;br /&gt; &lt;br /&gt; What happened? Was that real?</t>
   </si>
   <si>
-    <t>&lt;p&gt;If you spent any time manually attacking, which will happen in some cases – such as with raid critters and some special locations in game, you will notice that the timer for attacking is very slow. You have to wait a whole 10 seconds!&lt;/p&gt;&lt;p&gt;So lets train Fighters Resilience skill to level 20 this will reduce the fight time out bar by a smidge, you can see the percentage if you click on the skill name i the skill section.&lt;/p&gt;&lt;p&gt;One of the pieces of information on this skill is that it has a Fighters Timeout Mod on it, which was raised to a max of 50 seconds, can cut down manual fighting by 5 seconds.&lt;/p&gt;&lt;p&gt;This skill will also raise your Armour Class and Damage over time.&lt;/p&gt;</t>
+    <t>&lt;p&gt;If you spent any time manually attacking, which will happen in some cases – such as with raid critters and some special locations in game, you will notice that the timer for attacking is very slow. You have to wait a whole 10 seconds!&lt;/p&gt;&lt;p&gt;So lets train Fighters Resilience skill to level 20 this will reduce the fight time out bar by a smidge, you can see the percentage if you click on the skill name in the skill section.&lt;/p&gt;&lt;p&gt;One of the pieces of information on this skill is that it has a Fight Timeout Mod on it, which when raised, to a maximum of 50%, can cut down manual fighting timer by 5 seconds.&lt;/p&gt;&lt;p&gt;This skill will also raise your Armour Class and Damage over time.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Fighter's Resilience</t>
@@ -191,10 +191,10 @@
     <t>Blacksmiths Life</t>
   </si>
   <si>
-    <t>Sitting in the INN, you stare into the large fire place with the wood burning and the crackling of the wood. It’s almost as if time stops for a moment and you can gather your thoughts.&lt;br /&gt; &lt;br /&gt; All you do is slaughter creatures, gather loot and slowly get better at hitting the enemies and even slightly faster.&lt;br /&gt; &lt;br /&gt; The flames of the fire seem to stand still, the smell of the fire has dissipated from the air. You look around and no one is moving, like they have been frozen in time.&lt;br /&gt; &lt;br /&gt; You turn back to the fire and see a young man, about twenty-five standing before the fire, his back to you. You call out to him, and he doesn’t turn around but he does speak.&lt;br /&gt; &lt;br /&gt; “Child. I have found something most mysterious. The gates have opened.”&lt;br /&gt; &lt;br /&gt; The gates? What gates?&lt;br /&gt; &lt;br /&gt; “Listen to me child.” The young man turns and faces you. You recognize the face, The Old Man from the dream, but he is much younger now.&lt;br /&gt; &lt;br /&gt; “I need you to speak with the local blacksmith, work with him for a while. Train a different set of skills. Important skills. I need you to craft your own gear.”&lt;br /&gt; &lt;br /&gt; You tell him that the gear you have found, the stuff you can buy from the local blacksmith is better then what you can craft.&lt;br /&gt; &lt;br /&gt; “True, however, you can craft even more powerful gear then that of which you can buy.”&lt;br /&gt; &lt;br /&gt; Before you can ask further questions the flames returning to their burning motion, the wood crackles, the INN is full of voices again and the smell of food fills the air.&lt;br /&gt; &lt;br /&gt; Where did he go?</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Today we are going to learn about &lt;a href="/information/crafting" target="_blank"&gt;crafting&lt;/a&gt;. There are various types of crafting, but we want to focus on weapons and Armour for now.&lt;/p&gt;&lt;p&gt;At first you will fail a lot, even with the suggested &lt;a href="/information/quest-items" target="_blank"&gt;quest items&lt;/a&gt; this quest will take roughly &lt;strong&gt;4 hours to complete&lt;/strong&gt;. Do not worry about trying to rush through it. Instead focus on your gear that you get from exploration and if any of it increases your Weapon Crafting or Armour Crafting – equip it.&lt;/p&gt;&lt;p&gt;Eventually you will craft beyond what the &lt;a href="/information/shop" target="_blank"&gt;shop&lt;/a&gt; sells. The Shop stops at two billion gold, where as players can craft up to 36+ Billion gold items that are much better then shop gear.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Crafting cannot be automated. Keep an eye on Server Messages section to see successes, failures and if you have new items to craft.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- First we want to find the items we need, quest items are automatically used. You can open the Teleport Map Action to then select the location: Ruined Port City Of Kalize (X/Y): 32/368 and click teleport if you can afford the cost. This will get you the: Weapon Smith’s Book which adds 25% to Skill Bonus and XP.&lt;/p&gt;&lt;p&gt;- Repeat the above step to then go to: Dragon cliffs (X/Y): 192/176 to get the Blacksmith’s book for the same bonuses towards Armour Crafting.&lt;/p&gt;&lt;p&gt;Both of these can be upgraded later on when we have access to Labyrinth. There are some One Off &lt;a href="/information/quests" target="_blank"&gt;quests&lt;/a&gt; that will upgrade these.&lt;/p&gt;&lt;p&gt;- Now lets craft, first set up exploration for an hour or two – or what ever you feel like doing, Exploration will run while logged out. Remember to set it up with a monster you can kill in one hit.&lt;/p&gt;&lt;p&gt;- Close exploration and then from the drop down Craft/Enchant select craft, select weapons, select Broken Dagger and then click craft.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Select Map from the actions drop down.&lt;/p&gt;&lt;p&gt;- Click Teleport from the actions under the map.&lt;/p&gt;&lt;p&gt;- Select the location: Ruined Port City Of Kalize (X/Y): 32/368 and click teleport if you can afford the cost. This will get you the: Weapon Smith’s Book which adds 25% to Skill Bonus and XP.&lt;/p&gt;&lt;p&gt;- Repeat the above step to then go to: Dragon cliffs (X/Y): 192/176 to get the Blacksmith’s book for the same bonuses towards Armour Crafting.&lt;/p&gt;&lt;p&gt;Both of these can be upgraded later on when we have access to Labyrinth. There are some One off &lt;a href="/information/quests" target="_blank"&gt;quests&lt;/a&gt; that will upgrade these.&lt;/p&gt;&lt;p&gt;- Now lets craft, first set up exploration for an hour or two – or what ever you feel like doing, Exploration will run while logged out. Remember to set it up with a monster you can kill in one hit.&lt;/p&gt;&lt;p&gt;- Close exploration, select Craft from the drop down and then select Craft from the Craft/Enchant&lt;/p&gt;&lt;p&gt;- Select Weapons, Broken Dagger – Click craft.&lt;/p&gt;&lt;p&gt;- When ready, click Change Type, select Armour, select an Armour to craft and click craft.&lt;/p&gt;&lt;p&gt;Over time new items will be added to the list. That’s all there is to it. When you are ready, click Change Type, select Armour, pick an item to craft and repeat.&lt;/p&gt;</t>
+    <t>Sitting in the INN, you stare into the large fire place with the wood burning and the smell of the old oak as it burns. It’s almost as if time stops for a moment and you can gather your thoughts.&lt;br /&gt; &lt;br /&gt; All you do is slaughter creatures, gather loot and slowly get better at hitting the enemies and even slightly faster.&lt;br /&gt; &lt;br /&gt; The flames of the fire seem to stand still, the smell of the fire has dissipated from the air. You look around and no one is moving, like they have been frozen in time.&lt;br /&gt; &lt;br /&gt; You turn back to the fire and see a young man, about twenty-five standing before the fire, his back to you. You call out to him, and he doesn’t turn around but he does speak.&lt;br /&gt; &lt;br /&gt; “Child. I have found something most mysterious. The gates have opened.”&lt;br /&gt; &lt;br /&gt; The gates? What gates?&lt;br /&gt; &lt;br /&gt; “Listen to me child.” The young man turns and faces you. You recognize the face, The Old Man from the dream, but he is much younger now.&lt;br /&gt; &lt;br /&gt; “I need you to speak with the local blacksmith, work with him for a while. Train a different set of skills. Important skills. I need you to craft your own gear.”&lt;br /&gt; &lt;br /&gt; You tell him that the gear you have found, the stuff you can buy from the local blacksmith is better then what you can craft.&lt;br /&gt; &lt;br /&gt; “True, however, you can craft even more powerful gear then that of which you can buy.”&lt;br /&gt; &lt;br /&gt; Before you can ask further questions the flames returning to their burning motion, the wood crackles, the INN is full of voices again and the smell of food fills the air.&lt;br /&gt; &lt;br /&gt; Where did he go?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Today we are going to learn about &lt;a href="/information/crafting" target="_blank"&gt;crafting&lt;/a&gt;. There are various types of crafting, but we want to focus on weapons and Armour for now.&lt;/p&gt;&lt;p&gt;At first you will fail a lot, even with the suggested &lt;a href="/information/quest-items" target="_blank"&gt;quest items&lt;/a&gt; this quest can take a minute to complete. If you have any enchanted gear that has dropped that has Weapon/Armour Crafting Enchantments on them, I would suggest equipping them, even at the cost of damage.&lt;/p&gt;&lt;p&gt;Eventually you will craft beyond what the &lt;a href="/information/shop" target="_blank"&gt;shop&lt;/a&gt; sells. The Shop stops at two billion gold, where as players can craft up to 36+ Billion gold items that are much better then shop gear.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Crafting cannot be automated. Keep an eye on Server Messages section to see successes, failures and if you have new items to craft.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- First we want to find the items we need, quest items are automatically used. You can open the Teleport Map Action to then select the location: Ruined Port City Of Kalize (X/Y): 32/368 and click teleport if you can afford the cost. This will get you the: Weapon Smith’s Book which adds 25% to Skill Bonus and XP.&lt;/p&gt;&lt;p&gt;- Repeat the above step to then go to: Dragon cliffs (X/Y): 192/176 to get the Blacksmith’s book for the same bonuses towards Armour Crafting.&lt;/p&gt;&lt;p&gt;Both of these can be upgraded later on when we have access to Labyrinth. There are some One Off &lt;a href="/information/quests" target="_blank"&gt;quests&lt;/a&gt; that will upgrade these.&lt;/p&gt;&lt;p&gt;- Now lets craft, first set up exploration for an hour or two – or what ever you feel like doing, Exploration will run while logged out. Remember to set it up with a monster you can kill in one hit.&lt;/p&gt;&lt;p&gt;- Close exploration and then from the drop down Craft/Enchant select craft, select weapons, select Broken Dagger and then click craft.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Select Map from the actions drop down.&lt;/p&gt;&lt;p&gt;- Click Teleport from the actions under the map.&lt;/p&gt;&lt;p&gt;- Select the location: Ruined Port City Of Kalize (X/Y): 32/368 and click teleport if you can afford the cost. This will get you the: Weapon Smith’s Book which adds 25% to Skill Bonus and XP.&lt;/p&gt;&lt;p&gt;- Repeat the above step to then go to: Dragon cliffs (X/Y): 192/176 to get the Blacksmith’s book for the same bonuses towards Armour Crafting.&lt;/p&gt;&lt;p&gt;Both of these can be upgraded later on when we have access to Labyrinth. There are some One off &lt;a href="/information/quests" target="_blank"&gt;quests&lt;/a&gt; that will upgrade these.&lt;/p&gt;&lt;p&gt;- Now lets craft, first set up exploration for an hour or two – or what ever you feel like doing, Exploration will run while logged out. Remember to set it up with a monster you can kill in one hit.&lt;/p&gt;&lt;p&gt;- Close exploration, select Craft from the drop down and then select Craft from the Craft/Enchant&lt;/p&gt;&lt;p&gt;- Select Weapons, Broken Dagger – Click craft.&lt;/p&gt;&lt;p&gt;- When ready, click Change Type, select Armour, select an Armour to craft and click craft.&lt;/p&gt;&lt;p&gt;Over time new items will be added to the list. That’s all there is to it. When you are ready, click Change Type, select Armour, pick an item to craft and repeat.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Weapon Crafting</t>
@@ -330,6 +330,21 @@
   </si>
   <si>
     <t>&lt;p&gt;Today we are going to learn about &lt;a href="/information/class-ranks" target="_blank"&gt;Class Ranks&lt;/a&gt;. Class Ranks allows a character to do a couple of things:&lt;/p&gt;&lt;p&gt;- Switch classes at any time&lt;/p&gt;&lt;p&gt;- Gain more attack towards specific weapons&lt;/p&gt;&lt;p&gt;- Equip Special abilities that can do damage and increase aspects of your character&lt;/p&gt;&lt;p&gt;- Unlock new classes&lt;/p&gt;&lt;p&gt;A character may only have a total of three specialties equipped an of the three only one may of a specialty that deals damage.&lt;/p&gt;&lt;p&gt;Finally, specialties unlock as you level the class rank. So lets get into how to manage your class ranks on your character:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Click on Character Sheet tab&lt;/p&gt;&lt;p&gt;- Click the orange button called Class Ranks&lt;/p&gt;&lt;p&gt;- Here you see a list of the games classes including some, marked by star, that require you to level other class ranks to specific levels.&lt;/p&gt;&lt;p&gt;- Click on your class in the list.&lt;/p&gt;&lt;p&gt;- Here you can you see details about your class, including the class masteries. These masteries are leveled over time by your having the weapon/spell type equipped at the time of fighting monsters.&lt;/p&gt;&lt;p&gt; - Above the class name is a red circle with a minus through it, clicking this will close this section, where as clicking X or the cancel button will close the class masteries modal.&lt;/p&gt;&lt;p&gt;- Next click “Manage Specialties”, this will open a secondary modal.&lt;/p&gt;&lt;p&gt;- These are specialties that unlock at the class rank level, you should – by now – have two specialties you can equip.&lt;/p&gt;&lt;p&gt;- You can investigate the specialties to see what they do. There are two types: Ones that increase specific attributes of your character over time, which are leveled by just fighting monsters and ones that do damage – which fire automatically when fighting monsters.&lt;/p&gt;&lt;p&gt;- Equip the required amount of specialties.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Tap on Character Sheet tab&lt;/p&gt;&lt;p&gt;- Open the top section and tap on the orange button called Class Ranks&lt;/p&gt;&lt;p&gt;- Here you see a list of the games classes including some, marked by star, that require you to level other class ranks to specific levels.&lt;/p&gt;&lt;p&gt;- Click on your class in the list.&lt;/p&gt;&lt;p&gt;- Here you can you see details about your class, including the class masteries. These masteries are leveled over time by your having the weapon/spell type equipped at the time of fighting monsters.&lt;/p&gt;&lt;p&gt; - Above the class name is a red circle with a minus through it, clicking this will close this section, where as clicking X or the cancel button will close the class masteries modal.&lt;/p&gt;&lt;p&gt;- Next click “Manage Specialties”, this will open a secondary modal.&lt;/p&gt;&lt;p&gt;- These are specialties that unlock at the class rank level, you should – by now – have two specialties you can equip.&lt;/p&gt;&lt;p&gt;- You can investigate the specialties to see what they do. There are two types: Ones that increase specific attributes of your character over time, which are leveled by just fighting monsters and ones that do damage – which fire automatically when fighting monsters.&lt;/p&gt;&lt;p&gt;- Equip the required amount of specialties.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;: Under Equipped Specialties, you can unequipped them to then equip other specialties from other classes. As you switch classes and play around, you can mix and match specialties equipped for maximum damage and stats.&lt;/p&gt;&lt;p&gt;All of these specialties, masteries and class ranks will level over time by you killing monsters. No XP will be sacrificed like when you train skills, instead this is a separate XP curve for each of the sections.&lt;/p&gt;&lt;p&gt;You server message section will also, as you may have seen, show you when you get levels in class specialties, ranks or masteries.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>The void in your heart</t>
+  </si>
+  <si>
+    <t>You find it hard to breathe. Your vision is blurred, you grasp for a sense of stability.&lt;br /&gt; &lt;br /&gt; A slap across the face, the ringing pain of the hand connecting with your face, reality comes back.&lt;br /&gt; &lt;br /&gt; Your parents are not your parents. Everything is a lie.&lt;br /&gt; &lt;br /&gt; You stare at the man who slapped you. What is going on?&lt;br /&gt; &lt;br /&gt; The Poet …&lt;br /&gt; &lt;br /&gt; “… He said something about how we need a way to lock The Creator back up. He mentioned that we could use the magic of the universe to open portals, to create lives, to build an army of … Well you …”&lt;br /&gt; &lt;br /&gt; You look at your hands, your body before you. A creation of universal magic?&lt;br /&gt; &lt;br /&gt; “You are real … Not just some kind of magical construct. You are …. real.”&lt;br /&gt; &lt;br /&gt; Real.&lt;br /&gt; &lt;br /&gt; Vomit.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Today we want to learn about &lt;a href="/information/voidance" target="_blank"&gt;Devouring Light/Darkness&lt;/a&gt;. One lets you void your enemy so their enchantments do not fire and over all they do less damage.&lt;/p&gt;&lt;p&gt;The problem with that. Is that enemies can do the same to you. So to counter an enemy voiding you, making your character use only raw stats and no enchantments, you use whats called Devoid.&lt;/p&gt;&lt;p&gt;Devoid allows you to “Void the enemies ability to void your enchantments.” Which in turn allows the you to then: Void the enemy, so their enchantments do not fire.&lt;/p&gt;&lt;p&gt;On top of this there is also Resistance to both of these that character can obtain, so that you can resist the enemies ability to void you, even if you fail to “Devoid” them.&lt;/p&gt;&lt;p&gt;From Surface to Hell, you will devoid followed by a void first, where as in Purgatory Enemies will devoid followed by a void first, which is where the resistance comes in handy.&lt;/p&gt;&lt;p&gt;To get the Devouring Light/Darkness % up, which can be seen on The Character Sheet: Additional Information (Orange Button) → Voidance tab, you will have to complete the Quest, on Surface called: Return of the King’s Crown.&lt;/p&gt;&lt;p&gt;This will cost a lot of Gold Dust and the easiest way to get it, while you train Looting is to train Enchanting, enchant and then disenchant to gain gold dust.&lt;/p&gt;&lt;p&gt;The item you receive is called: Dead King's Crown. This allows you to gain 100% in Devouring Light (Voidance) and 85% in Devouring Darkness (DeVoid), which will make harder creatures much easier to take on.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>The Return of the King's Crown</t>
+  </si>
+  <si>
+    <t>Dead King's Crown</t>
   </si>
 </sst>
 </file>
@@ -669,7 +684,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AP15"/>
+  <dimension ref="A1:AP16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -696,7 +711,7 @@
     <col min="17" max="17" width="23.423" bestFit="true" customWidth="true" style="0"/>
     <col min="18" max="18" width="26.993" bestFit="true" customWidth="true" style="0"/>
     <col min="19" max="19" width="24.708" bestFit="true" customWidth="true" style="0"/>
-    <col min="20" max="20" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="20" max="20" width="36.42" bestFit="true" customWidth="true" style="0"/>
     <col min="21" max="21" width="26.993" bestFit="true" customWidth="true" style="0"/>
     <col min="22" max="22" width="31.707" bestFit="true" customWidth="true" style="0"/>
     <col min="23" max="23" width="16.425" bestFit="true" customWidth="true" style="0"/>
@@ -924,7 +939,7 @@
         <v>15</v>
       </c>
       <c r="AE4">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="AO4">
         <v>1000</v>
@@ -982,28 +997,25 @@
         <v>59</v>
       </c>
       <c r="E6">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="F6" t="s">
         <v>60</v>
       </c>
       <c r="G6">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="H6" t="s">
         <v>61</v>
       </c>
       <c r="I6">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="U6" t="s">
         <v>62</v>
       </c>
       <c r="V6" t="s">
         <v>63</v>
-      </c>
-      <c r="AE6">
-        <v>100</v>
       </c>
       <c r="AO6">
         <v>1000</v>
@@ -1349,6 +1361,53 @@
       </c>
       <c r="AP15">
         <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16">
+        <v>500</v>
+      </c>
+      <c r="F16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16">
+        <v>75</v>
+      </c>
+      <c r="H16" t="s">
+        <v>78</v>
+      </c>
+      <c r="I16">
+        <v>50</v>
+      </c>
+      <c r="T16" t="s">
+        <v>108</v>
+      </c>
+      <c r="U16" t="s">
+        <v>109</v>
+      </c>
+      <c r="AM16">
+        <v>5000</v>
+      </c>
+      <c r="AN16">
+        <v>1000</v>
+      </c>
+      <c r="AO16">
+        <v>1000000</v>
+      </c>
+      <c r="AP16">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Split out how battle rewards are handled.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -215,7 +215,7 @@
     <t>You are exhausted, tired, confused.&lt;br /&gt; &lt;br /&gt; “Child” comes a familiar voice as you sit up on your bed.&lt;br /&gt; &lt;br /&gt; The INN is creaky, noisy and musty. The single candle flame that burns in the room barley illuminates the room.&lt;br /&gt; &lt;br /&gt; As he walks from the shadows The Guide stands before you, not young and handsome, but old and wise, dressed in robes. His skin is brown from the sun.&lt;br /&gt; &lt;br /&gt; “Downstairs sits a woman, an attractive woman.” he states.&lt;br /&gt; &lt;br /&gt; “She will teach you about magic and its properties, specifically in the art of enchanting and disenchanting.”&lt;br /&gt; &lt;br /&gt; You ask him why he can’t teach you and he deflects the question.&lt;br /&gt; &lt;br /&gt; “Go now child. She isn’t to be kept waiting.”&lt;br /&gt; &lt;br /&gt; You head down the stairs to meet the Enchantress.&lt;br /&gt; &lt;br /&gt; She waits for you at a table, a woman in black, instantly recognizable by her long black hair and pale complexion. She radiates beauty.&lt;br /&gt; &lt;br /&gt; You walk over and sit down at the table. “Hello child.” She starts, he voice is soft and entrancing. “have you heard of the queen?” You shake your head no. “She has gifted you with some of those green shiny unique’s in your inventory.”&lt;br /&gt; &lt;br /&gt; You remember those. Killing monsters gets you faction with the plane and its people and as a reward they give you a shiny green item that makes you feel much much stronger.&lt;br /&gt; &lt;br /&gt; “She can give you more powerful ones, but you have to face the most fearsome of creatures to earn her attention. In the mean time lets discuss the art of magic. Lets start small with spells …”</t>
   </si>
   <si>
-    <t>&lt;p&gt;&lt;strong&gt;Note: &lt;/strong&gt;This quest can take up to 2 hours to complete. Do not feel like you have to rush through it.&lt;/p&gt;&lt;p&gt;Lets start learning about spells.&lt;/p&gt;&lt;p&gt;You have just spent a ton f time crafting weapons and Armour, we will repeat this to craft spells. Spells are useful for caster classes, as well as any one who wants to use them.&lt;/p&gt;&lt;p&gt;Damage spells and Staves (Two Handed weapons) can raise the characters intelligence, both of which can be bought from the shop or crafted.&lt;/p&gt;&lt;p&gt;Healing spells are great for characters who want to do Cast and attack or Attack and Cast, like Prophets.&lt;/p&gt;&lt;p&gt;To get the quest item required, you will need to kill: Umbering Spirit Lord on Surface. This creature is further down the list and may require you to upgrade your gear through the shop before being able to take him down. This creature has a 15% chance to drop the item, so exploration might be a good choice here.&lt;/p&gt;</t>
+    <t>&lt;p&gt;Lets start learning about spells.&lt;/p&gt;&lt;p&gt;You have just spent a ton of time crafting weapons and Armour, we will repeat this to craft spells. Spells are useful for caster classes, as well as any one who wants to use them, be they healing or damage based.&lt;/p&gt;&lt;p&gt;Damage spells and Staves (Two Handed weapons) can raise the characters intelligence, both of which can be bought from the shop or crafted.&lt;/p&gt;&lt;p&gt;Healing spells are great for characters who want to do Cast and attack or Attack and Cast, like Prophets.&lt;/p&gt;&lt;p&gt;To get the quest item required, you will need to kill: &lt;strong&gt;Umbering Spirit Lord&lt;/strong&gt; on Surface. This creature is further down the list and may require you to upgrade your gear through the shop before being able to take him down. &lt;/p&gt;&lt;p&gt;This creature has a 15% chance to drop the item, so exploration might be a good choice here.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Spell Crafting</t>
@@ -236,7 +236,7 @@
     <t>&lt;p&gt;Time to stop training and fight a monster. This will drop weather you use exploration or not. Find the Key of Labyrinth by fighting the Labyrinth Fiend on Surface&lt;/p&gt;&lt;p&gt;To make it easier lets also raise our looting skill.&lt;/p&gt;&lt;p&gt;Once you have the key, lets:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;Click traverse under the map.&lt;/p&gt;&lt;p&gt;- Select Labyrinth from the plane drop down.&lt;/p&gt;&lt;p&gt;- Click traverse.&lt;/p&gt;&lt;p&gt;- Welcome to labyrinth. Monsters down here have the same strength as surface but are new.&lt;/p&gt;&lt;p&gt;- Kill enough until your faction level with surface is level 1.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- From the action drop down select Map Movement&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;Click traverse under the map.&lt;/p&gt;&lt;p&gt;- Select Labyrinth from the plane drop down.&lt;/p&gt;&lt;p&gt;- Click traverse.&lt;/p&gt;&lt;p&gt;- Welcome to labyrinth. Monsters down here have the same strength as surface but are new.&lt;/p&gt;&lt;p&gt;- Kill enough until your faction level with surface is level 1.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>Quick Feet</t>
+    <t>Labyrinth</t>
   </si>
   <si>
     <t>Key of the Labyrinth</t>
@@ -1038,13 +1038,13 @@
         <v>66</v>
       </c>
       <c r="E7">
-        <v>160</v>
+        <v>90</v>
       </c>
       <c r="F7" t="s">
         <v>67</v>
       </c>
       <c r="G7">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="H7" t="s">
         <v>68</v>
@@ -1079,7 +1079,7 @@
         <v>72</v>
       </c>
       <c r="E8">
-        <v>220</v>
+        <v>120</v>
       </c>
       <c r="F8" t="s">
         <v>52</v>
@@ -1087,11 +1087,14 @@
       <c r="G8">
         <v>25</v>
       </c>
-      <c r="H8" t="s">
+      <c r="Q8" t="s">
         <v>73</v>
       </c>
-      <c r="I8">
-        <v>10</v>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8" t="s">
+        <v>73</v>
       </c>
       <c r="U8" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
Minor fixes to guide quests.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="111">
   <si>
     <t>id</t>
   </si>
@@ -248,7 +248,7 @@
     <t>You have been on another planes, a plane full of ruins, broken pieces of multiple labyrinths. The entire plane was covered with them.&lt;br /&gt; &lt;br /&gt; As you recover from your travels, slaughtering a whole new group of fearsome creatures, gaining notoriety with the inhabitants of said plane.&lt;br /&gt; &lt;br /&gt; Still no sign of the Enchantress and no sign of The Guide. You take a moment to relax before your next adventure.&lt;br /&gt; &lt;br /&gt; As you rise to the new dawn of a new day you have a knock at the door. You rise and greet the stranger. The Enchantress walks in. Today she wares a red robe and you can see deep into her blue eyes.&lt;br /&gt; &lt;br /&gt; “My darling child, I hear you have been adventuring. Shall we pick up where we left off? The art of enchanting.”&lt;br /&gt; &lt;br /&gt; You tell her you have plenty of enchanted gear.&lt;br /&gt; &lt;br /&gt; “Wouldn’t you like better gear? Stronger gear?”</t>
   </si>
   <si>
-    <t>&lt;p&gt;Today's lesson is about &lt;a href="/information/enchanting" target="_blank"&gt;enchanting&lt;/a&gt; and &lt;a href="/information/disenchanting" target="_blank"&gt;disenchanting&lt;/a&gt;. Just like crafting, enchanting is wildly important. As you may know, you cannot buy enchanted gear from the shop. Some players will sell it on the &lt;a href="/information/market-board" target="_blank"&gt;market place&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;More importantly, you want a &lt;a href="/information/currencies" target="_blank"&gt;currency&lt;/a&gt; you can get from it: Gold Dust. This currency is used in a lot of quests we are going to start doing soon. So lets get a lot of it.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop/Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;To enchant, from the crafting drop down select enchant.&lt;/p&gt;&lt;p&gt;- Here you have an item to select, a suffix and a prefix to select. The cost of enchanting can get widely expensive so exploration is required. Since you need items: weapons, Armour, spells and Rings, you will also want to be crafting. You can also re-enchant enchanted items but that gets more costly.&lt;/p&gt;&lt;p&gt;You can also just go to the shop and buy multiple items to enchant, like broken daggers.&lt;/p&gt;&lt;p&gt;- Next, when you have enchanted, ideally 75 items, next go to your inventory&lt;/p&gt;&lt;p&gt;- From the actions on the inventory section of your character sheet, click Disenchant All.&lt;/p&gt;&lt;p&gt;- This will raise your disenchanting skill, and slowly over time your enchanting skill as well.&lt;/p&gt;&lt;p&gt;- Repeat till you meet the quest requirements.&lt;/p&gt;</t>
+    <t>&lt;p&gt;Today's lesson is about &lt;a href="/information/enchanting" target="_blank"&gt;enchanting&lt;/a&gt; and &lt;a href="/information/disenchanting" target="_blank"&gt;disenchanting&lt;/a&gt;. Just like crafting, enchanting is wildly important. As you may know, you cannot buy enchanted gear from the shop. Some players will sell it on the &lt;a href="/information/market-board" target="_blank"&gt;market place&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;More importantly, you want a &lt;a href="/information/currencies" target="_blank"&gt;currency&lt;/a&gt; you can get from it: Gold Dust. This currency is used in a lot of quests we are going to start doing soon. So lets get a lot of it.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop/Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;To enchant, from the crafting drop down select enchant.&lt;/p&gt;&lt;p&gt;- Here you have an item to select, a suffix and a prefix to select. The cost of enchanting can get widely expensive so exploration is required. Since you need items: weapons, Armour, spells and Rings, you will also want to be crafting. You can also re-enchant enchanted items but that gets more costly.&lt;/p&gt;&lt;p&gt;You can also just go to the shop and buy multiple items to enchant, like broken daggers.&lt;/p&gt;&lt;p&gt;- Next, when you have enchanted, ideally 75 items, next go to your inventory&lt;/p&gt;&lt;p&gt;- From the actions on the inventory section of your character sheet, click Disenchant All.&lt;/p&gt;&lt;p&gt;- This will raise your disenchanting skill, and slowly over time your enchanting skill as well.&lt;/p&gt;&lt;p&gt;- Repeat till you meet the quest requirements.&lt;/p&gt;&lt;p&gt;The &lt;strong&gt;Skill Type Crafting to level 10&lt;/strong&gt; basically means, level any rafting skill you want to level 10 or higher.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Enchanting</t>
@@ -263,19 +263,22 @@
     <t>Traveling To Dungeons</t>
   </si>
   <si>
-    <t>You have come a long way since you first set out. Learning more of the world, learning more about your self and developing your skills.&lt;br /&gt; &lt;br /&gt; You sit under the tree outside of town and watch the merchants go by. A few stop and ask if you would like to purchase some of their wares, a few have some interesting knickknacks, and a few others have some food worth buying.&lt;br /&gt; &lt;br /&gt; As the day passes by and the sun begins to set you think of heading back to town to wash, relax and get a good nights sleep.&lt;br /&gt; &lt;br /&gt; “Hello there” comes an unfamiliar voice.&lt;br /&gt; &lt;br /&gt; You look and see a man in a Fedora, Green Tunic and Black leather pants. He seems older, but moves as if he is younger then his age.&lt;br /&gt; &lt;br /&gt; He comes closer and introduces him self, “I am The Poet and have been sent by The Guide to ask a favor of you, one from him.”&lt;br /&gt; &lt;br /&gt; You ask why he doesn’t come himself and ask this favor.&lt;br /&gt; &lt;br /&gt; “There is a darkness that is seeping from the depths into all the Planes. It is corrupting the Planes and causing the creatures to become vile and wicked. The Guide is busy investigating something deep with in Dungeons. Where he wants you to meet him.”&lt;br /&gt; &lt;br /&gt; You remember how you go to labyrinth, how hard can it be to get to Dungeons? You agree and The Poet tells you how to set off.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;This is another &lt;a href="/information/quests" target="_blank"&gt;quest&lt;/a&gt; where we are going to a new &lt;a href="/information/planes" target="_blank"&gt;plane&lt;/a&gt;. How ever, to get there we have to complete a few quests.&lt;/p&gt;&lt;p&gt;Quests are how a lot of Tlessas features are unlocked for players. These quests, much like Guide Quests, will have a story – before and after completion – as well as explicit instructions on how to complete them, much like these.&lt;/p&gt;&lt;p&gt;Since you already know how to &lt;a href="/information/traverse" target="_blank"&gt;traverse&lt;/a&gt;, we just need to get you a quest item that allows you to traverse down to Dungeons.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; The required secondary quest item, will require you to complete a quest from Labyrinth under the One Off Quest section called: &lt;strong&gt;Ring Lord.&lt;/strong&gt; Click the quest, and click on the Requirements tab to see what you have to do.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Click the Quests tab&lt;/p&gt;&lt;p&gt;- Here you can see a list of quests for the plane you are on (if you are not on surface, select the Surface plane from the Planes drop down.)&lt;/p&gt;&lt;p&gt;- On the Surface quests you will see a quest (to the left) called Light The Way, complete the quests working down the tree until you complete it. Locked Quests are red, quests you can complete are Blue and Completed Quests are Green.&lt;/p&gt;&lt;p&gt;- Click on the quest to read the story, see the requirements and the reward.&lt;/p&gt;&lt;p&gt;- The Requirements tab will have explicit instructions beside each requirement.&lt;/p&gt;&lt;p&gt;- Much like Guide Quests, you can see your completed quests in the sidebar (Hamburger menu to the top left) under: Quest Log → Completed Quests.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Tap the Quests tab&lt;/p&gt;&lt;p&gt;- Here you can see a list of quests for the plane you are on (if you are not on surface, select the Surface plane from the Planes drop down.)&lt;/p&gt;&lt;p&gt;- On the Surface quests you will see a quest (to the left – you can scroll left/right) called Light The Way, complete the quests working down the tree until you complete it. Locked Quests are red, quests you can complete are Blue and Completed Quests are Green.&lt;/p&gt;&lt;p&gt;- Tap on the quest to read the story, see the requirements and the reward.&lt;/p&gt;&lt;p&gt;- The Requirements tab will have explicit instructions beside each requirement.&lt;/p&gt;&lt;p&gt;- Much like Guide Quests, you can see your completed quests in the sidebar (Hamburger menu to the top left) under: Quest Log → Completed Quests.&lt;/p&gt;&lt;p&gt;Quests, much like Enchanting are vitally important to progress not only the over all story of the game, but also to get access to new features, new planes and so on of the game.&lt;/p&gt;&lt;p&gt;Each Plane will tell a story that all come together to tell a general story of The Creator (not the game Creator – an NPC) Quest chains going straight down tell their own story.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Ring Crafting</t>
+    <t>You have come a long way since you first set out. Learning more of the world, learning more about your self and developing your skills.&lt;br /&gt; &lt;br /&gt; You sit under the tree outside of town and watch the merchants go by. A few stop and ask if you would like to purchase some of their wares, a few have some interesting knickknacks, and a few others have some food worth buying.&lt;br /&gt; &lt;br /&gt; As the day passes by and the sun begins to set you think of heading back to town to wash, relax and get a good nights sleep.&lt;br /&gt; &lt;br /&gt; “Hello there” comes an unfamiliar voice.&lt;br /&gt; &lt;br /&gt; You look and see a man in a Fedora, Green Tunic and black leather pants. He seems older, but moves as if he is younger then his age.&lt;br /&gt; &lt;br /&gt; He comes closer and introduces himself, “I am The Poet and have been sent by The Guide to ask a favor of you, one from him.”&lt;br /&gt; &lt;br /&gt; You ask why he doesn’t come himself and ask this favor.&lt;br /&gt; &lt;br /&gt; “There is a darkness that is seeping from the depths into all the Planes. It is corrupting the Planes and causing the creatures to become vile and wicked. The Guide is busy investigating something deep with in Dungeons. Where he wants you to meet him.”&lt;br /&gt; &lt;br /&gt; You remember how you got to labyrinth, how hard can it be to get to Dungeons? You agree and The Poet tells you how to set off.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This is another &lt;a href="/information/quests" target="_blank"&gt;quest&lt;/a&gt; where we are going to a new &lt;a href="/information/planes" target="_blank"&gt;plane&lt;/a&gt;. How ever, to get there we have to complete a few quests.&lt;/p&gt;&lt;p&gt;Quests are how a lot of Tlessas features are unlocked for players. These quests, much like Guide Quests, will have a story – before and after completion – as well as explicit instructions on how to complete them, much like these.&lt;/p&gt;&lt;p&gt;Since you already know how to &lt;a href="/information/traverse" target="_blank"&gt;traverse&lt;/a&gt;, we just need to get you a quest item that allows you to traverse down to Dungeons.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; The required secondary quest item, will require you to complete a quest from Labyrinth under the One Off Quest section called: &lt;strong&gt;Dark Enchantress.&lt;/strong&gt; Click the quest, and click on the Requirements tab to see what you have to do.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Click the Quests tab&lt;/p&gt;&lt;p&gt;- Here you can see a list of quests for the plane you are on (if you are not on surface, select the Surface plane from the Planes drop down.)&lt;/p&gt;&lt;p&gt;- On the Surface quests you will see a quest (to the left) called Light The Way, complete the quests working down the tree until you complete it. Locked Quests are red, quests you can complete are Blue and Completed Quests are Green.&lt;/p&gt;&lt;p&gt;- Click on the quest to read the story, see the requirements and the reward.&lt;/p&gt;&lt;p&gt;- The Requirements tab will have explicit instructions beside each requirement.&lt;/p&gt;&lt;p&gt;- Much like Guide Quests, you can see your completed quests in the sidebar (Hamburger menu to the top left) under: Quest Log → Completed Quests.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Tap the Quests tab&lt;/p&gt;&lt;p&gt;- Here you can see a list of quests for the plane you are on (if you are not on surface, select the Surface plane from the Planes drop down.)&lt;/p&gt;&lt;p&gt;- On the Surface quests you will see a quest (to the left – you can scroll left/right) called Light The Way, complete the quests working down the tree until you complete it. Locked Quests are red, quests you can complete are Blue and Completed Quests are Green.&lt;/p&gt;&lt;p&gt;- Tap on the quest to read the story, see the requirements and the reward.&lt;/p&gt;&lt;p&gt;- The Requirements tab will have explicit instructions beside each requirement.&lt;/p&gt;&lt;p&gt;- Much like Guide Quests, you can see your completed quests in the sidebar (Hamburger menu to the top left) under: Quest Log → Completed Quests.&lt;/p&gt;&lt;p&gt;Quests, much like Enchanting are vitally important to progress not only the over all story of the game, but also to get access to new features, new planes and so on of the game.&lt;/p&gt;&lt;p&gt;Each Plane will tell a story that all come together to tell a general story of The Creator (not the game Creator – an NPC) Quest chains going straight down tell their own story.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Dungeons</t>
+  </si>
+  <si>
+    <t>Light the way</t>
   </si>
   <si>
     <t>Torch</t>
   </si>
   <si>
-    <t>Ring Crafter's Master Book</t>
+    <t>Enchantress' Diary</t>
   </si>
   <si>
     <t>Death is something special</t>
@@ -713,7 +716,7 @@
     <col min="19" max="19" width="24.708" bestFit="true" customWidth="true" style="0"/>
     <col min="20" max="20" width="36.42" bestFit="true" customWidth="true" style="0"/>
     <col min="21" max="21" width="26.993" bestFit="true" customWidth="true" style="0"/>
-    <col min="22" max="22" width="31.707" bestFit="true" customWidth="true" style="0"/>
+    <col min="22" max="22" width="28.136" bestFit="true" customWidth="true" style="0"/>
     <col min="23" max="23" width="16.425" bestFit="true" customWidth="true" style="0"/>
     <col min="24" max="24" width="22.28" bestFit="true" customWidth="true" style="0"/>
     <col min="25" max="25" width="18.71" bestFit="true" customWidth="true" style="0"/>
@@ -1123,7 +1126,7 @@
         <v>77</v>
       </c>
       <c r="E9">
-        <v>250</v>
+        <v>160</v>
       </c>
       <c r="F9" t="s">
         <v>78</v>
@@ -1135,16 +1138,22 @@
         <v>79</v>
       </c>
       <c r="I9">
-        <v>12</v>
+        <v>5</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>10</v>
       </c>
       <c r="U9" t="s">
         <v>80</v>
       </c>
       <c r="X9">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="AE9">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="AM9">
         <v>5000</v>
@@ -1173,7 +1182,7 @@
         <v>83</v>
       </c>
       <c r="E10">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="F10" t="s">
         <v>52</v>
@@ -1181,20 +1190,23 @@
       <c r="G10">
         <v>50</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="S10" t="s">
         <v>84</v>
       </c>
-      <c r="I10">
-        <v>10</v>
+      <c r="T10" t="s">
+        <v>85</v>
       </c>
       <c r="U10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="V10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AE10">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="AO10">
         <v>250000</v>
@@ -1208,13 +1220,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E11">
         <v>350</v>
@@ -1246,22 +1258,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D12" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E12">
         <v>400</v>
       </c>
       <c r="L12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M12" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N12">
         <v>1</v>
@@ -1290,13 +1302,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C13" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D13" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Z13">
         <v>1</v>
@@ -1319,13 +1331,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D14" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AA14">
         <v>10</v>
@@ -1334,7 +1346,7 @@
         <v>200</v>
       </c>
       <c r="AC14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AO14">
         <v>2500</v>
@@ -1348,13 +1360,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="P15">
         <v>2</v>
@@ -1371,13 +1383,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D16" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E16">
         <v>500</v>
@@ -1395,10 +1407,10 @@
         <v>50</v>
       </c>
       <c r="T16" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="U16" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AM16">
         <v>5000</v>

</xml_diff>

<commit_message>
Guide quest updates. Minor fixes and changes to quests
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="112">
   <si>
     <t>id</t>
   </si>
@@ -194,7 +194,7 @@
     <t>Sitting in the INN, you stare into the large fire place with the wood burning and the smell of the old oak as it burns. It’s almost as if time stops for a moment and you can gather your thoughts.&lt;br /&gt; &lt;br /&gt; All you do is slaughter creatures, gather loot and slowly get better at hitting the enemies and even slightly faster.&lt;br /&gt; &lt;br /&gt; The flames of the fire seem to stand still, the smell of the fire has dissipated from the air. You look around and no one is moving, like they have been frozen in time.&lt;br /&gt; &lt;br /&gt; You turn back to the fire and see a young man, about twenty-five standing before the fire, his back to you. You call out to him, and he doesn’t turn around but he does speak.&lt;br /&gt; &lt;br /&gt; “Child. I have found something most mysterious. The gates have opened.”&lt;br /&gt; &lt;br /&gt; The gates? What gates?&lt;br /&gt; &lt;br /&gt; “Listen to me child.” The young man turns and faces you. You recognize the face, The Old Man from the dream, but he is much younger now.&lt;br /&gt; &lt;br /&gt; “I need you to speak with the local blacksmith, work with him for a while. Train a different set of skills. Important skills. I need you to craft your own gear.”&lt;br /&gt; &lt;br /&gt; You tell him that the gear you have found, the stuff you can buy from the local blacksmith is better then what you can craft.&lt;br /&gt; &lt;br /&gt; “True, however, you can craft even more powerful gear then that of which you can buy.”&lt;br /&gt; &lt;br /&gt; Before you can ask further questions the flames returning to their burning motion, the wood crackles, the INN is full of voices again and the smell of food fills the air.&lt;br /&gt; &lt;br /&gt; Where did he go?</t>
   </si>
   <si>
-    <t>&lt;p&gt;Today we are going to learn about &lt;a href="/information/crafting" target="_blank"&gt;crafting&lt;/a&gt;. There are various types of crafting, but we want to focus on weapons and Armour for now.&lt;/p&gt;&lt;p&gt;At first you will fail a lot, even with the suggested &lt;a href="/information/quest-items" target="_blank"&gt;quest items&lt;/a&gt; this quest can take a minute to complete. If you have any enchanted gear that has dropped that has Weapon/Armour Crafting Enchantments on them, I would suggest equipping them, even at the cost of damage.&lt;/p&gt;&lt;p&gt;Eventually you will craft beyond what the &lt;a href="/information/shop" target="_blank"&gt;shop&lt;/a&gt; sells. The Shop stops at two billion gold, where as players can craft up to 36+ Billion gold items that are much better then shop gear.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Crafting cannot be automated. Keep an eye on Server Messages section to see successes, failures and if you have new items to craft.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- First we want to find the items we need, quest items are automatically used. You can open the Teleport Map Action to then select the location: Ruined Port City Of Kalize (X/Y): 32/368 and click teleport if you can afford the cost. This will get you the: Weapon Smith’s Book which adds 25% to Skill Bonus and XP.&lt;/p&gt;&lt;p&gt;- Repeat the above step to then go to: Dragon cliffs (X/Y): 192/176 to get the Blacksmith’s book for the same bonuses towards Armour Crafting.&lt;/p&gt;&lt;p&gt;Both of these can be upgraded later on when we have access to Labyrinth. There are some One Off &lt;a href="/information/quests" target="_blank"&gt;quests&lt;/a&gt; that will upgrade these.&lt;/p&gt;&lt;p&gt;- Now lets craft, first set up exploration for an hour or two – or what ever you feel like doing, Exploration will run while logged out. Remember to set it up with a monster you can kill in one hit.&lt;/p&gt;&lt;p&gt;- Close exploration and then from the drop down Craft/Enchant select craft, select weapons, select Broken Dagger and then click craft.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Select Map from the actions drop down.&lt;/p&gt;&lt;p&gt;- Click Teleport from the actions under the map.&lt;/p&gt;&lt;p&gt;- Select the location: Ruined Port City Of Kalize (X/Y): 32/368 and click teleport if you can afford the cost. This will get you the: Weapon Smith’s Book which adds 25% to Skill Bonus and XP.&lt;/p&gt;&lt;p&gt;- Repeat the above step to then go to: Dragon cliffs (X/Y): 192/176 to get the Blacksmith’s book for the same bonuses towards Armour Crafting.&lt;/p&gt;&lt;p&gt;Both of these can be upgraded later on when we have access to Labyrinth. There are some One off &lt;a href="/information/quests" target="_blank"&gt;quests&lt;/a&gt; that will upgrade these.&lt;/p&gt;&lt;p&gt;- Now lets craft, first set up exploration for an hour or two – or what ever you feel like doing, Exploration will run while logged out. Remember to set it up with a monster you can kill in one hit.&lt;/p&gt;&lt;p&gt;- Close exploration, select Craft from the drop down and then select Craft from the Craft/Enchant&lt;/p&gt;&lt;p&gt;- Select Weapons, Broken Dagger – Click craft.&lt;/p&gt;&lt;p&gt;- When ready, click Change Type, select Armour, select an Armour to craft and click craft.&lt;/p&gt;&lt;p&gt;Over time new items will be added to the list. That’s all there is to it. When you are ready, click Change Type, select Armour, pick an item to craft and repeat.&lt;/p&gt;</t>
+    <t>&lt;p&gt;Today we are going to learn about &lt;a href="/information/crafting" target="_blank"&gt;crafting&lt;/a&gt;. There are various types of crafting, but we want to focus on weapons and Armour for now.&lt;/p&gt;&lt;p&gt;At first you will fail a lot, even with the suggested &lt;a href="/information/quest-items" target="_blank"&gt;quest items&lt;/a&gt; this quest can take a minute to complete. If you have any enchanted gear that has dropped that has Weapon/Armour Crafting Enchantments on them, I would suggest equipping them, even at the cost of damage.&lt;/p&gt;&lt;p&gt;Eventually you will craft beyond what the &lt;a href="/information/shop" target="_blank"&gt;shop&lt;/a&gt; sells. The Shop stops at two billion gold, where as players can craft up to 36+ Billion gold items that are much better then shop gear.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Crafting cannot be automated. Keep an eye on Server Messages section to see successes, failures and if you have new items to craft.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Remember to keep crafting - even after this quest. Stick to weapons (any type) - but do experiment with others, like Armour. A later quest will be less painful.&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- First we want to find the items we need, quest items are automatically used. You can open the Teleport Map Action to then select the location: Ruined Port City Of Kalize (X/Y): 32/368 and click teleport if you can afford the cost. This will get you the: Weapon Smith’s Book which adds 25% to Skill Bonus and XP.&lt;/p&gt;&lt;p&gt;- Repeat the above step to then go to: Dragon cliffs (X/Y): 192/176 to get the Blacksmith’s book for the same bonuses towards Armour Crafting.&lt;/p&gt;&lt;p&gt;Both of these can be upgraded later on when we have access to Labyrinth. There are some One Off &lt;a href="/information/quests" target="_blank"&gt;quests&lt;/a&gt; that will upgrade these.&lt;/p&gt;&lt;p&gt;- Now lets craft, first set up exploration for an hour or two – or what ever you feel like doing, Exploration will run while logged out. Remember to set it up with a monster you can kill in one hit.&lt;/p&gt;&lt;p&gt;- Close exploration and then from the drop down Craft/Enchant select craft, select weapons, select Broken Dagger and then click craft.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Select Map from the actions drop down.&lt;/p&gt;&lt;p&gt;- Click Teleport from the actions under the map.&lt;/p&gt;&lt;p&gt;- Select the location: Ruined Port City Of Kalize (X/Y): 32/368 and click teleport if you can afford the cost. This will get you the: Weapon Smith’s Book which adds 25% to Skill Bonus and XP.&lt;/p&gt;&lt;p&gt;- Repeat the above step to then go to: Dragon cliffs (X/Y): 192/176 to get the Blacksmith’s book for the same bonuses towards Armour Crafting.&lt;/p&gt;&lt;p&gt;Both of these can be upgraded later on when we have access to Labyrinth. There are some One off &lt;a href="/information/quests" target="_blank"&gt;quests&lt;/a&gt; that will upgrade these.&lt;/p&gt;&lt;p&gt;- Now lets craft, first set up exploration for an hour or two – or what ever you feel like doing, Exploration will run while logged out. Remember to set it up with a monster you can kill in one hit.&lt;/p&gt;&lt;p&gt;- Close exploration, select Craft from the drop down and then select Craft from the Craft/Enchant&lt;/p&gt;&lt;p&gt;- Select Weapons, Broken Dagger – Click craft.&lt;/p&gt;&lt;p&gt;- When ready, click Change Type, select Armour, select an Armour to craft and click craft.&lt;/p&gt;&lt;p&gt;Over time new items will be added to the list. That’s all there is to it. When you are ready, click Change Type, select Armour, pick an item to craft and repeat.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Weapon Crafting</t>
@@ -248,7 +248,7 @@
     <t>You have been on another planes, a plane full of ruins, broken pieces of multiple labyrinths. The entire plane was covered with them.&lt;br /&gt; &lt;br /&gt; As you recover from your travels, slaughtering a whole new group of fearsome creatures, gaining notoriety with the inhabitants of said plane.&lt;br /&gt; &lt;br /&gt; Still no sign of the Enchantress and no sign of The Guide. You take a moment to relax before your next adventure.&lt;br /&gt; &lt;br /&gt; As you rise to the new dawn of a new day you have a knock at the door. You rise and greet the stranger. The Enchantress walks in. Today she wares a red robe and you can see deep into her blue eyes.&lt;br /&gt; &lt;br /&gt; “My darling child, I hear you have been adventuring. Shall we pick up where we left off? The art of enchanting.”&lt;br /&gt; &lt;br /&gt; You tell her you have plenty of enchanted gear.&lt;br /&gt; &lt;br /&gt; “Wouldn’t you like better gear? Stronger gear?”</t>
   </si>
   <si>
-    <t>&lt;p&gt;Today's lesson is about &lt;a href="/information/enchanting" target="_blank"&gt;enchanting&lt;/a&gt; and &lt;a href="/information/disenchanting" target="_blank"&gt;disenchanting&lt;/a&gt;. Just like crafting, enchanting is wildly important. As you may know, you cannot buy enchanted gear from the shop. Some players will sell it on the &lt;a href="/information/market-board" target="_blank"&gt;market place&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;More importantly, you want a &lt;a href="/information/currencies" target="_blank"&gt;currency&lt;/a&gt; you can get from it: Gold Dust. This currency is used in a lot of quests we are going to start doing soon. So lets get a lot of it.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop/Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;To enchant, from the crafting drop down select enchant.&lt;/p&gt;&lt;p&gt;- Here you have an item to select, a suffix and a prefix to select. The cost of enchanting can get widely expensive so exploration is required. Since you need items: weapons, Armour, spells and Rings, you will also want to be crafting. You can also re-enchant enchanted items but that gets more costly.&lt;/p&gt;&lt;p&gt;You can also just go to the shop and buy multiple items to enchant, like broken daggers.&lt;/p&gt;&lt;p&gt;- Next, when you have enchanted, ideally 75 items, next go to your inventory&lt;/p&gt;&lt;p&gt;- From the actions on the inventory section of your character sheet, click Disenchant All.&lt;/p&gt;&lt;p&gt;- This will raise your disenchanting skill, and slowly over time your enchanting skill as well.&lt;/p&gt;&lt;p&gt;- Repeat till you meet the quest requirements.&lt;/p&gt;&lt;p&gt;The &lt;strong&gt;Skill Type Crafting to level 10&lt;/strong&gt; basically means, level any rafting skill you want to level 10 or higher.&lt;/p&gt;</t>
+    <t>&lt;p&gt;Today's lesson is about &lt;a href="/information/enchanting" target="_blank"&gt;enchanting&lt;/a&gt; and &lt;a href="/information/disenchanting" target="_blank"&gt;disenchanting&lt;/a&gt;. Just like crafting, enchanting is wildly important. As you may know, you cannot buy enchanted gear from the shop. Some players will sell it on the &lt;a href="/information/market-board" target="_blank"&gt;market place&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;More importantly, you want a &lt;a href="/information/currencies" target="_blank"&gt;currency&lt;/a&gt; you can get from it: Gold Dust. This currency is used in a lot of quests we are going to start doing soon. So lets get a lot of it.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Remember to keep enchanting and disenchanting items. A later quest will be less painful.&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop/Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;To enchant, from the crafting drop down select enchant.&lt;/p&gt;&lt;p&gt;- Here you have an item to select, a suffix and a prefix to select. The cost of enchanting can get widely expensive so exploration is required. Since you need items: weapons, Armour, spells and Rings, you will also want to be crafting. You can also re-enchant enchanted items but that gets more costly.&lt;/p&gt;&lt;p&gt;You can also just go to the shop and buy multiple items to enchant, like broken daggers.&lt;/p&gt;&lt;p&gt;- Next, when you have enchanted, ideally 75 items, next go to your inventory&lt;/p&gt;&lt;p&gt;- From the actions on the inventory section of your character sheet, click Disenchant All.&lt;/p&gt;&lt;p&gt;- This will raise your disenchanting skill, and slowly over time your enchanting skill as well.&lt;/p&gt;&lt;p&gt;- Repeat till you meet the quest requirements.&lt;/p&gt;&lt;p&gt;The &lt;strong&gt;Skill Type Crafting to level 10&lt;/strong&gt; basically means, level any rafting skill you want to level 10 or higher.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Enchanting</t>
@@ -287,13 +287,13 @@
     <t>The Dungeons plane crawls with death. There is a darkness that seeps across the ground, infecting and infesting everything that it touches. You seem to be immune to it. You know there is shadow in the distance that is watching you. A shade like creature that only makes it’s self visible every now and then to your eyes.&lt;br /&gt; &lt;br /&gt; “Child!” Comes a familiar voice. The Guide, young, handsome and every changing comes up to you.&lt;br /&gt; &lt;br /&gt; “You have come down the Dungeons. A place of ruins, crypts, caves and other bits of darkness that one can explore for loot.”&lt;br /&gt; &lt;br /&gt; You ask him about the darkness crawling across the land and the shade like creature you can see off in the distance.&lt;br /&gt; &lt;br /&gt; “The darkness is caused by the gates of Shadow Planes, which has opened. The shade creature is the Shade Lord. He is seeking something, something that escaped the darkness beneath the pits of Hell. Alas to take on any of these creatures you need to get stronger!”</t>
   </si>
   <si>
-    <t>&lt;p&gt;Now we learn about a new feature: &lt;a href="/information/class-skills" target="_blank"&gt;Class Skills&lt;/a&gt; and Class Bonus.&lt;/p&gt;&lt;p&gt;Class Skills are different for each &lt;a href="/information/races-and-classes#3" target="_blank"&gt;class&lt;/a&gt; in the game. Every class has a skill which you can see on your skills table under Training Tab. It has an icon beside it and is in orange text.&lt;/p&gt;&lt;p&gt;This skill important to level because it allows you to increase your Class Bonus which can be seen on the character sheet to the left, under inventory count or on mobile under Class Details, at the bottom of the details section.&lt;/p&gt;&lt;p&gt;Every class has a special attack that fires automatically based on Three Things:&lt;/p&gt;&lt;p&gt;- Class Bonus % (the higher, the more chance for the special to fire)&lt;/p&gt;&lt;p&gt;- Weapons&lt;/p&gt;&lt;p&gt;- Attack type&lt;/p&gt;&lt;p&gt;\For example, Heretics:&lt;/p&gt;&lt;p&gt;With a damage spell equipped you have a small chance to cast another spell. Enemies cannot avoid this.&lt;/p&gt;&lt;p&gt;This means while casting and with at least one damage spell, based on the % of your class bonus you can cast another spell, automatically. Each class has its own special which you can read about in the help docs for your specific class.&lt;/p&gt;&lt;p&gt;To do this:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop/Mobile&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- The instructions state to level a Effects Class to the specified level. To do this, go to your character sheet section, in your skill section – train the skill with the orange text to the specified level.&lt;/p&gt;&lt;p&gt;- To Get the Gold Dust you can disenchant items that drop you no longer need, or craft some items, enchant them and disenchant them. Now is the time to explore the &lt;a href="/information/enchanting" target="_blank"&gt;Enchanting&lt;/a&gt; list in the docs to see what types of enchantments you can apply to your equipment so you can start creating a gear set geared towards your needs.&lt;/p&gt;&lt;p&gt;That’s it. Now you might not see your class bonus fire off much at first, but over time, keep leveling this skill and you will start to see your special fire off automatically when manually fighting.&lt;/p&gt;</t>
+    <t>&lt;p&gt;Now we learn about a new feature: &lt;a href="/information/class-skills" target="_blank"&gt;Class Skills&lt;/a&gt; and Class Bonus.&lt;/p&gt;&lt;p&gt;Class Skills are different for each &lt;a href="/information/races-and-classes#3" target="_blank"&gt;class&lt;/a&gt; in the game. Every class has a skill which you can see on your skills table under Training Tab. It has an icon beside it and is in orange text.&lt;/p&gt;&lt;p&gt;This skill important to level because it allows you to increase your Class Bonus which can be seen on the character sheet to the left, under inventory count or on mobile under Class Details, at the bottom of the details section.&lt;/p&gt;&lt;p&gt;Every class has a special attack that fires automatically based on Three Things:&lt;/p&gt;&lt;p&gt;- Class Bonus % (the higher, the more chance for the special to fire)&lt;/p&gt;&lt;p&gt;- Weapons&lt;/p&gt;&lt;p&gt;- Attack type&lt;/p&gt;&lt;p&gt;To do this:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop/Mobile&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- The instructions state to level a Effects Class to the specified level. To do this, go to your character sheet section, in your skill section – train the skill with the orange text to the specified level.&lt;/p&gt;&lt;p&gt;- To Get the Gold Dust you can disenchant items that drop you no longer need, or craft some items, enchant them and disenchant them. Now is the time to explore the &lt;a href="/information/enchanting" target="_blank"&gt;Enchanting&lt;/a&gt; list in the docs to see what types of enchantments you can apply to your equipment so you can start creating a gear set geared towards your needs.&lt;/p&gt;&lt;p&gt;That’s it. Now you might not see your class bonus fire off much at first, but over time, keep leveling this skill and you will start to see your special fire off automatically when manually fighting.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Mercenary for hire</t>
   </si>
   <si>
-    <t>You managed to survive long enough to drag your broken, bruised and bloody body back to the surface. You stop at an abandoned farm to mend your wounds and rest after such excursions.&lt;br /&gt; &lt;br /&gt; The farm looks familiar, but the names of the people that lived here has escaped your mind. You pay it no heed as you spend your time at this farm.&lt;br /&gt; &lt;br /&gt; A knock at the door, you open it and there stand The Poet.&lt;br /&gt; &lt;br /&gt; “Hello child.” He pushes past you and lets him self in.&lt;br /&gt; &lt;br /&gt; “You came back here.” he states.&lt;br /&gt; &lt;br /&gt; You look at him, confused.&lt;br /&gt; &lt;br /&gt; “Do you not know where you are child? You are home.”&lt;br /&gt; &lt;br /&gt; It comes back to you, your home. Abandoned. No parent, no one. Where did they go? You ask The poet in a rush, frantic and worried about your parents.&lt;br /&gt; &lt;br /&gt; “Child. Calm your self. They are here, some where. You’ll have to find them eventually.”&lt;br /&gt; &lt;br /&gt; Find them? What has he done with them? You start to get angry but The Port waves his hand and calmness washes over you.&lt;br /&gt; &lt;br /&gt; “For now I need you to head down to Labyrinth and complete some tasks to unlock Mercenaries. They can help you with getting shiny coins, dust and shards and later on some Copper.”&lt;br /&gt; &lt;br /&gt; My parents, where are they?&lt;br /&gt; &lt;br /&gt; “They are not where you think, they are not whom you think. I have lifted the spell that you lived with for so long. Do this, and I will tell you more.”&lt;br /&gt; &lt;br /&gt; He refuses to discuss the matter anymore.</t>
+    <t>You managed to survive long enough to drag your broken, bruised and bloody body back to the surface. You stop at an abandoned farm to mend your wounds and rest after such excursions.&lt;br /&gt; &lt;br /&gt; The farm looks familiar, but the names of the people that lived here has escaped your mind. You pay it no heed as you spend your time at this farm.&lt;br /&gt; &lt;br /&gt; A knock at the door, you open it and there stand The Poet.&lt;br /&gt; &lt;br /&gt; “Hello child.” He pushes past you and lets him self in.&lt;br /&gt; &lt;br /&gt; “You came back here.” he states.&lt;br /&gt; &lt;br /&gt; You look at him, confused.&lt;br /&gt; &lt;br /&gt; “Do you not know where you are child? You are home.”&lt;br /&gt; &lt;br /&gt; It comes back to you, your home. Abandoned. No parent, no one. Where did they go? You ask The Poet in a rush, frantic and worried about your parents.&lt;br /&gt; &lt;br /&gt; “Child. Calm your self. They are here, somewhere. You’ll have to find them eventually.”&lt;br /&gt; &lt;br /&gt; Find them? What has he done with them? You start to get angry but The Poet waves his hand and calmness washes over you.&lt;br /&gt; &lt;br /&gt; “For now I need you to head down to Labyrinth and complete some tasks to unlock Mercenaries. They can help you with getting shiny coins, dust and shards and later on some Copper.”&lt;br /&gt; &lt;br /&gt; My parents, where are they?&lt;br /&gt; &lt;br /&gt; “They are not where you think, they are not whom you think. I have lifted the spell that you lived with for so long. Do this, and I will tell you more.”&lt;br /&gt; &lt;br /&gt; He refuses to discuss the matter anymore.</t>
   </si>
   <si>
     <t>&lt;p&gt;Lets learn about &lt;a href="/information/currencies" target="_blank"&gt;currencies&lt;/a&gt;. You know about Gold Dust – that it can be used in quests and Alchemy.&lt;/p&gt;&lt;p&gt;You also know about Gold, the core currency. Shards and Copper Coins are another two types of currencies. Both can be earned from a feature called &lt;a href="/information/slots" target="_blank"&gt;Slots&lt;/a&gt;. However, there is a way to cheat the system and that’s to level &lt;a href="/information/mercenary" target="_blank"&gt;Mercenaries&lt;/a&gt;. You will need to complete a quest in Labyrinth. You can see this by going to the quests tab and selecting Labyrinth from the Planes drop down. Look for the quest: &lt;strong&gt;&lt;u&gt;Powers of The Children&lt;/u&gt;&lt;/strong&gt; to the right.&lt;/p&gt;&lt;p&gt;You can also see these quests if you traverse down to Labyrinth and then select the Quests tab.&lt;/p&gt;&lt;p&gt;Complete this quest to unlock a new feature called Mercenaries, who as they are leveled up will help you with getting more and more currencies from Slots and Farming creatures.&lt;/p&gt;&lt;p&gt;You can see these mercenaries who you must purchase by going to your character sheet and tapping/clicking the tab: Mercenaries. You can purchase them after completing the quest line above.&lt;/p&gt;&lt;p&gt;As you level these Mercenaries, you will eventually be able to reincarnate them – at their max level – and re-level them up to get even more % bonus towards currency drops. Some currencies such as Copper Coins only drop on a specific plane called Purgatory which you are not strong enough for yet, thus Slots will not drop them as you are missing an item to get into Purgatory.&lt;/p&gt;&lt;p&gt;For now, lets focus on Gold Dust and Shards, which you can do through Slots:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- In the actions section click Slots.&lt;/p&gt;&lt;p&gt;- Play slots or, if you cannot afford slots, kill monsters to get the currency requirements of this quest.&lt;/p&gt;&lt;p&gt;- Level a specific mercenary to the required level by killing creatures.&lt;/p&gt;&lt;p&gt;You can craft and play slots and explore at the same time. Which will be needed for this particular quest.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile&lt;/strong&gt;:&lt;/p&gt;&lt;p&gt;- In the actions section select Slots from the action drop down.&lt;/p&gt;&lt;p&gt;- Play slots or, if you cannot afford slots, kill monsters to get the currency requirements of this quest.&lt;/p&gt;&lt;p&gt;- Level a specific mercenary to the required level by killing creatures.&lt;/p&gt;&lt;p&gt;You can only do one action at a time on mobile, for example craft or play slots while exploration is running.&lt;/p&gt;</t>
@@ -303,6 +303,9 @@
   </si>
   <si>
     <t>child-of-shards</t>
+  </si>
+  <si>
+    <t>The truth is out there</t>
   </si>
   <si>
     <t>A place to call home</t>
@@ -1190,9 +1193,6 @@
       <c r="G10">
         <v>50</v>
       </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
       <c r="S10" t="s">
         <v>84</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>87</v>
       </c>
       <c r="AE10">
-        <v>500</v>
+        <v>350</v>
       </c>
       <c r="AO10">
         <v>250000</v>
@@ -1229,16 +1229,16 @@
         <v>90</v>
       </c>
       <c r="E11">
-        <v>350</v>
+        <v>250</v>
       </c>
       <c r="J11">
         <v>13</v>
       </c>
       <c r="K11">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="AE11">
-        <v>600</v>
+        <v>450</v>
       </c>
       <c r="AM11">
         <v>10000</v>
@@ -1281,6 +1281,9 @@
       <c r="O12">
         <v>1</v>
       </c>
+      <c r="T12" t="s">
+        <v>96</v>
+      </c>
       <c r="AE12">
         <v>800</v>
       </c>
@@ -1302,13 +1305,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C13" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D13" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="Z13">
         <v>1</v>
@@ -1331,13 +1334,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C14" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AA14">
         <v>10</v>
@@ -1346,7 +1349,7 @@
         <v>200</v>
       </c>
       <c r="AC14" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AO14">
         <v>2500</v>
@@ -1360,13 +1363,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="P15">
         <v>2</v>
@@ -1383,13 +1386,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C16" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D16" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E16">
         <v>500</v>
@@ -1407,10 +1410,10 @@
         <v>50</v>
       </c>
       <c r="T16" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="U16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AM16">
         <v>5000</v>

</xml_diff>

<commit_message>
updated guide quests import
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -1267,7 +1267,7 @@
         <v>93</v>
       </c>
       <c r="E12">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="L12" t="s">
         <v>94</v>
@@ -1276,16 +1276,16 @@
         <v>95</v>
       </c>
       <c r="N12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T12" t="s">
         <v>96</v>
       </c>
       <c r="AE12">
-        <v>800</v>
+        <v>550</v>
       </c>
       <c r="AM12">
         <v>1000</v>

</xml_diff>

<commit_message>
Various fixes and even more guide quests have been addded.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="139">
   <si>
     <t>id</t>
   </si>
@@ -311,10 +311,10 @@
     <t>A place to call home</t>
   </si>
   <si>
-    <t>You are exhausted, emotionally, mentally and physically. You fight, you kill, you train, you craft and enchant. You sit under a tree with a small fire burning as the moon rises high in the night sky. You notice how bright, how clear, how large the moon is in the night sky.&lt;br /&gt; &lt;br /&gt; As you sit and mull over the last few months, your mind wonders back to what The Poet stated, about the abandoned house, your house, your family house.&lt;br /&gt; &lt;br /&gt; Are they dead? Are they alive? Where are they? Winy did they leave the farm? So many questions, yet no answers.&lt;br /&gt; &lt;br /&gt; A slight breeze kicks up and the flames flicker and dance in the night.&lt;br /&gt; &lt;br /&gt; A voice comes from the shadows of the night, beyond the flames light and reach.&lt;br /&gt; &lt;br /&gt; “Child, I am back.” Comes the voice of The Guide.&lt;br /&gt; &lt;br /&gt; You look up from your fire and see The Guide, he is young again, keeps changing between young and old. Alas he looks bruised, broken and is limping.&lt;br /&gt; &lt;br /&gt; You ask him what happened but he shrugs it off. “it is not important. What is though is that you put your feet up. Gather some soldiers, build some walls, create a home for your self.”&lt;br /&gt; &lt;br /&gt; You tell him what The Poet said about your parents.&lt;br /&gt; &lt;br /&gt; “Silly child, there is so much for you to learn. Alas for now, Lets get you to settle down and call some place home.”&lt;br /&gt; &lt;br /&gt; You insist he explains more, but he refuse’s and starts to get angry at your demands.&lt;br /&gt; &lt;br /&gt; “Now you listen here, there is a darkness descending on this world, one escaping the pits of hell, some of it I am sure you have learned about, others you don’t know yet, but soon will. All will be answered in time. But for now, you have a job to do.”&lt;br /&gt; &lt;br /&gt; You think for a moment of refusing until you get the answers, but a swath of land you can call your own does sound enticing.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Lets take a break from questing, crafting, enchanting and fighting and lets focus on kingdoms and what they can provide for you.&lt;/p&gt;&lt;p&gt;You can settle a &lt;a href="/information/kingdoms" target="_blank"&gt;kingdom&lt;/a&gt; for free once, assuming you have no kingdoms.&lt;/p&gt;&lt;p&gt;Each kingdom after the first one will cost 10,000 Gold x the amount of kingdoms you already own.&lt;/p&gt;&lt;p&gt;Your first kingdom, again assuming you have no kingdoms, will have a 7 day protection on it, meaning no one can attack it.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; the quest requires a kingdom level, this means you need you need to level the buildings, by resources or gold, over time to reach the required objective. You can level one building or multiple as the kingdom level is a sum of all the building levels in one kingdom.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;Find a place on either Surface, Labyrinth or Dungeons where you can access and what to settle a kingdom.&lt;/p&gt;&lt;p&gt;- Click Settle Kingdom under the map and give your kingdom a name.&lt;/p&gt;&lt;p&gt;- Now you can click on the Kingdoms tab and see your kingdom&lt;/p&gt;&lt;p&gt;- From there you can click on the kingdom name and see further details.&lt;/p&gt;&lt;p&gt;- On the map you will see an icon on the map that represents your kingdom and you can also click on that to get basic details as well as teleport to it, assuming you have the gold to teleport the distance.&lt;/p&gt;&lt;p&gt;- When you click on the kingdom via the kingdoms tab, you can see information like buildings and units as well as kingdom resources that will replenish over time, every hour.&lt;/p&gt;&lt;p&gt;- Lets recruit some units and upgrade our buildings which can be done with either resources, as stated, or gold. Both of which will require (real world) time to recruit the units and build the buildings.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;Find a place on either Surface, Labyrinth or Dungeons where you can access and what to settle a kingdom.&lt;/p&gt;&lt;p&gt;- In the Actions drop down, select Map Movement&lt;/p&gt;&lt;p&gt;- Tap Settle Kingdom under the map and give your kingdom a name.&lt;/p&gt;&lt;p&gt;- Now you can tap on the Kingdoms tab and see your kingdom&lt;/p&gt;&lt;p&gt;- From there you can tap on the kingdom name and see further details.&lt;/p&gt;&lt;p&gt;- On the map you will see your kingdom icon, but due to how the map works on mobile, you wont be able to tap on it for basic details unlike on desktop. How ever if you tap Teleport you can choose from a list of your kingdoms on that Plane to teleport to.&lt;/p&gt;&lt;p&gt;- When you tap on the kingdom via the kingdoms tab, you can see information like buildings and units as well as kingdom resources that will replenish over time, every hour.&lt;/p&gt;&lt;p&gt;- Lets recruit some units and upgrade our buildings which can be done with either resources, as stated, or gold. Both of which will require (real world) time to recruit the units and build the buildings.&lt;/p&gt;</t>
+    <t>You are exhausted, emotionally, mentally and physically. You fight, you kill, you train, you craft and enchant. You sit under a tree with a small fire burning as the moon rises high in the night sky. You notice how bright, how clear, how large the moon is in the night sky.&lt;br /&gt; &lt;br /&gt; As you sit and mull over the last few months, your mind wonders back to what The Poet stated, about the abandoned house, your house, your family house.&lt;br /&gt; &lt;br /&gt; Are they dead? Are they alive? Where are they? Why did they leave the farm? So many questions, yet no answers.&lt;br /&gt; &lt;br /&gt; A slight breeze kicks up and the flames flicker and dance in the night.&lt;br /&gt; &lt;br /&gt; A voice comes from the shadows of the night, beyond the flames light and reach.&lt;br /&gt; &lt;br /&gt; “Child, I am back.” The Guide steps from the shadows.&lt;br /&gt; &lt;br /&gt; You look up from your fire and see that he is young again, keeps changing between young and old. Alas he looks bruised, broken and is limping.&lt;br /&gt; &lt;br /&gt; You ask him what happened but he shrugs it off. “It is not important. What is though is that you put your feet up. Gather some soldiers, build some walls, create a home for your self.”&lt;br /&gt; &lt;br /&gt; You tell him what The Poet said about your parents.&lt;br /&gt; &lt;br /&gt; “Silly child, there is so much for you to learn. Alas for now, Lets get you to settle down and call some place home.”&lt;br /&gt; &lt;br /&gt; You insist he explains more, but he refuse’s and starts to get angry at your demands.&lt;br /&gt; &lt;br /&gt; “Now you listen here, there is a darkness descending on this world, one escaping the pits of hell, some of it I am sure you have learned about, others you don’t know yet, but soon will. All will be answered in time. But for now, you have a job to do.”&lt;br /&gt; &lt;br /&gt; You think for a moment of refusing until you get the answers, but a swath of land you can call your own does sound enticing.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Lets take a break from questing, crafting, enchanting and fighting and lets focus on kingdoms and what they can provide for you.&lt;/p&gt;&lt;p&gt;You can settle a &lt;a href="/information/kingdoms" target="_blank"&gt;kingdom&lt;/a&gt; for free once, assuming you have no kingdoms.&lt;/p&gt;&lt;p&gt;Each kingdom after the first one will cost 10,000 Gold x the amount of kingdoms you already own.&lt;/p&gt;&lt;p&gt;Your first kingdom, again assuming you have no kingdoms, will have a 7 day protection on it, meaning no one can attack it.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; the quest requires a kingdom level, this means you need you need to level the buildings, by resources or gold, over time to reach the required objective. You can level one building or multiple as the kingdom level is a sum of all the building levels in one kingdom.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Note: The quest requires you to purchase with gold or resources units. If you purchased your buildings (2 at level 10) to will notice that you have no population. On the right hand side under Kingdom Actions for desktop or under kingdoms details for mobile, you will find a Buy Population button that lets you buy people for gold. Caution as to not exceed the max amount of population your kingdom can have or an angry NPC might come knocking.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Final Note: Kingdom resource replenishment and treasury interest for deposited gold occurs every hour and can be seen in the Server Message section if you go to your &lt;/strong&gt;&lt;a href="//information/settings" target="_blank"&gt;&lt;strong&gt;settings&lt;/strong&gt;&lt;/a&gt;&lt;strong&gt; and enable the messages if they wish. &lt;em&gt;This can get quite spammy so it is disabled by default.&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;Find a place on either Surface, Labyrinth or Dungeons where you can access and what to settle a kingdom.&lt;/p&gt;&lt;p&gt;- Click Settle Kingdom under the map and give your kingdom a name.&lt;/p&gt;&lt;p&gt;- Now you can click on the Kingdoms tab and see your kingdom&lt;/p&gt;&lt;p&gt;- From there you can click on the kingdom name and see further details.&lt;/p&gt;&lt;p&gt;- On the map you will see an icon on the map that represents your kingdom and you can also click on that to get basic details as well as teleport to it, assuming you have the gold to teleport the distance.&lt;/p&gt;&lt;p&gt;- When you click on the kingdom via the kingdoms tab, you can see information like buildings and units as well as kingdom resources that will replenish over time, every hour.&lt;/p&gt;&lt;p&gt;- Lets recruit some units and upgrade our buildings which can be done with either resources, as stated, or gold. Both of which will require (real world) time to recruit the units and build the buildings.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;Find a place on either Surface, Labyrinth or Dungeons where you can access and what to settle a kingdom.&lt;/p&gt;&lt;p&gt;- In the Actions drop down, select Map Movement&lt;/p&gt;&lt;p&gt;- Tap Settle Kingdom under the map and give your kingdom a name.&lt;/p&gt;&lt;p&gt;- Now you can tap on the Kingdoms tab and see your kingdom&lt;/p&gt;&lt;p&gt;- From there you can tap on the kingdom name and see further details.&lt;/p&gt;&lt;p&gt;- On the map you will see your kingdom icon, but due to how the map works on mobile, you wont be able to tap on it for basic details unlike on desktop. How ever if you tap Teleport you can choose from a list of your kingdoms on that Plane to teleport to.&lt;/p&gt;&lt;p&gt;- When you tap on the kingdom via the kingdoms tab, you can see information like buildings and units as well as kingdom resources that will replenish over time, every hour.&lt;/p&gt;&lt;p&gt;- Lets recruit some units and upgrade our buildings which can be done with either resources, as stated, or gold. Both of which will require (real world) time to recruit the units and build the buildings.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Growing the population</t>
@@ -351,6 +351,87 @@
   </si>
   <si>
     <t>Dead King's Crown</t>
+  </si>
+  <si>
+    <t>Discovering the truth pt. 1</t>
+  </si>
+  <si>
+    <t>You manage to awaken from your dreams, dreams of the void. Dreams of the nothingness that haunts your mind. Haunts you in a way where you question your own existence. One that isn’t even yours, if you understood correctly.&lt;br /&gt; &lt;br /&gt; You leave the room of your INN and head down stairs to the bar area for the food. There is a message for you, left by The Guide. The Barmaid hands you the note as she brings over your food.&lt;br /&gt; &lt;br /&gt; “Child” The letter starts.&lt;br /&gt; &lt;br /&gt; “I have found answers to your questions, and solutions to our current predicament with The Creator. Alas I need you to get much, much stronger – to do this, lets trade in some books and visit a friendly goblin. By the time you are done, I shall be back.&lt;br /&gt; &lt;br /&gt; Signed,&lt;br /&gt; &lt;br /&gt; Guide.”&lt;br /&gt; &lt;br /&gt; Goblin? I have to speak to one of those foul creatures?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Lets start diving into the game now that we have some of the basics under our belt, lets visit the goblin for some quests.&lt;/p&gt;&lt;p&gt;Go to surface and under the Quests tab you will see - to the right, a quest called Goblins Lust for Gold. This is the story of the goblin as well as some story around The Creator for more context.&lt;/p&gt;&lt;p&gt;This should be an easy quest to do.&lt;/p&gt;&lt;p&gt;The item you get from the quest, will give additional faction points per kill, this will help you with other quests in the game where specific faction levels are a requirement.&lt;/p&gt;&lt;p&gt;&lt;em&gt;Note: The Creator is not the developer of the game, this is an in game NPC&lt;/em&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Faction Hunter</t>
+  </si>
+  <si>
+    <t>Weaponsmith's Master Book</t>
+  </si>
+  <si>
+    <t>Blacksmith's Master Recipes</t>
+  </si>
+  <si>
+    <t>Discovering the truth pt. 2</t>
+  </si>
+  <si>
+    <t>You spoke with The Goblin and completed some tasks for some rewards. Alas you return to the INN with a new set of books and The Guide is not here.&lt;br /&gt; &lt;br /&gt; You wait well into the night, and he still doesn’t show.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Might as well head back to that goblin.&lt;/p&gt;&lt;p&gt;The item you get from this quest chain will help you not only hit better, much much better, but also gain levels - which will make the skill requirement easier.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Goblins Accuracy</t>
+  </si>
+  <si>
+    <t>Discovering the truth pt. 3</t>
+  </si>
+  <si>
+    <t>You decided to check in on that stretch of land you call your home. Your advisors have told you about a ring in which The Goblin might be willing to trade with you.&lt;br /&gt; &lt;br /&gt; You inquire more about it and they tell you about how your ability to be a king (or queen) is shown through your kingmanship.&lt;br /&gt; &lt;br /&gt; You head out to investigate, all while handling a few bits and bobs around the kingdom.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;One of your training skills is called Kingmanship, which helps in recruiting larger amounts of units and reducing time around both recruiting and upgrading as well as the cost.&lt;/p&gt;&lt;p&gt;The Goblin has a fun item for you to help level this skill.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Kingmanship</t>
+  </si>
+  <si>
+    <t>Leading Armies</t>
+  </si>
+  <si>
+    <t>Discovering the truth pt. 4</t>
+  </si>
+  <si>
+    <t>You have been speaking with the local Blacksmith of the little village you are building, when The Guide appears. You excuse your self from the conversation and walk off to the side with The Guide.&lt;br /&gt; &lt;br /&gt; “You have a nice little hamlet here.” he states.&lt;br /&gt; &lt;br /&gt; You ask him, with hushed and angry tones where the hell he has been.&lt;br /&gt; &lt;br /&gt; “I have been to the land where the Shade Lord calls home. The Shadow Planes.”&lt;br /&gt; &lt;br /&gt; What could possibly be down there?&lt;br /&gt; &lt;br /&gt; “There is rumors of a cloak that makes it’s wearer invisible.”&lt;br /&gt; &lt;br /&gt; You ask him if you are to fetch it for him and he shakes his head and starts to laugh.&lt;br /&gt; &lt;br /&gt; “Child you still depend on the shop for all your shabby gear. You need much more powerful gear.” He walks off and you follow him.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;I really hope you have been crafting this whole time like I told you to be long ago. This is the painful quest if you haven’t been.&lt;/p&gt;&lt;p&gt;The reason the levels are selected is because, you will unlock the first item – of many – that cannot be bought in the shop.&lt;/p&gt;&lt;p&gt;The books we got you, a couple quests back, will help a bit. If you have been enchanting, then search for weapon/armor crafting and create your first &lt;a href="/information/equipment-sets" target="_blank"&gt;set&lt;/a&gt; of armor crafting and weapon crafting enchantments to make it even easier and faster.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Hint, I pray you have been enchanting as well child ...&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Surface</t>
+  </si>
+  <si>
+    <t>Discovering the truth pt. 5</t>
+  </si>
+  <si>
+    <t>The Guide has been staying in your little village for the last couple weeks, while you work day and day, night after night – crafting and creating Armour and weapons that even the local merchants don’t sell.&lt;br /&gt; &lt;br /&gt; “Now, enchant it all.” The Guide states as you two are having dinner and discussing your latest accomplishments.&lt;br /&gt; &lt;br /&gt; “I would also pay attention to your kingdom.” He states before going back to his dinner. You stare at him with rage in your eyes.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Now its time to enchant – the better the enchant on the gear, the better chance you have to survive. There are &lt;a href="/information/enchanting?table[filters][types]=16" target="_blank"&gt;enchantments&lt;/a&gt; that can help with enchanting.&lt;/p&gt;&lt;p&gt;At this stage, you should have a grasp on the core concept of the game: Gear. The Better the gear you can craft, the better enchantment and mixture of enchantments that you apply to your gear all determines if you can kill a monster in one hit.&lt;/p&gt;&lt;p&gt;Soon you will be going to places where creatures are much harder, where your gear matters, where your skills need to be leveled up and where you should be experimenting with &lt;a href="/information/class-ranks" target="_blank"&gt;class ranks&lt;/a&gt;, mixing and matching different classes abilities together and leveling them up for even more power.&lt;/p&gt;&lt;p&gt;Keep crafting, keep enchanting and keep leveling and soon you can take on the first challenge before you:&lt;a href="/information/celestials" target="_blank"&gt; Celestial Entities&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Discovering the truth pt. 6</t>
+  </si>
+  <si>
+    <t>You have been telling your advisors on how you want to expand, when a merchants comes walking into the meeting room, completely uninvited.&lt;br /&gt; &lt;br /&gt; “Who are you?!” Exclaims one of the advisors.&lt;br /&gt; &lt;br /&gt; The guards bust in and attempt to grab the man who dodges their attempts.&lt;br /&gt; &lt;br /&gt; “I am the Merchant!” he exclaims. You wave your hand and your guards stand down.&lt;br /&gt; &lt;br /&gt; Your advisors attempt to interject but you refuse to listen and instead turn and as The Merchant who and why he is here.&lt;br /&gt; &lt;br /&gt; “I have come to teach you the story of the wondrous world of Alchemy. Alas you need something first. Now where is my room?”&lt;br /&gt; &lt;br /&gt; Alchemy? The Merchant? Like The Poet?&lt;br /&gt; &lt;br /&gt; “That’s right! Like The Poet!” he states in a happy boasted voice.&lt;br /&gt; &lt;br /&gt; What is going on.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;I want you to learn about Alchemy. &lt;a href="/information/alchemy" target="_blank"&gt;Alchemy&lt;/a&gt; is good for three things:&lt;/p&gt;&lt;p&gt;- Boons, which apply effects to your character for a limited amount of time but can greatly power your character.&lt;/p&gt;&lt;p&gt;- Kingdom Destroying Items that you can drop on other players kingdoms to deal large amounts of damage.&lt;/p&gt;&lt;p&gt;- Holy Oils, which you can apply to your gear later on, to give your self even more power.&lt;/p&gt;&lt;p&gt;You will need to complete a One Off quest on surface first to enable the new skill to appear in your craft/enchant section.&lt;/p&gt;&lt;p&gt;Once this is quest is done you will be able to select Alchemy and then select the item you want to craft.&lt;/p&gt;&lt;p&gt;Alchemy needs Gold Dust which you can get from disenchanting enchanted items. It also needs Shards, which an only be gotten from a location you cannot access yet or from fighting Celestials, which you are not strong enough for. Instead lets use what shards you do have to level Alchemy just a little bit.&lt;/p&gt;&lt;p&gt;Alchemy items can be seen in your inventory, under the Type Drop down called: Usable. These can be listed on the market or destroyed&lt;/p&gt;&lt;p&gt;We will come back to this skill later.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Alchemy</t>
+  </si>
+  <si>
+    <t>I dream of Alchemy</t>
   </si>
 </sst>
 </file>
@@ -690,7 +771,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AP16"/>
+  <dimension ref="A1:AP22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -700,8 +781,8 @@
   <cols>
     <col min="1" max="1" width="3.428" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="36.42" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="2197.749" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="4361.221" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="2194.179" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="4370.79" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="24.708" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="24.708" bestFit="true" customWidth="true" style="0"/>
@@ -718,8 +799,8 @@
     <col min="18" max="18" width="26.993" bestFit="true" customWidth="true" style="0"/>
     <col min="19" max="19" width="24.708" bestFit="true" customWidth="true" style="0"/>
     <col min="20" max="20" width="36.42" bestFit="true" customWidth="true" style="0"/>
-    <col min="21" max="21" width="26.993" bestFit="true" customWidth="true" style="0"/>
-    <col min="22" max="22" width="28.136" bestFit="true" customWidth="true" style="0"/>
+    <col min="21" max="21" width="30.564" bestFit="true" customWidth="true" style="0"/>
+    <col min="22" max="22" width="32.992" bestFit="true" customWidth="true" style="0"/>
     <col min="23" max="23" width="16.425" bestFit="true" customWidth="true" style="0"/>
     <col min="24" max="24" width="22.28" bestFit="true" customWidth="true" style="0"/>
     <col min="25" max="25" width="18.71" bestFit="true" customWidth="true" style="0"/>
@@ -1317,7 +1398,7 @@
         <v>1</v>
       </c>
       <c r="AA13">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AB13">
         <v>100</v>
@@ -1343,13 +1424,16 @@
         <v>102</v>
       </c>
       <c r="AA14">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="AB14">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="AC14" t="s">
         <v>103</v>
+      </c>
+      <c r="AD14">
+        <v>1</v>
       </c>
       <c r="AO14">
         <v>2500</v>
@@ -1425,6 +1509,216 @@
         <v>1000000</v>
       </c>
       <c r="AP16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" t="s">
+        <v>114</v>
+      </c>
+      <c r="T17" t="s">
+        <v>115</v>
+      </c>
+      <c r="U17" t="s">
+        <v>116</v>
+      </c>
+      <c r="V17" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO17">
+        <v>10000</v>
+      </c>
+      <c r="AP17">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:42">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F18" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18">
+        <v>100</v>
+      </c>
+      <c r="T18" t="s">
+        <v>121</v>
+      </c>
+      <c r="AO18">
+        <v>10000</v>
+      </c>
+      <c r="AP18">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" t="s">
+        <v>124</v>
+      </c>
+      <c r="F19" t="s">
+        <v>125</v>
+      </c>
+      <c r="G19">
+        <v>15</v>
+      </c>
+      <c r="T19" t="s">
+        <v>126</v>
+      </c>
+      <c r="AA19">
+        <v>80</v>
+      </c>
+      <c r="AB19">
+        <v>1000</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>103</v>
+      </c>
+      <c r="AD19">
+        <v>3</v>
+      </c>
+      <c r="AM19">
+        <v>1000</v>
+      </c>
+      <c r="AO19">
+        <v>50000</v>
+      </c>
+      <c r="AP19">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:42">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C20" t="s">
+        <v>128</v>
+      </c>
+      <c r="D20" t="s">
+        <v>129</v>
+      </c>
+      <c r="F20" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20">
+        <v>225</v>
+      </c>
+      <c r="H20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I20">
+        <v>294</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>130</v>
+      </c>
+      <c r="R20">
+        <v>5</v>
+      </c>
+      <c r="AO20">
+        <v>2000000000</v>
+      </c>
+      <c r="AP20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:42">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" t="s">
+        <v>132</v>
+      </c>
+      <c r="D21" t="s">
+        <v>133</v>
+      </c>
+      <c r="F21" t="s">
+        <v>78</v>
+      </c>
+      <c r="G21">
+        <v>200</v>
+      </c>
+      <c r="AO21">
+        <v>2000000000</v>
+      </c>
+      <c r="AP21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>134</v>
+      </c>
+      <c r="C22" t="s">
+        <v>135</v>
+      </c>
+      <c r="D22" t="s">
+        <v>136</v>
+      </c>
+      <c r="F22" t="s">
+        <v>137</v>
+      </c>
+      <c r="G22">
+        <v>5</v>
+      </c>
+      <c r="T22" t="s">
+        <v>138</v>
+      </c>
+      <c r="Z22">
+        <v>2</v>
+      </c>
+      <c r="AA22">
+        <v>150</v>
+      </c>
+      <c r="AB22">
+        <v>2000</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>103</v>
+      </c>
+      <c r="AD22">
+        <v>4</v>
+      </c>
+      <c r="AO22">
+        <v>1000000000</v>
+      </c>
+      <c r="AP22">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Started setting up aspects of generating alchemy items
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="139">
   <si>
     <t>id</t>
   </si>
@@ -407,22 +407,19 @@
     <t>You ask The Guide about your parents.&lt;br /&gt; &lt;br /&gt; “They, your parents, were The Child’s parents. They came to this world, this plane of existence from another world, another dimension – much like The Child.”&lt;br /&gt; &lt;br /&gt; Another world?&lt;br /&gt; &lt;br /&gt; “To be honest, another time – with in this world. A time of war and strife.”&lt;br /&gt; &lt;br /&gt; Another time?&lt;br /&gt; &lt;br /&gt; “Listen, I would love to chat about this all day and I know you have the questions the dive deep onto the bones of the world it’s self, alas you have to discover that for your self.”&lt;br /&gt; &lt;br /&gt; But you need to be stronger don’t you? You ask.&lt;br /&gt; &lt;br /&gt; “You can craft beyond the shop now child … “&lt;br /&gt; &lt;br /&gt; He’s not wrong.</t>
   </si>
   <si>
-    <t>&lt;p&gt;At this state, you should be able to craft gear above the shop - even with how expensive it is. You could be exploring and playing the slots to win more gold. As you level your mercenaries, you will gain more currencies when you win jackpots, and when you get currency drops in general.&lt;/p&gt;&lt;p&gt;Now you need to start crafting your self better gear and reading through the enchantment section, specifically the table, to build sets that not only do damage but also raise your stats. Clicking on your class name will tell you a bit about your class. experimenting with Affixes on your gear can make the difference in fighting harder creatures and surviving.&lt;/p&gt;&lt;p&gt;Here is a hint: A vampire wants life stealing and durability, while a heretic wants intelligence and base damage modifiers.&lt;/p&gt;&lt;p&gt;lets raise our stats shall we now that we can craft better gear.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Take a potion or two with you</t>
-  </si>
-  <si>
-    <t>“There is …. One more thing.”&lt;br /&gt; &lt;br /&gt; What now?&lt;br /&gt; &lt;br /&gt; “You might not yet be strong enough, what about some alchemy. You should have tones of Gold Dust by now child.”&lt;br /&gt; &lt;br /&gt; Alchemy? What’s that?&lt;br /&gt; &lt;br /&gt; “A way to create potions that give you strength, items you can use to deal damage to other kingdoms and oils to imbue your items with even more strength.”&lt;br /&gt; &lt;br /&gt; Sounds interesting. Lets investigate.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;I want you to learn about Alchemy. &lt;a href="/information/alchemy" target="_blank"&gt;Alchemy&lt;/a&gt; is good for three things:&lt;/p&gt;&lt;p&gt;- Boons, which apply effects to your character for a limited amount of time but can greatly power your character.&lt;/p&gt;&lt;p&gt;- Kingdom Destroying Items that you can drop on other players kingdoms to deal large amounts of damage.&lt;/p&gt;&lt;p&gt;- Holy Oils, which you can apply to your gear later on, to give your self even more power.&lt;/p&gt;&lt;p&gt;You will need to complete a One Off quest on surface first to enable the new skill to appear in your craft/enchant section.&lt;/p&gt;&lt;p&gt;Once this is quest is done you will be able to select Alchemy and then select the item you want to craft.&lt;/p&gt;&lt;p&gt;Alchemy needs Gold Dust which you can get from disenchanting enchanted items. It also needs Shards, which an only be gotten from a location you cannot access yet or from fighting Celestials, which you are not &lt;/p&gt;&lt;p&gt;strong enough for. Instead lets use what shards you do have to level Alchemy just a little bit.&lt;/p&gt;&lt;p&gt;Alchemy items can be seen in your inventory, under the Type Drop down called: Usable. These can be listed on the market or destroyed&lt;/p&gt;&lt;p&gt;We will come back to this skill later.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Alchemy</t>
-  </si>
-  <si>
-    <t>I dream of Alchemy</t>
+    <t>&lt;p&gt;At this state, you should be able to craft gear above the shop - even with how expensive it is. You could be exploring and playing the slots to win more gold. As you level your mercenaries, you will gain more currencies &lt;/p&gt;&lt;p&gt;when you win jackpots, and when you get currency drops in general.&lt;/p&gt;&lt;p&gt;Now you need to start crafting your self better gear and reading through the &lt;a href="/information/enchanting" target="_blank"&gt;enchantment&lt;/a&gt; section, specifically the table, to build sets that not only do damage but also raise your stats. Clicking on your class name will tell&lt;/p&gt;&lt;p&gt;you a bit about your class. experimenting with Affixes on your gear can make the difference in fighting harder creatures and surviving.&lt;/p&gt;&lt;p&gt;Let's raise our stats shall we now that we can craft better gear.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Note: &lt;/strong&gt;The easiest way to do this is to craft a full set of gear (including two rings and two spells) one or two levels beyond the shop and enchant them with the most powerful enchants you can afford that fit your class, for example Stat Modifier on every piece + one suffix that plays to your classes specialty. You will also need to level your character a bit to get the required stats.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Preparing for a celestial encounter</t>
+  </si>
+  <si>
+    <t>“Have you heard of the Celestial Goblin?” The Guide asks as he looks across the table at you. The pub is silent tonight, far from your kingdom.&lt;br /&gt; &lt;br /&gt; The two of you have been traveling, crafting, fighting and generally adventuring while you seek a way to lock away The Creator.&lt;br /&gt; &lt;br /&gt; It has weighed on you a bit about the fact that The Creator is searching for a way to get his love back.&lt;br /&gt; &lt;br /&gt; “Child are you listening?” The Guide asks as he stares at you with furrowed brows.&lt;br /&gt; &lt;br /&gt; “I was telling you about the Celestial Goblin that I wanted you to hunt down.”&lt;br /&gt; &lt;br /&gt; The what now? Another creature? Sounds easy enough.&lt;br /&gt; &lt;br /&gt; “Alas child, I need you to keep up on that crafting journey of yours and become MUCH stronger.”&lt;br /&gt; &lt;br /&gt; How much stronger? Why am I always getting stronger? Am I not strong enough? Am I going up against a god?&lt;br /&gt; &lt;br /&gt; The Guide smiles and lets out a bit of a laugh.&lt;br /&gt; &lt;br /&gt; “This world is full of pain and misery, full of hate and despair. This world requires you to always be getting strong child. Death comes for the weak, even those who are strong of muscle can be killed because they are weak of mind. Weak of heart. Weak of strength.”</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;I want you to start preparing for your first &lt;a href="/information/celestials" target="_blank"&gt;Celestial&lt;/a&gt;!&lt;/p&gt;&lt;p&gt;Before we can take ones of these fearsome beasts down, we need much better gear and enchantments. We need to be higher level and have higher stats.&lt;/p&gt;&lt;p&gt;This is where you can make use of the &lt;a href="/information/mercenary" target="_blank"&gt;Mercenaries&lt;/a&gt; and the bonuses they give you for playing the &lt;a href="/information/slots" target="_blank"&gt;slots&lt;/a&gt; and killing monsters.&lt;/p&gt;&lt;p&gt;Crafting and Enchanting at this point are wildly expensive, so exploration can help you get the gold you need with those sweet, sweet gold rushes.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;If you have not already, go ahead of purchase the Child of Gambling.&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>child-of-gambling</t>
   </si>
   <si>
     <t>Breaking the limits</t>
@@ -783,7 +780,7 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="3.428" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="36.42" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="42.418" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="2194.179" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="4370.79" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="17.567" bestFit="true" customWidth="true" style="0"/>
@@ -1654,7 +1651,7 @@
         <v>130</v>
       </c>
       <c r="AE21">
-        <v>2000</v>
+        <v>1100</v>
       </c>
       <c r="AM21">
         <v>10000</v>
@@ -1682,20 +1679,23 @@
       <c r="D22" t="s">
         <v>133</v>
       </c>
-      <c r="F22" t="s">
+      <c r="E22">
+        <v>400</v>
+      </c>
+      <c r="L22" t="s">
         <v>134</v>
       </c>
-      <c r="G22">
-        <v>5</v>
-      </c>
-      <c r="T22" t="s">
-        <v>135</v>
+      <c r="N22">
+        <v>10</v>
+      </c>
+      <c r="AE22">
+        <v>1500</v>
       </c>
       <c r="AM22">
-        <v>25000</v>
+        <v>2500</v>
       </c>
       <c r="AN22">
-        <v>5000</v>
+        <v>250</v>
       </c>
       <c r="AO22">
         <v>2000000000</v>
@@ -1709,16 +1709,16 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" t="s">
         <v>136</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>137</v>
       </c>
-      <c r="D23" t="s">
+      <c r="T23" t="s">
         <v>138</v>
-      </c>
-      <c r="T23" t="s">
-        <v>139</v>
       </c>
       <c r="AM23">
         <v>100000</v>

</xml_diff>

<commit_message>
Minor fixes and changes
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="133">
   <si>
     <t>id</t>
   </si>
@@ -158,7 +158,7 @@
     <t>You managed to slaughter the creatures and make your way forward to a small ramshackle town. The buildings are falling apart, the houses seem empty and lifeless. There is however a small INN before you, the roof looks like it could cave in at any moment. The lawn before it is overgrown with weeds and patches of dead grass where people and their pets have relieved themselves.&lt;br /&gt; &lt;br /&gt; You enter the INN and sit at an empty table by the fire. The barmaid, a heavy set women with an apron around her waist walks over and asks what she can get you. You tell her you are looking for a man who calls him self The Guide. She states she has never heard of such a person and tells you she will be back with the drink and food.&lt;br /&gt; &lt;br /&gt; You sit alone wondering what to do now.</t>
   </si>
   <si>
-    <t>&lt;p&gt;I want you to get to level 10. I do not want you to do this manually. Instead we are going to &lt;a href="/information/automation" target="_blank"&gt;explore&lt;/a&gt; for an hour. During this time you may gain a Faction level for Surface. The map you are currently on.&lt;/p&gt;&lt;p&gt;&lt;a href="/information/factions" target="_blank"&gt;Factions&lt;/a&gt; can be seen on your character sheet (tab) under the tab: Factions. As you kill creatures you gain faction points. As you level the faction, you can get what are called &lt;a href="/information/random-enchants" target="_blank"&gt;Unique’s&lt;/a&gt;. These can be powerful items and you may only have one equipped at a time.&lt;/p&gt;&lt;p&gt;To do this:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- First, find a monster in the drop down list you can kill in one hit.&lt;/p&gt;&lt;p&gt;- Next, click the Exploration green button.&lt;/p&gt;&lt;p&gt;- Select the monster you could kill, 1 hour, Attack.&lt;/p&gt;&lt;p&gt;- Click explore&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;Select the action Fight from the list of actions behind this modal.&lt;/p&gt;&lt;p&gt;- Find a monster you can kill in one shot.&lt;/p&gt;&lt;p&gt;- Next, close the fight section, select Exploration from the actions section&lt;/p&gt;&lt;p&gt;- Select the monster you could kill, 1 hour, 20 levels and Attack.&lt;/p&gt;&lt;p&gt;- Tap explore&lt;/p&gt;&lt;p&gt;Exploring will allow you to log out and idling gain items, exp, gold and possible quest item if the monster drops a quest item. There are things you cannot do while exploring such as change equipment, buy items from the &lt;a href="/information/shop" target="_blank"&gt;shop&lt;/a&gt; or &lt;a href="/information/market-board" target="_blank"&gt;market board&lt;/a&gt;. You will be told if you can do an action or not while exploring.&lt;/p&gt;&lt;p&gt;Exploration messages will appear, while logged in, in the Exploration chat tab below.&lt;/p&gt;</t>
+    <t>&lt;p&gt;I want you to get to level 10. I do not want you to do this manually. Instead we are going to &lt;a href="/information/automation" target="_blank"&gt;explore&lt;/a&gt; for an hour. During this time you may gain a Faction level for Surface. The map you are currently on.&lt;/p&gt;&lt;p&gt;&lt;a href="/information/factions" target="_blank"&gt;Factions&lt;/a&gt; can be seen on your character sheet (tab) under the tab: Factions. As you kill creatures you gain faction points. As you level the faction, you can get what are called &lt;a href="/information/random-enchants" target="_blank"&gt;Unique’s&lt;/a&gt;. These can be powerful items and you may only have one equipped at a time.&lt;/p&gt;&lt;p&gt;To do this:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Desktop:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- First, find a monster in the drop down list you can kill in one hit.&lt;/p&gt;&lt;p&gt;- You might want to buy more gear from the shop or better gear, to do this click the hamburger menu at the top left&lt;/p&gt;&lt;p&gt;- Click Shop, Under General Shop (Uses Gold), click Buy.&lt;/p&gt;&lt;p&gt;- Here you can buy better gear, eventually you can craft beyond this, how ever right now you might want to spend some of that pretty gold. You can even compare and buy and replace items. How neat!&lt;/p&gt;&lt;p&gt;- Next, click the Exploration green button (Back on the game page)&lt;/p&gt;&lt;p&gt;- Select the monster you could kill, 1 hour, Attack.&lt;/p&gt;&lt;p&gt;- Click explore&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Mobile:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;Select the action Fight from the list of actions behind this modal.&lt;/p&gt;&lt;p&gt;- Find a monster you can kill in one shot.&lt;/p&gt;&lt;p&gt;- You might want to buy more gear from the shop or better gear, to do this tap the hamburger menu at the top left&lt;/p&gt;&lt;p&gt;- Tap Shop, Under General Shop (Uses Gold), click Buy.&lt;/p&gt;&lt;p&gt;- Here you can buy better gear, eventually you can craft beyond this, how ever right now you might want to spend some of that pretty gold. You can even compare and buy and replace items. How neat!&lt;/p&gt;&lt;p&gt;- Next (Back on the game page), close the fight section, select Exploration from the actions section.&lt;/p&gt;&lt;p&gt;- Select the monster you could kill, 1 hour, 20 levels and Attack.&lt;/p&gt;&lt;p&gt;- Tap explore&lt;/p&gt;&lt;p&gt;Exploring will allow you to log out and idly gain items, exp, gold and possible quest item if the monster drops a quest item. There are things you cannot do while exploring such as change equipment, buy items from the &lt;a href="/information/shop" target="_blank"&gt;shop&lt;/a&gt; or &lt;a href="/information/market-board" target="_blank"&gt;market board&lt;/a&gt;. You will be told if you can do an action or not while exploring. Exploring should not just be used to level and log out, you &lt;a href="/information/some-clicking-required" target="_blank"&gt;won't get very far&lt;/a&gt; if you do that, there is much more to do and we will do it very soon! exploration is a way of gaining levels while doing other things in game.&lt;/p&gt;&lt;p&gt;Exploration messages will appear, while logged in, in the Exploration chat tab below.&lt;/p&gt;</t>
   </si>
   <si>
     <t>The Letter</t>
@@ -272,9 +272,6 @@
     <t>Dungeons</t>
   </si>
   <si>
-    <t>Light the way</t>
-  </si>
-  <si>
     <t>Torch</t>
   </si>
   <si>
@@ -305,9 +302,6 @@
     <t>child-of-shards</t>
   </si>
   <si>
-    <t>The truth is out there</t>
-  </si>
-  <si>
     <t>A place to call home</t>
   </si>
   <si>
@@ -347,9 +341,6 @@
     <t>&lt;p&gt;Today we want to learn about &lt;a href="/information/voidance" target="_blank"&gt;Devouring Light/Darkness&lt;/a&gt;. One lets you void your enemy so their enchantments do not fire and over all they do less damage.&lt;/p&gt;&lt;p&gt;The problem with that. Is that enemies can do the same to you. So to counter an enemy voiding you, making your character use only raw stats and no enchantments, you use whats called Devoid.&lt;/p&gt;&lt;p&gt;Devoid allows you to “Void the enemies ability to void your enchantments.” Which in turn allows the you to then: Void the enemy, so their enchantments do not fire.&lt;/p&gt;&lt;p&gt;On top of this there is also Resistance to both of these that character can obtain, so that you can resist the enemies ability to void you, even if you fail to “Devoid” them.&lt;/p&gt;&lt;p&gt;From Surface to Hell, you will devoid followed by a void first, where as in Purgatory Enemies will devoid followed by a void first, which is where the resistance comes in handy.&lt;/p&gt;&lt;p&gt;To get the Devouring Light/Darkness % up, which can be seen on The Character Sheet: Additional Information (Orange Button) → Voidance tab, you will have to complete the Quest, on Surface called: Return of the King’s Crown.&lt;/p&gt;&lt;p&gt;This will cost a lot of Gold Dust and the easiest way to get it, while you train Looting is to train Enchanting, enchant and then disenchant to gain gold dust.&lt;/p&gt;&lt;p&gt;The item you receive is called: Dead King's Crown. This allows you to gain 100% in Devouring Light (Voidance) and 85% in Devouring Darkness (DeVoid), which will make harder creatures much easier to take on.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>The Return of the King's Crown</t>
-  </si>
-  <si>
     <t>Dead King's Crown</t>
   </si>
   <si>
@@ -362,9 +353,6 @@
     <t>&lt;p&gt;Lets start diving into the game now that we have some of the basics under our belt, lets visit the goblin for some quests.&lt;/p&gt;&lt;p&gt;Go to surface and under the Quests tab you will see - to the right, a quest called Goblins Lust for Gold. This is the story of the goblin as well as some story around The Creator for more context.&lt;/p&gt;&lt;p&gt;This should be an easy quest to do.&lt;/p&gt;&lt;p&gt;The item you get from the quest, will give additional faction points per kill, this will help you with other quests in the game where specific faction levels are a requirement.&lt;/p&gt;&lt;p&gt;&lt;em&gt;Note: The Creator is not the developer of the game, this is an in game NPC&lt;/em&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>Faction Hunter</t>
-  </si>
-  <si>
     <t>Weaponsmith's Master Book</t>
   </si>
   <si>
@@ -380,9 +368,6 @@
     <t>&lt;p&gt;Might as well head back to that goblin.&lt;/p&gt;&lt;p&gt;The item you get from this quest chain will help you not only hit better, much much better, but also gain levels - which will make the skill requirement easier.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>Goblins Accuracy</t>
-  </si>
-  <si>
     <t>Discovering the truth pt. 3</t>
   </si>
   <si>
@@ -429,9 +414,6 @@
   </si>
   <si>
     <t>&lt;p&gt;All you have to do is complete the quest above, which is a One Off Quest on Labyrinth. You have been crafting, enchanting and using alchemy to make your self stronger. You will need that strength to get the reward of this quest which is a magical sash that allows you level beyond level 1,000 to the max 5,000.&lt;/p&gt;&lt;p&gt;Gear is how you progress, keep crafting, keep enchanting until you have maxed the skills and then craft your self a full suit of max level gear with powerful max level enchants on them. &lt;/p&gt;&lt;p&gt;&lt;strong&gt;The rest of the guide quests from here will have you unlock new planes, advance your class rank, level factions and your mercenaries as well delve more into kingdoms to unlock new features.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;This quest marks the end the basic tutorial on features.&lt;/strong&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Reach for the stars</t>
   </si>
 </sst>
 </file>
@@ -798,7 +780,7 @@
     <col min="17" max="17" width="23.423" bestFit="true" customWidth="true" style="0"/>
     <col min="18" max="18" width="26.993" bestFit="true" customWidth="true" style="0"/>
     <col min="19" max="19" width="24.708" bestFit="true" customWidth="true" style="0"/>
-    <col min="20" max="20" width="36.42" bestFit="true" customWidth="true" style="0"/>
+    <col min="20" max="20" width="21.138" bestFit="true" customWidth="true" style="0"/>
     <col min="21" max="21" width="30.564" bestFit="true" customWidth="true" style="0"/>
     <col min="22" max="22" width="32.992" bestFit="true" customWidth="true" style="0"/>
     <col min="23" max="23" width="16.425" bestFit="true" customWidth="true" style="0"/>
@@ -1174,12 +1156,6 @@
       <c r="G8">
         <v>25</v>
       </c>
-      <c r="Q8" t="s">
-        <v>73</v>
-      </c>
-      <c r="R8">
-        <v>1</v>
-      </c>
       <c r="S8" t="s">
         <v>73</v>
       </c>
@@ -1277,14 +1253,11 @@
       <c r="S10" t="s">
         <v>84</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
         <v>85</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" t="s">
         <v>86</v>
-      </c>
-      <c r="V10" t="s">
-        <v>87</v>
       </c>
       <c r="AE10">
         <v>350</v>
@@ -1301,13 +1274,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" t="s">
         <v>88</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>89</v>
-      </c>
-      <c r="D11" t="s">
-        <v>90</v>
       </c>
       <c r="E11">
         <v>250</v>
@@ -1339,31 +1312,28 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" t="s">
         <v>91</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>92</v>
-      </c>
-      <c r="D12" t="s">
-        <v>93</v>
       </c>
       <c r="E12">
         <v>300</v>
       </c>
       <c r="L12" t="s">
+        <v>93</v>
+      </c>
+      <c r="M12" t="s">
         <v>94</v>
-      </c>
-      <c r="M12" t="s">
-        <v>95</v>
       </c>
       <c r="N12">
         <v>2</v>
       </c>
       <c r="O12">
         <v>2</v>
-      </c>
-      <c r="T12" t="s">
-        <v>96</v>
       </c>
       <c r="AE12">
         <v>550</v>
@@ -1386,13 +1356,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" t="s">
         <v>97</v>
-      </c>
-      <c r="C13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D13" t="s">
-        <v>99</v>
       </c>
       <c r="Z13">
         <v>1</v>
@@ -1415,13 +1385,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" t="s">
         <v>100</v>
-      </c>
-      <c r="C14" t="s">
-        <v>101</v>
-      </c>
-      <c r="D14" t="s">
-        <v>102</v>
       </c>
       <c r="AA14">
         <v>40</v>
@@ -1430,7 +1400,7 @@
         <v>500</v>
       </c>
       <c r="AC14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="AD14">
         <v>1</v>
@@ -1447,13 +1417,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" t="s">
         <v>104</v>
-      </c>
-      <c r="C15" t="s">
-        <v>105</v>
-      </c>
-      <c r="D15" t="s">
-        <v>106</v>
       </c>
       <c r="P15">
         <v>2</v>
@@ -1470,13 +1440,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" t="s">
         <v>107</v>
-      </c>
-      <c r="C16" t="s">
-        <v>108</v>
-      </c>
-      <c r="D16" t="s">
-        <v>109</v>
       </c>
       <c r="F16" t="s">
         <v>52</v>
@@ -1490,11 +1460,8 @@
       <c r="I16">
         <v>50</v>
       </c>
-      <c r="T16" t="s">
-        <v>110</v>
-      </c>
       <c r="U16" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="AM16">
         <v>5000</v>
@@ -1514,22 +1481,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" t="s">
+        <v>111</v>
+      </c>
+      <c r="U17" t="s">
         <v>112</v>
       </c>
-      <c r="C17" t="s">
+      <c r="V17" t="s">
         <v>113</v>
-      </c>
-      <c r="D17" t="s">
-        <v>114</v>
-      </c>
-      <c r="T17" t="s">
-        <v>115</v>
-      </c>
-      <c r="U17" t="s">
-        <v>116</v>
-      </c>
-      <c r="V17" t="s">
-        <v>117</v>
       </c>
       <c r="AO17">
         <v>10000</v>
@@ -1543,22 +1507,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C18" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D18" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F18" t="s">
         <v>51</v>
       </c>
       <c r="G18">
         <v>50</v>
-      </c>
-      <c r="T18" t="s">
-        <v>121</v>
       </c>
       <c r="AO18">
         <v>10000</v>
@@ -1572,13 +1533,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C19" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D19" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F19" t="s">
         <v>60</v>
@@ -1610,13 +1571,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C20" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D20" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F20" t="s">
         <v>78</v>
@@ -1642,13 +1603,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C21" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D21" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="AE21">
         <v>1100</v>
@@ -1671,19 +1632,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C22" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D22" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E22">
         <v>400</v>
       </c>
       <c r="L22" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="N22">
         <v>10</v>
@@ -1706,19 +1667,16 @@
     </row>
     <row r="23" spans="1:42">
       <c r="A23">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C23" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D23" t="s">
-        <v>137</v>
-      </c>
-      <c r="T23" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="AM23">
         <v>100000</v>

</xml_diff>

<commit_message>
Various changes and fixes
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -158,7 +158,7 @@
     <t>&lt;p&gt;I want you to get your self to level 2. For this you will gain an additional 10XP per kill (until you reach level 2). It will take roughly ten kills (maybe less) to achieve this goal.&lt;/p&gt;&lt;p&gt;To do this:&lt;/p&gt;&lt;p&gt;There are various &lt;a href="/information/combat" target="_blank"&gt;attacks&lt;/a&gt;, as you will see – when fighting a monster:&lt;/p&gt;&lt;p&gt;- Attack (uses both weapons equipped)&lt;/p&gt;&lt;p&gt;- Cast (Uses both spells equipped)&lt;/p&gt;&lt;p&gt;- Cast and Attack (Uses spell in spell slot 1 and right handed weapon)&lt;/p&gt;&lt;p&gt;- Attack and Cast (uses spell in spell slot 2 and left handed weapon)&lt;/p&gt;&lt;p&gt;- Defend (Uses your shields and armour to defend)&lt;/p&gt;&lt;p&gt;For now, focus on using attack. Later on when you are more established, your &lt;a href="/information/races-and-classes#3" target="_blank"&gt;class&lt;/a&gt; will determine the type of attack you select, for example Heretics love Cast, while Prophets love Cast and Attack (or attack and Cast)&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;- Select a monster from the list behind this modal (start with Sewer Rat and work your way down)&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;- Click the attack button.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;- Click the first attack button.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;- Repeat until level 2.&lt;/p&gt;</t>
+    <t>&lt;p&gt;- Select a monster from the list behind this modal (start with Sewer Rat and work your way down)&lt;/p&gt;&lt;p&gt;- Click the attack button.&lt;/p&gt;&lt;p&gt;- Click the first attack button.&lt;/p&gt;&lt;p&gt;- Repeat until level 2.&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;- Select the action Fight from the list of actions behind this modal.&lt;/p&gt;&lt;p&gt;- Select a monster, start with Sewer Rat and work your way down.&lt;/p&gt;&lt;p&gt;- Tap the attack button&lt;/p&gt;&lt;p&gt;- Tap the first attack option.&lt;/p&gt;&lt;p&gt;- Repeat until level 2.&lt;/p&gt;</t>
@@ -173,7 +173,7 @@
     <t>&lt;p&gt;I want you to get to level 10. I do not want you to do this manually. Instead we are going to &lt;a href="/information/automation" target="_blank"&gt;explore&lt;/a&gt; for an hour. During this time you may gain a Faction level for Surface. The &lt;a href="/information/planes" target="_blank"&gt;map&lt;/a&gt; you are currently on.&lt;/p&gt;&lt;p&gt;&lt;a href="/information/factions" target="_blank"&gt;Factions&lt;/a&gt; can be seen on your character sheet (tab) under the tab: Factions. As you kill creatures you gain faction points. As you level the faction, you can get what are called &lt;a href="/information/random-enchants" target="_blank"&gt;Unique’s&lt;/a&gt;. These can be powerful items and you may only have one equipped at a time.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; For mobile players Factions will be on the character sheet tab in the closed top section which you can expand by clicking the blue cross in the top right.&lt;/p&gt;&lt;p&gt;Exploring will allow you to log out and idly gain items, exp, gold and possible quest item if the monster drops a quest item. There are things you cannot do while exploring such as change equipment, buy items from the &lt;a href="/information/shop" target="_blank"&gt;shop&lt;/a&gt; or &lt;a href="/information/market-board" target="_blank"&gt;market board&lt;/a&gt;. You will be told if you can do an action or not while exploring. Exploring should not just be used to level and log out, you &lt;a href="/information/some-clicking-required" target="_blank"&gt;won't get very far&lt;/a&gt; if you do that, there is much more to do and we will do it very soon! exploration is a way of gaining levels while doing other things in game.&lt;/p&gt;&lt;p&gt;Exploration messages will appear, while logged in, in the Exploration chat tab below.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;- First lets investigate the gear we have been given. &lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;We can do this by going to the character sheet tab and on the bottom right is the inventory management. You can click item names here to investigate, equip and do other types of actions with the item. For now if you find gear that raises your stats (ie, STR Modifier +x%) equip it. &lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;You may also need to visit the shop, which you can do by clicking the top left Hamburger menu to open the menu and select Shop. From here select Buy under General Shop. here you can buy gear, buy multiple pieces of gear or even compare and equip gear (auto purchase/equip).&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;- Next go back to the drop down for monsters and select a stronger monster and click Attack&lt;/p&gt;&lt;p&gt;- Select Attack and if you can kill it in one hit, which is ideal, move down the list to the next, rinse and repeat till you cannot move any further.&lt;/p&gt;&lt;p&gt;- Now that we have a monster, click Explore to the left of the attack section.&lt;/p&gt;&lt;p&gt;- Select the same monster, select 1 hour, ignore the move down and then select Attack, click Explore.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;This will run a set of battles every 5 minutes for 1 hour where you can fight between 1-8 enemies back to back. The reason we ignored the move down aspect is because it allows you to state: Move down the list every x levels that I gain, and for now we do not want that.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+    <t>&lt;p&gt;- First lets investigate the gear we have been given.&lt;/p&gt;&lt;p&gt;We can do this by going to the character sheet tab and on the bottom right is the inventory management. You can click item names here to investigate, equip and do other types of actions with the item. For now if you find gear that raises your stats (ie, STR Modifier +x%) equip it.&lt;/p&gt;&lt;p&gt;You may also need to visit the shop, which you can do by clicking the top left Hamburger menu to open the menu and select Shop. From here select Buy under General Shop. here you can buy gear, buy multiple pieces of gear or even compare and equip gear (auto purchase/equip).&lt;/p&gt;&lt;p&gt;- Next go back to the drop down for monsters and select a stronger monster and click Attack&lt;/p&gt;&lt;p&gt;- Select Attack and if you can kill it in one hit, which is ideal, move down the list to the next, rinse and repeat till you cannot move any further.&lt;/p&gt;&lt;p&gt;- Now that we have a monster, click Explore to the left of the attack section.&lt;/p&gt;&lt;p&gt;- Select the same monster, select 1 hour, ignore the move down and then select Attack, click Explore.&lt;/p&gt;&lt;p&gt;This will run a set of battles every 5 minutes for 1 hour where you can fight between 1-8 enemies back to back. The reason we ignored the move down aspect is because it allows you to state: Move down the list every x levels that I gain, and for now we do not want that.&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;- First lets investigate the gear we have been given.&lt;/p&gt;&lt;p&gt;We can now this by going to the character sheet, and from the drop down select Inventory Management. Now we can see all out gear we found - which might not be much, but we can filter through and look for Stat Raising gear, ie: STR Modifier +X%.&lt;/p&gt;&lt;p&gt;You may also need to visit the shop, which you can do by clicking the top left Hamburger menu to open the menu and select Shop. From here select Buy under General Shop. here you can buy gear, buy multiple pieces of gear or even compare and equip gear (auto purchase/equip).&lt;/p&gt;&lt;p&gt;Now that we have some gear lets go back to the game section and select:&lt;/p&gt;&lt;p&gt;- Fight from the action drop down&lt;/p&gt;&lt;p&gt;- Select a harder monster to fight, click Attack and if you kill it in one hit, move down the list.&lt;/p&gt;&lt;p&gt;- Repeat till you either die or find a monster you cannot kill in one hit, then move back to the one you could before.&lt;/p&gt;&lt;p&gt;- Close the fight section, select Exploration.&lt;/p&gt;&lt;p&gt;- Select the same monster, select 1 hour, ignore the move down and then select Attack, click Explore.&lt;/p&gt;&lt;p&gt;This will run a set of battles every 5 minutes for 1 hour where you can fight between 1-8 enemies back to back. The reason we ignored the move down aspect is because it allows you to state: Move down the list every x levels that I gain, and for now we do not want that.&lt;/p&gt;</t>
@@ -765,7 +765,7 @@
     <col min="2" max="2" width="36.42" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="2194.179" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="2102.201" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="1662.166" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="1594.896" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="1625.603" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="18.71" bestFit="true" customWidth="true" style="0"/>
@@ -1045,7 +1045,7 @@
     </row>
     <row r="5" spans="1:44">
       <c r="A5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>61</v>
@@ -1092,7 +1092,7 @@
     </row>
     <row r="6" spans="1:44">
       <c r="A6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>70</v>
@@ -1139,7 +1139,7 @@
     </row>
     <row r="7" spans="1:44">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>77</v>
@@ -1183,7 +1183,7 @@
     </row>
     <row r="8" spans="1:44">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>84</v>
@@ -1245,7 +1245,7 @@
     </row>
     <row r="9" spans="1:44">
       <c r="A9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>92</v>
@@ -1292,7 +1292,7 @@
     </row>
     <row r="10" spans="1:44">
       <c r="A10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>100</v>
@@ -1336,7 +1336,7 @@
     </row>
     <row r="11" spans="1:44">
       <c r="A11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>104</v>
@@ -1386,7 +1386,7 @@
     </row>
     <row r="12" spans="1:44">
       <c r="A12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>111</v>
@@ -1421,7 +1421,7 @@
     </row>
     <row r="13" spans="1:44">
       <c r="A13">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>116</v>
@@ -1459,7 +1459,7 @@
     </row>
     <row r="14" spans="1:44">
       <c r="A14">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>122</v>
@@ -1488,7 +1488,7 @@
     </row>
     <row r="15" spans="1:44">
       <c r="A15">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>127</v>

</xml_diff>

<commit_message>
Minore adjustments and fixes
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -185,13 +185,13 @@
     <t>You explore, you slaughter, you bathe in the enemies blood before you. You collect the shiny loot. You were gifted a green unique item from the towns people as a way of thanking you for your hard work.&lt;br /&gt; &lt;br /&gt; They told you that there are many other places one could explore, but that you could continue around here gain more favor with the people of the Surface plane.&lt;br /&gt; &lt;br /&gt; You wait for days and then weeks at the INN, where the hell is The Guide?&lt;br /&gt; &lt;br /&gt; “A letter for you” the barmaid states as she drops off your ale. You open it and read the following:&lt;br /&gt; &lt;br /&gt; Child. Listen, I am The Guide, alas I am investigating a situation. There is a magical spell upon your very being that allows the creatures you slaughter to gift you with the bounty of loot you have now, but that won’t last forever.&lt;br /&gt; &lt;br /&gt; You have to learn how to properly loot. You also have to have to learn how to wield your weapon, even casters can get into sticky situations where they need a weapon, and if you can’t hit anything – death will greet you faster then I.&lt;br /&gt; &lt;br /&gt; I also want you to investigate your gear, visit a shop. You gear is what makes you child. Know that.&lt;br /&gt; &lt;br /&gt; -- The Guide&lt;br /&gt; &lt;br /&gt; That’s it? Just barks orders through paper at you? You look around and contemplate doing what he want’s knowing full well you could just bugger off on your own adventure.&lt;br /&gt; &lt;br /&gt; By morning you have made up your mind on what to do.</t>
   </si>
   <si>
-    <t>&lt;p&gt;We are going to learn about two things today: &lt;a href="/information/character-stats" target="_blank"&gt;Stats&lt;/a&gt; and &lt;a href="/information/skill-information" target="_blank"&gt;Skills&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;Characters under level 12, get a boost to their looting skill making drops a lot more fun. How ever as you will soon reach level 12 you will see the drop rate disappear. This is where skills come in handy.&lt;/p&gt;&lt;p&gt;At any time, when leveling a skill as you will do here, you may click on the skill name to see applicable bonuses, XP, level and so on, The Skill Bonus refers to the bonus the skill applies when using it, such as for Accuracy or Looting. &lt;/p&gt;&lt;p&gt;Because you will be utilizing exploration to do this next part, you cannot switch skills in the middle of an exploration, you can stop exploration, switch to another skill and then resume your exploration.&lt;/p&gt;&lt;p&gt;Later on, and maybe even swith some of the gear you have found, you will see &lt;a href="/information/enchanting" target="_blank"&gt;enchantments&lt;/a&gt; with skill modifiers on them.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- Click the Character Sheet tab&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;- Scroll down to skills.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;- Find Accuracy, click train, select 10% of your XP and train the skill.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Follow these same steps to train Looting after clicking Stop training on Accuracy.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- Tap the Character Sheet tab.&lt;/p&gt;&lt;p&gt;- Select Manage Skills&lt;/p&gt;&lt;p&gt;- Tap Train on the Accuracy Skill&lt;/p&gt;&lt;p&gt;- Select 10% of your XP and train the skill&lt;/p&gt;&lt;p&gt;Follow these same steps to train Looting after clicking Stop training on Accuracy.&lt;/p&gt;</t>
+    <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; &lt;em&gt;This quest can take up to two hours to complete.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;We are going to learn about two things today: &lt;a href="/information/character-stats" target="_blank"&gt;Stats&lt;/a&gt; and &lt;a href="/information/skill-information" target="_blank"&gt;Skills&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;Characters under level 12, get a boost to their looting skill making drops a lot more fun. How ever as you will soon reach level 12 you will see the drop rate disappear. This is where skills come in handy.&lt;/p&gt;&lt;p&gt;At any time, when leveling a skill as you will do here, you may click on the skill name to see applicable bonuses, XP, level and so on, The Skill Bonus refers to the bonus the skill applies when using it, such as for Accuracy or Looting.&lt;/p&gt;&lt;p&gt;Because you will be utilizing exploration to do this next part, you cannot switch skills in the middle of an exploration, you can stop exploration, switch to another skill and then resume your exploration.&lt;/p&gt;&lt;p&gt;Later on, and maybe even the gear you have found, you will see &lt;a href="/information/enchanting" target="_blank"&gt;enchantments&lt;/a&gt; with skill modifiers on them.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;- Click the Character Sheet tab&lt;/p&gt;&lt;p&gt;- Scroll down to skills.&lt;/p&gt;&lt;p&gt;- Find Accuracy, click train, select 10% of your XP and train the skill.&lt;/p&gt;&lt;p&gt;Follow these same steps to train Looting after clicking Stop training on Accuracy.&lt;/p&gt;&lt;p&gt;If the gear you have found is not raising your stats to the required amount, try visiting the &lt;a href="/information/shop" target="_blank"&gt;shop&lt;/a&gt; and purchasing better gear. It migth not be enchanted but the % for stats that it raises, which stack, might be better then what you have on.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;- Tap the Character Sheet tab.&lt;/p&gt;&lt;p&gt;- Select Manage Skills&lt;/p&gt;&lt;p&gt;- Tap Train on the Accuracy Skill&lt;/p&gt;&lt;p&gt;- Select 10% of your XP and train the skill&lt;/p&gt;&lt;p&gt;Follow these same steps to train Looting after clicking Stop training on Accuracy.&lt;/p&gt;&lt;p&gt;If the gear you have found is not raising your stats to the required amount, try visiting the &lt;a href="http://127.0.0.1:8000/information/shop" target="_blank"&gt;shop&lt;/a&gt; and purchasing better gear. It migth not be enchanted but the % for stats that it raises, which stack, might be better then what you have on.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Accuracy</t>
@@ -203,10 +203,10 @@
     <t>Blacksmiths Life</t>
   </si>
   <si>
-    <t>Sitting in the INN, you stare into the large fire place with the wood burning and the smell of the old oak as it burns. It’s almost as if time stops for a moment and you can gather your thoughts.&lt;br /&gt; &lt;br /&gt; All you do is slaughter creatures, gather loot and slowly get better at hitting the enemies and even slightly faster.&lt;br /&gt; &lt;br /&gt; The flames of the fire seem to stand still, the smell of the fire has dissipated from the air. You look around and no one is moving, like they have been frozen in time.&lt;br /&gt; &lt;br /&gt; You turn back to the fire and see a young man, about twenty-five standing before the fire, his back to you. You call out to him, and he doesn’t turn around but he does speak.&lt;br /&gt; &lt;br /&gt; “Child. I have found something most mysterious. The gates have opened.”&lt;br /&gt; &lt;br /&gt; The gates? What gates?&lt;br /&gt; &lt;br /&gt; “Listen to me child.” The young man turns and faces you. You recognize the face, The Old Man from the dream, but he is much younger now.&lt;br /&gt; &lt;br /&gt; “I need you to speak with the local blacksmith, work with him for a while. Train a different set of skills. Important skills. I need you to craft your own gear.”&lt;br /&gt; &lt;br /&gt; You tell him that the gear you have found, the stuff you can buy from the local blacksmith is better then what you can craft.&lt;br /&gt; &lt;br /&gt; “True, however, you can craft even more powerful gear then that of which you can buy.”&lt;br /&gt; &lt;br /&gt; Before you can ask further questions the flames returning to their burning motion, the wood crackles, the INN is full of voices again and the smell of food fills the air.&lt;br /&gt; &lt;br /&gt; Where did he go?</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Today we are going to learn about &lt;a href="/information/crafting" target="_blank"&gt;crafting&lt;/a&gt;. There are various types of crafting, but we want to focus on weapons and Armour for now.&lt;/p&gt;&lt;p&gt;At first you will fail a lot, even with the suggested &lt;a href="/information/quest-items" target="_blank"&gt;quest items&lt;/a&gt; this quest can take a minute to complete. If you have any enchanted gear that has dropped that has Weapon/Armour Crafting Enchantments on them, I would suggest equipping them, even at the cost of damage.&lt;/p&gt;&lt;p&gt;Eventually you will craft beyond what the &lt;a href="/information/shop" target="_blank"&gt;shop&lt;/a&gt; sells. The Shop stops at two billion gold, where as players can craft up to 36+ Billion gold items that are much better then shop gear.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Crafting cannot be automated. Keep an eye on Server Messages section to see successes, failures and if you have new items to craft.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Remember to keep crafting - even after this quest. Stick to weapons (any type) - but do experiment with others, like Armour, Ring and Spell Crafting. A later quest will be less painful.&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;</t>
+    <t>Sitting in the INN, you stare into the large fire place with the wood burning and the smell of the old oak as it burns. It’s almost as if time stops for a moment and you can gather your thoughts.&lt;br /&gt; &lt;br /&gt; All you do is slaughter creatures, gather loot and slowly get better at hitting the enemies and even slightly faster.&lt;br /&gt; &lt;br /&gt; The flames of the fire seem to stand still, the smell of the fire has dissipated from the air. You look around and no one is moving, like they have been frozen in time.&lt;br /&gt; &lt;br /&gt; You turn back to the fire and see a young man, about twenty-five standing before the fire, his back to you. You call out to him, and he doesn’t turn around but he does speak.&lt;br /&gt; &lt;br /&gt; “Child. I have found something most mysterious. The gates have opened.”&lt;br /&gt; &lt;br /&gt; The gates? What gates?&lt;br /&gt; &lt;br /&gt; “Listen to me child.” The young man turns and faces you.&lt;br /&gt; &lt;br /&gt; “I need you to speak with the local blacksmith, work with him for a while. Train a different set of skills. Important skills. I need you to craft your own gear.”&lt;br /&gt; &lt;br /&gt; You tell him that the gear you have found, the stuff you can buy from the local blacksmith is better then what you can craft.&lt;br /&gt; &lt;br /&gt; “True, however, you can craft even more powerful gear then that of which you can buy.”&lt;br /&gt; &lt;br /&gt; Before you can ask further questions the flames returning to their burning motion, the wood crackles, the INN is full of voices again and the smell of food fills the air.&lt;br /&gt; &lt;br /&gt; Where did he go?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Today we are going to learn about &lt;a href="/information/crafting" target="_blank"&gt;crafting&lt;/a&gt;. There are various types of crafting, but we want to focus on weapons and armour for now.&lt;/p&gt;&lt;p&gt;At first you will fail a lot, even with the suggested &lt;a href="/information/quest-items" target="_blank"&gt;quest items&lt;/a&gt; this quest can take a minute to complete. If you have any enchanted gear that has dropped that has Weapon/Armour Crafting Enchantments on them, I would suggest equipping them, even at the cost of damage.&lt;/p&gt;&lt;p&gt;Eventually you will craft beyond what the &lt;a href="/information/shop" target="_blank"&gt;shop&lt;/a&gt; sells. The Shop stops at two billion gold, where as players can craft up to 36+ Billion gold items that are much better then shop gear.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Crafting cannot be automated. Keep an eye on Server Messages section to see successes, failures and if you have new items to craft.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Remember to keep crafting - even after this quest. Stick to weapons (any type) - but do experiment with others, like Armour, Ring and Spell Crafting. A later quest will be less painful.&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;- First we want to find the items we need, quest items are automatically used. You can open the Teleport Map Action to then select the location: Ruined Port City Of Kalize (X/Y): 32/368 and click teleport if you can afford the cost. This will get you the: Weapon Smith’s Book which adds 25% to Skill Bonus and XP.&lt;/p&gt;&lt;p&gt;- Repeat the above step to then go to: Dragon cliffs (X/Y): 192/176 to get the Blacksmith’s book for the same bonuses towards Armour Crafting.&lt;/p&gt;&lt;p&gt;Both of these can be upgraded later on when we have access to Labyrinth. There are some One Off &lt;a href="http://127.0.0.1:8000/information/quests" target="_blank"&gt;quests&lt;/a&gt; that will upgrade these.&lt;/p&gt;&lt;p&gt;- Now lets craft, first set up exploration for an hour or two – or what ever you feel like doing, Exploration will run while logged out. Remember to set it up with a monster you can kill in one hit.&lt;/p&gt;&lt;p&gt;- Close exploration and then from the drop down Craft/Enchant select craft, select weapons, select Broken Dagger and then click craft.&lt;/p&gt;</t>

</xml_diff>

<commit_message>
Minor updates and guide quest changes. Fixes to the side bar.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -206,7 +206,7 @@
     <t>Sitting in the INN, you stare into the large fire place with the wood burning and the smell of the old oak as it burns. It’s almost as if time stops for a moment and you can gather your thoughts.&lt;br /&gt; &lt;br /&gt; All you do is slaughter creatures, gather loot and slowly get better at hitting the enemies and even slightly faster.&lt;br /&gt; &lt;br /&gt; The flames of the fire seem to stand still, the smell of the fire has dissipated from the air. You look around and no one is moving, like they have been frozen in time.&lt;br /&gt; &lt;br /&gt; You turn back to the fire and see a young man, about twenty-five standing before the fire, his back to you. You call out to him, and he doesn’t turn around but he does speak.&lt;br /&gt; &lt;br /&gt; “Child. I have found something most mysterious. The gates have opened.”&lt;br /&gt; &lt;br /&gt; The gates? What gates?&lt;br /&gt; &lt;br /&gt; “Listen to me child.” The young man turns and faces you.&lt;br /&gt; &lt;br /&gt; “I need you to speak with the local blacksmith, work with him for a while. Train a different set of skills. Important skills. I need you to craft your own gear.”&lt;br /&gt; &lt;br /&gt; You tell him that the gear you have found, the stuff you can buy from the local blacksmith is better then what you can craft.&lt;br /&gt; &lt;br /&gt; “True, however, you can craft even more powerful gear then that of which you can buy.”&lt;br /&gt; &lt;br /&gt; Before you can ask further questions the flames returning to their burning motion, the wood crackles, the INN is full of voices again and the smell of food fills the air.&lt;br /&gt; &lt;br /&gt; Where did he go?</t>
   </si>
   <si>
-    <t>&lt;p&gt;Today we are going to learn about &lt;a href="/information/crafting" target="_blank"&gt;crafting&lt;/a&gt;. There are various types of crafting, but we want to focus on weapons and armour for now.&lt;/p&gt;&lt;p&gt;At first you will fail a lot, even with the suggested &lt;a href="/information/quest-items" target="_blank"&gt;quest items&lt;/a&gt; this quest can take a minute to complete. If you have any enchanted gear that has dropped that has Weapon/Armour Crafting Enchantments on them, I would suggest equipping them, even at the cost of damage.&lt;/p&gt;&lt;p&gt;Eventually you will craft beyond what the &lt;a href="/information/shop" target="_blank"&gt;shop&lt;/a&gt; sells. The Shop stops at two billion gold, where as players can craft up to 36+ Billion gold items that are much better then shop gear.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Crafting cannot be automated. Keep an eye on Server Messages section to see successes, failures and if you have new items to craft.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Remember to keep crafting - even after this quest. Stick to weapons (any type) - but do experiment with others, like Armour, Ring and Spell Crafting. A later quest will be less painful.&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;</t>
+    <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; &lt;em&gt;This quest can take up to two hours to complete. One for crafting and one to reach the required level.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Today we are going to learn about &lt;a href="/information/crafting" target="_blank"&gt;crafting&lt;/a&gt;. There are various types of crafting, but we want to focus on weapons and armour for now.&lt;/p&gt;&lt;p&gt;At first you will fail a lot, even with the suggested &lt;a href="/information/quest-items" target="_blank"&gt;quest items&lt;/a&gt; this quest can take a minute to complete. If you have any enchanted gear that has dropped that has Weapon/Armour Crafting Enchantments on them, I would suggest equipping them, even at the cost of damage.&lt;/p&gt;&lt;p&gt;Eventually you will craft beyond what the &lt;a href="/information/shop" target="_blank"&gt;shop&lt;/a&gt; sells. The Shop stops at two billion gold, where as players can craft up to 36+ Billion gold items that are much better then shop gear.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Crafting cannot be automated. Keep an eye on Server Messages section to see successes, failures and if you have new items to craft.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Remember to keep crafting - even after this quest. Stick to weapons (any type) - but do experiment with others, like Armour, Ring and Spell Crafting. A later quest will be less painful.&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;- First we want to find the items we need, quest items are automatically used. You can open the Teleport Map Action to then select the location: Ruined Port City Of Kalize (X/Y): 32/368 and click teleport if you can afford the cost. This will get you the: Weapon Smith’s Book which adds 25% to Skill Bonus and XP.&lt;/p&gt;&lt;p&gt;- Repeat the above step to then go to: Dragon cliffs (X/Y): 192/176 to get the Blacksmith’s book for the same bonuses towards Armour Crafting.&lt;/p&gt;&lt;p&gt;Both of these can be upgraded later on when we have access to Labyrinth. There are some One Off &lt;a href="http://127.0.0.1:8000/information/quests" target="_blank"&gt;quests&lt;/a&gt; that will upgrade these.&lt;/p&gt;&lt;p&gt;- Now lets craft, first set up exploration for an hour or two – or what ever you feel like doing, Exploration will run while logged out. Remember to set it up with a monster you can kill in one hit.&lt;/p&gt;&lt;p&gt;- Close exploration and then from the drop down Craft/Enchant select craft, select weapons, select Broken Dagger and then click craft.&lt;/p&gt;</t>
@@ -230,13 +230,13 @@
     <t>The Enchantress</t>
   </si>
   <si>
-    <t>You are exhausted, tired, confused.&lt;br /&gt; &lt;br /&gt; “Child” comes a familiar voice as you sit up on your bed.&lt;br /&gt; &lt;br /&gt; The INN is creaky, noisy and musty. The single candle flame that burns in the room barley illuminates the room.&lt;br /&gt; &lt;br /&gt; As he walks from the shadows The Guide stands before you, not young and handsome, but old and wise, dressed in robes. His skin is brown from the sun.&lt;br /&gt; &lt;br /&gt; “Downstairs sits a woman, an attractive woman.” he states.&lt;br /&gt; &lt;br /&gt; “She will teach you about magic and its properties, specifically in the art of enchanting and disenchanting.”&lt;br /&gt; &lt;br /&gt; You ask him why he can’t teach you and he deflects the question.&lt;br /&gt; &lt;br /&gt; “Go now child. She isn’t to be kept waiting.”&lt;br /&gt; &lt;br /&gt; You head down the stairs to meet the Enchantress.&lt;br /&gt; &lt;br /&gt; She waits for you at a table, a woman in black, instantly recognizable by her long black hair and pale complexion. She radiates beauty.&lt;br /&gt; &lt;br /&gt; You walk over and sit down at the table. “Hello child.” She starts, he voice is soft and entrancing. “have you heard of the queen?” You shake your head no. “She has gifted you with some of those green shiny unique’s in your inventory.”&lt;br /&gt; &lt;br /&gt; You remember those. Killing monsters gets you faction with the plane and its people and as a reward they give you a shiny green item that makes you feel much much stronger.&lt;br /&gt; &lt;br /&gt; “She can give you more powerful ones, but you have to face the most fearsome of creatures to earn her attention. In the mean time lets discuss the art of magic. Lets start small with spells …”</t>
+    <t>You are exhausted, tired, confused.&lt;br /&gt; &lt;br /&gt; “Child” comes a familiar voice as you sit up on your bed.&lt;br /&gt; &lt;br /&gt; The INN is creaky, noisy and musty. The single candle flame that burns in the room barley illuminates the area.&lt;br /&gt; &lt;br /&gt; As he walks from the shadows The Guide stands before you, not young and handsome, but old and wise, dressed in robes. His skin is brown from the sun.&lt;br /&gt; &lt;br /&gt; “Downstairs sits a woman, an attractive woman.” he states with a bit of a smirk.&lt;br /&gt; &lt;br /&gt; “She will teach you about magic and its properties, specifically in the art of enchanting and disenchanting.”&lt;br /&gt; &lt;br /&gt; You ask him why he can’t teach you and he deflects the question.&lt;br /&gt; &lt;br /&gt; “Go now child. She isn’t to be kept waiting.”&lt;br /&gt; &lt;br /&gt; You head down the stairs to meet the Enchantress.&lt;br /&gt; &lt;br /&gt; She waits for you at a table, a woman in black, instantly recognizable by her long black hair and pale complexion. She radiates beauty.&lt;br /&gt; &lt;br /&gt; You walk over and sit down at the table. “Hello child.” She starts, he voice is soft and entrancing. “have you heard of The Queen?” You shake your head no. “She has gifted you with some of those green shiny unique’s in your inventory.”&lt;br /&gt; &lt;br /&gt; You remember those. Killing monsters gets you faction with the plane and its people. As a reward they give you a shiny green item that makes you feel much much stronger.&lt;br /&gt; &lt;br /&gt; “She can give you more powerful ones, but you have to face the most fearsome of creatures to earn her attention. In the mean time lets discuss the art of magic. Lets start small with spells …”</t>
   </si>
   <si>
     <t>&lt;p&gt;Lets start learning about spells.&lt;/p&gt;&lt;p&gt;You have just spent a ton of time crafting weapons and Armour, we will repeat this to craft spells. Spells are useful for caster classes, as well as any one who wants to use them, be they healing or damage based.&lt;/p&gt;&lt;p&gt;Damage spells and Staves (Two Handed weapons) can raise the characters intelligence, both of which can be bought from the shop or crafted.&lt;/p&gt;&lt;p&gt;Healing spells are great for characters who want to do Cast and attack or Attack and Cast, like Prophets. healing spells will heal the player when they are cast and cannot ever miss, damage spells how ever require a character to train the skill: Casting Accuracy to have a better chance at hitting the enemies with their damage spells. Healing spells can also resurrect the player and have a resurrection chance. resurrection automatically happens based on the resurrection chance of both of your equipped healing spells.&lt;/p&gt;&lt;p&gt;To get the quest item required, you will need to kill: &lt;strong&gt;Umbering Spirit Lord&lt;/strong&gt; on Surface. This creature is further down the list and may require you to upgrade your gear through the shop before being able to take him down.&lt;/p&gt;&lt;p&gt;This creature has a 15% chance to drop the item, so exploration might be a good choice here.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Just like we did for crafting, lets select spells instead of weapons or armour. When crafting spells, you will always have one of each type to equip: Damage and Healing.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Remember to set up exploration while this runs.&lt;/strong&gt;&lt;/p&gt;</t>
+    <t>&lt;p&gt;Just like we did for crafting, lets select spells instead of weapons or armour. When crafting spells, you will always have one of each type to equip: Damage and Healing.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Remember to set up exploration with a creature you can reliably kill in one hit. Continue investigating and upgrading your gear to take on harder creature.&lt;/strong&gt;&lt;/p&gt;</t>
   </si>
   <si>
     <t>Spell Crafting</t>
@@ -1063,7 +1063,7 @@
         <v>65</v>
       </c>
       <c r="G5">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="H5" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
Added a new guide quest requirement. redoing some guide quests - other minor fixes
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="105">
   <si>
     <t>id</t>
   </si>
@@ -71,6 +71,9 @@
     <t>required_class_specials_equipped</t>
   </si>
   <si>
+    <t>required_class_rank_level</t>
+  </si>
+  <si>
     <t>required_faction_id</t>
   </si>
   <si>
@@ -272,10 +275,10 @@
     <t>Enchanting is key</t>
   </si>
   <si>
-    <t>You have been on another planes, a plane full of ruins, broken pieces of multiple labyrinths. The entire plane was covered with them.&lt;br /&gt; &lt;br /&gt; As you recover from your travels, slaughtering a whole new group of fearsome creatures, gaining notoriety with the inhabitants of said plane.&lt;br /&gt; &lt;br /&gt; Still no sign of the Enchantress and no sign of The Guide. You take a moment to relax before your next adventure.&lt;br /&gt; &lt;br /&gt; As you rise to the new dawn of a new day you have a knock at the door. You rise and greet the stranger. The Enchantress walks in. Today she wares a red robe and you can see deep into her blue eyes.&lt;br /&gt; &lt;br /&gt; “My darling child, I hear you have been adventuring. Shall we pick up where we left off? The art of enchanting.”&lt;br /&gt; &lt;br /&gt; You tell her you have plenty of enchanted gear.&lt;br /&gt; &lt;br /&gt; “Wouldn’t you like better gear? Stronger gear?”</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Today's lesson is about &lt;a href="/information/enchanting" target="_blank"&gt;enchanting&lt;/a&gt; and &lt;a href="/information/disenchanting" target="_blank"&gt;disenchanting&lt;/a&gt;. Just like crafting, enchanting is wildly important. As you may know, you cannot buy enchanted gear from the shop. Some players will sell it on the &lt;a href="/information/market-board" target="_blank"&gt;market place&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;More importantly, you want a &lt;a href="/information/currencies" target="_blank"&gt;currency&lt;/a&gt; you can get from it: Gold Dust. This currency is used in a lot of quests we are going to start doing soon. So lets get a lot of it.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Remember to keep enchanting and disenchanting items. A later quest will be less painful.&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;The &lt;strong&gt;Skill Type Crafting to level 10&lt;/strong&gt; basically means, level any rafting skill you want to level 10 or higher.&lt;/p&gt;</t>
+    <t>You have been on another plane, a plane full of ruins, broken pieces of multiple labyrinths. The entire plane was covered with them.&lt;br /&gt; &lt;br /&gt; As you recover from your travels, slaughtering a whole new group of fearsome creatures, gaining notoriety with the inhabitants of said plane.&lt;br /&gt; &lt;br /&gt; Still no sign of the Enchantress and no sign of The Guide. You take a moment to relax before your next adventure.&lt;br /&gt; &lt;br /&gt; As you rise to the new dawn of a new day you have a knock at the door. You rise and greet the stranger. The Enchantress walks in. Today she wares a set of red robes and you can see deep into her blue eyes.&lt;br /&gt; &lt;br /&gt; “My darling child, I hear you have been adventuring. Shall we pick up where we left off? The art of enchanting.”&lt;br /&gt; &lt;br /&gt; You tell her you have plenty of enchanted gear.&lt;br /&gt; &lt;br /&gt; “Wouldn’t you like better gear? Stronger gear?”</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; &lt;em&gt;This quest can take up to two hours to complete&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Today's lesson is about &lt;a href="/information/enchanting" target="_blank"&gt;enchanting&lt;/a&gt; and &lt;a href="/information/disenchanting" target="_blank"&gt;disenchanting&lt;/a&gt;. Just like crafting, enchanting is wildly important. As you may know, you cannot buy enchanted gear from the shop. Some players will sell it on the &lt;a href="/information/market-board" target="_blank"&gt;market place&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;More importantly, you want a &lt;a href="/information/currencies" target="_blank"&gt;currency&lt;/a&gt; you can get from it: Gold Dust. This currency is used in a lot of quests we are going to start doing soon. So lets get a lot of it.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Remember to keep enchanting and disenchanting items. A later quest will be less painful.&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;The &lt;strong&gt;Skill Type Crafting to level 10&lt;/strong&gt; means: level any crafting skill you want to level 10 or higher.&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;To enchant, from the crafting drop down select enchant.&lt;/p&gt;&lt;p&gt;- Here you have an item to select, a suffix and a prefix to select. The cost of enchanting can get widely expensive so exploration is required. Since you need items: weapons, Armour, spells and Rings, you will also want to be crafting. You can also re-enchant enchanted items but that gets more costly.&lt;/p&gt;&lt;p&gt;You can also just go to the shop and buy multiple items to enchant, like broken daggers.&lt;/p&gt;&lt;p&gt;- Next, when you have enchanted, ideally 75 items, next go to your inventory&lt;/p&gt;&lt;p&gt;- From the actions on the inventory section of your character sheet, click Disenchant All.&lt;/p&gt;&lt;p&gt;- This will raise your disenchanting skill, and slowly over time your enchanting skill as well.&lt;/p&gt;&lt;p&gt;- Repeat till you meet the quest requirements.&lt;/p&gt;</t>
@@ -299,7 +302,7 @@
     <t>You have come a long way since you first set out. Learning more of the world, learning more about your self and developing your skills.&lt;br /&gt; &lt;br /&gt; You sit under the tree outside of town and watch the merchants go by. A few stop and ask if you would like to purchase some of their wares, a few have some interesting knickknacks, and a few others have some food worth buying.&lt;br /&gt; &lt;br /&gt; As the day passes by and the sun begins to set you think of heading back to town to wash, relax and get a good nights sleep.&lt;br /&gt; &lt;br /&gt; “Hello there” comes an unfamiliar voice.&lt;br /&gt; &lt;br /&gt; You look and see a man in a Fedora, Green Tunic and black leather pants. He seems older, but moves as if he is younger then his age.&lt;br /&gt; &lt;br /&gt; He comes closer and introduces himself, “I am The Poet and have been sent by The Guide to ask a favor of you, one from him.”&lt;br /&gt; &lt;br /&gt; You ask why he doesn’t come himself and ask this favor.&lt;br /&gt; &lt;br /&gt; “There is a darkness that is seeping from the depths into all the Planes. It is corrupting the Planes and causing the creatures to become vile and wicked. The Guide is busy investigating something deep with in Dungeons. Where he wants you to meet him.”&lt;br /&gt; &lt;br /&gt; You remember how you got to labyrinth, how hard can it be to get to Dungeons? You agree and The Poet tells you how to set off.</t>
   </si>
   <si>
-    <t>&lt;p&gt;This is another &lt;a href="/information/quests" target="_blank"&gt;quest&lt;/a&gt; where we are going to a new &lt;a href="/information/planes" target="_blank"&gt;plane&lt;/a&gt;. However, to get there we have to complete a few quests to unlock access.&lt;/p&gt;&lt;p&gt;Quests are how a lot of Tlessas features are unlocked for players. These quests, much like Guide Quests, will have a story – before and after completion – as well as explicit instructions on how to complete them, much like these.&lt;/p&gt;&lt;p&gt;Since you already know how to &lt;a href="/information/traverse" target="_blank"&gt;traverse&lt;/a&gt;, we just need to get you a quest item that allows you to traverse down to Dungeons.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; The required secondary quest item, will require you to complete a quest from Labyrinth under the One Off Quest section called: &lt;strong&gt;Dark Enchantress.&lt;/strong&gt; Click the quest, and click on the Requirements tab to see what you have to do.&lt;/p&gt;</t>
+    <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; &lt;em&gt;This quest can take 2+ hours to complete as you will need to earn Gold Dust for some of the requirements to be completed.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;This is another &lt;a href="/information/quests" target="_blank"&gt;quest&lt;/a&gt; where we are going to a new &lt;a href="/information/planes" target="_blank"&gt;plane&lt;/a&gt;. However, to get there we have to complete a few quests to unlock access.&lt;/p&gt;&lt;p&gt;Quests are how a lot of Tlessas features are unlocked for players. These quests, much like Guide Quests, will have a story – before and after completion – as well as explicit instructions on how to complete them, much like these.&lt;/p&gt;&lt;p&gt;Since you already know how to &lt;a href="/information/traverse" target="_blank"&gt;traverse&lt;/a&gt;, we just need to get you a quest item that allows you to traverse down to Dungeons.&lt;/p&gt;&lt;p&gt;For the requirement of getting access to Dungeons, some quests will require the player to earn Gold Dust as part of the quest requirements, by now you know of two ways: Craft → Enchant → Disenchant All items and Fight monsters and disenchant what you don’t want.&lt;/p&gt;&lt;p&gt;There is a third way: Weekly Currency Events. These give players Gold Dust, Crystal Shards (Shards) and (you wont have the quest item for them yet) Copper Coins.&lt;/p&gt;&lt;p&gt;Using exploration on these days can get you 1-50 of each currency (minus copper coins) for each monster you kill. Exploration can pit you up against 8 monsters at a time, which can be roughly 400 of each currency (roughly, as its random amount).&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; The required secondary quest item, will require you to complete a quest from Labyrinth under the One Off Quest section called: &lt;strong&gt;Dark Enchantress.&lt;/strong&gt; Click the quest, and click on the Requirements tab to see what you have to do.&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;- Click the Quests tab&lt;/p&gt;&lt;p&gt;- Here you can see a list of quests for the plane you are on (if you are not on surface, select the Surface plane from the Planes drop down.)&lt;/p&gt;&lt;p&gt;- On the Surface quests you will see a quest (to the left) called Light The Way, complete the quests working down the tree until you complete it. Locked Quests are red, quests you can complete are Blue and Completed Quests are Green.&lt;/p&gt;&lt;p&gt;- Click on the quest to read the story, see the requirements and the reward.&lt;/p&gt;&lt;p&gt;- The Requirements tab will have explicit instructions beside each requirement.&lt;/p&gt;&lt;p&gt;- Much like Guide Quests, you can see your completed quests in the sidebar (Hamburger menu to the top left) under: Quest Log → Completed Quests.&lt;/p&gt;</t>
@@ -320,100 +323,13 @@
     <t>Death is something special</t>
   </si>
   <si>
-    <t>The Dungeons plane crawls with death. There is a darkness that seeps across the ground, infecting and infesting everything that it touches. You seem to be immune to it. You know there is shadow in the distance that is watching you. A shade like creature that only makes it’s self visible every now and then to your eyes.&lt;br /&gt; &lt;br /&gt; “Child!” Comes a familiar voice. The Guide, young, handsome and every changing comes up to you.&lt;br /&gt; &lt;br /&gt; “You have come down the Dungeons. A place of ruins, crypts, caves and other bits of darkness that one can explore for loot.”&lt;br /&gt; &lt;br /&gt; You ask him about the darkness crawling across the land and the shade like creature you can see off in the distance.&lt;br /&gt; &lt;br /&gt; “The darkness is caused by the gates of Shadow Planes, which has opened. The shade creature is the Shade Lord. He is seeking something, something that escaped the darkness beneath the pits of Hell. Alas to take on any of these creatures you need to get stronger!”</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Now we learn about a new feature: &lt;a href="/information/class-skills" target="_blank"&gt;Class Skills&lt;/a&gt; and Class Bonus.&lt;/p&gt;&lt;p&gt;Class Skills are different for each &lt;a href="/information/races-and-classes#3" target="_blank"&gt;class&lt;/a&gt; in the game. Every class has a skill which you can see on your skills table under Training Tab. It has an icon beside it and is in orange text.&lt;/p&gt;&lt;p&gt;This skill important to level because it allows you to increase your Class Bonus which can be seen on the character sheet to the left, under inventory count or on mobile under Class Details, at the bottom of the details section.&lt;/p&gt;&lt;p&gt;Every class has a special attack that fires automatically based on Three Things:&lt;/p&gt;&lt;p&gt;- Class Bonus % (the higher, the more chance for the special to fire)&lt;/p&gt;&lt;p&gt;- Weapons&lt;/p&gt;&lt;p&gt;- Attack type&lt;/p&gt;</t>
+    <t>The Dungeons plane crawls with death. There is a darkness that seeps across the ground, infecting and infesting everything that it touches. You seem to be immune to it. You know there is shadow in the distance that is watching you. A shade like creature that only makes it’s self visible every now and then to your eyes.&lt;br /&gt; &lt;br /&gt; “Child!” Comes a familiar voice. The Guide, young, handsome and ever changing comes up to you.&lt;br /&gt; &lt;br /&gt; “You have come down the Dungeons. A place of ruins, crypts, caves and other bits of darkness that one can explore for loot.”&lt;br /&gt; &lt;br /&gt; You ask him about the darkness crawling across the land and the shade like creature you can see off in the distance.&lt;br /&gt; &lt;br /&gt; “The darkness is caused by the gates of Shadow Planes, which has opened. The shade creature is the Shade Lord. He is seeking something, something that escaped the darkness beneath the pits of Hell. Alas to take on any of these creatures you need to get stronger!”</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Now we learn about a new feature: &lt;a href="/information/class-skills" target="_blank"&gt;Class Skills&lt;/a&gt; and Class Bonus.&lt;/p&gt;&lt;p&gt;Class Skills are different for each &lt;a href="/information/races-and-classes#3" target="_blank"&gt;class&lt;/a&gt; in the game. Every class has a skill which you can see on your skills table under Training Tab. It has an icon beside it and is in orange text.&lt;/p&gt;&lt;p&gt;This skill important to level because it allows you to increase your Class Bonus which can be seen on the character sheet to the left, under inventory count or on mobile under Class Details, at the bottom of the details section.&lt;/p&gt;&lt;p&gt;Your class will tell you, if you click/tap on the class name in the top bar where you basic details are, the requirements for your class special attack to fire. This means what weapons or spells you must have equipped and how many. If you also need to use a specific attack type or not.&lt;/p&gt;&lt;p&gt;Based on those factors and the % of your class bonus, your special can just fire in the middle of an attack, which you will see when manually fighting.&lt;/p&gt;&lt;p&gt;Each class has it’s own special attack and special rules for those attacks.&lt;/p&gt;&lt;p&gt;Class Skills can also raise specific attributes about the class such as damage, healing and armour class bonuses that stack with all other bonuses.&lt;/p&gt;&lt;p&gt;At this stage in the game, the one important thing I can tell you is: unless it states that it wont stack, everything stacks together to raise your stats, damage, armour class, healing as well as stats, skills and so on.&lt;/p&gt;&lt;p&gt;When utilizing, as we will soon, &lt;a href="/information/class-ranks" target="_blank"&gt;Class Ranks&lt;/a&gt; to switch classes, you will notice that one skill on your Skills tab on the Character Sheet, will change. Every time you change a class your character will switch their class skill.&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;- The instructions state to level a Effects Class to the specified level. To do this, go to your character sheet section, in your skill section – train the skill with the orange text to the specified level.&lt;/p&gt;&lt;p&gt;- To Get the Gold Dust you can disenchant items that drop you no longer need, or craft some items, enchant them and disenchant them. Now is the time to explore the &lt;a href="http://127.0.0.1:8000/information/enchanting" target="_blank"&gt;Enchanting&lt;/a&gt; list in the docs to see what types of enchantments you can apply to your equipment so you can start creating a gear set geared towards your needs.&lt;/p&gt;&lt;p&gt;That’s it. Now you might not see your class bonus fire off much at first, but over time, keep leveling this skill and you will start to see your special fire off automatically when manually fighting.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Mercenary for hire</t>
-  </si>
-  <si>
-    <t>You managed to survive long enough to drag your broken, bruised and bloody body back to the surface. You stop at an abandoned farm to mend your wounds and rest after such excursions.&lt;br /&gt; &lt;br /&gt; The farm looks familiar, but the names of the people that lived here has escaped your mind. You pay it no heed as you spend your time at this farm.&lt;br /&gt; &lt;br /&gt; A knock at the door, you open it and there stand The Poet.&lt;br /&gt; &lt;br /&gt; “Hello child.” He pushes past you and lets him self in.&lt;br /&gt; &lt;br /&gt; “You came back here.” he states.&lt;br /&gt; &lt;br /&gt; You look at him, confused.&lt;br /&gt; &lt;br /&gt; “Do you not know where you are child? You are home.”&lt;br /&gt; &lt;br /&gt; It comes back to you, your home. Abandoned. No parent, no one. Where did they go? You ask The Poet in a rush, frantic and worried about your parents.&lt;br /&gt; &lt;br /&gt; “Child. Calm your self. They are here, somewhere. You’ll have to find them eventually.”&lt;br /&gt; &lt;br /&gt; Find them? What has he done with them? You start to get angry but The Poet waves his hand and calmness washes over you.&lt;br /&gt; &lt;br /&gt; “For now I need you to head down to Labyrinth and complete some tasks to unlock Mercenaries. They can help you with getting shiny coins, dust and shards and later on some Copper.”&lt;br /&gt; &lt;br /&gt; My parents, where are they?&lt;br /&gt; &lt;br /&gt; “They are not where you think, they are not whom you think. I have lifted the spell that you lived with for so long. Do this, and I will tell you more.”&lt;br /&gt; &lt;br /&gt; He refuses to discuss the matter anymore.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Lets learn about &lt;a href="/information/currencies" target="_blank"&gt;currencies&lt;/a&gt;. You know about Gold Dust – that it can be used in quests and Alchemy.&lt;/p&gt;&lt;p&gt;You also know about Gold, the core currency. Shards and Copper Coins are another two types of currencies. Both can be earned from a feature called &lt;a href="/information/slots" target="_blank"&gt;Slots&lt;/a&gt;. However, there is a way to cheat the system and that’s to &lt;/p&gt;&lt;p&gt;level &lt;a href="/information/mercenary" target="_blank"&gt;Mercenaries&lt;/a&gt;. You will need to complete a quest in Labyrinth. You can see this by going to the quests tab and selecting Labyrinth from the Planes drop down. Look for the quest: &lt;strong&gt;&lt;u&gt;Powers of The Children&lt;/u&gt;&lt;/strong&gt; to the right.&lt;/p&gt;&lt;p&gt;You can also see these quests if you traverse down to Labyrinth and then select the Quests tab.&lt;/p&gt;&lt;p&gt;Complete this quest to unlock a new feature called Mercenaries, who as they are leveled up will help you with getting more and more currencies from Slots and Farming creatures.&lt;/p&gt;&lt;p&gt;You can see these mercenaries who you must purchase by going to your character sheet and tapping/clicking the tab: Mercenaries. You can purchase them after completing the quest line above.&lt;/p&gt;&lt;p&gt;As you level these Mercenaries, you will eventually be able to reincarnate them – at their max level – and re-level them up to get even more % bonus towards currency drops. Some currencies such as Copper Coins only drop on a specific plane called Purgatory which you are not strong enough for yet, thus Slots will not drop them as you are missing an item to get into Purgatory.&lt;/p&gt;&lt;p&gt;For now, lets focus on Gold Dust and Shards, which you can do through Slots.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- In the actions section click Slots.&lt;/p&gt;&lt;p&gt;- Play slots or, if you cannot afford slots, kill monsters to get the currency requirements of this quest.&lt;/p&gt;&lt;p&gt;- Level a specific mercenary to the required level by killing creatures.&lt;/p&gt;&lt;p&gt;You can craft and play slots and explore at the same time. Which will be needed for this particular quest.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- In the actions section select Slots from the action drop down.&lt;/p&gt;&lt;p&gt;- Play slots or, if you cannot afford slots, kill monsters to get the currency requirements of this quest.&lt;/p&gt;&lt;p&gt;- Level a specific mercenary to the required level by killing creatures.&lt;/p&gt;&lt;p&gt;You can only do one action at a time on mobile, for example craft or play slots while exploration is running.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>child-of-gold-dust</t>
-  </si>
-  <si>
-    <t>child-of-shards</t>
-  </si>
-  <si>
-    <t>A place to call home</t>
-  </si>
-  <si>
-    <t>You are exhausted, emotionally, mentally and physically. You fight, you kill, you train, you craft and enchant. You sit under a tree with a small fire burning as the moon rises high in the night sky. You notice how bright, how clear, how large the moon is in the night sky.&lt;br /&gt; &lt;br /&gt; As you sit and mull over the last few months, your mind wonders back to what The Poet stated, about the abandoned house, your house, your family house.&lt;br /&gt; &lt;br /&gt; Are they dead? Are they alive? Where are they? Why did they leave the farm? So many questions, yet no answers.&lt;br /&gt; &lt;br /&gt; A slight breeze kicks up and the flames flicker and dance in the night.&lt;br /&gt; &lt;br /&gt; A voice comes from the shadows of the night, beyond the flames light and reach.&lt;br /&gt; &lt;br /&gt; “Child, I am back.” The Guide steps from the shadows.&lt;br /&gt; &lt;br /&gt; You look up from your fire and see that he is young again, keeps changing between young and old. Alas he looks bruised, broken and is limping.&lt;br /&gt; &lt;br /&gt; You ask him what happened but he shrugs it off. “It is not important. What is though is that you put your feet up. Gather some soldiers, build some walls, create a home for your self.”&lt;br /&gt; &lt;br /&gt; You tell him what The Poet said about your parents.&lt;br /&gt; &lt;br /&gt; “Silly child, there is so much for you to learn. Alas for now, Lets get you to settle down and call some place home.”&lt;br /&gt; &lt;br /&gt; You insist he explains more, but he refuse’s and starts to get angry at your demands.&lt;br /&gt; &lt;br /&gt; “Now you listen here, there is a darkness descending on this world, one escaping the pits of hell, some of it I am sure you have learned about, others you don’t know yet, but soon will. All will be answered in time. But for now, you have a job to do.”&lt;br /&gt; &lt;br /&gt; You think for a moment of refusing until you get the answers, but a swath of land you can call your own does sound enticing.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Lets take a break from questing, crafting, enchanting and fighting and lets focus on kingdoms and what they can provide for you.&lt;/p&gt;&lt;p&gt;You can settle a &lt;a href="/information/kingdoms" target="_blank"&gt;kingdom&lt;/a&gt; for free once, assuming you have no kingdoms.&lt;/p&gt;&lt;p&gt;Each kingdom after the first one will cost 10,000 Gold x the amount of kingdoms you already own.&lt;/p&gt;&lt;p&gt;Your first kingdom, again assuming you have no kingdoms, will have a 7 day protection on it, meaning no one can attack it.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; The quest requires a kingdom level, this means you need you need to level the buildings, by resources or gold, over time to reach the required objective. You can level one building or multiple as the kingdom level is a sum of all the building levels in one kingdom.&lt;/p&gt;&lt;p&gt;The quest requires you to purchase with gold or resources units. If you purchased your buildings (2 at level 10) to will notice that you have no population. On the right hand side under Kingdom Actions for desktop or under kingdoms details for mobile, you will find a Buy Population button that lets you buy people for gold. Caution as to not exceed the max amount of population your kingdom can have or an angry NPC might come knocking.&lt;/p&gt;&lt;p&gt;Kingdom resource replenishment and treasury interest for deposited gold occurs every hour and can be seen in the Server Message section if you go to your &lt;a href="//information/settings" target="_blank"&gt;settings&lt;/a&gt; and enable the messages if they wish. &lt;em&gt;This can get quite spammy so it is disabled by default.&lt;/em&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;Find a place on either Surface, Labyrinth or Dungeons where you can access and what to settle a kingdom.&lt;/p&gt;&lt;p&gt;- Click Settle Kingdom under the map and give your kingdom a name.&lt;/p&gt;&lt;p&gt;- Now you can click on the Kingdoms tab and see your kingdom&lt;/p&gt;&lt;p&gt;- From there you can click on the kingdom name and see further details.&lt;/p&gt;&lt;p&gt;- On the map you will see an icon on the map that represents your kingdom and you can also click on that to get basic details as well as teleport to it, assuming you have the gold to teleport the distance.&lt;/p&gt;&lt;p&gt;- When you click on the kingdom via the kingdoms tab, you can see information like buildings and units as well as kingdom resources that will replenish over time, every hour.&lt;/p&gt;&lt;p&gt;- Lets recruit some units and upgrade our buildings which can be done with either resources, as stated, or gold. Both of which will require (real world) time to recruit the units and build the buildings.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;Find a place on either Surface, Labyrinth or Dungeons where you can access and what to settle a kingdom.&lt;/p&gt;&lt;p&gt;- In the Actions drop down, select Map Movement&lt;/p&gt;&lt;p&gt;- Tap Settle Kingdom under the map and give your kingdom a name.&lt;/p&gt;&lt;p&gt;- Now you can tap on the Kingdoms tab and see your kingdom&lt;/p&gt;&lt;p&gt;- From there you can tap on the kingdom name and see further details.&lt;/p&gt;&lt;p&gt;- On the map you will see your kingdom icon, but due to how the map works on mobile, you wont be able to tap on it for basic details unlike on desktop. How ever if you tap Teleport you can choose from a list of your kingdoms on that Plane to teleport to.&lt;/p&gt;&lt;p&gt;- When you tap on the kingdom via the kingdoms tab, you can see information like buildings and units as well as kingdom resources that will replenish over time, every hour.&lt;/p&gt;&lt;p&gt;- Lets recruit some units and upgrade our buildings which can be done with either resources, as stated, or gold. Both of which will require (real world) time to recruit the units and build the buildings.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Growing the population</t>
-  </si>
-  <si>
-    <t>You managed to build a small town, people come to live here as there is tons of work, farming, construction and even a developing industrial and military aspect. You look for new ways to grow the kingdom and to make the people happy as well as building more homes and forms of work for the people.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Now that we have settled a kingdom, lets look into a new set of skills, which instead of killing creatures, takes real world time to complete. These are called Kingdom Passives which, as the name states, help your kingdom(s) grow over time. &lt;/p&gt;&lt;p&gt;Each passive is only unlocked after the parent passive reaches a specific level.&lt;/p&gt;&lt;p&gt;These skills, as stated, take real world time to train and will continue to train even if you are logged out.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- Click on the character sheet tab&lt;/p&gt;&lt;p&gt;- In the skill section, click on Kingdom Passives&lt;/p&gt;&lt;p&gt;- Click on Kingdom Management and click train&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- Tap on the character sheet tab&lt;/p&gt;&lt;p&gt;- Select Skill Management from the drop down&lt;/p&gt;&lt;p&gt;- Tap on the Kingdom Passive tab&lt;/p&gt;&lt;p&gt;- Tap on the Kingdom Management in the tree and click train.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Kingdom Management</t>
-  </si>
-  <si>
-    <t>Mastering your own specialties</t>
-  </si>
-  <si>
-    <t>You sit before the fire of your home, sifting through papers and contemplating what the next project will be.&lt;br /&gt; &lt;br /&gt; One of your counselors knocks on the door and you rise to greet them, beckoning them to come in.&lt;br /&gt; &lt;br /&gt; “Your majesty, there is a letter from a man known as The Guide, for you to meet him at the Dragon Cliffs.”&lt;br /&gt; &lt;br /&gt; You take the letter and read it twice.&lt;br /&gt; &lt;br /&gt; After two days of preparations, you set out, alone, towards your destination. It takes two weeks to arrive at your destination. You make you way to the cliffs, shaped like a dragons head and see the guide sitting on ground looking ahead. He is young again.&lt;br /&gt; &lt;br /&gt; You approach him and announce your self. He stands and turns to greet you.&lt;br /&gt; &lt;br /&gt; “Child. I have news of your parents. They are dead.”&lt;br /&gt; &lt;br /&gt; The world stops for what seems like an eternity. Dead, how could they be dead. You set out not so long ago, you worked so hard to get to where you are. But the news of your parents being dead ---&lt;br /&gt; &lt;br /&gt; “Child! Pay attention.” A screeching voice interrupts your racing thoughts.&lt;br /&gt; &lt;br /&gt; “They were never your parents. It was all an illusion set up by The Poet.”&lt;br /&gt; &lt;br /&gt; Your entire life is a lie…</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Today we are going to learn about &lt;a href="/information/class-ranks" target="_blank"&gt;Class Ranks&lt;/a&gt;. Class Ranks allows a character to do a couple of things:&lt;/p&gt;&lt;p&gt;- Switch classes at any time&lt;/p&gt;&lt;p&gt;- Gain more attack towards specific weapons&lt;/p&gt;&lt;p&gt;- Equip Special abilities that can do damage and increase aspects of your character&lt;/p&gt;&lt;p&gt;- Unlock new classes&lt;/p&gt;&lt;p&gt;A character may only have a total of three specialties equipped an of the three only one may of a specialty that deals damage.&lt;/p&gt;&lt;p&gt;Finally, specialties unlock as you level the class rank. So lets get into how to manage your class ranks on your character:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;: Under Equipped Specialties, you can unequipped them to then equip other specialties from other classes. As you switch classes and play around, you can mix and match specialties equipped for maximum damage and stats.&lt;/p&gt;&lt;p&gt;All of these specialties, masteries and class ranks will level over time by you killing monsters. No XP will be sacrificed like when you train skills, instead this is a separate XP curve for each of the sections.&lt;/p&gt;&lt;p&gt;You server message section will also, as you may have seen, show you when you get levels in class specialties, ranks or masteries. For example maybe your class has recently level Weapon Masteries or Spell Masteries if you have been using those as your primary attack.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- Click on Character Sheet tab&lt;/p&gt;&lt;p&gt;- Click the orange button called Class Ranks&lt;/p&gt;&lt;p&gt;- Here you see a list of the games classes including some, marked by star, that require you to level other class ranks to specific levels.&lt;/p&gt;&lt;p&gt;- Click on your class in the list.&lt;/p&gt;&lt;p&gt;- Here you can you see details about your class, including the class masteries. These masteries are leveled over time by your having the weapon/spell type equipped at the time of fighting monsters.&lt;/p&gt;&lt;p&gt;- Above the class name is a red circle with a minus through it, clicking this will close this section, where as clicking X or the cancel button will close the class masteries modal.&lt;/p&gt;&lt;p&gt;- Next click “Manage Specialties”, this will open a secondary modal.&lt;/p&gt;&lt;p&gt;- These are specialties that unlock at the class rank level, you should – by now – have two specialties you can equip.&lt;/p&gt;&lt;p&gt;- You can investigate the specialties to see what they do. There are two types: Ones that increase specific attributes of your character over time, which are leveled by just fighting monsters and ones that do damage – which fire automatically when fighting monsters.&lt;/p&gt;&lt;p&gt;- Equip the required amount of specialties.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- Tap on Character Sheet tab&lt;/p&gt;&lt;p&gt;- Open the top section and tap on the orange button called Class Ranks&lt;/p&gt;&lt;p&gt;- Here you see a list of the games classes including some, marked by star, that require you to level other class ranks to specific levels.&lt;/p&gt;&lt;p&gt;- Click on your class in the list.&lt;/p&gt;&lt;p&gt;- Here you can you see details about your class, including the class masteries. These masteries are leveled over time by your having the weapon/spell type equipped at the time of fighting monsters.&lt;/p&gt;&lt;p&gt;- Above the class name is a red circle with a minus through it, clicking this will close this section, where as clicking X or the cancel button will close the class masteries modal.&lt;/p&gt;&lt;p&gt;- Next click “Manage Specialties”, this will open a secondary modal.&lt;/p&gt;&lt;p&gt;- These are specialties that unlock at the class rank level, you should – by now – have two specialties you can equip.&lt;/p&gt;&lt;p&gt;- You can investigate the specialties to see what they do. There are two types: Ones that increase specific attributes of your character over time, which are leveled by just fighting monsters and ones that do damage – which fire automatically when fighting monsters.&lt;/p&gt;&lt;p&gt;- Equip the required amount of specialties.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>The void in your heart</t>
-  </si>
-  <si>
-    <t>You find it hard to breathe. Your vision is blurred, you grasp for a sense of stability.&lt;br /&gt; &lt;br /&gt; A slap across the face, the ringing pain of the hand connecting with your face, reality comes back.&lt;br /&gt; &lt;br /&gt; Your parents are not your parents. Everything is a lie.&lt;br /&gt; &lt;br /&gt; You stare at the man who slapped you. What is going on?&lt;br /&gt; &lt;br /&gt; The Poet …&lt;br /&gt; &lt;br /&gt; “… He said something about how we need a way to lock The Creator back up. He mentioned that we could use the magic of the universe to open portals, to create lives, to build an army of … Well you …”&lt;br /&gt; &lt;br /&gt; You look at your hands, your body before you. A creation of universal magic?&lt;br /&gt; &lt;br /&gt; “You are real … Not just some kind of magical construct. You are …. real.”&lt;br /&gt; &lt;br /&gt; Real.&lt;br /&gt; &lt;br /&gt; Vomit.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Today we want to learn about &lt;a href="/information/voidance" target="_blank"&gt;Devouring Light/Darkness&lt;/a&gt;. One lets you void your enemy so their enchantments do not fire and over all they do less damage.&lt;/p&gt;&lt;p&gt;The problem with that. Is that enemies can do the same to you. So to counter an enemy voiding you, making your character use only raw stats and no enchantments, you use whats called Devoid.&lt;/p&gt;&lt;p&gt;Devoid allows you to “Void the enemies ability to void your enchantments.” Which in turn allows the you to then: Void the enemy, so their enchantments do not fire.&lt;/p&gt;&lt;p&gt;On top of this there is also Resistance to both of these that character can obtain, so that you can resist the enemies ability to void you, even if you fail to “Devoid” them.&lt;/p&gt;&lt;p&gt;From Surface to Hell, you will devoid followed by a void first, where as in Purgatory Enemies will devoid followed by a void first, which is where the resistance comes in handy.&lt;/p&gt;&lt;p&gt;To get the Devouring Light/Darkness % up, which can be seen on The Character Sheet: Additional Information (Orange Button) → Voidance tab, you will have to complete the Quest, on Surface called: Return of the King’s Crown.&lt;/p&gt;&lt;p&gt;This will cost a lot of Gold Dust and the easiest way to get it, while you train Looting is to train Enchanting, enchant and then disenchant to gain gold dust.&lt;/p&gt;&lt;p&gt;The item you receive is called: Dead King's Crown. This allows you to gain 100% in Devouring Light (Voidance) and 85% in Devouring Darkness (DeVoid), which will make harder creatures much easier to take on.&lt;/p&gt;&lt;p&gt;Voidance and Devoidance becomes useful in Shadow Planes, Hell and Purgatory (&lt;a href="/information/planes" target="_blank"&gt;Planes&lt;/a&gt;) as well as &lt;a href="/information/special-locations" target="_blank"&gt;Special Locations&lt;/a&gt;.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Complete the required quests needed to be able to complete the required quest. All these quests can be done on Surface.&lt;/p&gt;&lt;p&gt;You can see your voidance information by going to your character sheet and clicking Additional Information Orange button and from there click the voidance tab. Here you can see your Devouring Light and Darkness.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Complete the required quests needed to be able to complete the required quest. All these quests can be done on Surface.&lt;/p&gt;&lt;p&gt;You can see your voidance information by going to your character sheet, expanding the top section, and clicking Additional Information Orange button and from there click the voidance tab. Here you can see your Devouring Light and Darkness.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Dead King's Crown</t>
   </si>
 </sst>
 </file>
@@ -753,7 +669,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AR15"/>
+  <dimension ref="A1:AS10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -762,9 +678,9 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="3.428" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="36.42" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="2194.179" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="2102.201" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="31.707" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="1886.254" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="2145.762" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="1594.896" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="1625.603" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="17.567" bestFit="true" customWidth="true" style="0"/>
@@ -779,35 +695,36 @@
     <col min="16" max="16" width="29.421" bestFit="true" customWidth="true" style="0"/>
     <col min="17" max="17" width="41.133" bestFit="true" customWidth="true" style="0"/>
     <col min="18" max="18" width="38.848" bestFit="true" customWidth="true" style="0"/>
-    <col min="19" max="19" width="23.423" bestFit="true" customWidth="true" style="0"/>
-    <col min="20" max="20" width="26.993" bestFit="true" customWidth="true" style="0"/>
-    <col min="21" max="21" width="24.708" bestFit="true" customWidth="true" style="0"/>
-    <col min="22" max="22" width="21.138" bestFit="true" customWidth="true" style="0"/>
-    <col min="23" max="23" width="26.993" bestFit="true" customWidth="true" style="0"/>
-    <col min="24" max="24" width="28.136" bestFit="true" customWidth="true" style="0"/>
-    <col min="25" max="25" width="16.425" bestFit="true" customWidth="true" style="0"/>
-    <col min="26" max="26" width="22.28" bestFit="true" customWidth="true" style="0"/>
-    <col min="27" max="27" width="18.71" bestFit="true" customWidth="true" style="0"/>
-    <col min="28" max="28" width="21.138" bestFit="true" customWidth="true" style="0"/>
-    <col min="29" max="29" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="19" max="19" width="30.564" bestFit="true" customWidth="true" style="0"/>
+    <col min="20" max="20" width="23.423" bestFit="true" customWidth="true" style="0"/>
+    <col min="21" max="21" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="22" max="22" width="24.708" bestFit="true" customWidth="true" style="0"/>
+    <col min="23" max="23" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="24" max="24" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="25" max="25" width="28.136" bestFit="true" customWidth="true" style="0"/>
+    <col min="26" max="26" width="16.425" bestFit="true" customWidth="true" style="0"/>
+    <col min="27" max="27" width="22.28" bestFit="true" customWidth="true" style="0"/>
+    <col min="28" max="28" width="18.71" bestFit="true" customWidth="true" style="0"/>
+    <col min="29" max="29" width="21.138" bestFit="true" customWidth="true" style="0"/>
     <col min="30" max="30" width="26.993" bestFit="true" customWidth="true" style="0"/>
     <col min="31" max="31" width="26.993" bestFit="true" customWidth="true" style="0"/>
     <col min="32" max="32" width="26.993" bestFit="true" customWidth="true" style="0"/>
-    <col min="33" max="33" width="17.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="34" max="34" width="15.282" bestFit="true" customWidth="true" style="0"/>
+    <col min="33" max="33" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="34" max="34" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="35" max="35" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="36" max="36" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="37" max="37" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="38" max="38" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="39" max="39" width="15.282" bestFit="true" customWidth="true" style="0"/>
-    <col min="40" max="40" width="17.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="41" max="41" width="19.995" bestFit="true" customWidth="true" style="0"/>
-    <col min="42" max="42" width="16.425" bestFit="true" customWidth="true" style="0"/>
-    <col min="43" max="43" width="13.997" bestFit="true" customWidth="true" style="0"/>
-    <col min="44" max="44" width="11.711" bestFit="true" customWidth="true" style="0"/>
+    <col min="40" max="40" width="15.282" bestFit="true" customWidth="true" style="0"/>
+    <col min="41" max="41" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="42" max="42" width="19.995" bestFit="true" customWidth="true" style="0"/>
+    <col min="43" max="43" width="16.425" bestFit="true" customWidth="true" style="0"/>
+    <col min="44" max="44" width="13.997" bestFit="true" customWidth="true" style="0"/>
+    <col min="45" max="45" width="11.711" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44">
+    <row r="1" spans="1:45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -940,277 +857,286 @@
       <c r="AR1" t="s">
         <v>43</v>
       </c>
+      <c r="AS1" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="2" spans="1:44">
+    <row r="2" spans="1:45">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G2">
         <v>2</v>
       </c>
-      <c r="AQ2">
+      <c r="AR2">
         <v>500</v>
       </c>
-      <c r="AR2">
+      <c r="AS2">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:44">
+    <row r="3" spans="1:45">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G3">
         <v>10</v>
       </c>
-      <c r="AQ3">
+      <c r="AR3">
         <v>500</v>
       </c>
-      <c r="AR3">
+      <c r="AS3">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:44">
+    <row r="4" spans="1:45">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G4">
         <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I4">
         <v>10</v>
       </c>
       <c r="J4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="K4">
         <v>15</v>
       </c>
-      <c r="AG4">
+      <c r="AH4">
         <v>50</v>
       </c>
-      <c r="AQ4">
+      <c r="AR4">
         <v>1000</v>
       </c>
-      <c r="AR4">
+      <c r="AS4">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:44">
+    <row r="5" spans="1:45">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G5">
         <v>50</v>
       </c>
       <c r="H5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I5">
         <v>5</v>
       </c>
       <c r="J5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K5">
         <v>5</v>
       </c>
-      <c r="W5" t="s">
-        <v>68</v>
-      </c>
       <c r="X5" t="s">
         <v>69</v>
       </c>
-      <c r="AQ5">
+      <c r="Y5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR5">
         <v>1000</v>
       </c>
-      <c r="AR5">
+      <c r="AS5">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:44">
+    <row r="6" spans="1:45">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G6">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="H6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I6">
         <v>5</v>
       </c>
       <c r="J6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K6">
         <v>15</v>
       </c>
-      <c r="W6" t="s">
-        <v>76</v>
-      </c>
-      <c r="AK6">
-        <v>150</v>
-      </c>
-      <c r="AQ6">
+      <c r="X6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL6">
+        <v>125</v>
+      </c>
+      <c r="AR6">
         <v>10000</v>
       </c>
-      <c r="AR6">
+      <c r="AS6">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:44">
+    <row r="7" spans="1:45">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7">
         <v>80</v>
       </c>
-      <c r="F7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G7">
-        <v>120</v>
-      </c>
       <c r="H7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I7">
         <v>25</v>
       </c>
-      <c r="U7" t="s">
-        <v>82</v>
-      </c>
-      <c r="W7" t="s">
+      <c r="T7" t="s">
         <v>83</v>
       </c>
-      <c r="AG7">
-        <v>250</v>
-      </c>
-      <c r="AQ7">
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7" t="s">
+        <v>83</v>
+      </c>
+      <c r="X7" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH7">
+        <v>150</v>
+      </c>
+      <c r="AR7">
         <v>100000</v>
       </c>
-      <c r="AR7">
+      <c r="AS7">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:44">
+    <row r="8" spans="1:45">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G8">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="H8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I8">
         <v>15</v>
       </c>
       <c r="J8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K8">
         <v>5</v>
@@ -1221,93 +1147,93 @@
       <c r="M8">
         <v>10</v>
       </c>
-      <c r="W8" t="s">
-        <v>91</v>
-      </c>
-      <c r="Z8">
+      <c r="X8" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA8">
         <v>500</v>
       </c>
-      <c r="AG8">
+      <c r="AH8">
         <v>280</v>
-      </c>
-      <c r="AO8">
-        <v>5000</v>
       </c>
       <c r="AP8">
         <v>500</v>
       </c>
       <c r="AQ8">
+        <v>0</v>
+      </c>
+      <c r="AR8">
         <v>100000</v>
       </c>
-      <c r="AR8">
+      <c r="AS8">
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:44">
+    <row r="9" spans="1:45">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G9">
         <v>200</v>
       </c>
       <c r="H9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I9">
         <v>50</v>
       </c>
-      <c r="U9" t="s">
-        <v>97</v>
-      </c>
-      <c r="W9" t="s">
+      <c r="V9" t="s">
         <v>98</v>
       </c>
       <c r="X9" t="s">
         <v>99</v>
       </c>
-      <c r="AG9">
+      <c r="Y9" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH9">
         <v>350</v>
       </c>
-      <c r="AQ9">
+      <c r="AR9">
         <v>250000</v>
       </c>
-      <c r="AR9">
+      <c r="AS9">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:44">
+    <row r="10" spans="1:45">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G10">
         <v>250</v>
@@ -1316,220 +1242,27 @@
         <v>13</v>
       </c>
       <c r="M10">
-        <v>35</v>
-      </c>
-      <c r="AG10">
+        <v>10</v>
+      </c>
+      <c r="T10" t="s">
+        <v>98</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="AH10">
         <v>450</v>
       </c>
-      <c r="AO10">
+      <c r="AP10">
         <v>10000</v>
       </c>
-      <c r="AP10">
+      <c r="AQ10">
         <v>200</v>
       </c>
-      <c r="AQ10">
+      <c r="AR10">
         <v>100000</v>
       </c>
-      <c r="AR10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:44">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D11" t="s">
-        <v>106</v>
-      </c>
-      <c r="E11" t="s">
-        <v>107</v>
-      </c>
-      <c r="F11" t="s">
-        <v>108</v>
-      </c>
-      <c r="G11">
-        <v>300</v>
-      </c>
-      <c r="N11" t="s">
-        <v>109</v>
-      </c>
-      <c r="O11" t="s">
-        <v>110</v>
-      </c>
-      <c r="P11">
-        <v>2</v>
-      </c>
-      <c r="Q11">
-        <v>2</v>
-      </c>
-      <c r="AG11">
-        <v>550</v>
-      </c>
-      <c r="AO11">
-        <v>1000</v>
-      </c>
-      <c r="AP11">
-        <v>1000</v>
-      </c>
-      <c r="AQ11">
-        <v>1000000</v>
-      </c>
-      <c r="AR11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:44">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>111</v>
-      </c>
-      <c r="C12" t="s">
-        <v>112</v>
-      </c>
-      <c r="D12" t="s">
-        <v>113</v>
-      </c>
-      <c r="E12" t="s">
-        <v>114</v>
-      </c>
-      <c r="F12" t="s">
-        <v>115</v>
-      </c>
-      <c r="AB12">
-        <v>1</v>
-      </c>
-      <c r="AC12">
-        <v>20</v>
-      </c>
-      <c r="AD12">
-        <v>100</v>
-      </c>
-      <c r="AQ12">
-        <v>1000</v>
-      </c>
-      <c r="AR12">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:44">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>116</v>
-      </c>
-      <c r="C13" t="s">
-        <v>117</v>
-      </c>
-      <c r="D13" t="s">
-        <v>118</v>
-      </c>
-      <c r="E13" t="s">
-        <v>119</v>
-      </c>
-      <c r="F13" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC13">
-        <v>40</v>
-      </c>
-      <c r="AD13">
-        <v>500</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>121</v>
-      </c>
-      <c r="AF13">
-        <v>1</v>
-      </c>
-      <c r="AQ13">
-        <v>2500</v>
-      </c>
-      <c r="AR13">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:44">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>122</v>
-      </c>
-      <c r="C14" t="s">
-        <v>123</v>
-      </c>
-      <c r="D14" t="s">
-        <v>124</v>
-      </c>
-      <c r="E14" t="s">
-        <v>125</v>
-      </c>
-      <c r="F14" t="s">
-        <v>126</v>
-      </c>
-      <c r="R14">
-        <v>2</v>
-      </c>
-      <c r="AQ14">
-        <v>20000</v>
-      </c>
-      <c r="AR14">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:44">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>127</v>
-      </c>
-      <c r="C15" t="s">
-        <v>128</v>
-      </c>
-      <c r="D15" t="s">
-        <v>129</v>
-      </c>
-      <c r="E15" t="s">
-        <v>130</v>
-      </c>
-      <c r="F15" t="s">
-        <v>131</v>
-      </c>
-      <c r="H15" t="s">
-        <v>60</v>
-      </c>
-      <c r="I15">
-        <v>75</v>
-      </c>
-      <c r="J15" t="s">
-        <v>89</v>
-      </c>
-      <c r="K15">
-        <v>50</v>
-      </c>
-      <c r="W15" t="s">
-        <v>132</v>
-      </c>
-      <c r="AO15">
-        <v>5000</v>
-      </c>
-      <c r="AP15">
-        <v>1000</v>
-      </c>
-      <c r="AQ15">
-        <v>1000000</v>
-      </c>
-      <c r="AR15">
+      <c r="AS10">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Various fixes and updates as well as changes to guide quests.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="143">
   <si>
     <t>id</t>
   </si>
@@ -326,10 +326,124 @@
     <t>The Dungeons plane crawls with death. There is a darkness that seeps across the ground, infecting and infesting everything that it touches. You seem to be immune to it. You know there is shadow in the distance that is watching you. A shade like creature that only makes it’s self visible every now and then to your eyes.&lt;br /&gt; &lt;br /&gt; “Child!” Comes a familiar voice. The Guide, young, handsome and ever changing comes up to you.&lt;br /&gt; &lt;br /&gt; “You have come down the Dungeons. A place of ruins, crypts, caves and other bits of darkness that one can explore for loot.”&lt;br /&gt; &lt;br /&gt; You ask him about the darkness crawling across the land and the shade like creature you can see off in the distance.&lt;br /&gt; &lt;br /&gt; “The darkness is caused by the gates of Shadow Planes, which has opened. The shade creature is the Shade Lord. He is seeking something, something that escaped the darkness beneath the pits of Hell. Alas to take on any of these creatures you need to get stronger!”</t>
   </si>
   <si>
-    <t>&lt;p&gt;Now we learn about a new feature: &lt;a href="/information/class-skills" target="_blank"&gt;Class Skills&lt;/a&gt; and Class Bonus.&lt;/p&gt;&lt;p&gt;Class Skills are different for each &lt;a href="/information/races-and-classes#3" target="_blank"&gt;class&lt;/a&gt; in the game. Every class has a skill which you can see on your skills table under Training Tab. It has an icon beside it and is in orange text.&lt;/p&gt;&lt;p&gt;This skill important to level because it allows you to increase your Class Bonus which can be seen on the character sheet to the left, under inventory count or on mobile under Class Details, at the bottom of the details section.&lt;/p&gt;&lt;p&gt;Your class will tell you, if you click/tap on the class name in the top bar where you basic details are, the requirements for your class special attack to fire. This means what weapons or spells you must have equipped and how many. If you also need to use a specific attack type or not.&lt;/p&gt;&lt;p&gt;Based on those factors and the % of your class bonus, your special can just fire in the middle of an attack, which you will see when manually fighting.&lt;/p&gt;&lt;p&gt;Each class has it’s own special attack and special rules for those attacks.&lt;/p&gt;&lt;p&gt;Class Skills can also raise specific attributes about the class such as damage, healing and armour class bonuses that stack with all other bonuses.&lt;/p&gt;&lt;p&gt;At this stage in the game, the one important thing I can tell you is: unless it states that it wont stack, everything stacks together to raise your stats, damage, armour class, healing as well as stats, skills and so on.&lt;/p&gt;&lt;p&gt;When utilizing, as we will soon, &lt;a href="/information/class-ranks" target="_blank"&gt;Class Ranks&lt;/a&gt; to switch classes, you will notice that one skill on your Skills tab on the Character Sheet, will change. Every time you change a class your character will switch their class skill.&lt;/p&gt;</t>
+    <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; &lt;em&gt;This quest can take 2 hours or more to complete.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Now we learn about a new feature: &lt;a href="/information/class-skills" target="_blank"&gt;Class Skills&lt;/a&gt; and Class Bonus.&lt;/p&gt;&lt;p&gt;Class Skills are different for each &lt;a href="/information/races-and-classes#3" target="_blank"&gt;class&lt;/a&gt; in the game. Every class has a skill which you can see on your skills table under Training Tab. It has an icon beside it and is in orange text.&lt;/p&gt;&lt;p&gt;This skill important to level because it allows you to increase your Class Bonus which can be seen on the character sheet to the left, under inventory count or on mobile under Class Details, at the bottom of the details section.&lt;/p&gt;&lt;p&gt;Your class will tell you, if you click/tap on the class name in the top bar where you basic details are, the requirements for your class special attack to fire. This means what weapons or spells you must have equipped and how many. If you also need to use a specific attack type or not.&lt;/p&gt;&lt;p&gt;Based on those factors and the % of your class bonus, your special can just fire in the middle of an attack, which you will see when manually fighting.&lt;/p&gt;&lt;p&gt;Each class has it’s own special attack and special rules for those attacks.&lt;/p&gt;&lt;p&gt;Class Skills can also raise specific attributes about the class such as damage, healing and armour class bonuses that stack with all other bonuses.&lt;/p&gt;&lt;p&gt;At this stage in the game, the one important thing I can tell you is: unless it states that it wont stack, everything stacks together to raise your stats, damage, armour class, healing as well as stats, skills and so on.&lt;/p&gt;&lt;p&gt;When utilizing, as we will soon, &lt;a href="/information/class-ranks" target="_blank"&gt;Class Ranks&lt;/a&gt; to switch classes, you will notice that one skill on your Skills tab on the Character Sheet, will change. Every time you change a class your character will switch their class skill.&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;- The instructions state to level a Effects Class to the specified level. To do this, go to your character sheet section, in your skill section – train the skill with the orange text to the specified level.&lt;/p&gt;&lt;p&gt;- To Get the Gold Dust you can disenchant items that drop you no longer need, or craft some items, enchant them and disenchant them. Now is the time to explore the &lt;a href="http://127.0.0.1:8000/information/enchanting" target="_blank"&gt;Enchanting&lt;/a&gt; list in the docs to see what types of enchantments you can apply to your equipment so you can start creating a gear set geared towards your needs.&lt;/p&gt;&lt;p&gt;That’s it. Now you might not see your class bonus fire off much at first, but over time, keep leveling this skill and you will start to see your special fire off automatically when manually fighting.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Dancing Shadows</t>
+  </si>
+  <si>
+    <t>You're bones ache, your body is bruised, your strength is depleted. You lie upon the ground, broken bits of buildings, scattered across the ground show you the ruins of this plane.&lt;br /&gt; &lt;br /&gt; Your memory drifts back to the days when you were carefree, young and playing in the fields while your parents worked in the fields.&lt;br /&gt; &lt;br /&gt; You remember the house, the laughter, the Sunday dinners and the other farm kids when it came time to harvest. The bountiful parties, the celebrations of summer transitioning to fall.&lt;br /&gt; &lt;br /&gt; You miss your home, you miss your family.&lt;br /&gt; &lt;br /&gt; Your eye catches the shadow in the distance, a shadow on the end of the small campfire flame that you burn in the darkness of this plane.&lt;br /&gt; &lt;br /&gt; The shadow dances.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; &lt;em&gt;This quest can take 2 hours or more to complete.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Lets learn about &lt;a href="/information/class-ranks" target="_blank"&gt;Class Ranks&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;Class ranks are, for those familiar, similar to Final Fantasy Job Switching mechanics – which are present in a verity of other RPG’s.&lt;/p&gt;&lt;p&gt;At any time, a character may switch classes by utilizing the class rank system. Each class is leveled by simply killing creatures, as you level the class you unlock special abilities that you can equip and further level to gain additional benefits and modifiers.&lt;/p&gt;&lt;p&gt;Some abilities can only be equipped when you have leveled that class rank (by being that class and killing creatures) to the required level. And other abilities, such as those that do damage, cannot stack or be equipped while others of that type are equipped.&lt;/p&gt;&lt;p&gt;This is another layer of character development, as you can mix and match abilities from various classes to create your own build.&lt;/p&gt;&lt;p&gt;Some classes in Class Ranks cannot be switched to until you have leveled other classes to a specific class rank, these classes, like Prisoner – for example – cannot be selected at registration for this reason.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Lets level our current Class Rank and equip a class special.&lt;/p&gt;&lt;p&gt;To do this:&lt;/p&gt;&lt;p&gt;- Go to your Character Sheet Tab.&lt;/p&gt;&lt;p&gt;- Click the orange button called Class Ranks&lt;/p&gt;&lt;p&gt;- Find your class in the list, beside the name is the level – you will need to raise this to meet the requirement. You do this via exploration.&lt;/p&gt;&lt;p&gt;- Click the class name. Here you can see details about your class, including mastery's which level in the same fashion as Class Ranks, by killing creatures – with the caveat that you have the item equipped.&lt;/p&gt;&lt;p&gt;- You will also see a red circle with a minus in it. Click this at any time to close the class details and see your class rank list. Clicking cancel at this state will close this modal.&lt;/p&gt;&lt;p&gt;- Click Manage Specialties. This will open a secondary modal that shows you the class specials you can equip. You may only equip 3, and only one of those three may be a special that deals damage. If you have one that deals damage (click the name to see further details) – and you can equip it, do so. If not find one that you can equip and equip it.&lt;/p&gt;&lt;p&gt;By equipping a class special, you will level it via killing creatures. The longer you leave it equipped the more levels, the more benefit it gives.&lt;/p&gt;&lt;p&gt;- Now, kill something – many times over. These will not take long to level, keep an eye on the Server Messages tab for levels – you may have already seen these pop up over time.&lt;/p&gt;&lt;p&gt;Let’s also do some crafting. Consider this a “where are you in your crafting and enchanting?”&lt;/p&gt;&lt;p&gt;If you can, equip a full set of the crafting type required enchantments on the best gear you can craft. This will help you reach the crafting requirement faster. If you then switch to a set of enchantment skill raising enchantments and then enchant all that crafted gear and finally disenchant it all, you will level both enchanting and disenchanting, and leveling disenchanting gets you more Gold Dust per disenchanted item.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Lets level our current Class Rank and equip a class special.&lt;/p&gt;&lt;p&gt;To do this:&lt;/p&gt;&lt;p&gt;- Tap Character Sheet Tab&lt;/p&gt;&lt;p&gt;- Tap to expand the Character Details&lt;/p&gt;&lt;p&gt;- Find the Orange Button: Class Ranks, Tap It.&lt;/p&gt;&lt;p&gt;- Tap the class name. Here you can see details about your class, including mastery's which level in the same fashion as Class Ranks, by killing creatures – with the caveat that you have the item equipped.&lt;/p&gt;&lt;p&gt;- You will also see a red circle with a minus in it. Click this at any time to close the class details and see your class rank list. Clicking cancel at this state will close this modal.&lt;/p&gt;&lt;p&gt;- Tap Manage Specialties. This will open a secondary modal that shows you the class specials you can equip. You may only equip 3, and only one of those three may be a special that deals damage. If you have one that deals damage (click the name to see further details) – and you can equip it, do so. If not find one that you can equip and equip it.&lt;/p&gt;&lt;p&gt;By equipping a class special, you will level it via killing creatures. The longer you leave it equipped the more levels, the more benefit it gives.&lt;/p&gt;&lt;p&gt;- Now, kill something – many times over. These will not take long to level, keep an eye on the Server Messages tab for levels – you may have already seen these pop up over time.&lt;/p&gt;&lt;p&gt;Let’s also do some crafting. Consider this a “where are you in your crafting and enchanting?”&lt;/p&gt;&lt;p&gt;If you can, equip a full set of the crafting type required enchantments on the best gear you can craft. This will help you reach the crafting requirement faster. If you then switch to a set of enchantment skill raising enchantments and then enchant all that crafted gear and finally disenchant it all, you will level both enchanting and disenchanting, and leveling disenchanting gets you more Gold Dust per disenchanted item.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Hired Help</t>
+  </si>
+  <si>
+    <t>Your strength seems to be restored from a night by the fire. The ruins of the various dungeons, castles and other structures that litter this land much like labyrinth, holds an eerie silence in the early morning hours.&lt;br /&gt; &lt;br /&gt; The fog and the dampness in the air create a chill that seeps into your bones and causes a shiver. Suddenly on the outskirts of the fog is a shade like creature that stands there, watching, waiting. You stand and shout, but the fog makes the creature disappear deeper into the silence.&lt;br /&gt; &lt;br /&gt; You head off towards the direction of the creature, weapons ready and spells glowing. You search th fog, turning this way and that – you see nothing, you feel the presence. It touches you and you feel weaker, your enchantments, your own magic- it all melts away.&lt;br /&gt; &lt;br /&gt; A whisper: Strength.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;:&lt;strong&gt; &lt;/strong&gt;&lt;em&gt;This quest can take 2+ Hours to complete&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Lets learn about &lt;a href="/information/mercenary" target="_blank"&gt;mercenaries&lt;/a&gt;, which help with getting currencies through a mini game called &lt;a href="/information/slots" target="_blank"&gt;slots&lt;/a&gt;. How fun! Gambling!&lt;/p&gt;&lt;p&gt;Mercenaries are NPC’s who grant you a passive buff the more you level them and reincarnate them. The buff they give you is a % bonus towards the drop amount of that currency from slots and other aspects of the game.&lt;/p&gt;&lt;p&gt;For example, The child of gold dust is a mercenary that allows you to gain +x% based on it’s current level, towards any action that would give you gold dust.&lt;/p&gt;&lt;p&gt;The beauty with mercenaries is that they also stack with the event: Weekly Currency Drop for even more currencies.&lt;/p&gt;&lt;p&gt;Mercenaries, once they reach level 100, can be reincarnated to increase the bonus towards currency acquisition. Mercenaries are purchased and require you to complete the quest listed to unlock them.&lt;/p&gt;&lt;p&gt;Mercenaries gain levels by you fighting monsters.&lt;/p&gt;&lt;p&gt;Purchase the mercenaries required for this quest, after completing the required quest.&lt;/p&gt;&lt;p&gt;Slots are a way for characters to make passive income. You can get Gold, Shards, Gold Dust and Copper Coins. Copper coins will not drop for you yet because you do not have the required quest item yet.&lt;/p&gt;&lt;p&gt;Slots take gold to spin and can, with the aid of mercenaries, reward the player with a godly amount of currency.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;By now we know how to utilize exploration and question. So lets quest to unlock mercenaries and then use a new feature while we have exploration running to gain some currencies from slots.&lt;/p&gt;&lt;p&gt;- First complete the quest: &lt;strong&gt;The truth is Out There&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Next go to Character Sheet and click on the Mercenaries Tab&lt;/p&gt;&lt;p&gt;- Select the required mercenaries as shown above and purchase them.&lt;/p&gt;&lt;p&gt;- Level them to the required level via exploration.&lt;/p&gt;&lt;p&gt;- Next, in the action section, click slots.&lt;/p&gt;&lt;p&gt;- Spin baby spin!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;By now we know how to utilize exploration and question. So lets quest to unlock mercenaries and then use a new feature while we have exploration running to gain some currencies from slots.&lt;/p&gt;&lt;p&gt;- First complete the quest: &lt;strong&gt;The truth is Out There&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Next go to Character Sheet and tap on the Mercenaries Tab&lt;/p&gt;&lt;p&gt;- Select the required mercenaries as shown above and purchase them.&lt;/p&gt;&lt;p&gt;- Level them to the required level via exploration.&lt;/p&gt;&lt;p&gt;- Next, in the action section, select slots from the action drop down.&lt;/p&gt;&lt;p&gt;- Spin baby spin!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>child-of-gold-dust</t>
+  </si>
+  <si>
+    <t>child-of-shards</t>
+  </si>
+  <si>
+    <t>The truth is out there</t>
+  </si>
+  <si>
+    <t>Alchemical dreams</t>
+  </si>
+  <si>
+    <t>An old man sits on the edge of your vision. He walks, slowly towards you. The bottles clink together and he speaks in riddles. Your head spins. The shade is at the other side of the horizon. Follow him child and create the doors you need to open.&lt;br /&gt; &lt;br /&gt; You can hear a bang in the distance, once that gets louder and passes you buy. A scream, a cry, a death curdling scream of pain and loss permeates your heart.&lt;br /&gt; &lt;br /&gt; You feel the pain, you see the darkness, you can feel the blood, coming from your head. Why are you bleeding.&lt;br /&gt; &lt;br /&gt; You collapse into the sweet embrace of the shadows arms as it reaches out to take your limp body into the horizon.&lt;br /&gt; &lt;br /&gt; “Child.” You awaken in a strange place, but you recognize the man before you, The Poet.&lt;br /&gt; &lt;br /&gt; Why is here.&lt;br /&gt; &lt;br /&gt; “I want to tell you about the potions, the drinks for the various ways you can craft your own power, if only limited for a time.”&lt;br /&gt; &lt;br /&gt; His voice fades, and you fall to the ground.&lt;br /&gt; &lt;br /&gt; “Child?”</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;:&lt;strong&gt; &lt;/strong&gt;&lt;em&gt;This quest can take 2+ Hours to complete&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Another mechanic that players can user to make them selves powerful, even if only for a brief time is through the concept of boons. &lt;a href="/information/alchemy" target="_blank"&gt;Boons&lt;/a&gt; are timed effects that last minutes on a character and can, in some cases and unless otherwise stated, stack with each other to give you even more power.&lt;/p&gt;&lt;p&gt;There are two ways to get boons: &lt;a href="/information/goblin-shop" target="_blank"&gt;The Goblin shop&lt;/a&gt; sells some powerful ones for Gold bars which are only obtainable by owning kingdoms and making vast amounts of gold, and then Alchemy. Which we will talk about.&lt;/p&gt;&lt;p&gt;Alchemy is a crafting skill that requires you to complete a one off quest on Surface called &lt;strong&gt;I dream of Alchemy&lt;/strong&gt;.&lt;/p&gt;&lt;p&gt;Once you have this quest complete the option will show up under the Craft/Enchant section.&lt;/p&gt;&lt;p&gt;Alchemy requires Gold Dust and Crystal Shards (Shards). One you get from disenchanting enchanted items and the other you get from killing &lt;a href="/information/celestials" target="_blank"&gt;celestials&lt;/a&gt;, which you are too weak for.&lt;/p&gt;&lt;p&gt;Alchemy items come in many forms, but there are three kinds: Stat Boosting, Kingdom Damage Dealing and Holy Oils for a later type of crafting. Some alchemy items like &lt;a href="/information/holy-items" target="_blank"&gt;Holy Oils&lt;/a&gt; can be applied to items, while kingdom damaging items can be used on other players kingdoms and stat boosting are usable items that can be used on your self to create boons.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;- Complete the quest: &lt;strong&gt;I dream of Alchemy&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Open Craft/Enchant&lt;/p&gt;&lt;p&gt;- Select Alchemy&lt;/p&gt;&lt;p&gt;- Select an item&lt;/p&gt;&lt;p&gt;- Craft the item, repeat.&lt;/p&gt;&lt;p&gt;You should have enough shards and gold dust to reach the desired level.&lt;/p&gt;&lt;p&gt;To use an item on your self, assuming it is usable on you, follow the below steps:&lt;/p&gt;&lt;p&gt;- Click Character Sheet Tab&lt;/p&gt;&lt;p&gt;- Select Usable From the Type drop down in your inventory section.&lt;/p&gt;&lt;p&gt;- Here you can see your usable items.&lt;/p&gt;&lt;p&gt;- You can either use your items individually from the actions drop down beside them, or you can select Use Many from the Actions drop down above the usable table.&lt;/p&gt;&lt;p&gt;- Use many will filter out any item that cannot stack, that is, you cannot select multiple to apply to your self.&lt;/p&gt;&lt;p&gt;Items you use on your self will show up in the Active Boons Tab of the character information in the top left of the character sheet tab.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;- Complete the quest: &lt;strong&gt;I dream of Alchemy&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;Open Crafting from the actions drop down&lt;/p&gt;&lt;p&gt;- Open Craft/Enchant&lt;/p&gt;&lt;p&gt;- Select Alchemy&lt;/p&gt;&lt;p&gt;- Select an item&lt;/p&gt;&lt;p&gt;- Craft the item, repeat.&lt;/p&gt;&lt;p&gt;You should have enough shards and gold dust to reach the desired level.&lt;/p&gt;&lt;p&gt;To use an item on your self, assuming it is usable on you, follow the below steps:&lt;/p&gt;&lt;p&gt;- Tap Character Sheet Tab&lt;/p&gt;&lt;p&gt;- Select Inventory management from the drop down&lt;/p&gt;&lt;p&gt;- Select Usable From the Type drop down in your inventory section.&lt;/p&gt;&lt;p&gt;- Here you can see your usable items.&lt;/p&gt;&lt;p&gt;- You can either use your items individually from the actions drop down beside them, or you can select Use Many from the Actions drop down above the usable table.&lt;/p&gt;&lt;p&gt;- Use many will filter out any item that cannot stack, that is, you cannot select multiple to apply to your self.&lt;/p&gt;&lt;p&gt;Items you use on your self will show up in the Active Boons Tab which you can get to by expanding Character Details and tapping the Active Boons tab.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Alchemy</t>
+  </si>
+  <si>
+    <t>Ring Crafting</t>
+  </si>
+  <si>
+    <t>Home again Pt. 1</t>
+  </si>
+  <si>
+    <t>“Hullo?”&lt;br /&gt; &lt;br /&gt; A voice comes from the darkness of your dreams.&lt;br /&gt; &lt;br /&gt; You open your eyes and see a goblin standing before you, gently poking you with a stick. Yo8u bat away the stick and stand to greet this creature. He doesn’t seem dangerous.&lt;br /&gt; &lt;br /&gt; “You are alive!” The Goblin shrieks in joy.&lt;br /&gt; &lt;br /&gt; You ask him where you are rubbing the back of your neck and trying to orient your self to your surroundings.&lt;br /&gt; &lt;br /&gt; “Silly you. You are on surface.”&lt;br /&gt; &lt;br /&gt; You look around, the trees, the sky, the smells. How?&lt;br /&gt; &lt;br /&gt; “Do you want to play?"</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Look at you go, look at the distance you have traveled. The Gear, the monsters, the power! Alas, child you still have a long way to go and the next few steps will prepare you for the next leg of your journey!&lt;/p&gt;&lt;p&gt;We will help this goblin complete a few tasks and gain some items that will help our character out skill wise and for later quests.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Complete the required objectives using the knowledge you have gained so gar.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Surface</t>
+  </si>
+  <si>
+    <t>Faction Hunter</t>
+  </si>
+  <si>
+    <t>Home again pt. 2</t>
+  </si>
+  <si>
+    <t>You hang out with The Goblin for a while, realizing he is not as helpless as he appears to be. You slaughter a few creatures here and there, share a meal and discuss the events and his life.&lt;br /&gt; &lt;br /&gt; You stare at the stars each night wondering if everything you just experienced was a dream. You close your eyes.&lt;br /&gt; &lt;br /&gt; Blood, dripping down the wall, a metallic object on the floor, the lifeless and still hands of boy no older then 25 sits hunched against the wall, blood drips down from a wound in the head.&lt;br /&gt; &lt;br /&gt; A cream, a women. A scream. She rushes over. A scream – she grabs the child and holds his lifeless body close.&lt;br /&gt; &lt;br /&gt; “Child.”&lt;br /&gt; &lt;br /&gt; You turn around, a clearing, fields – summer breeze.&lt;br /&gt; &lt;br /&gt; “Wake up child.”&lt;br /&gt; &lt;br /&gt; The Poet. What is he doing here, you turn back but there stretches the ruins of a old world road, yellow paint lines the middle of the cracked and broken road.&lt;br /&gt; &lt;br /&gt; “Child.”&lt;br /&gt; &lt;br /&gt; You turn back, The Poet. He glows. The light is too bright.&lt;br /&gt; &lt;br /&gt; “It is not your time. Wake up.”&lt;br /&gt; &lt;br /&gt; You awaken to The Goblin staring at you.&lt;br /&gt; &lt;br /&gt; “You ok child?”</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Lets get some items that help with dodging enemies attacks and an item for helping with accuracy. To do this, we will do two more quests for The Goblin:&lt;/p&gt;&lt;p&gt;- &lt;strong&gt;Goblins gift&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- Goblins Accuracy&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;These can both be found on surface.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Golden Ring of Blur</t>
+  </si>
+  <si>
+    <t>The Book of Guidance</t>
+  </si>
+  <si>
+    <t>Dreams of the Dead</t>
+  </si>
+  <si>
+    <t>Days have gone by and no dream has haunted you like the previous one.&lt;br /&gt; &lt;br /&gt; Odd chores and bits and bobs around the small ramshackle camp you and The Goblin have set up.&lt;br /&gt; &lt;br /&gt; He comes into the camp with his bits and bobs and stolen items that he pick pocketed off wondering merchants. You peer through his treasures and find a letter.&lt;br /&gt; &lt;br /&gt; “Whats ya got there?” The goblin asks snatching the letter away.&lt;br /&gt; &lt;br /&gt; “Seems to be addressed to you! How unique!”&lt;br /&gt; &lt;br /&gt; You take the letter back from him and read the contents, it’s from The Poet&lt;br /&gt; &lt;br /&gt; Seems you have been busy my child. I need your assistance in a place far from the comforts of home. Alas for you to open such gates you must survive the trials and become stronger, unlocking a power with in your self.&lt;br /&gt; &lt;br /&gt; There is a crown, from a king long dead. His crown will help you take on even stronger creatures, creatures that can look at you and make you weak! Make your spells fail, your enchantments fizzle and fail. These creatures are fearsome.&lt;br /&gt; &lt;br /&gt; Alas, your adventures will take you deeper into those dreams of yours …&lt;br /&gt; &lt;br /&gt; The Poet&lt;br /&gt; &lt;br /&gt; You look up from the letter and The Goblin looks at you:&lt;br /&gt; &lt;br /&gt; “Whats up?Where are we off too?”</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;The Poet is correct, you need a new tool in your tool belt to help you take on stronger creatures and new planes and even further down the list on the critter list.&lt;/p&gt;&lt;p&gt;The concept we need to learn is &lt;a href="/information/voidance" target="_blank"&gt;Voidance/Devoidance&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;The basics of this is simple, voiding something means its enchantments will fizzle and fail making you much much weaker, as if you just have base gear equipped.&lt;/p&gt;&lt;p&gt;This means death for you.&lt;/p&gt;&lt;p&gt;However, there is an opposite side to voidance called: devoidance, where you make the enemies voidance fail to fire, thus your enchantments do not fizzle and fail and you get to live to fight another day!&lt;/p&gt;&lt;p&gt;The concept is known as Devouring Light (Voidance) and Devouring Darkness (Devoidance).&lt;/p&gt;&lt;p&gt;The quest item in question , can be gotten by completing the quest: The Return of The Kings Crown, and will give you a percentage chance to void/devoid your enemy.&lt;/p&gt;&lt;p&gt;This concept works in pvp, celestial fights, raids and regular critter fights. There is one small exception to this: In all battles you attempt to devoid then the enemy, then you try and void the enemy (assuming you are not devoided) and if the enemy is not voided and not devoided, they will try and void your enchantments.&lt;/p&gt;&lt;p&gt;Where this changes is Purgatory, where the order is reversed, enemy first, you last.&lt;/p&gt;&lt;p&gt;The first quest item requirement, will help you with disenchanting and gaining more Gold Dust when you do so, which will be important soon.0&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Complete the required objectives using the knowledge you have gained so gar.&lt;/p&gt;&lt;p&gt;You can see your voidance, devoidance by doing:&lt;/p&gt;&lt;p&gt;- Click Character Sheet tab&lt;/p&gt;&lt;p&gt;- Click Additional Information orange button.&lt;/p&gt;&lt;p&gt;- Click Voidance tab&lt;/p&gt;&lt;p&gt;Now you can see your resistance to such effects as well as your chance to do said action to the enemy.&lt;/p&gt;&lt;p&gt;The quest line in question will get you an item that raises these significantly, but you can enchant devouring light on your gear by going to the enchantment list here, and searching the filters for: &lt;a href="/information/enchanting?table[filters][types]=3" target="_blank"&gt;Skill/Res Reduction + Devouring Light&lt;/a&gt; and applying those enchants to your gear.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Complete the required objectives using the knowledge you have gained so gar.&lt;/p&gt;&lt;p&gt;You can see your voidance, devoidance by doing:&lt;/p&gt;&lt;p&gt;- Tap Character Sheet tab&lt;/p&gt;&lt;p&gt;- Open the Character Details Section&lt;/p&gt;&lt;p&gt;- Tap Additional Information orange button.&lt;/p&gt;&lt;p&gt;- Tap Voidance tab&lt;/p&gt;&lt;p&gt;Now you can see your resistance to such effects as well as your chance to do said action to the enemy.&lt;/p&gt;&lt;p&gt;The quest line in question will get you an item that raises these significantly, but you can enchant devouring light on your gear by going to the enchantment list here, and searching the filters for: &lt;a href="/information/enchanting?table[filters][types]=3" target="_blank"&gt;Skill/Res Reduction + Devouring Light&lt;/a&gt; and applying those enchants to your gear.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Disenchanter's Magnifying Glass</t>
+  </si>
+  <si>
+    <t>Dead King's Crown</t>
   </si>
 </sst>
 </file>
@@ -669,7 +783,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AS10"/>
+  <dimension ref="A1:AS16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -680,9 +794,9 @@
     <col min="1" max="1" width="3.428" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="31.707" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="1886.254" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="2145.762" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="1594.896" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="1625.603" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="2248.451" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="2309.722" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="2172.898" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="18.71" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="24.708" bestFit="true" customWidth="true" style="0"/>
@@ -699,8 +813,8 @@
     <col min="20" max="20" width="23.423" bestFit="true" customWidth="true" style="0"/>
     <col min="21" max="21" width="26.993" bestFit="true" customWidth="true" style="0"/>
     <col min="22" max="22" width="24.708" bestFit="true" customWidth="true" style="0"/>
-    <col min="23" max="23" width="21.138" bestFit="true" customWidth="true" style="0"/>
-    <col min="24" max="24" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="23" max="23" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="24" max="24" width="37.705" bestFit="true" customWidth="true" style="0"/>
     <col min="25" max="25" width="28.136" bestFit="true" customWidth="true" style="0"/>
     <col min="26" max="26" width="16.425" bestFit="true" customWidth="true" style="0"/>
     <col min="27" max="27" width="22.28" bestFit="true" customWidth="true" style="0"/>
@@ -1242,7 +1356,7 @@
         <v>13</v>
       </c>
       <c r="M10">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="T10" t="s">
         <v>98</v>
@@ -1263,6 +1377,288 @@
         <v>100000</v>
       </c>
       <c r="AS10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:45">
+      <c r="A11">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" t="s">
+        <v>108</v>
+      </c>
+      <c r="F11" t="s">
+        <v>109</v>
+      </c>
+      <c r="G11">
+        <v>350</v>
+      </c>
+      <c r="H11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11">
+        <v>100</v>
+      </c>
+      <c r="J11" t="s">
+        <v>90</v>
+      </c>
+      <c r="K11">
+        <v>100</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>5</v>
+      </c>
+      <c r="AH11">
+        <v>500</v>
+      </c>
+      <c r="AP11">
+        <v>1000</v>
+      </c>
+      <c r="AR11">
+        <v>500000</v>
+      </c>
+      <c r="AS11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:45">
+      <c r="A12">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" t="s">
+        <v>112</v>
+      </c>
+      <c r="E12" t="s">
+        <v>113</v>
+      </c>
+      <c r="F12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G12">
+        <v>400</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>150</v>
+      </c>
+      <c r="N12" t="s">
+        <v>115</v>
+      </c>
+      <c r="O12" t="s">
+        <v>116</v>
+      </c>
+      <c r="P12">
+        <v>2</v>
+      </c>
+      <c r="Q12">
+        <v>2</v>
+      </c>
+      <c r="W12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH12">
+        <v>750</v>
+      </c>
+      <c r="AP12">
+        <v>5000</v>
+      </c>
+      <c r="AQ12">
+        <v>1000</v>
+      </c>
+      <c r="AR12">
+        <v>5000000</v>
+      </c>
+      <c r="AS12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:45">
+      <c r="A13">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" t="s">
+        <v>120</v>
+      </c>
+      <c r="E13" t="s">
+        <v>121</v>
+      </c>
+      <c r="F13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G13">
+        <v>500</v>
+      </c>
+      <c r="H13" t="s">
+        <v>123</v>
+      </c>
+      <c r="I13">
+        <v>5</v>
+      </c>
+      <c r="J13" t="s">
+        <v>124</v>
+      </c>
+      <c r="K13">
+        <v>10</v>
+      </c>
+      <c r="L13">
+        <v>13</v>
+      </c>
+      <c r="M13">
+        <v>30</v>
+      </c>
+      <c r="AP13">
+        <v>10000</v>
+      </c>
+      <c r="AQ13">
+        <v>5000</v>
+      </c>
+      <c r="AR13">
+        <v>10000000</v>
+      </c>
+      <c r="AS13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:45">
+      <c r="A14">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14" t="s">
+        <v>127</v>
+      </c>
+      <c r="E14" t="s">
+        <v>128</v>
+      </c>
+      <c r="F14" t="s">
+        <v>128</v>
+      </c>
+      <c r="T14" t="s">
+        <v>129</v>
+      </c>
+      <c r="U14">
+        <v>2</v>
+      </c>
+      <c r="W14" t="s">
+        <v>130</v>
+      </c>
+      <c r="AP14">
+        <v>1000</v>
+      </c>
+      <c r="AQ14">
+        <v>10</v>
+      </c>
+      <c r="AR14">
+        <v>10000000</v>
+      </c>
+      <c r="AS14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:45">
+      <c r="A15">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>131</v>
+      </c>
+      <c r="C15" t="s">
+        <v>132</v>
+      </c>
+      <c r="D15" t="s">
+        <v>133</v>
+      </c>
+      <c r="E15" t="s">
+        <v>128</v>
+      </c>
+      <c r="F15" t="s">
+        <v>128</v>
+      </c>
+      <c r="X15" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>135</v>
+      </c>
+      <c r="AP15">
+        <v>1000</v>
+      </c>
+      <c r="AQ15">
+        <v>10</v>
+      </c>
+      <c r="AR15">
+        <v>5000000</v>
+      </c>
+      <c r="AS15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:45">
+      <c r="A16">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>136</v>
+      </c>
+      <c r="C16" t="s">
+        <v>137</v>
+      </c>
+      <c r="D16" t="s">
+        <v>138</v>
+      </c>
+      <c r="E16" t="s">
+        <v>139</v>
+      </c>
+      <c r="F16" t="s">
+        <v>140</v>
+      </c>
+      <c r="G16">
+        <v>600</v>
+      </c>
+      <c r="X16" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>142</v>
+      </c>
+      <c r="AP16">
+        <v>5000</v>
+      </c>
+      <c r="AR16">
+        <v>10000000</v>
+      </c>
+      <c r="AS16">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor guide quest changes
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -416,7 +416,7 @@
     <t>You hang out with The Goblin for a while, realizing he is not as helpless as he appears to be. You slaughter a few creatures here and there, share a meal and discuss the events and his life.&lt;br /&gt; &lt;br /&gt; You stare at the stars each night wondering if everything you just experienced was a dream. You close your eyes.&lt;br /&gt; &lt;br /&gt; Blood, dripping down the wall, a metallic object on the floor, the lifeless and still hands of boy no older then 25 sits hunched against the wall, blood drips down from a wound in the head.&lt;br /&gt; &lt;br /&gt; A cream, a women. A scream. She rushes over. A scream – she grabs the child and holds his lifeless body close.&lt;br /&gt; &lt;br /&gt; “Child.”&lt;br /&gt; &lt;br /&gt; You turn around, a clearing, fields – summer breeze.&lt;br /&gt; &lt;br /&gt; “Wake up child.”&lt;br /&gt; &lt;br /&gt; The Poet. What is he doing here, you turn back but there stretches the ruins of a old world road, yellow paint lines the middle of the cracked and broken road.&lt;br /&gt; &lt;br /&gt; “Child.”&lt;br /&gt; &lt;br /&gt; You turn back, The Poet. He glows. The light is too bright.&lt;br /&gt; &lt;br /&gt; “It is not your time. Wake up.”&lt;br /&gt; &lt;br /&gt; You awaken to The Goblin staring at you.&lt;br /&gt; &lt;br /&gt; “You ok child?”</t>
   </si>
   <si>
-    <t>&lt;p&gt;Lets get some items that help with dodging enemies attacks and an item for helping with accuracy. To do this, we will do two more quests for The Goblin:&lt;/p&gt;&lt;p&gt;- &lt;strong&gt;Goblins gift&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- Goblins Accuracy&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;These can both be found on surface.&lt;/p&gt;</t>
+    <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; &lt;em&gt;This quest can take 2+ Hours to complete.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Lets get some items that help with dodging enemies attacks and an item for helping with accuracy. To do this, we will do two more quests for The Goblin:&lt;/p&gt;&lt;p&gt;- &lt;strong&gt;Goblins gift&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- Goblins Accuracy&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;These can both be found on surface.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Golden Ring of Blur</t>
@@ -431,7 +431,7 @@
     <t>Days have gone by and no dream has haunted you like the previous one.&lt;br /&gt; &lt;br /&gt; Odd chores and bits and bobs around the small ramshackle camp you and The Goblin have set up.&lt;br /&gt; &lt;br /&gt; He comes into the camp with his bits and bobs and stolen items that he pick pocketed off wondering merchants. You peer through his treasures and find a letter.&lt;br /&gt; &lt;br /&gt; “Whats ya got there?” The goblin asks snatching the letter away.&lt;br /&gt; &lt;br /&gt; “Seems to be addressed to you! How unique!”&lt;br /&gt; &lt;br /&gt; You take the letter back from him and read the contents, it’s from The Poet&lt;br /&gt; &lt;br /&gt; Seems you have been busy my child. I need your assistance in a place far from the comforts of home. Alas for you to open such gates you must survive the trials and become stronger, unlocking a power with in your self.&lt;br /&gt; &lt;br /&gt; There is a crown, from a king long dead. His crown will help you take on even stronger creatures, creatures that can look at you and make you weak! Make your spells fail, your enchantments fizzle and fail. These creatures are fearsome.&lt;br /&gt; &lt;br /&gt; Alas, your adventures will take you deeper into those dreams of yours …&lt;br /&gt; &lt;br /&gt; The Poet&lt;br /&gt; &lt;br /&gt; You look up from the letter and The Goblin looks at you:&lt;br /&gt; &lt;br /&gt; “Whats up?Where are we off too?”</t>
   </si>
   <si>
-    <t>&lt;p&gt;The Poet is correct, you need a new tool in your tool belt to help you take on stronger creatures and new planes and even further down the list on the critter list.&lt;/p&gt;&lt;p&gt;The concept we need to learn is &lt;a href="/information/voidance" target="_blank"&gt;Voidance/Devoidance&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;The basics of this is simple, voiding something means its enchantments will fizzle and fail making you much much weaker, as if you just have base gear equipped.&lt;/p&gt;&lt;p&gt;This means death for you.&lt;/p&gt;&lt;p&gt;However, there is an opposite side to voidance called: devoidance, where you make the enemies voidance fail to fire, thus your enchantments do not fizzle and fail and you get to live to fight another day!&lt;/p&gt;&lt;p&gt;The concept is known as Devouring Light (Voidance) and Devouring Darkness (Devoidance).&lt;/p&gt;&lt;p&gt;The quest item in question , can be gotten by completing the quest: The Return of The Kings Crown, and will give you a percentage chance to void/devoid your enemy.&lt;/p&gt;&lt;p&gt;This concept works in pvp, celestial fights, raids and regular critter fights. There is one small exception to this: In all battles you attempt to devoid then the enemy, then you try and void the enemy (assuming you are not devoided) and if the enemy is not voided and not devoided, they will try and void your enchantments.&lt;/p&gt;&lt;p&gt;Where this changes is Purgatory, where the order is reversed, enemy first, you last.&lt;/p&gt;&lt;p&gt;The first quest item requirement, will help you with disenchanting and gaining more Gold Dust when you do so, which will be important soon.0&lt;/p&gt;</t>
+    <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; &lt;em&gt;This quest can take 2+ Hours to complete.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;The Poet is correct, you need a new tool in your tool belt to help you take on stronger creatures and new planes and even further down the list on the critter list.&lt;/p&gt;&lt;p&gt;The concept we need to learn is &lt;a href="/information/voidance" target="_blank"&gt;Voidance/Devoidance&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;The basics of this is simple, voiding something means its enchantments will fizzle and fail making you much much weaker, as if you just have base gear equipped.&lt;/p&gt;&lt;p&gt;This means death for you.&lt;/p&gt;&lt;p&gt;However, there is an opposite side to voidance called: devoidance, where you make the enemies voidance fail to fire, thus your enchantments do not fizzle and fail and you get to live to fight another day!&lt;/p&gt;&lt;p&gt;The concept is known as Devouring Light (Voidance) and Devouring Darkness (Devoidance).&lt;/p&gt;&lt;p&gt;The quest item in question , can be gotten by completing the quest: The Return of The Kings Crown, and will give you a percentage chance to void/devoid your enemy.&lt;/p&gt;&lt;p&gt;This concept works in pvp, celestial fights, raids and regular critter fights. There is one small exception to this: In all battles you attempt to devoid then the enemy, then you try and void the enemy (assuming you are not devoided) and if the enemy is not voided and not devoided, they will try and void your enchantments.&lt;/p&gt;&lt;p&gt;Where this changes is Purgatory, where the order is reversed, enemy first, you last.&lt;/p&gt;&lt;p&gt;The first quest item requirement, will help you with disenchanting and gaining more Gold Dust when you do so, which will be important soon.0&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Complete the required objectives using the knowledge you have gained so gar.&lt;/p&gt;&lt;p&gt;You can see your voidance, devoidance by doing:&lt;/p&gt;&lt;p&gt;- Click Character Sheet tab&lt;/p&gt;&lt;p&gt;- Click Additional Information orange button.&lt;/p&gt;&lt;p&gt;- Click Voidance tab&lt;/p&gt;&lt;p&gt;Now you can see your resistance to such effects as well as your chance to do said action to the enemy.&lt;/p&gt;&lt;p&gt;The quest line in question will get you an item that raises these significantly, but you can enchant devouring light on your gear by going to the enchantment list here, and searching the filters for: &lt;a href="/information/enchanting?table[filters][types]=3" target="_blank"&gt;Skill/Res Reduction + Devouring Light&lt;/a&gt; and applying those enchants to your gear.&lt;/p&gt;</t>
@@ -1644,7 +1644,7 @@
         <v>140</v>
       </c>
       <c r="G16">
-        <v>600</v>
+        <v>550</v>
       </c>
       <c r="X16" t="s">
         <v>141</v>

</xml_diff>

<commit_message>
Fixed a slight bug and redid some of the guide quests
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="117">
   <si>
     <t>id</t>
   </si>
@@ -209,7 +209,7 @@
     <t>Sitting in the INN, you stare into the large fire place with the wood burning and the smell of the old oak as it burns. It’s almost as if time stops for a moment and you can gather your thoughts.&lt;br /&gt; &lt;br /&gt; All you do is slaughter creatures, gather loot and slowly get better at hitting the enemies and even slightly faster.&lt;br /&gt; &lt;br /&gt; The flames of the fire seem to stand still, the smell of the fire has dissipated from the air. You look around and no one is moving, like they have been frozen in time.&lt;br /&gt; &lt;br /&gt; You turn back to the fire and see a young man, about twenty-five standing before the fire, his back to you. You call out to him, and he doesn’t turn around but he does speak.&lt;br /&gt; &lt;br /&gt; “Child. I have found something most mysterious. The gates have opened.”&lt;br /&gt; &lt;br /&gt; The gates? What gates?&lt;br /&gt; &lt;br /&gt; “Listen to me child.” The young man turns and faces you.&lt;br /&gt; &lt;br /&gt; “I need you to speak with the local blacksmith, work with him for a while. Train a different set of skills. Important skills. I need you to craft your own gear.”&lt;br /&gt; &lt;br /&gt; You tell him that the gear you have found, the stuff you can buy from the local blacksmith is better then what you can craft.&lt;br /&gt; &lt;br /&gt; “True, however, you can craft even more powerful gear then that of which you can buy.”&lt;br /&gt; &lt;br /&gt; Before you can ask further questions the flames returning to their burning motion, the wood crackles, the INN is full of voices again and the smell of food fills the air.&lt;br /&gt; &lt;br /&gt; Where did he go?</t>
   </si>
   <si>
-    <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; &lt;em&gt;This quest can take up to two hours to complete. One for crafting and one to reach the required level.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Today we are going to learn about &lt;a href="/information/crafting" target="_blank"&gt;crafting&lt;/a&gt;. There are various types of crafting, but we want to focus on weapons and armour for now.&lt;/p&gt;&lt;p&gt;At first you will fail a lot, even with the suggested &lt;a href="/information/quest-items" target="_blank"&gt;quest items&lt;/a&gt; this quest can take a minute to complete. If you have any enchanted gear that has dropped that has Weapon/Armour Crafting Enchantments on them, I would suggest equipping them, even at the cost of damage.&lt;/p&gt;&lt;p&gt;Eventually you will craft beyond what the &lt;a href="/information/shop" target="_blank"&gt;shop&lt;/a&gt; sells. The Shop stops at two billion gold, where as players can craft up to 36+ Billion gold items that are much better then shop gear.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Crafting cannot be automated. Keep an eye on Server Messages section to see successes, failures and if you have new items to craft.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Remember to keep crafting - even after this quest. Stick to weapons (any type) - but do experiment with others, like Armour, Ring and Spell Crafting. A later quest will be less painful.&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;</t>
+    <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; &lt;em&gt;This quest can take 2+ hours to complete. It is suggested you explore and craft at the same time.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Today lets learn how to &lt;a href="/information/crafting" target="_blank"&gt;craft&lt;/a&gt; weapons and armour. You can also craft other things like spells, rings, trinkets and alchemy.&lt;/p&gt;&lt;p&gt;Crafting is wildly important because the &lt;a href="/information/shop" target="_blank"&gt;shop&lt;/a&gt; will only take you so far. For example, later in the game you can get gear sets: &lt;a href="/information/hell-forged-set" target="_blank"&gt;Hell Forged&lt;/a&gt; and then &lt;a href="/information/purgatory-chains-set" target="_blank"&gt;Purgatory Chains&lt;/a&gt;. In order to get a piece of Hell Forged gear you need to craft or have a crafting level 400 item, which is beyond what the shop sells.&lt;/p&gt;&lt;p&gt;Crafting cannot be done with any form of automation, and instead works well while you set up &lt;a href="/information/exploration" target="_blank"&gt;exploration&lt;/a&gt;. It is vitally important you find a creature in the list, further down if possible, that you can manually kill in one hit a few times to use for exploration.&lt;/p&gt;&lt;p&gt;The further down the list, for monsters, you go the harder they get yes – but the more XP you get. All Monsters have a maximum level and when a player reaches that maximum level and beyond, they will only get 1/3rd the XP for killing it.&lt;/p&gt;&lt;p&gt;This quest will also have you find, by visiting two locations, &lt;a href="/information/quest-items" target="_blank"&gt;quest items&lt;/a&gt; which you will automatically be picked up and automatically used. You can see that they are being used after you get them by going to your skill section (see instructions) and clicking on the skill name. The bonuses are automatically applied for you.&lt;/p&gt;&lt;p&gt;With that said my suggestion for this is to set up exploration for 2 or more hours and then start crafting while exploration runs. Put on a good show/movie/podcast and lets start grinding shall we?&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Keep crafting after this quest, it will hurt less in a later guide quest.&lt;/strong&gt;&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;- First we want to find the items we need, quest items are automatically used. You can open the Teleport Map Action to then select the location: Ruined Port City Of Kalize (X/Y): 32/368 and click teleport if you can afford the cost. This will get you the: Weapon Smith’s Book which adds 25% to Skill Bonus and XP.&lt;/p&gt;&lt;p&gt;- Repeat the above step to then go to: Dragon cliffs (X/Y): 192/176 to get the Blacksmith’s book for the same bonuses towards Armour Crafting.&lt;/p&gt;&lt;p&gt;Both of these can be upgraded later on when we have access to Labyrinth. There are some One Off &lt;a href="http://127.0.0.1:8000/information/quests" target="_blank"&gt;quests&lt;/a&gt; that will upgrade these.&lt;/p&gt;&lt;p&gt;- Now lets craft, first set up exploration for an hour or two – or what ever you feel like doing, Exploration will run while logged out. Remember to set it up with a monster you can kill in one hit.&lt;/p&gt;&lt;p&gt;- Close exploration and then from the drop down Craft/Enchant select craft, select weapons, select Broken Dagger and then click craft.&lt;/p&gt;</t>
@@ -236,7 +236,7 @@
     <t>You are exhausted, tired, confused.&lt;br /&gt; &lt;br /&gt; “Child” comes a familiar voice as you sit up on your bed.&lt;br /&gt; &lt;br /&gt; The INN is creaky, noisy and musty. The single candle flame that burns in the room barley illuminates the area.&lt;br /&gt; &lt;br /&gt; As he walks from the shadows The Guide stands before you, not young and handsome, but old and wise, dressed in robes. His skin is brown from the sun.&lt;br /&gt; &lt;br /&gt; “Downstairs sits a woman, an attractive woman.” he states with a bit of a smirk.&lt;br /&gt; &lt;br /&gt; “She will teach you about magic and its properties, specifically in the art of enchanting and disenchanting.”&lt;br /&gt; &lt;br /&gt; You ask him why he can’t teach you and he deflects the question.&lt;br /&gt; &lt;br /&gt; “Go now child. She isn’t to be kept waiting.”&lt;br /&gt; &lt;br /&gt; You head down the stairs to meet the Enchantress.&lt;br /&gt; &lt;br /&gt; She waits for you at a table, a woman in black, instantly recognizable by her long black hair and pale complexion. She radiates beauty.&lt;br /&gt; &lt;br /&gt; You walk over and sit down at the table. “Hello child.” She starts, he voice is soft and entrancing. “have you heard of The Queen?” You shake your head no. “She has gifted you with some of those green shiny unique’s in your inventory.”&lt;br /&gt; &lt;br /&gt; You remember those. Killing monsters gets you faction with the plane and its people. As a reward they give you a shiny green item that makes you feel much much stronger.&lt;br /&gt; &lt;br /&gt; “She can give you more powerful ones, but you have to face the most fearsome of creatures to earn her attention. In the mean time lets discuss the art of magic. Lets start small with spells …”</t>
   </si>
   <si>
-    <t>&lt;p&gt;Lets start learning about spells.&lt;/p&gt;&lt;p&gt;You have just spent a ton of time crafting weapons and Armour, we will repeat this to craft spells. Spells are useful for caster classes, as well as any one who wants to use them, be they healing or damage based.&lt;/p&gt;&lt;p&gt;Damage spells and Staves (Two Handed weapons) can raise the characters intelligence, both of which can be bought from the shop or crafted.&lt;/p&gt;&lt;p&gt;Healing spells are great for characters who want to do Cast and attack or Attack and Cast, like Prophets. healing spells will heal the player when they are cast and cannot ever miss, damage spells how ever require a character to train the skill: Casting Accuracy to have a better chance at hitting the enemies with their damage spells. Healing spells can also resurrect the player and have a resurrection chance. resurrection automatically happens based on the resurrection chance of both of your equipped healing spells.&lt;/p&gt;&lt;p&gt;To get the quest item required, you will need to kill: &lt;strong&gt;Umbering Spirit Lord&lt;/strong&gt; on Surface. This creature is further down the list and may require you to upgrade your gear through the shop before being able to take him down.&lt;/p&gt;&lt;p&gt;This creature has a 15% chance to drop the item, so exploration might be a good choice here.&lt;/p&gt;</t>
+    <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; &lt;em&gt;This quest can take 2+ hours to do. It is suggested you craft and explore at the same time.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Lets learn about spells and spell casting.&lt;/p&gt;&lt;p&gt;You might not be a caster &lt;a href="/information/races-and-classes#3" target="_blank"&gt;class&lt;/a&gt; like a Heretic, Arcane Alchemist or Prophet, but every class can use spells. You just need to train the skill &lt;a href="/information/skill-information" target="_blank"&gt;Casting Accuracy&lt;/a&gt; for damage based spells.&lt;/p&gt;&lt;p&gt;Healing spells – never miss and will heal you when you use &lt;a href="/information/combat" target="_blank"&gt;Cast, Cast and Attack or Attack&lt;/a&gt; and cast (depending on healing spell location (right or left hand respectively) for the last two attack types).&lt;/p&gt;&lt;p&gt;Crafting spells is done the same way as you would for crafting armour or weapons or rings.&lt;/p&gt;&lt;p&gt;Casting Accuracy will, over time, make it easier for you to hit the enemy. Caster classes want to focus on this skill and start using Cast once their spells, via using Cast and Attack or Attack and Cast, are landing more frequently.&lt;/p&gt;&lt;p&gt;Prophets can also use damage spells and should also start focusing on Cast and Attack or Attack and cast depending on which hand their healing spell is in.&lt;/p&gt;&lt;p&gt;Intelligence here is a stat we want to raise, you can do this via buying, crafting or enchanting gear – since we have not learned about enchantments yet, lets try and use the gear we have found or buy some better gear (Body, Damage Spell x2 and/or Stave (weapon type – two handed)) to raise this stat.&lt;/p&gt;&lt;p&gt;Leveling your character will also help. Why raise Intelligence? For the next quest – Enchanting depends on intelligence in terms of what you can craft, we just want to make it easier for you.&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Just like we did for crafting, lets select spells instead of weapons or armour. When crafting spells, you will always have one of each type to equip: Damage and Healing.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Remember to set up exploration with a creature you can reliably kill in one hit. Continue investigating and upgrading your gear to take on harder creature.&lt;/strong&gt;&lt;/p&gt;</t>
@@ -251,19 +251,79 @@
     <t>Spell Weaving Book</t>
   </si>
   <si>
-    <t>Go To Labyrinth</t>
-  </si>
-  <si>
-    <t>You have been under the Enchantress’s tutelage for weeks now. She has been teaching the you about the art of magic and how it can be used to weave together powerful spells.&lt;br /&gt; &lt;br /&gt; She has told you that if you wait for her in the forest outside of town she will teach you the next step: Enchanting. She explained it is the use of powerful magic that can imbue items, such as weapons, armour, rings and even other spells with potent abilities that can turn the tide of a battle, similar to the items you find on the enemies corpses.&lt;br /&gt; &lt;br /&gt; You are waiting for her in the forest outside of the town you have been practically living in. She doesn’t appear and some time goes by.&lt;br /&gt; &lt;br /&gt; The old man appears, The Guide. Almost from thin air, one moment nothing, next he’s in front of you.&lt;br /&gt; &lt;br /&gt; “She isn’t coming.” He states.&lt;br /&gt; &lt;br /&gt; “Something foul is afoot and I need you to do some investigating for me. Find the Key of labyrinth child. Do it quickly.”</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Time to stop training and fight a monster. This will drop weather you use exploration or not. Find the Key of Labyrinth by fighting the Labyrinth Fiend on Surface&lt;/p&gt;&lt;p&gt;The way players manage to travel from Plane to Plane is by either finding a quest item, such as this one - or like the other planes: Dungeons, Shadow Planes, Hell and Purgatory are all locked behind quests, which we will get into a bit later. Right now, lets find a quest item by killing a creature that will eventually drop it.&lt;/p&gt;&lt;p&gt;Each plane has its own monsters. Some have their own quests and there is even more room for the eventual settling of kingdoms. Some planes such as Shadow Planes and Hell as well as Purgatory will weaken your character, making you put more time and effort into your gear, while strengthening monsters which makes you put more effort into which types of enchantments you put on that gear.&lt;/p&gt;&lt;p&gt;To make it easier lets also raise our looting skill.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;Click traverse under the map.&lt;/p&gt;&lt;p&gt;- Select Labyrinth from the plane drop down.&lt;/p&gt;&lt;p&gt;- Click traverse.&lt;/p&gt;&lt;p&gt;- Welcome to labyrinth. Monsters down here have the same strength as surface but are new.&lt;/p&gt;&lt;p&gt;- Kill enough until your faction level with surface is level 1.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- From the action drop down select Map Movement&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;Click traverse under the map.&lt;/p&gt;&lt;p&gt;- Select Labyrinth from the plane drop down.&lt;/p&gt;&lt;p&gt;- Click traverse.&lt;/p&gt;&lt;p&gt;- Welcome to labyrinth. Monsters down here have the same strength as surface but are new.&lt;/p&gt;&lt;p&gt;- Kill enough until your faction level with surface is level 1.&lt;/p&gt;</t>
+    <t>Enchanting is key</t>
+  </si>
+  <si>
+    <t>As you rise to the new dawn of a new day you have a knock at the door. You rise and greet the stranger. The Enchantress walks in. Today she wares a set of red robes and you can see deep into her blue eyes.&lt;br /&gt; &lt;br /&gt; “My darling child, I hear you have been adventuring. Shall we pick up where we left off? The art of enchanting.”&lt;br /&gt; &lt;br /&gt; You tell her you have plenty of enchanted gear.&lt;br /&gt; &lt;br /&gt; “Wouldn’t you like better gear? Stronger gear?”</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Note: &lt;/strong&gt;&lt;em&gt;This quest can take 2+ hours to complete. It is advised to explore and do the other objectives such as crafting and then enchanting while exploration is running.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;The &lt;/em&gt;&lt;strong&gt;&lt;em&gt;Skill Type Crafting to level 10&lt;/em&gt;&lt;/strong&gt;&lt;em&gt; means: level any crafting skill you want to level 10 or higher that you currently have access too.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Today's lesson is about &lt;a href="/information/enchanting" target="_blank"&gt;enchanting&lt;/a&gt; and &lt;a href="/information/disenchanting" target="_blank"&gt;disenchanting&lt;/a&gt;. Just like crafting, enchanting is wildly important. As you may know, you cannot buy enchanted gear from the shop. Some players will sell it on the &lt;a href="/information/market-board" target="_blank"&gt;market place&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;More importantly, you want a &lt;a href="/information/currencies" target="_blank"&gt;currency&lt;/a&gt; you can get from it: Gold Dust. This currency is used in a lot of quests we are going to start doing soon. So lets get a lot of it.&lt;/p&gt;&lt;p&gt;There re a verity of enchantments you can choose from, on the enchanting help page you can filter the different types of enchantments. All enchantments, unless otherwise stated, will stack.&lt;/p&gt;&lt;p&gt;You can see info about an enchantment on an item by either opening it from your inventory or from chat when it drops, selecting details – and from there as you scroll down you will see one or two orange buttons that when clicked will open up a modal for that items enchantment.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;&lt;u&gt;My tip for you is&lt;/u&gt;&lt;/em&gt;&lt;/strong&gt;: Filter the table on the help page by Accuracy (or Casting Accuracy if you are using spells) and then Stat Modifiers.&lt;/p&gt;&lt;p&gt;Find the level 1 enchantments for both, and enchant those – both – on to your freshly crafted items. Repeat until your inventory is full, equip what you want and then disenchant the rest.&lt;/p&gt;&lt;p&gt;You can also buy multiple items from the shop for the purposes of enchanting, but I recommend you continue crafting. Craft 75 items of what ever, enchant all 75 items, equip or disenchant the rest. You could also sell some stuff on the market board to make some coin back.&lt;/p&gt;&lt;p&gt;Rinse and Repeat, all while exploring to keep the steady flow of gold coming in.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Remember to keep enchanting and disenchanting items. A later quest will be less painful.&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;To enchant, from the crafting drop down select enchant.&lt;/p&gt;&lt;p&gt;- Here you have an item to select, a suffix and a prefix to select. The cost of enchanting can get widely expensive so exploration is required. Since you need items: weapons, Armour, spells and Rings, you will also want to be crafting. You can also re-enchant enchanted items but that gets more costly.&lt;/p&gt;&lt;p&gt;You can also just go to the shop and buy multiple items to enchant, like broken daggers.&lt;/p&gt;&lt;p&gt;- Next, when you have enchanted, ideally 75 items, next go to your inventory&lt;/p&gt;&lt;p&gt;- From the actions on the inventory section of your character sheet, click Disenchant All.&lt;/p&gt;&lt;p&gt;- This will raise your disenchanting skill, and slowly over time your enchanting skill as well.&lt;/p&gt;&lt;p&gt;- Repeat till you meet the quest requirements.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;- Open Craft from the drop down selection&lt;/p&gt;&lt;p&gt;- from the Craft/Enchant drop down select enchant&lt;/p&gt;&lt;p&gt;- Here you have an item to select, a suffix and a prefix to select. The cost of enchanting can get widely expensive so exploration is required. Since you need items: weapons, Armour, spells and Rings, you will also want to be crafting. You can also re-enchant enchanted items but that gets more costly.&lt;/p&gt;&lt;p&gt;You can also just go to the shop and buy multiple items to enchant, like broken daggers.&lt;/p&gt;&lt;p&gt;- Next, when you have enchanted, ideally 75 items, next go to your inventory&lt;/p&gt;&lt;p&gt;- From the actions on the inventory section of your character sheet, click Disenchant All.&lt;/p&gt;&lt;p&gt;- This will raise your disenchanting skill, and slowly over time your enchanting skill as well.&lt;/p&gt;&lt;p&gt;- Repeat till you meet the quest requirements.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Enchanting</t>
+  </si>
+  <si>
+    <t>Disenchanting</t>
+  </si>
+  <si>
+    <t>Enchanter's Book</t>
+  </si>
+  <si>
+    <t>The Mysterious Goblin Pt. 1</t>
+  </si>
+  <si>
+    <t>The magic crackles in the air and the spells weave and twist their way around the gear as you chant the incantations to lock the enchantments into the item before you. Sometimes you fail, sometimes your efforts are in-vain and infuriating as the world seems against you and your efforts, but with determination and passion you manage to complete The Enchantress’s request of learning more about the art of enchanting it’s self.&lt;br /&gt; &lt;br /&gt; The magic before you make you weak, tired, exhausted. You step outside the confines of the small INN, you have been using a back room for your magical training, The Enchantress has been paying a little extra for the privacy to learn.&lt;br /&gt; &lt;br /&gt; She has left to run an errand, much like The Guide. Trusting that you wont get swept away into an adventure and instead study and focus on what is before you.&lt;br /&gt; &lt;br /&gt; As you stand in the fresh air of the warm fall day, you realize that the seasons before you are changing, the color of the leaves and the smell in the air has a bit of a nip to it.&lt;br /&gt; &lt;br /&gt; Out of the corner of your eye stands a little goblin. He sees you and darts away. What did he steal? You decide to hunt him down and find out what this little thief is up to.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Note: &lt;/strong&gt;&lt;em&gt;This guide quest can take longer then 2 hours. This is because the quests you will complete will require Gold Dust, which you get by enchanting and then disenchanting items. Due to the fact that you will also be leveling a faction, while this quest is active, you will get 5 extra faction points per kill.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Lets move on from skills and crafting and engage with other systems of the game, such as &lt;a href="/information/quests" target="_blank"&gt;Quests&lt;/a&gt;. Quests are another vital aspect of the game because this is how you unlock new features of the game to play with.&lt;/p&gt;&lt;p&gt;Some games will hide these features behind a pay wall, instead here I hide them behind quests, which are very easy to complete and come with explicit instructions on how to do so.&lt;/p&gt;&lt;p&gt;Some quests like the one you will do, will give you items that help with you other aspects of the game, some quests simply upgrade existing quest items and some quests unlock new access to new &lt;a href="/information/planes" target="_blank"&gt;planes&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;All quests tell a story before and after you click the hand in button which gives you some lore on the world and your place in it.&lt;/p&gt;&lt;p&gt;There are two types of quests: Quest trees and One off quests. One off quests will usually upgrade or give you an item that unlocks a feature where as Quest Trees will usually have a chain of quests that continually upgrade the item given or gives you an item at the end of said quest line.&lt;/p&gt;&lt;p&gt;There are also &lt;a href="/information/raids" target="_blank"&gt;Raid&lt;/a&gt; Quests that will appear when a raid is currently running. These are also usually in the form a tree where the left side of the tree tells you more about the raid boss while the right hand side will reward players with a cosmetic feature.&lt;/p&gt;&lt;p&gt;Each plane has its own set of quests as well, which can further enhance or unlock features for that plane or game wide in general.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;- Click the Quests tab&lt;/p&gt;&lt;p&gt;- To the right you will see: Goblins List for Gold and Faction Hunter.&lt;/p&gt;&lt;p&gt;- Blue quests are quests you can complete, so start at the top of the tree and work your way down.&lt;/p&gt;&lt;p&gt;- Click on the first quest you can do.&lt;/p&gt;&lt;p&gt;- You will see three tab: &lt;a href="/information/npcs" target="_blank"&gt;NPC&lt;/a&gt; Details, Required to Complete and Quest Reward.&lt;/p&gt;&lt;p&gt;- NPC Details will give you details of the NPC as well as the “before” hand in story. When you hand in the quest, this story section will update to show “after” hand in story content&lt;/p&gt;&lt;p&gt;- Required to Complete will show you what you need to do in order to complete it. Beside each requirement is a help icon, clicking this will open a modal that gives you explicit instructions on how to get the requirement.&lt;/p&gt;&lt;p&gt;- Quest Reward Tab show you what rewards you get for completing the quest it’s self.&lt;/p&gt;&lt;p&gt;- Once you have met the requirements for a quest click the Hand in button and you will be, for free, with no timeout – transported across planes and locations to the NPC. The only caveat is you have to be able to reach them. For example if they are on water you must be able to walk on water.&lt;/p&gt;&lt;p&gt;You can walk on most forms of water with a quest item called Flask of Fresh Air which you can get by killing a Pirate Master on Surface.&lt;/p&gt;&lt;p&gt;Remember, to check your Factions by going to Character Sheet → Factions tab to see what level you are for surface as this guide quest has you complete a quest to help you level the factions a bit faster.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Mobile Instructions&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Tap the Quests tab&lt;/p&gt;&lt;p&gt;- To the right you will see: Goblins List for Gold and Faction Hunter.&lt;/p&gt;&lt;p&gt;- You can scroll left, right, up and down to view the quest tree. Scroll to the far right&lt;/p&gt;&lt;p&gt;- Blue quests are quests you can complete, so start at the top of the tree and work your way down.&lt;/p&gt;&lt;p&gt;- Tap on the first quest you can do.&lt;/p&gt;&lt;p&gt;- You will see three tab: &lt;a href="/information/npcs" target="_blank"&gt;NPC&lt;/a&gt; Details, Required to Complete and Quest Reward.&lt;/p&gt;&lt;p&gt;- NPC Details will give you details of the NPC as well as the “before” hand in story. When you hand in the quest, this story section will update to show “after” hand in story content&lt;/p&gt;&lt;p&gt;- Required to Complete will show you what you need to do in order to complete it. Beside each requirement is a help icon, clicking this will open a modal that gives you explicit instructions on how to get the requirement.&lt;/p&gt;&lt;p&gt;- Quest Reward Tab show you what rewards you get for completing the quest it’s self.&lt;/p&gt;&lt;p&gt;- Once you have met the requirements for a quest click the Hand in button and you will be, for free, with no timeout – transported across planes and locations to the NPC. The only caveat is you have to be able to reach them. For example if they are on water you must be able to walk on water.&lt;/p&gt;&lt;p&gt;You can walk on most forms of water with a quest item called Flask of Fresh Air which you can get by killing a Pirate Master on Surface.&lt;/p&gt;&lt;p&gt;Remember, to check your Factions by going to Character Sheet →expand the Character Details Section → Factions tab to see what level you are for surface as this guide quest has you complete a quest to help you level the factions a bit faster.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Surface</t>
+  </si>
+  <si>
+    <t>Faction Hunter</t>
+  </si>
+  <si>
+    <t>The Mysterious Goblin Pt. 2</t>
+  </si>
+  <si>
+    <t>This little helpless goblin does not seem dangerous at all. Curious if anything else. Full of surprises and strange little gifts for the errands you do for him.&lt;br /&gt; &lt;br /&gt; You have arrived back at the town after your little adventure and you find The Guide sitting at the INN waiting for you.&lt;br /&gt; &lt;br /&gt; “I see you have been out adventuring with our helpless little friend.”&lt;br /&gt; &lt;br /&gt; You tell him of your adventures, your crafting, enchanting, fighting, errands you did for the goblin.&lt;br /&gt; &lt;br /&gt; “Fantastic. The world is full of interesting people for you to meet. Some of them have more errands, their own stories and adventures for you to go on in exchange for knowledge and various fantastic rewards.”&lt;br /&gt; &lt;br /&gt; He pauses and you two sit in silence for a moment enjoying a drink and a spread before you.&lt;br /&gt; &lt;br /&gt; “You should work with that goblin for something special, A Book of Guidance.”&lt;br /&gt; &lt;br /&gt; You ask what this item is for.&lt;br /&gt; &lt;br /&gt; “You, to help you hit better child.”</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We know how to do quests now, so lets continue doing quests to get an item that will help you – especially if you are crafting items with Accuracy enchantments attached – level Accuracy rather quickly.&lt;/p&gt;&lt;p&gt;This right here shows you how two features of the game can work together to progress your character: Quest items that you get from doing quests that increase some aspect about your character. Enchanting, Crafting, Quests and Skills&lt;/p&gt;&lt;p&gt;As we progress we will open more systems that also work together with existing systems you have learned to continue to progress your character.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We already know how to complete a quest, and we know how to level our skills. So lets use that in conjunction with crafting and enchanting to get gold dust to complete the required objectives.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Goblins Accuracy</t>
+  </si>
+  <si>
+    <t>The Shadow and The Murder</t>
+  </si>
+  <si>
+    <t>Your ability to kill creatures is getting better and your able to find and hunt down stronger foes.&lt;br /&gt; &lt;br /&gt; Exhausted and tired you arrive back at the INN. It’s completely empty. Not a soul, not a single sound but the creaking of the old wood in the wind that blows outside.&lt;br /&gt; &lt;br /&gt; You call out but no one answers.&lt;br /&gt; &lt;br /&gt; A shadow moves across the wall and you move towards where the shadow went.&lt;br /&gt; &lt;br /&gt; No one there.&lt;br /&gt; &lt;br /&gt; You call out again, readying your weapon.&lt;br /&gt; &lt;br /&gt; Nothing.&lt;br /&gt; &lt;br /&gt; You enter into a back room, an office of sorts. Blood covers the wall. You back out and head back to the main room.&lt;br /&gt; &lt;br /&gt; Bodies. Bodies every where, torn, broken, damage and ripped apart. The gore, the fear, the pain the eyes of the dead.&lt;br /&gt; &lt;br /&gt; What the hell happened?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;It’s time we get off the &lt;a href="/information/planes" target="_blank"&gt;plane&lt;/a&gt;: Surface. To do this we just have to kill a single creature: Labyrinth Fiend until the Key of Labyrinth drops.&lt;/p&gt;&lt;p&gt;This will allow us to use a new feature called: &lt;a href="/information/traverse" target="_blank"&gt;Traverse&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;Traverse allows us to move to another plane of existence where we can fight monsters and interact with new features. For example, when we eventually get to Hell, those &lt;a href="/information/random-enchants" target="_blank"&gt;Green Uniques&lt;/a&gt; you have been getting – there is an NPC that allows you to buy better ones and even re-roll them and move the enchantments to other items. How fun!&lt;/p&gt;&lt;p&gt;Some Planes make you weaker and the creatures much, much stronger and also give you bonuses for killing creatures of that plane. As you go past Dungeons plane you will find your gear needs to be better with a set of enchantments that play to your classes strengths as well as the levels.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Kill Labyrinth fiend until the Key of Labyrinth drops.&lt;/p&gt;&lt;p&gt;Next:&lt;/p&gt;&lt;p&gt;- Click Traverse under the map&lt;/p&gt;&lt;p&gt;- Select labyrinth from the drop down&lt;/p&gt;&lt;p&gt;- Click Traverse&lt;/p&gt;&lt;p&gt;- Welcome to Labyrinth!plane&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Kill Labyrinth fiend until the Key of Labyrinth drops.&lt;/p&gt;&lt;p&gt;Next:&lt;/p&gt;&lt;p&gt;- Select Map Movement from the action drop down&lt;/p&gt;&lt;p&gt;- Tap Traverse under the map&lt;/p&gt;&lt;p&gt;- Select labyrinth from the drop down&lt;/p&gt;&lt;p&gt;- Tap Traverse&lt;/p&gt;&lt;p&gt;- Welcome to Labyrinth!&lt;/p&gt;</t>
   </si>
   <si>
     <t>Labyrinth</t>
@@ -272,178 +332,40 @@
     <t>Key of the Labyrinth</t>
   </si>
   <si>
-    <t>Enchanting is key</t>
-  </si>
-  <si>
-    <t>You have been on another plane, a plane full of ruins, broken pieces of multiple labyrinths. The entire plane was covered with them.&lt;br /&gt; &lt;br /&gt; As you recover from your travels, slaughtering a whole new group of fearsome creatures, gaining notoriety with the inhabitants of said plane.&lt;br /&gt; &lt;br /&gt; Still no sign of the Enchantress and no sign of The Guide. You take a moment to relax before your next adventure.&lt;br /&gt; &lt;br /&gt; As you rise to the new dawn of a new day you have a knock at the door. You rise and greet the stranger. The Enchantress walks in. Today she wares a set of red robes and you can see deep into her blue eyes.&lt;br /&gt; &lt;br /&gt; “My darling child, I hear you have been adventuring. Shall we pick up where we left off? The art of enchanting.”&lt;br /&gt; &lt;br /&gt; You tell her you have plenty of enchanted gear.&lt;br /&gt; &lt;br /&gt; “Wouldn’t you like better gear? Stronger gear?”</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; &lt;em&gt;This quest can take up to two hours to complete&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Today's lesson is about &lt;a href="/information/enchanting" target="_blank"&gt;enchanting&lt;/a&gt; and &lt;a href="/information/disenchanting" target="_blank"&gt;disenchanting&lt;/a&gt;. Just like crafting, enchanting is wildly important. As you may know, you cannot buy enchanted gear from the shop. Some players will sell it on the &lt;a href="/information/market-board" target="_blank"&gt;market place&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;More importantly, you want a &lt;a href="/information/currencies" target="_blank"&gt;currency&lt;/a&gt; you can get from it: Gold Dust. This currency is used in a lot of quests we are going to start doing soon. So lets get a lot of it.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Remember to keep enchanting and disenchanting items. A later quest will be less painful.&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;The &lt;strong&gt;Skill Type Crafting to level 10&lt;/strong&gt; means: level any crafting skill you want to level 10 or higher.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;To enchant, from the crafting drop down select enchant.&lt;/p&gt;&lt;p&gt;- Here you have an item to select, a suffix and a prefix to select. The cost of enchanting can get widely expensive so exploration is required. Since you need items: weapons, Armour, spells and Rings, you will also want to be crafting. You can also re-enchant enchanted items but that gets more costly.&lt;/p&gt;&lt;p&gt;You can also just go to the shop and buy multiple items to enchant, like broken daggers.&lt;/p&gt;&lt;p&gt;- Next, when you have enchanted, ideally 75 items, next go to your inventory&lt;/p&gt;&lt;p&gt;- From the actions on the inventory section of your character sheet, click Disenchant All.&lt;/p&gt;&lt;p&gt;- This will raise your disenchanting skill, and slowly over time your enchanting skill as well.&lt;/p&gt;&lt;p&gt;- Repeat till you meet the quest requirements.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- Open Craft from the drop down selection&lt;/p&gt;&lt;p&gt;- from the Craft/Enchant drop down select enchant&lt;/p&gt;&lt;p&gt;- Here you have an item to select, a suffix and a prefix to select. The cost of enchanting can get widely expensive so exploration is required. Since you need items: weapons, Armour, spells and Rings, you will also want to be crafting. You can also re-enchant enchanted items but that gets more costly.&lt;/p&gt;&lt;p&gt;You can also just go to the shop and buy multiple items to enchant, like broken daggers.&lt;/p&gt;&lt;p&gt;- Next, when you have enchanted, ideally 75 items, next go to your inventory&lt;/p&gt;&lt;p&gt;- From the actions on the inventory section of your character sheet, click Disenchant All.&lt;/p&gt;&lt;p&gt;- This will raise your disenchanting skill, and slowly over time your enchanting skill as well.&lt;/p&gt;&lt;p&gt;- Repeat till you meet the quest requirements.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Enchanting</t>
-  </si>
-  <si>
-    <t>Disenchanting</t>
-  </si>
-  <si>
-    <t>Enchanter's Book</t>
-  </si>
-  <si>
-    <t>Traveling To Dungeons</t>
-  </si>
-  <si>
-    <t>You have come a long way since you first set out. Learning more of the world, learning more about your self and developing your skills.&lt;br /&gt; &lt;br /&gt; You sit under the tree outside of town and watch the merchants go by. A few stop and ask if you would like to purchase some of their wares, a few have some interesting knickknacks, and a few others have some food worth buying.&lt;br /&gt; &lt;br /&gt; As the day passes by and the sun begins to set you think of heading back to town to wash, relax and get a good nights sleep.&lt;br /&gt; &lt;br /&gt; “Hello there” comes an unfamiliar voice.&lt;br /&gt; &lt;br /&gt; You look and see a man in a Fedora, Green Tunic and black leather pants. He seems older, but moves as if he is younger then his age.&lt;br /&gt; &lt;br /&gt; He comes closer and introduces himself, “I am The Poet and have been sent by The Guide to ask a favor of you, one from him.”&lt;br /&gt; &lt;br /&gt; You ask why he doesn’t come himself and ask this favor.&lt;br /&gt; &lt;br /&gt; “There is a darkness that is seeping from the depths into all the Planes. It is corrupting the Planes and causing the creatures to become vile and wicked. The Guide is busy investigating something deep with in Dungeons. Where he wants you to meet him.”&lt;br /&gt; &lt;br /&gt; You remember how you got to labyrinth, how hard can it be to get to Dungeons? You agree and The Poet tells you how to set off.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; &lt;em&gt;This quest can take 2+ hours to complete as you will need to earn Gold Dust for some of the requirements to be completed.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;This is another &lt;a href="/information/quests" target="_blank"&gt;quest&lt;/a&gt; where we are going to a new &lt;a href="/information/planes" target="_blank"&gt;plane&lt;/a&gt;. However, to get there we have to complete a few quests to unlock access.&lt;/p&gt;&lt;p&gt;Quests are how a lot of Tlessas features are unlocked for players. These quests, much like Guide Quests, will have a story – before and after completion – as well as explicit instructions on how to complete them, much like these.&lt;/p&gt;&lt;p&gt;Since you already know how to &lt;a href="/information/traverse" target="_blank"&gt;traverse&lt;/a&gt;, we just need to get you a quest item that allows you to traverse down to Dungeons.&lt;/p&gt;&lt;p&gt;For the requirement of getting access to Dungeons, some quests will require the player to earn Gold Dust as part of the quest requirements, by now you know of two ways: Craft → Enchant → Disenchant All items and Fight monsters and disenchant what you don’t want.&lt;/p&gt;&lt;p&gt;There is a third way: Weekly Currency Events. These give players Gold Dust, Crystal Shards (Shards) and (you wont have the quest item for them yet) Copper Coins.&lt;/p&gt;&lt;p&gt;Using exploration on these days can get you 1-50 of each currency (minus copper coins) for each monster you kill. Exploration can pit you up against 8 monsters at a time, which can be roughly 400 of each currency (roughly, as its random amount).&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; The required secondary quest item, will require you to complete a quest from Labyrinth under the One Off Quest section called: &lt;strong&gt;Dark Enchantress.&lt;/strong&gt; Click the quest, and click on the Requirements tab to see what you have to do.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- Click the Quests tab&lt;/p&gt;&lt;p&gt;- Here you can see a list of quests for the plane you are on (if you are not on surface, select the Surface plane from the Planes drop down.)&lt;/p&gt;&lt;p&gt;- On the Surface quests you will see a quest (to the left) called Light The Way, complete the quests working down the tree until you complete it. Locked Quests are red, quests you can complete are Blue and Completed Quests are Green.&lt;/p&gt;&lt;p&gt;- Click on the quest to read the story, see the requirements and the reward.&lt;/p&gt;&lt;p&gt;- The Requirements tab will have explicit instructions beside each requirement.&lt;/p&gt;&lt;p&gt;- Much like Guide Quests, you can see your completed quests in the sidebar (Hamburger menu to the top left) under: Quest Log → Completed Quests.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- Tap the Quests tab&lt;/p&gt;&lt;p&gt;- Here you can see a list of quests for the plane you are on (if you are not on surface, select the Surface plane from the Planes drop down.)&lt;/p&gt;&lt;p&gt;- On the Surface quests you will see a quest (to the left – you can scroll left/right) called Light The Way, complete the quests working down the tree until you complete it. Locked Quests are red, quests you can complete are Blue and Completed Quests are Green.&lt;/p&gt;&lt;p&gt;- Tap on the quest to read the story, see the requirements and the reward.&lt;/p&gt;&lt;p&gt;- The Requirements tab will have explicit instructions beside each requirement.&lt;/p&gt;&lt;p&gt;- Much like Guide Quests, you can see your completed quests in the sidebar (Hamburger menu to the top left) under: Quest Log → Completed Quests.&lt;/p&gt;&lt;p&gt;Quests, much like Enchanting are vitally important to progress not only the over all story of the game, but also to get access to new features, new planes and so on of the game.&lt;/p&gt;&lt;p&gt;Each Plane will tell a story that all come together to tell a general story of The Creator (not the game Creator – an NPC) Quest chains going straight down tell their own story.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Dungeons</t>
-  </si>
-  <si>
-    <t>Torch</t>
-  </si>
-  <si>
-    <t>Enchantress' Diary</t>
-  </si>
-  <si>
-    <t>Death is something special</t>
-  </si>
-  <si>
-    <t>The Dungeons plane crawls with death. There is a darkness that seeps across the ground, infecting and infesting everything that it touches. You seem to be immune to it. You know there is shadow in the distance that is watching you. A shade like creature that only makes it’s self visible every now and then to your eyes.&lt;br /&gt; &lt;br /&gt; “Child!” Comes a familiar voice. The Guide, young, handsome and ever changing comes up to you.&lt;br /&gt; &lt;br /&gt; “You have come down the Dungeons. A place of ruins, crypts, caves and other bits of darkness that one can explore for loot.”&lt;br /&gt; &lt;br /&gt; You ask him about the darkness crawling across the land and the shade like creature you can see off in the distance.&lt;br /&gt; &lt;br /&gt; “The darkness is caused by the gates of Shadow Planes, which has opened. The shade creature is the Shade Lord. He is seeking something, something that escaped the darkness beneath the pits of Hell. Alas to take on any of these creatures you need to get stronger!”</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; &lt;em&gt;This quest can take 2 hours or more to complete.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Now we learn about a new feature: &lt;a href="/information/class-skills" target="_blank"&gt;Class Skills&lt;/a&gt; and Class Bonus.&lt;/p&gt;&lt;p&gt;Class Skills are different for each &lt;a href="/information/races-and-classes#3" target="_blank"&gt;class&lt;/a&gt; in the game. Every class has a skill which you can see on your skills table under Training Tab. It has an icon beside it and is in orange text.&lt;/p&gt;&lt;p&gt;This skill important to level because it allows you to increase your Class Bonus which can be seen on the character sheet to the left, under inventory count or on mobile under Class Details, at the bottom of the details section.&lt;/p&gt;&lt;p&gt;Your class will tell you, if you click/tap on the class name in the top bar where you basic details are, the requirements for your class special attack to fire. This means what weapons or spells you must have equipped and how many. If you also need to use a specific attack type or not.&lt;/p&gt;&lt;p&gt;Based on those factors and the % of your class bonus, your special can just fire in the middle of an attack, which you will see when manually fighting.&lt;/p&gt;&lt;p&gt;Each class has it’s own special attack and special rules for those attacks.&lt;/p&gt;&lt;p&gt;Class Skills can also raise specific attributes about the class such as damage, healing and armour class bonuses that stack with all other bonuses.&lt;/p&gt;&lt;p&gt;At this stage in the game, the one important thing I can tell you is: unless it states that it wont stack, everything stacks together to raise your stats, damage, armour class, healing as well as stats, skills and so on.&lt;/p&gt;&lt;p&gt;When utilizing, as we will soon, &lt;a href="/information/class-ranks" target="_blank"&gt;Class Ranks&lt;/a&gt; to switch classes, you will notice that one skill on your Skills tab on the Character Sheet, will change. Every time you change a class your character will switch their class skill.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- The instructions state to level a Effects Class to the specified level. To do this, go to your character sheet section, in your skill section – train the skill with the orange text to the specified level.&lt;/p&gt;&lt;p&gt;- To Get the Gold Dust you can disenchant items that drop you no longer need, or craft some items, enchant them and disenchant them. Now is the time to explore the &lt;a href="http://127.0.0.1:8000/information/enchanting" target="_blank"&gt;Enchanting&lt;/a&gt; list in the docs to see what types of enchantments you can apply to your equipment so you can start creating a gear set geared towards your needs.&lt;/p&gt;&lt;p&gt;That’s it. Now you might not see your class bonus fire off much at first, but over time, keep leveling this skill and you will start to see your special fire off automatically when manually fighting.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Dancing Shadows</t>
-  </si>
-  <si>
-    <t>You're bones ache, your body is bruised, your strength is depleted. You lie upon the ground, broken bits of buildings, scattered across the ground show you the ruins of this plane.&lt;br /&gt; &lt;br /&gt; Your memory drifts back to the days when you were carefree, young and playing in the fields while your parents worked in the fields.&lt;br /&gt; &lt;br /&gt; You remember the house, the laughter, the Sunday dinners and the other farm kids when it came time to harvest. The bountiful parties, the celebrations of summer transitioning to fall.&lt;br /&gt; &lt;br /&gt; You miss your home, you miss your family.&lt;br /&gt; &lt;br /&gt; Your eye catches the shadow in the distance, a shadow on the end of the small campfire flame that you burn in the darkness of this plane.&lt;br /&gt; &lt;br /&gt; The shadow dances.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; &lt;em&gt;This quest can take 2 hours or more to complete.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Lets learn about &lt;a href="/information/class-ranks" target="_blank"&gt;Class Ranks&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;Class ranks are, for those familiar, similar to Final Fantasy Job Switching mechanics – which are present in a verity of other RPG’s.&lt;/p&gt;&lt;p&gt;At any time, a character may switch classes by utilizing the class rank system. Each class is leveled by simply killing creatures, as you level the class you unlock special abilities that you can equip and further level to gain additional benefits and modifiers.&lt;/p&gt;&lt;p&gt;Some abilities can only be equipped when you have leveled that class rank (by being that class and killing creatures) to the required level. And other abilities, such as those that do damage, cannot stack or be equipped while others of that type are equipped.&lt;/p&gt;&lt;p&gt;This is another layer of character development, as you can mix and match abilities from various classes to create your own build.&lt;/p&gt;&lt;p&gt;Some classes in Class Ranks cannot be switched to until you have leveled other classes to a specific class rank, these classes, like Prisoner – for example – cannot be selected at registration for this reason.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Lets level our current Class Rank and equip a class special.&lt;/p&gt;&lt;p&gt;To do this:&lt;/p&gt;&lt;p&gt;- Go to your Character Sheet Tab.&lt;/p&gt;&lt;p&gt;- Click the orange button called Class Ranks&lt;/p&gt;&lt;p&gt;- Find your class in the list, beside the name is the level – you will need to raise this to meet the requirement. You do this via exploration.&lt;/p&gt;&lt;p&gt;- Click the class name. Here you can see details about your class, including mastery's which level in the same fashion as Class Ranks, by killing creatures – with the caveat that you have the item equipped.&lt;/p&gt;&lt;p&gt;- You will also see a red circle with a minus in it. Click this at any time to close the class details and see your class rank list. Clicking cancel at this state will close this modal.&lt;/p&gt;&lt;p&gt;- Click Manage Specialties. This will open a secondary modal that shows you the class specials you can equip. You may only equip 3, and only one of those three may be a special that deals damage. If you have one that deals damage (click the name to see further details) – and you can equip it, do so. If not find one that you can equip and equip it.&lt;/p&gt;&lt;p&gt;By equipping a class special, you will level it via killing creatures. The longer you leave it equipped the more levels, the more benefit it gives.&lt;/p&gt;&lt;p&gt;- Now, kill something – many times over. These will not take long to level, keep an eye on the Server Messages tab for levels – you may have already seen these pop up over time.&lt;/p&gt;&lt;p&gt;Let’s also do some crafting. Consider this a “where are you in your crafting and enchanting?”&lt;/p&gt;&lt;p&gt;If you can, equip a full set of the crafting type required enchantments on the best gear you can craft. This will help you reach the crafting requirement faster. If you then switch to a set of enchantment skill raising enchantments and then enchant all that crafted gear and finally disenchant it all, you will level both enchanting and disenchanting, and leveling disenchanting gets you more Gold Dust per disenchanted item.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Lets level our current Class Rank and equip a class special.&lt;/p&gt;&lt;p&gt;To do this:&lt;/p&gt;&lt;p&gt;- Tap Character Sheet Tab&lt;/p&gt;&lt;p&gt;- Tap to expand the Character Details&lt;/p&gt;&lt;p&gt;- Find the Orange Button: Class Ranks, Tap It.&lt;/p&gt;&lt;p&gt;- Tap the class name. Here you can see details about your class, including mastery's which level in the same fashion as Class Ranks, by killing creatures – with the caveat that you have the item equipped.&lt;/p&gt;&lt;p&gt;- You will also see a red circle with a minus in it. Click this at any time to close the class details and see your class rank list. Clicking cancel at this state will close this modal.&lt;/p&gt;&lt;p&gt;- Tap Manage Specialties. This will open a secondary modal that shows you the class specials you can equip. You may only equip 3, and only one of those three may be a special that deals damage. If you have one that deals damage (click the name to see further details) – and you can equip it, do so. If not find one that you can equip and equip it.&lt;/p&gt;&lt;p&gt;By equipping a class special, you will level it via killing creatures. The longer you leave it equipped the more levels, the more benefit it gives.&lt;/p&gt;&lt;p&gt;- Now, kill something – many times over. These will not take long to level, keep an eye on the Server Messages tab for levels – you may have already seen these pop up over time.&lt;/p&gt;&lt;p&gt;Let’s also do some crafting. Consider this a “where are you in your crafting and enchanting?”&lt;/p&gt;&lt;p&gt;If you can, equip a full set of the crafting type required enchantments on the best gear you can craft. This will help you reach the crafting requirement faster. If you then switch to a set of enchantment skill raising enchantments and then enchant all that crafted gear and finally disenchant it all, you will level both enchanting and disenchanting, and leveling disenchanting gets you more Gold Dust per disenchanted item.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Hired Help</t>
-  </si>
-  <si>
-    <t>Your strength seems to be restored from a night by the fire. The ruins of the various dungeons, castles and other structures that litter this land much like labyrinth, holds an eerie silence in the early morning hours.&lt;br /&gt; &lt;br /&gt; The fog and the dampness in the air create a chill that seeps into your bones and causes a shiver. Suddenly on the outskirts of the fog is a shade like creature that stands there, watching, waiting. You stand and shout, but the fog makes the creature disappear deeper into the silence.&lt;br /&gt; &lt;br /&gt; You head off towards the direction of the creature, weapons ready and spells glowing. You search th fog, turning this way and that – you see nothing, you feel the presence. It touches you and you feel weaker, your enchantments, your own magic- it all melts away.&lt;br /&gt; &lt;br /&gt; A whisper: Strength.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;:&lt;strong&gt; &lt;/strong&gt;&lt;em&gt;This quest can take 2+ Hours to complete&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Lets learn about &lt;a href="/information/mercenary" target="_blank"&gt;mercenaries&lt;/a&gt;, which help with getting currencies through a mini game called &lt;a href="/information/slots" target="_blank"&gt;slots&lt;/a&gt;. How fun! Gambling!&lt;/p&gt;&lt;p&gt;Mercenaries are NPC’s who grant you a passive buff the more you level them and reincarnate them. The buff they give you is a % bonus towards the drop amount of that currency from slots and other aspects of the game.&lt;/p&gt;&lt;p&gt;For example, The child of gold dust is a mercenary that allows you to gain +x% based on it’s current level, towards any action that would give you gold dust.&lt;/p&gt;&lt;p&gt;The beauty with mercenaries is that they also stack with the event: Weekly Currency Drop for even more currencies.&lt;/p&gt;&lt;p&gt;Mercenaries, once they reach level 100, can be reincarnated to increase the bonus towards currency acquisition. Mercenaries are purchased and require you to complete the quest listed to unlock them.&lt;/p&gt;&lt;p&gt;Mercenaries gain levels by you fighting monsters.&lt;/p&gt;&lt;p&gt;Purchase the mercenaries required for this quest, after completing the required quest.&lt;/p&gt;&lt;p&gt;Slots are a way for characters to make passive income. You can get Gold, Shards, Gold Dust and Copper Coins. Copper coins will not drop for you yet because you do not have the required quest item yet.&lt;/p&gt;&lt;p&gt;Slots take gold to spin and can, with the aid of mercenaries, reward the player with a godly amount of currency.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;By now we know how to utilize exploration and question. So lets quest to unlock mercenaries and then use a new feature while we have exploration running to gain some currencies from slots.&lt;/p&gt;&lt;p&gt;- First complete the quest: &lt;strong&gt;The truth is Out There&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Next go to Character Sheet and click on the Mercenaries Tab&lt;/p&gt;&lt;p&gt;- Select the required mercenaries as shown above and purchase them.&lt;/p&gt;&lt;p&gt;- Level them to the required level via exploration.&lt;/p&gt;&lt;p&gt;- Next, in the action section, click slots.&lt;/p&gt;&lt;p&gt;- Spin baby spin!&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;By now we know how to utilize exploration and question. So lets quest to unlock mercenaries and then use a new feature while we have exploration running to gain some currencies from slots.&lt;/p&gt;&lt;p&gt;- First complete the quest: &lt;strong&gt;The truth is Out There&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Next go to Character Sheet and tap on the Mercenaries Tab&lt;/p&gt;&lt;p&gt;- Select the required mercenaries as shown above and purchase them.&lt;/p&gt;&lt;p&gt;- Level them to the required level via exploration.&lt;/p&gt;&lt;p&gt;- Next, in the action section, select slots from the action drop down.&lt;/p&gt;&lt;p&gt;- Spin baby spin!&lt;/p&gt;</t>
+    <t>Chasing Shadows</t>
+  </si>
+  <si>
+    <t>You stand in the ruins of a land covered in the memories of the gladiators who died in the many labyrinths that were built and destroyed over the years.&lt;br /&gt; &lt;br /&gt; It is said that a mad Architect created this world, who also then created one labyrinth after the other and then abandoned the world to its own ends only for it fall into ruins.&lt;br /&gt; &lt;br /&gt; You remember the death, the blood, the gore and the bodies.&lt;br /&gt; &lt;br /&gt; They were all dead, but it was also empty when you entered.&lt;br /&gt; &lt;br /&gt; You search the ruins for answers. You find nothing but shadows of memories lost to time.&lt;br /&gt; &lt;br /&gt; A shadow moves across the ruins. A shadow that you recognize for the INN.&lt;br /&gt; &lt;br /&gt; You chase the shadow, but it alludes you.&lt;br /&gt; &lt;br /&gt; “Child.”&lt;br /&gt; &lt;br /&gt; A familiar voice, you turn and see The Guide. He is old haggard and damaged. He coughs in a handkerchief that is covered in blood.&lt;br /&gt; &lt;br /&gt; “I must see The Poet.”&lt;br /&gt; &lt;br /&gt; he coughs and wheezes. You move towards to help him but he waives your advance off.&lt;br /&gt; &lt;br /&gt; “Learn something of your self.” he turns and walks away coughing and wheezing as he does.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Let’s do what the Guide stated: Learn something about our selves. Class Ranks.&lt;/p&gt;&lt;p&gt;&lt;a href="/information/class-ranks" target="_blank"&gt;Class Ranks&lt;/a&gt; allow you to switch classes and equip special abilities that can boost your character stats or even give you a special attack that will fire any time you attack an enemy allowing you to do even more damage.&lt;/p&gt;&lt;p&gt;Class Ranks comes with, as mentioned, Specialties which as leveled make your character even stronger. To level them you just have to equip the ones you want and then go kill things using exploration – as manual leveling will take a very long time and can be very grindy.&lt;/p&gt;&lt;p&gt;Class Ranks also come with masteries. As a character who has specific weapons equipped will level these masteries over time while killing creatures and gaining more bonuses to damage while using that weapon.&lt;/p&gt;&lt;p&gt;As mentioned before Characters can, at any time switch classes. You can level the rank of that class by killing creatures.&lt;/p&gt;&lt;p&gt;As you level the class it’s self and switch to other classes and level them, not only will you unlock the specialties you can equip (and thus mix and max) you will also eventually unlock other classes you can switch too that require you to level two or more classes.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;- Click Character Sheet Tab&lt;/p&gt;&lt;p&gt;- Click Class Ranks Orange Button&lt;/p&gt;&lt;p&gt;- Look for your class in the list and click the name&lt;/p&gt;&lt;p&gt;- This will open another window, to exit back to the class list click the red circle with the minus in the top right. Clicking cancel or the X will close the modal.&lt;/p&gt;&lt;p&gt;- Here you will see information about the class and the Class Masteries&lt;/p&gt;&lt;p&gt;- Click Manage Specialties&lt;/p&gt;&lt;p&gt;- Equip a specialty and boom done, now you just have to kill creatures.&lt;/p&gt;&lt;p&gt;- The server messages will tell you when you gain levels in your Masteries and your Specialties as well as your Class Rank&lt;/p&gt;&lt;p&gt;Now you just have to kill creatures till you meet the requirements.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;- Tap Character Sheet tab&lt;/p&gt;&lt;p&gt;- expand the Character Details Section&lt;/p&gt;&lt;p&gt;- Tap the Class Ranks orange button&lt;/p&gt;&lt;p&gt;- Look for your class in the list and tap the name&lt;/p&gt;&lt;p&gt;- This will open another window, to exit back to the class list tap the red circle with the minus in the top right. Tap cancel or the X will close the modal.&lt;/p&gt;&lt;p&gt;- Here you will see information about the class and the Class Masteries&lt;/p&gt;&lt;p&gt;- Tap Manage Specialties&lt;/p&gt;&lt;p&gt;- Equip a specialty and boom done, now you just have to kill creatures.&lt;/p&gt;&lt;p&gt;- The server messages will tell you when you gain levels in your Masteries and your Specialties as well as your Class Rank&lt;/p&gt;&lt;p&gt;Now you just have to kill creatures till you meet the requirements.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Gamble the horror away</t>
+  </si>
+  <si>
+    <t>You managed to make your way to Smugglers Port where you hear of a game that can be played and where one can attempt to win currencies!&lt;br /&gt; &lt;br /&gt; You asked around the port town and people have told you what they know and pointed you to a pub where a man stands by a weird looking box that magically seems to change and roll. People give money and watch this box split into three and roll, sometimes the images match, some times they don’t and the patrons leave with no money or even less then they had.&lt;br /&gt; &lt;br /&gt; You decide to take a gamble and take a moment for your self.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Lets gamble and have some fun! First we want to unlock a feature that will help us our, not just when gambling but also when fighting creatures! We need currencies – Gold Dust and eventually Shards – which are also used in quests and a new type of crafting we will soon unlock: &lt;a href="/information/alchemy" target="_blank"&gt;Alchemy&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;This new feature is called: &lt;a href="/information/mercenary" target="_blank"&gt;Mercenaries&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;Mercenaries allow you to gain more currencies as you level them and then reincarnate them. The will give a bonus which is equal to their level and the amount of times (to a max of 1100%) towards &lt;a href="/information/currencies" target="_blank"&gt;currency&lt;/a&gt; acquisition for Shards, Gold Dust and Copper Coins.&lt;/p&gt;&lt;p&gt;Mercenaries help out the most with &lt;a href="/information/slots" target="_blank"&gt;Slots&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;Slots is a way for players to gamble and potentially win currencies. The caveat is one of the currencies cannot be rewarded at this time, because you don’t have the right quest item, Copper Coins.&lt;/p&gt;&lt;p&gt;To level a Mercenary you need to complete a quest to unlock the feature and then pay gold to purchase the type of mercenary you want.&lt;/p&gt;&lt;p&gt;After that all you have to do is fight creatures and over time the Mercenaries will level. As you reach level 100 on one of them you can reincarnate them, re-level them up and gain 200% towards currency acquisition. Then just repeat this process 9 more times.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;- Complete the quest on Labyrinth: “The truth is out there”&lt;/p&gt;&lt;p&gt;- Click Character Sheet Tab&lt;/p&gt;&lt;p&gt;- Click the tab: Mercenaries&lt;/p&gt;&lt;p&gt;- Purchase the mercenaries required&lt;/p&gt;&lt;p&gt;- Level the Mercenary to the required leveling&lt;/p&gt;&lt;p&gt;- Play slots if you have the gold and kill creatures to level the mercenaries through exploration!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;- Complete the quest on Labyrinth: “The truth is out there”&lt;/p&gt;&lt;p&gt;- Tap Character Sheet Tab&lt;/p&gt;&lt;p&gt;- Tap the tab: Mercenaries&lt;/p&gt;&lt;p&gt;- Purchase the mercenaries required&lt;/p&gt;&lt;p&gt;- Level the Mercenary to the required leveling&lt;/p&gt;&lt;p&gt;- Play slots (select slots from the actions drop down) if you have the gold and kill creatures to level the mercenaries!&lt;/p&gt;</t>
   </si>
   <si>
     <t>child-of-gold-dust</t>
   </si>
   <si>
-    <t>child-of-shards</t>
-  </si>
-  <si>
-    <t>The truth is out there</t>
-  </si>
-  <si>
-    <t>Alchemical dreams</t>
-  </si>
-  <si>
-    <t>An old man sits on the edge of your vision. He walks, slowly towards you. The bottles clink together and he speaks in riddles. Your head spins. The shade is at the other side of the horizon. Follow him child and create the doors you need to open.&lt;br /&gt; &lt;br /&gt; You can hear a bang in the distance, once that gets louder and passes you buy. A scream, a cry, a death curdling scream of pain and loss permeates your heart.&lt;br /&gt; &lt;br /&gt; You feel the pain, you see the darkness, you can feel the blood, coming from your head. Why are you bleeding.&lt;br /&gt; &lt;br /&gt; You collapse into the sweet embrace of the shadows arms as it reaches out to take your limp body into the horizon.&lt;br /&gt; &lt;br /&gt; “Child.” You awaken in a strange place, but you recognize the man before you, The Poet.&lt;br /&gt; &lt;br /&gt; Why is here.&lt;br /&gt; &lt;br /&gt; “I want to tell you about the potions, the drinks for the various ways you can craft your own power, if only limited for a time.”&lt;br /&gt; &lt;br /&gt; His voice fades, and you fall to the ground.&lt;br /&gt; &lt;br /&gt; “Child?”</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;:&lt;strong&gt; &lt;/strong&gt;&lt;em&gt;This quest can take 2+ Hours to complete&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Another mechanic that players can user to make them selves powerful, even if only for a brief time is through the concept of boons. &lt;a href="/information/alchemy" target="_blank"&gt;Boons&lt;/a&gt; are timed effects that last minutes on a character and can, in some cases and unless otherwise stated, stack with each other to give you even more power.&lt;/p&gt;&lt;p&gt;There are two ways to get boons: &lt;a href="/information/goblin-shop" target="_blank"&gt;The Goblin shop&lt;/a&gt; sells some powerful ones for Gold bars which are only obtainable by owning kingdoms and making vast amounts of gold, and then Alchemy. Which we will talk about.&lt;/p&gt;&lt;p&gt;Alchemy is a crafting skill that requires you to complete a one off quest on Surface called &lt;strong&gt;I dream of Alchemy&lt;/strong&gt;.&lt;/p&gt;&lt;p&gt;Once you have this quest complete the option will show up under the Craft/Enchant section.&lt;/p&gt;&lt;p&gt;Alchemy requires Gold Dust and Crystal Shards (Shards). One you get from disenchanting enchanted items and the other you get from killing &lt;a href="/information/celestials" target="_blank"&gt;celestials&lt;/a&gt;, which you are too weak for.&lt;/p&gt;&lt;p&gt;Alchemy items come in many forms, but there are three kinds: Stat Boosting, Kingdom Damage Dealing and Holy Oils for a later type of crafting. Some alchemy items like &lt;a href="/information/holy-items" target="_blank"&gt;Holy Oils&lt;/a&gt; can be applied to items, while kingdom damaging items can be used on other players kingdoms and stat boosting are usable items that can be used on your self to create boons.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- Complete the quest: &lt;strong&gt;I dream of Alchemy&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Open Craft/Enchant&lt;/p&gt;&lt;p&gt;- Select Alchemy&lt;/p&gt;&lt;p&gt;- Select an item&lt;/p&gt;&lt;p&gt;- Craft the item, repeat.&lt;/p&gt;&lt;p&gt;You should have enough shards and gold dust to reach the desired level.&lt;/p&gt;&lt;p&gt;To use an item on your self, assuming it is usable on you, follow the below steps:&lt;/p&gt;&lt;p&gt;- Click Character Sheet Tab&lt;/p&gt;&lt;p&gt;- Select Usable From the Type drop down in your inventory section.&lt;/p&gt;&lt;p&gt;- Here you can see your usable items.&lt;/p&gt;&lt;p&gt;- You can either use your items individually from the actions drop down beside them, or you can select Use Many from the Actions drop down above the usable table.&lt;/p&gt;&lt;p&gt;- Use many will filter out any item that cannot stack, that is, you cannot select multiple to apply to your self.&lt;/p&gt;&lt;p&gt;Items you use on your self will show up in the Active Boons Tab of the character information in the top left of the character sheet tab.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- Complete the quest: &lt;strong&gt;I dream of Alchemy&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;Open Crafting from the actions drop down&lt;/p&gt;&lt;p&gt;- Open Craft/Enchant&lt;/p&gt;&lt;p&gt;- Select Alchemy&lt;/p&gt;&lt;p&gt;- Select an item&lt;/p&gt;&lt;p&gt;- Craft the item, repeat.&lt;/p&gt;&lt;p&gt;You should have enough shards and gold dust to reach the desired level.&lt;/p&gt;&lt;p&gt;To use an item on your self, assuming it is usable on you, follow the below steps:&lt;/p&gt;&lt;p&gt;- Tap Character Sheet Tab&lt;/p&gt;&lt;p&gt;- Select Inventory management from the drop down&lt;/p&gt;&lt;p&gt;- Select Usable From the Type drop down in your inventory section.&lt;/p&gt;&lt;p&gt;- Here you can see your usable items.&lt;/p&gt;&lt;p&gt;- You can either use your items individually from the actions drop down beside them, or you can select Use Many from the Actions drop down above the usable table.&lt;/p&gt;&lt;p&gt;- Use many will filter out any item that cannot stack, that is, you cannot select multiple to apply to your self.&lt;/p&gt;&lt;p&gt;Items you use on your self will show up in the Active Boons Tab which you can get to by expanding Character Details and tapping the Active Boons tab.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Alchemy</t>
-  </si>
-  <si>
-    <t>Ring Crafting</t>
-  </si>
-  <si>
-    <t>Home again Pt. 1</t>
-  </si>
-  <si>
-    <t>“Hullo?”&lt;br /&gt; &lt;br /&gt; A voice comes from the darkness of your dreams.&lt;br /&gt; &lt;br /&gt; You open your eyes and see a goblin standing before you, gently poking you with a stick. Yo8u bat away the stick and stand to greet this creature. He doesn’t seem dangerous.&lt;br /&gt; &lt;br /&gt; “You are alive!” The Goblin shrieks in joy.&lt;br /&gt; &lt;br /&gt; You ask him where you are rubbing the back of your neck and trying to orient your self to your surroundings.&lt;br /&gt; &lt;br /&gt; “Silly you. You are on surface.”&lt;br /&gt; &lt;br /&gt; You look around, the trees, the sky, the smells. How?&lt;br /&gt; &lt;br /&gt; “Do you want to play?"</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Look at you go, look at the distance you have traveled. The Gear, the monsters, the power! Alas, child you still have a long way to go and the next few steps will prepare you for the next leg of your journey!&lt;/p&gt;&lt;p&gt;We will help this goblin complete a few tasks and gain some items that will help our character out skill wise and for later quests.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Complete the required objectives using the knowledge you have gained so gar.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Surface</t>
-  </si>
-  <si>
-    <t>Faction Hunter</t>
-  </si>
-  <si>
-    <t>Home again pt. 2</t>
-  </si>
-  <si>
-    <t>You hang out with The Goblin for a while, realizing he is not as helpless as he appears to be. You slaughter a few creatures here and there, share a meal and discuss the events and his life.&lt;br /&gt; &lt;br /&gt; You stare at the stars each night wondering if everything you just experienced was a dream. You close your eyes.&lt;br /&gt; &lt;br /&gt; Blood, dripping down the wall, a metallic object on the floor, the lifeless and still hands of boy no older then 25 sits hunched against the wall, blood drips down from a wound in the head.&lt;br /&gt; &lt;br /&gt; A cream, a women. A scream. She rushes over. A scream – she grabs the child and holds his lifeless body close.&lt;br /&gt; &lt;br /&gt; “Child.”&lt;br /&gt; &lt;br /&gt; You turn around, a clearing, fields – summer breeze.&lt;br /&gt; &lt;br /&gt; “Wake up child.”&lt;br /&gt; &lt;br /&gt; The Poet. What is he doing here, you turn back but there stretches the ruins of a old world road, yellow paint lines the middle of the cracked and broken road.&lt;br /&gt; &lt;br /&gt; “Child.”&lt;br /&gt; &lt;br /&gt; You turn back, The Poet. He glows. The light is too bright.&lt;br /&gt; &lt;br /&gt; “It is not your time. Wake up.”&lt;br /&gt; &lt;br /&gt; You awaken to The Goblin staring at you.&lt;br /&gt; &lt;br /&gt; “You ok child?”</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; &lt;em&gt;This quest can take 2+ Hours to complete.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Lets get some items that help with dodging enemies attacks and an item for helping with accuracy. To do this, we will do two more quests for The Goblin:&lt;/p&gt;&lt;p&gt;- &lt;strong&gt;Goblins gift&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;- Goblins Accuracy&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;These can both be found on surface.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Golden Ring of Blur</t>
-  </si>
-  <si>
-    <t>The Book of Guidance</t>
-  </si>
-  <si>
-    <t>Dreams of the Dead</t>
-  </si>
-  <si>
-    <t>Days have gone by and no dream has haunted you like the previous one.&lt;br /&gt; &lt;br /&gt; Odd chores and bits and bobs around the small ramshackle camp you and The Goblin have set up.&lt;br /&gt; &lt;br /&gt; He comes into the camp with his bits and bobs and stolen items that he pick pocketed off wondering merchants. You peer through his treasures and find a letter.&lt;br /&gt; &lt;br /&gt; “Whats ya got there?” The goblin asks snatching the letter away.&lt;br /&gt; &lt;br /&gt; “Seems to be addressed to you! How unique!”&lt;br /&gt; &lt;br /&gt; You take the letter back from him and read the contents, it’s from The Poet&lt;br /&gt; &lt;br /&gt; Seems you have been busy my child. I need your assistance in a place far from the comforts of home. Alas for you to open such gates you must survive the trials and become stronger, unlocking a power with in your self.&lt;br /&gt; &lt;br /&gt; There is a crown, from a king long dead. His crown will help you take on even stronger creatures, creatures that can look at you and make you weak! Make your spells fail, your enchantments fizzle and fail. These creatures are fearsome.&lt;br /&gt; &lt;br /&gt; Alas, your adventures will take you deeper into those dreams of yours …&lt;br /&gt; &lt;br /&gt; The Poet&lt;br /&gt; &lt;br /&gt; You look up from the letter and The Goblin looks at you:&lt;br /&gt; &lt;br /&gt; “Whats up?Where are we off too?”</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; &lt;em&gt;This quest can take 2+ Hours to complete.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;The Poet is correct, you need a new tool in your tool belt to help you take on stronger creatures and new planes and even further down the list on the critter list.&lt;/p&gt;&lt;p&gt;The concept we need to learn is &lt;a href="/information/voidance" target="_blank"&gt;Voidance/Devoidance&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;The basics of this is simple, voiding something means its enchantments will fizzle and fail making you much much weaker, as if you just have base gear equipped.&lt;/p&gt;&lt;p&gt;This means death for you.&lt;/p&gt;&lt;p&gt;However, there is an opposite side to voidance called: devoidance, where you make the enemies voidance fail to fire, thus your enchantments do not fizzle and fail and you get to live to fight another day!&lt;/p&gt;&lt;p&gt;The concept is known as Devouring Light (Voidance) and Devouring Darkness (Devoidance).&lt;/p&gt;&lt;p&gt;The quest item in question , can be gotten by completing the quest: The Return of The Kings Crown, and will give you a percentage chance to void/devoid your enemy.&lt;/p&gt;&lt;p&gt;This concept works in pvp, celestial fights, raids and regular critter fights. There is one small exception to this: In all battles you attempt to devoid then the enemy, then you try and void the enemy (assuming you are not devoided) and if the enemy is not voided and not devoided, they will try and void your enchantments.&lt;/p&gt;&lt;p&gt;Where this changes is Purgatory, where the order is reversed, enemy first, you last.&lt;/p&gt;&lt;p&gt;The first quest item requirement, will help you with disenchanting and gaining more Gold Dust when you do so, which will be important soon.0&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Complete the required objectives using the knowledge you have gained so gar.&lt;/p&gt;&lt;p&gt;You can see your voidance, devoidance by doing:&lt;/p&gt;&lt;p&gt;- Click Character Sheet tab&lt;/p&gt;&lt;p&gt;- Click Additional Information orange button.&lt;/p&gt;&lt;p&gt;- Click Voidance tab&lt;/p&gt;&lt;p&gt;Now you can see your resistance to such effects as well as your chance to do said action to the enemy.&lt;/p&gt;&lt;p&gt;The quest line in question will get you an item that raises these significantly, but you can enchant devouring light on your gear by going to the enchantment list here, and searching the filters for: &lt;a href="/information/enchanting?table[filters][types]=3" target="_blank"&gt;Skill/Res Reduction + Devouring Light&lt;/a&gt; and applying those enchants to your gear.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Complete the required objectives using the knowledge you have gained so gar.&lt;/p&gt;&lt;p&gt;You can see your voidance, devoidance by doing:&lt;/p&gt;&lt;p&gt;- Tap Character Sheet tab&lt;/p&gt;&lt;p&gt;- Open the Character Details Section&lt;/p&gt;&lt;p&gt;- Tap Additional Information orange button.&lt;/p&gt;&lt;p&gt;- Tap Voidance tab&lt;/p&gt;&lt;p&gt;Now you can see your resistance to such effects as well as your chance to do said action to the enemy.&lt;/p&gt;&lt;p&gt;The quest line in question will get you an item that raises these significantly, but you can enchant devouring light on your gear by going to the enchantment list here, and searching the filters for: &lt;a href="/information/enchanting?table[filters][types]=3" target="_blank"&gt;Skill/Res Reduction + Devouring Light&lt;/a&gt; and applying those enchants to your gear.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Disenchanter's Magnifying Glass</t>
-  </si>
-  <si>
-    <t>Dead King's Crown</t>
+    <t>child-of-gambling</t>
   </si>
 </sst>
 </file>
@@ -783,7 +705,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AS16"/>
+  <dimension ref="A1:AS12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -792,11 +714,11 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="3.428" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="31.707" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="32.992" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="1886.254" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="2248.451" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="2309.722" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="2172.898" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="2760.469" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="1827.268" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="2031.361" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="18.71" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="24.708" bestFit="true" customWidth="true" style="0"/>
@@ -813,8 +735,8 @@
     <col min="20" max="20" width="23.423" bestFit="true" customWidth="true" style="0"/>
     <col min="21" max="21" width="26.993" bestFit="true" customWidth="true" style="0"/>
     <col min="22" max="22" width="24.708" bestFit="true" customWidth="true" style="0"/>
-    <col min="23" max="23" width="26.993" bestFit="true" customWidth="true" style="0"/>
-    <col min="24" max="24" width="37.705" bestFit="true" customWidth="true" style="0"/>
+    <col min="23" max="23" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="24" max="24" width="26.993" bestFit="true" customWidth="true" style="0"/>
     <col min="25" max="25" width="28.136" bestFit="true" customWidth="true" style="0"/>
     <col min="26" max="26" width="16.425" bestFit="true" customWidth="true" style="0"/>
     <col min="27" max="27" width="22.28" bestFit="true" customWidth="true" style="0"/>
@@ -1173,7 +1095,7 @@
     </row>
     <row r="7" spans="1:45">
       <c r="A7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>78</v>
@@ -1191,101 +1113,92 @@
         <v>82</v>
       </c>
       <c r="G7">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="H7" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="I7">
-        <v>25</v>
-      </c>
-      <c r="T7" t="s">
-        <v>83</v>
-      </c>
-      <c r="U7">
+        <v>15</v>
+      </c>
+      <c r="J7" t="s">
+        <v>84</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="L7">
         <v>1</v>
       </c>
-      <c r="V7" t="s">
-        <v>83</v>
+      <c r="M7">
+        <v>10</v>
       </c>
       <c r="X7" t="s">
-        <v>84</v>
+        <v>85</v>
+      </c>
+      <c r="AA7">
+        <v>500</v>
       </c>
       <c r="AH7">
-        <v>150</v>
+        <v>210</v>
+      </c>
+      <c r="AP7">
+        <v>500</v>
+      </c>
+      <c r="AQ7">
+        <v>0</v>
       </c>
       <c r="AR7">
         <v>100000</v>
       </c>
       <c r="AS7">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:45">
       <c r="A8">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F8" t="s">
-        <v>89</v>
-      </c>
-      <c r="G8">
-        <v>120</v>
-      </c>
-      <c r="H8" t="s">
         <v>90</v>
       </c>
-      <c r="I8">
-        <v>15</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="T8" t="s">
         <v>91</v>
       </c>
-      <c r="K8">
-        <v>5</v>
-      </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
-      <c r="M8">
-        <v>10</v>
-      </c>
-      <c r="X8" t="s">
+      <c r="U8">
+        <v>3</v>
+      </c>
+      <c r="W8" t="s">
         <v>92</v>
       </c>
-      <c r="AA8">
-        <v>500</v>
-      </c>
-      <c r="AH8">
-        <v>210</v>
-      </c>
       <c r="AP8">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="AQ8">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AR8">
         <v>100000</v>
       </c>
       <c r="AS8">
-        <v>75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:45">
       <c r="A9">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
         <v>93</v>
@@ -1300,31 +1213,25 @@
         <v>96</v>
       </c>
       <c r="F9" t="s">
-        <v>97</v>
-      </c>
-      <c r="G9">
-        <v>150</v>
+        <v>96</v>
       </c>
       <c r="H9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I9">
         <v>50</v>
       </c>
-      <c r="V9" t="s">
-        <v>98</v>
-      </c>
-      <c r="X9" t="s">
-        <v>99</v>
-      </c>
-      <c r="Y9" t="s">
+      <c r="W9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AP9">
+        <v>2500</v>
+      </c>
+      <c r="AQ9">
         <v>100</v>
       </c>
-      <c r="AH9">
-        <v>350</v>
-      </c>
       <c r="AR9">
-        <v>250000</v>
+        <v>100000</v>
       </c>
       <c r="AS9">
         <v>100</v>
@@ -1332,49 +1239,43 @@
     </row>
     <row r="10" spans="1:45">
       <c r="A10">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" t="s">
         <v>101</v>
       </c>
-      <c r="C10" t="s">
+      <c r="F10" t="s">
         <v>102</v>
       </c>
-      <c r="D10" t="s">
+      <c r="G10">
+        <v>300</v>
+      </c>
+      <c r="T10" t="s">
         <v>103</v>
       </c>
-      <c r="E10" t="s">
+      <c r="U10">
+        <v>2</v>
+      </c>
+      <c r="V10" t="s">
+        <v>103</v>
+      </c>
+      <c r="X10" t="s">
         <v>104</v>
       </c>
-      <c r="F10" t="s">
-        <v>104</v>
-      </c>
-      <c r="G10">
-        <v>200</v>
-      </c>
-      <c r="L10">
-        <v>13</v>
-      </c>
-      <c r="M10">
-        <v>20</v>
-      </c>
-      <c r="T10" t="s">
-        <v>98</v>
-      </c>
-      <c r="U10">
-        <v>1</v>
-      </c>
-      <c r="AH10">
-        <v>380</v>
-      </c>
       <c r="AP10">
-        <v>10000</v>
-      </c>
-      <c r="AQ10">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="AR10">
-        <v>100000</v>
+        <v>500000</v>
       </c>
       <c r="AS10">
         <v>100</v>
@@ -1382,7 +1283,7 @@
     </row>
     <row r="11" spans="1:45">
       <c r="A11">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>105</v>
@@ -1399,32 +1300,11 @@
       <c r="F11" t="s">
         <v>109</v>
       </c>
-      <c r="G11">
-        <v>350</v>
-      </c>
-      <c r="H11" t="s">
-        <v>67</v>
-      </c>
-      <c r="I11">
-        <v>100</v>
-      </c>
-      <c r="J11" t="s">
-        <v>90</v>
-      </c>
-      <c r="K11">
-        <v>100</v>
-      </c>
       <c r="R11">
         <v>1</v>
       </c>
       <c r="S11">
-        <v>5</v>
-      </c>
-      <c r="AH11">
-        <v>500</v>
-      </c>
-      <c r="AP11">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="AR11">
         <v>500000</v>
@@ -1435,7 +1315,7 @@
     </row>
     <row r="12" spans="1:45">
       <c r="A12">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
         <v>110</v>
@@ -1452,15 +1332,6 @@
       <c r="F12" t="s">
         <v>114</v>
       </c>
-      <c r="G12">
-        <v>400</v>
-      </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
-      <c r="M12">
-        <v>150</v>
-      </c>
       <c r="N12" t="s">
         <v>115</v>
       </c>
@@ -1468,197 +1339,21 @@
         <v>116</v>
       </c>
       <c r="P12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q12">
-        <v>2</v>
-      </c>
-      <c r="W12" t="s">
-        <v>117</v>
-      </c>
-      <c r="AH12">
-        <v>750</v>
+        <v>1</v>
       </c>
       <c r="AP12">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="AQ12">
         <v>1000</v>
       </c>
       <c r="AR12">
-        <v>5000000</v>
+        <v>1000000</v>
       </c>
       <c r="AS12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:45">
-      <c r="A13">
-        <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>118</v>
-      </c>
-      <c r="C13" t="s">
-        <v>119</v>
-      </c>
-      <c r="D13" t="s">
-        <v>120</v>
-      </c>
-      <c r="E13" t="s">
-        <v>121</v>
-      </c>
-      <c r="F13" t="s">
-        <v>122</v>
-      </c>
-      <c r="G13">
-        <v>500</v>
-      </c>
-      <c r="H13" t="s">
-        <v>123</v>
-      </c>
-      <c r="I13">
-        <v>5</v>
-      </c>
-      <c r="J13" t="s">
-        <v>124</v>
-      </c>
-      <c r="K13">
-        <v>10</v>
-      </c>
-      <c r="L13">
-        <v>13</v>
-      </c>
-      <c r="M13">
-        <v>30</v>
-      </c>
-      <c r="AP13">
-        <v>10000</v>
-      </c>
-      <c r="AQ13">
-        <v>5000</v>
-      </c>
-      <c r="AR13">
-        <v>10000000</v>
-      </c>
-      <c r="AS13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:45">
-      <c r="A14">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>125</v>
-      </c>
-      <c r="C14" t="s">
-        <v>126</v>
-      </c>
-      <c r="D14" t="s">
-        <v>127</v>
-      </c>
-      <c r="E14" t="s">
-        <v>128</v>
-      </c>
-      <c r="F14" t="s">
-        <v>128</v>
-      </c>
-      <c r="T14" t="s">
-        <v>129</v>
-      </c>
-      <c r="U14">
-        <v>2</v>
-      </c>
-      <c r="W14" t="s">
-        <v>130</v>
-      </c>
-      <c r="AP14">
-        <v>1000</v>
-      </c>
-      <c r="AQ14">
-        <v>10</v>
-      </c>
-      <c r="AR14">
-        <v>10000000</v>
-      </c>
-      <c r="AS14">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:45">
-      <c r="A15">
-        <v>19</v>
-      </c>
-      <c r="B15" t="s">
-        <v>131</v>
-      </c>
-      <c r="C15" t="s">
-        <v>132</v>
-      </c>
-      <c r="D15" t="s">
-        <v>133</v>
-      </c>
-      <c r="E15" t="s">
-        <v>128</v>
-      </c>
-      <c r="F15" t="s">
-        <v>128</v>
-      </c>
-      <c r="X15" t="s">
-        <v>134</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>135</v>
-      </c>
-      <c r="AP15">
-        <v>1000</v>
-      </c>
-      <c r="AQ15">
-        <v>10</v>
-      </c>
-      <c r="AR15">
-        <v>5000000</v>
-      </c>
-      <c r="AS15">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:45">
-      <c r="A16">
-        <v>20</v>
-      </c>
-      <c r="B16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C16" t="s">
-        <v>137</v>
-      </c>
-      <c r="D16" t="s">
-        <v>138</v>
-      </c>
-      <c r="E16" t="s">
-        <v>139</v>
-      </c>
-      <c r="F16" t="s">
-        <v>140</v>
-      </c>
-      <c r="G16">
-        <v>550</v>
-      </c>
-      <c r="X16" t="s">
-        <v>141</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>142</v>
-      </c>
-      <c r="AP16">
-        <v>5000</v>
-      </c>
-      <c r="AR16">
-        <v>10000000</v>
-      </c>
-      <c r="AS16">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated quests and guide quests
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="140">
   <si>
     <t>id</t>
   </si>
@@ -302,7 +302,7 @@
     <t>This little helpless goblin does not seem dangerous at all. Curious if anything else. Full of surprises and strange little gifts for the errands you do for him.&lt;br /&gt; &lt;br /&gt; You have arrived back at the town after your little adventure and you find The Guide sitting at the INN waiting for you.&lt;br /&gt; &lt;br /&gt; “I see you have been out adventuring with our helpless little friend.”&lt;br /&gt; &lt;br /&gt; You tell him of your adventures, your crafting, enchanting, fighting, errands you did for the goblin.&lt;br /&gt; &lt;br /&gt; “Fantastic. The world is full of interesting people for you to meet. Some of them have more errands, their own stories and adventures for you to go on in exchange for knowledge and various fantastic rewards.”&lt;br /&gt; &lt;br /&gt; He pauses and you two sit in silence for a moment enjoying a drink and a spread before you.&lt;br /&gt; &lt;br /&gt; “You should work with that goblin for something special, A Book of Guidance.”&lt;br /&gt; &lt;br /&gt; You ask what this item is for.&lt;br /&gt; &lt;br /&gt; “You, to help you hit better child.”</t>
   </si>
   <si>
-    <t>&lt;p&gt;We know how to do quests now, so lets continue doing quests to get an item that will help you – especially if you are crafting items with Accuracy enchantments attached – level Accuracy rather quickly.&lt;/p&gt;&lt;p&gt;This right here shows you how two features of the game can work together to progress your character: Quest items that you get from doing quests that increase some aspect about your character. Enchanting, Crafting, Quests and Skills&lt;/p&gt;&lt;p&gt;As we progress we will open more systems that also work together with existing systems you have learned to continue to progress your character.&lt;/p&gt;</t>
+    <t>&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;: &lt;em&gt;This quest might take a moment, longer then two hours, because you need the gold dust which you get from enchanting and then disenchanting.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;We know how to do quests now, so lets continue doing quests to get an item that will help you – especially if you are crafting items with Accuracy enchantments attached – level Accuracy rather quickly.&lt;/p&gt;&lt;p&gt;This right here shows you how two features of the game can work together to progress your character: Quest items that you get from doing quests that increase some aspect about your character. Enchanting, Crafting, Quests and Skills&lt;/p&gt;&lt;p&gt;As we progress we will open more systems that also work together with existing systems you have learned to continue to progress your character.&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;We already know how to complete a quest, and we know how to level our skills. So lets use that in conjunction with crafting and enchanting to get gold dust to complete the required objectives.&lt;/p&gt;</t>
@@ -317,7 +317,7 @@
     <t>Your ability to kill creatures is getting better and your able to find and hunt down stronger foes.&lt;br /&gt; &lt;br /&gt; Exhausted and tired you arrive back at the INN. It’s completely empty. Not a soul, not a single sound but the creaking of the old wood in the wind that blows outside.&lt;br /&gt; &lt;br /&gt; You call out but no one answers.&lt;br /&gt; &lt;br /&gt; A shadow moves across the wall and you move towards where the shadow went.&lt;br /&gt; &lt;br /&gt; No one there.&lt;br /&gt; &lt;br /&gt; You call out again, readying your weapon.&lt;br /&gt; &lt;br /&gt; Nothing.&lt;br /&gt; &lt;br /&gt; You enter into a back room, an office of sorts. Blood covers the wall. You back out and head back to the main room.&lt;br /&gt; &lt;br /&gt; Bodies. Bodies every where, torn, broken, damage and ripped apart. The gore, the fear, the pain the eyes of the dead.&lt;br /&gt; &lt;br /&gt; What the hell happened?</t>
   </si>
   <si>
-    <t>&lt;p&gt;It’s time we get off the &lt;a href="/information/planes" target="_blank"&gt;plane&lt;/a&gt;: Surface. To do this we just have to kill a single creature: Labyrinth Fiend until the Key of Labyrinth drops.&lt;/p&gt;&lt;p&gt;This will allow us to use a new feature called: &lt;a href="/information/traverse" target="_blank"&gt;Traverse&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;Traverse allows us to move to another plane of existence where we can fight monsters and interact with new features. For example, when we eventually get to Hell, those &lt;a href="/information/random-enchants" target="_blank"&gt;Green Uniques&lt;/a&gt; you have been getting – there is an NPC that allows you to buy better ones and even re-roll them and move the enchantments to other items. How fun!&lt;/p&gt;&lt;p&gt;Some Planes make you weaker and the creatures much, much stronger and also give you bonuses for killing creatures of that plane. As you go past Dungeons plane you will find your gear needs to be better with a set of enchantments that play to your classes strengths as well as the levels.&lt;/p&gt;</t>
+    <t>&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;: &lt;em&gt;This quest can take two plus hours to complete. I recommend exploration while crafting and enchanting.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;It’s time we get off the &lt;a href="/information/planes" target="_blank"&gt;plane&lt;/a&gt;: Surface. To do this we just have to kill a single creature: Labyrinth Fiend until the Key of Labyrinth drops.&lt;/p&gt;&lt;p&gt;This will allow us to use a new feature called: &lt;a href="/information/traverse" target="_blank"&gt;Traverse&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;Traverse allows us to move to another plane of existence where we can fight monsters and interact with new features. For example, when we eventually get to Hell, those &lt;a href="/information/random-enchants" target="_blank"&gt;Green Uniques&lt;/a&gt; you have been getting – there is an NPC that allows you to buy better ones and even re-roll them and move the enchantments to other items. How fun!&lt;/p&gt;&lt;p&gt;Some Planes make you weaker and the creatures much, much stronger and also give you bonuses for killing creatures of that plane. As you go past Dungeons plane you will find your gear needs to be better with a set of enchantments that play to your classes strengths as well as the levels.&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Kill Labyrinth fiend until the Key of Labyrinth drops.&lt;/p&gt;&lt;p&gt;Next:&lt;/p&gt;&lt;p&gt;- Click Traverse under the map&lt;/p&gt;&lt;p&gt;- Select labyrinth from the drop down&lt;/p&gt;&lt;p&gt;- Click Traverse&lt;/p&gt;&lt;p&gt;- Welcome to Labyrinth!plane&lt;/p&gt;</t>
@@ -365,7 +365,76 @@
     <t>child-of-gold-dust</t>
   </si>
   <si>
-    <t>child-of-gambling</t>
+    <t>child-of-shards</t>
+  </si>
+  <si>
+    <t>Farmers in the fields</t>
+  </si>
+  <si>
+    <t>You spent your coin, weather you won or lost is up for debate, but you were able to get your mind off the horrors of the INN.&lt;br /&gt; &lt;br /&gt; You wonder for days passing through farm fields, stopping to speak to a few farmers who tell you of their lord, their lady, their king, their queen.&lt;br /&gt; &lt;br /&gt; Seems like there is a lot of a kingdoms around with various lords and ladies and since you haven’t seen The Guide since he last appear coughing up blood and looking half dead, you decide to investigate this kingdom concept.&lt;br /&gt; &lt;br /&gt; Can you just settle any where?&lt;br /&gt; &lt;br /&gt; “Yup, that’s how it works.” Stats a farmer before he walks off back to his fields, leaving you to stand alone in the warm fall day.&lt;br /&gt; &lt;br /&gt; Winter is coming after all, the nights are getting colder and with every one murdered by something, a mysterious shadow perhaps, you need a new home.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Lets settle a &lt;a href="/information/kingdoms" target="_blank"&gt;kingdom&lt;/a&gt;. Kingdoms become important later on in the game and require the player to be vigilant because after 7 days from settling your first kingdom, it is open to everyone to attack and take.&lt;/p&gt;&lt;p&gt;One of the systems that kingdoms impact is a later system called &lt;a href="/information/gems" target="_blank"&gt;Atonement&lt;/a&gt;, which includes adding sockets and gems to your gear to build up resistance and elemental damage for end game &lt;a href="/information/raids" target="_blank"&gt;Raids&lt;/a&gt; and associated critters as well as &lt;a href="/information/player-vs-player" target="_blank"&gt;PVP&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;To socket gems on to items you will need something called Gold Bars, which you can only get by owning one or more kingdoms.&lt;/p&gt;&lt;p&gt;For now, lets focus on settling a kingdom and building up a bit of defense, you can do this with gold or with kingdom resources which slowly accumulate once per hour.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Caution&lt;/strong&gt;: There is an option in your kingdom to allow you to buy population. Your kingdom, based on the farm level, has a maximum population. You can buy population beyond this. But, should the hour be up and you have not brought that population down to your current max, an NPC: The Old Man, will stomp around in chat. He will first take payment from your Gold Bars. Since you won’t have any he next takes what he can from your treasury, if there's not enough or no gold he will take the rest from your personal gold. If you have no gold or not enough he will demolish your kingdom.&lt;/p&gt;&lt;p&gt;&lt;a href="/information/npc-kingdoms" target="_blank"&gt;&lt;strong&gt;Yellow Kingdoms&lt;/strong&gt;&lt;/a&gt;: You might see Yellow Kingdoms on the map, these are abandoned or neglected kingdoms. Kingdoms will loose morale if you do not visit them enough, by actually going to them once a month at least. This is called walking the kingdoms. Failure to do this once per 30 days can see your kingdom become abandoned, these can be bought by other players from The Old Man.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Red Kingdoms:&lt;/strong&gt; These are enemy kingdoms. Simple as that. You can attack them and later on, when you have settlers, take kingdoms. Some Alchemy items can be dropped on them to do wild amounts of damage, making the process of taking them with settlers much easier.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;- Find a spot on the map you can move to, could be Surface or Labyrinth since you also have access to Labyrinth. The only plane you cannot settle on is Purgatory.&lt;/p&gt;&lt;p&gt;- This location must be 1 space away from any location or port – there must be one space between your kingdom and a port for example, in all directions.&lt;/p&gt;&lt;p&gt;- Under the map click Settle Kingdom.&lt;/p&gt;&lt;p&gt;- Name your kingdom.&lt;/p&gt;&lt;p&gt;- Click settle.&lt;/p&gt;&lt;p&gt;- Boom done!&lt;/p&gt;&lt;p&gt;You could also look to see if there is a yellow kingdom around. If so click it and purchase it, it will be free. You can rename it from the kingdom section.&lt;/p&gt;&lt;p&gt;Your very first, even if you loose all your kingdoms, kingdom is always fee, every kingdom after that, including settling, is 10,000 Gold x Kingdom amount. Ie, 6 kingdoms: 60K god your 7&lt;sup&gt;th&lt;/sup&gt; kingdom.&lt;/p&gt;&lt;p&gt;- Click the kingdoms tab.&lt;/p&gt;&lt;p&gt;- Click your kingdom name.&lt;/p&gt;&lt;p&gt;Here you will see all the info about this kingdom, including buildings and their levels as well as other actions.&lt;/p&gt;&lt;p&gt;You can click on buildings and the unit names to then upgrade or, if they have been damaged in someone attacking, repair them. You can do this with gold or resources.&lt;/p&gt;&lt;p&gt;The requirements wants a sum total of the levels of the your kingdom – this means total level of all your buildings. You could do one or multiple, I suggest the farm, walls and barracks but I’ll let you explore. Buildings and unit can take minutes or hours or even days to process.&lt;/p&gt;&lt;p&gt;The other requirement for units, is the same concept – the sum total of one or more sets of units.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;- Select Map Movement from the actions section&lt;/p&gt;&lt;p&gt;- Find a spot on the map you can move to, could be Surface or Labyrinth since you also have access to Labyrinth. The only plane you cannot settle on is Purgatory.&lt;/p&gt;&lt;p&gt;- This location must be 1 space away from any location or port – there must be one space between your kingdom and a port for example, in all directions.&lt;/p&gt;&lt;p&gt;- Under the map tap Settle Kingdom.&lt;/p&gt;&lt;p&gt;- Name your kingdom.&lt;/p&gt;&lt;p&gt;- tap settle.&lt;/p&gt;&lt;p&gt;- Boom done!&lt;/p&gt;&lt;p&gt;You could also look to see if there is a yellow kingdom around. If so teleport to it by selecting a NPC Kingdom from the NPC Kingdoms Drop down. Purchase it. It will be free. You can rename it from the kingdom section.&lt;/p&gt;&lt;p&gt;Your very first, even if you loose all your kingdoms, kingdom is always fee, every kingdom after that, including settling, is 10,000 Gold x Kingdom amount. Ie, 6 kingdoms: 60K god your 7&lt;sup&gt;th&lt;/sup&gt; kingdom.&lt;/p&gt;&lt;p&gt;- Tap the kingdoms tab.&lt;/p&gt;&lt;p&gt;- Tap your kingdom name.&lt;/p&gt;&lt;p&gt;Here you will see all the info about this kingdom, including buildings and their levels as well as other actions.&lt;/p&gt;&lt;p&gt;You can tap on buildings and the unit names to then upgrade or, if they have been damaged in someone attacking, repair them. You can do this with gold or resources.&lt;/p&gt;&lt;p&gt;The requirements wants a sum total of the levels of the your kingdom – this means total level of all your buildings. You could do one or multiple, I suggest the farm, walls and barracks but I’ll let you explore. Buildings and unit can take minutes or hours or even days to process.&lt;/p&gt;&lt;p&gt;The other requirement for units, is the same concept – the sum total of one or more sets of units.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Blasting shadows</t>
+  </si>
+  <si>
+    <t>It has been months, the winter has come and gone and the fields are starting to grow bountiful food. You start the plans for the next leg of your building adventure.&lt;br /&gt; &lt;br /&gt; The back of your mind is still haunted by the visions of death, most of them have faded into the distance, into the shadows.&lt;br /&gt; &lt;br /&gt; You look up from your papers and plans and see a shadow cross the dimly lit room. You stand and ready your magics, you illuminate the room and the light blasts through the room and out the windows into the darkness of the night.&lt;br /&gt; &lt;br /&gt; The people below look up and see the room you are in brightly lit up, such that they must shield their eyes.&lt;br /&gt; &lt;br /&gt; The shadow is gone, but the fear still stands in the back of your mind.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;: &lt;em&gt;This quest will take two or more hours to complete. Utilize exploration to level your class ranks and mercenaries while you craft and then enchant and then – if it’s not better then what you have equiped – disenchant it.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Lets learn about &lt;a href="/information/kingdom-passive-skills" target="_blank"&gt;Kingdom Passives&lt;/a&gt;, these are a special set of skills that take real world hours to train a single level which increases as the level of the passive increases.&lt;/p&gt;&lt;p&gt;Each child skill will require it’s parent to be at a specific level to unlock the ability to level it, for this reason it’s advised players go after the Passive they want, in our case – we are going to head for Goblin Coin Bank and while we do that were going to work on our crafting and enchanting.&lt;/p&gt;&lt;p&gt;Kingdom Passives help you gain bonuses towards all kingdoms as well as unlock new buildings and units. For example the thing we want: Goblin Coin Bank, will allow you to construct and level this building to take 2 billion gold and store it in your kingdom as 1 gold bar. A single kingdom have 1000 of these bars. Gold bars are then used in things like Sockets and the &lt;a href="/information/goblin-shop" target="_blank"&gt;Goblin Shop&lt;/a&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;- Click Character Sheet tab&lt;/p&gt;&lt;p&gt;- Under skills section is a tab called Kingdom Passives&lt;/p&gt;&lt;p&gt;- Click the top Skill and begin training it to level 1.&lt;/p&gt;&lt;p&gt;These passives will level while you are logged out.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;- Tap Character Sheet tab&lt;/p&gt;&lt;p&gt;- Select Skill management from the drop down&lt;/p&gt;&lt;p&gt;- Under skills section is a tab called Kingdom Passives&lt;/p&gt;&lt;p&gt;- Tap the top Skill and begin training it to level 1.&lt;/p&gt;&lt;p&gt;These passives will level while you are logged out.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Ring Crafting</t>
+  </si>
+  <si>
+    <t>Kingdom Management</t>
+  </si>
+  <si>
+    <t>Sliding into despair</t>
+  </si>
+  <si>
+    <t>You have heard reports of the wars that have been raging between the various kingdoms in your area. You are worried that your kingdom could be next and you hurry to build the defenses around your kingdom fearing that it’s only a matter of time, slowly drifting into the shadows of delusion while the shadow haunts you.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We are going to continue training out kingdom passives. This might take a couple days. The reason is, I want you to train the skill: Building Management to level 2. To do that you need to train the parent skill to level 4. This alone is another 4 hours, on top of 4 hours to get the required skill to level 2.&lt;/p&gt;&lt;p&gt;In the mean time lets focus on crafting and enchanting.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Repeat the steps of the previous quest. The required passive will become unlocked when your parent skill is level 4, so come back often to check the status of the passive.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Building Management</t>
+  </si>
+  <si>
+    <t>Goblins and Armies</t>
+  </si>
+  <si>
+    <t>Kingdoms have fallen, the death of the lords around you, the blood of their soldiers soak the lands. You are sitting in your throne room, in the darkness, in the shadows of your mind. Haunted by death, haunted by the people you rule, the people you lead, the people you protect.&lt;br /&gt; &lt;br /&gt; The days have gone by, the plans have the been seeded and they flower into your ambitious outcomes.&lt;br /&gt; &lt;br /&gt; You have heard of the goblins who run special banks that allow the super rich to store their vast wealth and exchange them for goods and services at special shops. Now might be the time to distract our self from the death and carnage and look into this concept.&lt;br /&gt; &lt;br /&gt; Wonder if The Helpless Goblin might have anything of use.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; &lt;em&gt;This quest will take up to 4 or more hours to complete&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Now lets go and get out Goblin Coin Bank to level 1 and this will unlock the new Goblin Bank Building that you can upgrade to level 5.&lt;/p&gt;&lt;p&gt;Once the building is level 5 anew action button will appear where you can manage the gold bars in your kingdom.&lt;/p&gt;&lt;p&gt;One thing to note: Kingdom Defense&lt;/p&gt;&lt;p&gt;Your kingdom defense will protect you, along with your units, against incoming attacks as well as alchemical items that get dropped on your kingdom.&lt;/p&gt;&lt;p&gt;This defense is made up of the level of your wall, how much treasury you have, how many gold bars you have and other factors. The more gold in the treasury and the more bars in the bank, the higher the defense, the wall will also help with defense as you level it.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;At this point we are just repeating the steps of the past and leveling some other aspects of our character.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Leading Armies</t>
+  </si>
+  <si>
+    <t>Goblin Coin Bank</t>
   </si>
 </sst>
 </file>
@@ -705,7 +774,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AS12"/>
+  <dimension ref="A1:AS16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -717,7 +786,7 @@
     <col min="2" max="2" width="32.992" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="1886.254" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="2760.469" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="1827.268" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="1851.976" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="2031.361" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="18.71" bestFit="true" customWidth="true" style="0"/>
@@ -1339,10 +1408,10 @@
         <v>116</v>
       </c>
       <c r="P12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AP12">
         <v>1000</v>
@@ -1354,6 +1423,188 @@
         <v>1000000</v>
       </c>
       <c r="AS12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:45">
+      <c r="A13">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" t="s">
+        <v>120</v>
+      </c>
+      <c r="F13" t="s">
+        <v>121</v>
+      </c>
+      <c r="AC13">
+        <v>1</v>
+      </c>
+      <c r="AD13">
+        <v>30</v>
+      </c>
+      <c r="AE13">
+        <v>100</v>
+      </c>
+      <c r="AR13">
+        <v>1000000</v>
+      </c>
+      <c r="AS13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:45">
+      <c r="A14">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" t="s">
+        <v>124</v>
+      </c>
+      <c r="E14" t="s">
+        <v>125</v>
+      </c>
+      <c r="F14" t="s">
+        <v>126</v>
+      </c>
+      <c r="H14" t="s">
+        <v>83</v>
+      </c>
+      <c r="I14">
+        <v>25</v>
+      </c>
+      <c r="J14" t="s">
+        <v>127</v>
+      </c>
+      <c r="K14">
+        <v>5</v>
+      </c>
+      <c r="AD14">
+        <v>60</v>
+      </c>
+      <c r="AE14">
+        <v>500</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>128</v>
+      </c>
+      <c r="AG14">
+        <v>1</v>
+      </c>
+      <c r="AR14">
+        <v>2000000</v>
+      </c>
+      <c r="AS14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:45">
+      <c r="A15">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" t="s">
+        <v>131</v>
+      </c>
+      <c r="E15" t="s">
+        <v>132</v>
+      </c>
+      <c r="F15" t="s">
+        <v>132</v>
+      </c>
+      <c r="AD15">
+        <v>75</v>
+      </c>
+      <c r="AE15">
+        <v>2000</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>133</v>
+      </c>
+      <c r="AG15">
+        <v>2</v>
+      </c>
+      <c r="AR15">
+        <v>2000000</v>
+      </c>
+      <c r="AS15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:45">
+      <c r="A16">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16" t="s">
+        <v>135</v>
+      </c>
+      <c r="D16" t="s">
+        <v>136</v>
+      </c>
+      <c r="E16" t="s">
+        <v>137</v>
+      </c>
+      <c r="F16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H16" t="s">
+        <v>68</v>
+      </c>
+      <c r="I16">
+        <v>25</v>
+      </c>
+      <c r="J16" t="s">
+        <v>83</v>
+      </c>
+      <c r="K16">
+        <v>50</v>
+      </c>
+      <c r="R16">
+        <v>2</v>
+      </c>
+      <c r="S16">
+        <v>10</v>
+      </c>
+      <c r="W16" t="s">
+        <v>138</v>
+      </c>
+      <c r="AD16">
+        <v>100</v>
+      </c>
+      <c r="AE16">
+        <v>3000</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>139</v>
+      </c>
+      <c r="AG16">
+        <v>1</v>
+      </c>
+      <c r="AR16">
+        <v>5000000</v>
+      </c>
+      <c r="AS16">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated guide-quests and fixed armour crafting list to update properly.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -1226,7 +1226,7 @@
     </row>
     <row r="8" spans="1:45">
       <c r="A8">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>86</v>
@@ -1267,7 +1267,7 @@
     </row>
     <row r="9" spans="1:45">
       <c r="A9">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>93</v>
@@ -1308,7 +1308,7 @@
     </row>
     <row r="10" spans="1:45">
       <c r="A10">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>98</v>
@@ -1352,7 +1352,7 @@
     </row>
     <row r="11" spans="1:45">
       <c r="A11">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
         <v>105</v>
@@ -1384,7 +1384,7 @@
     </row>
     <row r="12" spans="1:45">
       <c r="A12">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
         <v>110</v>
@@ -1428,7 +1428,7 @@
     </row>
     <row r="13" spans="1:45">
       <c r="A13">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
         <v>117</v>
@@ -1463,7 +1463,7 @@
     </row>
     <row r="14" spans="1:45">
       <c r="A14">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
         <v>122</v>
@@ -1513,7 +1513,7 @@
     </row>
     <row r="15" spans="1:45">
       <c r="A15">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
         <v>129</v>
@@ -1551,7 +1551,7 @@
     </row>
     <row r="16" spans="1:45">
       <c r="A16">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
         <v>134</v>

</xml_diff>

<commit_message>
Added a way for the total kills to be tracked. Added additional guide quest requirements.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="216">
   <si>
     <t>id</t>
   </si>
@@ -161,6 +161,27 @@
     <t>xp_reward</t>
   </si>
   <si>
+    <t>parent_id</t>
+  </si>
+  <si>
+    <t>unlock_at_level</t>
+  </si>
+  <si>
+    <t>only_during_event</t>
+  </si>
+  <si>
+    <t>be_on_game_map</t>
+  </si>
+  <si>
+    <t>require_event_goal_participation</t>
+  </si>
+  <si>
+    <t>required_holy_stacks</t>
+  </si>
+  <si>
+    <t>required_attached_gems</t>
+  </si>
+  <si>
     <t>Welcome to Tlessa</t>
   </si>
   <si>
@@ -549,6 +570,99 @@
   </si>
   <si>
     <t>&lt;p&gt;Super simple, but time consuming:&lt;/p&gt;&lt;p&gt;- Level the Goblin Bank in one of your kingdoms to the desired level, doesn’t matter which kingdom.&lt;/p&gt;&lt;p&gt;- Train your class Skill, this will be a skill under training skills that is orange and has an icon beside it.&lt;/p&gt;&lt;p&gt;- Your class skill is responsible for raising specific attributes about your character such as damage, armour and healing. Your class skill can also raise something called Class Bonus, each class a specific special attack that fires off based on your class bonus which is based on your class skill level. Each class in the game has it’s own class skill, if you switch classes, you have to level it’s skill from scratch if it’s a new class you have not previous leveled.&lt;/p&gt;&lt;p&gt;- Setup exploration in Gold Mines in Shadow Planes&lt;/p&gt;&lt;p&gt;- Craft Alchemy until the desired level.&lt;/p&gt;&lt;p&gt;- Once you have a Goblin Bank at the desired level, use the Goblin Bank Action in the kingdom you leveled the Goblin bank in, to then create the required amount of gold bars.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Winter has come to Tlessa!</t>
+  </si>
+  <si>
+    <t>“Child!” Comes a call and a hail.&lt;br /&gt; &lt;br /&gt; It’s The Guide as he walks down the trail to greet you. “I know you have been busy and probably are busy with some errand or task or some such, but I have something I wanted to show you!”&lt;br /&gt; &lt;br /&gt; You ask him what it is and he smiles: “Something magical! Winter has finally come to Tlessa!”&lt;br /&gt; &lt;br /&gt; Winter has come?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;That’s right! Winter has come and with it has come a new map that is only available during The Winter Event which is currently running!&lt;/p&gt;&lt;p&gt;I wanted to take a moment to get you situated with the new event before returning you to your regular scheduled programming!&lt;/p&gt;&lt;p&gt;With the winter event comes a new set of story based quests, slight harder creatures and even harder creatures for those in more later stages of the game. Whats really fun down here is that players can work together to earn Top end gear! Doesn’t matter your level.&lt;/p&gt;&lt;p&gt;You might be worried, Hey I am new and you are just handing out end game gear? Don’t worry my child, it’s all percent based, so even a +250% Strength item will do nothing for you 14 Strength, but as you level and that base 14 strength becomes 1000 strength – now the item is helping you. Item’s scale in Tlessa as you level.&lt;/p&gt;&lt;p&gt;These items that I reward players with for participating in whats called a global event – which only happens on the map you are going to – come with something called Uniques, which also limits players to only be able to equip one of the items that you are rewarded with, due to the rules: Players may only equip one Unique or Mythic (but not both).&lt;/p&gt;&lt;p&gt;Enough explanation! Lets get you on this map and participating!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Traversing is how we move from one plane to another. Special events such as this one will allow players regardless of level to traverse to to the map, while other maps might require quest items or quests to be completed.&lt;/p&gt;&lt;p&gt;- Click Traverse under the map&lt;/p&gt;&lt;p&gt;- Select The Ice Plane&lt;/p&gt;&lt;p&gt;- Click Traverse.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Traversing is how we move from one plane to another. Special events such as this one will allow players regardless of level to traverse to to the map, while other maps might require quest items or quests to be completed.&lt;/p&gt;&lt;p&gt;- Select Map Move from the Action Drop down&lt;/p&gt;&lt;p&gt;- Tap Traverse under the map&lt;/p&gt;&lt;p&gt;- Select The Ice Plane&lt;/p&gt;&lt;p&gt;- Tap Traverse.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>The Ice Plane</t>
+  </si>
+  <si>
+    <t>Working together in the chill</t>
+  </si>
+  <si>
+    <t>You shiver as you enter into a new world covered in Ice. The snow falls in a gentle breeze and the world is silent.&lt;br /&gt; &lt;br /&gt; “Child.” You jump in your spot as The Guide startles you. He pays no heed of this and continues.&lt;br /&gt; &lt;br /&gt; “Welcome to The Ice Plane! Down here you’ll notice that creatures are a hit stronger, but nothing you can’t handle. Just don’t be so hasty to take on the strongest critter, you might also find what you hunted on Surface might be a bit stronger down here!”&lt;br /&gt; &lt;br /&gt; You look out at the barren, frozen wind swept waste land covered in ice and wonder what could be out there. What adventures await you?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Now that we made it to The Ice Plane – lets start killing things. You’ll notice on your map (for desktop) there is a new Event Goal tab. For Mobile, you can see this by opening the Map Movement fro the main Action Drop down.&lt;/p&gt;&lt;p&gt;Here you will see an over all creature kill which then broken down into phases that increase by 1,000.&lt;/p&gt;&lt;p&gt;By working together either using exploration or manual fighting players can increase the bars and get rewarded for completing each phase.&lt;/p&gt;&lt;p&gt;To be rewarded you will see a “Amount of kills required to gain phase reward”, this is based on the average number of players on the map participating and their total kill count versus what you need to kill in order to gain a reward. Essentially its the average.&lt;/p&gt;&lt;p&gt;Below this you will see your total kills. This amount will reset to 0 once all phases are complete and the global Event Goal resets.&lt;/p&gt;&lt;p&gt;Lets help others out and get a reward shall we?!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This quest might get you a phase reward and might not. It depends when you do it and how far the main progress bar has moved. If the bar is close to being completed, the Event Goal will reset allowing players to participate again. The reset of this bar is hourly if it has been completely filled.&lt;/p&gt;&lt;p&gt;- Select any monster that you can kill in one hit.&lt;/p&gt;&lt;p&gt;- Participate by either using exploration or manual fighting&lt;/p&gt;&lt;p&gt;- Earn the required amount of points.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This quest might get you a phase reward and might not. It depends when you do it and how far the main progress bar has moved. If the bar is close to being completed, the Event Goal will reset allowing players to participate again. The reset of this bar is hourly if it has been completely filled.&lt;/p&gt;&lt;p&gt;- Select any monster that you can kill in one hit.&lt;/p&gt;&lt;p&gt;- Participate by either using exploration or manual fighting&lt;/p&gt;&lt;p&gt;- Earn the required amount of points.&lt;/p&gt;&lt;p&gt;- Select The Ice Plane&lt;/p&gt;&lt;p&gt;- Tap Traverse.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Who is The Ice Queen?</t>
+  </si>
+  <si>
+    <t>The last of the critters falls and the snow around you is covered I blood. You release a sight of relief as the silence falls over the land and the snow continues to fall slowly burying the bodies of the enemies before you.&lt;br /&gt; &lt;br /&gt; You stand for a moment in the silence of the falling snow before heading off towards a rumored wreck where it is said the Ice Queen has originated from.&lt;br /&gt; &lt;br /&gt; The Guide has not been seen in the last few days. He did mention something about a location called The Fathers tomb, but didn’t indicate which direction it was.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Let’s complete some of the story based &lt;a href="/information/quests" target="_blank"&gt;quests&lt;/a&gt; of this event and unlock other locations that progress the story of this map.&lt;/p&gt;&lt;p&gt;Story in Tlessa is done through quests. Quests also unlock features of the game and allow you to progress beyond level 1,000.&lt;/p&gt;&lt;p&gt;One this specific event map, which is only available during this event – once per year – there is a story that is told in a specific order which when complete tells an over arching story of who The Ice Queen in and why this plane is frozen.&lt;/p&gt;&lt;p&gt;Quests will always tell you how to complete them with specific instructions listed in the requirements section of the quest it’s self.&lt;/p&gt;&lt;p&gt;You can see the quests by tapping or clicking on the Quest tab. Red quests are ones that cannot be completed yet until the parent is completed. Blue quests can be completed provided you meet the requirements.&lt;/p&gt;&lt;p&gt;Green Quests are ones you have completed. All quests have a Before and After completion story which progresses the over all story of the game forward.&lt;/p&gt;&lt;p&gt;Lets participate in the event maps quests!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We will complete quests until we have completed the above required quest. To do this simply click on the quest tab, click the first quest – click the required tab and click on the help icons to see how to get each item.&lt;/p&gt;&lt;p&gt;In event maps, characters will just fight monsters – manually – at specific locations, known as special locations, to then gain the items at random chance.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Frozen in time</t>
+  </si>
+  <si>
+    <t>Skating though misery</t>
+  </si>
+  <si>
+    <t>The more you learn about The Queen and who she is to The Creator, the more curious you get. As you are about to set out exploring the world and helping those who have need of your skill set, you see The Guide approach the wreck.&lt;br /&gt; &lt;br /&gt; “She died here …” he states as he approaches and stands before you.&lt;br /&gt; &lt;br /&gt; You both stand in the silence of the falling snow as the winds pick up and the bitter chill of this frozen land sets in.&lt;br /&gt; &lt;br /&gt; “You should continue on. Reach the house of the fathers tomb. It will make more sense.”&lt;br /&gt; &lt;br /&gt; You stare at him for a moment and then look off into the distance.&lt;br /&gt; &lt;br /&gt; A grieving mother. A widow. You need to learn more.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;By now we know how to complete quests and participate in the events story and its event goals. So lets continue putting that together and push more of the story as well as participate more in the event goals.&lt;/p&gt;&lt;p&gt;The Quest you will complete will give you a &lt;a href="/information/quest-items" target="_blank"&gt;quest item&lt;/a&gt;, which is used automatically, to allow you to walk on Ice while down here.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Continue to kill creatures and participate in the quest line until the desired goals are reached.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>The Key</t>
+  </si>
+  <si>
+    <t>The Fathers Tomb</t>
+  </si>
+  <si>
+    <t>It has been weeks with out the presence of The Guide any where. You wonder if he might be at the Fathers Tomb.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We want to continue the story moving forward to gain access to the Fathers Tomb location as this is where a raid, depending on when you are doing this guide quest, will trigger and if layers want to participate they will need to complete quests to unlock this location.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Complete the required quest by following the story.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>The Whisper</t>
+  </si>
+  <si>
+    <t>Ruling The Ice Plane</t>
+  </si>
+  <si>
+    <t>“You are learning who she is.” The Guide Whispers as you two walk side by side in the falling snow, seeking out a warm shelter to hunker down in.&lt;br /&gt; &lt;br /&gt; You take a moment and reflect back on the adventure you have been on while on this plane of existence. The pain, the hurt, the loss – all of it.&lt;br /&gt; &lt;br /&gt; “She is frozen in her own her own grief, unable to let go and completely blinded by it. Such that it turns her wrathful.”&lt;br /&gt; &lt;br /&gt; You say nothing and give no indication to The Guide that you heard him, but by the long stare in your eyes, he knows what you know – you have to let go to move on.&lt;br /&gt; &lt;br /&gt; Moments go by and eventually a small ramshackle hut appears on the snowy horizon. You both head in that direction, longing to get out of the snow – maybe start a fire and get warm.&lt;br /&gt; &lt;br /&gt; “You could settle here.”&lt;br /&gt; &lt;br /&gt; You look over at him and then around at the night covered, snow covered frozen waste land.&lt;br /&gt; &lt;br /&gt; Why?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We are going to learn about kingdoms with this quest. You can, for this quest, settle any where you want – either here or on surface. Ideally though you would want to settle down here, for one specific reason: &lt;strong&gt;The Player with the most kingdoms will win a full set of Corrupted Ice gear at the end of event.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;You have a few pieces that are Unique by now – and as stated when we started this adventure, you could only equip one of those. With this prize, they come with no enchants allowing players to modify the gear to their liking.&lt;/p&gt;&lt;p&gt;For new players who have not maxed out &lt;a href="/information/enchanting" target="_blank"&gt;enchanting&lt;/a&gt;, it is suggested, if you win this gear, to not enchant it until you have maxed out enchanting as you could end up destroying the gear you worked so hard to get.&lt;/p&gt;&lt;p&gt;Kingdoms are a passive way of doing PVP, you can settle a kingdom any where you can move, with the exception of settling on locations or with in one space of a location in all directions.&lt;/p&gt;&lt;p&gt;You can also train &lt;a href="/information/kingdom-passive-skills" target="_blank"&gt;Kingdom Passives&lt;/a&gt; to unlock new buildings, units and passive buffs for your kingdoms.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt;&lt;em&gt; This quest wants you to have a kingdom at a specific level, this means level the buildings, one or more, to the required level such that all buildings combined meet the required level.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Complete the required quest to unlock the ability to settle a kingdom on this plane.&lt;/p&gt;&lt;p&gt;To settle a kingdom:&lt;/p&gt;&lt;p&gt;- Click Settle under the map, name the kingdom and click settle button.&lt;/p&gt;&lt;p&gt;- Click Kingdoms tab&lt;/p&gt;&lt;p&gt;- Click on your kingdom.&lt;/p&gt;&lt;p&gt;Here you can recruit units with gold or with resources, purchase additional population and manage your kingdom.&lt;/p&gt;&lt;p&gt;It should be noted that unlike Surface or other maps, due to the competitive nature of this Event specific map, kingdoms down here will not come with a seven day protection applied.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Passive&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;This quest also wants you to train a passive, these take real world hours to complete and provide bonuses your kingdoms across all planes.&lt;/p&gt;&lt;p&gt;To do this, head to your Character Sheet tab and under Skills, you will see a tab called Kingdom Passives. Here you will see a tree of skills, click the first one and click train. This will create a timer that will count down until the passive is trained to the next level.&lt;/p&gt;&lt;p&gt;You can logout and the timer will run behind the scenes.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; &lt;em&gt;This quest wants you to have a kingdom at a specific level, this means level the buildings, one or more, to the required level such that all buildings combined meet the required level.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Complete the required quest to unlock the ability to settle a kingdom on this plane.&lt;/p&gt;&lt;p&gt;To settle a kingdom:&lt;/p&gt;&lt;p&gt;- Select Map Movement From the Action drop down.&lt;/p&gt;&lt;p&gt;- Tap on settle after moving to a valid location.&lt;/p&gt;&lt;p&gt;- Name the kingdom and tap Settle.&lt;/p&gt;&lt;p&gt;- Tap the kingdom tab at the top to see your settled kingdoms.&lt;/p&gt;&lt;p&gt;- Here you can tap on a kingdom you want to manage and then either select from the drop down:&lt;/p&gt;&lt;p&gt;- Building Management or Unit Management to recruit Units and upgrade buildings.&lt;/p&gt;&lt;p&gt;- You can expand the Kingdom Details section to see additional information about your kingdom as well as additional actions such as purchasing population.&lt;/p&gt;&lt;p&gt;It should be noted that unlike Surface or other maps, due to the competitive nature of this Event specific map, kingdoms down here will not come with a seven day protection applied.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Passive&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;This quest also wants you to train a passive, these take real world hours to complete and provide bonuses your kingdoms across all planes.&lt;/p&gt;&lt;p&gt;To do this, tap the character sheet tab, select Skill Management from the drop down.&lt;/p&gt;&lt;p&gt;Here you will see a tab called Kingdom Passives.&lt;/p&gt;&lt;p&gt;Tapping the tab will show you a tree of skills, tap the first one and tap train. This will create a timer that will count down until the passive is trained to the next level.&lt;/p&gt;&lt;p&gt;You can logout and the timer will run behind the scenes.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -888,7 +1002,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AV22"/>
+  <dimension ref="A1:BF28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -897,7 +1011,7 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="3.428" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="32.992" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="35.277" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="1886.254" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="2760.469" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="1851.976" bestFit="true" customWidth="true" style="0"/>
@@ -944,9 +1058,19 @@
     <col min="46" max="46" width="16.425" bestFit="true" customWidth="true" style="0"/>
     <col min="47" max="47" width="13.997" bestFit="true" customWidth="true" style="0"/>
     <col min="48" max="48" width="11.711" bestFit="true" customWidth="true" style="0"/>
+    <col min="49" max="49" width="35.277" bestFit="true" customWidth="true" style="0"/>
+    <col min="50" max="50" width="9.10" bestFit="true" style="0"/>
+    <col min="51" max="51" width="18.71" bestFit="true" customWidth="true" style="0"/>
+    <col min="52" max="52" width="9.10" bestFit="true" style="0"/>
+    <col min="53" max="53" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="54" max="54" width="9.10" bestFit="true" style="0"/>
+    <col min="55" max="55" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="56" max="56" width="38.848" bestFit="true" customWidth="true" style="0"/>
+    <col min="57" max="57" width="24.708" bestFit="true" customWidth="true" style="0"/>
+    <col min="58" max="58" width="26.993" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48">
+    <row r="1" spans="1:58">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1091,25 +1215,46 @@
       <c r="AV1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:48">
+      <c r="AW1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:58">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -1121,24 +1266,24 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:48">
+    <row r="3" spans="1:58">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="G3">
         <v>10</v>
@@ -1150,36 +1295,36 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:48">
+    <row r="4" spans="1:58">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="G4">
         <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I4">
         <v>10</v>
       </c>
       <c r="J4" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="K4">
         <v>15</v>
@@ -1194,45 +1339,45 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:48">
+    <row r="5" spans="1:58">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="G5">
         <v>50</v>
       </c>
       <c r="H5" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="I5">
         <v>5</v>
       </c>
       <c r="J5" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="K5">
         <v>5</v>
       </c>
       <c r="X5" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="Y5" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="AU5">
         <v>1000</v>
@@ -1241,42 +1386,42 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:48">
+    <row r="6" spans="1:58">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="E6" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="F6" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="G6">
         <v>60</v>
       </c>
       <c r="H6" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="I6">
         <v>5</v>
       </c>
       <c r="J6" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="K6">
         <v>15</v>
       </c>
       <c r="X6" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="AO6">
         <v>125</v>
@@ -1288,36 +1433,36 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:48">
+    <row r="7" spans="1:58">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="E7" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="F7" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="G7">
         <v>120</v>
       </c>
       <c r="H7" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="I7">
         <v>15</v>
       </c>
       <c r="J7" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="K7">
         <v>5</v>
@@ -1329,7 +1474,7 @@
         <v>10</v>
       </c>
       <c r="X7" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="AA7">
         <v>500</v>
@@ -1350,33 +1495,33 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:48">
+    <row r="8" spans="1:58">
       <c r="A8">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D8" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="E8" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="F8" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="T8" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="U8">
         <v>3</v>
       </c>
       <c r="W8" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="AS8">
         <v>1000</v>
@@ -1391,33 +1536,33 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:48">
+    <row r="9" spans="1:58">
       <c r="A9">
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C9" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="E9" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="F9" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="H9" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I9">
         <v>50</v>
       </c>
       <c r="W9" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="AS9">
         <v>2500</v>
@@ -1432,39 +1577,39 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:48">
+    <row r="10" spans="1:58">
       <c r="A10">
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="D10" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="E10" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="F10" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="G10">
         <v>300</v>
       </c>
       <c r="T10" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="U10">
         <v>2</v>
       </c>
       <c r="V10" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="X10" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="AS10">
         <v>1000</v>
@@ -1476,24 +1621,24 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:48">
+    <row r="11" spans="1:58">
       <c r="A11">
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="C11" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D11" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E11" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="F11" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="R11">
         <v>1</v>
@@ -1508,30 +1653,30 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:48">
+    <row r="12" spans="1:58">
       <c r="A12">
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="C12" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="D12" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="E12" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="F12" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="N12" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="O12" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="P12">
         <v>2</v>
@@ -1552,24 +1697,24 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:48">
+    <row r="13" spans="1:58">
       <c r="A13">
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="C13" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="D13" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="E13" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="F13" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="AD13">
         <v>1</v>
@@ -1587,33 +1732,33 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:48">
+    <row r="14" spans="1:58">
       <c r="A14">
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="C14" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D14" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="E14" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="F14" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="H14" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="I14">
         <v>25</v>
       </c>
       <c r="J14" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="K14">
         <v>5</v>
@@ -1625,7 +1770,7 @@
         <v>500</v>
       </c>
       <c r="AI14" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="AJ14">
         <v>1</v>
@@ -1637,24 +1782,24 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:48">
+    <row r="15" spans="1:58">
       <c r="A15">
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="C15" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="D15" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="E15" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="F15" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="AE15">
         <v>75</v>
@@ -1663,7 +1808,7 @@
         <v>2000</v>
       </c>
       <c r="AI15" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="AJ15">
         <v>2</v>
@@ -1675,33 +1820,33 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:48">
+    <row r="16" spans="1:58">
       <c r="A16">
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="C16" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="D16" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="E16" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="F16" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="H16" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="I16">
         <v>25</v>
       </c>
       <c r="J16" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="K16">
         <v>50</v>
@@ -1713,7 +1858,7 @@
         <v>10</v>
       </c>
       <c r="W16" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="AE16">
         <v>100</v>
@@ -1722,7 +1867,7 @@
         <v>3000</v>
       </c>
       <c r="AI16" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="AJ16">
         <v>1</v>
@@ -1734,36 +1879,36 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:48">
+    <row r="17" spans="1:58">
       <c r="A17">
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="C17" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="D17" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="E17" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="F17" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="G17">
         <v>500</v>
       </c>
       <c r="H17" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="I17">
         <v>100</v>
       </c>
       <c r="J17" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="K17">
         <v>50</v>
@@ -1775,22 +1920,22 @@
         <v>100</v>
       </c>
       <c r="T17" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="U17">
         <v>3</v>
       </c>
       <c r="V17" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="W17" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="X17" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="Y17" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="AA17">
         <v>25000</v>
@@ -1805,30 +1950,30 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:48">
+    <row r="18" spans="1:58">
       <c r="A18">
         <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="C18" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="D18" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E18" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="F18" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="G18">
         <v>600</v>
       </c>
       <c r="H18" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="I18">
         <v>3</v>
@@ -1852,30 +1997,30 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:48">
+    <row r="19" spans="1:58">
       <c r="A19">
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="C19" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="D19" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="E19" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="F19" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="G19">
         <v>1000</v>
       </c>
       <c r="J19" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="K19">
         <v>400</v>
@@ -1893,7 +2038,7 @@
         <v>30</v>
       </c>
       <c r="W19" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="AK19">
         <v>6000</v>
@@ -1911,39 +2056,39 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="1:48">
+    <row r="20" spans="1:58">
       <c r="A20">
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="C20" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="D20" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E20" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="F20" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="G20">
         <v>1500</v>
       </c>
       <c r="T20" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="U20">
         <v>2</v>
       </c>
       <c r="V20" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="X20" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="AK20">
         <v>7000</v>
@@ -1955,30 +2100,30 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="21" spans="1:48">
+    <row r="21" spans="1:58">
       <c r="A21">
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="C21" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="D21" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="E21" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="F21" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="G21">
         <v>2000</v>
       </c>
       <c r="W21" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="AU21">
         <v>2000000000</v>
@@ -1987,30 +2132,30 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="22" spans="1:48">
+    <row r="22" spans="1:58">
       <c r="A22">
         <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="C22" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="D22" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="E22" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="F22" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="G22">
         <v>2500</v>
       </c>
       <c r="H22" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="I22">
         <v>50</v>
@@ -2022,7 +2167,7 @@
         <v>50</v>
       </c>
       <c r="T22" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="U22">
         <v>5</v>
@@ -2037,7 +2182,7 @@
         <v>20000</v>
       </c>
       <c r="AG22" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="AH22">
         <v>5</v>
@@ -2053,6 +2198,270 @@
       </c>
       <c r="AV22">
         <v>1500</v>
+      </c>
+    </row>
+    <row r="23" spans="1:58">
+      <c r="A23">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>185</v>
+      </c>
+      <c r="C23" t="s">
+        <v>186</v>
+      </c>
+      <c r="D23" t="s">
+        <v>187</v>
+      </c>
+      <c r="E23" t="s">
+        <v>188</v>
+      </c>
+      <c r="F23" t="s">
+        <v>189</v>
+      </c>
+      <c r="AU23">
+        <v>100000</v>
+      </c>
+      <c r="AV23">
+        <v>50</v>
+      </c>
+      <c r="AY23">
+        <v>25</v>
+      </c>
+      <c r="BA23">
+        <v>4</v>
+      </c>
+      <c r="BC23" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="24" spans="1:58">
+      <c r="A24">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>191</v>
+      </c>
+      <c r="C24" t="s">
+        <v>192</v>
+      </c>
+      <c r="D24" t="s">
+        <v>193</v>
+      </c>
+      <c r="E24" t="s">
+        <v>194</v>
+      </c>
+      <c r="F24" t="s">
+        <v>195</v>
+      </c>
+      <c r="AU24">
+        <v>100000</v>
+      </c>
+      <c r="AV24">
+        <v>75</v>
+      </c>
+      <c r="AW24" t="s">
+        <v>185</v>
+      </c>
+      <c r="AY24">
+        <v>25</v>
+      </c>
+      <c r="BA24">
+        <v>0</v>
+      </c>
+      <c r="BD24">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:58">
+      <c r="A25">
+        <v>29</v>
+      </c>
+      <c r="B25" t="s">
+        <v>196</v>
+      </c>
+      <c r="C25" t="s">
+        <v>197</v>
+      </c>
+      <c r="D25" t="s">
+        <v>198</v>
+      </c>
+      <c r="E25" t="s">
+        <v>199</v>
+      </c>
+      <c r="F25" t="s">
+        <v>199</v>
+      </c>
+      <c r="W25" t="s">
+        <v>200</v>
+      </c>
+      <c r="AS25">
+        <v>5000</v>
+      </c>
+      <c r="AT25">
+        <v>5000</v>
+      </c>
+      <c r="AU25">
+        <v>100000</v>
+      </c>
+      <c r="AV25">
+        <v>100</v>
+      </c>
+      <c r="AW25" t="s">
+        <v>191</v>
+      </c>
+      <c r="AY25">
+        <v>25</v>
+      </c>
+      <c r="BA25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:58">
+      <c r="A26">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>201</v>
+      </c>
+      <c r="C26" t="s">
+        <v>202</v>
+      </c>
+      <c r="D26" t="s">
+        <v>203</v>
+      </c>
+      <c r="E26" t="s">
+        <v>204</v>
+      </c>
+      <c r="F26" t="s">
+        <v>204</v>
+      </c>
+      <c r="W26" t="s">
+        <v>205</v>
+      </c>
+      <c r="AS26">
+        <v>1000</v>
+      </c>
+      <c r="AT26">
+        <v>1000</v>
+      </c>
+      <c r="AU26">
+        <v>500000</v>
+      </c>
+      <c r="AV26">
+        <v>100</v>
+      </c>
+      <c r="AW26" t="s">
+        <v>196</v>
+      </c>
+      <c r="AY26">
+        <v>25</v>
+      </c>
+      <c r="BA26">
+        <v>4</v>
+      </c>
+      <c r="BD26">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:58">
+      <c r="A27">
+        <v>31</v>
+      </c>
+      <c r="B27" t="s">
+        <v>206</v>
+      </c>
+      <c r="C27" t="s">
+        <v>207</v>
+      </c>
+      <c r="D27" t="s">
+        <v>208</v>
+      </c>
+      <c r="E27" t="s">
+        <v>209</v>
+      </c>
+      <c r="F27" t="s">
+        <v>209</v>
+      </c>
+      <c r="W27" t="s">
+        <v>210</v>
+      </c>
+      <c r="AS27">
+        <v>2000</v>
+      </c>
+      <c r="AT27">
+        <v>2000</v>
+      </c>
+      <c r="AU27">
+        <v>500000</v>
+      </c>
+      <c r="AV27">
+        <v>100</v>
+      </c>
+      <c r="AW27" t="s">
+        <v>201</v>
+      </c>
+      <c r="AY27">
+        <v>25</v>
+      </c>
+      <c r="BA27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:58">
+      <c r="A28">
+        <v>32</v>
+      </c>
+      <c r="B28" t="s">
+        <v>211</v>
+      </c>
+      <c r="C28" t="s">
+        <v>212</v>
+      </c>
+      <c r="D28" t="s">
+        <v>213</v>
+      </c>
+      <c r="E28" t="s">
+        <v>214</v>
+      </c>
+      <c r="F28" t="s">
+        <v>215</v>
+      </c>
+      <c r="AD28">
+        <v>1</v>
+      </c>
+      <c r="AE28">
+        <v>30</v>
+      </c>
+      <c r="AF28">
+        <v>500</v>
+      </c>
+      <c r="AI28" t="s">
+        <v>138</v>
+      </c>
+      <c r="AJ28">
+        <v>1</v>
+      </c>
+      <c r="AS28">
+        <v>1000</v>
+      </c>
+      <c r="AT28">
+        <v>1000</v>
+      </c>
+      <c r="AU28">
+        <v>1000000</v>
+      </c>
+      <c r="AV28">
+        <v>100</v>
+      </c>
+      <c r="AW28" t="s">
+        <v>206</v>
+      </c>
+      <c r="AY28">
+        <v>25</v>
+      </c>
+      <c r="BA28">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor changes - working on DI for event management.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="217">
   <si>
     <t>id</t>
   </si>
@@ -663,6 +663,9 @@
   </si>
   <si>
     <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; &lt;em&gt;This quest wants you to have a kingdom at a specific level, this means level the buildings, one or more, to the required level such that all buildings combined meet the required level.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Complete the required quest to unlock the ability to settle a kingdom on this plane.&lt;/p&gt;&lt;p&gt;To settle a kingdom:&lt;/p&gt;&lt;p&gt;- Select Map Movement From the Action drop down.&lt;/p&gt;&lt;p&gt;- Tap on settle after moving to a valid location.&lt;/p&gt;&lt;p&gt;- Name the kingdom and tap Settle.&lt;/p&gt;&lt;p&gt;- Tap the kingdom tab at the top to see your settled kingdoms.&lt;/p&gt;&lt;p&gt;- Here you can tap on a kingdom you want to manage and then either select from the drop down:&lt;/p&gt;&lt;p&gt;- Building Management or Unit Management to recruit Units and upgrade buildings.&lt;/p&gt;&lt;p&gt;- You can expand the Kingdom Details section to see additional information about your kingdom as well as additional actions such as purchasing population.&lt;/p&gt;&lt;p&gt;It should be noted that unlike Surface or other maps, due to the competitive nature of this Event specific map, kingdoms down here will not come with a seven day protection applied.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Passive&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;This quest also wants you to train a passive, these take real world hours to complete and provide bonuses your kingdoms across all planes.&lt;/p&gt;&lt;p&gt;To do this, tap the character sheet tab, select Skill Management from the drop down.&lt;/p&gt;&lt;p&gt;Here you will see a tab called Kingdom Passives.&lt;/p&gt;&lt;p&gt;Tapping the tab will show you a tree of skills, tap the first one and tap train. This will create a timer that will count down until the passive is trained to the next level.&lt;/p&gt;&lt;p&gt;You can logout and the timer will run behind the scenes.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Reuniting Two Old Flames</t>
   </si>
 </sst>
 </file>
@@ -1032,7 +1035,7 @@
     <col min="20" max="20" width="23.423" bestFit="true" customWidth="true" style="0"/>
     <col min="21" max="21" width="26.993" bestFit="true" customWidth="true" style="0"/>
     <col min="22" max="22" width="24.708" bestFit="true" customWidth="true" style="0"/>
-    <col min="23" max="23" width="25.851" bestFit="true" customWidth="true" style="0"/>
+    <col min="23" max="23" width="29.421" bestFit="true" customWidth="true" style="0"/>
     <col min="24" max="24" width="26.993" bestFit="true" customWidth="true" style="0"/>
     <col min="25" max="25" width="28.136" bestFit="true" customWidth="true" style="0"/>
     <col min="26" max="26" width="16.425" bestFit="true" customWidth="true" style="0"/>
@@ -2427,6 +2430,9 @@
       <c r="F28" t="s">
         <v>215</v>
       </c>
+      <c r="W28" t="s">
+        <v>216</v>
+      </c>
       <c r="AD28">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Fixed guide quests to use proper parent
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -1061,7 +1061,7 @@
     <col min="46" max="46" width="16.425" bestFit="true" customWidth="true" style="0"/>
     <col min="47" max="47" width="13.997" bestFit="true" customWidth="true" style="0"/>
     <col min="48" max="48" width="11.711" bestFit="true" customWidth="true" style="0"/>
-    <col min="49" max="49" width="35.277" bestFit="true" customWidth="true" style="0"/>
+    <col min="49" max="49" width="31.707" bestFit="true" customWidth="true" style="0"/>
     <col min="50" max="50" width="9.10" bestFit="true" style="0"/>
     <col min="51" max="51" width="18.71" bestFit="true" customWidth="true" style="0"/>
     <col min="52" max="52" width="9.10" bestFit="true" style="0"/>
@@ -2311,7 +2311,7 @@
         <v>100</v>
       </c>
       <c r="AW25" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="AY25">
         <v>25</v>
@@ -2399,7 +2399,7 @@
         <v>100</v>
       </c>
       <c r="AW27" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="AY27">
         <v>25</v>
@@ -2458,7 +2458,7 @@
         <v>100</v>
       </c>
       <c r="AW28" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="AY28">
         <v>25</v>

</xml_diff>

<commit_message>
Added more guide quests for getting players into purgatory.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="263">
   <si>
     <t>id</t>
   </si>
@@ -101,6 +101,9 @@
     <t>required_shards</t>
   </si>
   <si>
+    <t>required_copper_coins</t>
+  </si>
+  <si>
     <t>required_gold_bars</t>
   </si>
   <si>
@@ -182,6 +185,9 @@
     <t>required_attached_gems</t>
   </si>
   <si>
+    <t>required_specialty_type</t>
+  </si>
+  <si>
     <t>Welcome to Tlessa</t>
   </si>
   <si>
@@ -666,6 +672,138 @@
   </si>
   <si>
     <t>Reuniting Two Old Flames</t>
+  </si>
+  <si>
+    <t>Hell's Gates Swing Open</t>
+  </si>
+  <si>
+    <t>The days have gone by, the moon has rose and fallen and the sun rises and sets. The days bleed together and the lands become a blur. Slaughter, kill, loot, steal – repeat.&lt;br /&gt; &lt;br /&gt; You study the books of The Witch who lives on Labyrinth. Her books tell stories of The Church, back when The Red Hawks – a group of rebels – stood against The Federation. But it also tells stories of the alchemical concoctions and the twisted corrupted magics these Priests manage to create.&lt;br /&gt; &lt;br /&gt; You study the research, the formulas and the recipes hoping for some glimmer of the past to be the answer you want, your involvement in all of this, your responsible for The Creator escaping Purgatory, how are you responsible for something you played no part in?&lt;br /&gt; &lt;br /&gt; You look up from your studies and see the shadows of the flames dance in the fire place before you.&lt;br /&gt; &lt;br /&gt; Sitting in the study of your keep, high above the kingdom you have settled. The wars you have waged, the battles you have fought, the blood that stains your hands. You stare into the depths of hell it’s self.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Let’s go to Hell. Literally.&lt;/p&gt;&lt;p&gt;Hell is where the &lt;a href="/information/random-enchants" target="_blank"&gt;Queen of Hearts&lt;/a&gt; lives, she allows you to re-roll Uniques and Mythics as well as transfer those enchantments from one price of gear to another.&lt;/p&gt;&lt;p&gt;Shadow Planes was the first plane that slightly reduces you in power and slightly makes the creatures harder. You have discovered this from completing quests that require you to get items from specific locations also known as special locations. These types of locations would make creatures slightly harder.&lt;/p&gt;&lt;p&gt;At this stage, you should have a full set of crafting level 400 gear which contains enchantment level 400 enchantments.&lt;/p&gt;&lt;p&gt;Hell is also where you can start getting your end game gear: &lt;a href="/information/hell-forged-set" target="_blank"&gt;Hell Forged&lt;/a&gt;, who’s base stats are better then level 400 non enchanted gear.&lt;/p&gt;&lt;p&gt;For now, let’s focus on going to Hell.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We already know how to complete quests at this stage – so lets continue questing!&lt;/p&gt;&lt;p&gt;To get to hell and therefore get access to The Queen of Hearts, we need to complete two quests:&lt;/p&gt;&lt;p&gt;- Hells gates&lt;/p&gt;&lt;p&gt;- Queens Decision&lt;/p&gt;&lt;p&gt;The first Quest gets us into Hell, and the second quest will allow us access to The Queen of Hearts.&lt;/p&gt;&lt;p&gt;So what are you waiting for? Let’s go to Hell!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Hell</t>
+  </si>
+  <si>
+    <t>Hells Gates</t>
+  </si>
+  <si>
+    <t>Bag of Chance</t>
+  </si>
+  <si>
+    <t>Dressing up for The Queen</t>
+  </si>
+  <si>
+    <t>The heat of the land wafts over you, the sounds of death haunt you. You look around and see a barren waste land of loneliness and hollow soulless screams that ride on a dead wind.&lt;br /&gt; &lt;br /&gt; You heard the stories of gear that was once forged in the depths of Hell it’s self. You have heard the songs of The Queen her self. She sings a lust-filled laughter laced song full of sexual tension and desire.&lt;br /&gt; &lt;br /&gt; You search out the one man you came to find, one man who is said to be hidden among the barren desolate waste land of hate filled souls. You search him out for the questions that rage in your veins. You search for The Guide.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Let’s investigate how to obtain a piece of &lt;a href="/information/hell-forged-set" target="_blank"&gt;Hell Forged&lt;/a&gt; gear. To do this, you will need to craft a level 400 piece of gear, but you should already have some, equipped.&lt;/p&gt;&lt;p&gt;Hell Forged gear allows you to then Trade it later on for Purgatory Chains gear. When you purchase a piece of Hell Forged gear, you will trade a piece of your gear and the currencies needed.&lt;/p&gt;&lt;p&gt;I want you to purchase your first piece of Hell Forged gear, I also want you to trade one of the equipped items you have. Unequip a level 400 item (or remove it from a set) and then Purchase a Hell Forged gear piece of that type, for example: Ring for Ring or Spell for Spell.&lt;/p&gt;&lt;p&gt;You will see that your enchantments will be transferred, for free, from your existing gear to the new Hell Forged gear piece. This way, all your hard work is not lost.&lt;/p&gt;&lt;p&gt;This is what we call: End Game gear. Your progression starts here, your next set will be &lt;a href="/information/purgatory-chains-set" target="_blank"&gt;Purgatory Chains&lt;/a&gt;, followed by &lt;a href="/information/pirate-lord-leather-set" target="_blank"&gt;Pirate Lord Leather&lt;/a&gt; and then &lt;a href="/information/corrupted-ice" target="_blank"&gt;Corrupted Ice&lt;/a&gt;. Each set gets slightly higher stats.&lt;/p&gt;&lt;p&gt;Purgatory Chains gear, your next set, can also be obtained the same way as Hell Forged, but only while on Purgatory.&lt;/p&gt;&lt;p&gt;Pirate Lord Leather can, at the time of this guide quest, only be obtained via defeating the raid boss in a Surface Raid.&lt;/p&gt;&lt;p&gt;Corrupted Ice gear can, at the time of this guide quest, only be obtained via participating in the Winter Event and being on the Ice Plane.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;First we need to manage our inventory and either unequip an item that you have which is crafting level 400, and make sure it’s in your inventory. You can also craft a level 400 item if you please instead, but this gets rather expensive, best to use one if you have one.&lt;/p&gt;&lt;p&gt;Next:&lt;/p&gt;&lt;p&gt;- In the Actions section you will see, while on Hell, a new button called: Hell Forged gear – click it.&lt;/p&gt;&lt;p&gt;- Next select a piece of gear that matches the item type in your inventory. For example – if you unequipped a level 400 ring, select a ring. If you crafted a level 400 Body piece, select Body.&lt;/p&gt;&lt;p&gt;- Click Purchase Item if you can afford, if not go earn the currencies.&lt;/p&gt;&lt;p&gt;- Now you should have a Hell Forged Item in your inventory, any enchants on the previous item are now transferred to this one.&lt;/p&gt;&lt;p&gt;- Equip it.&lt;/p&gt;&lt;p&gt;- Repeat for each item you have equipped that meets the requirements.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; This quest only cares about you doing one item. It is suggested you replace all your items with Hell Forged.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;First we need to manage our inventory and either unequip an item that you have which is crafting level 400, and make sure it’s in your inventory. You can also craft a level 400 item if you please instead, but this gets rather expensive, best to use one if you have one.&lt;/p&gt;&lt;p&gt;Next:&lt;/p&gt;&lt;p&gt;- From the Actions drop down, select: Hell Forged gear while in Hell.&lt;/p&gt;&lt;p&gt;- Next select a piece of gear that matches the item type in your inventory. For example – if you unequipped a level 400 ring, select a ring. If you crafted a level 400 Body piece, select Body.&lt;/p&gt;&lt;p&gt;- Click Purchase Item if you can afford, if not go earn the currencies.&lt;/p&gt;&lt;p&gt;- Now you should have a Hell Forged Item in your inventory, any enchants on the previous item are now transferred to this one.&lt;/p&gt;&lt;p&gt;- Equip it.&lt;/p&gt;&lt;p&gt;- Repeat for each item you have equipped that meets the requirements.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Note: &lt;/strong&gt;This quest only cares about you doing one item. It is suggested you replace all your items with Hell Forged.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Hell Forged</t>
+  </si>
+  <si>
+    <t>The Queens got the Info, if you have the coin</t>
+  </si>
+  <si>
+    <t>“Ooooh hooo hoo hoo!” Comes a flitatious laughter. A busty beautiful woman comes walking from seemingly no where. “Hello my beautiful child. How are e today? I! I am The Queen of Hearts!”&lt;br /&gt; &lt;br /&gt; You stare at her radiant beauty. Her eyes are a blue unlike any other blue. Her hair is a dust flowing red that dances in the dead air.&lt;br /&gt; &lt;br /&gt; You have heard of her, a women whose power is beyond any you have seen. She can create, from thin air, powerful unique items. She is also the women that can altar Uniques and Mythical items the Enchantress would tell you about.&lt;br /&gt; &lt;br /&gt; “My child, is there something I can help you with down here in this fabulously hot plane of scorching torment and pain? Oooooh hoo hooo hoo!”&lt;br /&gt; &lt;br /&gt; You explain that you are searching for The Guide and if she has seen him.&lt;br /&gt; &lt;br /&gt; “Maybe you should please me with your coin and when I'm well and satisfied I can tell you what you want.” She winks at you and shes her chest in your face. Do you shove your gold in hers?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;The Queen of Hearts is an NPC who allows you to purchase more powerful Uniques, Legendary Uniques are what you want for now and are apart of your end game progression until you can get a mythical item.&lt;/p&gt;&lt;p&gt;Up until now you have been able to get Basic Uniques, which were, at the time, better then any enchantment you had and worked well in conjunction to your enchantments, but then you might have went to Gold Mines on the Shadow Plane and earned your self A “medium” unique item.&lt;/p&gt;&lt;p&gt;But now, you can purchase Legendary Uniques, this tier of enchantments is one below Mythical which are currently, at the time of this guide quest, the best enchantment type you can have in game.&lt;/p&gt;&lt;p&gt;The Queen, as mentioned, also allows you to re-roll uniques (basic, medium and legendary) as well as mythical enchantments. You can re-roll all aspects about the enchantment to get the best stats you can in an RNG world.&lt;/p&gt;&lt;p&gt;Finally, The Queen allows players to take enchantments – Uniques and Mythics and move them from one item to an item of their choosing!&lt;/p&gt;&lt;p&gt;Ideally, you should purchase a legendary unique from the queen – keep buying till you get an item with two enchants on it. Then use the queen to re-roll that unique aiming for higher stats and base damage for example. Lastly you would move these uniques to a body Hell Forged gear piece you own for maximum effect.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;The instructions will tell you how to do this should you want to, but this guide quest focuses on faction leveling.&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;How to use the queen!&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- From the Craft/Enchant drop down – and while on hell – select Queen of Hearts&lt;/p&gt;&lt;p&gt;- Select Buy Item from the drop down.&lt;/p&gt;&lt;p&gt;- Select Legendary from the drop down.&lt;/p&gt;&lt;p&gt;- Purchase, check the server message section.&lt;/p&gt;&lt;p&gt;Repeat this until you have an item that has two enchants.&lt;/p&gt;&lt;p&gt;Next, lets re-roll the unique. First, make sure to inspect the item, but clicking on it from your inventory or the server message section and clicking details.&lt;/p&gt;&lt;p&gt;On the details section you will see two orange buttons whose label is that of the attached enchants.&lt;/p&gt;&lt;p&gt;If you click on these it will tell you more about the attached affixes. Most characters at this point want to increase their stats as high as they can afford and the RNG will allow them. You can, for example as a vampire, focus more on raising a specific stat (DUR) and attribute: Life Stealing. To do this, we need to re-roll the affixes. The queen can help us:&lt;/p&gt;&lt;p&gt;- Click Change Action&lt;/p&gt;&lt;p&gt;- Select Re-roll item&lt;/p&gt;&lt;p&gt;- Select the item you wanted, this list only has your Uniques and Mythics in your inventory.&lt;/p&gt;&lt;p&gt;- Select Either the Prefix, the Suffix or both&lt;/p&gt;&lt;p&gt;- Select the aspect of the affix(es) you want to re-roll and click re-roll.&lt;/p&gt;&lt;p&gt;The item will then appear in your server message section so you can easily investigate the item and see if you should re-roll or not. Keep doing this until you have the enchantments where you want them. Next we move them:&lt;/p&gt;&lt;p&gt;To do this, the item you want the enchantments to be move to, needs to be in your inventory. Ideally – this would be your body and it would be Hell Forged (Maximum stat gain). But you are free to do as you wish.&lt;/p&gt;&lt;p&gt;- Click Change Action&lt;/p&gt;&lt;p&gt;- Select Move Enchants&lt;/p&gt;&lt;p&gt;- Select The Unique you spent time re-rolling&lt;/p&gt;&lt;p&gt;- Select Both for the affixes to move&lt;/p&gt;&lt;p&gt;- Select the item you want to move them to.&lt;/p&gt;&lt;p&gt;Click Move Enchants and boom done!&lt;/p&gt;&lt;p&gt;Now go get some faction points!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;How to use the queen!&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- From the actions drop down select Craft&lt;/p&gt;&lt;p&gt;- From the Craft drop down – and while on hell – select Queen of Hearts&lt;/p&gt;&lt;p&gt;- Select Buy Item from the drop down.&lt;/p&gt;&lt;p&gt;- Select Legendary from the drop down.&lt;/p&gt;&lt;p&gt;- Purchase, check the server message section.&lt;/p&gt;&lt;p&gt;Repeat this until you have an item that has two enchants.&lt;/p&gt;&lt;p&gt;Next, lets re-roll the unique. First, make sure to inspect the item, but clicking on it from your inventory or the server message section and clicking details.&lt;/p&gt;&lt;p&gt;On the details section you will see two orange buttons whose label is that of the attached enchants.&lt;/p&gt;&lt;p&gt;If you click on these it will tell you more about the attached affixes. Most characters at this point want to increase their stats as high as they can afford and the RNG will allow them. You can, for example as a vampire, focus more on raising a specific stat (DUR) and attribute: Life Stealing. To do this, we need to re-roll the affixes. The queen can help us:&lt;/p&gt;&lt;p&gt;- Tap Change Action&lt;/p&gt;&lt;p&gt;- Select Re-roll item&lt;/p&gt;&lt;p&gt;- Select the item you wanted, this list only has your Uniques and Mythics in your inventory.&lt;/p&gt;&lt;p&gt;- Select Either the Prefix, the Suffix or both&lt;/p&gt;&lt;p&gt;- Select the aspect of the affix(es) you want to re-roll and click re-roll.&lt;/p&gt;&lt;p&gt;The item will then appear in your server message section so you can easily investigate the item and see if you should re-roll or not. Keep doing this until you have the enchantments where you want them. Next we move them:&lt;/p&gt;&lt;p&gt;To do this, the item you want the enchantments to be move to, needs to be in your inventory. Ideally – this would be your body and it would be Hell Forged (Maximum stat gain). But you are free to do as you wish.&lt;/p&gt;&lt;p&gt;- Tap Change Action&lt;/p&gt;&lt;p&gt;- Select Move Enchants&lt;/p&gt;&lt;p&gt;- Select The Unique you spent time re-rolling&lt;/p&gt;&lt;p&gt;- Select Both for the affixes to move&lt;/p&gt;&lt;p&gt;- Select the item you want to move them to.&lt;/p&gt;&lt;p&gt;Tap Move Enchants and boom done!&lt;/p&gt;&lt;p&gt;Now go get some faction points!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Seeking out darkness</t>
+  </si>
+  <si>
+    <t>You told the Queen everything. Your entire adventure. She sits and enjoys the coin and she gives you the shiny items. When your done telling her your tale, she stares off for a moment, as if in deep though only to then perk up with laughter:&lt;br /&gt; &lt;br /&gt; “Oooooh hooo hooo hooo child! I, The Queen of all that there is, can tell you this:&lt;br /&gt; &lt;br /&gt; The Guide is hunting a darkness that has escaped the shadows of a land only whispered in the shadows of midnight. And it’s never midnight down here! Ooooh hooo hooo hooo!”&lt;br /&gt; &lt;br /&gt; She vanishes and leaves you with more questions then answers, but then again – after all you have been through, its the least of your concerns.&lt;br /&gt; &lt;br /&gt; She never answered where The Guide is. She never gave any insight. She just gave you items. How do you even proceede?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We need to go to Purgatory to really start the End game. But to get there, we have some quests to complete.&lt;/p&gt;&lt;p&gt;Purgatory is the last, at the time of this guide quest, Plane that players have access to out side of special events like the Winter Event, who comes with the Ice Plane&lt;/p&gt;&lt;p&gt;Purgatory has a special location called: Purgatory Smiths House where numerous amounts of currencies drop for end game crafting like &lt;a href="/information/trinketry" target="_blank"&gt;Trinketry&lt;/a&gt;, &lt;a href="/information/gems" target="_blank"&gt;Gem Crafting&lt;/a&gt; and later on Alchemy crafting.&lt;/p&gt;&lt;p&gt;For now, lets complete some quests to get us to Purgatory. You’ll need to be able to walk on magma in Hell, so there is that too.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Easy peasy, lemon squeesy – complete some quests and traverse down!&lt;/p&gt;&lt;p&gt;Oh! Wait, one more thing: You must teleport or walk, once you can walk on magma to the location: Tear in the Fabric of Time (X/Y): 208/64 in Hell. Only from here will Purgatory appear in your traverse drop down list.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Purgatory</t>
+  </si>
+  <si>
+    <t>Don't burn now</t>
+  </si>
+  <si>
+    <t>The End and The Beginning</t>
+  </si>
+  <si>
+    <t>There is a darkness in this land. One that creeps into your very being, the fabric of your soul.&lt;br /&gt; &lt;br /&gt; “Welcome to purgatory.” The Guide appears before you, young and handsome. His appearance changes so often and so much its confusing as to who he even is. But alas, he stands beside you.&lt;br /&gt; &lt;br /&gt; “This is where it started. This is where it ended. This is where he escaped from. I seek The smith. When The Child escaped this place, he set loose the blacksmiths - a set of smiths from Purgatory. These smiths are corrupted in their soul, like you – a fragment of a larger structure, a crystalline structure – shattered and scattered across the sands of time.”&lt;br /&gt; &lt;br /&gt; He falls silent and the two of you stand staring out across the desolate waste land of emptiness. So many lands that feel so empty, so lonely, so depressing.&lt;br /&gt; &lt;br /&gt; “Down here.” The Guide starts: “There is a darkness that corrupts the air we breathe. It makes us much weaker, much more susceptible to death. There are ways child – ways you can get around this. You’ll need to seek out the alchemical books and teachings for a special kind of oil.”&lt;br /&gt; &lt;br /&gt; He looks at you and you him, neither of you speak for a moment as you both go back to staring out at the land.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welcome to Purgatory. This is where the hardest creatures live and the rewards are the greatest. Alas to begin our journey towards the ultimate goal of reincarnation – we need stronger gear. By now you should have a full set of Hell Forged gear enchanted our the ass with level 400 enchants and at least 2 legendary enchantments on one item – ideally the body.&lt;/p&gt;&lt;p&gt;Your Accuracy, Looting and possibly Casting Accuracy should be maxed out.&lt;/p&gt;&lt;p&gt;Your gear will only take you so far down the critter list. You need something: Holy Oils. You can unlock this through Alchemy – so lets begin training until we have unlocked &lt;a href="/information/holy-items" target="_blank"&gt;Holy Oils&lt;/a&gt;. I would stay out of special locations for now, you are far too weak!&lt;/p&gt;&lt;p&gt;Instead lets explore down here and do some Alchemical crafting. If you start to run low on Gold Dust and Shards I suggest heading to the Gold Mines on Shadow Plane until we have unlocked the Purgatory Smith House.&lt;/p&gt;&lt;p&gt;While manually battling in Gold Mines you can get enough currencies to continue level alchemy.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Raise your alchemy skill child. Raise it on high so we can slaughter the beasts before us!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Oiling up for combat</t>
+  </si>
+  <si>
+    <t>You poured over the texts and plunged deep into the depths of the mines hunting the creatures who carry the currency you needed to complete your studies. It has been such a long road.&lt;br /&gt; &lt;br /&gt; Now you have the tools, the starts of the tools you need, to take on the depths of dungeons in purgatory.&lt;br /&gt; &lt;br /&gt; You also need the coin, a rare currency that was once used back in the days of old, during the war – a currency made of copper.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;One of the things you need, to survive in purgatory, is extra stats and devouring percentage. You can get this through applying &lt;a href="/information/holy-items" target="_blank"&gt;Holy Oils&lt;/a&gt;, that you craft through alchemy to items in your inventory. To do this you need to go to Purgatory and use The Work Bench.&lt;/p&gt;&lt;p&gt;This guide quest will have you craft alchemy Holy Oils and then apply them to your equipment. Consider this the third step in your end game gear progression. First we upgraded our crafted gear to Hell Forged, then we applied our best rolled Legendary enchantments to one piece of that gear and now we shall apply some holy oils.&lt;/p&gt;&lt;p&gt;Each item – at level 400 in crafting and all specialty gear sets – have 20 stacks of oils that can be applied. Caution though, there are different oils and you only really care about one of them: The Creators Holy Oil&lt;/p&gt;&lt;p&gt;If you apply other oils, you could end up with less then ideal stats and since there is no way to re-roll or remove oils, you should use caution to only apply the best.&lt;/p&gt;&lt;p&gt;When you apply an oil to the item you will raise your stats by a % a small % that stacks with the more oils you apply to an item.&lt;/p&gt;&lt;p&gt;Lets start by upgrading two of our items with oils!&lt;/p&gt;&lt;p&gt;You will also need to complete a quest: The Magic of Purgatory in Hell – this will give you a quest item that allows you to gain Copper Coins, we need them for the next quest. So kill some cratures on creatures for the coins to drop. You can also play slots to gain the currency and purchase the Child of Copper coins Mercenary to help with the drop rates till we can get into the house.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;First, craft 40 The Creators Holy Oil’s. This might take a moment and might require a trip to The Gold Mines on Shadow Planes.&lt;/p&gt;&lt;p&gt;Next unequip two items, ideally Body and Weapon to start (or spell if you are a caster). These should be your Hell Forged gear items.&lt;/p&gt;&lt;p&gt;Head down to Purgatory. Now the fun begins:&lt;/p&gt;&lt;p&gt;- Select Workbench from Craft/Enchant&lt;/p&gt;&lt;p&gt;- Select an item to apply the oils to&lt;/p&gt;&lt;p&gt;- Select an oil from the second drop down&lt;/p&gt;&lt;p&gt;- Click Apply Oil&lt;/p&gt;&lt;p&gt;You will see that your Applied Holy Stacks will increase by one. When the count reaches the max holy stacks, below it, the item will leave the list as you have applied the maximum amount of oils to the item.&lt;/p&gt;&lt;p&gt;When the item has an oil applied to it, it will appear in your server message section. Click the item, click details, and scroll down to the Holy Info section. Here you can click view info to see each stack and what was rolled. The Creators Holy Oil is the best oil for stat and devouring bonus increase. This will become very handy in Purgatory where you are severely weakened, the more stats and devouring the better chances you have to survive.&lt;/p&gt;&lt;p&gt;Repeat applying oils until you have maxed the 20 stacks on each item. You can see your Holy Information on your character sheet if you click on Show additional details, and then select the Holy tab you will see how this affects your character in the big picture.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;First, craft 40 The Creators Holy Oil’s. This might take a moment and might require a trip to The Gold Mines on Shadow Planes.&lt;/p&gt;&lt;p&gt;Next unequip two items, ideally Body and Weapon to start (or spell if you are a caster). These should be your Hell Forged gear items.&lt;/p&gt;&lt;p&gt;Head down to Purgatory. Now the fun begins:&lt;/p&gt;&lt;p&gt;- Select Craft from the Actions drop down&lt;/p&gt;&lt;p&gt;- Select Workbench from Crafting drop down&lt;/p&gt;&lt;p&gt;- Select an item to apply the oils to&lt;/p&gt;&lt;p&gt;- Select an oil from the second drop down&lt;/p&gt;&lt;p&gt;- Tap Apply Oil&lt;/p&gt;&lt;p&gt;You will see that your Applied Holy Stacks will increase by one. When the count reaches the max holy stacks, below it, the item will leave the list as you have applied the maximum amount of oils to the item.&lt;/p&gt;&lt;p&gt;When the item has an oil applied to it, it will appear in your server message section. tap the item, tap details, and scroll down to the Holy Info section. Here you can tap view info to see each stack and what was rolled. The Creators Holy Oil is the best oil for stat and devouring bonus increase. This will become very handy in Purgatory where you are severely weakened, the more stats and devouring the better chances you have to survive.&lt;/p&gt;&lt;p&gt;Repeat applying oils until you have maxed the 20 stacks on each item. You can see your Holy Information on your character sheet if you tap on Show additional details – by expanding the top section, and then select the Holy tab you will see how this affects your character in the big picture.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>The Magic of Purgatory</t>
+  </si>
+  <si>
+    <t>The Smith and The Cage</t>
+  </si>
+  <si>
+    <t>“Have you seen the house?” Comes a voice. You look up from your plate while sitting in a pub in Smugglers Port.&lt;br /&gt; &lt;br /&gt; The House? What house?&lt;br /&gt; &lt;br /&gt; “There is a house where a man known as The Purgatory Smith, lived. No one knows where he went once The Child escaped Purgatory. Some say he came to Surface, some say he just vanished, the magic that had created him has withered and died.”&lt;br /&gt; &lt;br /&gt; He pauses and takes a sip from his mug, you stare in silence and absorb the words, digesting the meaning.&lt;br /&gt; &lt;br /&gt; But me, what does this have to do with me? You ponder this.&lt;br /&gt; &lt;br /&gt; “You, child, come in to place where you are a piece of the structure that held The Child in place. All of these people are. All of the adventurers are who come and seek out the riches and fame of this land and all the lands connected.”&lt;br /&gt; &lt;br /&gt; A piece of the structure. What structure?&lt;br /&gt; &lt;br /&gt; “That cage.”</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Now that we have Copper Coins and We have applied oils to our weapons and armour and coated our selves up. We have another upgrade for gear to do. &lt;a href="/information/purgatory-chains-set" target="_blank"&gt;Purgatory Chains&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;This process is very similar to that of Hell Forged, don’t worry – all your hard work will be copied over to your new item.&lt;/p&gt;&lt;p&gt;Purgatory Chains gear is as far as you will be able to take your gear – at this time – by the process of upgrading through specialty shops like this.&lt;/p&gt;&lt;p&gt;At this stage, with a full set of Purgatory Chain covered in holy oils and dripping in high end enchants that define your build – allow you to do unimaginable damage, you still have a ways to go before you have truly reached your full potential.&lt;/p&gt;&lt;p&gt;After this, the last set of upgrades we have to work on is &lt;a href="/information/trinketry" target="_blank"&gt;trinkets&lt;/a&gt; and &lt;a href="/information/gems" target="_blank"&gt;gems&lt;/a&gt;. But one thing at a time child, lets get some chains on our body shall we?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;At this stage we have already done the upgrade process for Crafted gear to hell Forged. Now we go from Hell Forged to Purgatory Chains. Repeat the same steps you did for the upgrade, this time the specialty shop is in purgatory so head on down and get your gear, assuming you can afford it.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Purgatory Chains</t>
+  </si>
+  <si>
+    <t>Shattering the illusion</t>
+  </si>
+  <si>
+    <t>The Cage, its a mythical and legendary place – like the one that held Satan in the depths of Hell. It was created after that cage was created. It was created by the same man who create the first one. It was create by The Poet.&lt;br /&gt; &lt;br /&gt; “The Poet trapped Satan in a cage deep in the bowls of Hell, but even that was not enough magic to hold such a mighty beast. To hold a creature of the worlds power and beyond, The poet used the last of his immortal and angelic power to trap The Child in another plane, another dimension, where his own misery and loneliness could no longer corrupt the world around him.”&lt;br /&gt; &lt;br /&gt; The Guide stops to drink his ale and eat off his plate. The barmaid comes over and takes away the plates after some time.&lt;br /&gt; &lt;br /&gt; “The world is now the cage, the world, the people, the magic of it all. It’s all we have – but he is close to his ultimate goal.”&lt;br /&gt; &lt;br /&gt; His ultimate goal?&lt;br /&gt; &lt;br /&gt; “To shatter reality.”</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We have some copper coins and we have seen that even with maxed out Holy Oils, powerful Enchants and end game gear – we cannot make it very far down the list. We keep getting &lt;a href="/information/ambush-and-counter" target="_blank"&gt;ambushed, countered&lt;/a&gt; and slaughtered.&lt;/p&gt;&lt;p&gt;This is where &lt;a href="/information/trinketry" target="_blank"&gt;trinkets&lt;/a&gt; come into play and a new concept: Ambush and Counter.&lt;/p&gt;&lt;p&gt;Ambush is where you have a chance to ambush the enemy and deal immense damage to the enemy before they can think, there's a chance for this to kill the enemy outright.&lt;/p&gt;&lt;p&gt;Alas, the enemy can Ambush you as well. Down here – in Purgatory – creatures will always ambush first – hence the second aspect of trinkets: Ambush Resistance. You can resit the enemies ambush.&lt;/p&gt;&lt;p&gt;The other aspects of trinkets that you might have also discovered down here is: Counter.&lt;/p&gt;&lt;p&gt;Countering is when you or the enemy jump in, after an action like Weapon Damage or Spell Damage and counter the attack with one of your own. This can also kill you or the enemy.&lt;/p&gt;&lt;p&gt;Characters can equip a single trinket and the only way to get them is to craft them.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;To stand a chance to make it further down the list in Purgatory we have to craft a trinket. These cannot be enchanted or have holy oils applied to them and they cannot be sold to the shop. The can be destroyed and listed on the market.&lt;/p&gt;&lt;p&gt;To be able to do any of this though, we need to craft them. So how do we do that?&lt;/p&gt;&lt;p&gt;- From Craft/Enchant select Trinketry – while on any plane.&lt;/p&gt;&lt;p&gt;- Select a trinket. These require Gold Dust and Copper Coins.&lt;/p&gt;&lt;p&gt;- Craft&lt;/p&gt;&lt;p&gt;That's all there is to it.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;To stand a chance to make it further down the list in Purgatory we have to craft a trinket. These cannot be enchanted or have holy oils applied to them and they cannot be sold to the shop. The can be destroyed and listed on the market.&lt;/p&gt;&lt;p&gt;To be able to do any of this though, we need to craft them. So how do we do that?&lt;/p&gt;&lt;p&gt;- Select Craft from the Actions Drop Down&lt;/p&gt;&lt;p&gt;- Select Trinketry – while on any plane.&lt;/p&gt;&lt;p&gt;- Select a trinket. These require Gold Dust and Copper Coins.&lt;/p&gt;&lt;p&gt;- Craft&lt;/p&gt;&lt;p&gt;That's all there is to it.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -1005,7 +1143,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:BF28"/>
+  <dimension ref="A1:BH36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1014,11 +1152,11 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="3.428" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="35.277" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="54.13" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="1886.254" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="2760.469" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="1851.976" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="2031.361" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="2355.71" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="2395.844" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="18.71" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="24.708" bestFit="true" customWidth="true" style="0"/>
@@ -1041,39 +1179,41 @@
     <col min="26" max="26" width="16.425" bestFit="true" customWidth="true" style="0"/>
     <col min="27" max="27" width="22.28" bestFit="true" customWidth="true" style="0"/>
     <col min="28" max="28" width="18.71" bestFit="true" customWidth="true" style="0"/>
-    <col min="29" max="29" width="22.28" bestFit="true" customWidth="true" style="0"/>
-    <col min="30" max="30" width="21.138" bestFit="true" customWidth="true" style="0"/>
-    <col min="31" max="31" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="29" max="29" width="25.851" bestFit="true" customWidth="true" style="0"/>
+    <col min="30" max="30" width="22.28" bestFit="true" customWidth="true" style="0"/>
+    <col min="31" max="31" width="21.138" bestFit="true" customWidth="true" style="0"/>
     <col min="32" max="32" width="26.993" bestFit="true" customWidth="true" style="0"/>
-    <col min="33" max="33" width="34.135" bestFit="true" customWidth="true" style="0"/>
-    <col min="34" max="34" width="37.705" bestFit="true" customWidth="true" style="0"/>
-    <col min="35" max="35" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="33" max="33" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="34" max="34" width="34.135" bestFit="true" customWidth="true" style="0"/>
+    <col min="35" max="35" width="37.705" bestFit="true" customWidth="true" style="0"/>
     <col min="36" max="36" width="26.993" bestFit="true" customWidth="true" style="0"/>
-    <col min="37" max="37" width="17.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="38" max="38" width="15.282" bestFit="true" customWidth="true" style="0"/>
+    <col min="37" max="37" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="38" max="38" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="39" max="39" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="40" max="40" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="41" max="41" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="42" max="42" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="43" max="43" width="15.282" bestFit="true" customWidth="true" style="0"/>
-    <col min="44" max="44" width="17.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="45" max="45" width="19.995" bestFit="true" customWidth="true" style="0"/>
-    <col min="46" max="46" width="16.425" bestFit="true" customWidth="true" style="0"/>
-    <col min="47" max="47" width="13.997" bestFit="true" customWidth="true" style="0"/>
-    <col min="48" max="48" width="11.711" bestFit="true" customWidth="true" style="0"/>
-    <col min="49" max="49" width="31.707" bestFit="true" customWidth="true" style="0"/>
-    <col min="50" max="50" width="9.10" bestFit="true" style="0"/>
-    <col min="51" max="51" width="18.71" bestFit="true" customWidth="true" style="0"/>
-    <col min="52" max="52" width="9.10" bestFit="true" style="0"/>
-    <col min="53" max="53" width="21.138" bestFit="true" customWidth="true" style="0"/>
-    <col min="54" max="54" width="9.10" bestFit="true" style="0"/>
-    <col min="55" max="55" width="17.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="56" max="56" width="39.99" bestFit="true" customWidth="true" style="0"/>
-    <col min="57" max="57" width="24.708" bestFit="true" customWidth="true" style="0"/>
-    <col min="58" max="58" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="44" max="44" width="15.282" bestFit="true" customWidth="true" style="0"/>
+    <col min="45" max="45" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="46" max="46" width="19.995" bestFit="true" customWidth="true" style="0"/>
+    <col min="47" max="47" width="16.425" bestFit="true" customWidth="true" style="0"/>
+    <col min="48" max="48" width="13.997" bestFit="true" customWidth="true" style="0"/>
+    <col min="49" max="49" width="11.711" bestFit="true" customWidth="true" style="0"/>
+    <col min="50" max="50" width="31.707" bestFit="true" customWidth="true" style="0"/>
+    <col min="51" max="51" width="9.10" bestFit="true" style="0"/>
+    <col min="52" max="52" width="18.71" bestFit="true" customWidth="true" style="0"/>
+    <col min="53" max="53" width="9.10" bestFit="true" style="0"/>
+    <col min="54" max="54" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="55" max="55" width="9.10" bestFit="true" style="0"/>
+    <col min="56" max="56" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="57" max="57" width="39.99" bestFit="true" customWidth="true" style="0"/>
+    <col min="58" max="58" width="24.708" bestFit="true" customWidth="true" style="0"/>
+    <col min="59" max="59" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="60" max="60" width="28.136" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58">
+    <row r="1" spans="1:60">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1221,13 +1361,13 @@
       <c r="AW1" t="s">
         <v>48</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AX1" t="s">
         <v>49</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="AZ1" t="s">
         <v>50</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BB1" t="s">
         <v>51</v>
       </c>
       <c r="BD1" t="s">
@@ -1239,233 +1379,239 @@
       <c r="BF1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:58">
+      <c r="BG1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:60">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G2">
         <v>2</v>
       </c>
-      <c r="AU2">
+      <c r="AV2">
         <v>500</v>
       </c>
-      <c r="AV2">
+      <c r="AW2">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:58">
+    <row r="3" spans="1:60">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G3">
         <v>10</v>
       </c>
-      <c r="AU3">
+      <c r="AV3">
         <v>500</v>
       </c>
-      <c r="AV3">
+      <c r="AW3">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:58">
+    <row r="4" spans="1:60">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G4">
         <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I4">
         <v>10</v>
       </c>
       <c r="J4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K4">
         <v>15</v>
       </c>
-      <c r="AK4">
+      <c r="AL4">
         <v>50</v>
       </c>
-      <c r="AU4">
+      <c r="AV4">
         <v>1000</v>
       </c>
-      <c r="AV4">
+      <c r="AW4">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:58">
+    <row r="5" spans="1:60">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G5">
         <v>50</v>
       </c>
       <c r="H5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I5">
         <v>5</v>
       </c>
       <c r="J5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K5">
         <v>5</v>
       </c>
       <c r="X5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="Y5" t="s">
-        <v>80</v>
-      </c>
-      <c r="AU5">
+        <v>82</v>
+      </c>
+      <c r="AV5">
         <v>1000</v>
       </c>
-      <c r="AV5">
+      <c r="AW5">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:58">
+    <row r="6" spans="1:60">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G6">
         <v>60</v>
       </c>
       <c r="H6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="I6">
         <v>5</v>
       </c>
       <c r="J6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="K6">
         <v>15</v>
       </c>
       <c r="X6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AO6">
+        <v>89</v>
+      </c>
+      <c r="AP6">
         <v>125</v>
       </c>
-      <c r="AU6">
+      <c r="AV6">
         <v>10000</v>
       </c>
-      <c r="AV6">
+      <c r="AW6">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:58">
+    <row r="7" spans="1:60">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E7" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G7">
         <v>120</v>
       </c>
       <c r="H7" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I7">
         <v>15</v>
       </c>
       <c r="J7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K7">
         <v>5</v>
@@ -1477,171 +1623,171 @@
         <v>10</v>
       </c>
       <c r="X7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AA7">
         <v>500</v>
       </c>
-      <c r="AK7">
+      <c r="AL7">
         <v>210</v>
       </c>
-      <c r="AS7">
+      <c r="AT7">
         <v>500</v>
       </c>
-      <c r="AT7">
+      <c r="AU7">
         <v>0</v>
       </c>
-      <c r="AU7">
+      <c r="AV7">
         <v>100000</v>
       </c>
-      <c r="AV7">
+      <c r="AW7">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:58">
+    <row r="8" spans="1:60">
       <c r="A8">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C8" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E8" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F8" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="T8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="U8">
         <v>3</v>
       </c>
       <c r="W8" t="s">
-        <v>102</v>
-      </c>
-      <c r="AS8">
+        <v>104</v>
+      </c>
+      <c r="AT8">
         <v>1000</v>
       </c>
-      <c r="AT8">
+      <c r="AU8">
         <v>100</v>
       </c>
-      <c r="AU8">
+      <c r="AV8">
         <v>100000</v>
       </c>
-      <c r="AV8">
+      <c r="AW8">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:58">
+    <row r="9" spans="1:60">
       <c r="A9">
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D9" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E9" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F9" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H9" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I9">
         <v>50</v>
       </c>
       <c r="W9" t="s">
-        <v>107</v>
-      </c>
-      <c r="AS9">
+        <v>109</v>
+      </c>
+      <c r="AT9">
         <v>2500</v>
       </c>
-      <c r="AT9">
+      <c r="AU9">
         <v>100</v>
       </c>
-      <c r="AU9">
+      <c r="AV9">
         <v>100000</v>
       </c>
-      <c r="AV9">
+      <c r="AW9">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:58">
+    <row r="10" spans="1:60">
       <c r="A10">
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E10" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F10" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G10">
         <v>300</v>
       </c>
       <c r="T10" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="U10">
         <v>2</v>
       </c>
       <c r="V10" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="X10" t="s">
-        <v>114</v>
-      </c>
-      <c r="AS10">
+        <v>116</v>
+      </c>
+      <c r="AT10">
         <v>1000</v>
       </c>
-      <c r="AU10">
+      <c r="AV10">
         <v>500000</v>
       </c>
-      <c r="AV10">
+      <c r="AW10">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:58">
+    <row r="11" spans="1:60">
       <c r="A11">
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C11" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D11" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E11" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F11" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="R11">
         <v>1</v>
@@ -1649,37 +1795,37 @@
       <c r="S11">
         <v>1</v>
       </c>
-      <c r="AU11">
+      <c r="AV11">
         <v>500000</v>
       </c>
-      <c r="AV11">
+      <c r="AW11">
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:58">
+    <row r="12" spans="1:60">
       <c r="A12">
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C12" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D12" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E12" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F12" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="N12" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="O12" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="P12">
         <v>2</v>
@@ -1687,169 +1833,169 @@
       <c r="Q12">
         <v>2</v>
       </c>
-      <c r="AS12">
-        <v>1000</v>
-      </c>
       <c r="AT12">
         <v>1000</v>
       </c>
       <c r="AU12">
+        <v>1000</v>
+      </c>
+      <c r="AV12">
         <v>1000000</v>
       </c>
-      <c r="AV12">
+      <c r="AW12">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:58">
+    <row r="13" spans="1:60">
       <c r="A13">
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C13" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D13" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E13" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F13" t="s">
-        <v>131</v>
-      </c>
-      <c r="AD13">
+        <v>133</v>
+      </c>
+      <c r="AE13">
         <v>1</v>
       </c>
-      <c r="AE13">
+      <c r="AF13">
         <v>30</v>
       </c>
-      <c r="AF13">
+      <c r="AG13">
         <v>100</v>
       </c>
-      <c r="AU13">
+      <c r="AV13">
         <v>1000000</v>
       </c>
-      <c r="AV13">
+      <c r="AW13">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:58">
+    <row r="14" spans="1:60">
       <c r="A14">
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C14" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D14" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E14" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F14" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H14" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I14">
         <v>25</v>
       </c>
       <c r="J14" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="K14">
         <v>5</v>
       </c>
-      <c r="AE14">
+      <c r="AF14">
         <v>60</v>
       </c>
-      <c r="AF14">
+      <c r="AG14">
         <v>500</v>
       </c>
-      <c r="AI14" t="s">
-        <v>138</v>
-      </c>
-      <c r="AJ14">
+      <c r="AJ14" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK14">
         <v>1</v>
       </c>
-      <c r="AU14">
+      <c r="AV14">
         <v>2000000</v>
       </c>
-      <c r="AV14">
+      <c r="AW14">
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:58">
+    <row r="15" spans="1:60">
       <c r="A15">
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C15" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D15" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E15" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F15" t="s">
-        <v>142</v>
-      </c>
-      <c r="AE15">
+        <v>144</v>
+      </c>
+      <c r="AF15">
         <v>75</v>
       </c>
-      <c r="AF15">
+      <c r="AG15">
         <v>2000</v>
       </c>
-      <c r="AI15" t="s">
-        <v>143</v>
-      </c>
-      <c r="AJ15">
+      <c r="AJ15" t="s">
+        <v>145</v>
+      </c>
+      <c r="AK15">
         <v>2</v>
       </c>
-      <c r="AU15">
+      <c r="AV15">
         <v>2000000</v>
       </c>
-      <c r="AV15">
+      <c r="AW15">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:58">
+    <row r="16" spans="1:60">
       <c r="A16">
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C16" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D16" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E16" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F16" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H16" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I16">
         <v>25</v>
       </c>
       <c r="J16" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="K16">
         <v>50</v>
@@ -1861,57 +2007,57 @@
         <v>10</v>
       </c>
       <c r="W16" t="s">
-        <v>148</v>
-      </c>
-      <c r="AE16">
+        <v>150</v>
+      </c>
+      <c r="AF16">
         <v>100</v>
       </c>
-      <c r="AF16">
+      <c r="AG16">
         <v>3000</v>
       </c>
-      <c r="AI16" t="s">
-        <v>149</v>
-      </c>
-      <c r="AJ16">
+      <c r="AJ16" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK16">
         <v>1</v>
       </c>
-      <c r="AU16">
+      <c r="AV16">
         <v>5000000</v>
       </c>
-      <c r="AV16">
+      <c r="AW16">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:58">
+    <row r="17" spans="1:60">
       <c r="A17">
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C17" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D17" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E17" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F17" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G17">
         <v>500</v>
       </c>
       <c r="H17" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I17">
         <v>100</v>
       </c>
       <c r="J17" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K17">
         <v>50</v>
@@ -1923,60 +2069,60 @@
         <v>100</v>
       </c>
       <c r="T17" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="U17">
         <v>3</v>
       </c>
       <c r="V17" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="W17" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="X17" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="Y17" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="AA17">
         <v>25000</v>
       </c>
-      <c r="AT17">
+      <c r="AU17">
         <v>1000</v>
       </c>
-      <c r="AU17">
+      <c r="AV17">
         <v>50000000</v>
       </c>
-      <c r="AV17">
+      <c r="AW17">
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:58">
+    <row r="18" spans="1:60">
       <c r="A18">
         <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C18" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D18" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E18" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F18" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="G18">
         <v>600</v>
       </c>
       <c r="H18" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I18">
         <v>3</v>
@@ -1987,43 +2133,43 @@
       <c r="S18">
         <v>10</v>
       </c>
-      <c r="AS18">
+      <c r="AT18">
         <v>25000</v>
       </c>
-      <c r="AT18">
+      <c r="AU18">
         <v>1000</v>
       </c>
-      <c r="AU18">
+      <c r="AV18">
         <v>75000000</v>
       </c>
-      <c r="AV18">
+      <c r="AW18">
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:58">
+    <row r="19" spans="1:60">
       <c r="A19">
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C19" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D19" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E19" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F19" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G19">
         <v>1000</v>
       </c>
       <c r="J19" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="K19">
         <v>400</v>
@@ -2041,124 +2187,124 @@
         <v>30</v>
       </c>
       <c r="W19" t="s">
-        <v>169</v>
-      </c>
-      <c r="AK19">
+        <v>171</v>
+      </c>
+      <c r="AL19">
         <v>6000</v>
       </c>
-      <c r="AS19">
+      <c r="AT19">
         <v>50000</v>
       </c>
-      <c r="AT19">
+      <c r="AU19">
         <v>5000</v>
       </c>
-      <c r="AU19">
+      <c r="AV19">
         <v>2000000000</v>
       </c>
-      <c r="AV19">
+      <c r="AW19">
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="1:58">
+    <row r="20" spans="1:60">
       <c r="A20">
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C20" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D20" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E20" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F20" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G20">
         <v>1500</v>
       </c>
       <c r="T20" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="U20">
         <v>2</v>
       </c>
       <c r="V20" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="X20" t="s">
-        <v>175</v>
-      </c>
-      <c r="AK20">
+        <v>177</v>
+      </c>
+      <c r="AL20">
         <v>7000</v>
       </c>
-      <c r="AU20">
+      <c r="AV20">
         <v>2000000000</v>
       </c>
-      <c r="AV20">
+      <c r="AW20">
         <v>1000</v>
       </c>
     </row>
-    <row r="21" spans="1:58">
+    <row r="21" spans="1:60">
       <c r="A21">
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C21" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D21" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E21" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F21" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="G21">
         <v>2000</v>
       </c>
       <c r="W21" t="s">
-        <v>180</v>
-      </c>
-      <c r="AU21">
+        <v>182</v>
+      </c>
+      <c r="AV21">
         <v>2000000000</v>
       </c>
-      <c r="AV21">
+      <c r="AW21">
         <v>1000</v>
       </c>
     </row>
-    <row r="22" spans="1:58">
+    <row r="22" spans="1:60">
       <c r="A22">
         <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C22" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D22" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E22" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F22" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="G22">
         <v>2500</v>
       </c>
       <c r="H22" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I22">
         <v>50</v>
@@ -2170,301 +2316,617 @@
         <v>50</v>
       </c>
       <c r="T22" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="U22">
         <v>5</v>
       </c>
-      <c r="AC22">
+      <c r="AD22">
         <v>100</v>
       </c>
-      <c r="AD22">
+      <c r="AE22">
         <v>2</v>
       </c>
-      <c r="AF22">
+      <c r="AG22">
         <v>20000</v>
       </c>
-      <c r="AG22" t="s">
-        <v>149</v>
-      </c>
-      <c r="AH22">
+      <c r="AH22" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI22">
         <v>5</v>
       </c>
-      <c r="AS22">
+      <c r="AT22">
         <v>20000</v>
       </c>
-      <c r="AT22">
+      <c r="AU22">
         <v>2000</v>
       </c>
-      <c r="AU22">
+      <c r="AV22">
         <v>5000000000</v>
       </c>
-      <c r="AV22">
+      <c r="AW22">
         <v>1500</v>
       </c>
     </row>
-    <row r="23" spans="1:58">
+    <row r="23" spans="1:60">
       <c r="A23">
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C23" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D23" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E23" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="F23" t="s">
-        <v>189</v>
-      </c>
-      <c r="AU23">
+        <v>191</v>
+      </c>
+      <c r="AV23">
         <v>100000</v>
       </c>
-      <c r="AV23">
+      <c r="AW23">
         <v>50</v>
       </c>
-      <c r="AY23">
+      <c r="AZ23">
         <v>25</v>
       </c>
-      <c r="BA23">
+      <c r="BB23">
         <v>4</v>
       </c>
-      <c r="BC23" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="24" spans="1:58">
+      <c r="BD23" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="24" spans="1:60">
       <c r="A24">
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C24" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D24" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="E24" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="F24" t="s">
-        <v>195</v>
-      </c>
-      <c r="AU24">
+        <v>197</v>
+      </c>
+      <c r="AV24">
         <v>100000</v>
       </c>
-      <c r="AV24">
+      <c r="AW24">
         <v>75</v>
       </c>
-      <c r="AW24" t="s">
-        <v>185</v>
-      </c>
-      <c r="AY24">
+      <c r="AX24" t="s">
+        <v>187</v>
+      </c>
+      <c r="AZ24">
         <v>25</v>
       </c>
-      <c r="BA24">
+      <c r="BB24">
         <v>4</v>
       </c>
-      <c r="BD24">
+      <c r="BE24">
         <v>1000</v>
       </c>
     </row>
-    <row r="25" spans="1:58">
+    <row r="25" spans="1:60">
       <c r="A25">
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C25" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D25" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E25" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F25" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="W25" t="s">
-        <v>200</v>
-      </c>
-      <c r="AS25">
-        <v>5000</v>
+        <v>202</v>
       </c>
       <c r="AT25">
         <v>5000</v>
       </c>
       <c r="AU25">
+        <v>5000</v>
+      </c>
+      <c r="AV25">
         <v>100000</v>
       </c>
-      <c r="AV25">
+      <c r="AW25">
         <v>100</v>
       </c>
-      <c r="AW25" t="s">
-        <v>185</v>
-      </c>
-      <c r="AY25">
+      <c r="AX25" t="s">
+        <v>187</v>
+      </c>
+      <c r="AZ25">
         <v>25</v>
       </c>
-      <c r="BA25">
+      <c r="BB25">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:58">
+    <row r="26" spans="1:60">
       <c r="A26">
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C26" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D26" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E26" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="F26" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="W26" t="s">
-        <v>205</v>
-      </c>
-      <c r="AS26">
-        <v>1000</v>
+        <v>207</v>
       </c>
       <c r="AT26">
         <v>1000</v>
       </c>
       <c r="AU26">
+        <v>1000</v>
+      </c>
+      <c r="AV26">
         <v>500000</v>
       </c>
-      <c r="AV26">
+      <c r="AW26">
         <v>100</v>
       </c>
-      <c r="AW26" t="s">
-        <v>196</v>
-      </c>
-      <c r="AY26">
+      <c r="AX26" t="s">
+        <v>198</v>
+      </c>
+      <c r="AZ26">
         <v>25</v>
       </c>
-      <c r="BA26">
+      <c r="BB26">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:58">
+    <row r="27" spans="1:60">
       <c r="A27">
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C27" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D27" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="E27" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="F27" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="W27" t="s">
-        <v>210</v>
-      </c>
-      <c r="AS27">
-        <v>2000</v>
+        <v>212</v>
       </c>
       <c r="AT27">
         <v>2000</v>
       </c>
       <c r="AU27">
+        <v>2000</v>
+      </c>
+      <c r="AV27">
         <v>500000</v>
       </c>
-      <c r="AV27">
+      <c r="AW27">
         <v>100</v>
       </c>
-      <c r="AW27" t="s">
-        <v>185</v>
-      </c>
-      <c r="AY27">
+      <c r="AX27" t="s">
+        <v>187</v>
+      </c>
+      <c r="AZ27">
         <v>25</v>
       </c>
-      <c r="BA27">
+      <c r="BB27">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:58">
+    <row r="28" spans="1:60">
       <c r="A28">
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C28" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D28" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E28" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="F28" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="W28" t="s">
-        <v>216</v>
-      </c>
-      <c r="AD28">
+        <v>218</v>
+      </c>
+      <c r="AE28">
         <v>1</v>
       </c>
-      <c r="AE28">
+      <c r="AF28">
         <v>30</v>
       </c>
-      <c r="AF28">
+      <c r="AG28">
         <v>500</v>
       </c>
-      <c r="AI28" t="s">
-        <v>138</v>
-      </c>
-      <c r="AJ28">
+      <c r="AJ28" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK28">
         <v>1</v>
-      </c>
-      <c r="AS28">
-        <v>1000</v>
       </c>
       <c r="AT28">
         <v>1000</v>
       </c>
       <c r="AU28">
+        <v>1000</v>
+      </c>
+      <c r="AV28">
         <v>1000000</v>
       </c>
-      <c r="AV28">
+      <c r="AW28">
         <v>100</v>
       </c>
-      <c r="AW28" t="s">
-        <v>185</v>
-      </c>
-      <c r="AY28">
+      <c r="AX28" t="s">
+        <v>187</v>
+      </c>
+      <c r="AZ28">
         <v>25</v>
       </c>
-      <c r="BA28">
+      <c r="BB28">
         <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:60">
+      <c r="A29">
+        <v>33</v>
+      </c>
+      <c r="B29" t="s">
+        <v>219</v>
+      </c>
+      <c r="C29" t="s">
+        <v>220</v>
+      </c>
+      <c r="D29" t="s">
+        <v>221</v>
+      </c>
+      <c r="E29" t="s">
+        <v>222</v>
+      </c>
+      <c r="F29" t="s">
+        <v>222</v>
+      </c>
+      <c r="V29" t="s">
+        <v>223</v>
+      </c>
+      <c r="W29" t="s">
+        <v>224</v>
+      </c>
+      <c r="X29" t="s">
+        <v>225</v>
+      </c>
+      <c r="AT29">
+        <v>25000</v>
+      </c>
+      <c r="AU29">
+        <v>3000</v>
+      </c>
+      <c r="AV29">
+        <v>8000000000</v>
+      </c>
+      <c r="AW29">
+        <v>2000</v>
+      </c>
+      <c r="BD29" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="30" spans="1:60">
+      <c r="A30">
+        <v>34</v>
+      </c>
+      <c r="B30" t="s">
+        <v>226</v>
+      </c>
+      <c r="C30" t="s">
+        <v>227</v>
+      </c>
+      <c r="D30" t="s">
+        <v>228</v>
+      </c>
+      <c r="E30" t="s">
+        <v>229</v>
+      </c>
+      <c r="F30" t="s">
+        <v>230</v>
+      </c>
+      <c r="T30" t="s">
+        <v>223</v>
+      </c>
+      <c r="U30">
+        <v>2</v>
+      </c>
+      <c r="AT30">
+        <v>25000</v>
+      </c>
+      <c r="AU30">
+        <v>3000</v>
+      </c>
+      <c r="AV30">
+        <v>8000000000</v>
+      </c>
+      <c r="AW30">
+        <v>2000</v>
+      </c>
+      <c r="BH30" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="31" spans="1:60">
+      <c r="A31">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>232</v>
+      </c>
+      <c r="C31" t="s">
+        <v>233</v>
+      </c>
+      <c r="D31" t="s">
+        <v>234</v>
+      </c>
+      <c r="E31" t="s">
+        <v>235</v>
+      </c>
+      <c r="F31" t="s">
+        <v>236</v>
+      </c>
+      <c r="T31" t="s">
+        <v>223</v>
+      </c>
+      <c r="U31">
+        <v>5</v>
+      </c>
+      <c r="AT31">
+        <v>25000</v>
+      </c>
+      <c r="AU31">
+        <v>3000</v>
+      </c>
+      <c r="AV31">
+        <v>8000000000</v>
+      </c>
+      <c r="AW31">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:60">
+      <c r="A32">
+        <v>36</v>
+      </c>
+      <c r="B32" t="s">
+        <v>237</v>
+      </c>
+      <c r="C32" t="s">
+        <v>238</v>
+      </c>
+      <c r="D32" t="s">
+        <v>239</v>
+      </c>
+      <c r="E32" t="s">
+        <v>240</v>
+      </c>
+      <c r="F32" t="s">
+        <v>240</v>
+      </c>
+      <c r="V32" t="s">
+        <v>241</v>
+      </c>
+      <c r="W32" t="s">
+        <v>242</v>
+      </c>
+      <c r="AT32">
+        <v>25000</v>
+      </c>
+      <c r="AU32">
+        <v>3000</v>
+      </c>
+      <c r="AV32">
+        <v>8000000000</v>
+      </c>
+      <c r="AW32">
+        <v>2000</v>
+      </c>
+      <c r="BD32" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="33" spans="1:60">
+      <c r="A33">
+        <v>37</v>
+      </c>
+      <c r="B33" t="s">
+        <v>243</v>
+      </c>
+      <c r="C33" t="s">
+        <v>244</v>
+      </c>
+      <c r="D33" t="s">
+        <v>245</v>
+      </c>
+      <c r="E33" t="s">
+        <v>246</v>
+      </c>
+      <c r="F33" t="s">
+        <v>246</v>
+      </c>
+      <c r="H33" t="s">
+        <v>166</v>
+      </c>
+      <c r="I33">
+        <v>200</v>
+      </c>
+      <c r="AT33">
+        <v>25000</v>
+      </c>
+      <c r="AU33">
+        <v>3000</v>
+      </c>
+      <c r="AV33">
+        <v>8000000000</v>
+      </c>
+      <c r="AW33">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:60">
+      <c r="A34">
+        <v>38</v>
+      </c>
+      <c r="B34" t="s">
+        <v>247</v>
+      </c>
+      <c r="C34" t="s">
+        <v>248</v>
+      </c>
+      <c r="D34" t="s">
+        <v>249</v>
+      </c>
+      <c r="E34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F34" t="s">
+        <v>251</v>
+      </c>
+      <c r="W34" t="s">
+        <v>252</v>
+      </c>
+      <c r="AC34">
+        <v>5000</v>
+      </c>
+      <c r="AT34">
+        <v>50000</v>
+      </c>
+      <c r="AU34">
+        <v>6000</v>
+      </c>
+      <c r="AV34">
+        <v>12000000000</v>
+      </c>
+      <c r="AW34">
+        <v>5000</v>
+      </c>
+      <c r="BF34">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:60">
+      <c r="A35">
+        <v>39</v>
+      </c>
+      <c r="B35" t="s">
+        <v>253</v>
+      </c>
+      <c r="C35" t="s">
+        <v>254</v>
+      </c>
+      <c r="D35" t="s">
+        <v>255</v>
+      </c>
+      <c r="E35" t="s">
+        <v>256</v>
+      </c>
+      <c r="F35" t="s">
+        <v>256</v>
+      </c>
+      <c r="AT35">
+        <v>50000</v>
+      </c>
+      <c r="AU35">
+        <v>6000</v>
+      </c>
+      <c r="AV35">
+        <v>12000000000</v>
+      </c>
+      <c r="AW35">
+        <v>5000</v>
+      </c>
+      <c r="BH35" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="36" spans="1:60">
+      <c r="A36">
+        <v>40</v>
+      </c>
+      <c r="B36" t="s">
+        <v>258</v>
+      </c>
+      <c r="C36" t="s">
+        <v>259</v>
+      </c>
+      <c r="D36" t="s">
+        <v>260</v>
+      </c>
+      <c r="E36" t="s">
+        <v>261</v>
+      </c>
+      <c r="F36" t="s">
+        <v>262</v>
+      </c>
+      <c r="L36">
+        <v>15</v>
+      </c>
+      <c r="M36">
+        <v>25</v>
+      </c>
+      <c r="AT36">
+        <v>100000</v>
+      </c>
+      <c r="AU36">
+        <v>12000</v>
+      </c>
+      <c r="AV36">
+        <v>16000000000</v>
+      </c>
+      <c r="AW36">
+        <v>8000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the guide quests, factions now need to be manually earned and info sections have been updated.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -212,13 +212,13 @@
     <t>You managed to slaughter the creatures and make your way forward to a small ramshackle town. The buildings are falling apart, the houses seem empty and lifeless. There is however a small INN before you, the roof looks like it could cave in at any moment. The lawn before it is overgrown with weeds and patches of dead grass where people and their pets have relieved themselves.&lt;br /&gt; &lt;br /&gt; You enter the INN and sit at an empty table by the fire. The barmaid, a heavy set women with an apron around her waist walks over and asks what she can get you. You tell her you are looking for a man who calls him self The Guide. She states she has never heard of such a person and tells you she will be back with the drink and food.&lt;br /&gt; &lt;br /&gt; You sit alone wondering what to do now.</t>
   </si>
   <si>
-    <t>&lt;p&gt;I want you to get to level 10. I do not want you to do this manually. Instead we are going to &lt;a href="/information/automation" target="_blank"&gt;explore&lt;/a&gt; for an hour. During this time you may gain a Faction level for Surface. The &lt;a href="/information/planes" target="_blank"&gt;map&lt;/a&gt; you are currently on.&lt;/p&gt;&lt;p&gt;&lt;a href="/information/factions" target="_blank"&gt;Factions&lt;/a&gt; can be seen on your character sheet (tab) under the tab: Factions. As you kill creatures you gain faction points. As you level the faction, you can get what are called &lt;a href="/information/random-enchants" target="_blank"&gt;Unique’s&lt;/a&gt;. These can be powerful items and you may only have one equipped at a time.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; For mobile players Factions will be on the character sheet tab in the closed top section which you can expand by clicking the blue cross in the top right.&lt;/p&gt;&lt;p&gt;Exploring will allow you to log out and idly gain items, exp, gold and possible quest item if the monster drops a quest item. There are things you cannot do while exploring such as change equipment, buy items from the &lt;a href="/information/shop" target="_blank"&gt;shop&lt;/a&gt; or &lt;a href="/information/market-board" target="_blank"&gt;market board&lt;/a&gt;. You will be told if you can do an action or not while exploring. Exploring should not just be used to level and log out, you &lt;a href="/information/some-clicking-required" target="_blank"&gt;won't get very far&lt;/a&gt; if you do that, there is much more to do and we will do it very soon! exploration is a way of gaining levels while doing other things in game.&lt;/p&gt;&lt;p&gt;Exploration messages will appear, while logged in, in the Exploration chat tab below.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- First lets investigate the gear we have been given.&lt;/p&gt;&lt;p&gt;We can do this by going to the character sheet tab and on the bottom right is the inventory management. You can click item names here to investigate, equip and do other types of actions with the item. For now if you find gear that raises your stats (IE, STR Modifier +x%) equip it.&lt;/p&gt;&lt;p&gt;You may also need to visit the shop, which you can do by clicking the top left Hamburger menu to open the menu and select Shop. From here select Buy under General Shop. here you can buy gear, buy multiple pieces of gear or even compare and equip gear (auto purchase/equip).&lt;/p&gt;&lt;p&gt;- Next go back to the drop down for monsters and select a stronger monster and click Attack&lt;/p&gt;&lt;p&gt;- Select Attack and if you can kill it in one hit, which is ideal, move down the list to the next, rinse and repeat till you cannot move any further.&lt;/p&gt;&lt;p&gt;- Now that we have a monster, click Explore to the left of the attack section.&lt;/p&gt;&lt;p&gt;- Select the same monster, select 1 hour, ignore the move down and then select Attack, click Explore.&lt;/p&gt;&lt;p&gt;This will run a set of battles every 5 minutes for 1 hour where you can fight between 1-8 enemies back to back. The reason we ignored the move down aspect is because it allows you to state: Move down the list every x levels that I gain, and for now we do not want that.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- First lets investigate the gear we have been given.&lt;/p&gt;&lt;p&gt;We can now this by going to the character sheet, and from the drop down select Inventory Management. Now we can see all out gear we found - which might not be much, but we can filter through and look for Stat Raising gear, IE: STR Modifier +X%.&lt;/p&gt;&lt;p&gt;You may also need to visit the shop, which you can do by clicking the top left Hamburger menu to open the menu and select Shop. From here select Buy under General Shop. here you can buy gear, buy multiple pieces of gear or even compare and equip gear (auto purchase/equip).&lt;/p&gt;&lt;p&gt;Now that we have some gear lets go back to the game section and select:&lt;/p&gt;&lt;p&gt;- Fight from the action drop down&lt;/p&gt;&lt;p&gt;- Select a harder monster to fight, click Attack and if you kill it in one hit, move down the list.&lt;/p&gt;&lt;p&gt;- Repeat till you either die or find a monster you cannot kill in one hit, then move back to the one you could before.&lt;/p&gt;&lt;p&gt;- Close the fight section, select Exploration.&lt;/p&gt;&lt;p&gt;- Select the same monster, select 1 hour, ignore the move down and then select Attack, click Explore.&lt;/p&gt;&lt;p&gt;This will run a set of battles every 5 minutes for 1 hour where you can fight between 1-8 enemies back to back. The reason we ignored the move down aspect is because it allows you to state: Move down the list every x levels that I gain, and for now we do not want that.&lt;/p&gt;</t>
+    <t>&lt;p&gt;I want you to learn about &lt;a href="/information/exploration" target="_blank"&gt;exploration&lt;/a&gt; – which allows you to automate the battle process of fighting but also has some draw backs.&lt;/p&gt;&lt;p&gt;Exploration allows you to log out of the game and still fight monsters, gain items, gain currencies and – most importantly – gain levels.&lt;/p&gt;&lt;p&gt;Exploration can be amazing while you &lt;a href="/information/crafting" target="_blank"&gt;craft&lt;/a&gt;, or if you have to step out – or go to work. However, there is a draw back: Exploration will not allow you to change your equipment, set sail from one port to another, teleport (You can still move) and a few other actions.&lt;/p&gt;&lt;p&gt;The down side to exploration is that some areas wont drop quest items, some places that give out bonus currencies and items geared towards mid and end game wont give out those bonus currencies and items.&lt;/p&gt;&lt;p&gt;And lastly, the sole part of this quest is that you cannot earn &lt;a href="/information/factions" target="_blank"&gt;Faction&lt;/a&gt; Points.&lt;/p&gt;&lt;p&gt;Faction Points allow you to gain &lt;a href="/information/random-enchants" target="_blank"&gt;unique items&lt;/a&gt; – which at first are weaker then ones you can earn later on – but are great to get you going.&lt;/p&gt;&lt;p&gt;Faction points can be seen on your character sheet. Once a player reaches level 5 in a given faction they can then pledge to it. We will discuss that later. Right now, to earn faction points – all you have to do is kill anything you want on the plane the faction is named after.&lt;/p&gt;&lt;p&gt;For this quest we will kill any creature we can on Surface to earn points to level the Faction to the required level. You will earn 50 points per kill from level 0 to 1 and the 75 points from level 1 to 5 per kill.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;- First lets investigate the gear we have been given.&lt;/p&gt;&lt;p&gt;We can do this by going to the character sheet tab and on the bottom right is the inventory management. You can click item names here to investigate, equip and do other types of actions with the item. For now if you find gear that raises your stats (IE, STR Modifier +x%) equip it.&lt;/p&gt;&lt;p&gt;You may also need to visit the shop, which you can do by clicking the top left Hamburger menu to open the menu and select Shop. From here select Buy under General Shop. here you can buy gear, buy multiple pieces of gear or even compare and equip gear (auto purchase/equip).&lt;/p&gt;&lt;p&gt;&lt;strong&gt;How to explore:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Next go back to the drop down for monsters and select a stronger monster and click Attack if you can kill it in one hit, which is ideal, move down the list to the next, rinse and repeat till you cannot move any further.&lt;/p&gt;&lt;p&gt;- Now that we have a monster, click Explore to the left of the attack section.&lt;/p&gt;&lt;p&gt;- Select the same monster, select 1 hour, ignore the move down and then select Attack, click Explore.&lt;/p&gt;&lt;p&gt;You will see your Exploration chat tab update – within 5 minutes both your exploration and server messages tab will update, one with info about your exploration including bonus faction points and how many creatures you kill, while the other – server messages – will show you the items you got, the currencies and so on.&lt;/p&gt;&lt;p&gt;Whats amazing about this is you can now sign out and be on your way and come back later to all your items, but why do that when we can earn some Factions and save exploration for when were ready to “just train.”&lt;/p&gt;&lt;p&gt;&lt;strong&gt;To earn Faction Points first:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Select a monster you can ideally kill in one hit and slaughter it. Do this about 10 times.&lt;/p&gt;&lt;p&gt;- Now to see that we gained some points, head over your character sheet and click the Factions tab in the card which is I the top left section of the sheet.&lt;/p&gt;&lt;p&gt;- Surface should be level 1 at this point. If you check your inventory you should have a green item. Investigate this – possibly equip it.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;First lets investigate the gear we have been given.&lt;/p&gt;&lt;p&gt;We can now this by going to the character sheet, and from the drop down select Inventory Management. Now we can see all out gear we found - which might not be much, but we can filter through and look for Stat Raising gear, IE: STR Modifier +X%.&lt;/p&gt;&lt;p&gt;You may also need to visit the shop, which you can do by clicking the top left Hamburger menu to open the menu and select Shop. From here select Buy under General Shop. here you can buy gear, buy multiple pieces of gear or even compare and equip gear (auto purchase/equip).&lt;/p&gt;&lt;p&gt;&lt;strong&gt;How to explore:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;-In the actions drop down, select Fight and select a monster you can kill it in one hit, which is ideal, move down the list to the next, rinse and repeat till you cannot move any further.&lt;/p&gt;&lt;p&gt;- Now that we have a monster, select Exploration fro the action drop down.&lt;/p&gt;&lt;p&gt;- Select the monster you could kill, select 1 hour for time – do not select anything for moving down the monster list every x levels and click explore.&lt;/p&gt;&lt;p&gt;- Tap Attack to begin. In five minutes the exploration chat tab and server message tab will update&lt;/p&gt;&lt;p&gt;You will see your Exploration chat tab update – within 5 minutes both your exploration and server messages tab will update, one with info about your exploration including bonus faction points and how many creatures you kill, while the other – server messages – will show you the items you got, the currencies and so on.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;To access this info, select exploration or server messages from the chat tab drop down under the actions section.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Whats amazing about this is you can now sign out and be on your way and come back later to all your items, but why do that when we can earn some Factions and save exploration for when were ready to “just train.”&lt;/p&gt;&lt;p&gt;T&lt;strong&gt;o earn Faction Points first:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- While exploration is not running, select attack from the actions drop down.&lt;/p&gt;&lt;p&gt;- Select a monster you can ideally kill in one hit and slaughter it. Do this about 10 times.&lt;/p&gt;&lt;p&gt;- Now to see that we gained some points, head over your character sheet and expand the top section, next tap the Factions tab.&lt;/p&gt;&lt;p&gt;- Surface should be level 1 at this point. If you check your inventory you should have a green item. Investigate this – possibly equip it.&lt;/p&gt;</t>
   </si>
   <si>
     <t>The Letter</t>
@@ -1176,8 +1176,8 @@
     <col min="2" max="2" width="54.13" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="1886.254" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="2760.469" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="2355.71" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="2395.844" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="2468.969" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="2786.32" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="18.71" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="24.708" bestFit="true" customWidth="true" style="0"/>

</xml_diff>

<commit_message>
Started fixing the text for guide quests. The first 10 are done.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -194,10 +194,10 @@
     <t>Welcome to Tlessa</t>
   </si>
   <si>
-    <t>You have been walking for days, You left your home in search of adventure. You left your mother and father to tend to the farm. You carry with you the memories of running through the fields as a small child, the sun’s warmth slowly browning your skin as you played with your friends in the local pond that everyone swam in on the hot days.&lt;br /&gt; &lt;br /&gt; Now you are standing on a path before you, with ravaging creatures. Foul beasts before you. It’s time to fight, to survive, to conquer.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;I want you to get your self to level 2. For this you will gain an additional 10XP per kill (until you reach level 2). It will take roughly ten kills (maybe less) to achieve this goal.&lt;/p&gt;&lt;p&gt;To do this:&lt;/p&gt;&lt;p&gt;There are various &lt;a href="/information/combat" target="_blank"&gt;attacks&lt;/a&gt;, as you will see – when fighting a monster:&lt;/p&gt;&lt;p&gt;- Attack (uses both weapons equipped)&lt;/p&gt;&lt;p&gt;- Cast (Uses both spells equipped)&lt;/p&gt;&lt;p&gt;- Cast and Attack (Uses spell in spell slot 1 and right handed weapon)&lt;/p&gt;&lt;p&gt;- Attack and Cast (uses spell in spell slot 2 and left handed weapon)&lt;/p&gt;&lt;p&gt;- Defend (Uses your shields and armour to defend)&lt;/p&gt;&lt;p&gt;For now, focus on using attack. Later on when you are more established, your &lt;a href="/information/races-and-classes#3" target="_blank"&gt;class&lt;/a&gt; will determine the type of attack you select, for example Heretics love Cast, while Prophets love Cast and Attack (or attack and Cast)&lt;/p&gt;</t>
+    <t>You have been walking for days. You left your home in search of adventure, leaving your mother and father to tend to the farm. Carrying with you the memories of running through the fields as a small child, the sun's warmth slowly browning your skin as you played with your friends in the local pond that everyone swam in on hot days.&lt;br /&gt; &lt;br /&gt; Now, you stand on a path with ravaging creatures, foul beasts before you. It's time to fight, to survive, to conquer.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;I want you to get yourself to level 2. For this, you will gain an additional 10XP per kill (until you reach level 2). It will take roughly ten kills (maybe less) to achieve this goal.&lt;/p&gt;&lt;p&gt;To do this:&lt;/p&gt;&lt;p&gt;There are various &lt;a href="/information/combat" target="_blank"&gt;attacks&lt;/a&gt;, as you will see when fighting a monster:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Attack (uses both weapons equipped)&lt;/li&gt;&lt;li&gt;Cast (Uses both spells equipped)&lt;/li&gt;&lt;li&gt;Cast and Attack (Uses the spell in spell slot 1 and the right-handed weapon)&lt;/li&gt;&lt;li&gt;Attack and Cast (uses the spell in spell slot 2 and the left-handed weapon)&lt;/li&gt;&lt;li&gt;Defend (Uses your shields and armor to defend)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;For now, focus on using the attack. Later on, when you are more established, your class will determine the type of attack you select. For example, Heretics love Cast, while Prophets love Cast and Attack (or Attack and Cast).&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;- Select a monster from the list behind this modal (start with Sewer Rat and work your way down)&lt;/p&gt;&lt;p&gt;- Click the attack button.&lt;/p&gt;&lt;p&gt;- Click the first attack button.&lt;/p&gt;&lt;p&gt;- Repeat until level 2.&lt;/p&gt;</t>
@@ -209,16 +209,16 @@
     <t>Exploring the town</t>
   </si>
   <si>
-    <t>You managed to slaughter the creatures and make your way forward to a small ramshackle town. The buildings are falling apart, the houses seem empty and lifeless. There is however a small INN before you, the roof looks like it could cave in at any moment. The lawn before it is overgrown with weeds and patches of dead grass where people and their pets have relieved themselves.&lt;br /&gt; &lt;br /&gt; You enter the INN and sit at an empty table by the fire. The barmaid, a heavy set women with an apron around her waist walks over and asks what she can get you. You tell her you are looking for a man who calls him self The Guide. She states she has never heard of such a person and tells you she will be back with the drink and food.&lt;br /&gt; &lt;br /&gt; You sit alone wondering what to do now.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;I want you to learn about &lt;a href="/information/exploration" target="_blank"&gt;exploration&lt;/a&gt; – which allows you to automate the battle process of fighting but also has some draw backs.&lt;/p&gt;&lt;p&gt;Exploration allows you to log out of the game and still fight monsters, gain items, gain currencies and – most importantly – gain levels.&lt;/p&gt;&lt;p&gt;Exploration can be amazing while you &lt;a href="/information/crafting" target="_blank"&gt;craft&lt;/a&gt;, or if you have to step out – or go to work. However, there is a draw back: Exploration will not allow you to change your equipment, set sail from one port to another, teleport (You can still move) and a few other actions.&lt;/p&gt;&lt;p&gt;The down side to exploration is that some areas wont drop quest items, some places that give out bonus currencies and items geared towards mid and end game wont give out those bonus currencies and items.&lt;/p&gt;&lt;p&gt;And lastly, the sole part of this quest is that you cannot earn &lt;a href="/information/factions" target="_blank"&gt;Faction&lt;/a&gt; Points.&lt;/p&gt;&lt;p&gt;Faction Points allow you to gain &lt;a href="/information/random-enchants" target="_blank"&gt;unique items&lt;/a&gt; – which at first are weaker then ones you can earn later on – but are great to get you going.&lt;/p&gt;&lt;p&gt;Faction points can be seen on your character sheet. Once a player reaches level 5 in a given faction they can then pledge to it. We will discuss that later. Right now, to earn faction points – all you have to do is kill anything you want on the plane the faction is named after.&lt;/p&gt;&lt;p&gt;For this quest we will kill any creature we can on Surface to earn points to level the Faction to the required level. You will earn 50 points per kill from level 0 to 1 and the 75 points from level 1 to 5 per kill.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- First lets investigate the gear we have been given.&lt;/p&gt;&lt;p&gt;We can do this by going to the character sheet tab and on the bottom right is the inventory management. You can click item names here to investigate, equip and do other types of actions with the item. For now if you find gear that raises your stats (IE, STR Modifier +x%) equip it.&lt;/p&gt;&lt;p&gt;You may also need to visit the shop, which you can do by clicking the top left Hamburger menu to open the menu and select Shop. From here select Buy under General Shop. here you can buy gear, buy multiple pieces of gear or even compare and equip gear (auto purchase/equip).&lt;/p&gt;&lt;p&gt;&lt;strong&gt;How to explore:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Next go back to the drop down for monsters and select a stronger monster and click Attack if you can kill it in one hit, which is ideal, move down the list to the next, rinse and repeat till you cannot move any further.&lt;/p&gt;&lt;p&gt;- Now that we have a monster, click Explore to the left of the attack section.&lt;/p&gt;&lt;p&gt;- Select the same monster, select 1 hour, ignore the move down and then select Attack, click Explore.&lt;/p&gt;&lt;p&gt;You will see your Exploration chat tab update – within 5 minutes both your exploration and server messages tab will update, one with info about your exploration including bonus faction points and how many creatures you kill, while the other – server messages – will show you the items you got, the currencies and so on.&lt;/p&gt;&lt;p&gt;Whats amazing about this is you can now sign out and be on your way and come back later to all your items, but why do that when we can earn some Factions and save exploration for when were ready to “just train.”&lt;/p&gt;&lt;p&gt;&lt;strong&gt;To earn Faction Points first:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Select a monster you can ideally kill in one hit and slaughter it. Do this about ~20 times.&lt;/p&gt;&lt;p&gt;- Now to see that we gained some points, head over your character sheet and click the Factions tab in the card which is I the top left section of the sheet.&lt;/p&gt;&lt;p&gt;- Surface should be level 2 at this point. If you check your inventory you should have a green item. Investigate this – possibly equip it.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;First lets investigate the gear we have been given.&lt;/p&gt;&lt;p&gt;We can now this by going to the character sheet, and from the drop down select Inventory Management. Now we can see all out gear we found - which might not be much, but we can filter through and look for Stat Raising gear, IE: STR Modifier +X%.&lt;/p&gt;&lt;p&gt;You may also need to visit the shop, which you can do by clicking the top left Hamburger menu to open the menu and select Shop. From here select Buy under General Shop. here you can buy gear, buy multiple pieces of gear or even compare and equip gear (auto purchase/equip).&lt;/p&gt;&lt;p&gt;&lt;strong&gt;How to explore:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;-In the actions drop down, select Fight and select a monster you can kill it in one hit, which is ideal, move down the list to the next, rinse and repeat till you cannot move any further.&lt;/p&gt;&lt;p&gt;- Now that we have a monster, select Exploration fro the action drop down.&lt;/p&gt;&lt;p&gt;- Select the monster you could kill, select 1 hour for time – do not select anything for moving down the monster list every x levels and click explore.&lt;/p&gt;&lt;p&gt;- Tap Attack to begin. In five minutes the exploration chat tab and server message tab will update&lt;/p&gt;&lt;p&gt;You will see your Exploration chat tab update – within 5 minutes both your exploration and server messages tab will update, one with info about your exploration including bonus faction points and how many creatures you kill, while the other – server messages – will show you the items you got, the currencies and so on.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;To access this info, select exploration or server messages from the chat tab drop down under the actions section.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Whats amazing about this is you can now sign out and be on your way and come back later to all your items, but why do that when we can earn some Factions and save exploration for when were ready to “just train.”&lt;/p&gt;&lt;p&gt;T&lt;strong&gt;o earn Faction Points first:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- While exploration is not running, select attack from the actions drop down.&lt;/p&gt;&lt;p&gt;- Select a monster you can ideally kill in one hit and slaughter it. Do this about ~20 times.&lt;/p&gt;&lt;p&gt;- Now to see that we gained some points, head over your character sheet and expand the top section, next tap the Factions tab.&lt;/p&gt;&lt;p&gt;- Surface should be level 2 at this point. If you check your inventory you should have a green item. Investigate this – possibly equip it.&lt;/p&gt;</t>
+    <t>You managed to slaughter the creatures and make your way forward to a small ramshackle town. The buildings are falling apart; the houses seem empty and lifeless. However, there is a small INN before you, and the roof looks like it could cave in at any moment. The lawn before it is overgrown with weeds and patches of dead grass where people and their pets have relieved themselves.&lt;br /&gt; &lt;br /&gt; You enter the INN and sit at an empty table by the fire. The barmaid, a heavy-set woman with an apron around her waist, walks over and asks what she can get you. You tell her you are looking for a man who calls himself The Guide. She states &lt;br /&gt; she has never heard of such a person and tells you she will be back with the drink and food.&lt;br /&gt; &lt;br /&gt; You sit alone, wondering what to do now.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;"I want you to learn about &lt;a href="/information/exploration" target="_blank"&gt;exploration&lt;/a&gt; – which allows you to automate the battle process of fighting but also has some drawbacks.&lt;/p&gt;&lt;p&gt;Exploration allows you to log out of the game and still fight monsters, gain items, gain currencies and – most importantly – gain levels.&lt;/p&gt;&lt;p&gt;Exploration can be amazing while you &lt;a href="/information/crafting" target="_blank"&gt;craft&lt;/a&gt;, or if you have to step out – or go to work. However, there is a drawback: Exploration will not allow you to change your equipment, set sail from one port to another, teleport (You can still move) and a few other actions.&lt;/p&gt;&lt;p&gt;The downside to exploration is that some areas won't drop quest items, some places that give out bonus currencies and items geared towards mid and end-game won't give out those bonus currencies and items.&lt;/p&gt;&lt;p&gt;Lastly, the sole part of this quest is that you cannot earn &lt;a href="/information/factions" target="_blank"&gt;Faction&lt;/a&gt; Points.&lt;/p&gt;&lt;p&gt;Faction Points allow you to gain &lt;a href="/information/random-enchants" target="_blank"&gt;unique items&lt;/a&gt; – which at first are weaker than ones you can earn later on – but are great to get you going.&lt;/p&gt;&lt;p&gt;Faction points can be seen on your character sheet. Once a player reaches level 5 in a given faction, they can then pledge to it. We will discuss that later. Right now, to earn faction points – all you have to do is kill anything you want on the plane the faction is named after.&lt;/p&gt;&lt;p&gt;For this quest, we will kill any creature we can on Surface to earn points to level the Faction to the required level. You will earn 50 points per kill from level 0 to 1 and then 75 points from level 1 to 5 per kill.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;First, let's investigate the gear we have been given.&lt;/p&gt;&lt;p&gt;We can do this by going to the character sheet tab, and on the bottom right is the inventory management. You can click item names here to investigate, equip, and do other types of actions with the item. For now, if you find gear that raises your stats (i.e., STR Modifier +x%), equip it.&lt;/p&gt;&lt;p&gt;You may also need to visit the shop, which you can do by clicking the top left Hamburger menu to open the menu and select Shop. From here, select Buy under General Shop. Here you can buy gear, buy multiple pieces of gear, or even compare and equip gear (auto purchase/equip).&lt;/p&gt;&lt;p&gt;&lt;strong&gt;How to explore&lt;/strong&gt;:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Next, go back to the drop-down for monsters and select a stronger monster and click Attack if you can kill it in one hit, which is ideal. Move down the list to the next, rinse and repeat till you cannot move any further.&lt;/li&gt;&lt;li&gt;Now that we have a monster, click Explore to the left of the attack section.&lt;/li&gt;&lt;li&gt;Select the same monster, select 1 hour, ignore the move down, and then select Attack. Click Explore.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;You will see your Exploration chat tab update – within 5 minutes both your exploration and server messages tab will update, one with info about your exploration including bonus faction points and how many creatures you kill, while the other – server messages – will show you the items you got, the currencies, and so on.&lt;/p&gt;&lt;p&gt;What's amazing about this is you can now sign out and be on your way and come back later to all your items, but why do that when we can earn some Factions and save exploration for when we're ready to "just train."&lt;/p&gt;&lt;p&gt;&lt;strong&gt;To earn Faction Points first&lt;/strong&gt;:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Select a monster you can ideally kill in one hit and slaughter it. Do this about ~20 times.&lt;/li&gt;&lt;li&gt;Now to see that we gained some points, head over to your character sheet and click the Factions tab in the card which is in the top left section of the sheet.&lt;/li&gt;&lt;li&gt;Surface should be level 2 at this point. If you check your inventory, you should have a green item. Investigate this – possibly equip it.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;First, let's investigate the gear we have been given.&lt;/p&gt;&lt;p&gt;We can do this by going to the character sheet, and from the drop-down select Inventory Management. Now we can see all our gear we found - which might not be much, but we can filter through and look for Stat Raising gear, i.e., STR Modifier +X%.&lt;/p&gt;&lt;p&gt;You may also need to visit the shop, which you can do by clicking the top left Hamburger menu to open the menu and select Shop. From here select Buy under General Shop. Here you can buy gear, buy multiple pieces of gear or even compare &lt;/p&gt;&lt;p&gt;and equip gear (auto purchase/equip).&lt;/p&gt;&lt;p&gt;&lt;strong&gt;How to explore&lt;/strong&gt;:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;In the actions drop-down, select Fight and select a monster you can kill in one hit, which is ideal, move down the list to the next, rinse and repeat till you cannot move any further.&lt;/li&gt;&lt;li&gt;Now that we have a monster, select Exploration from the action drop-down.&lt;/li&gt;&lt;li&gt;Select the monster you could kill, select 1 hour for time – do not select anything for moving down the monster list every x levels and click explore.&lt;/li&gt;&lt;li&gt;Tap Attack to begin. In five minutes, the exploration chat tab and server message tab will update.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;You will see your Exploration chat tab update – within 5 minutes both your exploration and server messages tab will update, one with info about your exploration including bonus faction points and how many creatures you kill, while the other – server messages – will show you the items you got, the currencies, and so on.&lt;/p&gt;&lt;p&gt;To access this info, select exploration or server messages from the chat tab drop down under the actions section.&lt;/p&gt;&lt;p&gt;What's amazing about this is you can now sign out and be on your way and come back later to all your items, but why do that when we can earn some Factions and save exploration for when we're ready to "just train."&lt;/p&gt;&lt;p&gt;&lt;strong&gt;To earn Faction Points first&lt;/strong&gt;:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;While exploration is not running, select attack from the actions drop-down.&lt;/li&gt;&lt;li&gt;Select a monster you can ideally kill in one hit and slaughter it. Do this about ~20 times.&lt;/li&gt;&lt;li&gt;Now to see that we gained some points, head over to your character sheet and expand the top section, next tap the Factions tab.&lt;/li&gt;&lt;li&gt;Surface should be level 2 at this point. If you check your inventory, you should have a green item. Investigate this – possibly equip it.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>Surface</t>
@@ -227,16 +227,16 @@
     <t>The Letter</t>
   </si>
   <si>
-    <t>You explore, you slaughter, you bathe in the enemies blood before you. You collect the shiny loot. You were gifted a green unique item from the towns people as a way of thanking you for your hard work.&lt;br /&gt; &lt;br /&gt; They told you that there are many other places one could explore, but that you could continue around here gain more favor with the people of the Surface plane.&lt;br /&gt; &lt;br /&gt; You wait for days and then weeks at the INN, where the hell is The Guide?&lt;br /&gt; &lt;br /&gt; “A letter for you” the barmaid states as she drops off your ale. You open it and read the following:&lt;br /&gt; &lt;br /&gt; Child. Listen, I am The Guide, alas I am investigating a situation. There is a magical spell upon your very being that allows the creatures you slaughter to gift you with the bounty of loot you have now, but that won’t last forever.&lt;br /&gt; &lt;br /&gt; You have to learn how to properly loot. You also have to have to learn how to wield your weapon, even casters can get into sticky situations where they need a weapon, and if you can’t hit anything – death will greet you faster then I.&lt;br /&gt; &lt;br /&gt; I also want you to investigate your gear, visit a shop. You gear is what makes you child. Know that.&lt;br /&gt; &lt;br /&gt; -- The Guide&lt;br /&gt; &lt;br /&gt; That’s it? Just barks orders through paper at you? You look around and contemplate doing what he want’s knowing full well you could just bugger off on your own adventure.&lt;br /&gt; &lt;br /&gt; By morning you have made up your mind on what to do.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; &lt;em&gt;This quest can take up to two hours to complete.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;We are going to learn about two things today: &lt;a href="/information/character-stats" target="_blank"&gt;Stats&lt;/a&gt; and &lt;a href="/information/skill-information" target="_blank"&gt;Skills&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;Characters under level 12, get a boost to their looting skill making drops a lot more fun. How ever as you will soon reach level 12 you will see the drop rate disappear. This is where skills come in handy.&lt;/p&gt;&lt;p&gt;At any time, when leveling a skill as you will do here, you may click on the skill name to see applicable bonuses, XP, level and so on, The Skill Bonus refers to the bonus the skill applies when using it, such as for Accuracy or Looting.&lt;/p&gt;&lt;p&gt;Because you will be utilizing exploration to do this next part, you cannot switch skills in the middle of an exploration, you can stop exploration, switch to another skill and then resume your exploration.&lt;/p&gt;&lt;p&gt;Later on, and maybe even the gear you have found, you will see &lt;a href="/information/enchanting" target="_blank"&gt;enchantments&lt;/a&gt; with skill modifiers on them.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- Click the Character Sheet tab&lt;/p&gt;&lt;p&gt;- Scroll down to skills.&lt;/p&gt;&lt;p&gt;- Find Accuracy, click train, select 10% of your XP and train the skill.&lt;/p&gt;&lt;p&gt;Follow these same steps to train Looting after clicking Stop training on Accuracy.&lt;/p&gt;&lt;p&gt;If the gear you have found is not raising your stats to the required amount, try visiting the &lt;a href="/information/shop" target="_blank"&gt;shop&lt;/a&gt; and purchasing better gear. It might not be enchanted but the % for stats that it raises, which stack, might be better then what you have on.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- Tap the Character Sheet tab.&lt;/p&gt;&lt;p&gt;- Select Manage Skills&lt;/p&gt;&lt;p&gt;- Tap Train on the Accuracy Skill&lt;/p&gt;&lt;p&gt;- Select 10% of your XP and train the skill&lt;/p&gt;&lt;p&gt;Follow these same steps to train Looting after clicking Stop training on Accuracy.&lt;/p&gt;&lt;p&gt;If the gear you have found is not raising your stats to the required amount, try visiting the &lt;a href="http://127.0.0.1:8000/information/shop" target="_blank"&gt;shop&lt;/a&gt; and purchasing better gear. It might not be enchanted but the % for stats that it raises, which stack, might be better then what you have on.&lt;/p&gt;</t>
+    <t>You explore, slaughter, and bathe in the enemies' blood before you. You collect shiny loot and receive a green unique item from the townspeople as a way of thanking you for your hard work.&lt;br /&gt; &lt;br /&gt; They inform you that many other places could be explored, but you could continue around here to gain more favor with the people of the Surface plane.&lt;br /&gt; &lt;br /&gt; You wait for days and then weeks at the INN. Where the hell is The Guide?&lt;br /&gt; &lt;br /&gt; "A letter for you," the barmaid states as she drops off your ale. You open it and read the following:&lt;br /&gt; &lt;br /&gt; "Child, listen. I am The Guide. Alas, I am investigating a situation. There is a magical spell upon your very being that allows the creatures you slaughter to gift you with the bounty of loot you have now, but that won’t last forever.&lt;br /&gt; &lt;br /&gt; You have to learn how to properly loot. You also have to learn how to wield your weapon; even casters can get into sticky situations where they need a weapon, and if you can’t hit anything – death will greet you faster than I.&lt;br /&gt; &lt;br /&gt; I also want you to investigate your gear, visit a shop. Your gear is what makes you, child. Know that."&lt;br /&gt; &lt;br /&gt; -- The Guide&lt;br /&gt; &lt;br /&gt; That’s it? Just barks orders through paper at you? You look around and contemplate doing what he wants, knowing full well you could just bugger off on your adventure.&lt;br /&gt; &lt;br /&gt; By morning, you have made up your mind on what to do.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Note: This quest can take up to two hours to complete.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;We are going to learn about two things today: &lt;a href="/information/character-stats" target="_blank"&gt;Stats&lt;/a&gt; and &lt;a href="/information/skill-information" target="_blank"&gt;Skills&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;Characters under level 12 get a boost to their looting skill, making drops a lot more fun. However, as you will soon reach level 12, you will see the drop rate disappear. This is where skills come in handy.&lt;/p&gt;&lt;p&gt;At any time, when leveling a skill as you will do here, you may click on the skill name to see applicable bonuses, XP, level, and so on. The Skill Bonus refers to the bonus the skill applies when using it, such as for Accuracy or Looting.&lt;/p&gt;&lt;p&gt;Because you will be utilizing exploration to do this next part, you cannot switch skills in the middle of an exploration; you can stop exploration, switch to another skill, and then resume your exploration.&lt;/p&gt;&lt;p&gt;Later on, and maybe even with the gear you have found, you will see &lt;a href="/information/enchanting" target="_blank"&gt;enchantments&lt;/a&gt; with skill modifiers on them.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Click the Character Sheet tab&lt;/li&gt;&lt;li&gt;Scroll down to skills.&lt;/li&gt;&lt;li&gt;Find Accuracy, click train, select 10% of your XP, and train the skill.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Follow these same steps to train Looting after clicking Stop training on Accuracy.&lt;/p&gt;&lt;p&gt;If the gear you have found is not raising your stats to the required amount, try visiting the &lt;a href="/information/shop" target="_blank"&gt;shop&lt;/a&gt; and purchasing better gear. It might not be enchanted, but the % for stats that it raises, which stack, might be better than what you have on.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Tap the Character Sheet tab.&lt;/li&gt;&lt;li&gt;Select Manage Skills&lt;/li&gt;&lt;li&gt;Tap Train on the Accuracy Skill&lt;/li&gt;&lt;li&gt;Select 10% of your XP and train the skill&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Follow these same steps to train Looting after clicking Stop training on Accuracy.&lt;/p&gt;&lt;p&gt;If the gear you have found is not raising your stats to the required amount, try visiting the &lt;a href="/information/shop" target="_blank"&gt;shop&lt;/a&gt; and purchasing better gear. It might not be enchanted, but the % for stats that it raises, which stack, might be better than what you have on.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Accuracy</t>
@@ -248,16 +248,16 @@
     <t>Blacksmiths Life</t>
   </si>
   <si>
-    <t>Sitting in the INN, you stare into the large fire place with the wood burning and the smell of the old oak as it burns. It’s almost as if time stops for a moment and you can gather your thoughts.&lt;br /&gt; &lt;br /&gt; All you do is slaughter creatures, gather loot and slowly get better at hitting the enemies and even slightly faster.&lt;br /&gt; &lt;br /&gt; The flames of the fire seem to stand still, the smell of the fire has dissipated from the air. You look around and no one is moving, like they have been frozen in time.&lt;br /&gt; &lt;br /&gt; You turn back to the fire and see a young man, about twenty-five standing before the fire, his back to you. You call out to him, and he doesn’t turn around but he does speak.&lt;br /&gt; &lt;br /&gt; “Child. I have found something most mysterious. The gates have opened.”&lt;br /&gt; &lt;br /&gt; The gates? What gates?&lt;br /&gt; &lt;br /&gt; “Listen to me child.” The young man turns and faces you.&lt;br /&gt; &lt;br /&gt; “I need you to speak with the local blacksmith, work with him for a while. Train a different set of skills. Important skills. I need you to craft your own gear.”&lt;br /&gt; &lt;br /&gt; You tell him that the gear you have found, the stuff you can buy from the local blacksmith is better then what you can craft.&lt;br /&gt; &lt;br /&gt; “True, however, you can craft even more powerful gear then that of which you can buy.”&lt;br /&gt; &lt;br /&gt; Before you can ask further questions the flames returning to their burning motion, the wood crackles, the INN is full of voices again and the smell of food fills the air.&lt;br /&gt; &lt;br /&gt; Where did he go?</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; &lt;em&gt;This quest can take 2+ hours to complete. It is suggested you explore and craft at the same time.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Today lets learn how to &lt;a href="/information/crafting" target="_blank"&gt;craft&lt;/a&gt; weapons and armour. You can also craft other things like spells, rings, trinkets and alchemy.&lt;/p&gt;&lt;p&gt;Crafting is wildly important because the &lt;a href="/information/shop" target="_blank"&gt;shop&lt;/a&gt; will only take you so far. For example, later in the game you can get gear sets: &lt;a href="/information/hell-forged-set" target="_blank"&gt;Hell Forged&lt;/a&gt; and then &lt;a href="/information/purgatory-chains-set" target="_blank"&gt;Purgatory Chains&lt;/a&gt;. In order to get a piece of Hell Forged gear you need to craft or have a crafting level 400 item, which is beyond what the shop sells.&lt;/p&gt;&lt;p&gt;Crafting cannot be done with any form of automation, and instead works well while you set up &lt;a href="/information/exploration" target="_blank"&gt;exploration&lt;/a&gt;. It is vitally important you find a creature in the list, further down if possible, that you can manually kill in one hit a few times to use for exploration.&lt;/p&gt;&lt;p&gt;The further down the list, for monsters, you go the harder they get yes – but the more XP you get. All Monsters have a maximum level and when a player reaches that maximum level and beyond, they will only get 1/3rd the XP for killing it.&lt;/p&gt;&lt;p&gt;This quest will also have you find, by visiting two locations, &lt;a href="/information/quest-items" target="_blank"&gt;quest items&lt;/a&gt; which you will automatically be picked up and automatically used. You can see that they are being used after you get them by going to your skill section (see instructions) and clicking on the skill name. The bonuses are automatically applied for you.&lt;/p&gt;&lt;p&gt;With that said my suggestion for this is to set up exploration for 2 or more hours and then start crafting while exploration runs. Put on a good show/movie/podcast and lets start grinding shall we?&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Keep crafting after this quest, it will hurt less in a later guide quest.&lt;/strong&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- First we want to find the items we need, quest items are automatically used. You can open the Teleport Map Action to then select the location: Ruined Port City Of Kalize (X/Y): 32/368 and click teleport if you can afford the cost. This will get you the: Weapon Smith’s Book which adds 25% to Skill Bonus and XP.&lt;/p&gt;&lt;p&gt;- Repeat the above step to then go to: Dragon cliffs (X/Y): 192/176 to get the Blacksmith’s book for the same bonuses towards Armour Crafting.&lt;/p&gt;&lt;p&gt;Both of these can be upgraded later on when we have access to Labyrinth. There are some One Off &lt;a href="http://127.0.0.1:8000/information/quests" target="_blank"&gt;quests&lt;/a&gt; that will upgrade these.&lt;/p&gt;&lt;p&gt;- Now lets craft, first set up exploration for an hour or two – or what ever you feel like doing, Exploration will run while logged out. Remember to set it up with a monster you can kill in one hit.&lt;/p&gt;&lt;p&gt;- Close exploration and then from the drop down Craft/Enchant select craft, select weapons, select Broken Dagger and then click craft.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- Select Map from the actions drop down.&lt;/p&gt;&lt;p&gt;- Click Teleport from the actions under the map.&lt;/p&gt;&lt;p&gt;- Select the location: Ruined Port City Of Kalize (X/Y): 32/368 and click teleport if you can afford the cost. This will get you the: Weapon Smith’s Book which adds 25% to Skill Bonus and XP.&lt;/p&gt;&lt;p&gt;- Repeat the above step to then go to: Dragon cliffs (X/Y): 192/176 to get the Blacksmith’s book for the same bonuses towards Armour Crafting.&lt;/p&gt;&lt;p&gt;Both of these can be upgraded later on when we have access to Labyrinth. There are some One off &lt;a href="http://127.0.0.1:8000/information/quests" target="_blank"&gt;quests&lt;/a&gt; that will upgrade these.&lt;/p&gt;&lt;p&gt;- Now lets craft, first set up exploration for an hour or two – or what ever you feel like doing, Exploration will run while logged out. Remember to set it up with a monster you can kill in one hit.&lt;/p&gt;&lt;p&gt;- Close exploration, select Craft from the drop down and then select Craft from the Craft/Enchant&lt;/p&gt;&lt;p&gt;- Select Weapons, Broken Dagger – Click craft.&lt;/p&gt;&lt;p&gt;- When ready, click Change Type, select Armour, select an Armour to craft and click craft.&lt;/p&gt;</t>
+    <t>Sitting in the INN, you stare into the large fireplace with the wood burning and the smell of the old oak as it burns. It’s almost as if time stops for a moment, and you can gather your thoughts.&lt;br /&gt; &lt;br /&gt; All you do is slaughter creatures, gather loot and slowly get better at hitting the enemies and even slightly faster.&lt;br /&gt; &lt;br /&gt; The flames of the fire seem to stand still, the smell of the fire has dissipated from the air. You look around, and no one is moving, like they have been frozen in time.&lt;br /&gt; &lt;br /&gt; You turn back to the fire and see a young man, about twenty-five, standing before the fire, his back to you. You call out to him, and he doesn’t turn around, but he does speak.&lt;br /&gt; &lt;br /&gt; “Child. I have found something most mysterious. The gates have opened.”&lt;br /&gt; &lt;br /&gt; The gates? What gates?&lt;br /&gt; &lt;br /&gt; “Listen to me, child.” The young man turns and faces you.&lt;br /&gt; &lt;br /&gt; “I need you to speak with the local blacksmith, work with him for a while. Train a different set of skills. Important skills. I need you to craft your gear.”&lt;br /&gt; &lt;br /&gt; You tell him that the gear you have found, the stuff you can buy from the local blacksmith, is better than what you can craft.&lt;br /&gt; &lt;br /&gt; “True, however, you can craft even more powerful gear than that of which you can buy.”&lt;br /&gt; &lt;br /&gt; Before you can ask further questions, the flames return to their burning motion, the wood crackles, the INN is full of voices again, and the smell of food fills the air.&lt;br /&gt; &lt;br /&gt; Where did he go?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;: This quest can take 2+ hours to complete. It is suggested you explore and craft at the same time.&lt;/p&gt;&lt;p&gt;Today let's learn how to &lt;a href="/information/crafting" target="_blank"&gt;craft&lt;/a&gt; weapons and armor. You can also craft other things like spells, rings, trinkets and alchemy.&lt;/p&gt;&lt;p&gt;Crafting is wildly important because the shop will only take you so far. For example, later in the game, you can get gear sets: &lt;a href="/information/hell-forged-set" target="_blank"&gt;Hell Forged&lt;/a&gt; and then &lt;a href="/information/purgatory-chains-set" target="_blank"&gt;Purgatory Chains&lt;/a&gt;. To get a piece of Hell Forged gear, you need to craft or have a crafting level 400 &lt;/p&gt;&lt;p&gt;items, which is beyond what the &lt;a href="/information/shop" target="_blank"&gt;shop&lt;/a&gt; sells.&lt;/p&gt;&lt;p&gt;Crafting cannot be done with any form of automation, and instead works well while you set up &lt;a href="/information/exploration" target="_blank"&gt;exploration&lt;/a&gt;. It is vitally important you find a creature in the list, further down if possible, that you can manually kill in one hit a few times to use for exploration.&lt;/p&gt;&lt;p&gt;The further down the list, for monsters, you go the harder they get yes – but the more XP you get. All Monsters have a maximum level, and when a player reaches that maximum level and beyond, they will only get 1/3rd the XP for killing it.&lt;/p&gt;&lt;p&gt;This quest will also have you find, by visiting two locations, &lt;a href="/information/quest-items" target="_blank"&gt;quest items&lt;/a&gt; which you will automatically be picked up and automatically used. You can see that they are being used after you get them by going to your skill section (see instructions) and &lt;/p&gt;&lt;p&gt;clicking on the skill name. The bonuses are automatically applied for you.&lt;/p&gt;&lt;p&gt;With that said my suggestion for this is to set up exploration for 2 or more hours and then start crafting while exploration runs. Put on a good show/movie/podcast and let's start grinding shall we?&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;u&gt;Keep crafting after this quest; it will hurt less in a later guide quest.&lt;/u&gt;&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;First, we want to find the items we need; quest items are automatically used. You can open the Teleport Map Action to then select the location: Ruined Port City Of Kalize (X/Y): 32/368 and click teleport if you can afford the cost. This will get you the: Weapon Smith’s Book which adds 25% to Skill Bonus and XP.&lt;/li&gt;&lt;li&gt;Repeat the above step to then go to: Dragon cliffs (X/Y): 192/176 to get the Blacksmith’s book for the same bonuses towards Armour Crafting.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Both of these can be upgraded later on when we have access to Labyrinth. There are some One-Off &lt;a href="/information/quests" target="_blank"&gt;quests&lt;/a&gt; that will upgrade these.&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Now let's craft, first set up exploration for an hour or two – or whatever you feel like doing, Exploration will run while logged out. Remember to set it up with a monster you can kill in one hit.&lt;/li&gt;&lt;li&gt;Close exploration and then from the drop-down Craft/Enchant select craft, select weapons, select Broken Dagger and then click craft.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Select Map from the actions drop-down.&lt;/li&gt;&lt;li&gt;Click Teleport from the actions under the map.&lt;/li&gt;&lt;li&gt;Select the location: Ruined Port City Of Kalize (X/Y): 32/368 and click teleport if you can afford the cost. This will get you the: Weapon Smith’s Book which adds 25% to Skill Bonus and XP.&lt;/li&gt;&lt;li&gt;Repeat the above step to then go to: Dragon cliffs (X/Y): 192/176 to get the Blacksmith’s book for the same bonuses towards Armour Crafting.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Both of these can be upgraded later on when we have access to Labyrinth. There are some One-off &lt;a href="information/quests" target="_blank"&gt;quests&lt;/a&gt; that will upgrade these.&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Now let's craft, first set up exploration for an hour or two – or whatever you feel like doing, Exploration will run while logged out. Remember to set it up with a monster you can kill in one hit.&lt;/li&gt;&lt;li&gt;Close exploration, select Craft from the drop-down and then select Craft from the Craft/Enchant&lt;/li&gt;&lt;li&gt;Select Weapons, Broken Dagger – Click craft.&lt;/li&gt;&lt;li&gt;When ready, click Change Type, select Armour, select an Armour to craft and click craft.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>Weapon Crafting</t>
@@ -275,13 +275,13 @@
     <t>The Enchantress</t>
   </si>
   <si>
-    <t>You are exhausted, tired, confused.&lt;br /&gt; &lt;br /&gt; “Child” comes a familiar voice as you sit up on your bed.&lt;br /&gt; &lt;br /&gt; The INN is creaky, noisy and musty. The single candle flame that burns in the room barley illuminates the area.&lt;br /&gt; &lt;br /&gt; As he walks from the shadows The Guide stands before you, not young and handsome, but old and wise, dressed in robes. His skin is brown from the sun.&lt;br /&gt; &lt;br /&gt; “Downstairs sits a woman, an attractive woman.” he states with a bit of a smirk.&lt;br /&gt; &lt;br /&gt; “She will teach you about magic and its properties, specifically in the art of enchanting and disenchanting.”&lt;br /&gt; &lt;br /&gt; You ask him why he can’t teach you and he deflects the question.&lt;br /&gt; &lt;br /&gt; “Go now child. She isn’t to be kept waiting.”&lt;br /&gt; &lt;br /&gt; You head down the stairs to meet the Enchantress.&lt;br /&gt; &lt;br /&gt; She waits for you at a table, a woman in black, instantly recognizable by her long black hair and pale complexion. She radiates beauty.&lt;br /&gt; &lt;br /&gt; You walk over and sit down at the table. “Hello child.” She starts, he voice is soft and entrancing. “have you heard of The Queen?” You shake your head no. “She has gifted you with some of those green shiny unique's in your inventory.”&lt;br /&gt; &lt;br /&gt; You remember those. Killing monsters gets you faction with the plane and its people. As a reward they give you a shiny green item that makes you feel much much stronger.&lt;br /&gt; &lt;br /&gt; “She can give you more powerful ones, but you have to face the most fearsome of creatures to earn her attention. In the mean time lets discuss the art of magic. Lets start small with spells …”</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; &lt;em&gt;This quest can take 2+ hours to do. It is suggested you craft and explore at the same time.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Lets learn about spells and spell casting.&lt;/p&gt;&lt;p&gt;You might not be a caster &lt;a href="/information/races-and-classes#3" target="_blank"&gt;class&lt;/a&gt; like a Heretic, Arcane Alchemist or Prophet, but every class can use spells. You just need to train the skill &lt;a href="/information/skill-information" target="_blank"&gt;Casting Accuracy&lt;/a&gt; for damage based spells.&lt;/p&gt;&lt;p&gt;Healing spells – never miss and will heal you when you use &lt;a href="/information/combat" target="_blank"&gt;Cast, Cast and Attack or Attack&lt;/a&gt; and cast (depending on healing spell location (right or left hand respectively) for the last two attack types).&lt;/p&gt;&lt;p&gt;Crafting spells is done the same way as you would for crafting armour or weapons or rings.&lt;/p&gt;&lt;p&gt;Casting Accuracy will, over time, make it easier for you to hit the enemy. Caster classes want to focus on this skill and start using Cast once their spells, via using Cast and Attack or Attack and Cast, are landing more frequently.&lt;/p&gt;&lt;p&gt;Prophets can also use damage spells and should also start focusing on Cast and Attack or Attack and cast depending on which hand their healing spell is in.&lt;/p&gt;&lt;p&gt;Intelligence here is a stat we want to raise, you can do this via buying, crafting or enchanting gear – since we have not learned about enchantments yet, lets try and use the gear we have found or buy some better gear (Body, Damage Spell x2 and/or Stave (weapon type – two handed)) to raise this stat.&lt;/p&gt;&lt;p&gt;Leveling your character will also help. Why raise Intelligence? For the next quest – Enchanting depends on intelligence in terms of what you can craft, we just want to make it easier for you.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Just like we did for crafting, lets select spells instead of weapons or armour. When crafting spells, you will always have one of each type to equip: Damage and Healing.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Remember to set up exploration with a creature you can reliably kill in one hit. Continue investigating and upgrading your gear to take on harder creature.&lt;/strong&gt;&lt;/p&gt;</t>
+    <t>You are exhausted, tired, confused.&lt;br /&gt; &lt;br /&gt; “Child,” comes a familiar voice as you sit up on your bed.&lt;br /&gt; &lt;br /&gt; The INN is creaky, noisy, and musty. The single candle flame that burns in the room barely illuminates the area.&lt;br /&gt; &lt;br /&gt; As he walks from the shadows, The Guide stands before you, not young and handsome, but old and wise, dressed in robes. His skin is brown from the sun.&lt;br /&gt; &lt;br /&gt; “Downstairs sits a woman, an attractive woman,” he states with a bit of a smirk.&lt;br /&gt; &lt;br /&gt; “She will teach you about magic and its properties, specifically in the art of enchanting and disenchanting.”&lt;br /&gt; &lt;br /&gt; You ask him why he can’t teach you, and he deflects the question.&lt;br /&gt; &lt;br /&gt; “Go now, child. She isn’t to be kept waiting.”&lt;br /&gt; &lt;br /&gt; You head down the stairs to meet the Enchantress.&lt;br /&gt; &lt;br /&gt; She waits for you at a table, a woman in black, instantly recognizable by her long black hair and pale complexion. She radiates beauty.&lt;br /&gt; &lt;br /&gt; You walk over and sit down at the table. “Hello, child,” she starts; her voice is soft and entrancing. “Have you heard of The Queen?” You shake your head no. “She has gifted you with some of those green shiny unique's in your inventory.”&lt;br /&gt; &lt;br /&gt; You remember those. Killing monsters gets you faction with the plane and its people. As a reward, they give you a shiny green item that makes you feel much stronger.&lt;br /&gt; &lt;br /&gt; “She can give you more powerful ones, but you have to face the most fearsome of creatures to earn her attention. In the meantime, let's discuss the art of magic. Let's start small with spells…”</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;: This quest can take 2+ hours to do. It is suggested you craft and explore at the same time.&lt;/p&gt;&lt;p&gt;Let's learn about spells and spell casting.&lt;/p&gt;&lt;p&gt;You might not be a caster &lt;a href="/information/races-and-classes#3" target="_blank"&gt;class&lt;/a&gt; like a Heretic, Arcane Alchemist, or Prophet, but every class can use spells. You just need to train the skill &lt;a href="/information/skill-information" target="_blank"&gt;Casting Accuracy&lt;/a&gt; for damage-based spells.&lt;/p&gt;&lt;p&gt;Healing spells – never miss and will heal you when you use &lt;a href="/information/combat" target="_blank"&gt;Cast, Cast and Attack, or Attack and cast&lt;/a&gt; (depending on the healing spell location (right or left hand respectively) for the last two attack types).&lt;/p&gt;&lt;p&gt;Crafting spells is done the same way as you would for crafting armor or weapons or rings.&lt;/p&gt;&lt;p&gt;Casting Accuracy will, over time, make it easier for you to hit the enemy. Caster classes want to focus on this skill and start using Cast once their spells, via using Cast and Attack or Attack and Cast, are landing more frequently.&lt;/p&gt;&lt;p&gt;Prophets can also use damage spells and should also start focusing on Cast and Attack or Attack and cast depending on which hand their healing spell is in.&lt;/p&gt;&lt;p&gt;Intelligence here is a stat we want to raise; you can do this via buying, crafting, or enchanting gear – since we have not learned about enchantments yet, let's try and use the gear we have found or buy some better gear (Body, Damage Spell x2 &lt;/p&gt;&lt;p&gt;and/or Stave (weapon type – two-handed)) to raise this stat.&lt;/p&gt;&lt;p&gt;Leveling your character will also help. Why raise Intelligence? For the next quest – Enchanting depends on intelligence in terms of what you can craft; we just want to make it easier for you.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Just like we did for crafting, let's select spells instead of weapons or armor. When crafting spells, you will always have one of each type to equip: Damage and Healing.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Remember to set up exploration with a creature you can reliably kill in one hit. Continue investigating and upgrading your gear to take on a harder creature.&lt;/strong&gt;&lt;/p&gt;</t>
   </si>
   <si>
     <t>Spell Crafting</t>
@@ -296,16 +296,16 @@
     <t>Enchanting is key</t>
   </si>
   <si>
-    <t>As you rise to the new dawn of a new day you have a knock at the door. You rise and greet the stranger. The Enchantress walks in. Today she wares a set of red robes and you can see deep into her blue eyes.&lt;br /&gt; &lt;br /&gt; “My darling child, I hear you have been adventuring. Shall we pick up where we left off? The art of enchanting.”&lt;br /&gt; &lt;br /&gt; You tell her you have plenty of enchanted gear.&lt;br /&gt; &lt;br /&gt; “Wouldn’t you like better gear? Stronger gear?”</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Note: &lt;/strong&gt;&lt;em&gt;This quest can take 2+ hours to complete. It is advised to explore and do the other objectives such as crafting and then enchanting while exploration is running.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;The &lt;/em&gt;&lt;strong&gt;&lt;em&gt;Skill Type Crafting to level 10&lt;/em&gt;&lt;/strong&gt;&lt;em&gt; means: level any crafting skill you want to level 10 or higher that you currently have access too.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Today's lesson is about &lt;a href="/information/enchanting" target="_blank"&gt;enchanting&lt;/a&gt; and &lt;a href="/information/disenchanting" target="_blank"&gt;disenchanting&lt;/a&gt;. Just like crafting, enchanting is wildly important. As you may know, you cannot buy enchanted gear from the shop. Some players will sell it on the &lt;a href="/information/market-board" target="_blank"&gt;market place&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;More importantly, you want a &lt;a href="/information/currencies" target="_blank"&gt;currency&lt;/a&gt; you can get from it: Gold Dust. This currency is used in a lot of quests we are going to start doing soon. So lets get a lot of it.&lt;/p&gt;&lt;p&gt;There re a verity of enchantments you can choose from, on the enchanting help page you can filter the different types of enchantments. All enchantments, unless otherwise stated, will stack.&lt;/p&gt;&lt;p&gt;You can see info about an enchantment on an item by either opening it from your inventory or from chat when it drops, selecting details – and from there as you scroll down you will see one or two orange buttons that when clicked will open up a modal for that items enchantment.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;&lt;u&gt;My tip for you is&lt;/u&gt;&lt;/em&gt;&lt;/strong&gt;: Filter the table on the help page by Accuracy (or Casting Accuracy if you are using spells) and then Stat Modifiers.&lt;/p&gt;&lt;p&gt;Find the level 1 enchantments for both, and enchant those – both – on to your freshly crafted items. Repeat until your inventory is full, equip what you want and then disenchant the rest.&lt;/p&gt;&lt;p&gt;You can also buy multiple items from the shop for the purposes of enchanting, but I recommend you continue crafting. Craft 75 items of what ever, enchant all 75 items, equip or disenchant the rest. You could also sell some stuff on the market board to make some coin back.&lt;/p&gt;&lt;p&gt;Rinse and Repeat, all while exploring to keep the steady flow of gold coming in.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Remember to keep enchanting and disenchanting items. A later quest will be less painful.&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;- &lt;/strong&gt;To enchant, from the crafting drop down select enchant.&lt;/p&gt;&lt;p&gt;- Here you have an item to select, a suffix and a prefix to select. The cost of enchanting can get widely expensive so exploration is required. Since you need items: weapons, Armour, spells and Rings, you will also want to be crafting. You can also re-enchant enchanted items but that gets more costly.&lt;/p&gt;&lt;p&gt;You can also just go to the shop and buy multiple items to enchant, like broken daggers.&lt;/p&gt;&lt;p&gt;- Next, when you have enchanted, ideally 75 items, next go to your inventory&lt;/p&gt;&lt;p&gt;- From the actions on the inventory section of your character sheet, click Disenchant All.&lt;/p&gt;&lt;p&gt;- This will raise your disenchanting skill, and slowly over time your enchanting skill as well.&lt;/p&gt;&lt;p&gt;- Repeat till you meet the quest requirements.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- Open Craft from the drop down selection&lt;/p&gt;&lt;p&gt;- from the Craft/Enchant drop down select enchant&lt;/p&gt;&lt;p&gt;- Here you have an item to select, a suffix and a prefix to select. The cost of enchanting can get widely expensive so exploration is required. Since you need items: weapons, Armour, spells and Rings, you will also want to be crafting. You can also re-enchant enchanted items but that gets more costly.&lt;/p&gt;&lt;p&gt;You can also just go to the shop and buy multiple items to enchant, like broken daggers.&lt;/p&gt;&lt;p&gt;- Next, when you have enchanted, ideally 75 items, next go to your inventory&lt;/p&gt;&lt;p&gt;- From the actions on the inventory section of your character sheet, click Disenchant All.&lt;/p&gt;&lt;p&gt;- This will raise your disenchanting skill, and slowly over time your enchanting skill as well.&lt;/p&gt;&lt;p&gt;- Repeat till you meet the quest requirements.&lt;/p&gt;</t>
+    <t>As you rise to the new dawn of a new day, you have a knock at the door. You rise and greet the stranger. The Enchantress walks in. Today she wears a set of red robes, and you can see deep into her blue eyes.&lt;br /&gt; &lt;br /&gt; “My darling child, I hear you have been adventuring. Shall we pick up where we left off? The art of enchanting.”&lt;br /&gt; &lt;br /&gt; You tell her you have plenty of enchanted gear.&lt;br /&gt; &lt;br /&gt; “Wouldn’t you like better gear? Stronger gear?”</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;: This quest can take 2+ hours to complete. It is advised to explore and do the other objectives such as crafting and then enchanting while exploration is running.&lt;/p&gt;&lt;p&gt;The &lt;strong&gt;&lt;u&gt;Skill Type Crafting to level 10 means&lt;/u&gt;&lt;/strong&gt;: level any crafting skill you want to level 10 or higher that you currently have access to.&lt;/p&gt;&lt;p&gt;Today's lesson is about &lt;a href="/information/enchanting" target="_blank"&gt;enchanting&lt;/a&gt; and &lt;a href="/information/disenchanting" target="_blank"&gt;disenchanting&lt;/a&gt;. Just like crafting, enchanting is wildly important. As you may know, you cannot buy enchanted gear from the shop. Some players will sell it on the &lt;a href="/information/market-board" target="_blank"&gt;marketplace&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;More importantly, you want a &lt;a href="/information/currencies" target="_blank"&gt;currency&lt;/a&gt; you can get from it: Gold Dust. This currency is used in a lot of quests we are going to start doing soon. So let's get a lot of it.&lt;/p&gt;&lt;p&gt;There are a variety of enchantments you can choose from; on the enchanting help page, you can filter the different types of enchantments. All enchantments, unless otherwise stated, will stack.&lt;/p&gt;&lt;p&gt;You can see info about an enchantment on an item by either opening it from your inventory or from chat when it drops, selecting details – and from there as you scroll down you will see one or two orange buttons that when clicked will open up a &lt;/p&gt;&lt;p&gt;modal for that item's enchantment.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;u&gt;My tip for you is&lt;/u&gt;&lt;/strong&gt;: Filter the table on the help page by Accuracy (or Casting Accuracy if you are using spells) and then Stat Modifiers.&lt;/p&gt;&lt;p&gt;Find the level 1 enchantments for both, and enchant those – both – onto your freshly crafted items. Repeat until your inventory is full, equip what you want and then disenchant the rest.&lt;/p&gt;&lt;p&gt;You can also buy multiple items from the shop for the purposes of enchanting, but I recommend you continue crafting. Craft 75 items of whatever, enchant all 75 items, equip or disenchant the rest. You could also sell some stuff on the market &lt;/p&gt;&lt;p&gt;board to make some coin back.&lt;/p&gt;&lt;p&gt;Rinse and Repeat, all while exploring to keep the steady flow of gold coming in.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;&lt;u&gt;Remember to keep enchanting and disenchanting items. A later quest will be less painful.&lt;/u&gt;&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;To enchant, from the crafting drop down, select enchant.&lt;/li&gt;&lt;li&gt;Here you have an item to select, a suffix and a prefix to select. The cost of enchanting can get widely expensive, so exploration is required. Since you need items: weapons, Armour, spells and Rings, you will also want to be crafting. You can also re-enchant enchanted items but that gets more costly.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;You can also just go to the shop and buy multiple items to enchant, like broken daggers.&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Next, when you have enchanted, ideally 75 items, next go to your inventory.&lt;/li&gt;&lt;li&gt;From the actions on the inventory section of your character sheet, click Disenchant All.&lt;/li&gt;&lt;li&gt;This will raise your disenchanting skill, and slowly over time your enchanting skill as well.&lt;/li&gt;&lt;li&gt;Repeat till you meet the quest requirements.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Open Craft from the drop-down selection.&lt;/li&gt;&lt;li&gt;From the Craft/Enchant drop-down, select enchant.&lt;/li&gt;&lt;li&gt;Here you have an item to select, a suffix and a prefix to select. The cost of enchanting can get widely expensive, so exploration is required. Since you need items: weapons, Armour, spells and Rings, you will also want to be crafting. You can also re-enchant enchanted items but that gets more costly.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;You can also just go to the shop and buy multiple items to enchant, like broken daggers.&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Next, when you have enchanted, ideally 75 items, next go to your inventory.&lt;/li&gt;&lt;li&gt;From the actions on the inventory section of your character sheet, click Disenchant All.&lt;/li&gt;&lt;li&gt;This will raise your disenchanting skill, and slowly over time your enchanting skill as well.&lt;/li&gt;&lt;li&gt;Repeat till you meet the quest requirements.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>Enchanting</t>
@@ -320,16 +320,16 @@
     <t>The Mysterious Goblin Pt. 1</t>
   </si>
   <si>
-    <t>The magic crackles in the air and the spells weave and twist their way around the gear as you chant the incantations to lock the enchantments into the item before you. Sometimes you fail, sometimes your efforts are in-vain and infuriating as the world seems against you and your efforts, but with determination and passion you manage to complete The Enchantress’s request of learning more about the art of enchanting it’s self.&lt;br /&gt; &lt;br /&gt; The magic before you make you weak, tired, exhausted. You step outside the confines of the small INN, you have been using a back room for your magical training, The Enchantress has been paying a little extra for the privacy to learn.&lt;br /&gt; &lt;br /&gt; She has left to run an errand, much like The Guide. Trusting that you wont get swept away into an adventure and instead study and focus on what is before you.&lt;br /&gt; &lt;br /&gt; As you stand in the fresh air of the warm fall day, you realize that the seasons before you are changing, the color of the leaves and the smell in the air has a bit of a nip to it.&lt;br /&gt; &lt;br /&gt; Out of the corner of your eye stands a little goblin. He sees you and darts away. What did he steal? You decide to hunt him down and find out what this little thief is up to.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Note: &lt;/strong&gt;&lt;em&gt;This guide quest can take longer then 2 hours. This is because the quests you will complete will require Gold Dust, which you get by enchanting and then disenchanting items. Due to the fact that you will also be leveling a faction, while this quest is active, you will get 5 extra faction points per kill.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Lets move on from skills and crafting and engage with other systems of the game, such as &lt;a href="/information/quests" target="_blank"&gt;Quests&lt;/a&gt;. Quests are another vital aspect of the game because this is how you unlock new features of the game to play with.&lt;/p&gt;&lt;p&gt;Some games will hide these features behind a pay wall, instead here I hide them behind quests, which are very easy to complete and come with explicit instructions on how to do so.&lt;/p&gt;&lt;p&gt;Some quests like the one you will do, will give you items that help with you other aspects of the game, some quests simply upgrade existing quest items and some quests unlock new access to new &lt;a href="/information/planes" target="_blank"&gt;planes&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;All quests tell a story before and after you click the hand in button which gives you some lore on the world and your place in it.&lt;/p&gt;&lt;p&gt;There are two types of quests: Quest trees and One off quests. One off quests will usually upgrade or give you an item that unlocks a feature where as Quest Trees will usually have a chain of quests that continually upgrade the item given or gives you an item at the end of said quest line.&lt;/p&gt;&lt;p&gt;There are also &lt;a href="/information/raids" target="_blank"&gt;Raid&lt;/a&gt; Quests that will appear when a raid is currently running. These are also usually in the form a tree where the left side of the tree tells you more about the raid boss while the right hand side will reward players with a cosmetic feature.&lt;/p&gt;&lt;p&gt;Each plane has its own set of quests as well, which can further enhance or unlock features for that plane or game wide in general.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- Click the Quests tab&lt;/p&gt;&lt;p&gt;- To the right you will see: Goblins List for Gold and Faction Hunter.&lt;/p&gt;&lt;p&gt;- Blue quests are quests you can complete, so start at the top of the tree and work your way down.&lt;/p&gt;&lt;p&gt;- Click on the first quest you can do.&lt;/p&gt;&lt;p&gt;- You will see three tab: &lt;a href="/information/npcs" target="_blank"&gt;NPC&lt;/a&gt; Details, Required to Complete and Quest Reward.&lt;/p&gt;&lt;p&gt;- NPC Details will give you details of the NPC as well as the “before” hand in story. When you hand in the quest, this story section will update to show “after” hand in story content&lt;/p&gt;&lt;p&gt;- Required to Complete will show you what you need to do in order to complete it. Beside each requirement is a help icon, clicking this will open a modal that gives you explicit instructions on how to get the requirement.&lt;/p&gt;&lt;p&gt;- Quest Reward Tab show you what rewards you get for completing the quest it’s self.&lt;/p&gt;&lt;p&gt;- Once you have met the requirements for a quest click the Hand in button and you will be, for free, with no timeout – transported across planes and locations to the NPC. The only caveat is you have to be able to reach them. For example if they are on water you must be able to walk on water.&lt;/p&gt;&lt;p&gt;You can walk on most forms of water with a quest item called Flask of Fresh Air which you can get by killing a Pirate Master on Surface.&lt;/p&gt;&lt;p&gt;Remember, to check your Factions by going to Character Sheet → Factions tab to see what level you are for surface as this guide quest has you complete a quest to help you level the factions a bit faster.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Mobile Instructions&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- Tap the Quests tab&lt;/p&gt;&lt;p&gt;- To the right you will see: Goblins List for Gold and Faction Hunter.&lt;/p&gt;&lt;p&gt;- You can scroll left, right, up and down to view the quest tree. Scroll to the far right&lt;/p&gt;&lt;p&gt;- Blue quests are quests you can complete, so start at the top of the tree and work your way down.&lt;/p&gt;&lt;p&gt;- Tap on the first quest you can do.&lt;/p&gt;&lt;p&gt;- You will see three tab: &lt;a href="/information/npcs" target="_blank"&gt;NPC&lt;/a&gt; Details, Required to Complete and Quest Reward.&lt;/p&gt;&lt;p&gt;- NPC Details will give you details of the NPC as well as the “before” hand in story. When you hand in the quest, this story section will update to show “after” hand in story content&lt;/p&gt;&lt;p&gt;- Required to Complete will show you what you need to do in order to complete it. Beside each requirement is a help icon, clicking this will open a modal that gives you explicit instructions on how to get the requirement.&lt;/p&gt;&lt;p&gt;- Quest Reward Tab show you what rewards you get for completing the quest it’s self.&lt;/p&gt;&lt;p&gt;- Once you have met the requirements for a quest click the Hand in button and you will be, for free, with no timeout – transported across planes and locations to the NPC. The only caveat is you have to be able to reach them. For example if they are on water you must be able to walk on water.&lt;/p&gt;&lt;p&gt;You can walk on most forms of water with a quest item called Flask of Fresh Air which you can get by killing a Pirate Master on Surface.&lt;/p&gt;&lt;p&gt;Remember, to check your Factions by going to Character Sheet →expand the Character Details Section → Factions tab to see what level you are for surface as this guide quest has you complete a quest to help you level the factions a bit faster.&lt;/p&gt;</t>
+    <t>The magic crackles in the air, and the spells weave and twist their way around the gear as you chant the incantations to lock the enchantments into the item before you. Sometimes you fail; sometimes your efforts are in vain and infuriating as the world seems against you and your efforts, but with determination and passion, you manage to complete The Enchantress’s request of learning more about the art of enchanting itself.&lt;br /&gt; &lt;br /&gt; The magic before you makes you weak, tired, exhausted. You step outside the confines of the small INN; you have been using a back room for your magical training. The Enchantress has been paying a little extra for the privacy to learn.&lt;br /&gt; &lt;br /&gt; She has left to run an errand, much like The Guide, trusting that you won't get swept away into an adventure and instead study and focus on what is before you.&lt;br /&gt; &lt;br /&gt; As you stand in the fresh air of the warm fall day, you realize that the seasons before you are changing; the color of the leaves and the smell in the air have a bit of a nip to it.&lt;br /&gt; &lt;br /&gt; Out of the corner of your eye stands a little goblin. He sees you and darts away. What did he steal? You decide to hunt him down and find out what this little thief is up to.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;: This guide quest can take longer than 2 hours. This is because the quests you will complete will require Gold Dust, which you get by enchanting and then disenchanting items. Due to the fact that you will also be leveling a faction, while this quest is active, you will get 5 extra faction points per kill.&lt;/p&gt;&lt;p&gt;Let's move on from skills and crafting and engage with other systems of the game, such as &lt;a href="/information/quests" target="_blank"&gt;Quests&lt;/a&gt;. Quests are another vital aspect of the game because this is how you unlock new features of the game to play with.&lt;/p&gt;&lt;p&gt;Some games will hide these features behind a pay wall; instead, here I hide them behind quests, which are very easy to complete and come with explicit instructions on how to do so.&lt;/p&gt;&lt;p&gt;Some quests like the one you will do will give you items that help with your other aspects of the game; some quests simply upgrade existing quest items, and some quests unlock new access to new &lt;a href="/information/planes" target="_blank"&gt;planes&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;All quests tell a story before and after you click the hand-in button which gives you some lore on the world and your place in it.&lt;/p&gt;&lt;p&gt;There are two types of quests: Quest trees and One-off quests. One-off quests will usually upgrade or give you an item that unlocks a feature, whereas Quest Trees will usually have a chain of quests that continually upgrade the item given or give &lt;/p&gt;&lt;p&gt;you an item at the end of the said quest line.&lt;/p&gt;&lt;p&gt;There are also &lt;a href="/information/raids" target="_blank"&gt;Raid&lt;/a&gt; Quests that will appear when a raid is currently running. These are also usually in the form of a tree where the left side of the tree tells you more about the raid boss while the right-hand side will reward players with a cosmetic feature.&lt;/p&gt;&lt;p&gt;Each plane has its own set of quests as well, which can further enhance or unlock features for that plane or game-wide in general.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Click the Quests tab&lt;/li&gt;&lt;li&gt;To the right you will see: Goblins List for Gold and Faction Hunter.&lt;/li&gt;&lt;li&gt;Blue quests are quests you can complete, so start at the top of the tree and work your way down.&lt;/li&gt;&lt;li&gt;Click on the first quest you can do.&lt;/li&gt;&lt;li&gt;You will see three tabs: &lt;a href="/information/npcs" target="_blank"&gt;NPC&lt;/a&gt; Details, Required to Complete and Quest Reward.&lt;/li&gt;&lt;li&gt;NPC Details will give you details of the NPC as well as the “before” hand-in story. When you hand in the quest, this story section will update to show “after” hand-in story content.&lt;/li&gt;&lt;li&gt;Required to Complete will show you what you need to do in order to complete it. Beside each requirement is a help icon, clicking this will open a modal that gives you explicit instructions on how to get the requirement.&lt;/li&gt;&lt;li&gt;Quest Reward Tab shows you what rewards you get for completing the quest itself.&lt;/li&gt;&lt;li&gt;Once you have met the requirements for a quest click the Hand in button and you will be, for free, with no timeout – transported across planes and locations to the NPC. The only caveat is you have to be able to reach them. For example, if they are on water, you must be able to walk on water.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;You can walk on most forms of water with a quest item called Flask of Fresh Air which you can get by killing a Pirate Master on Surface.&lt;/p&gt;&lt;p&gt;Remember, to check your Factions by going to Character Sheet → Factions tab to see what level you are for the surface as this guide quest has you complete a quest to help you level the factions a bit faster.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Tap the Quests tab&lt;/li&gt;&lt;li&gt;To the right you will see: Goblins List for Gold and Faction Hunter.&lt;/li&gt;&lt;li&gt;You can scroll left, right, up, and down to view the quest tree. Scroll to the far right&lt;/li&gt;&lt;li&gt;Blue quests are quests you can complete, so start at the top of the tree and work your way down.&lt;/li&gt;&lt;li&gt;Tap on the first quest you can do.&lt;/li&gt;&lt;li&gt;You will see three tabs: &lt;a href="/information/npcs" target="_blank"&gt;NPC&lt;/a&gt; Details, Required to Complete and Quest Reward.&lt;/li&gt;&lt;li&gt;NPC Details will give you details of the NPC as well as the “before” hand-in story. When you hand in the quest, this story section will update to show “after” hand-in story content.&lt;/li&gt;&lt;li&gt;Required to Complete will show you what you need to do in order to complete it. Beside each requirement is a help icon, clicking this will open a modal that gives you explicit instructions on how to get the requirement.&lt;/li&gt;&lt;li&gt;Quest Reward Tab shows you what rewards you get for completing the quest itself.&lt;/li&gt;&lt;li&gt;Once you have met the requirements for a quest click the Hand in button and you will be, for free, with no timeout – transported across planes and locations to the NPC. The only caveat is you have to be able to reach them. For example, if they are on water, you must be able to walk on water.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;You can walk on most forms of water with a quest item called Flask of Fresh Air which you can get by killing a Pirate Master on Surface.&lt;/p&gt;&lt;p&gt;Remember, to check your Factions by going to Character Sheet → expand the Character Details Section → Factions tab to see what level you are for the surface as this guide quest has you complete a quest to help you level the factions a bit faster.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Faction Hunter</t>
@@ -338,13 +338,13 @@
     <t>The Mysterious Goblin Pt. 2</t>
   </si>
   <si>
-    <t>This little helpless goblin does not seem dangerous at all. Curious if anything else. Full of surprises and strange little gifts for the errands you do for him.&lt;br /&gt; &lt;br /&gt; You have arrived back at the town after your little adventure and you find The Guide sitting at the INN waiting for you.&lt;br /&gt; &lt;br /&gt; “I see you have been out adventuring with our helpless little friend.”&lt;br /&gt; &lt;br /&gt; You tell him of your adventures, your crafting, enchanting, fighting, errands you did for the goblin.&lt;br /&gt; &lt;br /&gt; “Fantastic. The world is full of interesting people for you to meet. Some of them have more errands, their own stories and adventures for you to go on in exchange for knowledge and various fantastic rewards.”&lt;br /&gt; &lt;br /&gt; He pauses and you two sit in silence for a moment enjoying a drink and a spread before you.&lt;br /&gt; &lt;br /&gt; “You should work with that goblin for something special, A Book of Guidance.”&lt;br /&gt; &lt;br /&gt; You ask what this item is for.&lt;br /&gt; &lt;br /&gt; “You, to help you hit better child.”</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;: &lt;em&gt;This quest might take a moment, longer then two hours, because you need the gold dust which you get from enchanting and then disenchanting.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;We know how to do quests now, so lets continue doing quests to get an item that will help you – especially if you are crafting items with Accuracy enchantments attached – level Accuracy rather quickly.&lt;/p&gt;&lt;p&gt;This right here shows you how two features of the game can work together to progress your character: Quest items that you get from doing quests that increase some aspect about your character. Enchanting, Crafting, Quests and Skills&lt;/p&gt;&lt;p&gt;As we progress we will open more systems that also work together with existing systems you have learned to continue to progress your character.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;We already know how to complete a quest, and we know how to level our skills. So lets use that in conjunction with crafting and enchanting to get gold dust to complete the required objectives.&lt;/p&gt;</t>
+    <t>This little, helpless goblin does not seem dangerous at all. Curious, if anything else, he is full of surprises and strange little gifts for the errands you do for him.&lt;br /&gt; &lt;br /&gt; You have arrived back at the town after your little adventure, and you find The Guide sitting at the INN waiting for you.&lt;br /&gt; &lt;br /&gt; “I see you have been out adventuring with our helpless little friend.”&lt;br /&gt; &lt;br /&gt; You tell him of your adventures, your crafting, enchanting, fighting, and the errands you did for the goblin.&lt;br /&gt; &lt;br /&gt; “Fantastic. The world is full of interesting people for you to meet. Some of them have more errands, their own stories, and adventures for you to go on in exchange for knowledge and various fantastic rewards.”&lt;br /&gt; &lt;br /&gt; He pauses, and you two sit in silence for a moment, enjoying a drink and a spread before you.&lt;br /&gt; &lt;br /&gt; “You should work with that goblin for something special, A Book of Guidance.”&lt;br /&gt; &lt;br /&gt; You ask what this item is for.&lt;br /&gt; &lt;br /&gt; “You, to help you hit better, child.”</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;: This quest might take a moment, longer than two hours, because you need the gold dust which you get from enchanting and then disenchanting.&lt;/p&gt;&lt;p&gt;We know how to do quests now, so let's continue doing quests to get an item that will help you – especially if you are crafting items with Accuracy enchantments attached – level Accuracy rather quickly.&lt;/p&gt;&lt;p&gt;This right here shows you how two features of the game can work together to progress your character: Quest items that you get from doing quests that increase some aspect about your character. Enchanting, Crafting, Quests, and Skills.&lt;/p&gt;&lt;p&gt;As we progress, we will open more systems that also work together with existing systems you have learned to continue to progress your character.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We already know how to complete a quest, and we know how to level our skills. So let's use that in conjunction with crafting and enchanting to get gold dust to complete the required objectives.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Goblins Accuracy</t>
@@ -353,16 +353,16 @@
     <t>The Shadow and The Murder</t>
   </si>
   <si>
-    <t>Your ability to kill creatures is getting better and your able to find and hunt down stronger foes.&lt;br /&gt; &lt;br /&gt; Exhausted and tired you arrive back at the INN. It’s completely empty. Not a soul, not a single sound but the creaking of the old wood in the wind that blows outside.&lt;br /&gt; &lt;br /&gt; You call out but no one answers.&lt;br /&gt; &lt;br /&gt; A shadow moves across the wall and you move towards where the shadow went.&lt;br /&gt; &lt;br /&gt; No one there.&lt;br /&gt; &lt;br /&gt; You call out again, readying your weapon.&lt;br /&gt; &lt;br /&gt; Nothing.&lt;br /&gt; &lt;br /&gt; You enter into a back room, an office of sorts. Blood covers the wall. You back out and head back to the main room.&lt;br /&gt; &lt;br /&gt; Bodies. Bodies every where, torn, broken, damage and ripped apart. The gore, the fear, the pain the eyes of the dead.&lt;br /&gt; &lt;br /&gt; What the hell happened?</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;: &lt;em&gt;This quest can take two plus hours to complete. I recommend exploration while crafting and enchanting.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;It’s time we get off the &lt;a href="/information/planes" target="_blank"&gt;plane&lt;/a&gt;: Surface. To do this we just have to kill a single creature: Labyrinth Fiend until the Key of Labyrinth drops.&lt;/p&gt;&lt;p&gt;This will allow us to use a new feature called: &lt;a href="/information/traverse" target="_blank"&gt;Traverse&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;Traverse allows us to move to another plane of existence where we can fight monsters and interact with new features. For example, when we eventually get to Hell, those &lt;a href="/information/random-enchants" target="_blank"&gt;Green Uniques&lt;/a&gt; you have been getting – there is an NPC that allows you to buy better ones and even re-roll them and move the enchantments to other items. How fun!&lt;/p&gt;&lt;p&gt;Some Planes make you weaker and the creatures much, much stronger and also give you bonuses for killing creatures of that plane. As you go past Dungeons plane you will find your gear needs to be better with a set of enchantments that play to your classes strengths as well as the levels.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Kill Labyrinth fiend until the Key of Labyrinth drops.&lt;/p&gt;&lt;p&gt;Next:&lt;/p&gt;&lt;p&gt;- Click Traverse under the map&lt;/p&gt;&lt;p&gt;- Select labyrinth from the drop down&lt;/p&gt;&lt;p&gt;- Click Traverse&lt;/p&gt;&lt;p&gt;- Welcome to Labyrinth!plane&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Kill Labyrinth fiend until the Key of Labyrinth drops.&lt;/p&gt;&lt;p&gt;Next:&lt;/p&gt;&lt;p&gt;- Select Map Movement from the action drop down&lt;/p&gt;&lt;p&gt;- Tap Traverse under the map&lt;/p&gt;&lt;p&gt;- Select labyrinth from the drop down&lt;/p&gt;&lt;p&gt;- Tap Traverse&lt;/p&gt;&lt;p&gt;- Welcome to Labyrinth!&lt;/p&gt;</t>
+    <t>Your ability to kill creatures is getting better, and you're able to find and hunt down stronger foes.&lt;br /&gt; &lt;br /&gt; Exhausted and tired, you arrive back at the INN. It’s completely empty. Not a soul, not a single sound but the creaking of the old wood in the wind that blows outside.&lt;br /&gt; &lt;br /&gt; You call out, but no one answers.&lt;br /&gt; &lt;br /&gt; A shadow moves across the wall, and you move towards where the shadow went.&lt;br /&gt; &lt;br /&gt; No one there.&lt;br /&gt; &lt;br /&gt; You call out again, readying your weapon.&lt;br /&gt; &lt;br /&gt; Nothing.&lt;br /&gt; &lt;br /&gt; You enter into a back room, an office of sorts. Blood covers the wall. You back out and head back to the main room.&lt;br /&gt; &lt;br /&gt; Bodies. Bodies everywhere, torn, broken, damaged, and ripped apart. The gore, the fear, the pain, the eyes of the dead.&lt;br /&gt; &lt;br /&gt; What the hell happened?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;: This quest can take two-plus hours to complete. I recommend exploration while crafting and enchanting.&lt;/p&gt;&lt;p&gt;It’s time we get off the &lt;a href="/information/planes" target="_blank"&gt;plane&lt;/a&gt;: Surface. To do this, we just have to kill a single creature: Labyrinth Fiend until the Key of Labyrinth drops.&lt;/p&gt;&lt;p&gt;This will allow us to use a new feature called: &lt;a href="/information/traverse" target="_blank"&gt;Traverse&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;Traverse allows us to move to another plane of existence where we can fight monsters and interact with new features. For example, when we eventually get to Hell, those &lt;a href="/information/random-enchants" target="_blank"&gt;Green Uniques&lt;/a&gt; you have been getting – there is an NPC that allows you to &lt;/p&gt;&lt;p&gt;buy better ones and even re-roll them and move the enchantments to other items. How fun!&lt;/p&gt;&lt;p&gt;Some Planes make you weaker, and the creatures much, much stronger and also give you bonuses for killing creatures of that plane. As you go past Dungeons plane, you will find your gear needs to be better with a set of enchantments that play &lt;/p&gt;&lt;p&gt;to your class's strengths as well as the levels.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Kill Labyrinth Fiend until the Key of Labyrinth drops.&lt;/p&gt;&lt;p&gt;Next:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Click Traverse under the map.&lt;/li&gt;&lt;li&gt;Select Labyrinth from the drop-down.&lt;/li&gt;&lt;li&gt;Click Traverse.&lt;/li&gt;&lt;li&gt;Welcome to Labyrinth!plane.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Kill Labyrinth Fiend until the Key of Labyrinth drops.&lt;/p&gt;&lt;p&gt;Next:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Select Map Movement from the action drop-down.&lt;/li&gt;&lt;li&gt;Tap Traverse under the map.&lt;/li&gt;&lt;li&gt;Select Labyrinth from the drop-down.&lt;/li&gt;&lt;li&gt;Tap Traverse.&lt;/li&gt;&lt;li&gt;Welcome to Labyrinth!&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>Labyrinth</t>
@@ -374,16 +374,16 @@
     <t>Chasing Shadows</t>
   </si>
   <si>
-    <t>You stand in the ruins of a land covered in the memories of the gladiators who died in the many labyrinths that were built and destroyed over the years.&lt;br /&gt; &lt;br /&gt; It is said that a mad Architect created this world, who also then created one labyrinth after the other and then abandoned the world to its own ends only for it fall into ruins.&lt;br /&gt; &lt;br /&gt; You remember the death, the blood, the gore and the bodies.&lt;br /&gt; &lt;br /&gt; They were all dead, but it was also empty when you entered.&lt;br /&gt; &lt;br /&gt; You search the ruins for answers. You find nothing but shadows of memories lost to time.&lt;br /&gt; &lt;br /&gt; A shadow moves across the ruins. A shadow that you recognize for the INN.&lt;br /&gt; &lt;br /&gt; You chase the shadow, but it alludes you.&lt;br /&gt; &lt;br /&gt; “Child.”&lt;br /&gt; &lt;br /&gt; A familiar voice, you turn and see The Guide. He is old haggard and damaged. He coughs in a handkerchief that is covered in blood.&lt;br /&gt; &lt;br /&gt; “I must see The Poet.”&lt;br /&gt; &lt;br /&gt; he coughs and wheezes. You move towards to help him but he waives your advance off.&lt;br /&gt; &lt;br /&gt; “Learn something of your self.” he turns and walks away coughing and wheezing as he does.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Let’s do what the Guide stated: Learn something about our selves. Class Ranks.&lt;/p&gt;&lt;p&gt;&lt;a href="/information/class-ranks" target="_blank"&gt;Class Ranks&lt;/a&gt; allow you to switch classes and equip special abilities that can boost your character stats or even give you a special attack that will fire any time you attack an enemy allowing you to do even more damage.&lt;/p&gt;&lt;p&gt;Class Ranks comes with, as mentioned, Specialties which as leveled make your character even stronger. To level them you just have to equip the ones you want and then go kill things using exploration – as manual leveling will take a very long time and can be very grindy.&lt;/p&gt;&lt;p&gt;Class Ranks also come with masteries. As a character who has specific weapons equipped will level these masteries over time while killing creatures and gaining more bonuses to damage while using that weapon.&lt;/p&gt;&lt;p&gt;As mentioned before Characters can, at any time switch classes. You can level the rank of that class by killing creatures.&lt;/p&gt;&lt;p&gt;As you level the class it’s self and switch to other classes and level them, not only will you unlock the specialties you can equip (and thus mix and max) you will also eventually unlock other classes you can switch too that require you to level two or more classes.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- Click Character Sheet Tab&lt;/p&gt;&lt;p&gt;- Click Class Ranks Orange Button&lt;/p&gt;&lt;p&gt;- Look for your class in the list and click the name&lt;/p&gt;&lt;p&gt;- This will open another window, to exit back to the class list click the red circle with the minus in the top right. Clicking cancel or the X will close the modal.&lt;/p&gt;&lt;p&gt;- Here you will see information about the class and the Class Masteries&lt;/p&gt;&lt;p&gt;- Click Manage Specialties&lt;/p&gt;&lt;p&gt;- Equip a specialty and boom done, now you just have to kill creatures.&lt;/p&gt;&lt;p&gt;- The server messages will tell you when you gain levels in your Masteries and your Specialties as well as your Class Rank&lt;/p&gt;&lt;p&gt;Now you just have to kill creatures till you meet the requirements.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;- Tap Character Sheet tab&lt;/p&gt;&lt;p&gt;- expand the Character Details Section&lt;/p&gt;&lt;p&gt;- Tap the Class Ranks orange button&lt;/p&gt;&lt;p&gt;- Look for your class in the list and tap the name&lt;/p&gt;&lt;p&gt;- This will open another window, to exit back to the class list tap the red circle with the minus in the top right. Tap cancel or the X will close the modal.&lt;/p&gt;&lt;p&gt;- Here you will see information about the class and the Class Masteries&lt;/p&gt;&lt;p&gt;- Tap Manage Specialties&lt;/p&gt;&lt;p&gt;- Equip a specialty and boom done, now you just have to kill creatures.&lt;/p&gt;&lt;p&gt;- The server messages will tell you when you gain levels in your Masteries and your Specialties as well as your Class Rank&lt;/p&gt;&lt;p&gt;Now you just have to kill creatures till you meet the requirements.&lt;/p&gt;</t>
+    <t>You stand in the ruins of a land covered in the memories of the gladiators who died in the many labyrinths that were built and destroyed over the years.&lt;br /&gt; &lt;br /&gt; It is said that a mad Architect created this world, who also then created one labyrinth after the other and then abandoned the world to its own ends only for it fall into ruins.&lt;br /&gt; &lt;br /&gt; You remember the death, the blood, the gore, and the bodies.&lt;br /&gt; &lt;br /&gt; They were all dead, but it was also empty when you entered.&lt;br /&gt; &lt;br /&gt; You search the ruins for answers. You find nothing but shadows of memories lost to time.&lt;br /&gt; &lt;br /&gt; A shadow moves across the ruins. A shadow that you recognize from the INN.&lt;br /&gt; &lt;br /&gt; You chase the shadow, but it eludes you.&lt;br /&gt; &lt;br /&gt; “Child.”&lt;br /&gt; &lt;br /&gt; A familiar voice, you turn and see The Guide. He is old, haggard, and damaged. He coughs into a handkerchief that is covered in blood.&lt;br /&gt; &lt;br /&gt; “I must see The Poet.”&lt;br /&gt; &lt;br /&gt; He coughs and wheezes. You move towards to help him, but he waves your advance off.&lt;br /&gt; &lt;br /&gt; “Learn something of yourself.” he turns and walks away coughing and wheezing as he does.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Let’s do what the Guide stated: Learn something about ourselves. Class Ranks.&lt;/p&gt;&lt;p&gt;&lt;a href="/information/class-ranks" target="_blank"&gt;Class Ranks&lt;/a&gt; allow you to switch classes and equip special abilities that can boost your character stats or even give you a special attack that will fire any time you attack an enemy allowing you to do even more damage.&lt;/p&gt;&lt;p&gt;Class Ranks come with, as mentioned, Specialties which as leveled make your character even stronger. To level them you just have to equip the ones you want and then go kill things using exploration – as manual leveling will take a very long time &lt;/p&gt;&lt;p&gt;and can be very grindy.&lt;/p&gt;&lt;p&gt;Class Ranks also come with masteries. As a character who has specific weapons equipped will level these masteries over time while killing creatures and gaining more bonuses to damage while using that weapon.&lt;/p&gt;&lt;p&gt;As mentioned before Characters can, at any time switch classes. You can level the rank of that class by killing creatures.&lt;/p&gt;&lt;p&gt;As you level the class itself and switch to other classes and level them, not only will you unlock the specialties you can equip (and thus mix and match) you will also eventually unlock other classes you can switch too that require you to level two or more classes.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Click the Character Sheet Tab.&lt;/li&gt;&lt;li&gt;Click the Class Ranks Orange Button.&lt;/li&gt;&lt;li&gt;Look for your class in the list and click the name.&lt;/li&gt;&lt;li&gt;This will open another window, to exit back to the class list click the red circle with the minus in the top right. Clicking cancel or the X will close the modal.&lt;/li&gt;&lt;li&gt;Here you will see information about the class and the Class Masteries.&lt;/li&gt;&lt;li&gt;Click Manage Specialties.&lt;/li&gt;&lt;li&gt;Equip a specialty and boom done, now you just have to kill creatures.&lt;/li&gt;&lt;li&gt;The server messages will tell you when you gain levels in your Masteries and your Specialties as well as your Class Rank.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Now you just have to kill creatures till you meet the requirements.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Tap the Character Sheet tab.&lt;/li&gt;&lt;li&gt;Expand the Character Details Section.&lt;/li&gt;&lt;li&gt;Tap the Class Ranks orange button.&lt;/li&gt;&lt;li&gt;Look for your class in the list and tap the name.&lt;/li&gt;&lt;li&gt;This will open another window, to exit back to the class list tap the red circle with the minus in the top right. Tap cancel or the X will close the modal.&lt;/li&gt;&lt;li&gt;Here you will see information about the class and the Class Masteries.&lt;/li&gt;&lt;li&gt;Tap Manage Specialties.&lt;/li&gt;&lt;li&gt;Equip a specialty and boom done, now you just have to kill creatures.&lt;/li&gt;&lt;li&gt;The server messages will tell you when you gain levels in your Masteries and your Specialties as well as your Class Rank.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Now you just have to kill creatures till you meet the requirements.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Gamble the horror away</t>
@@ -1174,10 +1174,10 @@
   <cols>
     <col min="1" max="1" width="3.428" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="54.13" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="1886.254" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="2760.469" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="2470.254" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="2787.605" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="1890.967" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="2741.473" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="2512.672" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="2810.028" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="18.71" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="24.708" bestFit="true" customWidth="true" style="0"/>

</xml_diff>

<commit_message>
More guide quests are fix. 6 left to do
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -569,13 +569,13 @@
     <t>Take the edge off</t>
   </si>
   <si>
-    <t>You still have no answers. You are no closer to understanding your place in all of this.&lt;br /&gt; &lt;br /&gt; You decide to shake it off and focus on other things. Hunting stronger creatures. There were rumors down in Shadow Planes about a special location called Gold Mine where shards drop. You think back about when you learned alchemy and how it helped you kind of feel stronger, more competent and less fearful of the world around you.&lt;br /&gt; &lt;br /&gt; Maybe there is something you could make that would take he edge off. Make you feel strong and less confused.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Let’s level Alchemy some more and focus on our kingdom that we have since just abandoned. We need to protect and grow our home so we can eventually take our hard earned gold and create something called Gold Bars.&lt;/p&gt;&lt;p&gt;Gold Bars can be used in the &lt;a href="/information/goblin-shop" target="_blank"&gt;Goblin Shop&lt;/a&gt; to buy alchemist items that can make crafting easier and give your character XP boosts, these cost Gold Bars.&lt;/p&gt;&lt;p&gt;Each Gold bar costs 2 Billion Gold to make, and a kingdom can hold 1000 of them. Gold bars are also used later in the game for &lt;a href="/information/seer-camp" target="_blank"&gt;Socketing&lt;/a&gt; &lt;a href="/information/gems" target="_blank"&gt;Gems&lt;/a&gt; in to your gear to take on &lt;a href="/information/raids" target="_blank"&gt;Raid&lt;/a&gt; Bosses and for &lt;a href="/information/player-vs-player" target="_blank"&gt;PVP&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;Players will want well defended kingdoms to protect their loot. If you loose a kingdom, you also loose the Gold Bars.&lt;/p&gt;&lt;p&gt;Be careful when buying population and being over populated, The Old Man will take your Gold Bars as payment.&lt;/p&gt;&lt;p&gt;Since we last left our kingdom we unlocked the Goblin Coin bank. Now we want to continue on and upgrade a skill as well as recruit more units.&lt;/p&gt;&lt;p&gt;This one will take a while. Let’s set up some exploration in Gold Mines to get lots of shards and set up Auto Disenchant in our &lt;a href="/information/settings" target="_blank"&gt;settings&lt;/a&gt; so we also get a steady flow of Gold Dust, which will also require some looting.&lt;/p&gt;&lt;p&gt;We got work to do.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Super simple, but time consuming:&lt;/p&gt;&lt;p&gt;- Level the Goblin Bank in one of your kingdoms to the desired level, doesn’t matter which kingdom.&lt;/p&gt;&lt;p&gt;- Train your class Skill, this will be a skill under training skills that is orange and has an icon beside it.&lt;/p&gt;&lt;p&gt;- Your class skill is responsible for raising specific attributes about your character such as damage, armour and healing. Your class skill can also raise something called Class Bonus, each class a specific special attack that fires off based on your class bonus which is based on your class skill level. Each class in the game has it’s own class skill, if you switch classes, you have to level it’s skill from scratch if it’s a new class you have not previous leveled.&lt;/p&gt;&lt;p&gt;- Setup exploration in Gold Mines in Shadow Planes&lt;/p&gt;&lt;p&gt;- Craft Alchemy until the desired level.&lt;/p&gt;&lt;p&gt;- Once you have a Goblin Bank at the desired level, use the Goblin Bank Action in the kingdom you leveled the Goblin bank in, to then create the required amount of gold bars.&lt;/p&gt;</t>
+    <t>You still have no answers. You are no closer to understanding your place in all of this.&lt;br /&gt; &lt;br /&gt; You decide to shake it off and focus on other things. Hunting stronger creatures. There were rumors down in Shadow Planes about a special location called Gold Mine where shards drop. You think back to when you learned alchemy and how it &lt;br /&gt; helped you kind of feel stronger, more competent, and less fearful of the world around you.&lt;br /&gt; &lt;br /&gt; Maybe there is something you could make that would take the edge off. Make you feel strong and less confused.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Let’s level Alchemy some more and focus on our kingdom that we have since just abandoned. We need to protect and grow our home so we can eventually take our hard-earned gold and create something called Gold Bars.&lt;/p&gt;&lt;p&gt;Gold Bars can be used in the &lt;a href="/information/goblin-shop" target="_blank"&gt;Goblin Shop&lt;/a&gt; to buy alchemist items that can make crafting easier and give your character XP boosts; these cost Gold Bars.&lt;/p&gt;&lt;p&gt;Each Gold bar costs 2 Billion Gold to make, and a kingdom can hold 1000 of them. Gold bars are also used later in the game for &lt;a href="/information/seer-camp" target="_blank"&gt;Socketing Gems&lt;/a&gt; into your gear to take on &lt;a href="/information/raids" target="_blank"&gt;Raid&lt;/a&gt; Bosses and for &lt;a href="/information/player-vs-player" target="_blank"&gt;PVP&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;Players will want well-defended kingdoms to protect their loot. If you lose a kingdom, you also lose the Gold Bars.&lt;/p&gt;&lt;p&gt;Be careful when buying population and being overpopulated; The Old Man will take your Gold Bars as payment.&lt;/p&gt;&lt;p&gt;Since we last left our kingdom, we unlocked the Goblin Coin bank. Now we want to continue and upgrade a skill as well as recruit more units.&lt;/p&gt;&lt;p&gt;This one will take a while. Let’s set up some exploration in Gold Mines to get lots of shards and set up Auto Disenchant in our &lt;a href="/information/settings" target="_blank"&gt;settings&lt;/a&gt; so we also get a steady flow of Gold Dust, which will also require some looting.&lt;/p&gt;&lt;p&gt;We got work to do.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Super simple, but time-consuming:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Level the Goblin Bank in one of your kingdoms to the desired level; it doesn’t matter which kingdom.&lt;/li&gt;&lt;li&gt;Train your class Skill; this will be a skill under training skills that is orange and has an icon beside it.&lt;/li&gt;&lt;li&gt;Your class skill is responsible for raising specific attributes about your character such as damage, armor, and healing. Your class skill can also raise something called Class Bonus; each class has a specific special attack that fires off based on your class bonus, which is based on your class skill level. Each class in the game has its own class skill. If you switch classes, you have to level its skill from scratch if it’s a new class you have not previously leveled.&lt;/li&gt;&lt;li&gt;Set up exploration in Gold Mines in Shadow Planes.&lt;/li&gt;&lt;li&gt;Craft Alchemy until the desired level.&lt;/li&gt;&lt;li&gt;Once you have a Goblin Bank at the desired level, use the Goblin Bank Action in the kingdom you leveled the Goblin bank in to create the required amount of gold bars.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>Winter has come to Tlessa!</t>
@@ -584,13 +584,13 @@
     <t>“Child!” Comes a call and a hail.&lt;br /&gt; &lt;br /&gt; It’s The Guide as he walks down the trail to greet you. “I know you have been busy and probably are busy with some errand or task or some such, but I have something I wanted to show you!”&lt;br /&gt; &lt;br /&gt; You ask him what it is and he smiles: “Something magical! Winter has finally come to Tlessa!”&lt;br /&gt; &lt;br /&gt; Winter has come?</t>
   </si>
   <si>
-    <t>&lt;p&gt;That’s right! Winter has come and with it has come a new map that is only available during The Winter Event which is currently running!&lt;/p&gt;&lt;p&gt;I wanted to take a moment to get you situated with the new event before returning you to your regular scheduled programming!&lt;/p&gt;&lt;p&gt;With the winter event comes a new set of story based quests, slight harder creatures and even harder creatures for those in more later stages of the game. Whats really fun down here is that players can work together to earn Top end gear! Doesn’t matter your level.&lt;/p&gt;&lt;p&gt;You might be worried, Hey I am new and you are just handing out end game gear? Don’t worry my child, it’s all percent based, so even a +250% Strength item will do nothing for you 14 Strength, but as you level and that base 14 strength becomes 1000 strength – now the item is helping you. Item’s scale in Tlessa as you level.&lt;/p&gt;&lt;p&gt;These items that I reward players with for participating in whats called a global event – which only happens on the map you are going to – come with something called Uniques, which also limits players to only be able to equip one of the items that you are rewarded with, due to the rules: Players may only equip one Unique or Mythic (but not both).&lt;/p&gt;&lt;p&gt;Enough explanation! Lets get you on this map and participating!&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Traversing is how we move from one plane to another. Special events such as this one will allow players regardless of level to traverse to to the map, while other maps might require quest items or quests to be completed.&lt;/p&gt;&lt;p&gt;- Click Traverse under the map&lt;/p&gt;&lt;p&gt;- Select The Ice Plane&lt;/p&gt;&lt;p&gt;- Click Traverse.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Traversing is how we move from one plane to another. Special events such as this one will allow players regardless of level to traverse to to the map, while other maps might require quest items or quests to be completed.&lt;/p&gt;&lt;p&gt;- Select Map Move from the Action Drop down&lt;/p&gt;&lt;p&gt;- Tap Traverse under the map&lt;/p&gt;&lt;p&gt;- Select The Ice Plane&lt;/p&gt;&lt;p&gt;- Tap Traverse.&lt;/p&gt;</t>
+    <t>&lt;p&gt;That’s right! Winter has come, and with it, a new map is available during The Winter Event, which is currently running!&lt;/p&gt;&lt;p&gt;I wanted to take a moment to get you situated with the new event before returning you to your regularly scheduled programming!&lt;/p&gt;&lt;p&gt;With the winter event comes a new set of story-based quests, slightly harder creatures, and even harder creatures for those in more later stages of the game. What's really fun down here is that players can work together to earn top-end gear! It &lt;/p&gt;&lt;p&gt;doesn’t matter your level.&lt;/p&gt;&lt;p&gt;You might be worried, "Hey, I am new, and you are just handing out end game gear?" Don’t worry, my child, it’s all percent-based, so even a +250% Strength item will do nothing for your 14 Strength, but as you level and that base 14 strength &lt;/p&gt;&lt;p&gt;becomes 1000 strength – now the item is helping you. Items scale in Tlessa as you level.&lt;/p&gt;&lt;p&gt;These items that I reward players with for participating in what's called a global event – which only happens on the map you are going to – come with something called Uniques, which also limits players to only be able to equip one of the items that &lt;/p&gt;&lt;p&gt;you are rewarded with, due to the rules: Players may only equip one Unique or Mythic (but not both).&lt;/p&gt;&lt;p&gt;Enough explanation! Let’s get you on this map and participating!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Traversing is how we move from one plane to another. Special events such as this one will allow players, regardless of level, to traverse to the map, while other maps might require quest items or quests to be completed.&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Click Traverse under the map.&lt;/li&gt;&lt;li&gt;Select The Ice Plane.&lt;/li&gt;&lt;li&gt;Click Traverse.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Traversing is how we move from one plane to another. Special events such as this one will allow players, regardless of level, to traverse to the map, while other maps might require quest items or quests to be completed.&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Select Map Move from the Action Drop down.&lt;/li&gt;&lt;li&gt;Tap Traverse under the map.&lt;/li&gt;&lt;li&gt;Select The Ice Plane.&lt;/li&gt;&lt;li&gt;Tap Traverse.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>The Ice Plane</t>
@@ -599,28 +599,28 @@
     <t>Working together in the chill</t>
   </si>
   <si>
-    <t>You shiver as you enter into a new world covered in Ice. The snow falls in a gentle breeze and the world is silent.&lt;br /&gt; &lt;br /&gt; “Child.” You jump in your spot as The Guide startles you. He pays no heed of this and continues.&lt;br /&gt; &lt;br /&gt; “Welcome to The Ice Plane! Down here you’ll notice that creatures are a hit stronger, but nothing you can’t handle. Just don’t be so hasty to take on the strongest critter, you might also find what you hunted on Surface might be a bit stronger down here!”&lt;br /&gt; &lt;br /&gt; You look out at the barren, frozen wind swept waste land covered in ice and wonder what could be out there. What adventures await you?</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Now that we made it to The Ice Plane – lets start killing things. You’ll notice on your map (for desktop) there is a new Event Goal tab. For Mobile, you can see this by opening the Map Movement fro the main Action Drop down.&lt;/p&gt;&lt;p&gt;Here you will see an over all creature kill which then broken down into phases that increase by 1,000.&lt;/p&gt;&lt;p&gt;By working together either using exploration or manual fighting players can increase the bars and get rewarded for completing each phase.&lt;/p&gt;&lt;p&gt;To be rewarded you will see a “Amount of kills required to gain phase reward”, this is based on the average number of players on the map participating and their total kill count versus what you need to kill in order to gain a reward. Essentially its the average.&lt;/p&gt;&lt;p&gt;Below this you will see your total kills. This amount will reset to 0 once all phases are complete and the global Event Goal resets.&lt;/p&gt;&lt;p&gt;Lets help others out and get a reward shall we?!&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;This quest might get you a phase reward and might not. It depends when you do it and how far the main progress bar has moved. If the bar is close to being completed, the Event Goal will reset allowing players to participate again. The reset of this bar is hourly if it has been completely filled.&lt;/p&gt;&lt;p&gt;- Select any monster that you can kill in one hit.&lt;/p&gt;&lt;p&gt;- Participate by either using exploration or manual fighting&lt;/p&gt;&lt;p&gt;- Earn the required amount of points.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;This quest might get you a phase reward and might not. It depends when you do it and how far the main progress bar has moved. If the bar is close to being completed, the Event Goal will reset allowing players to participate again. The reset of this bar is hourly if it has been completely filled.&lt;/p&gt;&lt;p&gt;- Select any monster that you can kill in one hit.&lt;/p&gt;&lt;p&gt;- Participate by either using exploration or manual fighting&lt;/p&gt;&lt;p&gt;- Earn the required amount of points.&lt;/p&gt;&lt;p&gt;- Select The Ice Plane&lt;/p&gt;&lt;p&gt;- Tap Traverse.&lt;/p&gt;</t>
+    <t>You shiver as you enter into a new world covered in Ice. The snow falls in a gentle breeze, and the world is silent.&lt;br /&gt; &lt;br /&gt; “Child.” You jump in your spot as The Guide startles you. He pays no heed to this and continues.&lt;br /&gt; &lt;br /&gt; “Welcome to The Ice Plane! Down here you’ll notice that creatures are a bit stronger, but nothing you can’t handle. Just don’t be so hasty to take on the strongest critter; you might also find what you hunted on Surface might be a bit stronger down here!”&lt;br /&gt; &lt;br /&gt; You look out at the barren, frozen, wind-swept wasteland covered in ice and wonder what could be out there. What adventures await you?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Now that we made it to The Ice Plane – let's start killing things. You’ll notice on your map (for desktop) there is a new Event Goal tab. For Mobile, you can see this by opening the Map Movement from the main Action Drop down.&lt;/p&gt;&lt;p&gt;Here you will see an overall creature kill which is then broken down into phases that increase by 1,000.&lt;/p&gt;&lt;p&gt;By working together either using exploration or manual fighting, players can increase the bars and get rewarded for completing each phase.&lt;/p&gt;&lt;p&gt;To be rewarded, you will see an “Amount of kills required to gain phase reward,” this is based on the average number of players on the map participating and their total kill count versus what you need to kill in order to gain a reward. Essentially it's the average.&lt;/p&gt;&lt;p&gt;Below this, you will see your total kills. This amount will reset to 0 once all phases are complete and the global Event Goal resets.&lt;/p&gt;&lt;p&gt;Let's help others out and get a reward, shall we?!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This quest might get you a phase reward and might not. It depends on when you do it and how far the main progress bar has moved. If the bar is close to being completed, the Event Goal will reset, allowing players to participate again. The reset of this bar is hourly if it has been completely filled.&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Select any monster that you can kill in one hit.&lt;/li&gt;&lt;li&gt;Participate by either using exploration or manual fighting.&lt;/li&gt;&lt;li&gt;Earn the required amount of points.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This quest might get you a phase reward and might not. It depends on when you do it and how far the main progress bar has moved. If the bar is close to being completed, the Event Goal will reset, allowing players to participate again. The reset of this bar is hourly if it has been completely filled.&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Select any monster that you can kill in one hit.&lt;/li&gt;&lt;li&gt;Participate by either using exploration or manual fighting.&lt;/li&gt;&lt;li&gt;Earn the required amount of points.&lt;/li&gt;&lt;li&gt;Select The Ice Plane.&lt;/li&gt;&lt;li&gt;Tap Traverse.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>Who is The Ice Queen?</t>
   </si>
   <si>
-    <t>The last of the critters falls and the snow around you is covered I blood. You release a sight of relief as the silence falls over the land and the snow continues to fall slowly burying the bodies of the enemies before you.&lt;br /&gt; &lt;br /&gt; You stand for a moment in the silence of the falling snow before heading off towards a rumored wreck where it is said the Ice Queen has originated from.&lt;br /&gt; &lt;br /&gt; The Guide has not been seen in the last few days. He did mention something about a location called The Fathers tomb, but didn’t indicate which direction it was.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Let’s complete some of the story based &lt;a href="/information/quests" target="_blank"&gt;quests&lt;/a&gt; of this event and unlock other locations that progress the story of this map.&lt;/p&gt;&lt;p&gt;Story in Tlessa is done through quests. Quests also unlock features of the game and allow you to progress beyond level 1,000.&lt;/p&gt;&lt;p&gt;One this specific event map, which is only available during this event – once per year – there is a story that is told in a specific order which when complete tells an over arching story of who The Ice Queen in and why this plane is frozen.&lt;/p&gt;&lt;p&gt;Quests will always tell you how to complete them with specific instructions listed in the requirements section of the quest it’s self.&lt;/p&gt;&lt;p&gt;You can see the quests by tapping or clicking on the Quest tab. Red quests are ones that cannot be completed yet until the parent is completed. Blue quests can be completed provided you meet the requirements.&lt;/p&gt;&lt;p&gt;Green Quests are ones you have completed. All quests have a Before and After completion story which progresses the over all story of the game forward.&lt;/p&gt;&lt;p&gt;Lets participate in the event maps quests!&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;We will complete quests until we have completed the above required quest. To do this simply click on the quest tab, click the first quest – click the required tab and click on the help icons to see how to get each item.&lt;/p&gt;&lt;p&gt;In event maps, characters will just fight monsters – manually – at specific locations, known as special locations, to then gain the items at random chance.&lt;/p&gt;</t>
+    <t>The last of the critters falls, and the snow around you is covered in blood. You release a sigh of relief as the silence falls over the land, and the snow continues to fall, slowly burying the bodies of the enemies before you.&lt;br /&gt; &lt;br /&gt; You stand for a moment in the silence of the falling snow before heading off towards a rumored wreck where it is said the Ice Queen has originated from.&lt;br /&gt; &lt;br /&gt; The Guide has not been seen in the last few days. He did mention something about a location called The Fathers tomb but didn’t indicate which direction it was.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Let’s complete some of the story-based &lt;a href="/information/quests" target="_blank"&gt;quests&lt;/a&gt; of this event and unlock other locations that progress the story of this map.&lt;/p&gt;&lt;p&gt;Story in Tlessa is done through quests. Quests also unlock features of the game and allow you to progress beyond level 1,000.&lt;/p&gt;&lt;p&gt;On this specific event map, which is only available during this event – once per year – there is a story that is told in a specific order, which when complete tells an overarching story of who The Ice Queen is and why this plane is frozen.&lt;/p&gt;&lt;p&gt;Quests will always tell you how to complete them with specific instructions listed in the requirements section of the quest itself.&lt;/p&gt;&lt;p&gt;You can see the quests by tapping or clicking on the Quest tab. Red quests are ones that cannot be completed yet until the parent is completed. Blue quests can be completed provided you meet the requirements.&lt;/p&gt;&lt;p&gt;Green Quests are ones you have completed. All quests have a Before and After completion story which progresses the overall story of the game forward.&lt;/p&gt;&lt;p&gt;Let's participate in the event map's quests!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We will complete quests until we have completed the above required quest. To do this simply click on the quest tab, click the first quest – click the required tab, and click on the help icons to see how to get each item.&lt;/p&gt;&lt;p&gt;In event maps, characters will just fight monsters – manually – at specific locations, known as &lt;a href="/information/special-locations" target="_blank"&gt;special locations&lt;/a&gt;, to then gain the items at random chance.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Frozen in time</t>
@@ -632,7 +632,7 @@
     <t>The more you learn about The Queen and who she is to The Creator, the more curious you get. As you are about to set out exploring the world and helping those who have need of your skill set, you see The Guide approach the wreck.&lt;br /&gt; &lt;br /&gt; “She died here …” he states as he approaches and stands before you.&lt;br /&gt; &lt;br /&gt; You both stand in the silence of the falling snow as the winds pick up and the bitter chill of this frozen land sets in.&lt;br /&gt; &lt;br /&gt; “You should continue on. Reach the house of the fathers tomb. It will make more sense.”&lt;br /&gt; &lt;br /&gt; You stare at him for a moment and then look off into the distance.&lt;br /&gt; &lt;br /&gt; A grieving mother. A widow. You need to learn more.</t>
   </si>
   <si>
-    <t>&lt;p&gt;By now we know how to complete quests and participate in the events story and its event goals. So lets continue putting that together and push more of the story as well as participate more in the event goals.&lt;/p&gt;&lt;p&gt;The Quest you will complete will give you a &lt;a href="/information/quest-items" target="_blank"&gt;quest item&lt;/a&gt;, which is used automatically, to allow you to walk on Ice while down here.&lt;/p&gt;</t>
+    <t>&lt;p&gt;By now, we know how to complete quests and participate in the event's story and its event goals. So let's continue putting that together and push more of the story as well as participate more in the event goals.&lt;/p&gt;&lt;p&gt;The Quest you will complete will give you a &lt;a href="/information/quest-items" target="_blank"&gt;quest item&lt;/a&gt;, which is used automatically, to allow you to walk on Ice while down here.&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Continue to kill creatures and participate in the quest line until the desired goals are reached.&lt;/p&gt;</t>
@@ -659,16 +659,16 @@
     <t>Ruling The Ice Plane</t>
   </si>
   <si>
-    <t>“You are learning who she is.” The Guide Whispers as you two walk side by side in the falling snow, seeking out a warm shelter to hunker down in.&lt;br /&gt; &lt;br /&gt; You take a moment and reflect back on the adventure you have been on while on this plane of existence. The pain, the hurt, the loss – all of it.&lt;br /&gt; &lt;br /&gt; “She is frozen in her own her own grief, unable to let go and completely blinded by it. Such that it turns her wrathful.”&lt;br /&gt; &lt;br /&gt; You say nothing and give no indication to The Guide that you heard him, but by the long stare in your eyes, he knows what you know – you have to let go to move on.&lt;br /&gt; &lt;br /&gt; Moments go by and eventually a small ramshackle hut appears on the snowy horizon. You both head in that direction, longing to get out of the snow – maybe start a fire and get warm.&lt;br /&gt; &lt;br /&gt; “You could settle here.”&lt;br /&gt; &lt;br /&gt; You look over at him and then around at the night covered, snow covered frozen waste land.&lt;br /&gt; &lt;br /&gt; Why?</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;We are going to learn about kingdoms with this quest. You can, for this quest, settle any where you want – either here or on surface. Ideally though you would want to settle down here, for one specific reason: &lt;strong&gt;The Player with the most kingdoms will win a full set of &lt;/strong&gt;&lt;a href="/information/corrupted-ice" target="_blank"&gt;&lt;strong&gt;Corrupted Ice&lt;/strong&gt;&lt;/a&gt;&lt;strong&gt; gear at the end of event.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;You have a few pieces that are Unique by now – and as stated when we started this adventure, you could only equip one of those. With this prize, they come with no enchants allowing players to modify the gear to their liking.&lt;/p&gt;&lt;p&gt;For new players who have not maxed out &lt;a href="/information/enchanting" target="_blank"&gt;enchanting&lt;/a&gt;, it is suggested, if you win this gear, to not enchant it until you have maxed out enchanting as you could end up destroying the gear you worked so hard to get.&lt;/p&gt;&lt;p&gt;Kingdoms are a passive way of doing PVP, you can settle a kingdom any where you can move, with the exception of settling on locations or with in one space of a location in all directions.&lt;/p&gt;&lt;p&gt;You can also train &lt;a href="/information/kingdom-passive-skills" target="_blank"&gt;Kingdom Passives&lt;/a&gt; to unlock new buildings, units and passive buffs for your kingdoms.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt;&lt;em&gt; This quest wants you to have a kingdom at a specific level, this means level the buildings, one or more, to the required level such that all buildings combined meet the required level.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Complete the required quest to unlock the ability to settle a kingdom on this plane.&lt;/p&gt;&lt;p&gt;To settle a kingdom:&lt;/p&gt;&lt;p&gt;- Click Settle under the map, name the kingdom and click settle button.&lt;/p&gt;&lt;p&gt;- Click Kingdoms tab&lt;/p&gt;&lt;p&gt;- Click on your kingdom.&lt;/p&gt;&lt;p&gt;Here you can recruit units with gold or with resources, purchase additional population and manage your kingdom.&lt;/p&gt;&lt;p&gt;It should be noted that unlike Surface or other maps, due to the competitive nature of this Event specific map, kingdoms down here will not come with a seven day protection applied.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Passive&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;This quest also wants you to train a passive, these take real world hours to complete and provide bonuses your kingdoms across all planes.&lt;/p&gt;&lt;p&gt;To do this, head to your Character Sheet tab and under Skills, you will see a tab called Kingdom Passives. Here you will see a tree of skills, click the first one and click train. This will create a timer that will count down until the passive is trained to the next level.&lt;/p&gt;&lt;p&gt;You can logout and the timer will run behind the scenes.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; &lt;em&gt;This quest wants you to have a kingdom at a specific level, this means level the buildings, one or more, to the required level such that all buildings combined meet the required level.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Complete the required quest to unlock the ability to settle a kingdom on this plane.&lt;/p&gt;&lt;p&gt;To settle a kingdom:&lt;/p&gt;&lt;p&gt;- Select Map Movement From the Action drop down.&lt;/p&gt;&lt;p&gt;- Tap on settle after moving to a valid location.&lt;/p&gt;&lt;p&gt;- Name the kingdom and tap Settle.&lt;/p&gt;&lt;p&gt;- Tap the kingdom tab at the top to see your settled kingdoms.&lt;/p&gt;&lt;p&gt;- Here you can tap on a kingdom you want to manage and then either select from the drop down:&lt;/p&gt;&lt;p&gt;- Building Management or Unit Management to recruit Units and upgrade buildings.&lt;/p&gt;&lt;p&gt;- You can expand the Kingdom Details section to see additional information about your kingdom as well as additional actions such as purchasing population.&lt;/p&gt;&lt;p&gt;It should be noted that unlike Surface or other maps, due to the competitive nature of this Event specific map, kingdoms down here will not come with a seven day protection applied.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Passive&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;This quest also wants you to train a passive, these take real world hours to complete and provide bonuses your kingdoms across all planes.&lt;/p&gt;&lt;p&gt;To do this, tap the character sheet tab, select Skill Management from the drop down.&lt;/p&gt;&lt;p&gt;Here you will see a tab called Kingdom Passives.&lt;/p&gt;&lt;p&gt;Tapping the tab will show you a tree of skills, tap the first one and tap train. This will create a timer that will count down until the passive is trained to the next level.&lt;/p&gt;&lt;p&gt;You can logout and the timer will run behind the scenes.&lt;/p&gt;</t>
+    <t>“You are learning who she is.” The Guide whispers as you two walk side by side in the falling snow, seeking out a warm shelter to hunker down in.&lt;br /&gt; &lt;br /&gt; You take a moment and reflect back on the adventure you have been on while on this plane of existence. The pain, the hurt, the loss – all of it.&lt;br /&gt; &lt;br /&gt; “She is frozen in her own grief, unable to let go and completely blinded by it. Such that it turns her wrathful.”&lt;br /&gt; &lt;br /&gt; You say nothing and give no indication to The Guide that you heard him, but by the long stare in your eyes, he knows what you know – you have to let go to move on.&lt;br /&gt; &lt;br /&gt; Moments go by and eventually a small ramshackle hut appears on the snowy horizon. You both head in that direction, longing to get out of the snow – maybe start a fire and get warm.&lt;br /&gt; &lt;br /&gt; “You could settle here.”&lt;br /&gt; &lt;br /&gt; You look over at him and then around at the night-covered, snow-covered frozen wasteland.&lt;br /&gt; &lt;br /&gt; Why?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We are going to learn about kingdoms with this quest. You can, for this quest, settle anywhere you want – either here or on the surface. Ideally, though, you would want to settle down here, for one specific reason: The player with the most kingdoms will &lt;strong&gt;win a full set of &lt;/strong&gt;&lt;a href="/information/corrupted-ice" target="_blank"&gt;&lt;strong&gt;Corrupted Ice&lt;/strong&gt;&lt;/a&gt;&lt;strong&gt; gear at the end of the event&lt;/strong&gt;.&lt;/p&gt;&lt;p&gt;You have a few pieces that are Unique by now – and as stated when we started this adventure, you could only equip one of those. With this prize, they come with no enchants allowing players to modify the gear to their liking.&lt;/p&gt;&lt;p&gt;For new players who have not maxed out &lt;a href="/information/enchanting" target="_blank"&gt;enchanting&lt;/a&gt;, it is suggested, if you win this gear, to not enchant it until you have maxed out enchanting as you could end up destroying the gear you worked so hard to get.&lt;/p&gt;&lt;p&gt;Kingdoms are a passive way of doing PVP, you can settle a kingdom anywhere you can move, with the exception of settling on locations or within one space of a location in all directions.&lt;/p&gt;&lt;p&gt;You can also train &lt;a href="/information/kingdom-passive-skills" target="_blank"&gt;Kingdom Passives&lt;/a&gt; to unlock new buildings, units, and passive buffs for your kingdoms.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;:&lt;em&gt; This quest wants you to have a kingdom at a specific level; this means level the buildings, one or more, to the required level such that all buildings combined meet the required level.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Complete the required quest to unlock the ability to settle a kingdom on this plane.&lt;/p&gt;&lt;p&gt;To settle a &lt;a href="/information/kingdoms" target="_blank"&gt;kingdom&lt;/a&gt;:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Click Settle under the map, name the kingdom and click the settle button.&lt;/li&gt;&lt;li&gt;Click Kingdoms tab&lt;/li&gt;&lt;li&gt;Click on your kingdom.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Here you can recruit units with gold or with resources, purchase additional population and manage your kingdom.&lt;/p&gt;&lt;p&gt;It should be noted that unlike Surface or other maps, due to the competitive nature of this Event-specific map, kingdoms down here will not come with a seven-day protection applied.&lt;/p&gt;&lt;p&gt;&lt;a href="/information/kingdom-passive-skills" target="_blank"&gt;&lt;strong&gt;Passive&lt;/strong&gt;&lt;/a&gt;&lt;/p&gt;&lt;p&gt;This quest also wants you to train a passive; these take real-world hours to complete and provide bonuses to your kingdoms across all planes.&lt;/p&gt;&lt;p&gt;To do this, head to your Character Sheet tab and under Skills, you will see a tab called Kingdom Passives. Here you will see a tree of skills, click the first one and click train. This will create a timer that will count down until the passive is trained to &lt;/p&gt;&lt;p&gt;the next level.&lt;/p&gt;&lt;p&gt;You can log out and the timer will run behind the scenes.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;:&lt;em&gt; This quest wants you to have a kingdom at a specific level; this means level the buildings, one or more, to the required level such that all buildings combined meet the required level.&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Complete the required quest to unlock the ability to settle a kingdom on this plane.&lt;/p&gt;&lt;p&gt;To settle a &lt;a href="/information/kingdoms" target="_blank"&gt;kingdom&lt;/a&gt;:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Select Map Movement From the Action drop down.&lt;/li&gt;&lt;li&gt;Tap on settle after moving to a valid location.&lt;/li&gt;&lt;li&gt;Name the kingdom and tap Settle.&lt;/li&gt;&lt;li&gt;Tap the kingdom tab at the top to see your settled kingdoms.&lt;/li&gt;&lt;li&gt;Here you can tap on a kingdom you want to manage and then either select from the drop down:&lt;/li&gt;&lt;li&gt;Building Management or Unit Management to recruit Units and upgrade buildings.&lt;/li&gt;&lt;li&gt;You can expand the Kingdom Details section to see additional information about your kingdom as well as additional actions such as purchasing population.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;It should be noted that unlike Surface or other maps, due to the competitive nature of this Event-specific map, kingdoms down here will not come with a seven-day protection applied.&lt;/p&gt;&lt;p&gt;&lt;a href="/information/kingdom-passive-skills" target="_blank"&gt;&lt;strong&gt;Passive&lt;/strong&gt;&lt;/a&gt;&lt;/p&gt;&lt;p&gt;This quest also wants you to train a passive; these take real-world hours to complete and provide bonuses to your kingdoms across all planes.&lt;/p&gt;&lt;p&gt;To do this, tap the character sheet tab, select Skill Management from the drop down.&lt;/p&gt;&lt;p&gt;Here you will see a tab called Kingdom Passives.&lt;/p&gt;&lt;p&gt;Tapping the tab will show you a tree of skills, tap the first one and tap train. This will create a timer that will count down until the passive is trained to the next level.&lt;/p&gt;&lt;p&gt;You can log out, and the timer will run behind the scenes.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Reuniting Two Old Flames</t>
@@ -677,13 +677,13 @@
     <t>Hell's Gates Swing Open</t>
   </si>
   <si>
-    <t>The days have gone by, the moon has rose and fallen and the sun rises and sets. The days bleed together and the lands become a blur. Slaughter, kill, loot, steal – repeat.&lt;br /&gt; &lt;br /&gt; You study the books of The Witch who lives on Labyrinth. Her books tell stories of The Church, back when The Red Hawks – a group of rebels – stood against The Federation. But it also tells stories of the alchemical concoctions and the twisted corrupted magics these Priests manage to create.&lt;br /&gt; &lt;br /&gt; You study the research, the formulas and the recipes hoping for some glimmer of the past to be the answer you want, your involvement in all of this, your responsible for The Creator escaping Purgatory, how are you responsible for something you played no part in?&lt;br /&gt; &lt;br /&gt; You look up from your studies and see the shadows of the flames dance in the fire place before you.&lt;br /&gt; &lt;br /&gt; Sitting in the study of your keep, high above the kingdom you have settled. The wars you have waged, the battles you have fought, the blood that stains your hands. You stare into the depths of hell it’s self.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Let’s go to Hell. Literally.&lt;/p&gt;&lt;p&gt;Hell is where the &lt;a href="/information/random-enchants" target="_blank"&gt;Queen of Hearts&lt;/a&gt; lives, she allows you to re-roll Uniques and Mythics as well as transfer those enchantments from one price of gear to another.&lt;/p&gt;&lt;p&gt;Shadow Planes was the first plane that slightly reduces you in power and slightly makes the creatures harder. You have discovered this from completing quests that require you to get items from specific locations also known as special locations. These types of locations would make creatures slightly harder.&lt;/p&gt;&lt;p&gt;At this stage, you should have a full set of crafting level 400 gear which contains enchantment level 400 enchantments.&lt;/p&gt;&lt;p&gt;Hell is also where you can start getting your end game gear: &lt;a href="/information/hell-forged-set" target="_blank"&gt;Hell Forged&lt;/a&gt;, who’s base stats are better then level 400 non enchanted gear.&lt;/p&gt;&lt;p&gt;For now, let’s focus on going to Hell.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;We already know how to complete quests at this stage – so lets continue questing!&lt;/p&gt;&lt;p&gt;To get to hell and therefore get access to The Queen of Hearts, we need to complete two quests:&lt;/p&gt;&lt;p&gt;- Hells gates&lt;/p&gt;&lt;p&gt;- Queens Decision&lt;/p&gt;&lt;p&gt;The first Quest gets us into Hell, and the second quest will allow us access to The Queen of Hearts.&lt;/p&gt;&lt;p&gt;So what are you waiting for? Let’s go to Hell!&lt;/p&gt;</t>
+    <t>The days have gone by, the moon has risen and fallen, and the sun rises and sets. The days bleed together, and the lands become a blur. Slaughter, kill, loot, steal – repeat.&lt;br /&gt; &lt;br /&gt; You study the books of The Witch who lives on Labyrinth. Her books tell stories of The Church, back when The Red Hawks – a group of rebels – stood against The Federation. But they also tell stories of the alchemical concoctions and the twisted &lt;br /&gt; corrupted magics these Priests managed to create.&lt;br /&gt; &lt;br /&gt; You study the research, the formulas, and the recipes, hoping for some glimmer of the past to be the answer you want. Your involvement in all of this, your responsibility for The Creator escaping Purgatory – how are you responsible for something &lt;br /&gt; you played no part in?&lt;br /&gt; &lt;br /&gt; You look up from your studies and see the shadows of the flames dance in the fireplace before you.&lt;br /&gt; &lt;br /&gt; Sitting in the study of your keep, high above the kingdom you have settled. The wars you have waged, the battles you have fought, the blood that stains your hands. You stare into the depths of hell itself.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Let’s go to Hell. Literally.&lt;/p&gt;&lt;p&gt;Hell is where the &lt;a href="/information/random-enchants" target="_blank"&gt;Queen of Hearts&lt;/a&gt; lives; she allows you to re-roll Uniques and Mythics as well as transfer those enchantments from one piece of gear to another.&lt;/p&gt;&lt;p&gt;Shadow Planes was the first plane that slightly reduces your power and slightly makes the creatures harder. You have discovered this from completing quests that require you to get items from specific locations, also known as special locations. &lt;/p&gt;&lt;p&gt;These types of locations would make creatures slightly harder.&lt;/p&gt;&lt;p&gt;At this stage, you should have a full set of crafting level 400 gear which contains enchantment level 400 enchantments.&lt;/p&gt;&lt;p&gt;Hell is also where you can start getting your end game gear: &lt;a href="/information/hell-forged-set" target="_blank"&gt;Hell Forged&lt;/a&gt;, whose base stats are better than level 400 non-enchanted gear.&lt;/p&gt;&lt;p&gt;For now, let’s focus on going to Hell.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We already know how to complete quests at this stage – so let’s continue questing!&lt;/p&gt;&lt;p&gt;To get to hell and therefore get access to The Queen of Hearts, we need to complete two quests:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Hells gates&lt;/li&gt;&lt;li&gt;Queens Decision&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;The first Quest gets us into Hell, and the second quest will allow us access to The Queen of Hearts.&lt;/p&gt;&lt;p&gt;So what are you waiting for? Let’s go to Hell!&lt;/p&gt;</t>
   </si>
   <si>
     <t>Hell</t>
@@ -698,16 +698,16 @@
     <t>Dressing up for The Queen</t>
   </si>
   <si>
-    <t>The heat of the land wafts over you, the sounds of death haunt you. You look around and see a barren waste land of loneliness and hollow soulless screams that ride on a dead wind.&lt;br /&gt; &lt;br /&gt; You heard the stories of gear that was once forged in the depths of Hell it’s self. You have heard the songs of The Queen her self. She sings a lust-filled laughter laced song full of sexual tension and desire.&lt;br /&gt; &lt;br /&gt; You search out the one man you came to find, one man who is said to be hidden among the barren desolate waste land of hate filled souls. You search him out for the questions that rage in your veins. You search for The Guide.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Let’s investigate how to obtain a piece of &lt;a href="/information/hell-forged-set" target="_blank"&gt;Hell Forged&lt;/a&gt; gear. To do this, you will need to craft a level 400 piece of gear, but you should already have some, equipped.&lt;/p&gt;&lt;p&gt;Hell Forged gear allows you to then Trade it later on for Purgatory Chains gear. When you purchase a piece of Hell Forged gear, you will trade a piece of your gear and the currencies needed.&lt;/p&gt;&lt;p&gt;I want you to purchase your first piece of Hell Forged gear, I also want you to trade one of the equipped items you have. Unequip a level 400 item (or remove it from a set) and then Purchase a Hell Forged gear piece of that type, for example: Ring for Ring or Spell for Spell.&lt;/p&gt;&lt;p&gt;You will see that your enchantments will be transferred, for free, from your existing gear to the new Hell Forged gear piece. This way, all your hard work is not lost.&lt;/p&gt;&lt;p&gt;This is what we call: End Game gear. Your progression starts here, your next set will be &lt;a href="/information/purgatory-chains-set" target="_blank"&gt;Purgatory Chains&lt;/a&gt;, followed by &lt;a href="/information/pirate-lord-leather-set" target="_blank"&gt;Pirate Lord Leather&lt;/a&gt; and then &lt;a href="/information/corrupted-ice" target="_blank"&gt;Corrupted Ice&lt;/a&gt;. Each set gets slightly higher stats.&lt;/p&gt;&lt;p&gt;Purgatory Chains gear, your next set, can also be obtained the same way as Hell Forged, but only while on Purgatory.&lt;/p&gt;&lt;p&gt;Pirate Lord Leather can, at the time of this guide quest, only be obtained via defeating the raid boss in a Surface Raid.&lt;/p&gt;&lt;p&gt;Corrupted Ice gear can, at the time of this guide quest, only be obtained via participating in the Winter Event and being on the Ice Plane.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;First we need to manage our inventory and either unequip an item that you have which is crafting level 400, and make sure it’s in your inventory. You can also craft a level 400 item if you please instead, but this gets rather expensive, best to use one if you have one.&lt;/p&gt;&lt;p&gt;Next:&lt;/p&gt;&lt;p&gt;- In the Actions section you will see, while on Hell, a new button called: Hell Forged gear – click it.&lt;/p&gt;&lt;p&gt;- Next select a piece of gear that matches the item type in your inventory. For example – if you unequipped a level 400 ring, select a ring. If you crafted a level 400 Body piece, select Body.&lt;/p&gt;&lt;p&gt;- Click Purchase Item if you can afford, if not go earn the currencies.&lt;/p&gt;&lt;p&gt;- Now you should have a Hell Forged Item in your inventory, any enchants on the previous item are now transferred to this one.&lt;/p&gt;&lt;p&gt;- Equip it.&lt;/p&gt;&lt;p&gt;- Repeat for each item you have equipped that meets the requirements.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; This quest only cares about you doing one item. It is suggested you replace all your items with Hell Forged.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;First we need to manage our inventory and either unequip an item that you have which is crafting level 400, and make sure it’s in your inventory. You can also craft a level 400 item if you please instead, but this gets rather expensive, best to use one if you have one.&lt;/p&gt;&lt;p&gt;Next:&lt;/p&gt;&lt;p&gt;- From the Actions drop down, select: Hell Forged gear while in Hell.&lt;/p&gt;&lt;p&gt;- Next select a piece of gear that matches the item type in your inventory. For example – if you unequipped a level 400 ring, select a ring. If you crafted a level 400 Body piece, select Body.&lt;/p&gt;&lt;p&gt;- Click Purchase Item if you can afford, if not go earn the currencies.&lt;/p&gt;&lt;p&gt;- Now you should have a Hell Forged Item in your inventory, any enchants on the previous item are now transferred to this one.&lt;/p&gt;&lt;p&gt;- Equip it.&lt;/p&gt;&lt;p&gt;- Repeat for each item you have equipped that meets the requirements.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Note: &lt;/strong&gt;This quest only cares about you doing one item. It is suggested you replace all your items with Hell Forged.&lt;/p&gt;</t>
+    <t>The heat of the land wafts over you, the sounds of death haunt you. You look around and see a barren wasteland of loneliness and hollow soulless screams that ride on a dead wind.&lt;br /&gt; &lt;br /&gt; You've heard the stories of gear that was once forged in the depths of Hell itself. You have heard the songs of The Queen herself. She sings a lust-filled laughter-laced song full of sexual tension and desire.&lt;br /&gt; &lt;br /&gt; You search out the one man you came to find, one man who is said to be hidden among the barren desolate wasteland of hate-filled souls. You search him out for the questions that rage in your veins. You search for The Guide.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Let’s investigate how to obtain a piece of &lt;a href="/information/hell-forged-set" target="_blank"&gt;Hell Forged&lt;/a&gt; gear. To do this, you will need to craft a level 400 piece of gear, but you should already have some equipped.&lt;/p&gt;&lt;p&gt;Hell Forged gear allows you to then trade it later on for Purgatory Chains gear. When you purchase a piece of Hell Forged gear, you will trade a piece of your gear and the currencies needed.&lt;/p&gt;&lt;p&gt;I want you to purchase your first piece of Hell Forged gear, and I also want you to trade one of the equipped items you have. Unequip a level 400 item (or remove it from a set) and then purchase a Hell Forged gear piece of that type, for example: &lt;/p&gt;&lt;p&gt;Ring for Ring or Spell for Spell.&lt;/p&gt;&lt;p&gt;You will see that your enchantments will be transferred, for free, from your existing gear to the new Hell Forged gear piece. This way, all your hard work is not lost.&lt;/p&gt;&lt;p&gt;This is what we call: End Game gear. Your progression starts here, your next set will be &lt;a href="/information/purgatory-chains-set" target="_blank"&gt;Purgatory Chains&lt;/a&gt;, followed by &lt;a href="/information/pirate-lord-leather-set" target="_blank"&gt;Pirate Lord Leather&lt;/a&gt; and then &lt;a href="/information/corrupted-ice" target="_blank"&gt;Corrupted Ice&lt;/a&gt;. Each set gets slightly higher stats.&lt;/p&gt;&lt;p&gt;Purgatory Chains gear, your next set, can also be obtained the same way as Hell Forged, but only while on Purgatory.&lt;/p&gt;&lt;p&gt;Pirate Lord Leather can, at the time of this guide quest, only be obtained via defeating the raid boss in a Surface Raid.&lt;/p&gt;&lt;p&gt;Corrupted Ice gear can, at the time of this guide quest, only be obtained via participating in the Winter Event and being on the Ice Plane.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;First, we need to manage our inventory and either unequip an item that you have which is crafting level 400, and make sure it’s in your inventory. You can also craft a level 400 item if you please instead, but this gets rather expensive; it's best to use one if you have one.&lt;/p&gt;&lt;p&gt;Next:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;In the Actions section, you will see, while on Hell, a new button called: Hell Forged gear – click it.&lt;/li&gt;&lt;li&gt;Next, select a piece of gear that matches the item type in your inventory. For example – if you unequipped a level 400 ring, select a ring. If you crafted a level 400 Body piece, select Body.&lt;/li&gt;&lt;li&gt;Click Purchase Item if you can afford it; if not, go earn the currencies.&lt;/li&gt;&lt;li&gt;Now you should have a Hell Forged Item in your inventory; any enchants on the previous item are now transferred to this one.&lt;/li&gt;&lt;li&gt;Equip it.&lt;/li&gt;&lt;li&gt;Repeat for each item you have equipped that meets the requirements.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;: &lt;em&gt;This quest only cares about you doing one item. It is suggested you replace all your items with Hell Forged.&lt;/em&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;First, we need to manage our inventory and either unequip an item that you have which is crafting level 400, and make sure it’s in your inventory. You can also craft a level 400 item if you please instead, but this gets rather expensive; it's best to use one if you have one.&lt;/p&gt;&lt;p&gt;Next&lt;/p&gt;&lt;p&gt;:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;From the Actions drop down, select: Hell Forged gear while in Hell.&lt;/li&gt;&lt;li&gt;Next, select a piece of gear that matches the item type in your inventory. For example – if you unequipped a level 400 ring, select a ring. If you crafted a level 400 Body piece, select Body.&lt;/li&gt;&lt;li&gt;Click Purchase Item if you can afford it; if not, go earn the currencies.&lt;/li&gt;&lt;li&gt;Now you should have a Hell Forged Item in your inventory; any enchants on the previous item are now transferred to this one.&lt;/li&gt;&lt;li&gt;Equip it.&lt;/li&gt;&lt;li&gt;Repeat for each item you have equipped that meets the requirements.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;: &lt;em&gt;This quest only cares about you doing one item. It is suggested you replace all your items with Hell Forged.&lt;/em&gt;&lt;/p&gt;</t>
   </si>
   <si>
     <t>Hell Forged</t>
@@ -716,16 +716,16 @@
     <t>The Queens got the Info, if you have the coin</t>
   </si>
   <si>
-    <t>“Ooooh hooo hoo hoo!” Comes a flirtatious laughter. A busty beautiful woman comes walking from seemingly no where. “Hello my beautiful child. How are e today? I! I am The Queen of Hearts!”&lt;br /&gt; &lt;br /&gt; You stare at her radiant beauty. Her eyes are a blue unlike any other blue. Her hair is a dust flowing red that dances in the dead air.&lt;br /&gt; &lt;br /&gt; You have heard of her, a women whose power is beyond any you have seen. She can create, from thin air, powerful unique items. She is also the women that can altar Uniques and Mythical items the Enchantress would tell you about.&lt;br /&gt; &lt;br /&gt; “My child, is there something I can help you with down here in this fabulously hot plane of scorching torment and pain? Oooooh hoo hooo hoo!”&lt;br /&gt; &lt;br /&gt; You explain that you are searching for The Guide and if she has seen him.&lt;br /&gt; &lt;br /&gt; “Maybe you should please me with your coin and when I'm well and satisfied I can tell you what you want.” She winks at you and shes her chest in your face. Do you shove your gold in hers?</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;The Queen of Hearts is an NPC who allows you to purchase more powerful Uniques, Legendary Uniques are what you want for now and are apart of your end game progression until you can get a mythical item.&lt;/p&gt;&lt;p&gt;Up until now you have been able to get Basic Uniques, which were, at the time, better then any enchantment you had and worked well in conjunction to your enchantments, but then you might have went to Gold Mines on the Shadow Plane and earned your self A “medium” unique item.&lt;/p&gt;&lt;p&gt;But now, you can purchase Legendary Uniques, this tier of enchantments is one below Mythical which are currently, at the time of this guide quest, the best enchantment type you can have in game.&lt;/p&gt;&lt;p&gt;The Queen, as mentioned, also allows you to re-roll uniques (basic, medium and legendary) as well as mythical enchantments. You can re-roll all aspects about the enchantment to get the best stats you can in an RNG world.&lt;/p&gt;&lt;p&gt;Finally, The Queen allows players to take enchantments – Uniques and Mythics and move them from one item to an item of their choosing!&lt;/p&gt;&lt;p&gt;Ideally, you should purchase a legendary unique from the queen – keep buying till you get an item with two enchants on it. Then use the queen to re-roll that unique aiming for higher stats and base damage for example. Lastly you would move these uniques to a body Hell Forged gear piece you own for maximum effect.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;The instructions will tell you how to do this should you want to, but this guide quest focuses on faction leveling.&lt;/strong&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;How to use the queen!&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- From the Craft/Enchant drop down – and while on hell – select Queen of Hearts&lt;/p&gt;&lt;p&gt;- Select Buy Item from the drop down.&lt;/p&gt;&lt;p&gt;- Select Legendary from the drop down.&lt;/p&gt;&lt;p&gt;- Purchase, check the server message section.&lt;/p&gt;&lt;p&gt;Repeat this until you have an item that has two enchants.&lt;/p&gt;&lt;p&gt;Next, lets re-roll the unique. First, make sure to inspect the item, but clicking on it from your inventory or the server message section and clicking details.&lt;/p&gt;&lt;p&gt;On the details section you will see two orange buttons whose label is that of the attached enchants.&lt;/p&gt;&lt;p&gt;If you click on these it will tell you more about the attached affixes. Most characters at this point want to increase their stats as high as they can afford and the RNG will allow them. You can, for example as a vampire, focus more on raising a specific stat (DUR) and attribute: Life Stealing. To do this, we need to re-roll the affixes. The queen can help us:&lt;/p&gt;&lt;p&gt;- Click Change Action&lt;/p&gt;&lt;p&gt;- Select Re-roll item&lt;/p&gt;&lt;p&gt;- Select the item you wanted, this list only has your Uniques and Mythics in your inventory.&lt;/p&gt;&lt;p&gt;- Select Either the Prefix, the Suffix or both&lt;/p&gt;&lt;p&gt;- Select the aspect of the affix(es) you want to re-roll and click re-roll.&lt;/p&gt;&lt;p&gt;The item will then appear in your server message section so you can easily investigate the item and see if you should re-roll or not. Keep doing this until you have the enchantments where you want them. Next we move them:&lt;/p&gt;&lt;p&gt;To do this, the item you want the enchantments to be move to, needs to be in your inventory. Ideally – this would be your body and it would be Hell Forged (Maximum stat gain). But you are free to do as you wish.&lt;/p&gt;&lt;p&gt;- Click Change Action&lt;/p&gt;&lt;p&gt;- Select Move Enchants&lt;/p&gt;&lt;p&gt;- Select The Unique you spent time re-rolling&lt;/p&gt;&lt;p&gt;- Select Both for the affixes to move&lt;/p&gt;&lt;p&gt;- Select the item you want to move them to.&lt;/p&gt;&lt;p&gt;Click Move Enchants and boom done!&lt;/p&gt;&lt;p&gt;Now go get some faction points!&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;How to use the queen!&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;- From the actions drop down select Craft&lt;/p&gt;&lt;p&gt;- From the Craft drop down – and while on hell – select Queen of Hearts&lt;/p&gt;&lt;p&gt;- Select Buy Item from the drop down.&lt;/p&gt;&lt;p&gt;- Select Legendary from the drop down.&lt;/p&gt;&lt;p&gt;- Purchase, check the server message section.&lt;/p&gt;&lt;p&gt;Repeat this until you have an item that has two enchants.&lt;/p&gt;&lt;p&gt;Next, lets re-roll the unique. First, make sure to inspect the item, but clicking on it from your inventory or the server message section and clicking details.&lt;/p&gt;&lt;p&gt;On the details section you will see two orange buttons whose label is that of the attached enchants.&lt;/p&gt;&lt;p&gt;If you click on these it will tell you more about the attached affixes. Most characters at this point want to increase their stats as high as they can afford and the RNG will allow them. You can, for example as a vampire, focus more on raising a specific stat (DUR) and attribute: Life Stealing. To do this, we need to re-roll the affixes. The queen can help us:&lt;/p&gt;&lt;p&gt;- Tap Change Action&lt;/p&gt;&lt;p&gt;- Select Re-roll item&lt;/p&gt;&lt;p&gt;- Select the item you wanted, this list only has your Uniques and Mythics in your inventory.&lt;/p&gt;&lt;p&gt;- Select Either the Prefix, the Suffix or both&lt;/p&gt;&lt;p&gt;- Select the aspect of the affix(es) you want to re-roll and click re-roll.&lt;/p&gt;&lt;p&gt;The item will then appear in your server message section so you can easily investigate the item and see if you should re-roll or not. Keep doing this until you have the enchantments where you want them. Next we move them:&lt;/p&gt;&lt;p&gt;To do this, the item you want the enchantments to be move to, needs to be in your inventory. Ideally – this would be your body and it would be Hell Forged (Maximum stat gain). But you are free to do as you wish.&lt;/p&gt;&lt;p&gt;- Tap Change Action&lt;/p&gt;&lt;p&gt;- Select Move Enchants&lt;/p&gt;&lt;p&gt;- Select The Unique you spent time re-rolling&lt;/p&gt;&lt;p&gt;- Select Both for the affixes to move&lt;/p&gt;&lt;p&gt;- Select the item you want to move them to.&lt;/p&gt;&lt;p&gt;Tap Move Enchants and boom done!&lt;/p&gt;&lt;p&gt;Now go get some faction points!&lt;/p&gt;</t>
+    <t>"Ooooh hooo hoo hoo!" comes flirtatious laughter. A busty beautiful woman comes walking from seemingly nowhere. "Hello, my beautiful child. How are you today? I! I am The Queen of Hearts!"&lt;br /&gt; &lt;br /&gt; You stare at her radiant beauty. Her eyes are a blue unlike any other blue. Her hair is a dust-flowing red that dances in the dead air.&lt;br /&gt; &lt;br /&gt; You have heard of her, a woman whose power is beyond any you have seen. She can create, from thin air, powerful unique items. She is also the woman that can alter Uniques and Mythical items the Enchantress would tell you about.&lt;br /&gt; &lt;br /&gt; "My child, is there something I can help you with down here in this fabulously hot plane of scorching torment and pain? Oooooh hoo hooo hoo!"&lt;br /&gt; &lt;br /&gt; You explain that you are searching for The Guide and if she has seen him.&lt;br /&gt; &lt;br /&gt; "Maybe you should please me with your coin and when I'm well and satisfied I can tell you what you want." She winks at you and shoves her chest in your face. Do you shove your gold in hers?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;The Queen of Hearts is an NPC who allows you to purchase more powerful Uniques; Legendary Uniques are what you want for now and are a part of your end-game progression until you can get a mythical item.&lt;/p&gt;&lt;p&gt;Up until now, you have been able to get Basic Uniques, which were, at the time, better than any enchantment you had and worked well in conjunction with your enchantments. But then you might have gone to Gold Mines on the Shadow Plane and &lt;/p&gt;&lt;p&gt;earned yourself a "medium" unique item.&lt;/p&gt;&lt;p&gt;But now, you can purchase Legendary Uniques, this tier of enchantments is one below Mythical, which is currently, at the time of this guide quest, the best enchantment type you can have in the game.&lt;/p&gt;&lt;p&gt;The Queen, as mentioned, also allows you to re-roll uniques (basic, medium, and legendary) as well as mythical enchantments. You can re-roll all aspects about the enchantment to get the best stats you can in an RNG world.&lt;/p&gt;&lt;p&gt;Finally, The Queen allows players to take enchantments – Uniques and Mythics and move them from one item to an item of their choosing!&lt;/p&gt;&lt;p&gt;Ideally, you should purchase a legendary unique from the queen – keep buying till you get an item with two enchants on it. Then use the queen to re-roll that unique aiming for higher stats and base damage, for example. Lastly, you would move &lt;/p&gt;&lt;p&gt;these uniques to a body Hell Forged gear piece you own for maximum effect.&lt;/p&gt;&lt;p&gt;The instructions will tell you how to do this should you want to, but this guide quest focuses on faction leveling.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;How to use the queen!&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;From the Craft/Enchant drop-down – and while on hell – select Queen of Hearts&lt;/li&gt;&lt;li&gt;Select Buy Item from the drop-down.&lt;/li&gt;&lt;li&gt;Select Legendary from the drop-down.&lt;/li&gt;&lt;li&gt;Purchase, check the server message section.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Repeat this until you have an item that has two enchants.&lt;/p&gt;&lt;p&gt;Next, let's re-roll the unique. First, make sure to inspect the item, by clicking on it from your inventory or the server message section and clicking details.&lt;/p&gt;&lt;p&gt;On the details section, you will see two orange buttons whose label is that of the attached enchants.&lt;/p&gt;&lt;p&gt;If you click on these, it will tell you more about the attached affixes. Most characters at this point want to increase their stats as high as they can afford and the RNG will allow them. You can, for example as a vampire, focus more on raising a &lt;/p&gt;&lt;p&gt;specific stat (DUR) and attribute: Life Stealing. To do this, we need to re-roll the affixes. The queen can help us:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Click Change Action&lt;/li&gt;&lt;li&gt;Select Re-roll item&lt;/li&gt;&lt;li&gt;Select the item you wanted, this list only has your Uniques and Mythics in your inventory.&lt;/li&gt;&lt;li&gt;Select Either the Prefix, the Suffix or both&lt;/li&gt;&lt;li&gt;Select the aspect of the affix(es) you want to re-roll and click re-roll.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;The item will then appear in your server message section so you can easily investigate the item and see if you should re-roll or not. Keep doing this until you have the enchantments where you want them. Next, we move them:&lt;/p&gt;&lt;p&gt;To do this, the item you want the enchantments to be moved to needs to be in your inventory. Ideally – this would be your body and it would be Hell Forged (Maximum stat gain). But you are free to do as you wish.&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Click Change Action&lt;/li&gt;&lt;li&gt;Select Move Enchants&lt;/li&gt;&lt;li&gt;Select The Unique you spent time re-rolling&lt;/li&gt;&lt;li&gt;Select Both for the affixes to move&lt;/li&gt;&lt;li&gt;Select the item you want to move them to.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Click Move Enchants and boom done!&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Now go get some faction points!&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;How to use the queen!&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;From the actions drop-down select Craft&lt;/li&gt;&lt;li&gt;From the Craft drop-down – and while on hell – select Queen of Hearts&lt;/li&gt;&lt;li&gt;Select Buy Item from the drop-down.&lt;/li&gt;&lt;li&gt;Select Legendary from the drop-down.&lt;/li&gt;&lt;li&gt;Purchase, check the server message section.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Repeat this until you have an item that has two enchants.&lt;/p&gt;&lt;p&gt;Next, let's re-roll the unique. First, make sure to inspect the item, by clicking on it from your inventory or the server message section and clicking details.&lt;/p&gt;&lt;p&gt;On the details section, you will see two orange buttons whose label is that of the attached enchants.&lt;/p&gt;&lt;p&gt;If you click on these, it will tell you more about the attached affixes. Most characters at this point want to increase their stats as high as they can afford and the RNG will allow them. You can, for example as a vampire, focus more on raising a &lt;/p&gt;&lt;p&gt;specific stat (DUR) and attribute: Life Stealing. To do this, we need to re-roll the affixes. The queen can help us:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Tap Change Action&lt;/li&gt;&lt;li&gt;Select Re-roll item&lt;/li&gt;&lt;li&gt;Select the item you wanted, this list only has your Uniques and Mythics in your inventory.&lt;/li&gt;&lt;li&gt;Select Either the Prefix, the Suffix or both&lt;/li&gt;&lt;li&gt;Select the aspect of the affix(es) you want to re-roll and click re-roll.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;The item will then appear in your server message section so you can easily investigate the item and see if you should re-roll or not. Keep doing this until you have the enchantments where you want them. Next we move them:&lt;/p&gt;&lt;p&gt;To do this, the item you want the enchantments to be moved to needs to be in your inventory. Ideally – this would be your body and it would be Hell Forged (Maximum stat gain). But you are free to do as you wish.&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Tap Change Action&lt;/li&gt;&lt;li&gt;Select Move Enchants&lt;/li&gt;&lt;li&gt;Select The Unique you spent time re-rolling&lt;/li&gt;&lt;li&gt;Select Both for the affixes to move&lt;/li&gt;&lt;li&gt;Select the item you want to move them to.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Tap Move Enchants and boom done!&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Now go get some faction points!&lt;/strong&gt;&lt;/p&gt;</t>
   </si>
   <si>
     <t>Seeking out darkness</t>

</xml_diff>

<commit_message>
Updated - and finished - guide quests
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -731,13 +731,13 @@
     <t>Seeking out darkness</t>
   </si>
   <si>
-    <t>You told the Queen everything. Your entire adventure. She sits and enjoys the coin and she gives you the shiny items. When your done telling her your tale, she stares off for a moment, as if in deep though only to then perk up with laughter:&lt;br /&gt; &lt;br /&gt; “Oooooh hooo hooo hooo child! I, The Queen of all that there is, can tell you this:&lt;br /&gt; &lt;br /&gt; The Guide is hunting a darkness that has escaped the shadows of a land only whispered in the shadows of midnight. And it’s never midnight down here! Ooooh hooo hooo hooo!”&lt;br /&gt; &lt;br /&gt; She vanishes and leaves you with more questions then answers, but then again – after all you have been through, its the least of your concerns.&lt;br /&gt; &lt;br /&gt; She never answered where The Guide is. She never gave any insight. She just gave you items. How do you even proceed?</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;We need to go to Purgatory to really start the End game. But to get there, we have some quests to complete.&lt;/p&gt;&lt;p&gt;Purgatory is the last, at the time of this guide quest, Plane that players have access to out side of special events like the Winter Event, who comes with the Ice Plane&lt;/p&gt;&lt;p&gt;Purgatory has a special location called: Purgatory Smiths House where numerous amounts of currencies drop for end game crafting like &lt;a href="/information/trinketry" target="_blank"&gt;Trinketry&lt;/a&gt;, &lt;a href="/information/gems" target="_blank"&gt;Gem Crafting&lt;/a&gt; and later on Alchemy crafting.&lt;/p&gt;&lt;p&gt;For now, lets complete some quests to get us to Purgatory. You’ll need to be able to walk on magma in Hell, so there is that too.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Easy peasy, lemon squeesy – complete some quests and traverse down!&lt;/p&gt;&lt;p&gt;Oh! Wait, one more thing: You must teleport or walk, once you can walk on magma to the location: Tear in the Fabric of Time (X/Y): 208/64 in Hell. Only from here will Purgatory appear in your traverse drop down list.&lt;/p&gt;</t>
+    <t>You told the Queen everything about your entire adventure. As she sits and enjoys the coin, she gives you shiny items in return. When you're done telling her your tale, she stares off for a moment, as if in deep thought, only to then perk up with laughter:&lt;br /&gt; &lt;br /&gt; "Oooooh hooo hooo hooo, child! I, the Queen of all that there is, can tell you this:&lt;br /&gt; &lt;br /&gt; The Guide is hunting a darkness that has escaped the shadows of a land only whispered in the shadows of midnight. And it’s never midnight down here! Ooooh hooo hooo hooo!”&lt;br /&gt; &lt;br /&gt; She vanishes, leaving you with more questions than answers. But then again, after all you have been through, it's the least of your concerns. She never answered where The Guide is, never provided any insight. She simply gave you items. How do you even proceed?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We need to go to Purgatory to really start the end game. But to get there, we have some quests to complete.&lt;/p&gt;&lt;p&gt;Purgatory is the last plane that players have access to outside of special events like the Winter Event, which comes with the Ice Plane.&lt;/p&gt;&lt;p&gt;Purgatory has a special location called Purgatory Smith's House, where numerous amounts of currencies drop for end-game crafting, such as &lt;a href="/information/trinketry" target="_blank"&gt;Trinketry&lt;/a&gt;, &lt;a href="/information/gems" target="_blank"&gt;Gem Crafting&lt;/a&gt;, and later on, Alchemy crafting.&lt;/p&gt;&lt;p&gt;For now, let's complete some quests to get us to Purgatory. You'll need to be able to walk on magma in Hell, so there's that too.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Easy peasy, lemon squeezy – complete some quests and traverse down!&lt;/p&gt;&lt;p&gt;Oh! Wait, one more thing: You must teleport or walk, once you can walk on magma, to the location Tear in the Fabric of Time (X/Y): 208/64 in Hell. Only from here will Purgatory appear in your traverse drop-down list.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Purgatory</t>
@@ -749,10 +749,10 @@
     <t>The End and The Beginning</t>
   </si>
   <si>
-    <t>There is a darkness in this land. One that creeps into your very being, the fabric of your soul.&lt;br /&gt; &lt;br /&gt; “Welcome to purgatory.” The Guide appears before you, young and handsome. His appearance changes so often and so much its confusing as to who he even is. But alas, he stands beside you.&lt;br /&gt; &lt;br /&gt; “This is where it started. This is where it ended. This is where he escaped from. I seek The smith. When The Child escaped this place, he set loose the blacksmiths - a set of smiths from Purgatory. These smiths are corrupted in their soul, like you – a fragment of a larger structure, a crystalline structure – shattered and scattered across the sands of time.”&lt;br /&gt; &lt;br /&gt; He falls silent and the two of you stand staring out across the desolate waste land of emptiness. So many lands that feel so empty, so lonely, so depressing.&lt;br /&gt; &lt;br /&gt; “Down here.” The Guide starts: “There is a darkness that corrupts the air we breathe. It makes us much weaker, much more susceptible to death. There are ways child – ways you can get around this. You’ll need to seek out the alchemical books and teachings for a special kind of oil.”&lt;br /&gt; &lt;br /&gt; He looks at you and you him, neither of you speak for a moment as you both go back to staring out at the land.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Welcome to Purgatory. This is where the hardest creatures live and the rewards are the greatest. Alas to begin our journey towards the ultimate goal of reincarnation – we need stronger gear. By now you should have a full set of Hell Forged gear enchanted our the ass with level 400 enchants and at least 2 legendary enchantments on one item – ideally the body.&lt;/p&gt;&lt;p&gt;Your Accuracy, Looting and possibly Casting Accuracy should be maxed out.&lt;/p&gt;&lt;p&gt;Your gear will only take you so far down the critter list. You need something: Holy Oils. You can unlock this through Alchemy – so lets begin training until we have unlocked &lt;a href="/information/holy-items" target="_blank"&gt;Holy Oils&lt;/a&gt;. I would stay out of special locations for now, you are far too weak!&lt;/p&gt;&lt;p&gt;Instead lets explore down here and do some Alchemical crafting. If you start to run low on Gold Dust and Shards I suggest heading to the Gold Mines on Shadow Plane until we have unlocked the Purgatory Smith House.&lt;/p&gt;&lt;p&gt;While manually battling in Gold Mines you can get enough currencies to continue level alchemy.&lt;/p&gt;</t>
+    <t>There is a darkness in this land, one that creeps into your very being, the fabric of your soul.&lt;br /&gt; &lt;br /&gt; “Welcome to Purgatory.” The Guide appears before you, young and handsome. His appearance changes so often and so much that it's confusing as to who he even is. But alas, he stands beside you.&lt;br /&gt; &lt;br /&gt; “This is where it started. This is where it ended. This is where he escaped from. I seek The smith. When The Child escaped this place, he set loose the blacksmiths - a set of smiths from Purgatory. These smiths are corrupted in their soul, like you – a fragment of a larger structure, a crystalline structure – shattered and scattered across the sands of time.”&lt;br /&gt; &lt;br /&gt; He falls silent, and the two of you stand staring out across the desolate wasteland of emptiness. So many lands that feel so empty, so lonely, so depressing.&lt;br /&gt; &lt;br /&gt; “Down here,” The Guide starts, “there is a darkness that corrupts the air we breathe. It makes us much weaker, much more susceptible to death. There are ways, child – ways you can get around this. You’ll need to seek out the alchemical books &lt;br /&gt; and teachings for a special kind of oil.”&lt;br /&gt; &lt;br /&gt; He looks at you, and you look at him; neither of you speaks for a moment as you both go back to staring out at the land.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welcome to Purgatory. This is where the hardest creatures live, and the rewards are the greatest. Alas, to begin our journey towards the ultimate goal of reincarnation, we need stronger gear. By now, you should have a full set of Hell Forged gear enchanted out the wazoo with level 400 enchants and at least 2 legendary enchantments on one item – ideally the body.&lt;/p&gt;&lt;p&gt;Your Accuracy, Looting, and possibly Casting Accuracy should be maxed out.&lt;/p&gt;&lt;p&gt;Your gear will only take you so far down the critter list. You need something: Holy Oils. You can unlock this through Alchemy – so let's begin training until we have unlocked Holy Oils. I would stay out of special locations for now; you are far too &lt;/p&gt;&lt;p&gt;weak!&lt;/p&gt;&lt;p&gt;Instead, let's explore down here and do some Alchemical crafting. If you start to run low on Gold Dust and Shards, I suggest heading to the Gold Mines on Shadow Plane until we have unlocked the Purgatory Smith House.&lt;/p&gt;&lt;p&gt;While manually battling in Gold Mines, you can get enough currencies to continue leveling alchemy.&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Raise your alchemy skill child. Raise it on high so we can slaughter the beasts before us!&lt;/p&gt;</t>
@@ -761,16 +761,16 @@
     <t>Oiling up for combat</t>
   </si>
   <si>
-    <t>You poured over the texts and plunged deep into the depths of the mines hunting the creatures who carry the currency you needed to complete your studies. It has been such a long road.&lt;br /&gt; &lt;br /&gt; Now you have the tools, the starts of the tools you need, to take on the depths of dungeons in purgatory.&lt;br /&gt; &lt;br /&gt; You also need the coin, a rare currency that was once used back in the days of old, during the war – a currency made of copper.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;One of the things you need, to survive in purgatory, is extra stats and devouring percentage. You can get this through applying &lt;a href="/information/holy-items" target="_blank"&gt;Holy Oils&lt;/a&gt;, that you craft through alchemy to items in your inventory. To do this you need to go to Purgatory and use The Work Bench.&lt;/p&gt;&lt;p&gt;This guide quest will have you craft alchemy Holy Oils and then apply them to your equipment. Consider this the third step in your end game gear progression. First we upgraded our crafted gear to Hell Forged, then we applied our best rolled Legendary enchantments to one piece of that gear and now we shall apply some holy oils.&lt;/p&gt;&lt;p&gt;Each item – at level 400 in crafting and all specialty gear sets – have 20 stacks of oils that can be applied. Caution though, there are different oils and you only really care about one of them: The Creators Holy Oil&lt;/p&gt;&lt;p&gt;If you apply other oils, you could end up with less then ideal stats and since there is no way to re-roll or remove oils, you should use caution to only apply the best.&lt;/p&gt;&lt;p&gt;When you apply an oil to the item you will raise your stats by a % a small % that stacks with the more oils you apply to an item.&lt;/p&gt;&lt;p&gt;Lets start by upgrading two of our items with oils!&lt;/p&gt;&lt;p&gt;You will also need to complete a quest: The Magic of Purgatory in Hell – this will give you a quest item that allows you to gain Copper Coins, we need them for the next quest. So kill some creatures on creatures for the coins to drop. You can also play slots to gain the currency and purchase the Child of Copper coins Mercenary to help with the drop rates till we can get into the house.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;First, craft 40 The Creators Holy Oil’s. This might take a moment and might require a trip to The Gold Mines on Shadow Planes.&lt;/p&gt;&lt;p&gt;Next unequip two items, ideally Body and Weapon to start (or spell if you are a caster). These should be your Hell Forged gear items.&lt;/p&gt;&lt;p&gt;Head down to Purgatory. Now the fun begins:&lt;/p&gt;&lt;p&gt;- Select Workbench from Craft/Enchant&lt;/p&gt;&lt;p&gt;- Select an item to apply the oils to&lt;/p&gt;&lt;p&gt;- Select an oil from the second drop down&lt;/p&gt;&lt;p&gt;- Click Apply Oil&lt;/p&gt;&lt;p&gt;You will see that your Applied Holy Stacks will increase by one. When the count reaches the max holy stacks, below it, the item will leave the list as you have applied the maximum amount of oils to the item.&lt;/p&gt;&lt;p&gt;When the item has an oil applied to it, it will appear in your server message section. Click the item, click details, and scroll down to the Holy Info section. Here you can click view info to see each stack and what was rolled. The Creators Holy Oil is the best oil for stat and devouring bonus increase. This will become very handy in Purgatory where you are severely weakened, the more stats and devouring the better chances you have to survive.&lt;/p&gt;&lt;p&gt;Repeat applying oils until you have maxed the 20 stacks on each item. You can see your Holy Information on your character sheet if you click on Show additional details, and then select the Holy tab you will see how this affects your character in the big picture.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;First, craft 40 The Creators Holy Oil’s. This might take a moment and might require a trip to The Gold Mines on Shadow Planes.&lt;/p&gt;&lt;p&gt;Next unequip two items, ideally Body and Weapon to start (or spell if you are a caster). These should be your Hell Forged gear items.&lt;/p&gt;&lt;p&gt;Head down to Purgatory. Now the fun begins:&lt;/p&gt;&lt;p&gt;- Select Craft from the Actions drop down&lt;/p&gt;&lt;p&gt;- Select Workbench from Crafting drop down&lt;/p&gt;&lt;p&gt;- Select an item to apply the oils to&lt;/p&gt;&lt;p&gt;- Select an oil from the second drop down&lt;/p&gt;&lt;p&gt;- Tap Apply Oil&lt;/p&gt;&lt;p&gt;You will see that your Applied Holy Stacks will increase by one. When the count reaches the max holy stacks, below it, the item will leave the list as you have applied the maximum amount of oils to the item.&lt;/p&gt;&lt;p&gt;When the item has an oil applied to it, it will appear in your server message section. tap the item, tap details, and scroll down to the Holy Info section. Here you can tap view info to see each stack and what was rolled. The Creators Holy Oil is the best oil for stat and devouring bonus increase. This will become very handy in Purgatory where you are severely weakened, the more stats and devouring the better chances you have to survive.&lt;/p&gt;&lt;p&gt;Repeat applying oils until you have maxed the 20 stacks on each item. You can see your Holy Information on your character sheet if you tap on Show additional details – by expanding the top section, and then select the Holy tab you will see how this affects your character in the big picture.&lt;/p&gt;</t>
+    <t>You poured over the texts and plunged deep into the depths of the mines, hunting the creatures who carry the currency you needed to complete your studies. It has been such a long road.&lt;br /&gt; &lt;br /&gt; Now you have the tools, the starts of the tools you need, to take on the depths of dungeons in Purgatory.&lt;br /&gt; &lt;br /&gt; You also need the coin, a rare currency that was once used back in the days of old, during the war – a currency made of copper.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;One of the things you need to survive in Purgatory is extra stats and devouring percentage. You can get this through applying &lt;a href="/information/holy-items" target="_blank"&gt;Holy Oils&lt;/a&gt; that you craft through alchemy to items in your inventory. To do this, you need to go to Purgatory and use The Work Bench.&lt;/p&gt;&lt;p&gt;This guide quest will have you craft alchemy Holy Oils and then apply them to your equipment. Consider this the third step in your end-game gear progression. First, we upgraded our crafted gear to Hell Forged, then we applied our best rolled &lt;/p&gt;&lt;p&gt;Legendary enchantments to one piece of that gear, and now we shall apply some holy oils.&lt;/p&gt;&lt;p&gt;Each item – at level 400 in crafting and all specialty gear sets – has 20 stacks of oils that can be applied. Caution though, there are different oils, and you only really care about one of them: The Creators Holy Oil.&lt;/p&gt;&lt;p&gt;If you apply other oils, you could end up with less than ideal stats, and since there is no way to re-roll or remove oils, you should use caution to only apply the best.&lt;/p&gt;&lt;p&gt;When you apply an oil to the item, you will raise your stats by a %, a small % that stacks with the more oils you apply to an item.&lt;/p&gt;&lt;p&gt;Let's start by upgrading two of our items with oils!&lt;/p&gt;&lt;p&gt;You will also need to complete a quest: "The Magic of Purgatory" in Hell – this will give you a quest item that allows you to gain Copper Coins; we need them for the next quest. So kill some creatures for the coins to drop. You can also play slots to &lt;/p&gt;&lt;p&gt;gain the currency and purchase the Child of Copper coins Mercenary to help with the drop rates until we can get into the house.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;First, craft 40 The Creators Holy Oils. This might take a moment and might require a trip to The Gold Mines on Shadow Planes.&lt;/p&gt;&lt;p&gt;Next, unequip two items, ideally Body and Weapon to start (or spell if you are a caster). These should be your Hell Forged gear items.&lt;/p&gt;&lt;p&gt;Head down to Purgatory. Now the fun begins:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Select Workbench from Craft/Enchant&lt;/li&gt;&lt;li&gt;Select an item to apply the oils to&lt;/li&gt;&lt;li&gt;Select an oil from the second drop down&lt;/li&gt;&lt;li&gt;Click Apply Oil&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;You will see that your Applied Holy Stacks will increase by one. When the count reaches the max holy stacks, below it, the item will leave the list as you have applied the maximum amount of oils to the item.&lt;/p&gt;&lt;p&gt;When the item has an oil applied to it, it will appear in your server message section. Click the item, click details, and scroll down to the Holy Info section. Here you can click view info to see each stack and what was rolled. The Creators Holy Oil is the best oil for stat and devouring bonus increase. This will become very handy in Purgatory where you are severely weakened; the more stats and devouring, the better chances you have to survive.&lt;/p&gt;&lt;p&gt;Repeat applying oils until you have maxed the 20 stacks on each item. You can see your Holy Information on your character sheet if you click on Show additional details, and then select the Holy tab; you will see how this affects your character in the big picture.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;First, craft 40 The Creators Holy Oils. This might take a moment and might require a trip to The Gold Mines on Shadow Planes.&lt;/p&gt;&lt;p&gt;Next, unequip two items, ideally Body and Weapon to start (or spell if you are a caster). These should be your Hell Forged gear items.&lt;/p&gt;&lt;p&gt;Head down to Purgatory. Now the fun begins:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Select Craft from the Actions drop down&lt;/li&gt;&lt;li&gt;Select Workbench from Crafting drop down&lt;/li&gt;&lt;li&gt;Select an item to apply the oils to&lt;/li&gt;&lt;li&gt;Select an oil from the second drop down&lt;/li&gt;&lt;li&gt;Tap Apply Oil&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;You will see that your Applied Holy Stacks will increase by one. When the count reaches the max holy stacks, below it, the item will leave the list as you have applied the maximum amount of oils to the item.&lt;/p&gt;&lt;p&gt;When the item has an oil applied to it, it will appear in your server message section. Tap the item, tap details, and scroll down to the Holy Info section. Here you can tap view info to see each stack and what was rolled. The Creators Holy Oil is the &lt;/p&gt;&lt;p&gt;best oil for stat and devouring bonus increase. This will become very handy in Purgatory where you are severely weakened; the more stats and devouring, the better chances you have to survive.&lt;/p&gt;&lt;p&gt;Repeat applying oils until you have maxed the 20 stacks on each item. You can see your Holy Information on your character sheet if you tap on Show additional details – by expanding the top section, and then select the Holy tab; you will see how &lt;/p&gt;&lt;p&gt;this affects your character in the big picture.&lt;/p&gt;</t>
   </si>
   <si>
     <t>The Magic of Purgatory</t>
@@ -779,13 +779,13 @@
     <t>The Smith and The Cage</t>
   </si>
   <si>
-    <t>“Have you seen the house?” Comes a voice. You look up from your plate while sitting in a pub in Smugglers Port.&lt;br /&gt; &lt;br /&gt; The House? What house?&lt;br /&gt; &lt;br /&gt; “There is a house where a man known as The Purgatory Smith, lived. No one knows where he went once The Child escaped Purgatory. Some say he came to Surface, some say he just vanished, the magic that had created him has withered and died.”&lt;br /&gt; &lt;br /&gt; He pauses and takes a sip from his mug, you stare in silence and absorb the words, digesting the meaning.&lt;br /&gt; &lt;br /&gt; But me, what does this have to do with me? You ponder this.&lt;br /&gt; &lt;br /&gt; “You, child, come in to place where you are a piece of the structure that held The Child in place. All of these people are. All of the adventurers are who come and seek out the riches and fame of this land and all the lands connected.”&lt;br /&gt; &lt;br /&gt; A piece of the structure. What structure?&lt;br /&gt; &lt;br /&gt; “That cage.”</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Now that we have Copper Coins and We have applied oils to our weapons and armour and coated our selves up. We have another upgrade for gear to do. &lt;a href="/information/purgatory-chains-set" target="_blank"&gt;Purgatory Chains&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;This process is very similar to that of Hell Forged, don’t worry – all your hard work will be copied over to your new item.&lt;/p&gt;&lt;p&gt;Purgatory Chains gear is as far as you will be able to take your gear – at this time – by the process of upgrading through specialty shops like this.&lt;/p&gt;&lt;p&gt;At this stage, with a full set of Purgatory Chain covered in holy oils and dripping in high end enchants that define your build – allow you to do unimaginable damage, you still have a ways to go before you have truly reached your full potential.&lt;/p&gt;&lt;p&gt;After this, the last set of upgrades we have to work on is &lt;a href="/information/trinketry" target="_blank"&gt;trinkets&lt;/a&gt; and &lt;a href="/information/gems" target="_blank"&gt;gems&lt;/a&gt;. But one thing at a time child, lets get some chains on our body shall we?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;At this stage we have already done the upgrade process for Crafted gear to hell Forged. Now we go from Hell Forged to Purgatory Chains. Repeat the same steps you did for the upgrade, this time the specialty shop is in purgatory so head on down and get your gear, assuming you can afford it.&lt;/p&gt;</t>
+    <t>"Have you seen the house?" comes a voice. You look up from your plate while sitting in a pub in Smugglers Port.&lt;br /&gt; &lt;br /&gt; The House? What house?&lt;br /&gt; &lt;br /&gt; "There is a house where a man known as The Purgatory Smith lived. No one knows where he went once The Child escaped Purgatory. Some say he came to the Surface; some say he just vanished, the magic that created him has withered and died."&lt;br /&gt; &lt;br /&gt; He pauses and takes a sip from his mug; you stare in silence and absorb the words, digesting the meaning.&lt;br /&gt; &lt;br /&gt; But me, what does this have to do with me? You ponder this.&lt;br /&gt; &lt;br /&gt; "You, child, come into a place where you are a piece of the structure that held The Child in place. All of these people are. All of the adventurers are who come and seek out the riches and fame of this land and all the lands connected."&lt;br /&gt; &lt;br /&gt; A piece of the structure. What structure?&lt;br /&gt; &lt;br /&gt; "That cage."</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Now that we have Copper Coins and we have applied oils to our weapons and armor and coated ourselves up, we have another upgrade for gear to do: &lt;a href="/information/purgatory-chains-set" target="_blank"&gt;Purgatory Chains&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;This process is very similar to that of Hell Forged; don’t worry – all your hard work will be copied over to your new item.&lt;/p&gt;&lt;p&gt;Purgatory Chains gear is as far as you will be able to take your gear – at this time – by the process of upgrading through specialty shops like this.&lt;/p&gt;&lt;p&gt;At this stage, with a full set of Purgatory Chain covered in holy oils and dripping in high-end enchants that define your build – allowing you to do unimaginable damage – you still have a ways to go before you have truly reached your full potential.&lt;/p&gt;&lt;p&gt;After this, the last set of upgrades we have to work on is &lt;a href="/information/trinketry" target="_blank"&gt;trinkets&lt;/a&gt; and &lt;a href="/information/gems" target="_blank"&gt;gems&lt;/a&gt;. But one thing at a time, child; let's get some chains on our body, shall we?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;At this stage, we have already done the upgrade process for Crafted gear to Hell Forged. Now we go from Hell Forged to Purgatory Chains. Repeat the same steps you did for the upgrade; this time, the specialty shop is in Purgatory, so head on down and get your gear, assuming you can afford it.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Purgatory Chains</t>
@@ -794,16 +794,16 @@
     <t>Shattering the illusion</t>
   </si>
   <si>
-    <t>The Cage, its a mythical and legendary place – like the one that held Satan in the depths of Hell. It was created after that cage was created. It was created by the same man who create the first one. It was create by The Poet.&lt;br /&gt; &lt;br /&gt; “The Poet trapped Satan in a cage deep in the bowls of Hell, but even that was not enough magic to hold such a mighty beast. To hold a creature of the worlds power and beyond, The poet used the last of his immortal and angelic power to trap The Child in another plane, another dimension, where his own misery and loneliness could no longer corrupt the world around him.”&lt;br /&gt; &lt;br /&gt; The Guide stops to drink his ale and eat off his plate. The barmaid comes over and takes away the plates after some time.&lt;br /&gt; &lt;br /&gt; “The world is now the cage, the world, the people, the magic of it all. It’s all we have – but he is close to his ultimate goal.”&lt;br /&gt; &lt;br /&gt; His ultimate goal?&lt;br /&gt; &lt;br /&gt; “To shatter reality.”</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;We have some copper coins and we have seen that even with maxed out Holy Oils, powerful Enchants and end game gear – we cannot make it very far down the list. We keep getting &lt;a href="/information/ambush-and-counter" target="_blank"&gt;ambushed, countered&lt;/a&gt; and slaughtered.&lt;/p&gt;&lt;p&gt;This is where &lt;a href="/information/trinketry" target="_blank"&gt;trinkets&lt;/a&gt; come into play and a new concept: Ambush and Counter.&lt;/p&gt;&lt;p&gt;Ambush is where you have a chance to ambush the enemy and deal immense damage to the enemy before they can think, there's a chance for this to kill the enemy outright.&lt;/p&gt;&lt;p&gt;Alas, the enemy can Ambush you as well. Down here – in Purgatory – creatures will always ambush first – hence the second aspect of trinkets: Ambush Resistance. You can resit the enemies ambush.&lt;/p&gt;&lt;p&gt;The other aspects of trinkets that you might have also discovered down here is: Counter.&lt;/p&gt;&lt;p&gt;Countering is when you or the enemy jump in, after an action like Weapon Damage or Spell Damage and counter the attack with one of your own. This can also kill you or the enemy.&lt;/p&gt;&lt;p&gt;Characters can equip a single trinket and the only way to get them is to craft them.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;To stand a chance to make it further down the list in Purgatory we have to craft a trinket. These cannot be enchanted or have holy oils applied to them and they cannot be sold to the shop. The can be destroyed and listed on the market.&lt;/p&gt;&lt;p&gt;To be able to do any of this though, we need to craft them. So how do we do that?&lt;/p&gt;&lt;p&gt;- From Craft/Enchant select Trinketry – while on any plane.&lt;/p&gt;&lt;p&gt;- Select a trinket. These require Gold Dust and Copper Coins.&lt;/p&gt;&lt;p&gt;- Craft&lt;/p&gt;&lt;p&gt;That's all there is to it.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;To stand a chance to make it further down the list in Purgatory we have to craft a trinket. These cannot be enchanted or have holy oils applied to them and they cannot be sold to the shop. The can be destroyed and listed on the market.&lt;/p&gt;&lt;p&gt;To be able to do any of this though, we need to craft them. So how do we do that?&lt;/p&gt;&lt;p&gt;- Select Craft from the Actions Drop Down&lt;/p&gt;&lt;p&gt;- Select Trinketry – while on any plane.&lt;/p&gt;&lt;p&gt;- Select a trinket. These require Gold Dust and Copper Coins.&lt;/p&gt;&lt;p&gt;- Craft&lt;/p&gt;&lt;p&gt;That's all there is to it.&lt;/p&gt;</t>
+    <t>The Cage, it's a mythical and legendary place – like the one that held Satan in the depths of Hell. It was created after that cage was created. It was created by the same man who created the first one. It was created by The Poet.&lt;br /&gt; &lt;br /&gt; “The Poet trapped Satan in a cage deep in the bowels of Hell, but even that was not enough magic to hold such a mighty beast. To hold a creature of the world's power and beyond, The poet used the last of his immortal and angelic power to trap &lt;br /&gt; The Child in another plane, another dimension, where his own misery and loneliness could no longer corrupt the world around him.”&lt;br /&gt; &lt;br /&gt; The Guide stops to drink his ale and eat off his plate. The barmaid comes over and takes away the plates after some time.&lt;br /&gt; &lt;br /&gt; “The world is now the cage, the world, the people, the magic of it all. It’s all we have – but he is close to his ultimate goal.”&lt;br /&gt; &lt;br /&gt; His ultimate goal?&lt;br /&gt; &lt;br /&gt; “To shatter reality.”</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We have some copper coins, and we have seen that even with maxed out Holy Oils, powerful Enchants, and end-game gear – we cannot make it very far down the list. We keep getting &lt;a href="/information/ambush-and-counter" target="_blank"&gt;ambushed, countered&lt;/a&gt;, and slaughtered.&lt;/p&gt;&lt;p&gt;This is where &lt;a href="/information/trinketry" target="_blank"&gt;trinkets&lt;/a&gt; come into play and a new concept: Ambush and Counter.&lt;/p&gt;&lt;p&gt;Ambush is where you have a chance to ambush the enemy and deal immense damage to the enemy before they can think; there's a chance for this to kill the enemy outright.&lt;/p&gt;&lt;p&gt;Alas, the enemy can Ambush you as well. Down here – in Purgatory – creatures will always ambush first – hence the second aspect of trinkets: Ambush Resistance. You can resist the enemy's ambush.&lt;/p&gt;&lt;p&gt;The other aspects of trinkets that you might have also discovered down here are: Counter.&lt;/p&gt;&lt;p&gt;Countering is when you or the enemy jump in after an action like Weapon Damage or Spell Damage and counter the attack with one of your own. This can also kill you or the enemy.&lt;/p&gt;&lt;p&gt;Characters can equip a single trinket, and the only way to get them is to craft them.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;To stand a chance to make it further down the list in Purgatory, we have to craft a trinket. These cannot be enchanted or have holy oils applied to them, and they cannot be sold to the shop. They can be destroyed and listed on the market.&lt;/p&gt;&lt;p&gt;To be able to do any of this though, we need to craft them. So how do we do that?&lt;/p&gt;&lt;ul&gt;&lt;li&gt;From Craft/Enchant, select Trinketry – while on any plane.&lt;/li&gt;&lt;li&gt;Select a trinket. These require Gold Dust and Copper Coins.&lt;/li&gt;&lt;li&gt;Craft&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;That's all there is to it.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;To stand a chance to make it further down the list in Purgatory, we have to craft a trinket. These cannot be enchanted or have holy oils applied to them, and they cannot be sold to the shop. They can be destroyed and listed on the market.&lt;/p&gt;&lt;p&gt;To be able to do any of this though, we need to craft them. So how do we do that?&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Select Craft from the Actions Drop Down&lt;/li&gt;&lt;li&gt;Select Trinketry – while on any plane.&lt;/li&gt;&lt;li&gt;Select a trinket. These require Gold Dust and Copper Coins.&lt;/li&gt;&lt;li&gt;Craft&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;That's all there is to it.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Trinketry</t>
@@ -812,16 +812,16 @@
     <t>Introducing Faction Loyalty!!</t>
   </si>
   <si>
-    <t>A couple weeks back you heard of adventurers who were gaining some kind of loyalty with the citizens of their respective planes.&lt;br /&gt; &lt;br /&gt; You have poked around and asked a few of your own questions, in relation to this concept of fame and been told that through earning the highest achievement of faction with a plane with other citizens come and ask favors of you. As you assist them, you will make them happy and your relationship will deepen.&lt;br /&gt; &lt;br /&gt; You heard the rumors of currencies being handed out, valuable currencies needed for crafting. You also heard of better uniques then you currently have. How hard could it be to do a few mundane tasks for some citizens. But the question is, where do you start. The shiny rewards are calling but how do you collect them?</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Tlessa is expanding on the concept of &lt;a href="/information/factions" target="_blank"&gt;Factions&lt;/a&gt;. By now you know that killing creatures gets you faction points, which in turn gets you shiny unique items that make you feel more powerful.&lt;/p&gt;&lt;p&gt;This system is expanded to those who have maxed out their Faction with one or more planes. Characters who have &lt;a href="/information/faction-loyalty" target="_blank"&gt;will be able to click the Pledge button&lt;/a&gt; beside a faction to pledge to that Plane.&lt;/p&gt;&lt;p&gt;This then allows you to assist NPC’s with two types of tasks: Bounties and Crafting.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Bounties&lt;/strong&gt; are tasks where you must manually kill the creatures and a specific amount of them.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Crafting&lt;/strong&gt; is where you craft a specific item and a specific amount of them.&lt;/p&gt;&lt;p&gt;Both set of tasks are balanced such that even newer players who might have maxed Surface Faction to participate.&lt;/p&gt;&lt;p&gt;Players who assist the NPC with their tasks will earn fame. As you earn fame with an NPC you will be rewarded with rewards equal to the current level (or a default of 1x) x a base set of rewards. You’ll see the base rewards when you begin assisting an NPC.&lt;/p&gt;&lt;p&gt;Players can assist 1 NPC at a time and pledge to 1 Faction at a time. Players can switch at any time, but – aside from the rewards – it is suggested you stick with maxing out one NPC at a time due to the secondary passive fame provides: Kingdom Item Protection.&lt;/p&gt;&lt;p&gt;As you will learn later on, Players can craft items that can be dropped on kingdoms reducing them to smoldering ash – all that hard work – gone!&lt;/p&gt;&lt;p&gt;With Faction Loyalty – and therefore earning fame, kingdoms on the plane you are actively pledged to will gain a bonus % towards item damage resistance to a max of 100% making units the only way to attack a kingdom.&lt;/p&gt;&lt;p&gt;For now, lets focus on getting to know the NPC we want to assist.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;First, max out a faction. Weather is be Labyrinth, Surface – what ever you please. To do that, this quest will give you bonus faction points per kill to help you speed that process up.&lt;/p&gt;&lt;p&gt;Once you have the faction maxed out:&lt;/p&gt;&lt;p&gt;- Go to your character sheet, click on the Factions tab and click Pledge.&lt;/p&gt;&lt;p&gt;- Once Pledged, go back to your action section and you will see a new tab: Faction Loyalty.&lt;/p&gt;&lt;p&gt;- Click the new tab, which only appears while you are pledged to a faction.&lt;/p&gt;&lt;p&gt;- Find an NPC in the drop down to the top left, by default you will see the first NPC in the list. If you are assisting an NPC, every time you open this tab – you will see that NPC, instead of the first one.&lt;/p&gt;&lt;p&gt;- However, if you stop pledging to a faction or switch to another one, you will stop assisting the NPC and thus will not see it as the first NPC when you go back to pledging to that faction.&lt;/p&gt;&lt;p&gt;- Find an NPC you want to help and then click the blue button beside the drop down: Assist.&lt;/p&gt;&lt;p&gt;You are now assisting this NPC, any actions related to the bounties or the crafting can count towards their retirements. For example: If you are assisting The Poet and his bounty task is 25 Sewer Rat, you can select Sewer Rat and MANUALLY kill the creature 25 times. That’s easy.&lt;/p&gt;&lt;p&gt;If he has a crafting task of craft 15 Broken Daggers, you simply have to select that item in the crafting section for weapons and a new button will appear: Craft for NPC. Click this, instead of Craft to craft for the NPC. The same crafting rules apply as if you were crafting it for you.&lt;/p&gt;&lt;p&gt;When you craft for an NPC, you will not receive the item, you will pay the cost, but not receive the item. The NPC will thank you for assisting them when you craft an item.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;First, max out a faction. Weather is be Labyrinth, Surface – what ever you please. To do that, this quest will give you bonus faction points per kill to help you speed that process up.&lt;/p&gt;&lt;p&gt;Once you have the faction maxed out:&lt;/p&gt;&lt;p&gt;- Go to your character sheet, tap on the Factions tab after expanding the top section and tap Pledge.&lt;/p&gt;&lt;p&gt;- Once Pledged, go back to your action section and you will see a new tab: Faction Loyalty.&lt;/p&gt;&lt;p&gt;- Tap the new tab, which only appears while you are pledged to a faction.&lt;/p&gt;&lt;p&gt;- Find an NPC in the drop down to the top left, by default you will see the first NPC in the list. If you are assisting an NPC, every time you open this tab – you will see that NPC, instead of the first one.&lt;/p&gt;&lt;p&gt;- However, if you stop pledging to a faction or switch to another one, you will stop assisting the NPC and thus will not see it as the first NPC when you go back to pledging to that faction.&lt;/p&gt;&lt;p&gt;- Find an NPC you want to help and then tap the blue button beside the drop down: Assist.&lt;/p&gt;&lt;p&gt;You are now assisting this NPC, any actions related to the bounties or the crafting can count towards their retirements. For example: If you are assisting The Poet and his bounty task is 25 Sewer Rat, you can select Sewer Rat and MANUALLY kill the creature 25 times. That’s easy.&lt;/p&gt;</t>
+    <t>A couple of weeks back, you heard of adventurers who were gaining some kind of loyalty with the citizens of their respective planes.&lt;br /&gt; &lt;br /&gt; You have poked around and asked a few of your own questions, in relation to this concept of fame, and been told that through earning the highest achievement of faction with a plane, other citizens come and ask favors of you. As you assist them, &lt;br /&gt; you will make them happy, and your relationship will deepen.&lt;br /&gt; &lt;br /&gt; You heard the rumors of currencies being handed out, valuable currencies needed for crafting. You also heard of better uniques than you currently have. How hard could it be to do a few mundane tasks for some citizens? But the question is, where &lt;br /&gt; do you start? The shiny rewards are calling, but how do you collect them?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Tlessa is expanding on the concept of &lt;a href="/information/factions" target="_blank"&gt;Factions&lt;/a&gt;. By now, you know that killing creatures gets you faction points, which in turn gets you shiny unique items that make you feel more powerful.&lt;/p&gt;&lt;p&gt;This system is expanded to those who have maxed out their Faction with one or more planes. Characters &lt;a href="/information/faction-loyalty" target="_blank"&gt;who have, will be able to click the Pledge button&lt;/a&gt; beside a faction to pledge to that Plane.&lt;/p&gt;&lt;p&gt;This then allows you to assist NPC’s with two types of tasks: Bounties and Crafting.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Bounties&lt;/strong&gt; are tasks where you must manually kill the creatures and a specific amount of them.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Crafting&lt;/strong&gt; is where you craft a specific item and a specific amount of them.&lt;/p&gt;&lt;p&gt;Both sets of tasks are balanced such that even newer players who might have maxed Surface Faction to participate.&lt;/p&gt;&lt;p&gt;Players who assist the NPC with their tasks will earn fame. As you earn fame with an NPC, you will be rewarded with rewards equal to the current level (or a default of 1x) x a base set of rewards. You’ll see the base rewards when you begin &lt;/p&gt;&lt;p&gt;assisting an NPC.&lt;/p&gt;&lt;p&gt;Players can assist 1 NPC at a time and pledge to 1 Faction at a time. Players can switch at any time, but – aside from the rewards – it is suggested you stick with maxing out one NPC at a time due to the secondary passive fame provides: &lt;/p&gt;&lt;p&gt;Kingdom Item Protection.&lt;/p&gt;&lt;p&gt;As you will learn later on, Players can craft items that can be dropped on kingdoms reducing them to smoldering ash – all that hard work – gone!&lt;/p&gt;&lt;p&gt;With Faction Loyalty – and therefore earning fame, kingdoms on the plane you are actively pledged to will gain a bonus % towards item damage resistance to a max of 100% making units the only way to attack a kingdom.&lt;/p&gt;&lt;p&gt;For now, let's focus on getting to know the NPC we want to assist.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;First, max out a faction. Whether it be Labyrinth, Surface – whatever you please. To do that, this quest will give you bonus faction points per kill to help you speed up that process.&lt;/p&gt;&lt;p&gt;Once you have the faction maxed out:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Go to your character sheet, click on the Factions tab, and click Pledge.&lt;/li&gt;&lt;li&gt;Once Pledged, go back to your action section, and you will see a new tab: Faction Loyalty.&lt;/li&gt;&lt;li&gt;Click the new tab, which only appears while you are pledged to a faction.&lt;/li&gt;&lt;li&gt;Find an NPC in the drop-down to the top left, by default, you will see the first NPC in the list. If you are assisting an NPC, every time you open this tab – you will see that NPC, instead of the first one.&lt;/li&gt;&lt;li&gt;However, if you stop pledging to a faction or switch to another one, you will stop assisting the NPC and thus will not see it as the first NPC when you go back to pledging to that faction.&lt;/li&gt;&lt;li&gt;Find an NPC you want to help and then click the blue button beside the drop-down: Assist.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;You are now assisting this NPC, any actions related to the bounties or the crafting can count towards their retirements. For example: If you are assisting The Poet and his bounty task is 25 Sewer Rats, you can select Sewer Rats and MANUALLY &lt;/p&gt;&lt;p&gt;kill the creature 25 times. That’s easy.&lt;/p&gt;&lt;p&gt;If he has a crafting task of crafting 15 Broken Daggers, you simply have to select that item in the crafting section for weapons, and a new button will appear: Craft for NPC. Click this, instead of Craft to craft for the NPC. The same crafting rules &lt;/p&gt;&lt;p&gt;apply as if you were crafting it for yourself.&lt;/p&gt;&lt;p&gt;When you craft for an NPC, you will not receive the item; you will pay the cost but not receive the item. The NPC will thank you for assisting them when you craft an item.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;First, max out a faction. Whether it be Labyrinth, Surface – whatever you please. To do that, this quest will give you bonus faction points per kill to help you speed up that process.&lt;/p&gt;&lt;p&gt;Once you have the faction maxed out:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Go to your character sheet, tap on the Factions tab after expanding the top section and tap Pledge.&lt;/li&gt;&lt;li&gt;Once Pledged, go back to your action section, and you will see a new tab: Faction Loyalty.&lt;/li&gt;&lt;li&gt;Tap the new tab, which only appears while you are pledged to a faction.&lt;/li&gt;&lt;li&gt;Find an NPC in the drop-down to the top left, by default, you will see the first NPC in the list. If you are assisting an NPC, every time you open this tab – you will see that NPC, instead of the first one.&lt;/li&gt;&lt;li&gt;However, if you stop pledging to a faction or switch to another one, you will stop assisting the NPC and thus will not see it as the first NPC when you go back to pledging to that faction.&lt;/li&gt;&lt;li&gt;Find an NPC you want to help and then tap the blue button beside the drop-down: Assist.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;You are now assisting this NPC, any actions related to the bounties or the crafting can count towards their retirements. For example: If you are assisting The Poet and his bounty task is 25 Sewer Rats, you can select Sewer Rats and MANUALLY kill the creature 25 times. That’s easy.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Added a new skill, new alchemy item and new guide quests.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="290">
   <si>
     <t>id</t>
   </si>
@@ -374,6 +374,21 @@
     <t>&lt;ul&gt;&lt;li&gt;Tap the Character Sheet tab.&lt;/li&gt;&lt;li&gt;Expand the Character Details Section.&lt;/li&gt;&lt;li&gt;Tap the Class Ranks orange button.&lt;/li&gt;&lt;li&gt;Look for your class in the list and tap the name.&lt;/li&gt;&lt;li&gt;This will open another window, to exit back to the class list tap the red circle with the minus in the top right. Tap cancel or the X will close the modal.&lt;/li&gt;&lt;li&gt;Here you will see information about the class and the Class Masteries.&lt;/li&gt;&lt;li&gt;Tap Manage Specialties.&lt;/li&gt;&lt;li&gt;Equip a specialty and boom done, now you just have to kill creatures.&lt;/li&gt;&lt;li&gt;The server messages will tell you when you gain levels in your Masteries and your Specialties as well as your Class Rank.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Now you just have to kill creatures till you meet the requirements.&lt;/p&gt;</t>
   </si>
   <si>
+    <t>Gamble the horror away</t>
+  </si>
+  <si>
+    <t>You managed to make your way to Smugglers Port, where you heard of a game that can be played and where one can attempt to win currencies!&lt;br /&gt; &lt;br /&gt; You asked around the port town, and people have told you what they know and pointed you to a pub where a man stands by a weird-looking box that magically seems to change and roll. People give money and watch this box split into three and roll, sometimes the images match, sometimes they don’t, and the patrons leave with no money or even less than they had.&lt;br /&gt; &lt;br /&gt; You decide to take a gamble and take a moment for yourself.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Let's &lt;a href="/information/slots" target="_blank"&gt;gamble&lt;/a&gt; and have some fun! First, we want to unlock a feature that will help us, not just when gambling but also when fighting creatures! We need currencies – Gold Dust and eventually Shards – which are also used in quests and a new type of crafting we will soon unlock: &lt;a href="/information/alchemy" target="_blank"&gt;Alchemy&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;This new feature is called: &lt;a href="/information/mercenary" target="_blank"&gt;Mercenaries&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;Mercenaries allow you to gain more currencies as you level them and then reincarnate them. They will give a bonus which is equal to their level and the amount of times (to a max of 1100%) towards currency acquisition for Shards, Gold Dust, and Copper Coins.&lt;/p&gt;&lt;p&gt;Mercenaries help out the most with &lt;a href="/information/slots" target="_blank"&gt;Slots&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;Slots is a way for players to gamble and potentially win currencies. The caveat is one of the currencies cannot be rewarded at this time because you don’t have the right quest item, Copper Coins.&lt;/p&gt;&lt;p&gt;To level a Mercenary, you need to complete a quest to unlock the feature and then pay gold to purchase the type of mercenary you want.&lt;/p&gt;&lt;p&gt;After that, all you have to do is fight creatures, and over time the Mercenaries will level. As you reach level 100 on one of them, you can reincarnate them, re-level them up and gain 200% towards currency acquisition. Then just repeat this process 9 more times.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Complete the quest on Labyrinth: "The truth is out there."&lt;/li&gt;&lt;li&gt;Click the Character Sheet Tab.&lt;/li&gt;&lt;li&gt;Click the tab: Mercenaries.&lt;/li&gt;&lt;li&gt;Purchase the mercenaries required.&lt;/li&gt;&lt;li&gt;Level the Mercenary to the required leveling.&lt;/li&gt;&lt;li&gt;Play slots if you have the gold and kill creatures to level the mercenaries through exploration!&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Complete the quest on Labyrinth: "The truth is out there."&lt;/li&gt;&lt;li&gt;Tap the Character Sheet Tab.&lt;/li&gt;&lt;li&gt;Tap the tab: Mercenaries.&lt;/li&gt;&lt;li&gt;Purchase the mercenaries required.&lt;/li&gt;&lt;li&gt;Level the Mercenary to the required leveling.&lt;/li&gt;&lt;li&gt;Play slots (select slots from the actions drop-down) if you have the gold and kill creatures to level the mercenaries!&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>Farmers in the fields</t>
   </si>
   <si>
@@ -789,6 +804,87 @@
   </si>
   <si>
     <t>&lt;p&gt;First, max out a faction. Whether it be Labyrinth, Surface – whatever you please. To do that, this quest will give you bonus faction points per kill to help you speed up that process.&lt;/p&gt;&lt;p&gt;Once you have the faction maxed out:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Go to your character sheet, tap on the Factions tab after expanding the top section and tap Pledge.&lt;/li&gt;&lt;li&gt;Once Pledged, go back to your action section, and you will see a new tab: Faction Loyalty.&lt;/li&gt;&lt;li&gt;Tap the new tab, which only appears while you are pledged to a faction.&lt;/li&gt;&lt;li&gt;Find an NPC in the drop-down to the top left, by default, you will see the first NPC in the list. If you are assisting an NPC, every time you open this tab – you will see that NPC, instead of the first one.&lt;/li&gt;&lt;li&gt;However, if you stop pledging to a faction or switch to another one, you will stop assisting the NPC and thus will not see it as the first NPC when you go back to pledging to that faction.&lt;/li&gt;&lt;li&gt;Find an NPC you want to help and then tap the blue button beside the drop-down: Assist.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;You are now assisting this NPC, any actions related to the bounties or the crafting can count towards their retirements. For example: If you are assisting The Poet and his bounty task is 25 Sewer Rats, you can select Sewer Rats and MANUALLY kill the creature 25 times. That’s easy.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>The story continues</t>
+  </si>
+  <si>
+    <t>Reality. What is reality these days when it comes to the world you have been exploring? There is darkness, a sickness that infests the hearts and minds of this world. There is a truth that lingers in the shadows of depravity and washes over one's twisted and corrupted mind.&lt;br /&gt; &lt;br /&gt; The Shattering of reality. The Poet never went further into details, but something tells you this isn’t the first time such a situation has played itself out. It’s time to hunt for some answers.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Today, we are going to learn about quest chains. There are a lot of quests, as you have seen in Tlessa, and you have even participated in more than a few of them, but they don’t seem to come together all that much to give you a sense of the overarching storyline.&lt;/p&gt;&lt;p&gt;Starting in Dungeons is a quest line called: "Looking for a Prince."&lt;/p&gt;&lt;p&gt;If you then go to Shadow Planes and see the quest tree for that plane, you will see a new quest called "Hunting for a Lead." This carries on into Hell.&lt;/p&gt;&lt;p&gt;What's important here is that "Hunting for a new lead" is not green, red, or blue. It's yellow. Yellow quests indicate you must either complete a previous quest or, in this case, complete a previous quest chain.&lt;/p&gt;&lt;p&gt;The previous quest chain for "Hunting a new lead" is "Looking for a Prince," going straight down to "Twisted Paths."&lt;/p&gt;&lt;p&gt;These types of quests tell an entire story that plays off all the quests you have done so far to unify the story into one central theme.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We already know how to craft trinkets, so let's keep doing that. We also know how to complete quests, so let's complete the first quest line: "Looking for a Prince" all the way down to "Twisted Paths."&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Twisted Paths</t>
+  </si>
+  <si>
+    <t>Expanding our resources</t>
+  </si>
+  <si>
+    <t>It becomes evident to you, through the people you interact with, through the stories they tell, through the harrowing existences that they lead, that this world is full of a sadness and deep suffering you cannot comprehend.&lt;br /&gt; &lt;br /&gt; You seek out the solace of your own keep, your own kingdoms, the ones you have neglected since you have been on the road to what seems like nowhere. Cryptic puzzles, cryptic words, unending slaughter fest. You &lt;br /&gt; never quite feel strong enough and constantly wonder how you will survive the world around you, with all its pain and misery.&lt;br /&gt; &lt;br /&gt; Maybe you can feed off it. Or, at least – use it for company.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;As we ascend in level and contemplate reincarnation further, we need to consider our kingdoms. Creatures from here on out only grow more formidable, and survival at the bottom of the list is not guaranteed.&lt;/p&gt;&lt;p&gt;It becomes less about vanquishing the monster at the bottom of the list and more about fine-tuning your build, your class ranks. At this stage, you should have a class maxed out on your &lt;a href="/information/class-ranks" target="_blank"&gt;class rank&lt;/a&gt;, and you should also &lt;/p&gt;&lt;p&gt;have at least specialties equipped, whether you have been switching classes or not.&lt;/p&gt;&lt;p&gt;But, we also need &lt;a href="/information/currencies#1" target="_blank"&gt;Gold Bars&lt;/a&gt;. &lt;a href="/information/goblin-shop" target="_blank"&gt;The Goblin shop&lt;/a&gt; offers items like Dust of Darkness and Goblin Garbage Stew that aid players on the road to &lt;a href="/information/reincarnation" target="_blank"&gt;reincarnation&lt;/a&gt;. To do this, we want to fortify our kingdoms, so we need even more resources to recruit additional units for protection.&lt;/p&gt;&lt;p&gt;Let's train some new &lt;a href="/information/kingdom-passive-skills" target="_blank"&gt;passives&lt;/a&gt; while we work on our trinketry. We should also stock up on Gold Bars and units to fortify our kingdoms.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;There are passives that assist a kingdom once its resource-generating buildings are at max level, such as the Lumber Mill, Stone Quarry, Clay Pit, and Iron Mines. At max level, when you click on the building, you will see a new concept called expansion. These expansions take time, resources, and population to complete but increase your max amount of resources that building can generate. More resources mean more units.&lt;/p&gt;&lt;p&gt;Let's initiate this process by training Bountiful Resources to level 4.&lt;/p&gt;&lt;p&gt;In the meantime, let's also ensure our Lumber Mill in one of our kingdoms is at max level.&lt;/p&gt;&lt;p&gt;And finally, let's deposit some of our gold into our kingdoms, particularly those with the Goblin Coin Bank at level 5, so we have a stockpile of Gold Bars.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;There are passives that assist a kingdom once its resource-generating buildings are at max level, such as the Lumber Mill, Stone Quarry, Clay Pit, and Iron Mines. At max level, when you click on the building, you will &lt;/p&gt;&lt;p&gt;see a new concept called expansion. These expansions take time, resources, and population to complete but increase your max amount of resources that building can generate. More resources mean more units.&lt;/p&gt;&lt;p&gt;Let's initiate this process by training Bountiful Resources to level 4.&lt;/p&gt;&lt;p&gt;In the meantime, let's also ensure our Lumber Mill in one of our kingdoms is at max level.&lt;/p&gt;&lt;p&gt;And finally, let's deposit some of our gold into our kingdoms, particularly those with the Goblin Coin Bank at level 5, so we have a stockpile of Gold Bars.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Lumber Mill</t>
+  </si>
+  <si>
+    <t>Bountiful Resources</t>
+  </si>
+  <si>
+    <t>The Path Forward</t>
+  </si>
+  <si>
+    <t>It has been a few weeks since you left your kingdom. A letter arrives for you from The Wandering Merchant asking you to continue your investigations into the realm of Twisted things. He believes there is a force trying to break free from the other side of a gate that has appeared in Hell.&lt;br /&gt; &lt;br /&gt; You read the letter over and contemplate if you want to get involved in something that seems so beyond you and your abilities. As if you are meddling with forces beyond one's own comprehension.&lt;br /&gt; &lt;br /&gt; Are you even strong enough, not just physically and magically but mentally and emotionally? Do you really want to take on other people's baggage, drama, and issues of a time long past, of a time that seems to be haunting you, a person with no role in the past, only that of the present? A role you didn’t even ask for, one forced upon you.&lt;br /&gt; &lt;br /&gt; What do you do?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We are not quite strong enough; we need more trinket crafting – but aside from that, we want more stats. More damage. To do this, we should look at using alchemy items, like Solar Dust and those from the Goblin Shop.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;: To hand in this quest, you will need to make use of alchemy items and only hand it in when the alchemy items are active, under your Character Sheet → Active Boons section. If you are on mobile, that is phones – you have a button called Active Boons right above your actions section. Best to do this on the surface.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Continue your journeys into trinketry; that will be valuable. But also let's start crafting some Solar Dusts and purchasing some Goblin Shop Alchemy items like Dust of Darkness and others that will help you level.&lt;/p&gt;&lt;p&gt;You need boons, possibly, to achieve this as well as reincarnation. However you choose to accomplish this, if you are using alchemy items, make sure to turn the quest in while the alchemy items are in effect.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>The Twisted Gate</t>
+  </si>
+  <si>
+    <t>You sit on your bed in the silence of your chambers and pore over the letter from The Wandering Merchant that arrived three weeks ago.&lt;br /&gt; &lt;br /&gt; You had your maesters reach out and inform them that you will be headed to Shadow Planes soon enough. You feel slightly more powerful, but how powerful are you really? It’s not about the physical strength or the magical aptitude that one possesses. It's about the mental and emotional strength to carry the pain and torment of the twisted and delusional souls on your own frail shoulders.&lt;br /&gt; &lt;br /&gt; You pack the last of your things, sharpen your weapons, and hone your strength. Now is not the time to misstep; now is the time to hunt for answers. To put an end to this drama of some poor sobbing child, who like so many others – could not let go.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We are in the final stretches of trinketry training. We have utilized our kingdoms, our alchemy items – grown in power. But now we need more of it and to continue the story we started a while back with "Looking for a Prince." Continue that quest line until we are in the depths of hell itself.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;: If you make use of alchemy items, when the alchemy items are active, under your Character Sheet → Active Boons section. If you are on mobile, that is phones – you have a button called Active Boons right above &lt;/p&gt;&lt;p&gt;your actions section – and your stats match that of the required stats, hand in the quest! Best to do this on a surface.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We know how to craft trinkets, make use of alchemy items, and our class ranks, specialties, and class skills.&lt;/p&gt;&lt;p&gt;It’s time we wrap it all together and continue the main storyline headed for a new plane of existence!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Twisted Memories</t>
+  </si>
+  <si>
+    <t>Twisted Branches</t>
+  </si>
+  <si>
+    <t>Twisted Tree Branch</t>
+  </si>
+  <si>
+    <t>Twsited Memories</t>
+  </si>
+  <si>
+    <t>You made it. You stand before the gate in Hell, a gate to a world where the memories of those are twisted. You have learned more about The Shattering; you have tried to track down this mysterious Wandering Prince, some say he is the Prince of Emeralds himself, a man from another plane of existence where he shut away his world when The Shattering happened.&lt;br /&gt; &lt;br /&gt; You ponder for a moment if this is what The Creator wants: to shatter the realities, to fling forth the gates of despair and unleash the torment of suffering onto others. Has he not done enough damage to the people around him, the lovers of this world – the parents of another?&lt;br /&gt; &lt;br /&gt; The selfishness and the greediness. You shake your head for a moment, but can hear a whispering of another time and place that haunts you. You step through the gate.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We made it to the new world! To the new plane of existence. To Twisted Memories!&lt;/p&gt;&lt;p&gt;This is the second aspect of the endgame, a new map, with stronger creatures and steeper reductions. It is less about killing in one shot and more about utilizing alchemy items, your gear, and your class specialties to survive down here and slowly level your character through reincarnation.&lt;/p&gt;&lt;p&gt;There are new quests that continue the story of how you got here.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Continue using what you learned to raise your stats even higher. The trick is down here, though; you need to be on this plane to hand in the quest. So it might take some time and some reincarnations.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -1128,7 +1224,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:BE36"/>
+  <dimension ref="A1:BE42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1187,7 +1283,7 @@
     <col min="49" max="49" width="9.10" bestFit="true" style="0"/>
     <col min="50" max="50" width="21.138" bestFit="true" customWidth="true" style="0"/>
     <col min="51" max="51" width="9.10" bestFit="true" style="0"/>
-    <col min="52" max="52" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="52" max="52" width="19.995" bestFit="true" customWidth="true" style="0"/>
     <col min="53" max="53" width="39.99" bestFit="true" customWidth="true" style="0"/>
     <col min="54" max="54" width="24.708" bestFit="true" customWidth="true" style="0"/>
     <col min="55" max="55" width="26.993" bestFit="true" customWidth="true" style="0"/>
@@ -1783,7 +1879,7 @@
     </row>
     <row r="12" spans="1:57">
       <c r="A12">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
         <v>119</v>
@@ -1800,14 +1896,11 @@
       <c r="F12" t="s">
         <v>123</v>
       </c>
-      <c r="AA12">
-        <v>1</v>
-      </c>
-      <c r="AB12">
-        <v>30</v>
-      </c>
-      <c r="AC12">
-        <v>100</v>
+      <c r="AP12">
+        <v>1000</v>
+      </c>
+      <c r="AQ12">
+        <v>1000</v>
       </c>
       <c r="AR12">
         <v>1000000</v>
@@ -1818,7 +1911,7 @@
     </row>
     <row r="13" spans="1:57">
       <c r="A13">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
         <v>124</v>
@@ -1835,32 +1928,17 @@
       <c r="F13" t="s">
         <v>128</v>
       </c>
-      <c r="H13" t="s">
-        <v>93</v>
-      </c>
-      <c r="I13">
-        <v>25</v>
-      </c>
-      <c r="J13" t="s">
-        <v>129</v>
-      </c>
-      <c r="K13">
-        <v>5</v>
+      <c r="AA13">
+        <v>1</v>
       </c>
       <c r="AB13">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="AC13">
-        <v>500</v>
-      </c>
-      <c r="AF13" t="s">
-        <v>130</v>
-      </c>
-      <c r="AG13">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="AR13">
-        <v>2000000</v>
+        <v>1000000</v>
       </c>
       <c r="AS13">
         <v>100</v>
@@ -1868,34 +1946,46 @@
     </row>
     <row r="14" spans="1:57">
       <c r="A14">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D14" t="s">
         <v>131</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
         <v>132</v>
       </c>
-      <c r="D14" t="s">
+      <c r="F14" t="s">
         <v>133</v>
       </c>
-      <c r="E14" t="s">
+      <c r="H14" t="s">
+        <v>93</v>
+      </c>
+      <c r="I14">
+        <v>25</v>
+      </c>
+      <c r="J14" t="s">
         <v>134</v>
       </c>
-      <c r="F14" t="s">
-        <v>134</v>
+      <c r="K14">
+        <v>5</v>
       </c>
       <c r="AB14">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="AC14">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="AF14" t="s">
         <v>135</v>
       </c>
       <c r="AG14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AR14">
         <v>2000000</v>
@@ -1906,7 +1996,7 @@
     </row>
     <row r="15" spans="1:57">
       <c r="A15">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
         <v>136</v>
@@ -1923,41 +2013,20 @@
       <c r="F15" t="s">
         <v>139</v>
       </c>
-      <c r="H15" t="s">
-        <v>78</v>
-      </c>
-      <c r="I15">
-        <v>25</v>
-      </c>
-      <c r="J15" t="s">
-        <v>93</v>
-      </c>
-      <c r="K15">
-        <v>50</v>
-      </c>
-      <c r="N15">
+      <c r="AB15">
+        <v>75</v>
+      </c>
+      <c r="AC15">
+        <v>2000</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG15">
         <v>2</v>
       </c>
-      <c r="O15">
-        <v>10</v>
-      </c>
-      <c r="S15" t="s">
-        <v>140</v>
-      </c>
-      <c r="AB15">
-        <v>100</v>
-      </c>
-      <c r="AC15">
-        <v>3000</v>
-      </c>
-      <c r="AF15" t="s">
-        <v>141</v>
-      </c>
-      <c r="AG15">
-        <v>1</v>
-      </c>
       <c r="AR15">
-        <v>5000000</v>
+        <v>2000000</v>
       </c>
       <c r="AS15">
         <v>100</v>
@@ -1965,70 +2034,58 @@
     </row>
     <row r="16" spans="1:57">
       <c r="A16">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C16" t="s">
         <v>142</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>143</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>144</v>
       </c>
-      <c r="E16" t="s">
-        <v>145</v>
-      </c>
       <c r="F16" t="s">
-        <v>145</v>
-      </c>
-      <c r="G16">
-        <v>500</v>
+        <v>144</v>
       </c>
       <c r="H16" t="s">
+        <v>78</v>
+      </c>
+      <c r="I16">
+        <v>25</v>
+      </c>
+      <c r="J16" t="s">
         <v>93</v>
-      </c>
-      <c r="I16">
-        <v>100</v>
-      </c>
-      <c r="J16" t="s">
-        <v>94</v>
       </c>
       <c r="K16">
         <v>50</v>
       </c>
-      <c r="L16">
+      <c r="N16">
+        <v>2</v>
+      </c>
+      <c r="O16">
+        <v>10</v>
+      </c>
+      <c r="S16" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB16">
+        <v>100</v>
+      </c>
+      <c r="AC16">
+        <v>3000</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>146</v>
+      </c>
+      <c r="AG16">
         <v>1</v>
       </c>
-      <c r="M16">
-        <v>100</v>
-      </c>
-      <c r="P16" t="s">
-        <v>146</v>
-      </c>
-      <c r="Q16">
-        <v>3</v>
-      </c>
-      <c r="R16" t="s">
-        <v>146</v>
-      </c>
-      <c r="S16" t="s">
-        <v>147</v>
-      </c>
-      <c r="T16" t="s">
-        <v>148</v>
-      </c>
-      <c r="U16" t="s">
-        <v>149</v>
-      </c>
-      <c r="W16">
-        <v>25000</v>
-      </c>
-      <c r="AQ16">
-        <v>1000</v>
-      </c>
       <c r="AR16">
-        <v>50000000</v>
+        <v>5000000</v>
       </c>
       <c r="AS16">
         <v>100</v>
@@ -2036,46 +2093,70 @@
     </row>
     <row r="17" spans="1:57">
       <c r="A17">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D17" t="s">
+        <v>149</v>
+      </c>
+      <c r="E17" t="s">
         <v>150</v>
       </c>
-      <c r="C17" t="s">
+      <c r="F17" t="s">
+        <v>150</v>
+      </c>
+      <c r="G17">
+        <v>500</v>
+      </c>
+      <c r="H17" t="s">
+        <v>93</v>
+      </c>
+      <c r="I17">
+        <v>100</v>
+      </c>
+      <c r="J17" t="s">
+        <v>94</v>
+      </c>
+      <c r="K17">
+        <v>50</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>100</v>
+      </c>
+      <c r="P17" t="s">
         <v>151</v>
       </c>
-      <c r="D17" t="s">
+      <c r="Q17">
+        <v>3</v>
+      </c>
+      <c r="R17" t="s">
+        <v>151</v>
+      </c>
+      <c r="S17" t="s">
         <v>152</v>
       </c>
-      <c r="E17" t="s">
+      <c r="T17" t="s">
         <v>153</v>
       </c>
-      <c r="F17" t="s">
+      <c r="U17" t="s">
         <v>154</v>
       </c>
-      <c r="G17">
-        <v>600</v>
-      </c>
-      <c r="H17" t="s">
-        <v>155</v>
-      </c>
-      <c r="I17">
-        <v>3</v>
-      </c>
-      <c r="N17">
-        <v>3</v>
-      </c>
-      <c r="O17">
-        <v>10</v>
-      </c>
-      <c r="AP17">
+      <c r="W17">
         <v>25000</v>
       </c>
       <c r="AQ17">
         <v>1000</v>
       </c>
       <c r="AR17">
-        <v>75000000</v>
+        <v>50000000</v>
       </c>
       <c r="AS17">
         <v>100</v>
@@ -2083,66 +2164,54 @@
     </row>
     <row r="18" spans="1:57">
       <c r="A18">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
+        <v>155</v>
+      </c>
+      <c r="C18" t="s">
         <v>156</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>157</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>158</v>
-      </c>
-      <c r="E18" t="s">
-        <v>159</v>
       </c>
       <c r="F18" t="s">
         <v>159</v>
       </c>
       <c r="G18">
-        <v>1000</v>
-      </c>
-      <c r="J18" t="s">
-        <v>93</v>
-      </c>
-      <c r="K18">
-        <v>400</v>
-      </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
-      <c r="M18">
-        <v>400</v>
+        <v>600</v>
+      </c>
+      <c r="H18" t="s">
+        <v>160</v>
+      </c>
+      <c r="I18">
+        <v>3</v>
       </c>
       <c r="N18">
         <v>3</v>
       </c>
       <c r="O18">
-        <v>30</v>
-      </c>
-      <c r="S18" t="s">
-        <v>160</v>
-      </c>
-      <c r="AH18">
-        <v>6000</v>
+        <v>10</v>
       </c>
       <c r="AP18">
-        <v>50000</v>
+        <v>25000</v>
       </c>
       <c r="AQ18">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="AR18">
-        <v>2000000000</v>
+        <v>75000000</v>
       </c>
       <c r="AS18">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:57">
       <c r="A19">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
         <v>161</v>
@@ -2160,22 +2229,37 @@
         <v>164</v>
       </c>
       <c r="G19">
-        <v>1500</v>
-      </c>
-      <c r="P19" t="s">
+        <v>1000</v>
+      </c>
+      <c r="J19" t="s">
+        <v>93</v>
+      </c>
+      <c r="K19">
+        <v>400</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>400</v>
+      </c>
+      <c r="N19">
+        <v>3</v>
+      </c>
+      <c r="O19">
+        <v>30</v>
+      </c>
+      <c r="S19" t="s">
         <v>165</v>
       </c>
-      <c r="Q19">
-        <v>2</v>
-      </c>
-      <c r="R19" t="s">
-        <v>165</v>
-      </c>
-      <c r="T19" t="s">
-        <v>166</v>
-      </c>
       <c r="AH19">
-        <v>7000</v>
+        <v>6000</v>
+      </c>
+      <c r="AP19">
+        <v>50000</v>
+      </c>
+      <c r="AQ19">
+        <v>5000</v>
       </c>
       <c r="AR19">
         <v>2000000000</v>
@@ -2186,28 +2270,40 @@
     </row>
     <row r="20" spans="1:57">
       <c r="A20">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
+        <v>166</v>
+      </c>
+      <c r="C20" t="s">
         <v>167</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>168</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>169</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
+        <v>169</v>
+      </c>
+      <c r="G20">
+        <v>1500</v>
+      </c>
+      <c r="P20" t="s">
         <v>170</v>
       </c>
-      <c r="F20" t="s">
+      <c r="Q20">
+        <v>2</v>
+      </c>
+      <c r="R20" t="s">
         <v>170</v>
       </c>
-      <c r="G20">
-        <v>2000</v>
-      </c>
-      <c r="S20" t="s">
+      <c r="T20" t="s">
         <v>171</v>
+      </c>
+      <c r="AH20">
+        <v>7000</v>
       </c>
       <c r="AR20">
         <v>2000000000</v>
@@ -2218,7 +2314,7 @@
     </row>
     <row r="21" spans="1:57">
       <c r="A21">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
         <v>172</v>
@@ -2236,116 +2332,110 @@
         <v>175</v>
       </c>
       <c r="G21">
-        <v>2500</v>
-      </c>
-      <c r="H21" t="s">
-        <v>155</v>
-      </c>
-      <c r="I21">
-        <v>50</v>
-      </c>
-      <c r="L21">
-        <v>13</v>
-      </c>
-      <c r="M21">
-        <v>50</v>
-      </c>
-      <c r="P21" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q21">
-        <v>5</v>
-      </c>
-      <c r="Z21">
-        <v>100</v>
-      </c>
-      <c r="AA21">
-        <v>2</v>
-      </c>
-      <c r="AC21">
-        <v>20000</v>
-      </c>
-      <c r="AD21" t="s">
-        <v>141</v>
-      </c>
-      <c r="AE21">
-        <v>5</v>
-      </c>
-      <c r="AP21">
-        <v>20000</v>
-      </c>
-      <c r="AQ21">
         <v>2000</v>
       </c>
+      <c r="S21" t="s">
+        <v>176</v>
+      </c>
       <c r="AR21">
-        <v>5000000000</v>
+        <v>2000000000</v>
       </c>
       <c r="AS21">
-        <v>1500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="22" spans="1:57">
       <c r="A22">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C22" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D22" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E22" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F22" t="s">
         <v>180</v>
       </c>
+      <c r="G22">
+        <v>2500</v>
+      </c>
+      <c r="H22" t="s">
+        <v>160</v>
+      </c>
+      <c r="I22">
+        <v>50</v>
+      </c>
+      <c r="L22">
+        <v>13</v>
+      </c>
+      <c r="M22">
+        <v>50</v>
+      </c>
+      <c r="P22" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q22">
+        <v>5</v>
+      </c>
+      <c r="Z22">
+        <v>100</v>
+      </c>
+      <c r="AA22">
+        <v>2</v>
+      </c>
+      <c r="AC22">
+        <v>20000</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>146</v>
+      </c>
+      <c r="AE22">
+        <v>5</v>
+      </c>
+      <c r="AP22">
+        <v>20000</v>
+      </c>
+      <c r="AQ22">
+        <v>2000</v>
+      </c>
       <c r="AR22">
-        <v>100000</v>
+        <v>5000000000</v>
       </c>
       <c r="AS22">
-        <v>50</v>
-      </c>
-      <c r="AV22">
-        <v>25</v>
-      </c>
-      <c r="AX22">
-        <v>4</v>
-      </c>
-      <c r="AZ22" t="s">
-        <v>181</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="23" spans="1:57">
       <c r="A23">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
+        <v>181</v>
+      </c>
+      <c r="C23" t="s">
         <v>182</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>183</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>184</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>185</v>
-      </c>
-      <c r="F23" t="s">
-        <v>186</v>
       </c>
       <c r="AR23">
         <v>100000</v>
       </c>
       <c r="AS23">
-        <v>75</v>
-      </c>
-      <c r="AT23" t="s">
-        <v>176</v>
+        <v>50</v>
       </c>
       <c r="AV23">
         <v>25</v>
@@ -2353,13 +2443,13 @@
       <c r="AX23">
         <v>4</v>
       </c>
-      <c r="BA23">
-        <v>1000</v>
+      <c r="AZ23" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:57">
       <c r="A24">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
         <v>187</v>
@@ -2374,25 +2464,16 @@
         <v>190</v>
       </c>
       <c r="F24" t="s">
-        <v>190</v>
-      </c>
-      <c r="S24" t="s">
         <v>191</v>
-      </c>
-      <c r="AP24">
-        <v>5000</v>
-      </c>
-      <c r="AQ24">
-        <v>5000</v>
       </c>
       <c r="AR24">
         <v>100000</v>
       </c>
       <c r="AS24">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="AT24" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="AV24">
         <v>25</v>
@@ -2400,10 +2481,13 @@
       <c r="AX24">
         <v>4</v>
       </c>
+      <c r="BA24">
+        <v>1000</v>
+      </c>
     </row>
     <row r="25" spans="1:57">
       <c r="A25">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
         <v>192</v>
@@ -2424,19 +2508,19 @@
         <v>196</v>
       </c>
       <c r="AP25">
-        <v>1000</v>
+        <v>5000</v>
       </c>
       <c r="AQ25">
-        <v>1000</v>
+        <v>5000</v>
       </c>
       <c r="AR25">
-        <v>500000</v>
+        <v>100000</v>
       </c>
       <c r="AS25">
         <v>100</v>
       </c>
       <c r="AT25" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="AV25">
         <v>25</v>
@@ -2447,7 +2531,7 @@
     </row>
     <row r="26" spans="1:57">
       <c r="A26">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
         <v>197</v>
@@ -2468,10 +2552,10 @@
         <v>201</v>
       </c>
       <c r="AP26">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="AQ26">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="AR26">
         <v>500000</v>
@@ -2480,7 +2564,7 @@
         <v>100</v>
       </c>
       <c r="AT26" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="AV26">
         <v>25</v>
@@ -2491,7 +2575,7 @@
     </row>
     <row r="27" spans="1:57">
       <c r="A27">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
         <v>202</v>
@@ -2506,40 +2590,25 @@
         <v>205</v>
       </c>
       <c r="F27" t="s">
+        <v>205</v>
+      </c>
+      <c r="S27" t="s">
         <v>206</v>
       </c>
-      <c r="S27" t="s">
-        <v>207</v>
-      </c>
-      <c r="AA27">
-        <v>1</v>
-      </c>
-      <c r="AB27">
-        <v>30</v>
-      </c>
-      <c r="AC27">
-        <v>500</v>
-      </c>
-      <c r="AF27" t="s">
-        <v>130</v>
-      </c>
-      <c r="AG27">
-        <v>1</v>
-      </c>
       <c r="AP27">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="AQ27">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="AR27">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="AS27">
         <v>100</v>
       </c>
       <c r="AT27" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="AV27">
         <v>25</v>
@@ -2550,72 +2619,90 @@
     </row>
     <row r="28" spans="1:57">
       <c r="A28">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
+        <v>207</v>
+      </c>
+      <c r="C28" t="s">
         <v>208</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>209</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>210</v>
-      </c>
-      <c r="E28" t="s">
-        <v>211</v>
       </c>
       <c r="F28" t="s">
         <v>211</v>
       </c>
-      <c r="R28" t="s">
+      <c r="S28" t="s">
         <v>212</v>
       </c>
-      <c r="S28" t="s">
-        <v>213</v>
-      </c>
-      <c r="T28" t="s">
-        <v>214</v>
+      <c r="AA28">
+        <v>1</v>
+      </c>
+      <c r="AB28">
+        <v>30</v>
+      </c>
+      <c r="AC28">
+        <v>500</v>
+      </c>
+      <c r="AF28" t="s">
+        <v>135</v>
+      </c>
+      <c r="AG28">
+        <v>1</v>
       </c>
       <c r="AP28">
-        <v>25000</v>
+        <v>1000</v>
       </c>
       <c r="AQ28">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="AR28">
-        <v>8000000000</v>
+        <v>1000000</v>
       </c>
       <c r="AS28">
-        <v>2000</v>
-      </c>
-      <c r="AZ28" t="s">
-        <v>212</v>
+        <v>100</v>
+      </c>
+      <c r="AT28" t="s">
+        <v>181</v>
+      </c>
+      <c r="AV28">
+        <v>25</v>
+      </c>
+      <c r="AX28">
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:57">
       <c r="A29">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
+        <v>213</v>
+      </c>
+      <c r="C29" t="s">
+        <v>214</v>
+      </c>
+      <c r="D29" t="s">
         <v>215</v>
       </c>
-      <c r="C29" t="s">
+      <c r="E29" t="s">
         <v>216</v>
       </c>
-      <c r="D29" t="s">
+      <c r="F29" t="s">
+        <v>216</v>
+      </c>
+      <c r="R29" t="s">
         <v>217</v>
       </c>
-      <c r="E29" t="s">
+      <c r="S29" t="s">
         <v>218</v>
       </c>
-      <c r="F29" t="s">
+      <c r="T29" t="s">
         <v>219</v>
-      </c>
-      <c r="P29" t="s">
-        <v>212</v>
-      </c>
-      <c r="Q29">
-        <v>2</v>
       </c>
       <c r="AP29">
         <v>25000</v>
@@ -2629,34 +2716,34 @@
       <c r="AS29">
         <v>2000</v>
       </c>
-      <c r="BD29" t="s">
-        <v>220</v>
+      <c r="AZ29" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:57">
       <c r="A30">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" t="s">
+        <v>220</v>
+      </c>
+      <c r="C30" t="s">
         <v>221</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>222</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>223</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>224</v>
       </c>
-      <c r="F30" t="s">
-        <v>225</v>
-      </c>
       <c r="P30" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="Q30">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AP30">
         <v>25000</v>
@@ -2670,10 +2757,13 @@
       <c r="AS30">
         <v>2000</v>
       </c>
+      <c r="BD30" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="31" spans="1:57">
       <c r="A31">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
         <v>226</v>
@@ -2688,13 +2778,13 @@
         <v>229</v>
       </c>
       <c r="F31" t="s">
-        <v>229</v>
-      </c>
-      <c r="R31" t="s">
         <v>230</v>
       </c>
-      <c r="S31" t="s">
-        <v>231</v>
+      <c r="P31" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q31">
+        <v>5</v>
       </c>
       <c r="AP31">
         <v>25000</v>
@@ -2708,34 +2798,31 @@
       <c r="AS31">
         <v>2000</v>
       </c>
-      <c r="AZ31" t="s">
-        <v>230</v>
-      </c>
     </row>
     <row r="32" spans="1:57">
       <c r="A32">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" t="s">
+        <v>231</v>
+      </c>
+      <c r="C32" t="s">
         <v>232</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>233</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>234</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
+        <v>234</v>
+      </c>
+      <c r="R32" t="s">
         <v>235</v>
       </c>
-      <c r="F32" t="s">
-        <v>235</v>
-      </c>
-      <c r="H32" t="s">
-        <v>155</v>
-      </c>
-      <c r="I32">
-        <v>200</v>
+      <c r="S32" t="s">
+        <v>236</v>
       </c>
       <c r="AP32">
         <v>25000</v>
@@ -2749,67 +2836,73 @@
       <c r="AS32">
         <v>2000</v>
       </c>
+      <c r="AZ32" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="33" spans="1:57">
       <c r="A33">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C33" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D33" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E33" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F33" t="s">
         <v>240</v>
       </c>
-      <c r="S33" t="s">
-        <v>241</v>
-      </c>
-      <c r="Y33">
-        <v>5000</v>
+      <c r="H33" t="s">
+        <v>160</v>
+      </c>
+      <c r="I33">
+        <v>200</v>
       </c>
       <c r="AP33">
-        <v>50000</v>
+        <v>25000</v>
       </c>
       <c r="AQ33">
-        <v>6000</v>
+        <v>3000</v>
       </c>
       <c r="AR33">
-        <v>12000000000</v>
+        <v>8000000000</v>
       </c>
       <c r="AS33">
-        <v>5000</v>
-      </c>
-      <c r="BB33">
-        <v>40</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="34" spans="1:57">
       <c r="A34">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B34" t="s">
+        <v>241</v>
+      </c>
+      <c r="C34" t="s">
         <v>242</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>243</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>244</v>
-      </c>
-      <c r="E34" t="s">
-        <v>245</v>
       </c>
       <c r="F34" t="s">
         <v>245</v>
       </c>
+      <c r="S34" t="s">
+        <v>246</v>
+      </c>
+      <c r="Y34">
+        <v>5000</v>
+      </c>
       <c r="AP34">
         <v>50000</v>
       </c>
@@ -2822,13 +2915,13 @@
       <c r="AS34">
         <v>5000</v>
       </c>
-      <c r="BD34" t="s">
-        <v>246</v>
+      <c r="BB34">
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:57">
       <c r="A35">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B35" t="s">
         <v>247</v>
@@ -2843,69 +2936,345 @@
         <v>250</v>
       </c>
       <c r="F35" t="s">
+        <v>250</v>
+      </c>
+      <c r="AP35">
+        <v>50000</v>
+      </c>
+      <c r="AQ35">
+        <v>6000</v>
+      </c>
+      <c r="AR35">
+        <v>12000000000</v>
+      </c>
+      <c r="AS35">
+        <v>5000</v>
+      </c>
+      <c r="BD35" t="s">
         <v>251</v>
-      </c>
-      <c r="H35" t="s">
-        <v>252</v>
-      </c>
-      <c r="I35">
-        <v>25</v>
-      </c>
-      <c r="AP35">
-        <v>100000</v>
-      </c>
-      <c r="AQ35">
-        <v>12000</v>
-      </c>
-      <c r="AR35">
-        <v>16000000000</v>
-      </c>
-      <c r="AS35">
-        <v>8000</v>
       </c>
     </row>
     <row r="36" spans="1:57">
       <c r="A36">
+        <v>40</v>
+      </c>
+      <c r="B36" t="s">
+        <v>252</v>
+      </c>
+      <c r="C36" t="s">
+        <v>253</v>
+      </c>
+      <c r="D36" t="s">
+        <v>254</v>
+      </c>
+      <c r="E36" t="s">
+        <v>255</v>
+      </c>
+      <c r="F36" t="s">
+        <v>256</v>
+      </c>
+      <c r="H36" t="s">
+        <v>257</v>
+      </c>
+      <c r="I36">
+        <v>25</v>
+      </c>
+      <c r="AP36">
+        <v>100000</v>
+      </c>
+      <c r="AQ36">
+        <v>12000</v>
+      </c>
+      <c r="AR36">
+        <v>16000000000</v>
+      </c>
+      <c r="AS36">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:57">
+      <c r="A37">
         <v>41</v>
       </c>
-      <c r="B36" t="s">
-        <v>253</v>
-      </c>
-      <c r="C36" t="s">
-        <v>254</v>
-      </c>
-      <c r="D36" t="s">
-        <v>255</v>
-      </c>
-      <c r="E36" t="s">
-        <v>256</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="B37" t="s">
+        <v>258</v>
+      </c>
+      <c r="C37" t="s">
+        <v>259</v>
+      </c>
+      <c r="D37" t="s">
+        <v>260</v>
+      </c>
+      <c r="E37" t="s">
+        <v>261</v>
+      </c>
+      <c r="F37" t="s">
+        <v>262</v>
+      </c>
+      <c r="P37" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q37">
+        <v>5</v>
+      </c>
+      <c r="AP37">
+        <v>500</v>
+      </c>
+      <c r="AQ37">
+        <v>250</v>
+      </c>
+      <c r="AR37">
+        <v>100000</v>
+      </c>
+      <c r="AS37">
+        <v>100</v>
+      </c>
+      <c r="AV37">
+        <v>100</v>
+      </c>
+      <c r="BE37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:57">
+      <c r="A38">
+        <v>42</v>
+      </c>
+      <c r="B38" t="s">
+        <v>263</v>
+      </c>
+      <c r="C38" t="s">
+        <v>264</v>
+      </c>
+      <c r="D38" t="s">
+        <v>265</v>
+      </c>
+      <c r="E38" t="s">
+        <v>266</v>
+      </c>
+      <c r="F38" t="s">
+        <v>266</v>
+      </c>
+      <c r="H38" t="s">
         <v>257</v>
       </c>
-      <c r="P36" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q36">
+      <c r="I38">
+        <v>75</v>
+      </c>
+      <c r="S38" t="s">
+        <v>267</v>
+      </c>
+      <c r="AP38">
+        <v>150000</v>
+      </c>
+      <c r="AQ38">
+        <v>30000</v>
+      </c>
+      <c r="AR38">
+        <v>32000000000</v>
+      </c>
+      <c r="AS38">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:57">
+      <c r="A39">
+        <v>43</v>
+      </c>
+      <c r="B39" t="s">
+        <v>268</v>
+      </c>
+      <c r="C39" t="s">
+        <v>269</v>
+      </c>
+      <c r="D39" t="s">
+        <v>270</v>
+      </c>
+      <c r="E39" t="s">
+        <v>271</v>
+      </c>
+      <c r="F39" t="s">
+        <v>272</v>
+      </c>
+      <c r="H39" t="s">
+        <v>257</v>
+      </c>
+      <c r="I39">
+        <v>150</v>
+      </c>
+      <c r="N39">
+        <v>3</v>
+      </c>
+      <c r="O39">
+        <v>100</v>
+      </c>
+      <c r="Z39">
+        <v>10000</v>
+      </c>
+      <c r="AA39">
+        <v>10</v>
+      </c>
+      <c r="AC39">
+        <v>50000</v>
+      </c>
+      <c r="AD39" t="s">
+        <v>273</v>
+      </c>
+      <c r="AE39">
+        <v>31</v>
+      </c>
+      <c r="AF39" t="s">
+        <v>274</v>
+      </c>
+      <c r="AG39">
+        <v>4</v>
+      </c>
+      <c r="AP39">
+        <v>150000</v>
+      </c>
+      <c r="AQ39">
+        <v>30000</v>
+      </c>
+      <c r="AR39">
+        <v>32000000000</v>
+      </c>
+      <c r="AS39">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:57">
+      <c r="A40">
+        <v>44</v>
+      </c>
+      <c r="B40" t="s">
+        <v>275</v>
+      </c>
+      <c r="C40" t="s">
+        <v>276</v>
+      </c>
+      <c r="D40" t="s">
+        <v>277</v>
+      </c>
+      <c r="E40" t="s">
+        <v>278</v>
+      </c>
+      <c r="F40" t="s">
+        <v>278</v>
+      </c>
+      <c r="H40" t="s">
+        <v>257</v>
+      </c>
+      <c r="I40">
+        <v>300</v>
+      </c>
+      <c r="AH40">
+        <v>1000000</v>
+      </c>
+      <c r="AP40">
+        <v>150000</v>
+      </c>
+      <c r="AQ40">
+        <v>30000</v>
+      </c>
+      <c r="AR40">
+        <v>32000000000</v>
+      </c>
+      <c r="AS40">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:57">
+      <c r="A41">
+        <v>45</v>
+      </c>
+      <c r="B41" t="s">
+        <v>279</v>
+      </c>
+      <c r="C41" t="s">
+        <v>280</v>
+      </c>
+      <c r="D41" t="s">
+        <v>281</v>
+      </c>
+      <c r="E41" t="s">
+        <v>282</v>
+      </c>
+      <c r="F41" t="s">
+        <v>282</v>
+      </c>
+      <c r="H41" t="s">
+        <v>257</v>
+      </c>
+      <c r="I41">
+        <v>400</v>
+      </c>
+      <c r="R41" t="s">
+        <v>283</v>
+      </c>
+      <c r="S41" t="s">
+        <v>284</v>
+      </c>
+      <c r="T41" t="s">
+        <v>285</v>
+      </c>
+      <c r="AH41">
+        <v>2000000</v>
+      </c>
+      <c r="AP41">
+        <v>150000</v>
+      </c>
+      <c r="AQ41">
+        <v>30000</v>
+      </c>
+      <c r="AR41">
+        <v>32000000000</v>
+      </c>
+      <c r="AS41">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:57">
+      <c r="A42">
+        <v>46</v>
+      </c>
+      <c r="B42" t="s">
+        <v>286</v>
+      </c>
+      <c r="C42" t="s">
+        <v>287</v>
+      </c>
+      <c r="D42" t="s">
+        <v>288</v>
+      </c>
+      <c r="E42" t="s">
+        <v>289</v>
+      </c>
+      <c r="F42" t="s">
+        <v>289</v>
+      </c>
+      <c r="P42" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q42">
         <v>5</v>
       </c>
-      <c r="AP36">
-        <v>500</v>
-      </c>
-      <c r="AQ36">
-        <v>250</v>
-      </c>
-      <c r="AR36">
-        <v>100000</v>
-      </c>
-      <c r="AS36">
-        <v>100</v>
-      </c>
-      <c r="AV36">
-        <v>100</v>
-      </c>
-      <c r="BE36">
-        <v>2</v>
+      <c r="AH42">
+        <v>2500000</v>
+      </c>
+      <c r="AP42">
+        <v>150000</v>
+      </c>
+      <c r="AQ42">
+        <v>30000</v>
+      </c>
+      <c r="AR42">
+        <v>32000000000</v>
+      </c>
+      <c r="AS42">
+        <v>8000</v>
+      </c>
+      <c r="AZ42" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished the event survey
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -200,13 +200,13 @@
     <t>You managed to slaughter the creatures and make your way forward to a small ramshackle town. The buildings are falling apart; the houses seem empty and lifeless. However, there is a small INN before you, and the roof looks like it could cave in at any moment. The lawn before it is overgrown with weeds and patches of dead grass where people and their pets have relieved themselves.&lt;br /&gt; &lt;br /&gt; You enter the INN and sit at an empty table by the fire. The barmaid, a heavy-set woman with an apron around her waist, walks over and asks what she can get you. You tell her you are looking for a man who calls himself The Guide. She states &lt;br /&gt; she has never heard of such a person and tells you she will be back with the drink and food.&lt;br /&gt; &lt;br /&gt; You sit alone, wondering what to do now.</t>
   </si>
   <si>
-    <t>&lt;p&gt;"I want you to learn about &lt;a href="/information/exploration" target="_blank"&gt;exploration&lt;/a&gt; – which allows you to automate the battle process of fighting but also has some drawbacks.&lt;/p&gt;&lt;p&gt;Exploration allows you to log out of the game and still fight monsters, gain items, gain currencies and – most importantly – gain levels.&lt;/p&gt;&lt;p&gt;Exploration can be amazing while you &lt;a href="/information/crafting" target="_blank"&gt;craft&lt;/a&gt;, or if you have to step out – or go to work. However, there is a drawback: Exploration will not allow you to change your equipment, set sail from one port to another, teleport (You can still move) and a few other actions.&lt;/p&gt;&lt;p&gt;The downside to exploration is that some areas won't drop quest items, some places that give out bonus currencies and items geared towards mid and end-game won't give out those bonus currencies and items.&lt;/p&gt;&lt;p&gt;Lastly, the sole part of this quest is that you cannot earn &lt;a href="/information/factions" target="_blank"&gt;Faction&lt;/a&gt; Points.&lt;/p&gt;&lt;p&gt;Faction Points allow you to gain &lt;a href="/information/random-enchants" target="_blank"&gt;unique items&lt;/a&gt; – which at first are weaker than ones you can earn later on – but are great to get you going.&lt;/p&gt;&lt;p&gt;Faction points can be seen on your character sheet. Once a player reaches level 5 in a given faction, they can then pledge to it. We will discuss that later. Right now, to earn faction points – all you have to do is kill anything you want on the plane the faction is named after.&lt;/p&gt;&lt;p&gt;For this quest, we will kill any creature we can on Surface to earn points to level the Faction to the required level. You will earn 50 points per kill from level 0 to 1 and then 75 points from level 1 to 5 per kill.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;First, let's investigate the gear we have been given.&lt;/p&gt;&lt;p&gt;We can do this by going to the character sheet tab, and on the bottom right is the inventory management. You can click item names here to investigate, equip, and do other types of actions with the item. For now, if you find gear that raises your stats (i.e., STR Modifier +x%), equip it.&lt;/p&gt;&lt;p&gt;You may also need to visit the shop, which you can do by clicking the top left Hamburger menu to open the menu and select Shop. From here, select Buy under General Shop. Here you can buy gear, buy multiple pieces of gear, or even compare and equip gear (auto purchase/equip).&lt;/p&gt;&lt;p&gt;&lt;strong&gt;How to explore&lt;/strong&gt;:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Next, go back to the drop-down for monsters and select a stronger monster and click Attack if you can kill it in one hit, which is ideal. Move down the list to the next, rinse and repeat till you cannot move any further.&lt;/li&gt;&lt;li&gt;Now that we have a monster, click Explore to the left of the attack section.&lt;/li&gt;&lt;li&gt;Select the same monster, select 1 hour, ignore the move down, and then select Attack. Click Explore.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;You will see your Exploration chat tab update – within 5 minutes both your exploration and server messages tab will update, one with info about your exploration including bonus faction points and how many creatures you kill, while the other – server messages – will show you the items you got, the currencies, and so on.&lt;/p&gt;&lt;p&gt;What's amazing about this is you can now sign out and be on your way and come back later to all your items, but why do that when we can earn some Factions and save exploration for when we're ready to "just train."&lt;/p&gt;&lt;p&gt;&lt;strong&gt;To earn Faction Points first&lt;/strong&gt;:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Select a monster you can ideally kill in one hit and slaughter it. Do this about ~20 times.&lt;/li&gt;&lt;li&gt;Now to see that we gained some points, head over to your character sheet and click the Factions tab in the card which is in the top left section of the sheet.&lt;/li&gt;&lt;li&gt;Surface should be level 2 at this point. If you check your inventory, you should have a green item. Investigate this – possibly equip it.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;First, let's investigate the gear we have been given.&lt;/p&gt;&lt;p&gt;We can do this by going to the character sheet, and from the drop-down select Inventory Management. Now we can see all our gear we found - which might not be much, but we can filter through and look for Stat Raising gear, i.e., STR Modifier +X%.&lt;/p&gt;&lt;p&gt;You may also need to visit the shop, which you can do by clicking the top left Hamburger menu to open the menu and select Shop. From here select Buy under General Shop. Here you can buy gear, buy multiple pieces of gear or even compare &lt;/p&gt;&lt;p&gt;and equip gear (auto purchase/equip).&lt;/p&gt;&lt;p&gt;&lt;strong&gt;How to explore&lt;/strong&gt;:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;In the actions drop-down, select Fight and select a monster you can kill in one hit, which is ideal, move down the list to the next, rinse and repeat till you cannot move any further.&lt;/li&gt;&lt;li&gt;Now that we have a monster, select Exploration from the action drop-down.&lt;/li&gt;&lt;li&gt;Select the monster you could kill, select 1 hour for time – do not select anything for moving down the monster list every x levels and click explore.&lt;/li&gt;&lt;li&gt;Tap Attack to begin. In five minutes, the exploration chat tab and server message tab will update.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;You will see your Exploration chat tab update – within 5 minutes both your exploration and server messages tab will update, one with info about your exploration including bonus faction points and how many creatures you kill, while the other – server messages – will show you the items you got, the currencies, and so on.&lt;/p&gt;&lt;p&gt;To access this info, select exploration or server messages from the chat tab drop down under the actions section.&lt;/p&gt;&lt;p&gt;What's amazing about this is you can now sign out and be on your way and come back later to all your items, but why do that when we can earn some Factions and save exploration for when we're ready to "just train."&lt;/p&gt;&lt;p&gt;&lt;strong&gt;To earn Faction Points first&lt;/strong&gt;:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;While exploration is not running, select attack from the actions drop-down.&lt;/li&gt;&lt;li&gt;Select a monster you can ideally kill in one hit and slaughter it. Do this about ~20 times.&lt;/li&gt;&lt;li&gt;Now to see that we gained some points, head over to your character sheet and expand the top section, next tap the Factions tab.&lt;/li&gt;&lt;li&gt;Surface should be level 2 at this point. If you check your inventory, you should have a green item. Investigate this – possibly equip it.&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;p&gt;I want you to learn about &lt;a href="/information/exploration" target="_blank"&gt;exploration&lt;/a&gt; – which allows you to automate the battle process of fighting but also has some drawbacks.&lt;/p&gt;&lt;p&gt;Exploration allows you to log out of the game and still fight monsters, gain items, gain currencies and – most importantly – gain levels.&lt;/p&gt;&lt;p&gt;Exploration can be amazing while you &lt;a href="/information/crafting" target="_blank"&gt;craft&lt;/a&gt;, or if you have to step out – or go to work. However, there is a drawback: Exploration will not allow you to change your equipment, set sail from one port to another, teleport (You can still move) and a few other actions.&lt;/p&gt;&lt;p&gt;The downside to exploration is that some areas won't drop quest items, some places that give out bonus currencies and items geared towards mid and end-game won't give out those bonus currencies and items.&lt;/p&gt;&lt;p&gt;Lastly, the sole part of this quest is that you cannot earn &lt;a href="/information/factions" target="_blank"&gt;Faction&lt;/a&gt; Points with out &lt;strong&gt;manually fighting&lt;/strong&gt;. Exploration will not gain you faction points.&lt;/p&gt;&lt;p&gt;Faction Points allow you to gain &lt;a href="/information/random-enchants" target="_blank"&gt;unique items&lt;/a&gt; – which at first are weaker than ones you can earn later on – but are great to get you going.&lt;/p&gt;&lt;p&gt;When you max out a faction, you can then participate in &lt;a href="/information/faction-loyalty" target="_blank"&gt;Faction Loyalty&lt;/a&gt; - where you help NPC's with their tasks by Pledging to that faction. We will learn more about this later on, but these will be required for mid to end game quests.&lt;/p&gt;&lt;p&gt;Faction points can be seen on your character sheet. Once a player reaches level 5 in a given faction, they can then pledge to it. We will discuss that later. Right now, to earn faction points – all you have to do is kill &lt;/p&gt;&lt;p&gt;anything you want on the plane the faction is named after.&lt;/p&gt;&lt;p&gt;For this quest, we will kill any creature we can on Surface to earn points to level the Faction to the required level. You will earn 50 points per kill from level 0 to 1 and then 75 points from level 1 to 5 per kill.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;First, let's investigate the gear we have been given.&lt;/p&gt;&lt;p&gt;We can do this by going to the character sheet tab, and on the bottom right is the inventory management. You can click item names here to investigate, equip, and do other types of actions with the item. For now, if you find gear that raises your stats (i.e., STR Modifier +x%), equip it.&lt;/p&gt;&lt;p&gt;You may also need to visit the shop, which you can do by clicking the top left Hamburger menu to open the menu and select Shop. From here, select Buy under General Shop. Here you can buy gear, buy multiple pieces of gear, or even compare and equip gear (auto purchase/equip).&lt;/p&gt;&lt;p&gt;&lt;strong&gt;How to explore&lt;/strong&gt;:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Next, go back to the drop-down for monsters and select a stronger monster and click Attack if you can kill it in one hit, which is ideal. Move down the list to the next, rinse and repeat till you cannot move any further.&lt;/li&gt;&lt;li&gt;Now that we have a monster, click Explore to the left of the attack section.&lt;/li&gt;&lt;li&gt;Select the same monster, select 1 hour, ignore the move down, and then select Attack. Click Explore.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;You will see your Exploration chat tab update – within 5 minutes both your exploration and server messages tab will update, one with info about your exploration including bonus faction points and how many creatures you kill, while the other – server messages – will show you the items you got, the currencies, and so on.&lt;/p&gt;&lt;p&gt;What's amazing about this is you can now sign out and be on your way and come back later to all your items, but why do that when we can earn some Factions and save exploration for when we're ready to "just train."&lt;/p&gt;&lt;p&gt;&lt;strong&gt;To earn Faction Points first&lt;/strong&gt;:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Select a monster you can ideally kill in one hit and slaughter it. Do this about ~20 times.&lt;/li&gt;&lt;li&gt;Now to see that we gained some points, head over to your character sheet and click the Factions tab in the card which is in the top left section of the sheet.&lt;/li&gt;&lt;li&gt;Surface should be level 1 at this point. If you check your inventory, you should have a green item. Investigate this – possibly equip it.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;First, let's investigate the gear we have been given.&lt;/p&gt;&lt;p&gt;We can do this by going to the character sheet, and from the drop-down select Inventory Management. Now we can see all our gear we found - which might not be much, but we can filter through and look for Stat Raising gear, i.e., STR Modifier +X%.&lt;/p&gt;&lt;p&gt;You may also need to visit the shop, which you can do by clicking the top left Hamburger menu to open the menu and select Shop. From here select Buy under General Shop. Here you can buy gear, buy multiple pieces of gear or even compare&lt;/p&gt;&lt;p&gt;and equip gear (auto purchase/equip).&lt;/p&gt;&lt;p&gt;&lt;strong&gt;How to explore&lt;/strong&gt;:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;In the actions drop-down, select Fight and select a monster you can kill in one hit, which is ideal, move down the list to the next, rinse and repeat till you cannot move any further.&lt;/li&gt;&lt;li&gt;Now that we have a monster, select Exploration from the action drop-down.&lt;/li&gt;&lt;li&gt;Select the monster you could kill, select 1 hour for time – do not select anything for moving down the monster list every x levels and click explore.&lt;/li&gt;&lt;li&gt;Tap Attack to begin. In five minutes, the exploration chat tab and server message tab will update.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;You will see your Exploration chat tab update – within 5 minutes both your exploration and server messages tab will update, one with info about your exploration including bonus faction points and how many creatures you kill, while the other – server messages – will show you the items you got, the currencies, and so on.&lt;/p&gt;&lt;p&gt;To access this info, select exploration or server messages from the chat tab drop down under the actions section.&lt;/p&gt;&lt;p&gt;What's amazing about this is you can now sign out and be on your way and come back later to all your items, but why do that when we can earn some Factions and save exploration for when we're ready to "just train."&lt;/p&gt;&lt;p&gt;&lt;strong&gt;To earn Faction Points first&lt;/strong&gt;:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;While exploration is not running, select attack from the actions drop-down.&lt;/li&gt;&lt;li&gt;Select a monster you can ideally kill in one hit and slaughter it. Do this about ~20 times.&lt;/li&gt;&lt;li&gt;Now to see that we gained some points, head over to your character sheet and expand the top section, next tap the Factions tab.&lt;/li&gt;&lt;li&gt;Surface should be level 1 at this point. If you check your inventory, you should have a green item. Investigate this – possibly equip it.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>Surface</t>
@@ -866,27 +866,27 @@
     <t>&lt;p&gt;We know how to craft trinkets, make use of alchemy items, and our class ranks, specialties, and class skills.&lt;/p&gt;&lt;p&gt;It’s time we wrap it all together and continue the main storyline headed for a new plane of existence!&lt;/p&gt;</t>
   </si>
   <si>
+    <t>Twisted Branches</t>
+  </si>
+  <si>
+    <t>Twisted Tree Branch</t>
+  </si>
+  <si>
+    <t>Twsited Memories</t>
+  </si>
+  <si>
+    <t>You made it. You stand before the gate in Hell, a gate to a world where the memories of those are twisted. You have learned more about The Shattering; you have tried to track down this mysterious Wandering Prince, some say he is the Prince of Emeralds himself, a man from another plane of existence where he shut away his world when The Shattering happened.&lt;br /&gt; &lt;br /&gt; You ponder for a moment if this is what The Creator wants: to shatter the realities, to fling forth the gates of despair and unleash the torment of suffering onto others. Has he not done enough damage to the people around him, the lovers of this world – the parents of another?&lt;br /&gt; &lt;br /&gt; The selfishness and the greediness. You shake your head for a moment, but can hear a whispering of another time and place that haunts you. You step through the gate.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We made it to the new world! To the new plane of existence. To Twisted Memories!&lt;/p&gt;&lt;p&gt;This is the second aspect of the endgame, a new map, with stronger creatures and steeper reductions. It is less about killing in one shot and more about utilizing alchemy items, your gear, and your class specialties to survive down here and slowly level your character through reincarnation.&lt;/p&gt;&lt;p&gt;There are new quests that continue the story of how you got here.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Continue using what you learned to raise your stats even higher. The trick is down here, though; you need to be on this plane to hand in the quest. So it might take some time and some reincarnations.&lt;/p&gt;</t>
+  </si>
+  <si>
     <t>Twisted Memories</t>
   </si>
   <si>
-    <t>Twisted Branches</t>
-  </si>
-  <si>
-    <t>Twisted Tree Branch</t>
-  </si>
-  <si>
-    <t>Twsited Memories</t>
-  </si>
-  <si>
-    <t>You made it. You stand before the gate in Hell, a gate to a world where the memories of those are twisted. You have learned more about The Shattering; you have tried to track down this mysterious Wandering Prince, some say he is the Prince of Emeralds himself, a man from another plane of existence where he shut away his world when The Shattering happened.&lt;br /&gt; &lt;br /&gt; You ponder for a moment if this is what The Creator wants: to shatter the realities, to fling forth the gates of despair and unleash the torment of suffering onto others. Has he not done enough damage to the people around him, the lovers of this world – the parents of another?&lt;br /&gt; &lt;br /&gt; The selfishness and the greediness. You shake your head for a moment, but can hear a whispering of another time and place that haunts you. You step through the gate.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;We made it to the new world! To the new plane of existence. To Twisted Memories!&lt;/p&gt;&lt;p&gt;This is the second aspect of the endgame, a new map, with stronger creatures and steeper reductions. It is less about killing in one shot and more about utilizing alchemy items, your gear, and your class specialties to survive down here and slowly level your character through reincarnation.&lt;/p&gt;&lt;p&gt;There are new quests that continue the story of how you got here.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Continue using what you learned to raise your stats even higher. The trick is down here, though; you need to be on this plane to hand in the quest. So it might take some time and some reincarnations.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>Delusional Memories Opens It's Gates</t>
   </si>
   <si>
@@ -920,7 +920,7 @@
     <t>&lt;p&gt;- Manually fight monsters to gain faction points, which can be seen on your Character Sheet tab, under Factions (expand the top section). There will be one for Delusional Memories.&lt;/p&gt;&lt;p&gt;- You will get 1 Unique item when you reach level.&lt;/p&gt;&lt;p&gt;If the battle phase of the global event is currently running – which can be seen by selecting Map Movement from the actions dropdown, and then tapping Event Goals.&lt;/p&gt;&lt;p&gt;- Fight monsters manually until you achieve these quest kill amounts.&lt;/p&gt;&lt;p&gt;This can and will be done automatically while the phase is running, combined with the faction requirements.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>Delusional Children and their quests</t>
+    <t>Delusional children and their quests</t>
   </si>
   <si>
     <t>This place is different than any place you might have ever traveled to. On one hand, to the north, across the ocean, lie The Federation-controlled lands, while south, across the ocean, the free people of the south rise against The Federation and fight for their freedom.&lt;br /&gt; &lt;br /&gt; Alongside The Federation is The Church who spreads their religious dogma and subjugation of people's free will across the land.&lt;br /&gt; &lt;br /&gt; There is a man, a man who lives in the depths of yesterday. He is known as The Jester, and he might know more about this land. Let's find him, shall we?</t>
@@ -938,7 +938,7 @@
     <t>Looking for the Jester</t>
   </si>
   <si>
-    <t>The Delusional Machinations of a mad world</t>
+    <t>The Delusional machinations of a mad world</t>
   </si>
   <si>
     <t>The delusions of the mad men that live down here and the words they spew from their own twisted mouths of corruption exhausts you.&lt;br /&gt; &lt;br /&gt; The journeys through this land are unlike those you are used to. You come from humble beginnings, and this whole time you have been thrown into someone else’s battle, someone else’s drama.&lt;br /&gt; &lt;br /&gt; There is something here—something worth investigating. Let's go hunting.</t>
@@ -1303,7 +1303,7 @@
     <col min="3" max="3" width="1890.967" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="2753.328" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="2512.672" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="2810.028" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="2808.743" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="18.71" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="24.708" bestFit="true" customWidth="true" style="0"/>
@@ -1576,7 +1576,7 @@
         <v>64</v>
       </c>
       <c r="Q3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AR3">
         <v>500</v>
@@ -3187,7 +3187,7 @@
         <v>273</v>
       </c>
       <c r="AE39">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AF39" t="s">
         <v>274</v>
@@ -3274,14 +3274,11 @@
       <c r="I41">
         <v>400</v>
       </c>
-      <c r="R41" t="s">
+      <c r="S41" t="s">
         <v>283</v>
       </c>
-      <c r="S41" t="s">
+      <c r="T41" t="s">
         <v>284</v>
-      </c>
-      <c r="T41" t="s">
-        <v>285</v>
       </c>
       <c r="AH41">
         <v>2000000</v>
@@ -3304,19 +3301,19 @@
         <v>46</v>
       </c>
       <c r="B42" t="s">
+        <v>285</v>
+      </c>
+      <c r="C42" t="s">
         <v>286</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>287</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>288</v>
       </c>
-      <c r="E42" t="s">
-        <v>289</v>
-      </c>
       <c r="F42" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AH42">
         <v>2500000</v>
@@ -3334,7 +3331,7 @@
         <v>8000</v>
       </c>
       <c r="AZ42" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
     </row>
     <row r="43" spans="1:57">
@@ -3397,6 +3394,12 @@
       <c r="F44" t="s">
         <v>300</v>
       </c>
+      <c r="P44" t="s">
+        <v>295</v>
+      </c>
+      <c r="Q44">
+        <v>1</v>
+      </c>
       <c r="AP44">
         <v>100</v>
       </c>
@@ -3482,6 +3485,12 @@
       <c r="F46" t="s">
         <v>310</v>
       </c>
+      <c r="P46" t="s">
+        <v>295</v>
+      </c>
+      <c r="Q46">
+        <v>5</v>
+      </c>
       <c r="S46" t="s">
         <v>101</v>
       </c>
@@ -3505,6 +3514,9 @@
       </c>
       <c r="AX46">
         <v>8</v>
+      </c>
+      <c r="AZ46" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed spelling of the new quest item
</commit_message>
<xml_diff>
--- a/resources/data-imports/Admin Section/guide_quests.xlsx
+++ b/resources/data-imports/Admin Section/guide_quests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="307">
   <si>
     <t>id</t>
   </si>
@@ -344,7 +344,7 @@
     <t>Your ability to kill creatures is getting better, and you're able to find and hunt down stronger foes.&lt;br /&gt; &lt;br /&gt; Exhausted and tired, you arrive back at the INN. It’s completely empty. Not a soul, not a single sound but the creaking of the old wood in the wind that blows outside.&lt;br /&gt; &lt;br /&gt; You call out, but no one answers.&lt;br /&gt; &lt;br /&gt; A shadow moves across the wall, and you move towards where the shadow went.&lt;br /&gt; &lt;br /&gt; No one there.&lt;br /&gt; &lt;br /&gt; You call out again, readying your weapon.&lt;br /&gt; &lt;br /&gt; Nothing.&lt;br /&gt; &lt;br /&gt; You enter into a back room, an office of sorts. Blood covers the wall. You back out and head back to the main room.&lt;br /&gt; &lt;br /&gt; Bodies. Bodies everywhere, torn, broken, damaged, and ripped apart. The gore, the fear, the pain, the eyes of the dead.&lt;br /&gt; &lt;br /&gt; What the hell happened?</t>
   </si>
   <si>
-    <t>&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;: This quest can take two-plus hours to complete. I recommend exploration while crafting and enchanting.&lt;/p&gt;&lt;p&gt;It’s time we get off the &lt;a href="/information/planes" target="_blank"&gt;plane&lt;/a&gt;: Surface. To do this, we just have to kill a single creature: Labyrinth Fiend until the Key of Labyrinth drops.&lt;/p&gt;&lt;p&gt;This will allow us to use a new feature called: &lt;a href="/information/traverse" target="_blank"&gt;Traverse&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;Traverse allows us to move to another plane of existence where we can fight monsters and interact with new features. For example, when we eventually get to Hell, those &lt;a href="/information/random-enchants" target="_blank"&gt;Green Uniques&lt;/a&gt; you have been getting – there is an NPC that allows you to &lt;/p&gt;&lt;p&gt;buy better ones and even re-roll them and move the enchantments to other items. How fun!&lt;/p&gt;&lt;p&gt;Some Planes make you weaker, and the creatures much, much stronger and also give you bonuses for killing creatures of that plane. As you go past Dungeons plane, you will find your gear needs to be better with a set of enchantments that play &lt;/p&gt;&lt;p&gt;to your class's strengths as well as the levels.&lt;/p&gt;</t>
+    <t>&lt;p&gt;&lt;strong&gt;Note&lt;/strong&gt;: This quest can take two-plus hours to complete. I recommend exploration while crafting and enchanting.&lt;/p&gt;&lt;p&gt;It’s time we get off the &lt;a href="/information/planes" target="_blank"&gt;plane&lt;/a&gt;: Surface. To do this, We just have to complete the quest: Labyrinth and the Mind which has you kill the Labyrinth fiend on Surface to recieve the Broken key of the mind. With this we can complete the quest which is on surface and can be done after you complete Hunting Expedition.&lt;/p&gt;&lt;p&gt;This will allow us to use a new feature called: &lt;a href="/information/traverse" target="_blank"&gt;Traverse&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;Traverse allows us to move to another plane of existence where we can fight monsters and interact with new features. For example, when we eventually get to Hell, those &lt;a href="/information/random-enchants" target="_blank"&gt;Green Uniques&lt;/a&gt; you have been getting – there is an NPC that allows you to&lt;/p&gt;&lt;p&gt;buy better ones and even re-roll them and move the enchantments to other items. How fun!&lt;/p&gt;&lt;p&gt;Some Planes make you weaker, and the creatures much, much stronger and also give you bonuses for killing creatures of that plane. As you go past Dungeons plane, you will find your gear needs to be better with a set of enchantments that play&lt;/p&gt;&lt;p&gt;to your class's strengths as well as the levels.&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Kill Labyrinth Fiend until the Key of Labyrinth drops.&lt;/p&gt;&lt;p&gt;Next:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Click Traverse under the map.&lt;/li&gt;&lt;li&gt;Select Labyrinth from the drop-down.&lt;/li&gt;&lt;li&gt;Click Traverse.&lt;/li&gt;&lt;li&gt;Welcome to Labyrinth!plane.&lt;/li&gt;&lt;/ul&gt;</t>
@@ -372,21 +372,6 @@
   </si>
   <si>
     <t>&lt;ul&gt;&lt;li&gt;Tap the Character Sheet tab.&lt;/li&gt;&lt;li&gt;Expand the Character Details Section.&lt;/li&gt;&lt;li&gt;Tap the Class Ranks orange button.&lt;/li&gt;&lt;li&gt;Look for your class in the list and tap the name.&lt;/li&gt;&lt;li&gt;This will open another window, to exit back to the class list tap the red circle with the minus in the top right. Tap cancel or the X will close the modal.&lt;/li&gt;&lt;li&gt;Here you will see information about the class and the Class Masteries.&lt;/li&gt;&lt;li&gt;Tap Manage Specialties.&lt;/li&gt;&lt;li&gt;Equip a specialty and boom done, now you just have to kill creatures.&lt;/li&gt;&lt;li&gt;The server messages will tell you when you gain levels in your Masteries and your Specialties as well as your Class Rank.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Now you just have to kill creatures till you meet the requirements.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Gamble the horror away</t>
-  </si>
-  <si>
-    <t>You managed to make your way to Smugglers Port, where you heard of a game that can be played and where one can attempt to win currencies!&lt;br /&gt; &lt;br /&gt; You asked around the port town, and people have told you what they know and pointed you to a pub where a man stands by a weird-looking box that magically seems to change and roll. People give money and watch this box split into three and roll, sometimes the images match, sometimes they don’t, and the patrons leave with no money or even less than they had.&lt;br /&gt; &lt;br /&gt; You decide to take a gamble and take a moment for yourself.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Let's &lt;a href="/information/slots" target="_blank"&gt;gamble&lt;/a&gt; and have some fun! First, we want to unlock a feature that will help us, not just when gambling but also when fighting creatures! We need currencies – Gold Dust and eventually Shards – which are also used in quests and a new type of crafting we will soon unlock: &lt;a href="/information/alchemy" target="_blank"&gt;Alchemy&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;This new feature is called: &lt;a href="/information/mercenary" target="_blank"&gt;Mercenaries&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;Mercenaries allow you to gain more currencies as you level them and then reincarnate them. They will give a bonus which is equal to their level and the amount of times (to a max of 1100%) towards currency acquisition for Shards, Gold Dust, and Copper Coins.&lt;/p&gt;&lt;p&gt;Mercenaries help out the most with &lt;a href="/information/slots" target="_blank"&gt;Slots&lt;/a&gt;.&lt;/p&gt;&lt;p&gt;Slots is a way for players to gamble and potentially win currencies. The caveat is one of the currencies cannot be rewarded at this time because you don’t have the right quest item, Copper Coins.&lt;/p&gt;&lt;p&gt;To level a Mercenary, you need to complete a quest to unlock the feature and then pay gold to purchase the type of mercenary you want.&lt;/p&gt;&lt;p&gt;After that, all you have to do is fight creatures, and over time the Mercenaries will level. As you reach level 100 on one of them, you can reincarnate them, re-level them up and gain 200% towards currency acquisition. Then just repeat this process 9 more times.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Complete the quest on Labyrinth: "The truth is out there."&lt;/li&gt;&lt;li&gt;Click the Character Sheet Tab.&lt;/li&gt;&lt;li&gt;Click the tab: Mercenaries.&lt;/li&gt;&lt;li&gt;Purchase the mercenaries required.&lt;/li&gt;&lt;li&gt;Level the Mercenary to the required leveling.&lt;/li&gt;&lt;li&gt;Play slots if you have the gold and kill creatures to level the mercenaries through exploration!&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Complete the quest on Labyrinth: "The truth is out there."&lt;/li&gt;&lt;li&gt;Tap the Character Sheet Tab.&lt;/li&gt;&lt;li&gt;Tap the tab: Mercenaries.&lt;/li&gt;&lt;li&gt;Purchase the mercenaries required.&lt;/li&gt;&lt;li&gt;Level the Mercenary to the required leveling.&lt;/li&gt;&lt;li&gt;Play slots (select slots from the actions drop-down) if you have the gold and kill creatures to level the mercenaries!&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>Farmers in the fields</t>
@@ -1290,7 +1275,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:BE46"/>
+  <dimension ref="A1:BE45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1945,7 +1930,7 @@
     </row>
     <row r="12" spans="1:57">
       <c r="A12">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
         <v>119</v>
@@ -1962,11 +1947,14 @@
       <c r="F12" t="s">
         <v>123</v>
       </c>
-      <c r="AP12">
-        <v>1000</v>
-      </c>
-      <c r="AQ12">
-        <v>1000</v>
+      <c r="AA12">
+        <v>1</v>
+      </c>
+      <c r="AB12">
+        <v>30</v>
+      </c>
+      <c r="AC12">
+        <v>100</v>
       </c>
       <c r="AR12">
         <v>1000000</v>
@@ -1977,7 +1965,7 @@
     </row>
     <row r="13" spans="1:57">
       <c r="A13">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
         <v>124</v>
@@ -1994,17 +1982,32 @@
       <c r="F13" t="s">
         <v>128</v>
       </c>
-      <c r="AA13">
+      <c r="H13" t="s">
+        <v>93</v>
+      </c>
+      <c r="I13">
+        <v>25</v>
+      </c>
+      <c r="J13" t="s">
+        <v>129</v>
+      </c>
+      <c r="K13">
+        <v>5</v>
+      </c>
+      <c r="AB13">
+        <v>60</v>
+      </c>
+      <c r="AC13">
+        <v>500</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG13">
         <v>1</v>
       </c>
-      <c r="AB13">
-        <v>30</v>
-      </c>
-      <c r="AC13">
-        <v>100</v>
-      </c>
       <c r="AR13">
-        <v>1000000</v>
+        <v>2000000</v>
       </c>
       <c r="AS13">
         <v>100</v>
@@ -2012,46 +2015,34 @@
     </row>
     <row r="14" spans="1:57">
       <c r="A14">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C14" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D14" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E14" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F14" t="s">
-        <v>133</v>
-      </c>
-      <c r="H14" t="s">
-        <v>93</v>
-      </c>
-      <c r="I14">
-        <v>25</v>
-      </c>
-      <c r="J14" t="s">
         <v>134</v>
       </c>
-      <c r="K14">
-        <v>5</v>
-      </c>
       <c r="AB14">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="AC14">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="AF14" t="s">
         <v>135</v>
       </c>
       <c r="AG14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AR14">
         <v>2000000</v>
@@ -2062,7 +2053,7 @@
     </row>
     <row r="15" spans="1:57">
       <c r="A15">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
         <v>136</v>
@@ -2079,20 +2070,41 @@
       <c r="F15" t="s">
         <v>139</v>
       </c>
+      <c r="H15" t="s">
+        <v>78</v>
+      </c>
+      <c r="I15">
+        <v>25</v>
+      </c>
+      <c r="J15" t="s">
+        <v>93</v>
+      </c>
+      <c r="K15">
+        <v>50</v>
+      </c>
+      <c r="N15">
+        <v>2</v>
+      </c>
+      <c r="O15">
+        <v>10</v>
+      </c>
+      <c r="S15" t="s">
+        <v>140</v>
+      </c>
       <c r="AB15">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="AC15">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="AF15" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AG15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AR15">
-        <v>2000000</v>
+        <v>5000000</v>
       </c>
       <c r="AS15">
         <v>100</v>
@@ -2100,58 +2112,70 @@
     </row>
     <row r="16" spans="1:57">
       <c r="A16">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C16" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D16" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E16" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F16" t="s">
-        <v>144</v>
+        <v>145</v>
+      </c>
+      <c r="G16">
+        <v>500</v>
       </c>
       <c r="H16" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="I16">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="J16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K16">
         <v>50</v>
       </c>
-      <c r="N16">
-        <v>2</v>
-      </c>
-      <c r="O16">
-        <v>10</v>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>100</v>
+      </c>
+      <c r="P16" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q16">
+        <v>3</v>
+      </c>
+      <c r="R16" t="s">
+        <v>146</v>
       </c>
       <c r="S16" t="s">
-        <v>145</v>
-      </c>
-      <c r="AB16">
-        <v>100</v>
-      </c>
-      <c r="AC16">
-        <v>3000</v>
-      </c>
-      <c r="AF16" t="s">
-        <v>146</v>
-      </c>
-      <c r="AG16">
-        <v>1</v>
+        <v>147</v>
+      </c>
+      <c r="T16" t="s">
+        <v>148</v>
+      </c>
+      <c r="U16" t="s">
+        <v>149</v>
+      </c>
+      <c r="W16">
+        <v>25000</v>
+      </c>
+      <c r="AQ16">
+        <v>1000</v>
       </c>
       <c r="AR16">
-        <v>5000000</v>
+        <v>50000000</v>
       </c>
       <c r="AS16">
         <v>100</v>
@@ -2159,70 +2183,46 @@
     </row>
     <row r="17" spans="1:57">
       <c r="A17">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C17" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D17" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E17" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="F17" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="G17">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="H17" t="s">
-        <v>93</v>
+        <v>155</v>
       </c>
       <c r="I17">
-        <v>100</v>
-      </c>
-      <c r="J17" t="s">
-        <v>94</v>
-      </c>
-      <c r="K17">
-        <v>50</v>
-      </c>
-      <c r="L17">
-        <v>1</v>
-      </c>
-      <c r="M17">
-        <v>100</v>
-      </c>
-      <c r="P17" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q17">
         <v>3</v>
       </c>
-      <c r="R17" t="s">
-        <v>151</v>
-      </c>
-      <c r="S17" t="s">
-        <v>152</v>
-      </c>
-      <c r="T17" t="s">
-        <v>153</v>
-      </c>
-      <c r="U17" t="s">
-        <v>154</v>
-      </c>
-      <c r="W17">
+      <c r="N17">
+        <v>3</v>
+      </c>
+      <c r="O17">
+        <v>10</v>
+      </c>
+      <c r="AP17">
         <v>25000</v>
       </c>
       <c r="AQ17">
         <v>1000</v>
       </c>
       <c r="AR17">
-        <v>50000000</v>
+        <v>75000000</v>
       </c>
       <c r="AS17">
         <v>100</v>
@@ -2230,54 +2230,66 @@
     </row>
     <row r="18" spans="1:57">
       <c r="A18">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C18" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D18" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E18" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F18" t="s">
         <v>159</v>
       </c>
       <c r="G18">
-        <v>600</v>
-      </c>
-      <c r="H18" t="s">
-        <v>160</v>
-      </c>
-      <c r="I18">
-        <v>3</v>
+        <v>1000</v>
+      </c>
+      <c r="J18" t="s">
+        <v>93</v>
+      </c>
+      <c r="K18">
+        <v>400</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>400</v>
       </c>
       <c r="N18">
         <v>3</v>
       </c>
       <c r="O18">
-        <v>10</v>
+        <v>30</v>
+      </c>
+      <c r="S18" t="s">
+        <v>160</v>
+      </c>
+      <c r="AH18">
+        <v>6000</v>
       </c>
       <c r="AP18">
-        <v>25000</v>
+        <v>50000</v>
       </c>
       <c r="AQ18">
+        <v>5000</v>
+      </c>
+      <c r="AR18">
+        <v>2000000000</v>
+      </c>
+      <c r="AS18">
         <v>1000</v>
-      </c>
-      <c r="AR18">
-        <v>75000000</v>
-      </c>
-      <c r="AS18">
-        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:57">
       <c r="A19">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
         <v>161</v>
@@ -2295,37 +2307,22 @@
         <v>164</v>
       </c>
       <c r="G19">
-        <v>1000</v>
-      </c>
-      <c r="J19" t="s">
-        <v>93</v>
-      </c>
-      <c r="K19">
-        <v>400</v>
-      </c>
-      <c r="L19">
-        <v>1</v>
-      </c>
-      <c r="M19">
-        <v>400</v>
-      </c>
-      <c r="N19">
-        <v>3</v>
-      </c>
-      <c r="O19">
-        <v>30</v>
-      </c>
-      <c r="S19" t="s">
+        <v>1500</v>
+      </c>
+      <c r="P19" t="s">
         <v>165</v>
       </c>
+      <c r="Q19">
+        <v>2</v>
+      </c>
+      <c r="R19" t="s">
+        <v>165</v>
+      </c>
+      <c r="T19" t="s">
+        <v>166</v>
+      </c>
       <c r="AH19">
-        <v>6000</v>
-      </c>
-      <c r="AP19">
-        <v>50000</v>
-      </c>
-      <c r="AQ19">
-        <v>5000</v>
+        <v>7000</v>
       </c>
       <c r="AR19">
         <v>2000000000</v>
@@ -2336,40 +2333,28 @@
     </row>
     <row r="20" spans="1:57">
       <c r="A20">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C20" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D20" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E20" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F20" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G20">
-        <v>1500</v>
-      </c>
-      <c r="P20" t="s">
-        <v>170</v>
-      </c>
-      <c r="Q20">
-        <v>2</v>
-      </c>
-      <c r="R20" t="s">
-        <v>170</v>
-      </c>
-      <c r="T20" t="s">
+        <v>2000</v>
+      </c>
+      <c r="S20" t="s">
         <v>171</v>
-      </c>
-      <c r="AH20">
-        <v>7000</v>
       </c>
       <c r="AR20">
         <v>2000000000</v>
@@ -2380,7 +2365,7 @@
     </row>
     <row r="21" spans="1:57">
       <c r="A21">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
         <v>172</v>
@@ -2398,110 +2383,116 @@
         <v>175</v>
       </c>
       <c r="G21">
+        <v>2500</v>
+      </c>
+      <c r="H21" t="s">
+        <v>155</v>
+      </c>
+      <c r="I21">
+        <v>50</v>
+      </c>
+      <c r="L21">
+        <v>13</v>
+      </c>
+      <c r="M21">
+        <v>50</v>
+      </c>
+      <c r="P21" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q21">
+        <v>5</v>
+      </c>
+      <c r="Z21">
+        <v>100</v>
+      </c>
+      <c r="AA21">
+        <v>2</v>
+      </c>
+      <c r="AC21">
+        <v>20000</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>141</v>
+      </c>
+      <c r="AE21">
+        <v>5</v>
+      </c>
+      <c r="AP21">
+        <v>20000</v>
+      </c>
+      <c r="AQ21">
         <v>2000</v>
       </c>
-      <c r="S21" t="s">
-        <v>176</v>
-      </c>
       <c r="AR21">
-        <v>2000000000</v>
+        <v>5000000000</v>
       </c>
       <c r="AS21">
-        <v>1000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="22" spans="1:57">
       <c r="A22">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s">
+        <v>176</v>
+      </c>
+      <c r="C22" t="s">
         <v>177</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>178</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>179</v>
-      </c>
-      <c r="E22" t="s">
-        <v>180</v>
       </c>
       <c r="F22" t="s">
         <v>180</v>
       </c>
-      <c r="G22">
-        <v>2500</v>
-      </c>
-      <c r="H22" t="s">
-        <v>160</v>
-      </c>
-      <c r="I22">
+      <c r="AR22">
+        <v>100000</v>
+      </c>
+      <c r="AS22">
         <v>50</v>
       </c>
-      <c r="L22">
-        <v>13</v>
-      </c>
-      <c r="M22">
-        <v>50</v>
-      </c>
-      <c r="P22" t="s">
-        <v>170</v>
-      </c>
-      <c r="Q22">
-        <v>5</v>
-      </c>
-      <c r="Z22">
-        <v>100</v>
-      </c>
-      <c r="AA22">
-        <v>2</v>
-      </c>
-      <c r="AC22">
-        <v>20000</v>
-      </c>
-      <c r="AD22" t="s">
-        <v>146</v>
-      </c>
-      <c r="AE22">
-        <v>5</v>
-      </c>
-      <c r="AP22">
-        <v>20000</v>
-      </c>
-      <c r="AQ22">
-        <v>2000</v>
-      </c>
-      <c r="AR22">
-        <v>5000000000</v>
-      </c>
-      <c r="AS22">
-        <v>1500</v>
+      <c r="AV22">
+        <v>25</v>
+      </c>
+      <c r="AX22">
+        <v>4</v>
+      </c>
+      <c r="AZ22" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="23" spans="1:57">
       <c r="A23">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C23" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D23" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E23" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F23" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AR23">
         <v>100000</v>
       </c>
       <c r="AS23">
-        <v>50</v>
+        <v>75</v>
+      </c>
+      <c r="AT23" t="s">
+        <v>176</v>
       </c>
       <c r="AV23">
         <v>25</v>
@@ -2509,13 +2500,13 @@
       <c r="AX23">
         <v>4</v>
       </c>
-      <c r="AZ23" t="s">
-        <v>186</v>
+      <c r="BA23">
+        <v>1000</v>
       </c>
     </row>
     <row r="24" spans="1:57">
       <c r="A24">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
         <v>187</v>
@@ -2530,16 +2521,25 @@
         <v>190</v>
       </c>
       <c r="F24" t="s">
+        <v>190</v>
+      </c>
+      <c r="S24" t="s">
         <v>191</v>
+      </c>
+      <c r="AP24">
+        <v>5000</v>
+      </c>
+      <c r="AQ24">
+        <v>5000</v>
       </c>
       <c r="AR24">
         <v>100000</v>
       </c>
       <c r="AS24">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="AT24" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="AV24">
         <v>25</v>
@@ -2547,13 +2547,10 @@
       <c r="AX24">
         <v>4</v>
       </c>
-      <c r="BA24">
-        <v>1000</v>
-      </c>
     </row>
     <row r="25" spans="1:57">
       <c r="A25">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
         <v>192</v>
@@ -2574,19 +2571,19 @@
         <v>196</v>
       </c>
       <c r="AP25">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="AQ25">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="AR25">
-        <v>100000</v>
+        <v>500000</v>
       </c>
       <c r="AS25">
         <v>100</v>
       </c>
       <c r="AT25" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="AV25">
         <v>25</v>
@@ -2597,7 +2594,7 @@
     </row>
     <row r="26" spans="1:57">
       <c r="A26">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
         <v>197</v>
@@ -2618,10 +2615,10 @@
         <v>201</v>
       </c>
       <c r="AP26">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="AQ26">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="AR26">
         <v>500000</v>
@@ -2630,7 +2627,7 @@
         <v>100</v>
       </c>
       <c r="AT26" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="AV26">
         <v>25</v>
@@ -2641,7 +2638,7 @@
     </row>
     <row r="27" spans="1:57">
       <c r="A27">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s">
         <v>202</v>
@@ -2656,25 +2653,40 @@
         <v>205</v>
       </c>
       <c r="F27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="S27" t="s">
-        <v>206</v>
+        <v>207</v>
+      </c>
+      <c r="AA27">
+        <v>1</v>
+      </c>
+      <c r="AB27">
+        <v>30</v>
+      </c>
+      <c r="AC27">
+        <v>500</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG27">
+        <v>1</v>
       </c>
       <c r="AP27">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="AQ27">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="AR27">
-        <v>500000</v>
+        <v>1000000</v>
       </c>
       <c r="AS27">
         <v>100</v>
       </c>
       <c r="AT27" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="AV27">
         <v>25</v>
@@ -2685,90 +2697,72 @@
     </row>
     <row r="28" spans="1:57">
       <c r="A28">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C28" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D28" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E28" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F28" t="s">
         <v>211</v>
       </c>
+      <c r="R28" t="s">
+        <v>212</v>
+      </c>
       <c r="S28" t="s">
+        <v>213</v>
+      </c>
+      <c r="T28" t="s">
+        <v>214</v>
+      </c>
+      <c r="AP28">
+        <v>25000</v>
+      </c>
+      <c r="AQ28">
+        <v>3000</v>
+      </c>
+      <c r="AR28">
+        <v>8000000000</v>
+      </c>
+      <c r="AS28">
+        <v>2000</v>
+      </c>
+      <c r="AZ28" t="s">
         <v>212</v>
-      </c>
-      <c r="AA28">
-        <v>1</v>
-      </c>
-      <c r="AB28">
-        <v>30</v>
-      </c>
-      <c r="AC28">
-        <v>500</v>
-      </c>
-      <c r="AF28" t="s">
-        <v>135</v>
-      </c>
-      <c r="AG28">
-        <v>1</v>
-      </c>
-      <c r="AP28">
-        <v>1000</v>
-      </c>
-      <c r="AQ28">
-        <v>1000</v>
-      </c>
-      <c r="AR28">
-        <v>1000000</v>
-      </c>
-      <c r="AS28">
-        <v>100</v>
-      </c>
-      <c r="AT28" t="s">
-        <v>181</v>
-      </c>
-      <c r="AV28">
-        <v>25</v>
-      </c>
-      <c r="AX28">
-        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:57">
       <c r="A29">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C29" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D29" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E29" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="F29" t="s">
-        <v>216</v>
-      </c>
-      <c r="R29" t="s">
-        <v>217</v>
-      </c>
-      <c r="S29" t="s">
-        <v>218</v>
-      </c>
-      <c r="T29" t="s">
         <v>219</v>
+      </c>
+      <c r="P29" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q29">
+        <v>2</v>
       </c>
       <c r="AP29">
         <v>25000</v>
@@ -2782,34 +2776,34 @@
       <c r="AS29">
         <v>2000</v>
       </c>
-      <c r="AZ29" t="s">
-        <v>217</v>
+      <c r="BD29" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:57">
       <c r="A30">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C30" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D30" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E30" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F30" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="P30" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="Q30">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AP30">
         <v>25000</v>
@@ -2823,13 +2817,10 @@
       <c r="AS30">
         <v>2000</v>
       </c>
-      <c r="BD30" t="s">
-        <v>225</v>
-      </c>
     </row>
     <row r="31" spans="1:57">
       <c r="A31">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B31" t="s">
         <v>226</v>
@@ -2844,13 +2835,13 @@
         <v>229</v>
       </c>
       <c r="F31" t="s">
+        <v>229</v>
+      </c>
+      <c r="R31" t="s">
         <v>230</v>
       </c>
-      <c r="P31" t="s">
-        <v>217</v>
-      </c>
-      <c r="Q31">
-        <v>5</v>
+      <c r="S31" t="s">
+        <v>231</v>
       </c>
       <c r="AP31">
         <v>25000</v>
@@ -2864,31 +2855,34 @@
       <c r="AS31">
         <v>2000</v>
       </c>
+      <c r="AZ31" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="32" spans="1:57">
       <c r="A32">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C32" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D32" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E32" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F32" t="s">
-        <v>234</v>
-      </c>
-      <c r="R32" t="s">
         <v>235</v>
       </c>
-      <c r="S32" t="s">
-        <v>236</v>
+      <c r="H32" t="s">
+        <v>155</v>
+      </c>
+      <c r="I32">
+        <v>200</v>
       </c>
       <c r="AP32">
         <v>25000</v>
@@ -2902,73 +2896,67 @@
       <c r="AS32">
         <v>2000</v>
       </c>
-      <c r="AZ32" t="s">
-        <v>235</v>
-      </c>
     </row>
     <row r="33" spans="1:57">
       <c r="A33">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B33" t="s">
+        <v>236</v>
+      </c>
+      <c r="C33" t="s">
         <v>237</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>238</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>239</v>
-      </c>
-      <c r="E33" t="s">
-        <v>240</v>
       </c>
       <c r="F33" t="s">
         <v>240</v>
       </c>
-      <c r="H33" t="s">
-        <v>160</v>
-      </c>
-      <c r="I33">
-        <v>200</v>
+      <c r="S33" t="s">
+        <v>241</v>
+      </c>
+      <c r="Y33">
+        <v>5000</v>
       </c>
       <c r="AP33">
-        <v>25000</v>
+        <v>50000</v>
       </c>
       <c r="AQ33">
-        <v>3000</v>
+        <v>6000</v>
       </c>
       <c r="AR33">
-        <v>8000000000</v>
+        <v>12000000000</v>
       </c>
       <c r="AS33">
-        <v>2000</v>
+        <v>5000</v>
+      </c>
+      <c r="BB33">
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:57">
       <c r="A34">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C34" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D34" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E34" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F34" t="s">
         <v>245</v>
       </c>
-      <c r="S34" t="s">
-        <v>246</v>
-      </c>
-      <c r="Y34">
-        <v>5000</v>
-      </c>
       <c r="AP34">
         <v>50000</v>
       </c>
@@ -2981,13 +2969,13 @@
       <c r="AS34">
         <v>5000</v>
       </c>
-      <c r="BB34">
-        <v>40</v>
+      <c r="BD34" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="35" spans="1:57">
       <c r="A35">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B35" t="s">
         <v>247</v>
@@ -3002,65 +2990,74 @@
         <v>250</v>
       </c>
       <c r="F35" t="s">
-        <v>250</v>
+        <v>251</v>
+      </c>
+      <c r="H35" t="s">
+        <v>252</v>
+      </c>
+      <c r="I35">
+        <v>25</v>
       </c>
       <c r="AP35">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="AQ35">
-        <v>6000</v>
+        <v>12000</v>
       </c>
       <c r="AR35">
-        <v>12000000000</v>
+        <v>16000000000</v>
       </c>
       <c r="AS35">
-        <v>5000</v>
-      </c>
-      <c r="BD35" t="s">
-        <v>251</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="36" spans="1:57">
       <c r="A36">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B36" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C36" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D36" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E36" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F36" t="s">
-        <v>256</v>
-      </c>
-      <c r="H36" t="s">
         <v>257</v>
       </c>
-      <c r="I36">
-        <v>25</v>
+      <c r="P36" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q36">
+        <v>5</v>
       </c>
       <c r="AP36">
+        <v>500</v>
+      </c>
+      <c r="AQ36">
+        <v>250</v>
+      </c>
+      <c r="AR36">
         <v>100000</v>
       </c>
-      <c r="AQ36">
-        <v>12000</v>
-      </c>
-      <c r="AR36">
-        <v>16000000000</v>
-      </c>
       <c r="AS36">
-        <v>8000</v>
+        <v>100</v>
+      </c>
+      <c r="AV36">
+        <v>1500</v>
+      </c>
+      <c r="BE36">
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:57">
       <c r="A37">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B37" t="s">
         <v>258</v>
@@ -3075,36 +3072,33 @@
         <v>261</v>
       </c>
       <c r="F37" t="s">
+        <v>261</v>
+      </c>
+      <c r="H37" t="s">
+        <v>252</v>
+      </c>
+      <c r="I37">
+        <v>75</v>
+      </c>
+      <c r="S37" t="s">
         <v>262</v>
       </c>
-      <c r="P37" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q37">
-        <v>5</v>
-      </c>
       <c r="AP37">
-        <v>500</v>
+        <v>150000</v>
       </c>
       <c r="AQ37">
-        <v>250</v>
+        <v>30000</v>
       </c>
       <c r="AR37">
-        <v>100000</v>
+        <v>32000000000</v>
       </c>
       <c r="AS37">
-        <v>100</v>
-      </c>
-      <c r="AV37">
-        <v>100</v>
-      </c>
-      <c r="BE37">
-        <v>2</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="38" spans="1:57">
       <c r="A38">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B38" t="s">
         <v>263</v>
@@ -3119,16 +3113,40 @@
         <v>266</v>
       </c>
       <c r="F38" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="H38" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="I38">
-        <v>75</v>
-      </c>
-      <c r="S38" t="s">
-        <v>267</v>
+        <v>150</v>
+      </c>
+      <c r="N38">
+        <v>3</v>
+      </c>
+      <c r="O38">
+        <v>100</v>
+      </c>
+      <c r="Z38">
+        <v>10000</v>
+      </c>
+      <c r="AA38">
+        <v>10</v>
+      </c>
+      <c r="AC38">
+        <v>50000</v>
+      </c>
+      <c r="AD38" t="s">
+        <v>268</v>
+      </c>
+      <c r="AE38">
+        <v>30</v>
+      </c>
+      <c r="AF38" t="s">
+        <v>269</v>
+      </c>
+      <c r="AG38">
+        <v>4</v>
       </c>
       <c r="AP38">
         <v>150000</v>
@@ -3145,55 +3163,31 @@
     </row>
     <row r="39" spans="1:57">
       <c r="A39">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B39" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C39" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="D39" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="E39" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="F39" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="H39" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="I39">
-        <v>150</v>
-      </c>
-      <c r="N39">
-        <v>3</v>
-      </c>
-      <c r="O39">
-        <v>100</v>
-      </c>
-      <c r="Z39">
-        <v>10000</v>
-      </c>
-      <c r="AA39">
-        <v>10</v>
-      </c>
-      <c r="AC39">
-        <v>50000</v>
-      </c>
-      <c r="AD39" t="s">
-        <v>273</v>
-      </c>
-      <c r="AE39">
-        <v>30</v>
-      </c>
-      <c r="AF39" t="s">
-        <v>274</v>
-      </c>
-      <c r="AG39">
-        <v>4</v>
+        <v>300</v>
+      </c>
+      <c r="AH39">
+        <v>1000000</v>
       </c>
       <c r="AP39">
         <v>150000</v>
@@ -3210,31 +3204,37 @@
     </row>
     <row r="40" spans="1:57">
       <c r="A40">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B40" t="s">
+        <v>274</v>
+      </c>
+      <c r="C40" t="s">
         <v>275</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>276</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>277</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
+        <v>277</v>
+      </c>
+      <c r="H40" t="s">
+        <v>252</v>
+      </c>
+      <c r="I40">
+        <v>400</v>
+      </c>
+      <c r="S40" t="s">
         <v>278</v>
       </c>
-      <c r="F40" t="s">
-        <v>278</v>
-      </c>
-      <c r="H40" t="s">
-        <v>257</v>
-      </c>
-      <c r="I40">
-        <v>300</v>
+      <c r="T40" t="s">
+        <v>279</v>
       </c>
       <c r="AH40">
-        <v>1000000</v>
+        <v>2000000</v>
       </c>
       <c r="AP40">
         <v>150000</v>
@@ -3251,37 +3251,25 @@
     </row>
     <row r="41" spans="1:57">
       <c r="A41">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B41" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C41" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D41" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E41" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F41" t="s">
-        <v>282</v>
-      </c>
-      <c r="H41" t="s">
-        <v>257</v>
-      </c>
-      <c r="I41">
-        <v>400</v>
-      </c>
-      <c r="S41" t="s">
         <v>283</v>
       </c>
-      <c r="T41" t="s">
-        <v>284</v>
-      </c>
       <c r="AH41">
-        <v>2000000</v>
+        <v>2500000</v>
       </c>
       <c r="AP41">
         <v>150000</v>
@@ -3295,10 +3283,13 @@
       <c r="AS41">
         <v>8000</v>
       </c>
+      <c r="AZ41" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="42" spans="1:57">
       <c r="A42">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B42" t="s">
         <v>285</v>
@@ -3313,45 +3304,51 @@
         <v>288</v>
       </c>
       <c r="F42" t="s">
-        <v>288</v>
-      </c>
-      <c r="AH42">
-        <v>2500000</v>
+        <v>289</v>
       </c>
       <c r="AP42">
-        <v>150000</v>
+        <v>100</v>
       </c>
       <c r="AQ42">
-        <v>30000</v>
+        <v>100</v>
       </c>
       <c r="AR42">
-        <v>32000000000</v>
+        <v>1000</v>
       </c>
       <c r="AS42">
-        <v>8000</v>
+        <v>100</v>
+      </c>
+      <c r="AV42">
+        <v>10</v>
+      </c>
+      <c r="AX42">
+        <v>8</v>
       </c>
       <c r="AZ42" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="43" spans="1:57">
       <c r="A43">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B43" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C43" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D43" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E43" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F43" t="s">
-        <v>294</v>
+        <v>295</v>
+      </c>
+      <c r="Q43">
+        <v>1</v>
       </c>
       <c r="AP43">
         <v>100</v>
@@ -3365,19 +3362,22 @@
       <c r="AS43">
         <v>100</v>
       </c>
-      <c r="AV43">
-        <v>10</v>
+      <c r="AT43" t="s">
+        <v>285</v>
       </c>
       <c r="AX43">
         <v>8</v>
       </c>
       <c r="AZ43" t="s">
-        <v>295</v>
+        <v>290</v>
+      </c>
+      <c r="BA43">
+        <v>1000</v>
       </c>
     </row>
     <row r="44" spans="1:57">
       <c r="A44">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B44" t="s">
         <v>296</v>
@@ -3394,11 +3394,8 @@
       <c r="F44" t="s">
         <v>300</v>
       </c>
-      <c r="P44" t="s">
-        <v>295</v>
-      </c>
-      <c r="Q44">
-        <v>1</v>
+      <c r="S44" t="s">
+        <v>301</v>
       </c>
       <c r="AP44">
         <v>100</v>
@@ -3413,38 +3410,38 @@
         <v>100</v>
       </c>
       <c r="AT44" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="AX44">
         <v>8</v>
       </c>
-      <c r="AZ44" t="s">
-        <v>295</v>
-      </c>
-      <c r="BA44">
-        <v>1000</v>
-      </c>
     </row>
     <row r="45" spans="1:57">
       <c r="A45">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B45" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C45" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D45" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E45" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F45" t="s">
         <v>305</v>
       </c>
+      <c r="Q45">
+        <v>5</v>
+      </c>
       <c r="S45" t="s">
+        <v>101</v>
+      </c>
+      <c r="T45" t="s">
         <v>306</v>
       </c>
       <c r="AP45">
@@ -3465,58 +3462,8 @@
       <c r="AX45">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="1:57">
-      <c r="A46">
-        <v>50</v>
-      </c>
-      <c r="B46" t="s">
-        <v>307</v>
-      </c>
-      <c r="C46" t="s">
-        <v>308</v>
-      </c>
-      <c r="D46" t="s">
-        <v>309</v>
-      </c>
-      <c r="E46" t="s">
-        <v>310</v>
-      </c>
-      <c r="F46" t="s">
-        <v>310</v>
-      </c>
-      <c r="P46" t="s">
-        <v>295</v>
-      </c>
-      <c r="Q46">
-        <v>5</v>
-      </c>
-      <c r="S46" t="s">
-        <v>101</v>
-      </c>
-      <c r="T46" t="s">
-        <v>311</v>
-      </c>
-      <c r="AP46">
-        <v>100</v>
-      </c>
-      <c r="AQ46">
-        <v>100</v>
-      </c>
-      <c r="AR46">
-        <v>1000</v>
-      </c>
-      <c r="AS46">
-        <v>100</v>
-      </c>
-      <c r="AT46" t="s">
-        <v>301</v>
-      </c>
-      <c r="AX46">
-        <v>8</v>
-      </c>
-      <c r="AZ46" t="s">
-        <v>295</v>
+      <c r="AZ45" t="s">
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>